<commit_message>
client form: hide/show birth province
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="104">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -137,6 +137,15 @@
     <t xml:space="preserve">Family Name (Khmer)</t>
   </si>
   <si>
+    <t xml:space="preserve">birth_province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth Province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hide</t>
+  </si>
+  <si>
     <t xml:space="preserve">v_score</t>
   </si>
   <si>
@@ -231,9 +240,6 @@
   </si>
   <si>
     <t xml:space="preserve">Province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide</t>
   </si>
   <si>
     <t xml:space="preserve">district_id</t>
@@ -338,7 +344,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -420,6 +426,13 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -573,7 +586,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -674,6 +687,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -694,11 +711,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -803,17 +820,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.5"/>
@@ -1198,13 +1215,13 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="24" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="0"/>
@@ -1218,63 +1235,62 @@
         <v>0</v>
       </c>
       <c r="H14" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>24</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I14" s="23"/>
       <c r="J14" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="10" t="n">
+      <c r="E15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="25" t="n">
+      <c r="G16" s="26" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="10" t="n">
@@ -1287,11 +1303,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26" t="s">
+    <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="18" t="s">
@@ -1299,209 +1315,209 @@
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="30" t="s">
+      <c r="A18" s="27" t="s">
         <v>48</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="A19" s="27" t="s">
         <v>50</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="D19" s="0"/>
       <c r="E19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D20" s="0"/>
       <c r="E20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D23" s="0"/>
       <c r="E23" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="11" t="s">
+      <c r="J23" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="18" t="s">
@@ -1509,562 +1525,592 @@
       </c>
       <c r="D24" s="0"/>
       <c r="E24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D26" s="0"/>
       <c r="E26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="26" t="s">
+      <c r="A28" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J28" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="J29" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="31" t="s">
+      <c r="A30" s="27" t="s">
         <v>69</v>
       </c>
+      <c r="B30" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="29" t="n">
-        <v>1</v>
+      <c r="E30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="30" t="n">
+        <v>0</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="0"/>
+      <c r="E32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="0"/>
+      <c r="E33" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="0"/>
+      <c r="E34" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="0"/>
+      <c r="E35" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="0"/>
+      <c r="E36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="0"/>
+      <c r="E37" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="0"/>
-      <c r="E31" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="0"/>
-      <c r="E32" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="0"/>
-      <c r="E33" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J33" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="0"/>
-      <c r="E34" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J34" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="0"/>
-      <c r="E36" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="0"/>
-      <c r="E37" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>85</v>
-      </c>
       <c r="D38" s="0"/>
-      <c r="E38" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="29" t="n">
+      <c r="E38" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="29" t="s">
-        <v>70</v>
+      <c r="J38" s="30" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>87</v>
       </c>
       <c r="D39" s="0"/>
-      <c r="E39" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="32" t="s">
+      <c r="E39" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J39" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="36" t="s">
+      <c r="G40" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="0"/>
-      <c r="E40" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="32" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="0"/>
+      <c r="E41" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J40" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="0"/>
-      <c r="E41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" s="32" t="s">
+      <c r="G41" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="0"/>
+      <c r="E42" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J41" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="32" t="s">
+      <c r="G42" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="0"/>
-      <c r="E42" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="32" t="s">
+      <c r="C43" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="0"/>
+      <c r="E43" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J42" s="37" t="s">
-        <v>88</v>
+      <c r="G43" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="38" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2083,10 +2129,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2142,8 +2188,8 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>95</v>
+      <c r="D2" s="37" t="s">
+        <v>97</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2173,7 +2219,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>11</v>
@@ -2203,7 +2249,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>11</v>
@@ -2233,7 +2279,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>11</v>
@@ -2263,7 +2309,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>11</v>
@@ -2357,7 +2403,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>11</v>
@@ -2451,7 +2497,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>11</v>
@@ -2481,7 +2527,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>11</v>
@@ -2501,18 +2547,16 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="24" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>39</v>
-      </c>
+      <c r="D14" s="0"/>
       <c r="E14" s="22" t="s">
         <v>11</v>
       </c>
@@ -2523,67 +2567,65 @@
         <v>0</v>
       </c>
       <c r="H14" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>24</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I14" s="23"/>
       <c r="J14" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="6" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="25" t="n">
+      <c r="G16" s="26" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="10" t="n">
@@ -2596,11 +2638,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26" t="s">
+    <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="18" t="s">
@@ -2610,221 +2652,221 @@
         <v>46</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="29" t="n">
+      <c r="F18" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="A19" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>50</v>
+      <c r="B19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="29" t="n">
+        <v>47</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="11" t="s">
+      <c r="J23" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="18" t="s">
@@ -2834,576 +2876,608 @@
         <v>46</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="F25" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="29" t="n">
+      <c r="F26" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="26" t="s">
+      <c r="A28" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J28" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="29" t="n">
+        <v>61</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="J29" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="31" t="s">
+      <c r="A30" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="29" t="n">
-        <v>0</v>
+      <c r="B30" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="30" t="n">
+        <v>1</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="18"/>
+      <c r="E36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="18"/>
+      <c r="E37" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J33" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J34" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>85</v>
-      </c>
       <c r="D38" s="18"/>
-      <c r="E38" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="29" t="n">
+      <c r="E38" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="30" t="n">
         <v>0</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="29" t="s">
-        <v>70</v>
+      <c r="J38" s="30" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="32" t="s">
+      <c r="D39" s="18"/>
+      <c r="E39" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J39" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="36" t="s">
+      <c r="G40" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="32" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J40" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" s="32" t="s">
+      <c r="G41" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J41" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="32" t="s">
+      <c r="G42" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="32" t="s">
+      <c r="C43" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J42" s="37" t="s">
-        <v>88</v>
+      <c r="G43" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="38" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added client legacy_brcs_id column
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="109">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t xml:space="preserve">ID number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legacy_brcs_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legacy BRCS-ID number</t>
   </si>
   <si>
     <t xml:space="preserve">client_phone</t>
@@ -833,10 +839,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1112,61 +1118,61 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="0"/>
-      <c r="E10" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="E10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J10" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1200,13 +1206,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="0"/>
@@ -1220,11 +1226,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J13" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1262,7 +1270,7 @@
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="0"/>
@@ -1280,19 +1288,18 @@
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
+      <c r="B16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="23" t="s">
@@ -1305,42 +1312,41 @@
         <v>0</v>
       </c>
       <c r="H16" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>26</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I16" s="24"/>
       <c r="J16" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="10" t="n">
+      <c r="E17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1356,51 +1362,51 @@
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="s">
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="D19" s="0"/>
       <c r="E19" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="31" t="n">
+        <v>51</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1411,12 +1417,12 @@
       <c r="B20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="0"/>
       <c r="E20" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>13</v>
@@ -1441,12 +1447,12 @@
       <c r="B21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="32" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>13</v>
@@ -1476,7 +1482,7 @@
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>13</v>
@@ -1506,7 +1512,7 @@
       </c>
       <c r="D23" s="0"/>
       <c r="E23" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>13</v>
@@ -1536,7 +1542,7 @@
       </c>
       <c r="D24" s="0"/>
       <c r="E24" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F24" s="29" t="s">
         <v>13</v>
@@ -1555,78 +1561,78 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="10" t="n">
+        <v>51</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="31" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="0"/>
       <c r="E26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="31" t="n">
+        <v>65</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>13</v>
@@ -1652,11 +1658,11 @@
         <v>11</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>13</v>
@@ -1676,7 +1682,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>11</v>
@@ -1686,7 +1692,7 @@
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>13</v>
@@ -1706,17 +1712,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
@@ -1746,7 +1752,7 @@
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>13</v>
@@ -1771,12 +1777,12 @@
       <c r="B32" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D32" s="0"/>
-      <c r="E32" s="29" t="s">
-        <v>11</v>
+      <c r="E32" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>13</v>
@@ -1785,13 +1791,13 @@
         <v>0</v>
       </c>
       <c r="H32" s="31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J32" s="31" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1821,7 +1827,7 @@
         <v>26</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1851,7 +1857,7 @@
         <v>26</v>
       </c>
       <c r="J34" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1881,7 +1887,7 @@
         <v>26</v>
       </c>
       <c r="J35" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1911,7 +1917,7 @@
         <v>26</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1941,7 +1947,7 @@
         <v>26</v>
       </c>
       <c r="J37" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1971,7 +1977,7 @@
         <v>26</v>
       </c>
       <c r="J38" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1982,7 +1988,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D39" s="0"/>
       <c r="E39" s="29" t="s">
@@ -2001,18 +2007,18 @@
         <v>26</v>
       </c>
       <c r="J39" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D40" s="0"/>
       <c r="E40" s="29" t="s">
@@ -2031,52 +2037,52 @@
         <v>26</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="34" t="s">
+      <c r="B41" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="33" t="s">
         <v>91</v>
       </c>
       <c r="D41" s="0"/>
-      <c r="E41" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="36" t="n">
+      <c r="E41" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="31" t="n">
         <v>1</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J41" s="37" t="s">
-        <v>92</v>
+      <c r="J41" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="34" t="s">
         <v>93</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>94</v>
       </c>
       <c r="D42" s="0"/>
       <c r="E42" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F42" s="34" t="s">
         <v>4</v>
@@ -2091,7 +2097,7 @@
         <v>26</v>
       </c>
       <c r="J42" s="37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2099,9 +2105,9 @@
         <v>95</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D43" s="0"/>
@@ -2121,7 +2127,7 @@
         <v>26</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2129,7 +2135,7 @@
         <v>97</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>98</v>
@@ -2150,8 +2156,38 @@
       <c r="I44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="39" t="s">
-        <v>92</v>
+      <c r="J44" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" s="39" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2170,10 +2206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2230,7 +2266,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2260,7 +2296,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>11</v>
@@ -2290,7 +2326,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>11</v>
@@ -2320,7 +2356,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>11</v>
@@ -2350,7 +2386,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>11</v>
@@ -2380,7 +2416,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>11</v>
@@ -2464,22 +2500,20 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="D10" s="0"/>
+      <c r="E10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="10" t="n">
@@ -2488,41 +2522,41 @@
       <c r="H10" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J10" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2558,17 +2592,17 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>11</v>
@@ -2582,9 +2616,11 @@
       <c r="H13" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J13" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2598,7 +2634,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>11</v>
@@ -2624,10 +2660,12 @@
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="0"/>
+      <c r="D15" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="E15" s="23" t="s">
         <v>11</v>
       </c>
@@ -2638,50 +2676,46 @@
         <v>0</v>
       </c>
       <c r="H15" s="24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
+      <c r="B16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="0"/>
+      <c r="E16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
@@ -2690,22 +2724,22 @@
       <c r="D17" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="10" t="n">
+      <c r="E17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2723,53 +2757,53 @@
         <v>48</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="s">
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="31" t="n">
+      <c r="F19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2780,14 +2814,14 @@
       <c r="B20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="19" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>13</v>
@@ -2812,14 +2846,14 @@
       <c r="B21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="32" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>13</v>
@@ -2851,7 +2885,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>13</v>
@@ -2883,7 +2917,7 @@
         <v>59</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>13</v>
@@ -2915,7 +2949,7 @@
         <v>61</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F24" s="29" t="s">
         <v>13</v>
@@ -2934,84 +2968,84 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="10" t="n">
+        <v>51</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="31" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="31" t="n">
+        <v>65</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>13</v>
@@ -3037,13 +3071,13 @@
         <v>11</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>13</v>
@@ -3063,7 +3097,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>11</v>
@@ -3075,7 +3109,7 @@
         <v>57</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>13</v>
@@ -3095,19 +3129,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
@@ -3139,7 +3173,7 @@
         <v>72</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>13</v>
@@ -3164,12 +3198,14 @@
       <c r="B32" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="29" t="s">
-        <v>11</v>
+      <c r="D32" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>13</v>
@@ -3178,13 +3214,13 @@
         <v>0</v>
       </c>
       <c r="H32" s="31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J32" s="31" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3214,7 +3250,7 @@
         <v>26</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3244,7 +3280,7 @@
         <v>26</v>
       </c>
       <c r="J34" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3274,7 +3310,7 @@
         <v>26</v>
       </c>
       <c r="J35" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3304,7 +3340,7 @@
         <v>26</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3334,7 +3370,7 @@
         <v>26</v>
       </c>
       <c r="J37" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3364,7 +3400,7 @@
         <v>26</v>
       </c>
       <c r="J38" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3375,7 +3411,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="29" t="s">
@@ -3394,18 +3430,18 @@
         <v>26</v>
       </c>
       <c r="J39" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="29" t="s">
@@ -3424,52 +3460,52 @@
         <v>26</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="34" t="s">
+      <c r="B41" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="36" t="n">
+      <c r="D41" s="19"/>
+      <c r="E41" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="31" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J41" s="37" t="s">
-        <v>92</v>
+      <c r="J41" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="34" t="s">
         <v>93</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>94</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F42" s="34" t="s">
         <v>4</v>
@@ -3484,7 +3520,7 @@
         <v>26</v>
       </c>
       <c r="J42" s="37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3492,14 +3528,12 @@
         <v>95</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="34" t="s">
-        <v>96</v>
-      </c>
+      <c r="D43" s="34"/>
       <c r="E43" s="34" t="s">
         <v>95</v>
       </c>
@@ -3516,7 +3550,7 @@
         <v>26</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3524,7 +3558,7 @@
         <v>97</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>98</v>
@@ -3547,8 +3581,40 @@
       <c r="I44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="39" t="s">
-        <v>92</v>
+      <c r="J44" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" s="39" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverted hiding referee address
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="107">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -306,12 +306,6 @@
   </si>
   <si>
     <t xml:space="preserve">hide section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">referee_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referee</t>
   </si>
   <si>
     <t xml:space="preserve">family</t>
@@ -754,12 +748,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -839,10 +833,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2105,9 +2099,9 @@
         <v>95</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="34" t="s">
         <v>96</v>
       </c>
       <c r="D43" s="0"/>
@@ -2135,7 +2129,7 @@
         <v>97</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>98</v>
@@ -2156,37 +2150,7 @@
       <c r="I44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="0"/>
-      <c r="E45" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="39" t="s">
+      <c r="J44" s="38" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2206,10 +2170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2265,8 +2229,8 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="38" t="s">
-        <v>101</v>
+      <c r="D2" s="39" t="s">
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2296,7 +2260,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>11</v>
@@ -2326,7 +2290,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>11</v>
@@ -2356,7 +2320,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>11</v>
@@ -2386,7 +2350,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>11</v>
@@ -2416,7 +2380,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>11</v>
@@ -2540,7 +2504,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>11</v>
@@ -2634,7 +2598,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>11</v>
@@ -2664,7 +2628,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>11</v>
@@ -3528,12 +3492,14 @@
         <v>95</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="34"/>
+      <c r="D43" s="34" t="s">
+        <v>96</v>
+      </c>
       <c r="E43" s="34" t="s">
         <v>95</v>
       </c>
@@ -3558,7 +3524,7 @@
         <v>97</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>98</v>
@@ -3581,39 +3547,7 @@
       <c r="I44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="E45" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="39" t="s">
+      <c r="J44" s="38" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
combine city and settlement
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="106">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -197,151 +197,148 @@
     <t xml:space="preserve">PO BOX</t>
   </si>
   <si>
+    <t xml:space="preserve">current_settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City/Settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current_resident_own_or_rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc. type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current_household_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">island2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client_other_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po_box2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">settlement2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_own_or_rent2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_type2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">province_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District / Khan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commune_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commune / Sangkat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what3words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What3Words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client_school_information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client / School Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hide section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Families</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Worker / Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Referral Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone Number - Primary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name - Alternate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name - Alternate</t>
+  </si>
+  <si>
     <t xml:space="preserve">current_city</t>
   </si>
   <si>
     <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_settlement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settlement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_resident_own_or_rent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acc. type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_household_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">island2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_other_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">po_box2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">settlement2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resident_own_or_rent2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">household_type2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">province_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">district_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">District / Khan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commune_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commune / Sangkat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">house_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">House Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what3words</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What3Words</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_school_information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client / School Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Families</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partners</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Worker / Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial Referral Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number - Primary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name - Alternate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name - Alternate</t>
   </si>
 </sst>
 </file>
@@ -833,10 +830,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="1" sqref="D26 C31"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="D24 C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1557,7 +1554,7 @@
       <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="33" t="s">
         <v>63</v>
       </c>
       <c r="D25" s="0"/>
@@ -1581,78 +1578,78 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>65</v>
+      <c r="B26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="D26" s="0"/>
       <c r="E26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="31" t="n">
+        <v>65</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="10" t="n">
+        <v>65</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="31" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>13</v>
@@ -1678,11 +1675,11 @@
         <v>11</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>13</v>
@@ -1702,17 +1699,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
@@ -1732,17 +1729,17 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>13</v>
@@ -1762,17 +1759,17 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>63</v>
-      </c>
       <c r="D32" s="0"/>
-      <c r="E32" s="6" t="s">
-        <v>67</v>
+      <c r="E32" s="29" t="s">
+        <v>11</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>13</v>
@@ -1781,13 +1778,13 @@
         <v>0</v>
       </c>
       <c r="H32" s="31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J32" s="31" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1797,12 +1794,12 @@
       <c r="B33" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>65</v>
+      <c r="C33" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="D33" s="0"/>
-      <c r="E33" s="6" t="s">
-        <v>67</v>
+      <c r="E33" s="29" t="s">
+        <v>11</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>13</v>
@@ -1811,24 +1808,24 @@
         <v>0</v>
       </c>
       <c r="H33" s="31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="29" t="s">
@@ -1852,13 +1849,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="0"/>
       <c r="E35" s="29" t="s">
@@ -1882,13 +1879,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D36" s="0"/>
       <c r="E36" s="29" t="s">
@@ -1912,13 +1909,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D37" s="0"/>
       <c r="E37" s="29" t="s">
@@ -1942,13 +1939,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D38" s="0"/>
       <c r="E38" s="29" t="s">
@@ -1972,13 +1969,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D39" s="0"/>
       <c r="E39" s="29" t="s">
@@ -2031,78 +2028,78 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>65</v>
+      <c r="B41" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>90</v>
       </c>
       <c r="D41" s="0"/>
-      <c r="E41" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="31" t="n">
+      <c r="E41" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="36" t="n">
         <v>1</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J41" s="31" t="s">
-        <v>36</v>
+      <c r="J41" s="37" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="33" t="s">
+      <c r="A42" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="0"/>
+      <c r="E42" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" s="37" t="s">
         <v>91</v>
-      </c>
-      <c r="D42" s="0"/>
-      <c r="E42" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="34" t="s">
-        <v>11</v>
-      </c>
       <c r="C43" s="34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D43" s="0"/>
       <c r="E43" s="34" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F43" s="34" t="s">
         <v>4</v>
@@ -2116,68 +2113,8 @@
       <c r="I43" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J43" s="37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="0"/>
-      <c r="E44" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G44" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="0"/>
-      <c r="E45" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="38" t="s">
-        <v>94</v>
+      <c r="J43" s="38" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2196,10 +2133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2256,7 +2193,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2286,7 +2223,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>11</v>
@@ -2316,7 +2253,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>11</v>
@@ -2346,7 +2283,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>11</v>
@@ -2376,7 +2313,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>11</v>
@@ -2406,7 +2343,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>11</v>
@@ -2530,7 +2467,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>11</v>
@@ -2680,7 +2617,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>11</v>
@@ -2710,7 +2647,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>11</v>
@@ -2887,16 +2824,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>53</v>
@@ -2919,16 +2856,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>53</v>
@@ -2951,16 +2888,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>53</v>
@@ -2983,16 +2920,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>53</v>
@@ -3015,7 +2952,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>11</v>
@@ -3027,7 +2964,7 @@
         <v>52</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>13</v>
@@ -3047,7 +2984,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>11</v>
@@ -3059,7 +2996,7 @@
         <v>55</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>13</v>
@@ -3079,19 +3016,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>13</v>
@@ -3111,7 +3048,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
@@ -3123,7 +3060,7 @@
         <v>59</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
@@ -3143,7 +3080,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>11</v>
@@ -3155,7 +3092,7 @@
         <v>61</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>13</v>
@@ -3175,7 +3112,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>11</v>
@@ -3187,7 +3124,7 @@
         <v>63</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>13</v>
@@ -3207,19 +3144,17 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>67</v>
+      <c r="C33" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="29" t="s">
+        <v>11</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>13</v>
@@ -3228,24 +3163,24 @@
         <v>0</v>
       </c>
       <c r="H33" s="31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="33" t="s">
         <v>75</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>76</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="29" t="s">
@@ -3269,13 +3204,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="33" t="s">
         <v>77</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>78</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="29" t="s">
@@ -3299,13 +3234,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="33" t="s">
         <v>79</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>80</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="29" t="s">
@@ -3329,13 +3264,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>82</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="29" t="s">
@@ -3359,13 +3294,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="33" t="s">
         <v>83</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>84</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="29" t="s">
@@ -3389,13 +3324,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="33" t="s">
         <v>85</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>86</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="29" t="s">
@@ -3419,13 +3354,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="29" t="s">
@@ -3449,13 +3384,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="29" t="s">
@@ -3478,33 +3413,33 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="33" t="s">
+      <c r="D42" s="34"/>
+      <c r="E42" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" s="37" t="s">
         <v>91</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3512,12 +3447,14 @@
         <v>92</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="C43" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="34"/>
+      <c r="D43" s="34" t="s">
+        <v>93</v>
+      </c>
       <c r="E43" s="34" t="s">
         <v>92</v>
       </c>
@@ -3534,24 +3471,24 @@
         <v>26</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="D44" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="34" t="s">
-        <v>96</v>
-      </c>
       <c r="E44" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="34" t="s">
         <v>4</v>
@@ -3565,40 +3502,8 @@
       <c r="I44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="38" t="s">
-        <v>94</v>
+      <c r="J44" s="38" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added gender to family member
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AC7F25-8CA9-9646-BEE5-BCB768FD7E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="default" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="brc" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="default" sheetId="1" r:id="rId1"/>
+    <sheet name="brc" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -21,353 +26,341 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="105">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">klass_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for_instances</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Worker / Assigned Staff Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initial_referral_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Referral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given Name (Latin)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Name (Latin)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relevant_referral_information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relevant Referral Information / Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">presented_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presented ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legacy_brcs_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legacy BRCS-ID number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client Contact Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone_owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rated_for_id_poor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is client rated for ID Poor?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whatsapp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whatsapp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other_phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number - Alternate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">local_given_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given Name(Khmer)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">local_family_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Name (Khmer)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth_province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth Province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brsc_branch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRCS Branch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_current_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_po_box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PO BOX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_settlement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City/Settlement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_resident_own_or_rent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acc. type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_household_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">island2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_other_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">po_box2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">settlement2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resident_own_or_rent2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">household_type2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">province_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">district_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">District / Khan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commune_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commune / Sangkat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">house_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">House Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what3words</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What3Words</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_school_information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client / School Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partners</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Worker / Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial Referral Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number - Primary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name - Alternate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name - Alternate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="108">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>klass_name</t>
+  </si>
+  <si>
+    <t>current_label</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>for_instances</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>user_ids</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>Case Worker / Assigned Staff Manager</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>rename</t>
+  </si>
+  <si>
+    <t>initial_referral_date</t>
+  </si>
+  <si>
+    <t>Date of Referral</t>
+  </si>
+  <si>
+    <t>given_name</t>
+  </si>
+  <si>
+    <t>Given Name (Latin)</t>
+  </si>
+  <si>
+    <t>family_name</t>
+  </si>
+  <si>
+    <t>Family Name (Latin)</t>
+  </si>
+  <si>
+    <t>relevant_referral_information</t>
+  </si>
+  <si>
+    <t>Relevant Referral Information / Notes</t>
+  </si>
+  <si>
+    <t>presented_id</t>
+  </si>
+  <si>
+    <t>Presented ID</t>
+  </si>
+  <si>
+    <t>brc</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>id_number</t>
+  </si>
+  <si>
+    <t>ID number</t>
+  </si>
+  <si>
+    <t>legacy_brcs_id</t>
+  </si>
+  <si>
+    <t>Legacy BRCS-ID number</t>
+  </si>
+  <si>
+    <t>client_phone</t>
+  </si>
+  <si>
+    <t>Client Contact Phone</t>
+  </si>
+  <si>
+    <t>phone_owner</t>
+  </si>
+  <si>
+    <t>Phone Owner</t>
+  </si>
+  <si>
+    <t>hide</t>
+  </si>
+  <si>
+    <t>rated_for_id_poor</t>
+  </si>
+  <si>
+    <t>Is client rated for ID Poor?</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>Whatsapp</t>
+  </si>
+  <si>
+    <t>other_phone_number</t>
+  </si>
+  <si>
+    <t>Phone Number - Alternate</t>
+  </si>
+  <si>
+    <t>local_given_name</t>
+  </si>
+  <si>
+    <t>Given Name(Khmer)</t>
+  </si>
+  <si>
+    <t>local_family_name</t>
+  </si>
+  <si>
+    <t>Family Name (Khmer)</t>
+  </si>
+  <si>
+    <t>birth_province</t>
+  </si>
+  <si>
+    <t>Birth Province</t>
+  </si>
+  <si>
+    <t>brsc_branch</t>
+  </si>
+  <si>
+    <t>BRCS Branch</t>
+  </si>
+  <si>
+    <t>current_island</t>
+  </si>
+  <si>
+    <t>Island</t>
+  </si>
+  <si>
+    <t>client_current_address</t>
+  </si>
+  <si>
+    <t>current_street</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>current_po_box</t>
+  </si>
+  <si>
+    <t>PO BOX</t>
+  </si>
+  <si>
+    <t>current_settlement</t>
+  </si>
+  <si>
+    <t>City/Settlement</t>
+  </si>
+  <si>
+    <t>current_resident_own_or_rent</t>
+  </si>
+  <si>
+    <t>Acc. type</t>
+  </si>
+  <si>
+    <t>current_household_type</t>
+  </si>
+  <si>
+    <t>Address Type</t>
+  </si>
+  <si>
+    <t>island2</t>
+  </si>
+  <si>
+    <t>client_other_address</t>
+  </si>
+  <si>
+    <t>street2</t>
+  </si>
+  <si>
+    <t>po_box2</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>settlement2</t>
+  </si>
+  <si>
+    <t>resident_own_or_rent2</t>
+  </si>
+  <si>
+    <t>household_type2</t>
+  </si>
+  <si>
+    <t>province_id</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>district_id</t>
+  </si>
+  <si>
+    <t>District / Khan</t>
+  </si>
+  <si>
+    <t>commune_id</t>
+  </si>
+  <si>
+    <t>Commune / Sangkat</t>
+  </si>
+  <si>
+    <t>village_id</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>street_number</t>
+  </si>
+  <si>
+    <t>Street Number</t>
+  </si>
+  <si>
+    <t>house_number</t>
+  </si>
+  <si>
+    <t>House Number</t>
+  </si>
+  <si>
+    <t>current_address</t>
+  </si>
+  <si>
+    <t>Address Name</t>
+  </si>
+  <si>
+    <t>address_type</t>
+  </si>
+  <si>
+    <t>what3words</t>
+  </si>
+  <si>
+    <t>What3Words</t>
+  </si>
+  <si>
+    <t>client_school_information</t>
+  </si>
+  <si>
+    <t>Client / School Information</t>
+  </si>
+  <si>
+    <t>hide section</t>
+  </si>
+  <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Case Worker / Staff</t>
+  </si>
+  <si>
+    <t>Initial Referral Date</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>Phone Number - Primary</t>
+  </si>
+  <si>
+    <t>First Name - Alternate</t>
+  </si>
+  <si>
+    <t>Last Name - Alternate</t>
+  </si>
+  <si>
+    <t>current_city</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>family_member</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-  </numFmts>
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="13"/>
@@ -395,7 +388,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -410,7 +403,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
@@ -418,7 +411,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -435,11 +428,10 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -450,7 +442,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -469,60 +460,102 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="thin"/>
-      <top style="hair"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="hair"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
       </right>
-      <top style="hair"/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FFAAAAAA"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
@@ -535,230 +568,123 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -817,35 +743,346 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:IW43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="11" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="8.83"/>
+    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="1" customWidth="1"/>
+    <col min="6" max="8" width="11.5" style="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1"/>
+    <col min="11" max="257" width="8.83203125" style="1" customWidth="1"/>
+    <col min="258" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -877,7 +1114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -887,7 +1124,7 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0"/>
+      <c r="D2"/>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
@@ -905,7 +1142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -915,17 +1152,17 @@
       <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="0"/>
+      <c r="D3"/>
       <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10" t="n">
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
         <v>1</v>
       </c>
       <c r="I3" s="10"/>
@@ -933,7 +1170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -943,17 +1180,17 @@
       <c r="C4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="0"/>
+      <c r="D4"/>
       <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="16" t="n">
+      <c r="G4" s="15">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16">
         <v>1</v>
       </c>
       <c r="I4" s="16"/>
@@ -961,7 +1198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -971,17 +1208,17 @@
       <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="0"/>
+      <c r="D5"/>
       <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16" t="n">
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
         <v>1</v>
       </c>
       <c r="I5" s="16"/>
@@ -989,7 +1226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -999,17 +1236,17 @@
       <c r="C6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="0"/>
+      <c r="D6"/>
       <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16" t="n">
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
         <v>1</v>
       </c>
       <c r="I6" s="16"/>
@@ -1017,7 +1254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -1034,10 +1271,10 @@
       <c r="F7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="n">
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
         <v>1</v>
       </c>
       <c r="I7" s="16"/>
@@ -1045,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>24</v>
       </c>
@@ -1055,17 +1292,17 @@
       <c r="C8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="0"/>
+      <c r="D8"/>
       <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10" t="n">
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
         <v>0</v>
       </c>
       <c r="I8" s="10" t="s">
@@ -1075,7 +1312,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>28</v>
       </c>
@@ -1085,17 +1322,17 @@
       <c r="C9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="0"/>
+      <c r="D9"/>
       <c r="E9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="10" t="n">
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
         <v>0</v>
       </c>
       <c r="I9" s="10" t="s">
@@ -1105,7 +1342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -1115,17 +1352,17 @@
       <c r="C10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="0"/>
+      <c r="D10"/>
       <c r="E10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10" t="n">
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
         <v>0</v>
       </c>
       <c r="I10" s="10" t="s">
@@ -1135,7 +1372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1145,17 +1382,17 @@
       <c r="C11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="0"/>
+      <c r="D11"/>
       <c r="E11" s="21" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="10" t="n">
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
         <v>1</v>
       </c>
       <c r="I11" s="10"/>
@@ -1163,7 +1400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1173,17 +1410,17 @@
       <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="0"/>
+      <c r="D12"/>
       <c r="E12" s="21" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="10" t="n">
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
         <v>1</v>
       </c>
       <c r="I12" s="10"/>
@@ -1191,7 +1428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -1201,17 +1438,17 @@
       <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="D13"/>
       <c r="E13" s="21" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10" t="n">
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
         <v>1</v>
       </c>
       <c r="I13" s="10"/>
@@ -1219,7 +1456,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>39</v>
       </c>
@@ -1229,17 +1466,17 @@
       <c r="C14" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="0"/>
+      <c r="D14"/>
       <c r="E14" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="24" t="n">
+      <c r="G14" s="24">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
         <v>0</v>
       </c>
       <c r="I14" s="10" t="s">
@@ -1249,7 +1486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>41</v>
       </c>
@@ -1259,17 +1496,17 @@
       <c r="C15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="0"/>
+      <c r="D15"/>
       <c r="E15" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="24" t="n">
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
         <v>0</v>
       </c>
       <c r="I15" s="10" t="s">
@@ -1279,7 +1516,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
@@ -1289,17 +1526,17 @@
       <c r="C16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="0"/>
+      <c r="D16"/>
       <c r="E16" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24" t="n">
+      <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
         <v>1</v>
       </c>
       <c r="I16" s="24"/>
@@ -1307,7 +1544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>45</v>
       </c>
@@ -1317,17 +1554,17 @@
       <c r="C17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="0"/>
+      <c r="D17"/>
       <c r="E17" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="24" t="n">
+      <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
         <v>1</v>
       </c>
       <c r="I17" s="24"/>
@@ -1335,7 +1572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>47</v>
       </c>
@@ -1345,17 +1582,17 @@
       <c r="C18" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="0"/>
+      <c r="D18"/>
       <c r="E18" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="24" t="n">
+      <c r="G18" s="24">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24">
         <v>1</v>
       </c>
       <c r="I18" s="24"/>
@@ -1364,7 +1601,7 @@
       </c>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -1374,17 +1611,17 @@
       <c r="C19" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="0"/>
+      <c r="D19"/>
       <c r="E19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="10" t="n">
+      <c r="G19" s="27">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
         <v>0</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -1394,7 +1631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>51</v>
       </c>
@@ -1404,17 +1641,17 @@
       <c r="C20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="0"/>
+      <c r="D20"/>
       <c r="E20" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10" t="n">
+      <c r="G20" s="27">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
         <v>0</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -1424,7 +1661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>54</v>
       </c>
@@ -1434,17 +1671,17 @@
       <c r="C21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="0"/>
+      <c r="D21"/>
       <c r="E21" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="31" t="n">
+      <c r="G21" s="30">
+        <v>0</v>
+      </c>
+      <c r="H21" s="31">
         <v>0</v>
       </c>
       <c r="I21" s="10" t="s">
@@ -1454,7 +1691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
         <v>56</v>
       </c>
@@ -1464,17 +1701,17 @@
       <c r="C22" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="0"/>
+      <c r="D22"/>
       <c r="E22" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31" t="n">
+      <c r="G22" s="30">
+        <v>0</v>
+      </c>
+      <c r="H22" s="31">
         <v>0</v>
       </c>
       <c r="I22" s="10" t="s">
@@ -1484,7 +1721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
         <v>58</v>
       </c>
@@ -1494,17 +1731,17 @@
       <c r="C23" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="0"/>
+      <c r="D23"/>
       <c r="E23" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31" t="n">
+      <c r="G23" s="30">
+        <v>0</v>
+      </c>
+      <c r="H23" s="31">
         <v>0</v>
       </c>
       <c r="I23" s="10" t="s">
@@ -1514,7 +1751,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>60</v>
       </c>
@@ -1524,17 +1761,17 @@
       <c r="C24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="0"/>
+      <c r="D24"/>
       <c r="E24" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F24" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="31" t="n">
+      <c r="G24" s="30">
+        <v>0</v>
+      </c>
+      <c r="H24" s="31">
         <v>0</v>
       </c>
       <c r="I24" s="10" t="s">
@@ -1544,7 +1781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
         <v>62</v>
       </c>
@@ -1554,17 +1791,17 @@
       <c r="C25" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="0"/>
+      <c r="D25"/>
       <c r="E25" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F25" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="31" t="n">
+      <c r="G25" s="30">
+        <v>0</v>
+      </c>
+      <c r="H25" s="31">
         <v>0</v>
       </c>
       <c r="I25" s="10" t="s">
@@ -1574,7 +1811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
@@ -1584,17 +1821,17 @@
       <c r="C26" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="0"/>
+      <c r="D26"/>
       <c r="E26" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="10" t="n">
+      <c r="G26" s="27">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
         <v>0</v>
       </c>
       <c r="I26" s="10" t="s">
@@ -1604,7 +1841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
         <v>66</v>
       </c>
@@ -1614,17 +1851,17 @@
       <c r="C27" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="0"/>
+      <c r="D27"/>
       <c r="E27" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="31" t="n">
+      <c r="G27" s="30">
+        <v>0</v>
+      </c>
+      <c r="H27" s="31">
         <v>0</v>
       </c>
       <c r="I27" s="10" t="s">
@@ -1634,7 +1871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
         <v>67</v>
       </c>
@@ -1644,17 +1881,17 @@
       <c r="C28" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="0"/>
+      <c r="D28"/>
       <c r="E28" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="31" t="n">
+      <c r="G28" s="30">
+        <v>0</v>
+      </c>
+      <c r="H28" s="31">
         <v>0</v>
       </c>
       <c r="I28" s="10" t="s">
@@ -1664,7 +1901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
         <v>69</v>
       </c>
@@ -1674,17 +1911,17 @@
       <c r="C29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="0"/>
+      <c r="D29"/>
       <c r="E29" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="31" t="n">
+      <c r="G29" s="30">
+        <v>0</v>
+      </c>
+      <c r="H29" s="31">
         <v>0</v>
       </c>
       <c r="I29" s="10" t="s">
@@ -1694,7 +1931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
         <v>70</v>
       </c>
@@ -1704,17 +1941,17 @@
       <c r="C30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="0"/>
+      <c r="D30"/>
       <c r="E30" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="31" t="n">
+      <c r="G30" s="30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="31">
         <v>0</v>
       </c>
       <c r="I30" s="10" t="s">
@@ -1724,7 +1961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>71</v>
       </c>
@@ -1734,17 +1971,17 @@
       <c r="C31" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="0"/>
+      <c r="D31"/>
       <c r="E31" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="31" t="n">
+      <c r="G31" s="30">
+        <v>0</v>
+      </c>
+      <c r="H31" s="31">
         <v>0</v>
       </c>
       <c r="I31" s="10" t="s">
@@ -1754,7 +1991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
         <v>72</v>
       </c>
@@ -1764,17 +2001,17 @@
       <c r="C32" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="0"/>
+      <c r="D32"/>
       <c r="E32" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="31" t="n">
+      <c r="G32" s="30">
+        <v>0</v>
+      </c>
+      <c r="H32" s="31">
         <v>1</v>
       </c>
       <c r="I32" s="10" t="s">
@@ -1784,7 +2021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>74</v>
       </c>
@@ -1794,17 +2031,17 @@
       <c r="C33" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="0"/>
+      <c r="D33"/>
       <c r="E33" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="31" t="n">
+      <c r="G33" s="30">
+        <v>0</v>
+      </c>
+      <c r="H33" s="31">
         <v>1</v>
       </c>
       <c r="I33" s="10" t="s">
@@ -1814,7 +2051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>76</v>
       </c>
@@ -1824,17 +2061,17 @@
       <c r="C34" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="0"/>
+      <c r="D34"/>
       <c r="E34" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="31" t="n">
+      <c r="G34" s="30">
+        <v>0</v>
+      </c>
+      <c r="H34" s="31">
         <v>1</v>
       </c>
       <c r="I34" s="10" t="s">
@@ -1844,7 +2081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
         <v>78</v>
       </c>
@@ -1854,17 +2091,17 @@
       <c r="C35" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="0"/>
+      <c r="D35"/>
       <c r="E35" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="31" t="n">
+      <c r="G35" s="30">
+        <v>0</v>
+      </c>
+      <c r="H35" s="31">
         <v>1</v>
       </c>
       <c r="I35" s="10" t="s">
@@ -1874,7 +2111,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
         <v>80</v>
       </c>
@@ -1884,17 +2121,17 @@
       <c r="C36" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="0"/>
+      <c r="D36"/>
       <c r="E36" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="31" t="n">
+      <c r="G36" s="30">
+        <v>0</v>
+      </c>
+      <c r="H36" s="31">
         <v>1</v>
       </c>
       <c r="I36" s="10" t="s">
@@ -1904,7 +2141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
         <v>82</v>
       </c>
@@ -1914,17 +2151,17 @@
       <c r="C37" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="0"/>
+      <c r="D37"/>
       <c r="E37" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="31" t="n">
+      <c r="G37" s="30">
+        <v>0</v>
+      </c>
+      <c r="H37" s="31">
         <v>1</v>
       </c>
       <c r="I37" s="10" t="s">
@@ -1934,7 +2171,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
         <v>84</v>
       </c>
@@ -1944,17 +2181,17 @@
       <c r="C38" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="0"/>
+      <c r="D38"/>
       <c r="E38" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="31" t="n">
+      <c r="G38" s="30">
+        <v>0</v>
+      </c>
+      <c r="H38" s="31">
         <v>1</v>
       </c>
       <c r="I38" s="10" t="s">
@@ -1964,7 +2201,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
         <v>86</v>
       </c>
@@ -1974,17 +2211,17 @@
       <c r="C39" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="0"/>
+      <c r="D39"/>
       <c r="E39" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="31" t="n">
+      <c r="G39" s="30">
+        <v>0</v>
+      </c>
+      <c r="H39" s="31">
         <v>1</v>
       </c>
       <c r="I39" s="10" t="s">
@@ -1994,7 +2231,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
         <v>87</v>
       </c>
@@ -2004,17 +2241,17 @@
       <c r="C40" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="0"/>
+      <c r="D40"/>
       <c r="E40" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F40" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="31" t="n">
+      <c r="G40" s="30">
+        <v>0</v>
+      </c>
+      <c r="H40" s="31">
         <v>1</v>
       </c>
       <c r="I40" s="10" t="s">
@@ -2024,7 +2261,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="34" t="s">
         <v>89</v>
       </c>
@@ -2034,17 +2271,17 @@
       <c r="C41" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="0"/>
+      <c r="D41"/>
       <c r="E41" s="34" t="s">
         <v>89</v>
       </c>
       <c r="F41" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="36" t="n">
+      <c r="G41" s="35">
+        <v>0</v>
+      </c>
+      <c r="H41" s="36">
         <v>1</v>
       </c>
       <c r="I41" s="10" t="s">
@@ -2054,70 +2291,95 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42"/>
+      <c r="E42" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="35">
+        <v>0</v>
+      </c>
+      <c r="H42" s="36">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B43" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C43" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="0"/>
-      <c r="E42" s="34" t="s">
+      <c r="D43"/>
+      <c r="E43" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F43" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J42" s="38" t="s">
+      <c r="G43" s="35">
+        <v>0</v>
+      </c>
+      <c r="H43" s="36">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="38" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555555" footer="0.25"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:IW44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="26.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="11" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="8.83"/>
+    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="8" width="11.5" style="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1"/>
+    <col min="11" max="257" width="8.83203125" style="1" customWidth="1"/>
+    <col min="258" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2179,7 +2441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -2198,10 +2460,10 @@
       <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10" t="n">
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
         <v>1</v>
       </c>
       <c r="I3" s="10"/>
@@ -2209,7 +2471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -2228,10 +2490,10 @@
       <c r="F4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="16" t="n">
+      <c r="G4" s="15">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16">
         <v>1</v>
       </c>
       <c r="I4" s="16"/>
@@ -2239,7 +2501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -2258,10 +2520,10 @@
       <c r="F5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16" t="n">
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
         <v>1</v>
       </c>
       <c r="I5" s="16"/>
@@ -2269,7 +2531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -2288,10 +2550,10 @@
       <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16" t="n">
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
         <v>1</v>
       </c>
       <c r="I6" s="16"/>
@@ -2299,7 +2561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -2318,10 +2580,10 @@
       <c r="F7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="n">
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
         <v>1</v>
       </c>
       <c r="I7" s="16"/>
@@ -2329,7 +2591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>24</v>
       </c>
@@ -2348,10 +2610,10 @@
       <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10" t="n">
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
         <v>1</v>
       </c>
       <c r="I8" s="10" t="s">
@@ -2361,7 +2623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>28</v>
       </c>
@@ -2380,10 +2642,10 @@
       <c r="F9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="10" t="n">
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
         <v>1</v>
       </c>
       <c r="I9" s="10" t="s">
@@ -2393,7 +2655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -2403,17 +2665,17 @@
       <c r="C10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="0"/>
+      <c r="D10"/>
       <c r="E10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10" t="n">
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
         <v>1</v>
       </c>
       <c r="I10" s="10" t="s">
@@ -2423,7 +2685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -2442,10 +2704,10 @@
       <c r="F11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="10" t="n">
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
         <v>1</v>
       </c>
       <c r="I11" s="10"/>
@@ -2453,7 +2715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -2463,17 +2725,17 @@
       <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="0"/>
+      <c r="D12"/>
       <c r="E12" s="21" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="10" t="n">
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
         <v>0</v>
       </c>
       <c r="I12" s="10"/>
@@ -2481,7 +2743,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2491,17 +2753,17 @@
       <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="D13"/>
       <c r="E13" s="21" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10" t="n">
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
         <v>0</v>
       </c>
       <c r="I13" s="10"/>
@@ -2509,7 +2771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>39</v>
       </c>
@@ -2528,10 +2790,10 @@
       <c r="F14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="24" t="n">
+      <c r="G14" s="24">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
         <v>1</v>
       </c>
       <c r="I14" s="10" t="s">
@@ -2541,7 +2803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>41</v>
       </c>
@@ -2560,10 +2822,10 @@
       <c r="F15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="24" t="n">
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
         <v>1</v>
       </c>
       <c r="I15" s="10" t="s">
@@ -2573,7 +2835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
@@ -2592,10 +2854,10 @@
       <c r="F16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24" t="n">
+      <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
         <v>1</v>
       </c>
       <c r="I16" s="24"/>
@@ -2603,7 +2865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>45</v>
       </c>
@@ -2622,10 +2884,10 @@
       <c r="F17" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="24" t="n">
+      <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
         <v>1</v>
       </c>
       <c r="I17" s="24"/>
@@ -2633,7 +2895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>47</v>
       </c>
@@ -2643,17 +2905,17 @@
       <c r="C18" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="0"/>
+      <c r="D18"/>
       <c r="E18" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="24" t="n">
+      <c r="G18" s="24">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24">
         <v>0</v>
       </c>
       <c r="I18" s="24"/>
@@ -2661,7 +2923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2680,10 +2942,10 @@
       <c r="F19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="10" t="n">
+      <c r="G19" s="27">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
         <v>1</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -2693,7 +2955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>51</v>
       </c>
@@ -2712,10 +2974,10 @@
       <c r="F20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10" t="n">
+      <c r="G20" s="27">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
         <v>1</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -2725,7 +2987,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>54</v>
       </c>
@@ -2744,10 +3006,10 @@
       <c r="F21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="31" t="n">
+      <c r="G21" s="30">
+        <v>0</v>
+      </c>
+      <c r="H21" s="31">
         <v>1</v>
       </c>
       <c r="I21" s="10" t="s">
@@ -2757,7 +3019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
         <v>56</v>
       </c>
@@ -2776,10 +3038,10 @@
       <c r="F22" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31" t="n">
+      <c r="G22" s="30">
+        <v>0</v>
+      </c>
+      <c r="H22" s="31">
         <v>1</v>
       </c>
       <c r="I22" s="10" t="s">
@@ -2789,7 +3051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
         <v>103</v>
       </c>
@@ -2808,10 +3070,10 @@
       <c r="F23" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31" t="n">
+      <c r="G23" s="30">
+        <v>0</v>
+      </c>
+      <c r="H23" s="31">
         <v>1</v>
       </c>
       <c r="I23" s="10" t="s">
@@ -2821,7 +3083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>58</v>
       </c>
@@ -2840,10 +3102,10 @@
       <c r="F24" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="31" t="n">
+      <c r="G24" s="30">
+        <v>0</v>
+      </c>
+      <c r="H24" s="31">
         <v>1</v>
       </c>
       <c r="I24" s="10" t="s">
@@ -2853,7 +3115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
         <v>60</v>
       </c>
@@ -2872,10 +3134,10 @@
       <c r="F25" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="31" t="n">
+      <c r="G25" s="30">
+        <v>0</v>
+      </c>
+      <c r="H25" s="31">
         <v>1</v>
       </c>
       <c r="I25" s="10" t="s">
@@ -2885,7 +3147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
         <v>62</v>
       </c>
@@ -2904,10 +3166,10 @@
       <c r="F26" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="31" t="n">
+      <c r="G26" s="30">
+        <v>0</v>
+      </c>
+      <c r="H26" s="31">
         <v>1</v>
       </c>
       <c r="I26" s="10" t="s">
@@ -2917,7 +3179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
         <v>64</v>
       </c>
@@ -2936,10 +3198,10 @@
       <c r="F27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="10" t="n">
+      <c r="G27" s="27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
         <v>1</v>
       </c>
       <c r="I27" s="10" t="s">
@@ -2949,7 +3211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
         <v>66</v>
       </c>
@@ -2968,10 +3230,10 @@
       <c r="F28" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="31" t="n">
+      <c r="G28" s="30">
+        <v>0</v>
+      </c>
+      <c r="H28" s="31">
         <v>1</v>
       </c>
       <c r="I28" s="10" t="s">
@@ -2981,7 +3243,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
         <v>67</v>
       </c>
@@ -3000,10 +3262,10 @@
       <c r="F29" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="31" t="n">
+      <c r="G29" s="30">
+        <v>0</v>
+      </c>
+      <c r="H29" s="31">
         <v>1</v>
       </c>
       <c r="I29" s="10" t="s">
@@ -3013,7 +3275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
         <v>69</v>
       </c>
@@ -3032,10 +3294,10 @@
       <c r="F30" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="31" t="n">
+      <c r="G30" s="30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="31">
         <v>1</v>
       </c>
       <c r="I30" s="10" t="s">
@@ -3045,7 +3307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>70</v>
       </c>
@@ -3064,10 +3326,10 @@
       <c r="F31" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="31" t="n">
+      <c r="G31" s="30">
+        <v>0</v>
+      </c>
+      <c r="H31" s="31">
         <v>1</v>
       </c>
       <c r="I31" s="10" t="s">
@@ -3077,7 +3339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
         <v>71</v>
       </c>
@@ -3096,10 +3358,10 @@
       <c r="F32" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="31" t="n">
+      <c r="G32" s="30">
+        <v>0</v>
+      </c>
+      <c r="H32" s="31">
         <v>1</v>
       </c>
       <c r="I32" s="10" t="s">
@@ -3109,7 +3371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>72</v>
       </c>
@@ -3126,10 +3388,10 @@
       <c r="F33" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="31" t="n">
+      <c r="G33" s="30">
+        <v>0</v>
+      </c>
+      <c r="H33" s="31">
         <v>0</v>
       </c>
       <c r="I33" s="10" t="s">
@@ -3139,7 +3401,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>74</v>
       </c>
@@ -3156,10 +3418,10 @@
       <c r="F34" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="31" t="n">
+      <c r="G34" s="30">
+        <v>0</v>
+      </c>
+      <c r="H34" s="31">
         <v>0</v>
       </c>
       <c r="I34" s="10" t="s">
@@ -3169,7 +3431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
         <v>76</v>
       </c>
@@ -3186,10 +3448,10 @@
       <c r="F35" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="31" t="n">
+      <c r="G35" s="30">
+        <v>0</v>
+      </c>
+      <c r="H35" s="31">
         <v>0</v>
       </c>
       <c r="I35" s="10" t="s">
@@ -3199,7 +3461,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
         <v>78</v>
       </c>
@@ -3216,10 +3478,10 @@
       <c r="F36" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="31" t="n">
+      <c r="G36" s="30">
+        <v>0</v>
+      </c>
+      <c r="H36" s="31">
         <v>0</v>
       </c>
       <c r="I36" s="10" t="s">
@@ -3229,7 +3491,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
         <v>80</v>
       </c>
@@ -3246,10 +3508,10 @@
       <c r="F37" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="31" t="n">
+      <c r="G37" s="30">
+        <v>0</v>
+      </c>
+      <c r="H37" s="31">
         <v>0</v>
       </c>
       <c r="I37" s="10" t="s">
@@ -3259,7 +3521,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
         <v>82</v>
       </c>
@@ -3276,10 +3538,10 @@
       <c r="F38" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="31" t="n">
+      <c r="G38" s="30">
+        <v>0</v>
+      </c>
+      <c r="H38" s="31">
         <v>0</v>
       </c>
       <c r="I38" s="10" t="s">
@@ -3289,7 +3551,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
         <v>84</v>
       </c>
@@ -3306,10 +3568,10 @@
       <c r="F39" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="31" t="n">
+      <c r="G39" s="30">
+        <v>0</v>
+      </c>
+      <c r="H39" s="31">
         <v>0</v>
       </c>
       <c r="I39" s="10" t="s">
@@ -3319,7 +3581,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
         <v>86</v>
       </c>
@@ -3336,10 +3598,10 @@
       <c r="F40" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="31" t="n">
+      <c r="G40" s="30">
+        <v>0</v>
+      </c>
+      <c r="H40" s="31">
         <v>0</v>
       </c>
       <c r="I40" s="10" t="s">
@@ -3349,7 +3611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
         <v>87</v>
       </c>
@@ -3366,10 +3628,10 @@
       <c r="F41" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="31" t="n">
+      <c r="G41" s="30">
+        <v>0</v>
+      </c>
+      <c r="H41" s="31">
         <v>0</v>
       </c>
       <c r="I41" s="10" t="s">
@@ -3379,7 +3641,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="34" t="s">
         <v>89</v>
       </c>
@@ -3396,10 +3658,10 @@
       <c r="F42" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="36" t="n">
+      <c r="G42" s="35">
+        <v>0</v>
+      </c>
+      <c r="H42" s="36">
         <v>0</v>
       </c>
       <c r="I42" s="10" t="s">
@@ -3409,43 +3671,72 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43"/>
+      <c r="E43" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="35">
+        <v>0</v>
+      </c>
+      <c r="H43" s="36">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B44" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C44" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D44" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E44" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F44" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="38" t="s">
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="38" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;Cbrc</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
hide/show family member occupation
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AC7F25-8CA9-9646-BEE5-BCB768FD7E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC259F51-B884-3B40-BF74-752C00AD99A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="110">
   <si>
     <t>name</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>Occupation</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1070,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW43"/>
+  <dimension ref="A1:IW44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2323,31 +2329,59 @@
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="34" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D43"/>
       <c r="E43" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="35">
+        <v>0</v>
+      </c>
+      <c r="H43" s="36">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10"/>
+      <c r="J43" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="B44" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44"/>
+      <c r="E44" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="35">
-        <v>0</v>
-      </c>
-      <c r="H43" s="36">
-        <v>1</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="38" t="s">
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="38" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2362,10 +2396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IW44"/>
+  <dimension ref="A1:IW45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3703,33 +3737,61 @@
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44"/>
+      <c r="E44" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10"/>
+      <c r="J44" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B45" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C45" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D45" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E45" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F45" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="35">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36">
-        <v>0</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="38" t="s">
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" s="38" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hide/show family member relation and guardian fields
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC259F51-B884-3B40-BF74-752C00AD99A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF4ACA5-69BB-5B4C-ADBF-BF32FD852DDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="114">
   <si>
     <t>name</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>Occupation</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>Guardian</t>
   </si>
 </sst>
 </file>
@@ -628,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -685,6 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1070,10 +1083,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW44"/>
+  <dimension ref="A1:IW46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2329,13 +2342,13 @@
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="34" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B43" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="34" t="s">
-        <v>109</v>
+      <c r="C43" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="D43"/>
       <c r="E43" s="34" t="s">
@@ -2357,31 +2370,87 @@
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="D44"/>
       <c r="E44" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10"/>
+      <c r="J44" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36">
+        <v>1</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="B46" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46"/>
+      <c r="E46" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="35">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36">
-        <v>1</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="38" t="s">
+      <c r="G46" s="35">
+        <v>0</v>
+      </c>
+      <c r="H46" s="36">
+        <v>1</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" s="38" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2396,10 +2465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IW45"/>
+  <dimension ref="A1:IW47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3737,13 +3806,13 @@
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B44" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D44"/>
       <c r="E44" s="34" t="s">
@@ -3765,33 +3834,89 @@
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46"/>
+      <c r="E46" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="35">
+        <v>0</v>
+      </c>
+      <c r="H46" s="36">
+        <v>0</v>
+      </c>
+      <c r="I46" s="10"/>
+      <c r="J46" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B47" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C47" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D47" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E47" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="34" t="s">
+      <c r="F47" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="35">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36">
-        <v>0</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="38" t="s">
+      <c r="G47" s="35">
+        <v>0</v>
+      </c>
+      <c r="H47" s="36">
+        <v>0</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" s="38" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added family member note
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E687C435-B6C9-F54B-A958-F270869C0D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E935B208-54E6-334B-B24D-806B782F77F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="120">
   <si>
     <t>name</t>
   </si>
@@ -377,13 +377,22 @@
   </si>
   <si>
     <t>Whatsapp? (Phone Number - Alternate)</t>
+  </si>
+  <si>
+    <t>caregiver_information</t>
+  </si>
+  <si>
+    <t>Caregiver Information</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -470,6 +479,25 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -649,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -707,6 +735,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1092,10 +1124,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW47"/>
+  <dimension ref="A1:IW49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2349,19 +2381,19 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D43"/>
-      <c r="E43" s="34" t="s">
-        <v>105</v>
+        <v>93</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="42"/>
+      <c r="E43" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="F43" s="34" t="s">
         <v>13</v>
@@ -2372,22 +2404,20 @@
       <c r="H43" s="36">
         <v>0</v>
       </c>
-      <c r="I43" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="I43" s="10"/>
       <c r="J43" s="37" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B44" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="40" t="s">
-        <v>111</v>
+      <c r="C44" s="34" t="s">
+        <v>106</v>
       </c>
       <c r="D44"/>
       <c r="E44" s="34" t="s">
@@ -2400,22 +2430,24 @@
         <v>0</v>
       </c>
       <c r="H44" s="36">
-        <v>1</v>
-      </c>
-      <c r="I44" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J44" s="37" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B45" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="34" t="s">
-        <v>113</v>
+      <c r="C45" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="D45"/>
       <c r="E45" s="34" t="s">
@@ -2437,13 +2469,13 @@
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="34" t="s">
@@ -2463,33 +2495,91 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D47"/>
       <c r="E47" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="35">
+        <v>0</v>
+      </c>
+      <c r="H47" s="36">
+        <v>1</v>
+      </c>
+      <c r="I47" s="10"/>
+      <c r="J47" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48"/>
+      <c r="E48" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="35">
+        <v>0</v>
+      </c>
+      <c r="H48" s="36">
+        <v>0</v>
+      </c>
+      <c r="I48" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J48" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A49" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="34" t="s">
+      <c r="B49" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49"/>
+      <c r="E49" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="35">
-        <v>0</v>
-      </c>
-      <c r="H47" s="36">
-        <v>1</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J47" s="38" t="s">
+      <c r="G49" s="35">
+        <v>0</v>
+      </c>
+      <c r="H49" s="36">
+        <v>1</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J49" s="38" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2504,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IW48"/>
+  <dimension ref="A1:IW50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="A15:J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3845,19 +3935,21 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="34" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44"/>
-      <c r="E44" s="34" t="s">
-        <v>105</v>
+        <v>93</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="F44" s="34" t="s">
         <v>13</v>
@@ -3868,22 +3960,20 @@
       <c r="H44" s="36">
         <v>1</v>
       </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="I44" s="10"/>
       <c r="J44" s="37" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B45" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D45"/>
       <c r="E45" s="34" t="s">
@@ -3896,22 +3986,24 @@
         <v>0</v>
       </c>
       <c r="H45" s="36">
-        <v>0</v>
-      </c>
-      <c r="I45" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J45" s="37" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="34" t="s">
@@ -3933,13 +4025,13 @@
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B47" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D47"/>
       <c r="E47" s="34" t="s">
@@ -3961,33 +4053,93 @@
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48"/>
+      <c r="E48" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="35">
+        <v>0</v>
+      </c>
+      <c r="H48" s="36">
+        <v>0</v>
+      </c>
+      <c r="I48" s="10"/>
+      <c r="J48" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="35">
+        <v>0</v>
+      </c>
+      <c r="H49" s="36">
+        <v>1</v>
+      </c>
+      <c r="I49" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J49" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B50" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C50" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D50" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E50" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F48" s="34" t="s">
+      <c r="F50" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G48" s="35">
-        <v>0</v>
-      </c>
-      <c r="H48" s="36">
-        <v>0</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J48" s="38" t="s">
+      <c r="G50" s="35">
+        <v>0</v>
+      </c>
+      <c r="H50" s="36">
+        <v>0</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" s="38" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated select options + add preferred language
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E935B208-54E6-334B-B24D-806B782F77F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F738D18-BA67-CA4A-8E18-670A8C687C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>preferred_language</t>
+  </si>
+  <si>
+    <t>Preferred Language</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1130,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW49"/>
+  <dimension ref="A1:IW50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1344,15 +1350,15 @@
     </row>
     <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8"/>
+      <c r="C8" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="42"/>
       <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
@@ -1374,13 +1380,13 @@
     </row>
     <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="11" t="s">
@@ -1404,13 +1410,13 @@
     </row>
     <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="11" t="s">
@@ -1432,43 +1438,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>33</v>
+    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="D11"/>
-      <c r="E11" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="21" t="s">
+      <c r="E11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="10">
         <v>0</v>
       </c>
       <c r="H11" s="10">
-        <v>1</v>
-      </c>
-      <c r="I11" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J11" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12"/>
       <c r="E12" s="21" t="s">
@@ -1485,18 +1493,18 @@
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="11" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="21" t="s">
@@ -1516,47 +1524,45 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>40</v>
+    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="D14"/>
-      <c r="E14" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="24">
-        <v>0</v>
-      </c>
-      <c r="H14" s="24">
-        <v>0</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>27</v>
+      <c r="E14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="D15"/>
       <c r="E15" s="23" t="s">
         <v>11</v>
       </c>
@@ -1578,15 +1584,15 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16"/>
+        <v>116</v>
+      </c>
+      <c r="D16" s="19"/>
       <c r="E16" s="23" t="s">
         <v>11</v>
       </c>
@@ -1607,14 +1613,14 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>43</v>
+      <c r="A17" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
+      <c r="C17" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="23" t="s">
@@ -1627,22 +1633,24 @@
         <v>0</v>
       </c>
       <c r="H17" s="24">
-        <v>1</v>
-      </c>
-      <c r="I17" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J17" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18"/>
       <c r="E18" s="23" t="s">
@@ -1661,17 +1669,16 @@
       <c r="J18" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>48</v>
+      <c r="C19" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D19"/>
       <c r="E19" s="23" t="s">
@@ -1688,52 +1695,51 @@
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0</v>
+      </c>
+      <c r="H20" s="24">
+        <v>1</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="27">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
-        <v>0</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="D21"/>
       <c r="E21" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>13</v>
@@ -1751,45 +1757,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="28" t="s">
+    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D22"/>
       <c r="E22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="30">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31">
+      <c r="F22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="27">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
         <v>0</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="32" t="s">
-        <v>57</v>
+      <c r="C23" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="D23"/>
       <c r="E23" s="6" t="s">
@@ -1813,13 +1819,13 @@
     </row>
     <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>59</v>
+      <c r="C24" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="D24"/>
       <c r="E24" s="6" t="s">
@@ -1843,13 +1849,13 @@
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25"/>
       <c r="E25" s="6" t="s">
@@ -1873,13 +1879,13 @@
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="33" t="s">
-        <v>63</v>
+      <c r="C26" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="D26"/>
       <c r="E26" s="6" t="s">
@@ -1901,75 +1907,75 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>52</v>
+    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="D27"/>
       <c r="E27" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="27">
-        <v>0</v>
-      </c>
-      <c r="H27" s="10">
+        <v>53</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="30">
+        <v>0</v>
+      </c>
+      <c r="H27" s="31">
         <v>0</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="28" t="s">
+    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D28"/>
       <c r="E28" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="30">
-        <v>0</v>
-      </c>
-      <c r="H28" s="31">
+      <c r="F28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="27">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
         <v>0</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D29"/>
       <c r="E29" s="6" t="s">
@@ -1993,13 +1999,13 @@
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D30"/>
       <c r="E30" s="6" t="s">
@@ -2023,13 +2029,13 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D31"/>
       <c r="E31" s="6" t="s">
@@ -2053,13 +2059,13 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32"/>
       <c r="E32" s="6" t="s">
@@ -2083,17 +2089,17 @@
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="33" t="s">
-        <v>73</v>
+      <c r="C33" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="D33"/>
-      <c r="E33" s="29" t="s">
-        <v>11</v>
+      <c r="E33" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>13</v>
@@ -2102,24 +2108,24 @@
         <v>0</v>
       </c>
       <c r="H33" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D34"/>
       <c r="E34" s="29" t="s">
@@ -2143,13 +2149,13 @@
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D35"/>
       <c r="E35" s="29" t="s">
@@ -2173,13 +2179,13 @@
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D36"/>
       <c r="E36" s="29" t="s">
@@ -2203,13 +2209,13 @@
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D37"/>
       <c r="E37" s="29" t="s">
@@ -2233,13 +2239,13 @@
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D38"/>
       <c r="E38" s="29" t="s">
@@ -2263,13 +2269,13 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D39"/>
       <c r="E39" s="29" t="s">
@@ -2293,13 +2299,13 @@
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="D40"/>
       <c r="E40" s="29" t="s">
@@ -2323,13 +2329,13 @@
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D41"/>
       <c r="E41" s="29" t="s">
@@ -2351,103 +2357,103 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="34" t="s">
+    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42"/>
+      <c r="E42" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="30">
+        <v>0</v>
+      </c>
+      <c r="H42" s="31">
+        <v>1</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="34" t="s">
+      <c r="B43" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D42"/>
-      <c r="E42" s="34" t="s">
+      <c r="D43"/>
+      <c r="E43" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F43" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="35">
-        <v>0</v>
-      </c>
-      <c r="H42" s="36">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J42" s="37" t="s">
+      <c r="G43" s="35">
+        <v>0</v>
+      </c>
+      <c r="H43" s="36">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="34" t="s">
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B44" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C44" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43" t="s">
+      <c r="D44" s="42"/>
+      <c r="E44" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="35">
-        <v>0</v>
-      </c>
-      <c r="H43" s="36">
-        <v>0</v>
-      </c>
-      <c r="I43" s="10"/>
-      <c r="J43" s="37" t="s">
+      <c r="F44" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10"/>
+      <c r="J44" s="37" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44"/>
-      <c r="E44" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="35">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36">
-        <v>0</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B45" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="40" t="s">
-        <v>111</v>
+      <c r="C45" s="34" t="s">
+        <v>106</v>
       </c>
       <c r="D45"/>
       <c r="E45" s="34" t="s">
@@ -2460,22 +2466,24 @@
         <v>0</v>
       </c>
       <c r="H45" s="36">
-        <v>1</v>
-      </c>
-      <c r="I45" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J45" s="37" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="34" t="s">
-        <v>113</v>
+      <c r="C46" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="34" t="s">
@@ -2497,13 +2505,13 @@
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B47" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D47"/>
       <c r="E47" s="34" t="s">
@@ -2524,14 +2532,14 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="43" t="s">
-        <v>119</v>
+      <c r="A48" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="B48" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="42" t="s">
-        <v>23</v>
+      <c r="C48" s="34" t="s">
+        <v>109</v>
       </c>
       <c r="D48"/>
       <c r="E48" s="34" t="s">
@@ -2544,42 +2552,70 @@
         <v>0</v>
       </c>
       <c r="H48" s="36">
-        <v>0</v>
-      </c>
-      <c r="I48" s="44" t="s">
-        <v>26</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I48" s="10"/>
       <c r="J48" s="37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" s="34" t="s">
-        <v>92</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="43" t="s">
+        <v>119</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="34" t="s">
-        <v>94</v>
+        <v>105</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>23</v>
       </c>
       <c r="D49"/>
       <c r="E49" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="35">
+        <v>0</v>
+      </c>
+      <c r="H49" s="36">
+        <v>0</v>
+      </c>
+      <c r="I49" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J49" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A50" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F49" s="34" t="s">
+      <c r="B50" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50"/>
+      <c r="E50" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="35">
-        <v>0</v>
-      </c>
-      <c r="H49" s="36">
-        <v>1</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J49" s="38" t="s">
+      <c r="G50" s="35">
+        <v>0</v>
+      </c>
+      <c r="H50" s="36">
+        <v>1</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" s="38" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2594,10 +2630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IW50"/>
+  <dimension ref="A1:IW51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2825,16 +2861,16 @@
     </row>
     <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>25</v>
+      <c r="C8" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>121</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>11</v>
@@ -2857,16 +2893,16 @@
     </row>
     <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>11</v>
@@ -2889,15 +2925,17 @@
     </row>
     <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10"/>
+        <v>29</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="E10" s="11" t="s">
         <v>11</v>
       </c>
@@ -2917,23 +2955,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="21" t="s">
+    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="10">
@@ -2942,22 +2978,26 @@
       <c r="H11" s="10">
         <v>1</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J11" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12"/>
+        <v>33</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="E12" s="21" t="s">
         <v>11</v>
       </c>
@@ -2968,22 +3008,22 @@
         <v>0</v>
       </c>
       <c r="H12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="11" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="21" t="s">
@@ -3003,50 +3043,46 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="24">
-        <v>0</v>
-      </c>
-      <c r="H14" s="24">
-        <v>1</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>27</v>
+    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>11</v>
@@ -3069,16 +3105,16 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>11</v>
@@ -3100,17 +3136,17 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>43</v>
+      <c r="A17" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
+      <c r="C17" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>11</v>
@@ -3124,23 +3160,25 @@
       <c r="H17" s="24">
         <v>1</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J17" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>11</v>
@@ -3161,15 +3199,17 @@
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19"/>
+      <c r="C19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="E19" s="23" t="s">
         <v>11</v>
       </c>
@@ -3180,60 +3220,56 @@
         <v>0</v>
       </c>
       <c r="H19" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0</v>
+      </c>
+      <c r="H20" s="24">
+        <v>0</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="27">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
-        <v>1</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>13</v>
@@ -3251,50 +3287,50 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="28" t="s">
+    <row r="22" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="30">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31">
+      <c r="F22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="27">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
         <v>1</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>57</v>
+      <c r="C23" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>53</v>
@@ -3317,16 +3353,16 @@
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>104</v>
+      <c r="C24" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>53</v>
@@ -3349,16 +3385,16 @@
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>53</v>
@@ -3381,16 +3417,16 @@
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>53</v>
@@ -3413,16 +3449,16 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>63</v>
+      <c r="C27" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>53</v>
@@ -3443,82 +3479,82 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="30">
+        <v>0</v>
+      </c>
+      <c r="H28" s="31">
+        <v>1</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="19" t="s">
+      <c r="B29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="27">
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
-        <v>1</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="30">
-        <v>0</v>
-      </c>
-      <c r="H29" s="31">
+      <c r="F29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="27">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
         <v>1</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="31" t="s">
+      <c r="J29" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>65</v>
@@ -3541,16 +3577,16 @@
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>65</v>
@@ -3573,16 +3609,16 @@
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>65</v>
@@ -3605,16 +3641,16 @@
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>65</v>
@@ -3637,17 +3673,19 @@
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="29" t="s">
-        <v>11</v>
+      <c r="C34" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>13</v>
@@ -3656,24 +3694,24 @@
         <v>0</v>
       </c>
       <c r="H34" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J34" s="31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="29" t="s">
@@ -3697,13 +3735,13 @@
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="29" t="s">
@@ -3727,13 +3765,13 @@
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="29" t="s">
@@ -3757,13 +3795,13 @@
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="29" t="s">
@@ -3787,13 +3825,13 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="29" t="s">
@@ -3817,13 +3855,13 @@
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="29" t="s">
@@ -3847,13 +3885,13 @@
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="29" t="s">
@@ -3877,13 +3915,13 @@
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="29" t="s">
@@ -3905,105 +3943,105 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="34" t="s">
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="30">
+        <v>0</v>
+      </c>
+      <c r="H43" s="31">
+        <v>0</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="34" t="s">
+      <c r="B44" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34" t="s">
+      <c r="D44" s="34"/>
+      <c r="E44" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F44" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="35">
-        <v>0</v>
-      </c>
-      <c r="H43" s="36">
-        <v>0</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="37" t="s">
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B45" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C45" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D45" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="43" t="s">
+      <c r="E45" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="F44" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="35">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36">
-        <v>1</v>
-      </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="37" t="s">
+      <c r="F45" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36">
+        <v>1</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="37" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D45"/>
-      <c r="E45" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="35">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36">
-        <v>1</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="34" t="s">
@@ -4016,22 +4054,24 @@
         <v>0</v>
       </c>
       <c r="H46" s="36">
-        <v>0</v>
-      </c>
-      <c r="I46" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J46" s="37" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B47" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D47"/>
       <c r="E47" s="34" t="s">
@@ -4053,13 +4093,13 @@
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B48" s="34" t="s">
         <v>105</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D48"/>
       <c r="E48" s="34" t="s">
@@ -4079,19 +4119,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="43" t="s">
-        <v>119</v>
+    <row r="49" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="B49" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>23</v>
-      </c>
+      <c r="C49" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49"/>
       <c r="E49" s="34" t="s">
         <v>105</v>
       </c>
@@ -4102,46 +4140,570 @@
         <v>0</v>
       </c>
       <c r="H49" s="36">
-        <v>1</v>
-      </c>
-      <c r="I49" s="44" t="s">
-        <v>26</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I49" s="10"/>
       <c r="J49" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="35">
+        <v>0</v>
+      </c>
+      <c r="H50" s="36">
+        <v>1</v>
+      </c>
+      <c r="I50" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" s="37" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="34" t="s">
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50"/>
+      <c r="Y50"/>
+      <c r="Z50"/>
+      <c r="AA50"/>
+      <c r="AB50"/>
+      <c r="AC50"/>
+      <c r="AD50"/>
+      <c r="AE50"/>
+      <c r="AF50"/>
+      <c r="AG50"/>
+      <c r="AH50"/>
+      <c r="AI50"/>
+      <c r="AJ50"/>
+      <c r="AK50"/>
+      <c r="AL50"/>
+      <c r="AM50"/>
+      <c r="AN50"/>
+      <c r="AO50"/>
+      <c r="AP50"/>
+      <c r="AQ50"/>
+      <c r="AR50"/>
+      <c r="AS50"/>
+      <c r="AT50"/>
+      <c r="AU50"/>
+      <c r="AV50"/>
+      <c r="AW50"/>
+      <c r="AX50"/>
+      <c r="AY50"/>
+      <c r="AZ50"/>
+      <c r="BA50"/>
+      <c r="BB50"/>
+      <c r="BC50"/>
+      <c r="BD50"/>
+      <c r="BE50"/>
+      <c r="BF50"/>
+      <c r="BG50"/>
+      <c r="BH50"/>
+      <c r="BI50"/>
+      <c r="BJ50"/>
+      <c r="BK50"/>
+      <c r="BL50"/>
+      <c r="BM50"/>
+      <c r="BN50"/>
+      <c r="BO50"/>
+      <c r="BP50"/>
+      <c r="BQ50"/>
+      <c r="BR50"/>
+      <c r="BS50"/>
+      <c r="BT50"/>
+      <c r="BU50"/>
+      <c r="BV50"/>
+      <c r="BW50"/>
+      <c r="BX50"/>
+      <c r="BY50"/>
+      <c r="BZ50"/>
+      <c r="CA50"/>
+      <c r="CB50"/>
+      <c r="CC50"/>
+      <c r="CD50"/>
+      <c r="CE50"/>
+      <c r="CF50"/>
+      <c r="CG50"/>
+      <c r="CH50"/>
+      <c r="CI50"/>
+      <c r="CJ50"/>
+      <c r="CK50"/>
+      <c r="CL50"/>
+      <c r="CM50"/>
+      <c r="CN50"/>
+      <c r="CO50"/>
+      <c r="CP50"/>
+      <c r="CQ50"/>
+      <c r="CR50"/>
+      <c r="CS50"/>
+      <c r="CT50"/>
+      <c r="CU50"/>
+      <c r="CV50"/>
+      <c r="CW50"/>
+      <c r="CX50"/>
+      <c r="CY50"/>
+      <c r="CZ50"/>
+      <c r="DA50"/>
+      <c r="DB50"/>
+      <c r="DC50"/>
+      <c r="DD50"/>
+      <c r="DE50"/>
+      <c r="DF50"/>
+      <c r="DG50"/>
+      <c r="DH50"/>
+      <c r="DI50"/>
+      <c r="DJ50"/>
+      <c r="DK50"/>
+      <c r="DL50"/>
+      <c r="DM50"/>
+      <c r="DN50"/>
+      <c r="DO50"/>
+      <c r="DP50"/>
+      <c r="DQ50"/>
+      <c r="DR50"/>
+      <c r="DS50"/>
+      <c r="DT50"/>
+      <c r="DU50"/>
+      <c r="DV50"/>
+      <c r="DW50"/>
+      <c r="DX50"/>
+      <c r="DY50"/>
+      <c r="DZ50"/>
+      <c r="EA50"/>
+      <c r="EB50"/>
+      <c r="EC50"/>
+      <c r="ED50"/>
+      <c r="EE50"/>
+      <c r="EF50"/>
+      <c r="EG50"/>
+      <c r="EH50"/>
+      <c r="EI50"/>
+      <c r="EJ50"/>
+      <c r="EK50"/>
+      <c r="EL50"/>
+      <c r="EM50"/>
+      <c r="EN50"/>
+      <c r="EO50"/>
+      <c r="EP50"/>
+      <c r="EQ50"/>
+      <c r="ER50"/>
+      <c r="ES50"/>
+      <c r="ET50"/>
+      <c r="EU50"/>
+      <c r="EV50"/>
+      <c r="EW50"/>
+      <c r="EX50"/>
+      <c r="EY50"/>
+      <c r="EZ50"/>
+      <c r="FA50"/>
+      <c r="FB50"/>
+      <c r="FC50"/>
+      <c r="FD50"/>
+      <c r="FE50"/>
+      <c r="FF50"/>
+      <c r="FG50"/>
+      <c r="FH50"/>
+      <c r="FI50"/>
+      <c r="FJ50"/>
+      <c r="FK50"/>
+      <c r="FL50"/>
+      <c r="FM50"/>
+      <c r="FN50"/>
+      <c r="FO50"/>
+      <c r="FP50"/>
+      <c r="FQ50"/>
+      <c r="FR50"/>
+      <c r="FS50"/>
+      <c r="FT50"/>
+      <c r="FU50"/>
+      <c r="FV50"/>
+      <c r="FW50"/>
+      <c r="FX50"/>
+      <c r="FY50"/>
+      <c r="FZ50"/>
+      <c r="GA50"/>
+      <c r="GB50"/>
+      <c r="GC50"/>
+      <c r="GD50"/>
+      <c r="GE50"/>
+      <c r="GF50"/>
+      <c r="GG50"/>
+      <c r="GH50"/>
+      <c r="GI50"/>
+      <c r="GJ50"/>
+      <c r="GK50"/>
+      <c r="GL50"/>
+      <c r="GM50"/>
+      <c r="GN50"/>
+      <c r="GO50"/>
+      <c r="GP50"/>
+      <c r="GQ50"/>
+      <c r="GR50"/>
+      <c r="GS50"/>
+      <c r="GT50"/>
+      <c r="GU50"/>
+      <c r="GV50"/>
+      <c r="GW50"/>
+      <c r="GX50"/>
+      <c r="GY50"/>
+      <c r="GZ50"/>
+      <c r="HA50"/>
+      <c r="HB50"/>
+      <c r="HC50"/>
+      <c r="HD50"/>
+      <c r="HE50"/>
+      <c r="HF50"/>
+      <c r="HG50"/>
+      <c r="HH50"/>
+      <c r="HI50"/>
+      <c r="HJ50"/>
+      <c r="HK50"/>
+      <c r="HL50"/>
+      <c r="HM50"/>
+      <c r="HN50"/>
+      <c r="HO50"/>
+      <c r="HP50"/>
+      <c r="HQ50"/>
+      <c r="HR50"/>
+      <c r="HS50"/>
+      <c r="HT50"/>
+      <c r="HU50"/>
+      <c r="HV50"/>
+      <c r="HW50"/>
+      <c r="HX50"/>
+      <c r="HY50"/>
+      <c r="HZ50"/>
+      <c r="IA50"/>
+      <c r="IB50"/>
+      <c r="IC50"/>
+      <c r="ID50"/>
+      <c r="IE50"/>
+      <c r="IF50"/>
+      <c r="IG50"/>
+      <c r="IH50"/>
+      <c r="II50"/>
+      <c r="IJ50"/>
+      <c r="IK50"/>
+      <c r="IL50"/>
+      <c r="IM50"/>
+      <c r="IN50"/>
+      <c r="IO50"/>
+      <c r="IP50"/>
+      <c r="IQ50"/>
+      <c r="IR50"/>
+      <c r="IS50"/>
+      <c r="IT50"/>
+      <c r="IU50"/>
+      <c r="IV50"/>
+      <c r="IW50"/>
+    </row>
+    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B51" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C51" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D51" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E50" s="34" t="s">
+      <c r="E51" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F50" s="34" t="s">
+      <c r="F51" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G50" s="35">
-        <v>0</v>
-      </c>
-      <c r="H50" s="36">
-        <v>0</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" s="38" t="s">
+      <c r="G51" s="35">
+        <v>0</v>
+      </c>
+      <c r="H51" s="36">
+        <v>0</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J51" s="38" t="s">
         <v>91</v>
       </c>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51"/>
+      <c r="Y51"/>
+      <c r="Z51"/>
+      <c r="AA51"/>
+      <c r="AB51"/>
+      <c r="AC51"/>
+      <c r="AD51"/>
+      <c r="AE51"/>
+      <c r="AF51"/>
+      <c r="AG51"/>
+      <c r="AH51"/>
+      <c r="AI51"/>
+      <c r="AJ51"/>
+      <c r="AK51"/>
+      <c r="AL51"/>
+      <c r="AM51"/>
+      <c r="AN51"/>
+      <c r="AO51"/>
+      <c r="AP51"/>
+      <c r="AQ51"/>
+      <c r="AR51"/>
+      <c r="AS51"/>
+      <c r="AT51"/>
+      <c r="AU51"/>
+      <c r="AV51"/>
+      <c r="AW51"/>
+      <c r="AX51"/>
+      <c r="AY51"/>
+      <c r="AZ51"/>
+      <c r="BA51"/>
+      <c r="BB51"/>
+      <c r="BC51"/>
+      <c r="BD51"/>
+      <c r="BE51"/>
+      <c r="BF51"/>
+      <c r="BG51"/>
+      <c r="BH51"/>
+      <c r="BI51"/>
+      <c r="BJ51"/>
+      <c r="BK51"/>
+      <c r="BL51"/>
+      <c r="BM51"/>
+      <c r="BN51"/>
+      <c r="BO51"/>
+      <c r="BP51"/>
+      <c r="BQ51"/>
+      <c r="BR51"/>
+      <c r="BS51"/>
+      <c r="BT51"/>
+      <c r="BU51"/>
+      <c r="BV51"/>
+      <c r="BW51"/>
+      <c r="BX51"/>
+      <c r="BY51"/>
+      <c r="BZ51"/>
+      <c r="CA51"/>
+      <c r="CB51"/>
+      <c r="CC51"/>
+      <c r="CD51"/>
+      <c r="CE51"/>
+      <c r="CF51"/>
+      <c r="CG51"/>
+      <c r="CH51"/>
+      <c r="CI51"/>
+      <c r="CJ51"/>
+      <c r="CK51"/>
+      <c r="CL51"/>
+      <c r="CM51"/>
+      <c r="CN51"/>
+      <c r="CO51"/>
+      <c r="CP51"/>
+      <c r="CQ51"/>
+      <c r="CR51"/>
+      <c r="CS51"/>
+      <c r="CT51"/>
+      <c r="CU51"/>
+      <c r="CV51"/>
+      <c r="CW51"/>
+      <c r="CX51"/>
+      <c r="CY51"/>
+      <c r="CZ51"/>
+      <c r="DA51"/>
+      <c r="DB51"/>
+      <c r="DC51"/>
+      <c r="DD51"/>
+      <c r="DE51"/>
+      <c r="DF51"/>
+      <c r="DG51"/>
+      <c r="DH51"/>
+      <c r="DI51"/>
+      <c r="DJ51"/>
+      <c r="DK51"/>
+      <c r="DL51"/>
+      <c r="DM51"/>
+      <c r="DN51"/>
+      <c r="DO51"/>
+      <c r="DP51"/>
+      <c r="DQ51"/>
+      <c r="DR51"/>
+      <c r="DS51"/>
+      <c r="DT51"/>
+      <c r="DU51"/>
+      <c r="DV51"/>
+      <c r="DW51"/>
+      <c r="DX51"/>
+      <c r="DY51"/>
+      <c r="DZ51"/>
+      <c r="EA51"/>
+      <c r="EB51"/>
+      <c r="EC51"/>
+      <c r="ED51"/>
+      <c r="EE51"/>
+      <c r="EF51"/>
+      <c r="EG51"/>
+      <c r="EH51"/>
+      <c r="EI51"/>
+      <c r="EJ51"/>
+      <c r="EK51"/>
+      <c r="EL51"/>
+      <c r="EM51"/>
+      <c r="EN51"/>
+      <c r="EO51"/>
+      <c r="EP51"/>
+      <c r="EQ51"/>
+      <c r="ER51"/>
+      <c r="ES51"/>
+      <c r="ET51"/>
+      <c r="EU51"/>
+      <c r="EV51"/>
+      <c r="EW51"/>
+      <c r="EX51"/>
+      <c r="EY51"/>
+      <c r="EZ51"/>
+      <c r="FA51"/>
+      <c r="FB51"/>
+      <c r="FC51"/>
+      <c r="FD51"/>
+      <c r="FE51"/>
+      <c r="FF51"/>
+      <c r="FG51"/>
+      <c r="FH51"/>
+      <c r="FI51"/>
+      <c r="FJ51"/>
+      <c r="FK51"/>
+      <c r="FL51"/>
+      <c r="FM51"/>
+      <c r="FN51"/>
+      <c r="FO51"/>
+      <c r="FP51"/>
+      <c r="FQ51"/>
+      <c r="FR51"/>
+      <c r="FS51"/>
+      <c r="FT51"/>
+      <c r="FU51"/>
+      <c r="FV51"/>
+      <c r="FW51"/>
+      <c r="FX51"/>
+      <c r="FY51"/>
+      <c r="FZ51"/>
+      <c r="GA51"/>
+      <c r="GB51"/>
+      <c r="GC51"/>
+      <c r="GD51"/>
+      <c r="GE51"/>
+      <c r="GF51"/>
+      <c r="GG51"/>
+      <c r="GH51"/>
+      <c r="GI51"/>
+      <c r="GJ51"/>
+      <c r="GK51"/>
+      <c r="GL51"/>
+      <c r="GM51"/>
+      <c r="GN51"/>
+      <c r="GO51"/>
+      <c r="GP51"/>
+      <c r="GQ51"/>
+      <c r="GR51"/>
+      <c r="GS51"/>
+      <c r="GT51"/>
+      <c r="GU51"/>
+      <c r="GV51"/>
+      <c r="GW51"/>
+      <c r="GX51"/>
+      <c r="GY51"/>
+      <c r="GZ51"/>
+      <c r="HA51"/>
+      <c r="HB51"/>
+      <c r="HC51"/>
+      <c r="HD51"/>
+      <c r="HE51"/>
+      <c r="HF51"/>
+      <c r="HG51"/>
+      <c r="HH51"/>
+      <c r="HI51"/>
+      <c r="HJ51"/>
+      <c r="HK51"/>
+      <c r="HL51"/>
+      <c r="HM51"/>
+      <c r="HN51"/>
+      <c r="HO51"/>
+      <c r="HP51"/>
+      <c r="HQ51"/>
+      <c r="HR51"/>
+      <c r="HS51"/>
+      <c r="HT51"/>
+      <c r="HU51"/>
+      <c r="HV51"/>
+      <c r="HW51"/>
+      <c r="HX51"/>
+      <c r="HY51"/>
+      <c r="HZ51"/>
+      <c r="IA51"/>
+      <c r="IB51"/>
+      <c r="IC51"/>
+      <c r="ID51"/>
+      <c r="IE51"/>
+      <c r="IF51"/>
+      <c r="IG51"/>
+      <c r="IH51"/>
+      <c r="II51"/>
+      <c r="IJ51"/>
+      <c r="IK51"/>
+      <c r="IL51"/>
+      <c r="IM51"/>
+      <c r="IN51"/>
+      <c r="IO51"/>
+      <c r="IP51"/>
+      <c r="IQ51"/>
+      <c r="IR51"/>
+      <c r="IS51"/>
+      <c r="IT51"/>
+      <c r="IU51"/>
+      <c r="IV51"/>
+      <c r="IW51"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
changed label Gender to Sex
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12363EC3-7ACD-B44B-AC17-5CA04EAA3179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C228CB08-D99C-094A-BBBF-0CFDDE0461F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>Preferred Language</t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -676,11 +679,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -742,6 +756,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1127,10 +1142,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW50"/>
+  <dimension ref="A1:IW51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1291,15 +1306,15 @@
     </row>
     <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6"/>
+        <v>105</v>
+      </c>
+      <c r="D6" s="19"/>
       <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
@@ -1319,15 +1334,15 @@
     </row>
     <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="D7"/>
       <c r="E7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1345,47 +1360,45 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>26</v>
-      </c>
+    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16"/>
       <c r="J8" s="11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9"/>
+      <c r="C9" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="42"/>
       <c r="E9" s="11" t="s">
         <v>11</v>
       </c>
@@ -1407,13 +1420,13 @@
     </row>
     <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="11" t="s">
@@ -1437,13 +1450,13 @@
     </row>
     <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="11" t="s">
@@ -1465,43 +1478,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>33</v>
+    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="D12"/>
-      <c r="E12" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="21" t="s">
+      <c r="E12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="10">
         <v>0</v>
       </c>
       <c r="H12" s="10">
-        <v>1</v>
-      </c>
-      <c r="I12" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J12" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="21" t="s">
@@ -1518,18 +1533,18 @@
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="11" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14"/>
       <c r="E14" s="21" t="s">
@@ -1549,47 +1564,45 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>40</v>
+    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="D15"/>
-      <c r="E15" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="24">
-        <v>0</v>
-      </c>
-      <c r="H15" s="24">
-        <v>0</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>27</v>
+      <c r="E15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="D16"/>
       <c r="E16" s="23" t="s">
         <v>11</v>
       </c>
@@ -1611,15 +1624,15 @@
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17"/>
+        <v>115</v>
+      </c>
+      <c r="D17" s="19"/>
       <c r="E17" s="23" t="s">
         <v>11</v>
       </c>
@@ -1640,14 +1653,14 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
-        <v>43</v>
+      <c r="A18" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>44</v>
+      <c r="C18" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D18"/>
       <c r="E18" s="23" t="s">
@@ -1660,22 +1673,24 @@
         <v>0</v>
       </c>
       <c r="H18" s="24">
-        <v>1</v>
-      </c>
-      <c r="I18" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J18" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19"/>
       <c r="E19" s="23" t="s">
@@ -1694,17 +1709,16 @@
       <c r="J19" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>48</v>
+      <c r="C20" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D20"/>
       <c r="E20" s="23" t="s">
@@ -1721,52 +1735,51 @@
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0</v>
+      </c>
+      <c r="H21" s="24">
+        <v>1</v>
+      </c>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="B22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="D21"/>
-      <c r="E21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="27">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
-        <v>0</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="D22"/>
       <c r="E22" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>13</v>
@@ -1784,45 +1797,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="28" t="s">
+    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D23"/>
       <c r="E23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="30">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31">
+      <c r="F23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
         <v>0</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="32" t="s">
-        <v>57</v>
+      <c r="C24" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="D24"/>
       <c r="E24" s="6" t="s">
@@ -1846,13 +1859,13 @@
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>59</v>
+      <c r="C25" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="D25"/>
       <c r="E25" s="6" t="s">
@@ -1876,13 +1889,13 @@
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26"/>
       <c r="E26" s="6" t="s">
@@ -1906,13 +1919,13 @@
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="33" t="s">
-        <v>63</v>
+      <c r="C27" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="D27"/>
       <c r="E27" s="6" t="s">
@@ -1934,75 +1947,75 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>52</v>
+    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="D28"/>
       <c r="E28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="27">
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
+        <v>53</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="30">
+        <v>0</v>
+      </c>
+      <c r="H28" s="31">
         <v>0</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="J28" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D29"/>
       <c r="E29" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="30">
-        <v>0</v>
-      </c>
-      <c r="H29" s="31">
+      <c r="F29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="27">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
         <v>0</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="31" t="s">
+      <c r="J29" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="32" t="s">
-        <v>57</v>
+      <c r="C30" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="D30"/>
       <c r="E30" s="6" t="s">
@@ -2026,13 +2039,13 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>59</v>
+      <c r="C31" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="D31"/>
       <c r="E31" s="6" t="s">
@@ -2056,13 +2069,13 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32"/>
       <c r="E32" s="6" t="s">
@@ -2086,13 +2099,13 @@
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33"/>
       <c r="E33" s="6" t="s">
@@ -2116,17 +2129,17 @@
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="33" t="s">
-        <v>72</v>
+      <c r="C34" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="D34"/>
-      <c r="E34" s="29" t="s">
-        <v>11</v>
+      <c r="E34" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>13</v>
@@ -2135,24 +2148,24 @@
         <v>0</v>
       </c>
       <c r="H34" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J34" s="31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D35"/>
       <c r="E35" s="29" t="s">
@@ -2176,13 +2189,13 @@
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36"/>
       <c r="E36" s="29" t="s">
@@ -2206,13 +2219,13 @@
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37"/>
       <c r="E37" s="29" t="s">
@@ -2236,13 +2249,13 @@
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D38"/>
       <c r="E38" s="29" t="s">
@@ -2266,13 +2279,13 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D39"/>
       <c r="E39" s="29" t="s">
@@ -2296,13 +2309,13 @@
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D40"/>
       <c r="E40" s="29" t="s">
@@ -2326,13 +2339,13 @@
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D41"/>
       <c r="E41" s="29" t="s">
@@ -2356,13 +2369,13 @@
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D42"/>
       <c r="E42" s="29" t="s">
@@ -2384,103 +2397,103 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="34" t="s">
+    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43"/>
+      <c r="E43" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="30">
+        <v>0</v>
+      </c>
+      <c r="H43" s="31">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="34" t="s">
+      <c r="B44" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D43"/>
-      <c r="E43" s="34" t="s">
+      <c r="D44"/>
+      <c r="E44" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F44" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="35">
-        <v>0</v>
-      </c>
-      <c r="H43" s="36">
-        <v>1</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="37" t="s">
+      <c r="G44" s="35">
+        <v>0</v>
+      </c>
+      <c r="H44" s="36">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B45" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C45" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="43" t="s">
+      <c r="D45" s="42"/>
+      <c r="E45" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="35">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36">
-        <v>0</v>
-      </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="37" t="s">
+      <c r="F45" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="37" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45"/>
-      <c r="E45" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="35">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36">
-        <v>0</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="40" t="s">
-        <v>110</v>
+      <c r="C46" s="34" t="s">
+        <v>105</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="34" t="s">
@@ -2493,22 +2506,24 @@
         <v>0</v>
       </c>
       <c r="H46" s="36">
-        <v>1</v>
-      </c>
-      <c r="I46" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J46" s="37" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B47" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="34" t="s">
-        <v>112</v>
+      <c r="C47" s="40" t="s">
+        <v>110</v>
       </c>
       <c r="D47"/>
       <c r="E47" s="34" t="s">
@@ -2530,13 +2545,13 @@
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="34" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B48" s="34" t="s">
         <v>104</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D48"/>
       <c r="E48" s="34" t="s">
@@ -2557,14 +2572,14 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="43" t="s">
-        <v>118</v>
+      <c r="A49" s="34" t="s">
+        <v>107</v>
       </c>
       <c r="B49" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="42" t="s">
-        <v>23</v>
+      <c r="C49" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="D49"/>
       <c r="E49" s="34" t="s">
@@ -2577,42 +2592,70 @@
         <v>0</v>
       </c>
       <c r="H49" s="36">
-        <v>0</v>
-      </c>
-      <c r="I49" s="44" t="s">
-        <v>26</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I49" s="10"/>
       <c r="J49" s="37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" s="34" t="s">
-        <v>91</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="43" t="s">
+        <v>118</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="34" t="s">
-        <v>93</v>
+        <v>104</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>23</v>
       </c>
       <c r="D50"/>
       <c r="E50" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="35">
+        <v>0</v>
+      </c>
+      <c r="H50" s="36">
+        <v>0</v>
+      </c>
+      <c r="I50" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A51" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="34" t="s">
+      <c r="B51" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51"/>
+      <c r="E51" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F51" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G50" s="35">
-        <v>0</v>
-      </c>
-      <c r="H50" s="36">
-        <v>1</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" s="38" t="s">
+      <c r="G51" s="35">
+        <v>0</v>
+      </c>
+      <c r="H51" s="36">
+        <v>1</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J51" s="38" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2627,10 +2670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IW51"/>
+  <dimension ref="A1:IW52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2828,16 +2871,16 @@
     </row>
     <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>98</v>
+        <v>105</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>11</v>
@@ -2856,50 +2899,48 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
-        <v>1</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>26</v>
-      </c>
+    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16"/>
       <c r="J8" s="11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>25</v>
+      <c r="C9" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>120</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>11</v>
@@ -2922,16 +2963,16 @@
     </row>
     <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>11</v>
@@ -2954,15 +2995,17 @@
     </row>
     <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11"/>
+        <v>29</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="E11" s="11" t="s">
         <v>11</v>
       </c>
@@ -2982,23 +3025,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="21" t="s">
+    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="10">
@@ -3007,22 +3048,26 @@
       <c r="H12" s="10">
         <v>1</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J12" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13"/>
+        <v>33</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="E13" s="21" t="s">
         <v>11</v>
       </c>
@@ -3033,22 +3078,22 @@
         <v>0</v>
       </c>
       <c r="H13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="11" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14"/>
       <c r="E14" s="21" t="s">
@@ -3068,50 +3113,46 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="24">
-        <v>0</v>
-      </c>
-      <c r="H15" s="24">
-        <v>1</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>27</v>
+    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>11</v>
@@ -3134,16 +3175,16 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>11</v>
@@ -3165,17 +3206,17 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
-        <v>43</v>
+      <c r="A18" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>44</v>
+      <c r="C18" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>11</v>
@@ -3189,23 +3230,25 @@
       <c r="H18" s="24">
         <v>1</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J18" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>11</v>
@@ -3226,15 +3269,17 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20"/>
+      <c r="C20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="E20" s="23" t="s">
         <v>11</v>
       </c>
@@ -3245,60 +3290,56 @@
         <v>0</v>
       </c>
       <c r="H20" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0</v>
+      </c>
+      <c r="H21" s="24">
+        <v>1</v>
+      </c>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="27">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
-        <v>1</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>13</v>
@@ -3316,50 +3357,50 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="28" t="s">
+    <row r="23" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="30">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31">
+      <c r="F23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
         <v>1</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>57</v>
+      <c r="C24" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>53</v>
@@ -3382,16 +3423,16 @@
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>103</v>
+      <c r="C25" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>53</v>
@@ -3414,16 +3455,16 @@
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>53</v>
@@ -3446,16 +3487,16 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>53</v>
@@ -3478,16 +3519,16 @@
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>63</v>
+      <c r="C28" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>53</v>
@@ -3508,82 +3549,82 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="30">
+        <v>0</v>
+      </c>
+      <c r="H29" s="31">
+        <v>1</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="19" t="s">
+      <c r="B30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="27">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10">
-        <v>1</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="31">
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="27">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
         <v>1</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J30" s="31" t="s">
+      <c r="J30" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>57</v>
+      <c r="C31" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>65</v>
@@ -3606,16 +3647,16 @@
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>59</v>
+      <c r="C32" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>65</v>
@@ -3638,16 +3679,16 @@
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>65</v>
@@ -3670,16 +3711,16 @@
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>65</v>
@@ -3702,17 +3743,19 @@
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="29" t="s">
-        <v>11</v>
+      <c r="C35" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>13</v>
@@ -3721,24 +3764,24 @@
         <v>0</v>
       </c>
       <c r="H35" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J35" s="31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="29" t="s">
@@ -3762,13 +3805,13 @@
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="29" t="s">
@@ -3792,13 +3835,13 @@
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="29" t="s">
@@ -3822,13 +3865,13 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="29" t="s">
@@ -3852,13 +3895,13 @@
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="29" t="s">
@@ -3882,13 +3925,13 @@
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="29" t="s">
@@ -3912,13 +3955,13 @@
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="29" t="s">
@@ -3942,13 +3985,13 @@
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="29" t="s">
@@ -3970,107 +4013,109 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="34" t="s">
+    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="30">
+        <v>0</v>
+      </c>
+      <c r="H44" s="31">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="34" t="s">
+      <c r="B45" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34" t="s">
+      <c r="D45" s="34"/>
+      <c r="E45" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F45" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="35">
-        <v>0</v>
-      </c>
-      <c r="H44" s="36">
-        <v>0</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="37" t="s">
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="H45" s="36">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
+    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B46" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C46" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D46" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E46" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="35">
-        <v>0</v>
-      </c>
-      <c r="H45" s="36">
-        <v>1</v>
-      </c>
-      <c r="I45" s="10"/>
-      <c r="J45" s="37" t="s">
+      <c r="F46" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="35">
+        <v>0</v>
+      </c>
+      <c r="H46" s="36">
+        <v>1</v>
+      </c>
+      <c r="I46" s="10"/>
+      <c r="J46" s="37" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46"/>
-      <c r="E46" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="35">
-        <v>0</v>
-      </c>
-      <c r="H46" s="36">
-        <v>1</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J46" s="37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B47" s="34" t="s">
         <v>104</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D47"/>
+        <v>105</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>121</v>
+      </c>
       <c r="E47" s="34" t="s">
         <v>104</v>
       </c>
@@ -4081,22 +4126,24 @@
         <v>0</v>
       </c>
       <c r="H47" s="36">
-        <v>0</v>
-      </c>
-      <c r="I47" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="J47" s="37" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B48" s="34" t="s">
         <v>104</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D48"/>
       <c r="E48" s="34" t="s">
@@ -4118,13 +4165,13 @@
     </row>
     <row r="49" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="34" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B49" s="34" t="s">
         <v>104</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D49"/>
       <c r="E49" s="34" t="s">
@@ -4145,18 +4192,16 @@
       </c>
     </row>
     <row r="50" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="43" t="s">
-        <v>118</v>
+      <c r="A50" s="34" t="s">
+        <v>107</v>
       </c>
       <c r="B50" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="42" t="s">
-        <v>23</v>
-      </c>
+      <c r="C50" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50"/>
       <c r="E50" s="34" t="s">
         <v>104</v>
       </c>
@@ -4167,292 +4212,43 @@
         <v>0</v>
       </c>
       <c r="H50" s="36">
-        <v>1</v>
-      </c>
-      <c r="I50" s="44" t="s">
-        <v>26</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I50" s="10"/>
       <c r="J50" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="35">
+        <v>0</v>
+      </c>
+      <c r="H51" s="36">
+        <v>1</v>
+      </c>
+      <c r="I51" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J51" s="37" t="s">
         <v>27</v>
-      </c>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50"/>
-      <c r="S50"/>
-      <c r="T50"/>
-      <c r="U50"/>
-      <c r="V50"/>
-      <c r="W50"/>
-      <c r="X50"/>
-      <c r="Y50"/>
-      <c r="Z50"/>
-      <c r="AA50"/>
-      <c r="AB50"/>
-      <c r="AC50"/>
-      <c r="AD50"/>
-      <c r="AE50"/>
-      <c r="AF50"/>
-      <c r="AG50"/>
-      <c r="AH50"/>
-      <c r="AI50"/>
-      <c r="AJ50"/>
-      <c r="AK50"/>
-      <c r="AL50"/>
-      <c r="AM50"/>
-      <c r="AN50"/>
-      <c r="AO50"/>
-      <c r="AP50"/>
-      <c r="AQ50"/>
-      <c r="AR50"/>
-      <c r="AS50"/>
-      <c r="AT50"/>
-      <c r="AU50"/>
-      <c r="AV50"/>
-      <c r="AW50"/>
-      <c r="AX50"/>
-      <c r="AY50"/>
-      <c r="AZ50"/>
-      <c r="BA50"/>
-      <c r="BB50"/>
-      <c r="BC50"/>
-      <c r="BD50"/>
-      <c r="BE50"/>
-      <c r="BF50"/>
-      <c r="BG50"/>
-      <c r="BH50"/>
-      <c r="BI50"/>
-      <c r="BJ50"/>
-      <c r="BK50"/>
-      <c r="BL50"/>
-      <c r="BM50"/>
-      <c r="BN50"/>
-      <c r="BO50"/>
-      <c r="BP50"/>
-      <c r="BQ50"/>
-      <c r="BR50"/>
-      <c r="BS50"/>
-      <c r="BT50"/>
-      <c r="BU50"/>
-      <c r="BV50"/>
-      <c r="BW50"/>
-      <c r="BX50"/>
-      <c r="BY50"/>
-      <c r="BZ50"/>
-      <c r="CA50"/>
-      <c r="CB50"/>
-      <c r="CC50"/>
-      <c r="CD50"/>
-      <c r="CE50"/>
-      <c r="CF50"/>
-      <c r="CG50"/>
-      <c r="CH50"/>
-      <c r="CI50"/>
-      <c r="CJ50"/>
-      <c r="CK50"/>
-      <c r="CL50"/>
-      <c r="CM50"/>
-      <c r="CN50"/>
-      <c r="CO50"/>
-      <c r="CP50"/>
-      <c r="CQ50"/>
-      <c r="CR50"/>
-      <c r="CS50"/>
-      <c r="CT50"/>
-      <c r="CU50"/>
-      <c r="CV50"/>
-      <c r="CW50"/>
-      <c r="CX50"/>
-      <c r="CY50"/>
-      <c r="CZ50"/>
-      <c r="DA50"/>
-      <c r="DB50"/>
-      <c r="DC50"/>
-      <c r="DD50"/>
-      <c r="DE50"/>
-      <c r="DF50"/>
-      <c r="DG50"/>
-      <c r="DH50"/>
-      <c r="DI50"/>
-      <c r="DJ50"/>
-      <c r="DK50"/>
-      <c r="DL50"/>
-      <c r="DM50"/>
-      <c r="DN50"/>
-      <c r="DO50"/>
-      <c r="DP50"/>
-      <c r="DQ50"/>
-      <c r="DR50"/>
-      <c r="DS50"/>
-      <c r="DT50"/>
-      <c r="DU50"/>
-      <c r="DV50"/>
-      <c r="DW50"/>
-      <c r="DX50"/>
-      <c r="DY50"/>
-      <c r="DZ50"/>
-      <c r="EA50"/>
-      <c r="EB50"/>
-      <c r="EC50"/>
-      <c r="ED50"/>
-      <c r="EE50"/>
-      <c r="EF50"/>
-      <c r="EG50"/>
-      <c r="EH50"/>
-      <c r="EI50"/>
-      <c r="EJ50"/>
-      <c r="EK50"/>
-      <c r="EL50"/>
-      <c r="EM50"/>
-      <c r="EN50"/>
-      <c r="EO50"/>
-      <c r="EP50"/>
-      <c r="EQ50"/>
-      <c r="ER50"/>
-      <c r="ES50"/>
-      <c r="ET50"/>
-      <c r="EU50"/>
-      <c r="EV50"/>
-      <c r="EW50"/>
-      <c r="EX50"/>
-      <c r="EY50"/>
-      <c r="EZ50"/>
-      <c r="FA50"/>
-      <c r="FB50"/>
-      <c r="FC50"/>
-      <c r="FD50"/>
-      <c r="FE50"/>
-      <c r="FF50"/>
-      <c r="FG50"/>
-      <c r="FH50"/>
-      <c r="FI50"/>
-      <c r="FJ50"/>
-      <c r="FK50"/>
-      <c r="FL50"/>
-      <c r="FM50"/>
-      <c r="FN50"/>
-      <c r="FO50"/>
-      <c r="FP50"/>
-      <c r="FQ50"/>
-      <c r="FR50"/>
-      <c r="FS50"/>
-      <c r="FT50"/>
-      <c r="FU50"/>
-      <c r="FV50"/>
-      <c r="FW50"/>
-      <c r="FX50"/>
-      <c r="FY50"/>
-      <c r="FZ50"/>
-      <c r="GA50"/>
-      <c r="GB50"/>
-      <c r="GC50"/>
-      <c r="GD50"/>
-      <c r="GE50"/>
-      <c r="GF50"/>
-      <c r="GG50"/>
-      <c r="GH50"/>
-      <c r="GI50"/>
-      <c r="GJ50"/>
-      <c r="GK50"/>
-      <c r="GL50"/>
-      <c r="GM50"/>
-      <c r="GN50"/>
-      <c r="GO50"/>
-      <c r="GP50"/>
-      <c r="GQ50"/>
-      <c r="GR50"/>
-      <c r="GS50"/>
-      <c r="GT50"/>
-      <c r="GU50"/>
-      <c r="GV50"/>
-      <c r="GW50"/>
-      <c r="GX50"/>
-      <c r="GY50"/>
-      <c r="GZ50"/>
-      <c r="HA50"/>
-      <c r="HB50"/>
-      <c r="HC50"/>
-      <c r="HD50"/>
-      <c r="HE50"/>
-      <c r="HF50"/>
-      <c r="HG50"/>
-      <c r="HH50"/>
-      <c r="HI50"/>
-      <c r="HJ50"/>
-      <c r="HK50"/>
-      <c r="HL50"/>
-      <c r="HM50"/>
-      <c r="HN50"/>
-      <c r="HO50"/>
-      <c r="HP50"/>
-      <c r="HQ50"/>
-      <c r="HR50"/>
-      <c r="HS50"/>
-      <c r="HT50"/>
-      <c r="HU50"/>
-      <c r="HV50"/>
-      <c r="HW50"/>
-      <c r="HX50"/>
-      <c r="HY50"/>
-      <c r="HZ50"/>
-      <c r="IA50"/>
-      <c r="IB50"/>
-      <c r="IC50"/>
-      <c r="ID50"/>
-      <c r="IE50"/>
-      <c r="IF50"/>
-      <c r="IG50"/>
-      <c r="IH50"/>
-      <c r="II50"/>
-      <c r="IJ50"/>
-      <c r="IK50"/>
-      <c r="IL50"/>
-      <c r="IM50"/>
-      <c r="IN50"/>
-      <c r="IO50"/>
-      <c r="IP50"/>
-      <c r="IQ50"/>
-      <c r="IR50"/>
-      <c r="IS50"/>
-      <c r="IT50"/>
-      <c r="IU50"/>
-      <c r="IV50"/>
-      <c r="IW50"/>
-    </row>
-    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="F51" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" s="35">
-        <v>0</v>
-      </c>
-      <c r="H51" s="36">
-        <v>0</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J51" s="38" t="s">
-        <v>90</v>
       </c>
       <c r="K51"/>
       <c r="L51"/>
@@ -4702,6 +4498,285 @@
       <c r="IV51"/>
       <c r="IW51"/>
     </row>
+    <row r="52" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="35">
+        <v>0</v>
+      </c>
+      <c r="H52" s="36">
+        <v>0</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J52" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
+      <c r="AA52"/>
+      <c r="AB52"/>
+      <c r="AC52"/>
+      <c r="AD52"/>
+      <c r="AE52"/>
+      <c r="AF52"/>
+      <c r="AG52"/>
+      <c r="AH52"/>
+      <c r="AI52"/>
+      <c r="AJ52"/>
+      <c r="AK52"/>
+      <c r="AL52"/>
+      <c r="AM52"/>
+      <c r="AN52"/>
+      <c r="AO52"/>
+      <c r="AP52"/>
+      <c r="AQ52"/>
+      <c r="AR52"/>
+      <c r="AS52"/>
+      <c r="AT52"/>
+      <c r="AU52"/>
+      <c r="AV52"/>
+      <c r="AW52"/>
+      <c r="AX52"/>
+      <c r="AY52"/>
+      <c r="AZ52"/>
+      <c r="BA52"/>
+      <c r="BB52"/>
+      <c r="BC52"/>
+      <c r="BD52"/>
+      <c r="BE52"/>
+      <c r="BF52"/>
+      <c r="BG52"/>
+      <c r="BH52"/>
+      <c r="BI52"/>
+      <c r="BJ52"/>
+      <c r="BK52"/>
+      <c r="BL52"/>
+      <c r="BM52"/>
+      <c r="BN52"/>
+      <c r="BO52"/>
+      <c r="BP52"/>
+      <c r="BQ52"/>
+      <c r="BR52"/>
+      <c r="BS52"/>
+      <c r="BT52"/>
+      <c r="BU52"/>
+      <c r="BV52"/>
+      <c r="BW52"/>
+      <c r="BX52"/>
+      <c r="BY52"/>
+      <c r="BZ52"/>
+      <c r="CA52"/>
+      <c r="CB52"/>
+      <c r="CC52"/>
+      <c r="CD52"/>
+      <c r="CE52"/>
+      <c r="CF52"/>
+      <c r="CG52"/>
+      <c r="CH52"/>
+      <c r="CI52"/>
+      <c r="CJ52"/>
+      <c r="CK52"/>
+      <c r="CL52"/>
+      <c r="CM52"/>
+      <c r="CN52"/>
+      <c r="CO52"/>
+      <c r="CP52"/>
+      <c r="CQ52"/>
+      <c r="CR52"/>
+      <c r="CS52"/>
+      <c r="CT52"/>
+      <c r="CU52"/>
+      <c r="CV52"/>
+      <c r="CW52"/>
+      <c r="CX52"/>
+      <c r="CY52"/>
+      <c r="CZ52"/>
+      <c r="DA52"/>
+      <c r="DB52"/>
+      <c r="DC52"/>
+      <c r="DD52"/>
+      <c r="DE52"/>
+      <c r="DF52"/>
+      <c r="DG52"/>
+      <c r="DH52"/>
+      <c r="DI52"/>
+      <c r="DJ52"/>
+      <c r="DK52"/>
+      <c r="DL52"/>
+      <c r="DM52"/>
+      <c r="DN52"/>
+      <c r="DO52"/>
+      <c r="DP52"/>
+      <c r="DQ52"/>
+      <c r="DR52"/>
+      <c r="DS52"/>
+      <c r="DT52"/>
+      <c r="DU52"/>
+      <c r="DV52"/>
+      <c r="DW52"/>
+      <c r="DX52"/>
+      <c r="DY52"/>
+      <c r="DZ52"/>
+      <c r="EA52"/>
+      <c r="EB52"/>
+      <c r="EC52"/>
+      <c r="ED52"/>
+      <c r="EE52"/>
+      <c r="EF52"/>
+      <c r="EG52"/>
+      <c r="EH52"/>
+      <c r="EI52"/>
+      <c r="EJ52"/>
+      <c r="EK52"/>
+      <c r="EL52"/>
+      <c r="EM52"/>
+      <c r="EN52"/>
+      <c r="EO52"/>
+      <c r="EP52"/>
+      <c r="EQ52"/>
+      <c r="ER52"/>
+      <c r="ES52"/>
+      <c r="ET52"/>
+      <c r="EU52"/>
+      <c r="EV52"/>
+      <c r="EW52"/>
+      <c r="EX52"/>
+      <c r="EY52"/>
+      <c r="EZ52"/>
+      <c r="FA52"/>
+      <c r="FB52"/>
+      <c r="FC52"/>
+      <c r="FD52"/>
+      <c r="FE52"/>
+      <c r="FF52"/>
+      <c r="FG52"/>
+      <c r="FH52"/>
+      <c r="FI52"/>
+      <c r="FJ52"/>
+      <c r="FK52"/>
+      <c r="FL52"/>
+      <c r="FM52"/>
+      <c r="FN52"/>
+      <c r="FO52"/>
+      <c r="FP52"/>
+      <c r="FQ52"/>
+      <c r="FR52"/>
+      <c r="FS52"/>
+      <c r="FT52"/>
+      <c r="FU52"/>
+      <c r="FV52"/>
+      <c r="FW52"/>
+      <c r="FX52"/>
+      <c r="FY52"/>
+      <c r="FZ52"/>
+      <c r="GA52"/>
+      <c r="GB52"/>
+      <c r="GC52"/>
+      <c r="GD52"/>
+      <c r="GE52"/>
+      <c r="GF52"/>
+      <c r="GG52"/>
+      <c r="GH52"/>
+      <c r="GI52"/>
+      <c r="GJ52"/>
+      <c r="GK52"/>
+      <c r="GL52"/>
+      <c r="GM52"/>
+      <c r="GN52"/>
+      <c r="GO52"/>
+      <c r="GP52"/>
+      <c r="GQ52"/>
+      <c r="GR52"/>
+      <c r="GS52"/>
+      <c r="GT52"/>
+      <c r="GU52"/>
+      <c r="GV52"/>
+      <c r="GW52"/>
+      <c r="GX52"/>
+      <c r="GY52"/>
+      <c r="GZ52"/>
+      <c r="HA52"/>
+      <c r="HB52"/>
+      <c r="HC52"/>
+      <c r="HD52"/>
+      <c r="HE52"/>
+      <c r="HF52"/>
+      <c r="HG52"/>
+      <c r="HH52"/>
+      <c r="HI52"/>
+      <c r="HJ52"/>
+      <c r="HK52"/>
+      <c r="HL52"/>
+      <c r="HM52"/>
+      <c r="HN52"/>
+      <c r="HO52"/>
+      <c r="HP52"/>
+      <c r="HQ52"/>
+      <c r="HR52"/>
+      <c r="HS52"/>
+      <c r="HT52"/>
+      <c r="HU52"/>
+      <c r="HV52"/>
+      <c r="HW52"/>
+      <c r="HX52"/>
+      <c r="HY52"/>
+      <c r="HZ52"/>
+      <c r="IA52"/>
+      <c r="IB52"/>
+      <c r="IC52"/>
+      <c r="ID52"/>
+      <c r="IE52"/>
+      <c r="IF52"/>
+      <c r="IG52"/>
+      <c r="IH52"/>
+      <c r="II52"/>
+      <c r="IJ52"/>
+      <c r="IK52"/>
+      <c r="IL52"/>
+      <c r="IM52"/>
+      <c r="IN52"/>
+      <c r="IO52"/>
+      <c r="IP52"/>
+      <c r="IQ52"/>
+      <c r="IR52"/>
+      <c r="IS52"/>
+      <c r="IT52"/>
+      <c r="IU52"/>
+      <c r="IV52"/>
+      <c r="IW52"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
updated label + custom fields
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/office/oscar-web/db/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C38ECB1-AA88-A843-A315-DACA32096FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F77943-FA6F-3C45-9323-A0132652C732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="138">
   <si>
     <t>name</t>
   </si>
@@ -1284,8 +1284,8 @@
   </sheetPr>
   <dimension ref="A1:IW62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2590,9 +2590,7 @@
       <c r="H44" s="36">
         <v>1</v>
       </c>
-      <c r="I44" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="I44" s="10"/>
       <c r="J44" s="37" t="s">
         <v>90</v>
       </c>
@@ -3122,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IW63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4516,9 +4514,7 @@
       <c r="H45" s="36">
         <v>0</v>
       </c>
-      <c r="I45" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="I45" s="10"/>
       <c r="J45" s="37" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
updated the translation for ratanak
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiry/Documents/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4290E9C8-5699-1C47-8FEF-EDAC159C76BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2608C080-6086-044F-AD32-BB91ECB4946E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="141">
   <si>
     <t>name</t>
   </si>
@@ -434,6 +434,21 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>complete_screening_assessment</t>
+  </si>
+  <si>
+    <t>Complete Screening Assessment</t>
+  </si>
+  <si>
+    <t>legal_documents</t>
+  </si>
+  <si>
+    <t>Legal Documentations</t>
+  </si>
+  <si>
+    <t>raname</t>
   </si>
 </sst>
 </file>
@@ -581,7 +596,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -812,11 +827,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -895,6 +923,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,10 +1318,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW62"/>
+  <dimension ref="A1:IW64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1747,7 +1785,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -1777,7 +1815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>47</v>
       </c>
@@ -1806,15 +1844,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
-        <v>49</v>
+    <row r="19" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>50</v>
+      <c r="C19" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>11</v>
@@ -1828,48 +1866,321 @@
       <c r="H19" s="25">
         <v>1</v>
       </c>
-      <c r="I19" s="25"/>
+      <c r="I19" s="10"/>
       <c r="J19" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="IM19" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="IN19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="IO19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="IQ19" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="IR19" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="IS19" s="25">
+        <v>0</v>
+      </c>
+      <c r="IT19" s="25">
+        <v>1</v>
+      </c>
+      <c r="IU19" s="25"/>
+      <c r="IV19" s="25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="IW19" s="25"/>
+    </row>
+    <row r="20" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="67">
+        <v>0</v>
+      </c>
+      <c r="H20" s="67">
+        <v>1</v>
+      </c>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
+      <c r="BN20"/>
+      <c r="BO20"/>
+      <c r="BP20"/>
+      <c r="BQ20"/>
+      <c r="BR20"/>
+      <c r="BS20"/>
+      <c r="BT20"/>
+      <c r="BU20"/>
+      <c r="BV20"/>
+      <c r="BW20"/>
+      <c r="BX20"/>
+      <c r="BY20"/>
+      <c r="BZ20"/>
+      <c r="CA20"/>
+      <c r="CB20"/>
+      <c r="CC20"/>
+      <c r="CD20"/>
+      <c r="CE20"/>
+      <c r="CF20"/>
+      <c r="CG20"/>
+      <c r="CH20"/>
+      <c r="CI20"/>
+      <c r="CJ20"/>
+      <c r="CK20"/>
+      <c r="CL20"/>
+      <c r="CM20"/>
+      <c r="CN20"/>
+      <c r="CO20"/>
+      <c r="CP20"/>
+      <c r="CQ20"/>
+      <c r="CR20"/>
+      <c r="CS20"/>
+      <c r="CT20"/>
+      <c r="CU20"/>
+      <c r="CV20"/>
+      <c r="CW20"/>
+      <c r="CX20"/>
+      <c r="CY20"/>
+      <c r="CZ20"/>
+      <c r="DA20"/>
+      <c r="DB20"/>
+      <c r="DC20"/>
+      <c r="DD20"/>
+      <c r="DE20"/>
+      <c r="DF20"/>
+      <c r="DG20"/>
+      <c r="DH20"/>
+      <c r="DI20"/>
+      <c r="DJ20"/>
+      <c r="DK20"/>
+      <c r="DL20"/>
+      <c r="DM20"/>
+      <c r="DN20"/>
+      <c r="DO20"/>
+      <c r="DP20"/>
+      <c r="DQ20"/>
+      <c r="DR20"/>
+      <c r="DS20"/>
+      <c r="DT20"/>
+      <c r="DU20"/>
+      <c r="DV20"/>
+      <c r="DW20"/>
+      <c r="DX20"/>
+      <c r="DY20"/>
+      <c r="DZ20"/>
+      <c r="EA20"/>
+      <c r="EB20"/>
+      <c r="EC20"/>
+      <c r="ED20"/>
+      <c r="EE20"/>
+      <c r="EF20"/>
+      <c r="EG20"/>
+      <c r="EH20"/>
+      <c r="EI20"/>
+      <c r="EJ20"/>
+      <c r="EK20"/>
+      <c r="EL20"/>
+      <c r="EM20"/>
+      <c r="EN20"/>
+      <c r="EO20"/>
+      <c r="EP20"/>
+      <c r="EQ20"/>
+      <c r="ER20"/>
+      <c r="ES20"/>
+      <c r="ET20"/>
+      <c r="EU20"/>
+      <c r="EV20"/>
+      <c r="EW20"/>
+      <c r="EX20"/>
+      <c r="EY20"/>
+      <c r="EZ20"/>
+      <c r="FA20"/>
+      <c r="FB20"/>
+      <c r="FC20"/>
+      <c r="FD20"/>
+      <c r="FE20"/>
+      <c r="FF20"/>
+      <c r="FG20"/>
+      <c r="FH20"/>
+      <c r="FI20"/>
+      <c r="FJ20"/>
+      <c r="FK20"/>
+      <c r="FL20"/>
+      <c r="FM20"/>
+      <c r="FN20"/>
+      <c r="FO20"/>
+      <c r="FP20"/>
+      <c r="FQ20"/>
+      <c r="FR20"/>
+      <c r="FS20"/>
+      <c r="FT20"/>
+      <c r="FU20"/>
+      <c r="FV20"/>
+      <c r="FW20"/>
+      <c r="FX20"/>
+      <c r="FY20"/>
+      <c r="FZ20"/>
+      <c r="GA20"/>
+      <c r="GB20"/>
+      <c r="GC20"/>
+      <c r="GD20"/>
+      <c r="GE20"/>
+      <c r="GF20"/>
+      <c r="GG20"/>
+      <c r="GH20"/>
+      <c r="GI20"/>
+      <c r="GJ20"/>
+      <c r="GK20"/>
+      <c r="GL20"/>
+      <c r="GM20"/>
+      <c r="GN20"/>
+      <c r="GO20"/>
+      <c r="GP20"/>
+      <c r="GQ20"/>
+      <c r="GR20"/>
+      <c r="GS20"/>
+      <c r="GT20"/>
+      <c r="GU20"/>
+      <c r="GV20"/>
+      <c r="GW20"/>
+      <c r="GX20"/>
+      <c r="GY20"/>
+      <c r="GZ20"/>
+      <c r="HA20"/>
+      <c r="HB20"/>
+      <c r="HC20"/>
+      <c r="HD20"/>
+      <c r="HE20"/>
+      <c r="HF20"/>
+      <c r="HG20"/>
+      <c r="HH20"/>
+      <c r="HI20"/>
+      <c r="HJ20"/>
+      <c r="HK20"/>
+      <c r="HL20"/>
+      <c r="HM20"/>
+      <c r="HN20"/>
+      <c r="HO20"/>
+      <c r="HP20"/>
+      <c r="HQ20"/>
+      <c r="HR20"/>
+      <c r="HS20"/>
+      <c r="HT20"/>
+      <c r="HU20"/>
+      <c r="HV20"/>
+      <c r="HW20"/>
+      <c r="HX20"/>
+      <c r="HY20"/>
+      <c r="HZ20"/>
+      <c r="IA20"/>
+      <c r="IB20"/>
+      <c r="IC20"/>
+      <c r="ID20"/>
+      <c r="IE20"/>
+      <c r="IF20"/>
+      <c r="IG20"/>
+      <c r="IH20"/>
+      <c r="II20"/>
+      <c r="IJ20"/>
+      <c r="IK20"/>
+      <c r="IL20"/>
+      <c r="IM20"/>
+      <c r="IN20"/>
+      <c r="IO20"/>
+      <c r="IP20"/>
+      <c r="IQ20"/>
+      <c r="IR20"/>
+      <c r="IS20"/>
+      <c r="IT20"/>
+      <c r="IU20"/>
+      <c r="IV20"/>
+      <c r="IW20"/>
+    </row>
+    <row r="21" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="25">
-        <v>0</v>
-      </c>
-      <c r="H20" s="25">
-        <v>1</v>
-      </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="25"/>
-    </row>
-    <row r="21" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>54</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>11</v>
@@ -1885,50 +2196,49 @@
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="1:257" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="25">
+        <v>0</v>
+      </c>
+      <c r="H22" s="25">
+        <v>1</v>
+      </c>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:257" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="28">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <v>0</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>58</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>13</v>
@@ -1946,44 +2256,44 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="29" t="s">
+    <row r="24" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="31">
-        <v>0</v>
-      </c>
-      <c r="H24" s="32">
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="28">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
         <v>0</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="33" t="s">
-        <v>63</v>
+      <c r="C25" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>59</v>
@@ -2004,15 +2314,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>65</v>
+      <c r="C26" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>59</v>
@@ -2033,15 +2343,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>59</v>
@@ -2062,15 +2372,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>69</v>
+      <c r="C28" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>59</v>
@@ -2091,73 +2401,73 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>58</v>
+    <row r="29" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="28">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10">
+        <v>59</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="31">
+        <v>0</v>
+      </c>
+      <c r="H29" s="32">
         <v>0</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="29" t="s">
+    <row r="30" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="31">
-        <v>0</v>
-      </c>
-      <c r="H30" s="32">
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="28">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
         <v>0</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="J30" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="33" t="s">
-        <v>63</v>
+      <c r="C31" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>71</v>
@@ -2178,15 +2488,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>65</v>
+      <c r="C32" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>71</v>
@@ -2207,15 +2517,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" s="1" customFormat="1" ht="0" hidden="1" x14ac:dyDescent="0">
       <c r="A33" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>71</v>
@@ -2236,16 +2546,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>69</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="6" t="s">
         <v>71</v>
       </c>
@@ -2265,18 +2576,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>11</v>
+      <c r="C35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>13</v>
@@ -2285,25 +2597,26 @@
         <v>0</v>
       </c>
       <c r="H35" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>28</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>80</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="30" t="s">
         <v>11</v>
       </c>
@@ -2323,16 +2636,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>82</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="30" t="s">
         <v>11</v>
       </c>
@@ -2352,16 +2666,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>84</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="30" t="s">
         <v>11</v>
       </c>
@@ -2381,16 +2696,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>86</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="30" t="s">
         <v>11</v>
       </c>
@@ -2410,16 +2726,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>88</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="30" t="s">
         <v>11</v>
       </c>
@@ -2439,16 +2756,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>90</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="30" t="s">
         <v>11</v>
       </c>
@@ -2468,16 +2786,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>69</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="30" t="s">
         <v>11</v>
       </c>
@@ -2497,16 +2816,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>93</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="30" t="s">
         <v>11</v>
       </c>
@@ -2526,101 +2846,103 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="35" t="s">
+    <row r="44" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="31">
+        <v>0</v>
+      </c>
+      <c r="H44" s="32">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B45" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C45" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="37" t="s">
+      <c r="D45" s="20"/>
+      <c r="E45" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="F44" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="38">
-        <v>0</v>
-      </c>
-      <c r="H44" s="39">
-        <v>0</v>
-      </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="40" t="s">
+      <c r="F45" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="38">
+        <v>0</v>
+      </c>
+      <c r="H45" s="39">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="41" t="s">
+    <row r="46" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B46" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C46" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="41" t="s">
+      <c r="D46" s="20"/>
+      <c r="E46" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="44">
-        <v>0</v>
-      </c>
-      <c r="H45" s="44">
-        <v>1</v>
-      </c>
-      <c r="I45" s="44" t="s">
+      <c r="F46" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="44">
+        <v>0</v>
+      </c>
+      <c r="H46" s="44">
+        <v>1</v>
+      </c>
+      <c r="I46" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="J45" s="45" t="s">
+      <c r="J46" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="46" t="s">
+    <row r="47" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="46" t="s">
         <v>77</v>
-      </c>
-      <c r="B46" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="48">
-        <v>0</v>
-      </c>
-      <c r="H46" s="48">
-        <v>1</v>
-      </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="46" t="s">
-        <v>22</v>
       </c>
       <c r="B47" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="46" t="s">
@@ -2637,18 +2959,18 @@
       </c>
       <c r="I47" s="48"/>
       <c r="J47" s="49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="46" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="B48" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="46" t="s">
@@ -2665,18 +2987,18 @@
       </c>
       <c r="I48" s="48"/>
       <c r="J48" s="49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="46" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="B49" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="46" t="s">
@@ -2693,18 +3015,18 @@
       </c>
       <c r="I49" s="48"/>
       <c r="J49" s="49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="46" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B50" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="46" t="s">
@@ -2724,15 +3046,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="46" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B51" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="46" t="s">
@@ -2752,15 +3074,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="46" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B52" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="46" t="s">
@@ -2780,15 +3102,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B53" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="60" t="s">
-        <v>105</v>
+      <c r="C53" s="58" t="s">
+        <v>61</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="46" t="s">
@@ -2808,15 +3130,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="46" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B54" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="46" t="s">
@@ -2836,15 +3158,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="46" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B55" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="58" t="s">
-        <v>109</v>
+      <c r="C55" s="60" t="s">
+        <v>105</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="46" t="s">
@@ -2864,70 +3186,73 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="35" t="s">
+    <row r="56" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="20"/>
+      <c r="E56" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="48">
+        <v>0</v>
+      </c>
+      <c r="H56" s="48">
+        <v>1</v>
+      </c>
+      <c r="I56" s="48"/>
+      <c r="J56" s="49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="20"/>
+      <c r="E57" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="48">
+        <v>0</v>
+      </c>
+      <c r="H57" s="48">
+        <v>1</v>
+      </c>
+      <c r="I57" s="48"/>
+      <c r="J57" s="49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="35" t="s">
         <v>111</v>
-      </c>
-      <c r="B56" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="E56" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="F56" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="38">
-        <v>0</v>
-      </c>
-      <c r="H56" s="39">
-        <v>1</v>
-      </c>
-      <c r="I56" s="10"/>
-      <c r="J56" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B57" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="E57" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="F57" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="38">
-        <v>0</v>
-      </c>
-      <c r="H57" s="39">
-        <v>1</v>
-      </c>
-      <c r="I57" s="10"/>
-      <c r="J57" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="61" t="s">
-        <v>22</v>
       </c>
       <c r="B58" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C58" s="52" t="s">
-        <v>23</v>
-      </c>
+      <c r="C58" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="35" t="s">
         <v>110</v>
       </c>
@@ -2940,21 +3265,22 @@
       <c r="H58" s="39">
         <v>1</v>
       </c>
-      <c r="I58" s="53"/>
+      <c r="I58" s="10"/>
       <c r="J58" s="40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="52" t="s">
-        <v>116</v>
-      </c>
+      <c r="C59" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="35" t="s">
         <v>110</v>
       </c>
@@ -2967,21 +3293,22 @@
       <c r="H59" s="39">
         <v>1</v>
       </c>
-      <c r="I59" s="53"/>
+      <c r="I59" s="10"/>
       <c r="J59" s="40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="35" t="s">
-        <v>117</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="61" t="s">
+        <v>22</v>
       </c>
       <c r="B60" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C60" s="35" t="s">
-        <v>118</v>
-      </c>
+      <c r="C60" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="1"/>
       <c r="E60" s="35" t="s">
         <v>110</v>
       </c>
@@ -2994,21 +3321,22 @@
       <c r="H60" s="39">
         <v>1</v>
       </c>
-      <c r="I60" s="10"/>
+      <c r="I60" s="53"/>
       <c r="J60" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="37" t="s">
-        <v>119</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="35" t="s">
+        <v>115</v>
       </c>
       <c r="B61" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="C61" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="1"/>
       <c r="E61" s="35" t="s">
         <v>110</v>
       </c>
@@ -3019,41 +3347,98 @@
         <v>0</v>
       </c>
       <c r="H61" s="39">
-        <v>0</v>
-      </c>
-      <c r="I61" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" s="53"/>
+      <c r="J61" s="40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="38">
+        <v>0</v>
+      </c>
+      <c r="H62" s="39">
+        <v>1</v>
+      </c>
+      <c r="I62" s="10"/>
+      <c r="J62" s="40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="38">
+        <v>0</v>
+      </c>
+      <c r="H63" s="39">
+        <v>0</v>
+      </c>
+      <c r="I63" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J61" s="40" t="s">
+      <c r="J63" s="40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A62" s="35" t="s">
+    <row r="64" spans="1:10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="35" t="s">
+      <c r="B64" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C64" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="E62" s="35" t="s">
+      <c r="D64" s="1"/>
+      <c r="E64" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="F62" s="35" t="s">
+      <c r="F64" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="38">
-        <v>0</v>
-      </c>
-      <c r="H62" s="39">
-        <v>1</v>
-      </c>
-      <c r="I62" s="10" t="s">
+      <c r="G64" s="38">
+        <v>0</v>
+      </c>
+      <c r="H64" s="39">
+        <v>1</v>
+      </c>
+      <c r="I64" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J62" s="54" t="s">
+      <c r="J64" s="54" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3070,7 +3455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IW62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change care plan label for ratanak
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiry/Documents/oscar-web/db/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Home/Documents/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA519AC-1B24-4D4B-BD23-B89E07096A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE9AFA-6490-304F-AC1A-17C4312ABD51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1326,14 +1326,16 @@
   </sheetPr>
   <dimension ref="A1:IW65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="8" width="11.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
@@ -11375,8 +11377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IW62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
worked on added new fields to fields setting
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Home/Documents/oscar-web/db/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE9AFA-6490-304F-AC1A-17C4312ABD51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A04C3-7F51-0148-AE6A-5BFA1D650B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="440" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="179">
   <si>
     <t>name</t>
   </si>
@@ -456,6 +456,114 @@
   <si>
     <t>View Screening Assessment</t>
   </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> brc</t>
+  </si>
+  <si>
+    <t>meeting_date</t>
+  </si>
+  <si>
+    <t>attendants</t>
+  </si>
+  <si>
+    <t>client_strength</t>
+  </si>
+  <si>
+    <t>client_limitation</t>
+  </si>
+  <si>
+    <t>client_engagement</t>
+  </si>
+  <si>
+    <t>presenting_problem</t>
+  </si>
+  <si>
+    <t>local_resource</t>
+  </si>
+  <si>
+    <t>client_support</t>
+  </si>
+  <si>
+    <t>attachments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case_conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> field</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rename</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Case Conference Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Attendants</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Client strengths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Client limitations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Client engagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Presenting problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resources/services in local community</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Support and Barriers to client engagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Attachments</t>
+  </si>
+  <si>
+    <t>add_new_service_delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Add New Service Delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> service_delivery</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Category</t>
+  </si>
+  <si>
+    <t>service_deliveries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Service Deliveries</t>
+  </si>
+  <si>
+    <t>service_provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Service Provided</t>
+  </si>
+  <si>
+    <t>case_conference</t>
+  </si>
+  <si>
+    <t>service_delivery</t>
+  </si>
 </sst>
 </file>
 
@@ -602,7 +710,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -846,11 +954,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -939,6 +1086,33 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1324,10 +1498,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW65"/>
+  <dimension ref="A1:IW94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11089,31 +11263,31 @@
       <c r="IW64"/>
     </row>
     <row r="65" spans="1:257" x14ac:dyDescent="0.15">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="E65" s="35" t="s">
+      <c r="E65" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="F65" s="35" t="s">
+      <c r="F65" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G65" s="38">
+      <c r="G65" s="69">
         <v>0</v>
       </c>
-      <c r="H65" s="39">
+      <c r="H65" s="70">
         <v>1</v>
       </c>
-      <c r="I65" s="10" t="s">
+      <c r="I65" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="J65" s="54" t="s">
+      <c r="J65" s="72" t="s">
         <v>122</v>
       </c>
       <c r="K65"/>
@@ -11364,6 +11538,4339 @@
       <c r="IV65"/>
       <c r="IW65"/>
     </row>
+    <row r="66" spans="1:257" s="80" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" s="78"/>
+      <c r="E66" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F66" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G66" s="78">
+        <v>0</v>
+      </c>
+      <c r="H66" s="78">
+        <v>1</v>
+      </c>
+      <c r="I66" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J66" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K66" s="79"/>
+      <c r="L66" s="79"/>
+      <c r="M66" s="79"/>
+      <c r="N66" s="79"/>
+      <c r="O66" s="79"/>
+      <c r="P66" s="79"/>
+      <c r="Q66" s="79"/>
+      <c r="R66" s="79"/>
+      <c r="S66" s="79"/>
+      <c r="T66" s="79"/>
+      <c r="U66" s="79"/>
+      <c r="V66" s="79"/>
+      <c r="W66" s="79"/>
+      <c r="X66" s="79"/>
+      <c r="Y66" s="79"/>
+      <c r="Z66" s="79"/>
+      <c r="AA66" s="79"/>
+      <c r="AB66" s="79"/>
+      <c r="AC66" s="79"/>
+      <c r="AD66" s="79"/>
+      <c r="AE66" s="79"/>
+      <c r="AF66" s="79"/>
+      <c r="AG66" s="79"/>
+      <c r="AH66" s="79"/>
+      <c r="AI66" s="79"/>
+      <c r="AJ66" s="79"/>
+      <c r="AK66" s="79"/>
+      <c r="AL66" s="79"/>
+      <c r="AM66" s="79"/>
+      <c r="AN66" s="79"/>
+      <c r="AO66" s="79"/>
+      <c r="AP66" s="79"/>
+      <c r="AQ66" s="79"/>
+      <c r="AR66" s="79"/>
+      <c r="AS66" s="79"/>
+      <c r="AT66" s="79"/>
+      <c r="AU66" s="79"/>
+      <c r="AV66" s="79"/>
+      <c r="AW66" s="79"/>
+      <c r="AX66" s="79"/>
+      <c r="AY66" s="79"/>
+      <c r="AZ66" s="79"/>
+      <c r="BA66" s="79"/>
+      <c r="BB66" s="79"/>
+      <c r="BC66" s="79"/>
+      <c r="BD66" s="79"/>
+      <c r="BE66" s="79"/>
+      <c r="BF66" s="79"/>
+      <c r="BG66" s="79"/>
+      <c r="BH66" s="79"/>
+      <c r="BI66" s="79"/>
+      <c r="BJ66" s="79"/>
+      <c r="BK66" s="79"/>
+      <c r="BL66" s="79"/>
+      <c r="BM66" s="79"/>
+      <c r="BN66" s="79"/>
+      <c r="BO66" s="79"/>
+      <c r="BP66" s="79"/>
+      <c r="BQ66" s="79"/>
+      <c r="BR66" s="79"/>
+      <c r="BS66" s="79"/>
+      <c r="BT66" s="79"/>
+      <c r="BU66" s="79"/>
+      <c r="BV66" s="79"/>
+      <c r="BW66" s="79"/>
+      <c r="BX66" s="79"/>
+      <c r="BY66" s="79"/>
+      <c r="BZ66" s="79"/>
+      <c r="CA66" s="79"/>
+      <c r="CB66" s="79"/>
+      <c r="CC66" s="79"/>
+      <c r="CD66" s="79"/>
+      <c r="CE66" s="79"/>
+      <c r="CF66" s="79"/>
+      <c r="CG66" s="79"/>
+      <c r="CH66" s="79"/>
+      <c r="CI66" s="79"/>
+      <c r="CJ66" s="79"/>
+      <c r="CK66" s="79"/>
+      <c r="CL66" s="79"/>
+      <c r="CM66" s="79"/>
+      <c r="CN66" s="79"/>
+      <c r="CO66" s="79"/>
+      <c r="CP66" s="79"/>
+      <c r="CQ66" s="79"/>
+      <c r="CR66" s="79"/>
+      <c r="CS66" s="79"/>
+      <c r="CT66" s="79"/>
+      <c r="CU66" s="79"/>
+      <c r="CV66" s="79"/>
+      <c r="CW66" s="79"/>
+      <c r="CX66" s="79"/>
+      <c r="CY66" s="79"/>
+      <c r="CZ66" s="79"/>
+      <c r="DA66" s="79"/>
+      <c r="DB66" s="79"/>
+      <c r="DC66" s="79"/>
+      <c r="DD66" s="79"/>
+      <c r="DE66" s="79"/>
+      <c r="DF66" s="79"/>
+      <c r="DG66" s="79"/>
+      <c r="DH66" s="79"/>
+      <c r="DI66" s="79"/>
+      <c r="DJ66" s="79"/>
+      <c r="DK66" s="79"/>
+      <c r="DL66" s="79"/>
+      <c r="DM66" s="79"/>
+      <c r="DN66" s="79"/>
+      <c r="DO66" s="79"/>
+      <c r="DP66" s="79"/>
+      <c r="DQ66" s="79"/>
+      <c r="DR66" s="79"/>
+      <c r="DS66" s="79"/>
+      <c r="DT66" s="79"/>
+      <c r="DU66" s="79"/>
+      <c r="DV66" s="79"/>
+      <c r="DW66" s="79"/>
+      <c r="DX66" s="79"/>
+      <c r="DY66" s="79"/>
+      <c r="DZ66" s="79"/>
+      <c r="EA66" s="79"/>
+      <c r="EB66" s="79"/>
+      <c r="EC66" s="79"/>
+      <c r="ED66" s="79"/>
+      <c r="EE66" s="79"/>
+      <c r="EF66" s="79"/>
+      <c r="EG66" s="79"/>
+      <c r="EH66" s="79"/>
+      <c r="EI66" s="79"/>
+      <c r="EJ66" s="79"/>
+      <c r="EK66" s="79"/>
+      <c r="EL66" s="79"/>
+      <c r="EM66" s="79"/>
+      <c r="EN66" s="79"/>
+      <c r="EO66" s="79"/>
+      <c r="EP66" s="79"/>
+      <c r="EQ66" s="79"/>
+      <c r="ER66" s="79"/>
+      <c r="ES66" s="79"/>
+      <c r="ET66" s="79"/>
+      <c r="EU66" s="79"/>
+      <c r="EV66" s="79"/>
+      <c r="EW66" s="79"/>
+      <c r="EX66" s="79"/>
+      <c r="EY66" s="79"/>
+      <c r="EZ66" s="79"/>
+      <c r="FA66" s="79"/>
+      <c r="FB66" s="79"/>
+      <c r="FC66" s="79"/>
+      <c r="FD66" s="79"/>
+      <c r="FE66" s="79"/>
+      <c r="FF66" s="79"/>
+      <c r="FG66" s="79"/>
+      <c r="FH66" s="79"/>
+      <c r="FI66" s="79"/>
+      <c r="FJ66" s="79"/>
+      <c r="FK66" s="79"/>
+      <c r="FL66" s="79"/>
+      <c r="FM66" s="79"/>
+      <c r="FN66" s="79"/>
+      <c r="FO66" s="79"/>
+      <c r="FP66" s="79"/>
+      <c r="FQ66" s="79"/>
+      <c r="FR66" s="79"/>
+      <c r="FS66" s="79"/>
+      <c r="FT66" s="79"/>
+      <c r="FU66" s="79"/>
+      <c r="FV66" s="79"/>
+      <c r="FW66" s="79"/>
+      <c r="FX66" s="79"/>
+      <c r="FY66" s="79"/>
+      <c r="FZ66" s="79"/>
+      <c r="GA66" s="79"/>
+      <c r="GB66" s="79"/>
+      <c r="GC66" s="79"/>
+      <c r="GD66" s="79"/>
+      <c r="GE66" s="79"/>
+      <c r="GF66" s="79"/>
+      <c r="GG66" s="79"/>
+      <c r="GH66" s="79"/>
+      <c r="GI66" s="79"/>
+      <c r="GJ66" s="79"/>
+      <c r="GK66" s="79"/>
+      <c r="GL66" s="79"/>
+      <c r="GM66" s="79"/>
+      <c r="GN66" s="79"/>
+      <c r="GO66" s="79"/>
+      <c r="GP66" s="79"/>
+      <c r="GQ66" s="79"/>
+      <c r="GR66" s="79"/>
+      <c r="GS66" s="79"/>
+      <c r="GT66" s="79"/>
+      <c r="GU66" s="79"/>
+      <c r="GV66" s="79"/>
+      <c r="GW66" s="79"/>
+      <c r="GX66" s="79"/>
+      <c r="GY66" s="79"/>
+      <c r="GZ66" s="79"/>
+      <c r="HA66" s="79"/>
+      <c r="HB66" s="79"/>
+      <c r="HC66" s="79"/>
+      <c r="HD66" s="79"/>
+      <c r="HE66" s="79"/>
+      <c r="HF66" s="79"/>
+      <c r="HG66" s="79"/>
+      <c r="HH66" s="79"/>
+      <c r="HI66" s="79"/>
+      <c r="HJ66" s="79"/>
+      <c r="HK66" s="79"/>
+      <c r="HL66" s="79"/>
+      <c r="HM66" s="79"/>
+      <c r="HN66" s="79"/>
+      <c r="HO66" s="79"/>
+      <c r="HP66" s="79"/>
+      <c r="HQ66" s="79"/>
+      <c r="HR66" s="79"/>
+      <c r="HS66" s="79"/>
+      <c r="HT66" s="79"/>
+      <c r="HU66" s="79"/>
+      <c r="HV66" s="79"/>
+      <c r="HW66" s="79"/>
+      <c r="HX66" s="79"/>
+      <c r="HY66" s="79"/>
+      <c r="HZ66" s="79"/>
+      <c r="IA66" s="79"/>
+      <c r="IB66" s="79"/>
+      <c r="IC66" s="79"/>
+      <c r="ID66" s="79"/>
+      <c r="IE66" s="79"/>
+      <c r="IF66" s="79"/>
+      <c r="IG66" s="79"/>
+      <c r="IH66" s="79"/>
+      <c r="II66" s="79"/>
+      <c r="IJ66" s="79"/>
+      <c r="IK66" s="79"/>
+      <c r="IL66" s="79"/>
+      <c r="IM66" s="79"/>
+      <c r="IN66" s="79"/>
+      <c r="IO66" s="79"/>
+      <c r="IP66" s="79"/>
+      <c r="IQ66" s="79"/>
+      <c r="IR66" s="79"/>
+      <c r="IS66" s="79"/>
+      <c r="IT66" s="79"/>
+      <c r="IU66" s="79"/>
+      <c r="IV66" s="79"/>
+      <c r="IW66" s="79"/>
+    </row>
+    <row r="67" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C67" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="D67" s="78"/>
+      <c r="E67" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F67" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G67" s="78">
+        <v>0</v>
+      </c>
+      <c r="H67" s="78">
+        <v>1</v>
+      </c>
+      <c r="I67" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J67" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K67" s="79"/>
+      <c r="L67" s="79"/>
+      <c r="M67" s="79"/>
+      <c r="N67" s="79"/>
+      <c r="O67" s="79"/>
+      <c r="P67" s="79"/>
+      <c r="Q67" s="79"/>
+      <c r="R67" s="79"/>
+      <c r="S67" s="79"/>
+      <c r="T67" s="79"/>
+      <c r="U67" s="79"/>
+      <c r="V67" s="79"/>
+      <c r="W67" s="79"/>
+      <c r="X67" s="79"/>
+      <c r="Y67" s="79"/>
+      <c r="Z67" s="79"/>
+      <c r="AA67" s="79"/>
+      <c r="AB67" s="79"/>
+      <c r="AC67" s="79"/>
+      <c r="AD67" s="79"/>
+      <c r="AE67" s="79"/>
+      <c r="AF67" s="79"/>
+      <c r="AG67" s="79"/>
+      <c r="AH67" s="79"/>
+      <c r="AI67" s="79"/>
+      <c r="AJ67" s="79"/>
+      <c r="AK67" s="79"/>
+      <c r="AL67" s="79"/>
+      <c r="AM67" s="79"/>
+      <c r="AN67" s="79"/>
+      <c r="AO67" s="79"/>
+      <c r="AP67" s="79"/>
+      <c r="AQ67" s="79"/>
+      <c r="AR67" s="79"/>
+      <c r="AS67" s="79"/>
+      <c r="AT67" s="79"/>
+      <c r="AU67" s="79"/>
+      <c r="AV67" s="79"/>
+      <c r="AW67" s="79"/>
+      <c r="AX67" s="79"/>
+      <c r="AY67" s="79"/>
+      <c r="AZ67" s="79"/>
+      <c r="BA67" s="79"/>
+      <c r="BB67" s="79"/>
+      <c r="BC67" s="79"/>
+      <c r="BD67" s="79"/>
+      <c r="BE67" s="79"/>
+      <c r="BF67" s="79"/>
+      <c r="BG67" s="79"/>
+      <c r="BH67" s="79"/>
+      <c r="BI67" s="79"/>
+      <c r="BJ67" s="79"/>
+      <c r="BK67" s="79"/>
+      <c r="BL67" s="79"/>
+      <c r="BM67" s="79"/>
+      <c r="BN67" s="79"/>
+      <c r="BO67" s="79"/>
+      <c r="BP67" s="79"/>
+      <c r="BQ67" s="79"/>
+      <c r="BR67" s="79"/>
+      <c r="BS67" s="79"/>
+      <c r="BT67" s="79"/>
+      <c r="BU67" s="79"/>
+      <c r="BV67" s="79"/>
+      <c r="BW67" s="79"/>
+      <c r="BX67" s="79"/>
+      <c r="BY67" s="79"/>
+      <c r="BZ67" s="79"/>
+      <c r="CA67" s="79"/>
+      <c r="CB67" s="79"/>
+      <c r="CC67" s="79"/>
+      <c r="CD67" s="79"/>
+      <c r="CE67" s="79"/>
+      <c r="CF67" s="79"/>
+      <c r="CG67" s="79"/>
+      <c r="CH67" s="79"/>
+      <c r="CI67" s="79"/>
+      <c r="CJ67" s="79"/>
+      <c r="CK67" s="79"/>
+      <c r="CL67" s="79"/>
+      <c r="CM67" s="79"/>
+      <c r="CN67" s="79"/>
+      <c r="CO67" s="79"/>
+      <c r="CP67" s="79"/>
+      <c r="CQ67" s="79"/>
+      <c r="CR67" s="79"/>
+      <c r="CS67" s="79"/>
+      <c r="CT67" s="79"/>
+      <c r="CU67" s="79"/>
+      <c r="CV67" s="79"/>
+      <c r="CW67" s="79"/>
+      <c r="CX67" s="79"/>
+      <c r="CY67" s="79"/>
+      <c r="CZ67" s="79"/>
+      <c r="DA67" s="79"/>
+      <c r="DB67" s="79"/>
+      <c r="DC67" s="79"/>
+      <c r="DD67" s="79"/>
+      <c r="DE67" s="79"/>
+      <c r="DF67" s="79"/>
+      <c r="DG67" s="79"/>
+      <c r="DH67" s="79"/>
+      <c r="DI67" s="79"/>
+      <c r="DJ67" s="79"/>
+      <c r="DK67" s="79"/>
+      <c r="DL67" s="79"/>
+      <c r="DM67" s="79"/>
+      <c r="DN67" s="79"/>
+      <c r="DO67" s="79"/>
+      <c r="DP67" s="79"/>
+      <c r="DQ67" s="79"/>
+      <c r="DR67" s="79"/>
+      <c r="DS67" s="79"/>
+      <c r="DT67" s="79"/>
+      <c r="DU67" s="79"/>
+      <c r="DV67" s="79"/>
+      <c r="DW67" s="79"/>
+      <c r="DX67" s="79"/>
+      <c r="DY67" s="79"/>
+      <c r="DZ67" s="79"/>
+      <c r="EA67" s="79"/>
+      <c r="EB67" s="79"/>
+      <c r="EC67" s="79"/>
+      <c r="ED67" s="79"/>
+      <c r="EE67" s="79"/>
+      <c r="EF67" s="79"/>
+      <c r="EG67" s="79"/>
+      <c r="EH67" s="79"/>
+      <c r="EI67" s="79"/>
+      <c r="EJ67" s="79"/>
+      <c r="EK67" s="79"/>
+      <c r="EL67" s="79"/>
+      <c r="EM67" s="79"/>
+      <c r="EN67" s="79"/>
+      <c r="EO67" s="79"/>
+      <c r="EP67" s="79"/>
+      <c r="EQ67" s="79"/>
+      <c r="ER67" s="79"/>
+      <c r="ES67" s="79"/>
+      <c r="ET67" s="79"/>
+      <c r="EU67" s="79"/>
+      <c r="EV67" s="79"/>
+      <c r="EW67" s="79"/>
+      <c r="EX67" s="79"/>
+      <c r="EY67" s="79"/>
+      <c r="EZ67" s="79"/>
+      <c r="FA67" s="79"/>
+      <c r="FB67" s="79"/>
+      <c r="FC67" s="79"/>
+      <c r="FD67" s="79"/>
+      <c r="FE67" s="79"/>
+      <c r="FF67" s="79"/>
+      <c r="FG67" s="79"/>
+      <c r="FH67" s="79"/>
+      <c r="FI67" s="79"/>
+      <c r="FJ67" s="79"/>
+      <c r="FK67" s="79"/>
+      <c r="FL67" s="79"/>
+      <c r="FM67" s="79"/>
+      <c r="FN67" s="79"/>
+      <c r="FO67" s="79"/>
+      <c r="FP67" s="79"/>
+      <c r="FQ67" s="79"/>
+      <c r="FR67" s="79"/>
+      <c r="FS67" s="79"/>
+      <c r="FT67" s="79"/>
+      <c r="FU67" s="79"/>
+      <c r="FV67" s="79"/>
+      <c r="FW67" s="79"/>
+      <c r="FX67" s="79"/>
+      <c r="FY67" s="79"/>
+      <c r="FZ67" s="79"/>
+      <c r="GA67" s="79"/>
+      <c r="GB67" s="79"/>
+      <c r="GC67" s="79"/>
+      <c r="GD67" s="79"/>
+      <c r="GE67" s="79"/>
+      <c r="GF67" s="79"/>
+      <c r="GG67" s="79"/>
+      <c r="GH67" s="79"/>
+      <c r="GI67" s="79"/>
+      <c r="GJ67" s="79"/>
+      <c r="GK67" s="79"/>
+      <c r="GL67" s="79"/>
+      <c r="GM67" s="79"/>
+      <c r="GN67" s="79"/>
+      <c r="GO67" s="79"/>
+      <c r="GP67" s="79"/>
+      <c r="GQ67" s="79"/>
+      <c r="GR67" s="79"/>
+      <c r="GS67" s="79"/>
+      <c r="GT67" s="79"/>
+      <c r="GU67" s="79"/>
+      <c r="GV67" s="79"/>
+      <c r="GW67" s="79"/>
+      <c r="GX67" s="79"/>
+      <c r="GY67" s="79"/>
+      <c r="GZ67" s="79"/>
+      <c r="HA67" s="79"/>
+      <c r="HB67" s="79"/>
+      <c r="HC67" s="79"/>
+      <c r="HD67" s="79"/>
+      <c r="HE67" s="79"/>
+      <c r="HF67" s="79"/>
+      <c r="HG67" s="79"/>
+      <c r="HH67" s="79"/>
+      <c r="HI67" s="79"/>
+      <c r="HJ67" s="79"/>
+      <c r="HK67" s="79"/>
+      <c r="HL67" s="79"/>
+      <c r="HM67" s="79"/>
+      <c r="HN67" s="79"/>
+      <c r="HO67" s="79"/>
+      <c r="HP67" s="79"/>
+      <c r="HQ67" s="79"/>
+      <c r="HR67" s="79"/>
+      <c r="HS67" s="79"/>
+      <c r="HT67" s="79"/>
+      <c r="HU67" s="79"/>
+      <c r="HV67" s="79"/>
+      <c r="HW67" s="79"/>
+      <c r="HX67" s="79"/>
+      <c r="HY67" s="79"/>
+      <c r="HZ67" s="79"/>
+      <c r="IA67" s="79"/>
+      <c r="IB67" s="79"/>
+      <c r="IC67" s="79"/>
+      <c r="ID67" s="79"/>
+      <c r="IE67" s="79"/>
+      <c r="IF67" s="79"/>
+      <c r="IG67" s="79"/>
+      <c r="IH67" s="79"/>
+      <c r="II67" s="79"/>
+      <c r="IJ67" s="79"/>
+      <c r="IK67" s="79"/>
+      <c r="IL67" s="79"/>
+      <c r="IM67" s="79"/>
+      <c r="IN67" s="79"/>
+      <c r="IO67" s="79"/>
+      <c r="IP67" s="79"/>
+      <c r="IQ67" s="79"/>
+      <c r="IR67" s="79"/>
+      <c r="IS67" s="79"/>
+      <c r="IT67" s="79"/>
+      <c r="IU67" s="79"/>
+      <c r="IV67" s="79"/>
+      <c r="IW67" s="79"/>
+    </row>
+    <row r="68" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="77" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="78" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F68" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G68" s="78">
+        <v>0</v>
+      </c>
+      <c r="H68" s="78">
+        <v>1</v>
+      </c>
+      <c r="I68" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J68" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K68" s="79"/>
+      <c r="L68" s="79"/>
+      <c r="M68" s="79"/>
+      <c r="N68" s="79"/>
+      <c r="O68" s="79"/>
+      <c r="P68" s="79"/>
+      <c r="Q68" s="79"/>
+      <c r="R68" s="79"/>
+      <c r="S68" s="79"/>
+      <c r="T68" s="79"/>
+      <c r="U68" s="79"/>
+      <c r="V68" s="79"/>
+      <c r="W68" s="79"/>
+      <c r="X68" s="79"/>
+      <c r="Y68" s="79"/>
+      <c r="Z68" s="79"/>
+      <c r="AA68" s="79"/>
+      <c r="AB68" s="79"/>
+      <c r="AC68" s="79"/>
+      <c r="AD68" s="79"/>
+      <c r="AE68" s="79"/>
+      <c r="AF68" s="79"/>
+      <c r="AG68" s="79"/>
+      <c r="AH68" s="79"/>
+      <c r="AI68" s="79"/>
+      <c r="AJ68" s="79"/>
+      <c r="AK68" s="79"/>
+      <c r="AL68" s="79"/>
+      <c r="AM68" s="79"/>
+      <c r="AN68" s="79"/>
+      <c r="AO68" s="79"/>
+      <c r="AP68" s="79"/>
+      <c r="AQ68" s="79"/>
+      <c r="AR68" s="79"/>
+      <c r="AS68" s="79"/>
+      <c r="AT68" s="79"/>
+      <c r="AU68" s="79"/>
+      <c r="AV68" s="79"/>
+      <c r="AW68" s="79"/>
+      <c r="AX68" s="79"/>
+      <c r="AY68" s="79"/>
+      <c r="AZ68" s="79"/>
+      <c r="BA68" s="79"/>
+      <c r="BB68" s="79"/>
+      <c r="BC68" s="79"/>
+      <c r="BD68" s="79"/>
+      <c r="BE68" s="79"/>
+      <c r="BF68" s="79"/>
+      <c r="BG68" s="79"/>
+      <c r="BH68" s="79"/>
+      <c r="BI68" s="79"/>
+      <c r="BJ68" s="79"/>
+      <c r="BK68" s="79"/>
+      <c r="BL68" s="79"/>
+      <c r="BM68" s="79"/>
+      <c r="BN68" s="79"/>
+      <c r="BO68" s="79"/>
+      <c r="BP68" s="79"/>
+      <c r="BQ68" s="79"/>
+      <c r="BR68" s="79"/>
+      <c r="BS68" s="79"/>
+      <c r="BT68" s="79"/>
+      <c r="BU68" s="79"/>
+      <c r="BV68" s="79"/>
+      <c r="BW68" s="79"/>
+      <c r="BX68" s="79"/>
+      <c r="BY68" s="79"/>
+      <c r="BZ68" s="79"/>
+      <c r="CA68" s="79"/>
+      <c r="CB68" s="79"/>
+      <c r="CC68" s="79"/>
+      <c r="CD68" s="79"/>
+      <c r="CE68" s="79"/>
+      <c r="CF68" s="79"/>
+      <c r="CG68" s="79"/>
+      <c r="CH68" s="79"/>
+      <c r="CI68" s="79"/>
+      <c r="CJ68" s="79"/>
+      <c r="CK68" s="79"/>
+      <c r="CL68" s="79"/>
+      <c r="CM68" s="79"/>
+      <c r="CN68" s="79"/>
+      <c r="CO68" s="79"/>
+      <c r="CP68" s="79"/>
+      <c r="CQ68" s="79"/>
+      <c r="CR68" s="79"/>
+      <c r="CS68" s="79"/>
+      <c r="CT68" s="79"/>
+      <c r="CU68" s="79"/>
+      <c r="CV68" s="79"/>
+      <c r="CW68" s="79"/>
+      <c r="CX68" s="79"/>
+      <c r="CY68" s="79"/>
+      <c r="CZ68" s="79"/>
+      <c r="DA68" s="79"/>
+      <c r="DB68" s="79"/>
+      <c r="DC68" s="79"/>
+      <c r="DD68" s="79"/>
+      <c r="DE68" s="79"/>
+      <c r="DF68" s="79"/>
+      <c r="DG68" s="79"/>
+      <c r="DH68" s="79"/>
+      <c r="DI68" s="79"/>
+      <c r="DJ68" s="79"/>
+      <c r="DK68" s="79"/>
+      <c r="DL68" s="79"/>
+      <c r="DM68" s="79"/>
+      <c r="DN68" s="79"/>
+      <c r="DO68" s="79"/>
+      <c r="DP68" s="79"/>
+      <c r="DQ68" s="79"/>
+      <c r="DR68" s="79"/>
+      <c r="DS68" s="79"/>
+      <c r="DT68" s="79"/>
+      <c r="DU68" s="79"/>
+      <c r="DV68" s="79"/>
+      <c r="DW68" s="79"/>
+      <c r="DX68" s="79"/>
+      <c r="DY68" s="79"/>
+      <c r="DZ68" s="79"/>
+      <c r="EA68" s="79"/>
+      <c r="EB68" s="79"/>
+      <c r="EC68" s="79"/>
+      <c r="ED68" s="79"/>
+      <c r="EE68" s="79"/>
+      <c r="EF68" s="79"/>
+      <c r="EG68" s="79"/>
+      <c r="EH68" s="79"/>
+      <c r="EI68" s="79"/>
+      <c r="EJ68" s="79"/>
+      <c r="EK68" s="79"/>
+      <c r="EL68" s="79"/>
+      <c r="EM68" s="79"/>
+      <c r="EN68" s="79"/>
+      <c r="EO68" s="79"/>
+      <c r="EP68" s="79"/>
+      <c r="EQ68" s="79"/>
+      <c r="ER68" s="79"/>
+      <c r="ES68" s="79"/>
+      <c r="ET68" s="79"/>
+      <c r="EU68" s="79"/>
+      <c r="EV68" s="79"/>
+      <c r="EW68" s="79"/>
+      <c r="EX68" s="79"/>
+      <c r="EY68" s="79"/>
+      <c r="EZ68" s="79"/>
+      <c r="FA68" s="79"/>
+      <c r="FB68" s="79"/>
+      <c r="FC68" s="79"/>
+      <c r="FD68" s="79"/>
+      <c r="FE68" s="79"/>
+      <c r="FF68" s="79"/>
+      <c r="FG68" s="79"/>
+      <c r="FH68" s="79"/>
+      <c r="FI68" s="79"/>
+      <c r="FJ68" s="79"/>
+      <c r="FK68" s="79"/>
+      <c r="FL68" s="79"/>
+      <c r="FM68" s="79"/>
+      <c r="FN68" s="79"/>
+      <c r="FO68" s="79"/>
+      <c r="FP68" s="79"/>
+      <c r="FQ68" s="79"/>
+      <c r="FR68" s="79"/>
+      <c r="FS68" s="79"/>
+      <c r="FT68" s="79"/>
+      <c r="FU68" s="79"/>
+      <c r="FV68" s="79"/>
+      <c r="FW68" s="79"/>
+      <c r="FX68" s="79"/>
+      <c r="FY68" s="79"/>
+      <c r="FZ68" s="79"/>
+      <c r="GA68" s="79"/>
+      <c r="GB68" s="79"/>
+      <c r="GC68" s="79"/>
+      <c r="GD68" s="79"/>
+      <c r="GE68" s="79"/>
+      <c r="GF68" s="79"/>
+      <c r="GG68" s="79"/>
+      <c r="GH68" s="79"/>
+      <c r="GI68" s="79"/>
+      <c r="GJ68" s="79"/>
+      <c r="GK68" s="79"/>
+      <c r="GL68" s="79"/>
+      <c r="GM68" s="79"/>
+      <c r="GN68" s="79"/>
+      <c r="GO68" s="79"/>
+      <c r="GP68" s="79"/>
+      <c r="GQ68" s="79"/>
+      <c r="GR68" s="79"/>
+      <c r="GS68" s="79"/>
+      <c r="GT68" s="79"/>
+      <c r="GU68" s="79"/>
+      <c r="GV68" s="79"/>
+      <c r="GW68" s="79"/>
+      <c r="GX68" s="79"/>
+      <c r="GY68" s="79"/>
+      <c r="GZ68" s="79"/>
+      <c r="HA68" s="79"/>
+      <c r="HB68" s="79"/>
+      <c r="HC68" s="79"/>
+      <c r="HD68" s="79"/>
+      <c r="HE68" s="79"/>
+      <c r="HF68" s="79"/>
+      <c r="HG68" s="79"/>
+      <c r="HH68" s="79"/>
+      <c r="HI68" s="79"/>
+      <c r="HJ68" s="79"/>
+      <c r="HK68" s="79"/>
+      <c r="HL68" s="79"/>
+      <c r="HM68" s="79"/>
+      <c r="HN68" s="79"/>
+      <c r="HO68" s="79"/>
+      <c r="HP68" s="79"/>
+      <c r="HQ68" s="79"/>
+      <c r="HR68" s="79"/>
+      <c r="HS68" s="79"/>
+      <c r="HT68" s="79"/>
+      <c r="HU68" s="79"/>
+      <c r="HV68" s="79"/>
+      <c r="HW68" s="79"/>
+      <c r="HX68" s="79"/>
+      <c r="HY68" s="79"/>
+      <c r="HZ68" s="79"/>
+      <c r="IA68" s="79"/>
+      <c r="IB68" s="79"/>
+      <c r="IC68" s="79"/>
+      <c r="ID68" s="79"/>
+      <c r="IE68" s="79"/>
+      <c r="IF68" s="79"/>
+      <c r="IG68" s="79"/>
+      <c r="IH68" s="79"/>
+      <c r="II68" s="79"/>
+      <c r="IJ68" s="79"/>
+      <c r="IK68" s="79"/>
+      <c r="IL68" s="79"/>
+      <c r="IM68" s="79"/>
+      <c r="IN68" s="79"/>
+      <c r="IO68" s="79"/>
+      <c r="IP68" s="79"/>
+      <c r="IQ68" s="79"/>
+      <c r="IR68" s="79"/>
+      <c r="IS68" s="79"/>
+      <c r="IT68" s="79"/>
+      <c r="IU68" s="79"/>
+      <c r="IV68" s="79"/>
+      <c r="IW68" s="79"/>
+    </row>
+    <row r="69" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C69" s="78" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" s="78"/>
+      <c r="E69" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F69" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G69" s="78">
+        <v>0</v>
+      </c>
+      <c r="H69" s="78">
+        <v>1</v>
+      </c>
+      <c r="I69" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J69" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K69" s="79"/>
+      <c r="L69" s="79"/>
+      <c r="M69" s="79"/>
+      <c r="N69" s="79"/>
+      <c r="O69" s="79"/>
+      <c r="P69" s="79"/>
+      <c r="Q69" s="79"/>
+      <c r="R69" s="79"/>
+      <c r="S69" s="79"/>
+      <c r="T69" s="79"/>
+      <c r="U69" s="79"/>
+      <c r="V69" s="79"/>
+      <c r="W69" s="79"/>
+      <c r="X69" s="79"/>
+      <c r="Y69" s="79"/>
+      <c r="Z69" s="79"/>
+      <c r="AA69" s="79"/>
+      <c r="AB69" s="79"/>
+      <c r="AC69" s="79"/>
+      <c r="AD69" s="79"/>
+      <c r="AE69" s="79"/>
+      <c r="AF69" s="79"/>
+      <c r="AG69" s="79"/>
+      <c r="AH69" s="79"/>
+      <c r="AI69" s="79"/>
+      <c r="AJ69" s="79"/>
+      <c r="AK69" s="79"/>
+      <c r="AL69" s="79"/>
+      <c r="AM69" s="79"/>
+      <c r="AN69" s="79"/>
+      <c r="AO69" s="79"/>
+      <c r="AP69" s="79"/>
+      <c r="AQ69" s="79"/>
+      <c r="AR69" s="79"/>
+      <c r="AS69" s="79"/>
+      <c r="AT69" s="79"/>
+      <c r="AU69" s="79"/>
+      <c r="AV69" s="79"/>
+      <c r="AW69" s="79"/>
+      <c r="AX69" s="79"/>
+      <c r="AY69" s="79"/>
+      <c r="AZ69" s="79"/>
+      <c r="BA69" s="79"/>
+      <c r="BB69" s="79"/>
+      <c r="BC69" s="79"/>
+      <c r="BD69" s="79"/>
+      <c r="BE69" s="79"/>
+      <c r="BF69" s="79"/>
+      <c r="BG69" s="79"/>
+      <c r="BH69" s="79"/>
+      <c r="BI69" s="79"/>
+      <c r="BJ69" s="79"/>
+      <c r="BK69" s="79"/>
+      <c r="BL69" s="79"/>
+      <c r="BM69" s="79"/>
+      <c r="BN69" s="79"/>
+      <c r="BO69" s="79"/>
+      <c r="BP69" s="79"/>
+      <c r="BQ69" s="79"/>
+      <c r="BR69" s="79"/>
+      <c r="BS69" s="79"/>
+      <c r="BT69" s="79"/>
+      <c r="BU69" s="79"/>
+      <c r="BV69" s="79"/>
+      <c r="BW69" s="79"/>
+      <c r="BX69" s="79"/>
+      <c r="BY69" s="79"/>
+      <c r="BZ69" s="79"/>
+      <c r="CA69" s="79"/>
+      <c r="CB69" s="79"/>
+      <c r="CC69" s="79"/>
+      <c r="CD69" s="79"/>
+      <c r="CE69" s="79"/>
+      <c r="CF69" s="79"/>
+      <c r="CG69" s="79"/>
+      <c r="CH69" s="79"/>
+      <c r="CI69" s="79"/>
+      <c r="CJ69" s="79"/>
+      <c r="CK69" s="79"/>
+      <c r="CL69" s="79"/>
+      <c r="CM69" s="79"/>
+      <c r="CN69" s="79"/>
+      <c r="CO69" s="79"/>
+      <c r="CP69" s="79"/>
+      <c r="CQ69" s="79"/>
+      <c r="CR69" s="79"/>
+      <c r="CS69" s="79"/>
+      <c r="CT69" s="79"/>
+      <c r="CU69" s="79"/>
+      <c r="CV69" s="79"/>
+      <c r="CW69" s="79"/>
+      <c r="CX69" s="79"/>
+      <c r="CY69" s="79"/>
+      <c r="CZ69" s="79"/>
+      <c r="DA69" s="79"/>
+      <c r="DB69" s="79"/>
+      <c r="DC69" s="79"/>
+      <c r="DD69" s="79"/>
+      <c r="DE69" s="79"/>
+      <c r="DF69" s="79"/>
+      <c r="DG69" s="79"/>
+      <c r="DH69" s="79"/>
+      <c r="DI69" s="79"/>
+      <c r="DJ69" s="79"/>
+      <c r="DK69" s="79"/>
+      <c r="DL69" s="79"/>
+      <c r="DM69" s="79"/>
+      <c r="DN69" s="79"/>
+      <c r="DO69" s="79"/>
+      <c r="DP69" s="79"/>
+      <c r="DQ69" s="79"/>
+      <c r="DR69" s="79"/>
+      <c r="DS69" s="79"/>
+      <c r="DT69" s="79"/>
+      <c r="DU69" s="79"/>
+      <c r="DV69" s="79"/>
+      <c r="DW69" s="79"/>
+      <c r="DX69" s="79"/>
+      <c r="DY69" s="79"/>
+      <c r="DZ69" s="79"/>
+      <c r="EA69" s="79"/>
+      <c r="EB69" s="79"/>
+      <c r="EC69" s="79"/>
+      <c r="ED69" s="79"/>
+      <c r="EE69" s="79"/>
+      <c r="EF69" s="79"/>
+      <c r="EG69" s="79"/>
+      <c r="EH69" s="79"/>
+      <c r="EI69" s="79"/>
+      <c r="EJ69" s="79"/>
+      <c r="EK69" s="79"/>
+      <c r="EL69" s="79"/>
+      <c r="EM69" s="79"/>
+      <c r="EN69" s="79"/>
+      <c r="EO69" s="79"/>
+      <c r="EP69" s="79"/>
+      <c r="EQ69" s="79"/>
+      <c r="ER69" s="79"/>
+      <c r="ES69" s="79"/>
+      <c r="ET69" s="79"/>
+      <c r="EU69" s="79"/>
+      <c r="EV69" s="79"/>
+      <c r="EW69" s="79"/>
+      <c r="EX69" s="79"/>
+      <c r="EY69" s="79"/>
+      <c r="EZ69" s="79"/>
+      <c r="FA69" s="79"/>
+      <c r="FB69" s="79"/>
+      <c r="FC69" s="79"/>
+      <c r="FD69" s="79"/>
+      <c r="FE69" s="79"/>
+      <c r="FF69" s="79"/>
+      <c r="FG69" s="79"/>
+      <c r="FH69" s="79"/>
+      <c r="FI69" s="79"/>
+      <c r="FJ69" s="79"/>
+      <c r="FK69" s="79"/>
+      <c r="FL69" s="79"/>
+      <c r="FM69" s="79"/>
+      <c r="FN69" s="79"/>
+      <c r="FO69" s="79"/>
+      <c r="FP69" s="79"/>
+      <c r="FQ69" s="79"/>
+      <c r="FR69" s="79"/>
+      <c r="FS69" s="79"/>
+      <c r="FT69" s="79"/>
+      <c r="FU69" s="79"/>
+      <c r="FV69" s="79"/>
+      <c r="FW69" s="79"/>
+      <c r="FX69" s="79"/>
+      <c r="FY69" s="79"/>
+      <c r="FZ69" s="79"/>
+      <c r="GA69" s="79"/>
+      <c r="GB69" s="79"/>
+      <c r="GC69" s="79"/>
+      <c r="GD69" s="79"/>
+      <c r="GE69" s="79"/>
+      <c r="GF69" s="79"/>
+      <c r="GG69" s="79"/>
+      <c r="GH69" s="79"/>
+      <c r="GI69" s="79"/>
+      <c r="GJ69" s="79"/>
+      <c r="GK69" s="79"/>
+      <c r="GL69" s="79"/>
+      <c r="GM69" s="79"/>
+      <c r="GN69" s="79"/>
+      <c r="GO69" s="79"/>
+      <c r="GP69" s="79"/>
+      <c r="GQ69" s="79"/>
+      <c r="GR69" s="79"/>
+      <c r="GS69" s="79"/>
+      <c r="GT69" s="79"/>
+      <c r="GU69" s="79"/>
+      <c r="GV69" s="79"/>
+      <c r="GW69" s="79"/>
+      <c r="GX69" s="79"/>
+      <c r="GY69" s="79"/>
+      <c r="GZ69" s="79"/>
+      <c r="HA69" s="79"/>
+      <c r="HB69" s="79"/>
+      <c r="HC69" s="79"/>
+      <c r="HD69" s="79"/>
+      <c r="HE69" s="79"/>
+      <c r="HF69" s="79"/>
+      <c r="HG69" s="79"/>
+      <c r="HH69" s="79"/>
+      <c r="HI69" s="79"/>
+      <c r="HJ69" s="79"/>
+      <c r="HK69" s="79"/>
+      <c r="HL69" s="79"/>
+      <c r="HM69" s="79"/>
+      <c r="HN69" s="79"/>
+      <c r="HO69" s="79"/>
+      <c r="HP69" s="79"/>
+      <c r="HQ69" s="79"/>
+      <c r="HR69" s="79"/>
+      <c r="HS69" s="79"/>
+      <c r="HT69" s="79"/>
+      <c r="HU69" s="79"/>
+      <c r="HV69" s="79"/>
+      <c r="HW69" s="79"/>
+      <c r="HX69" s="79"/>
+      <c r="HY69" s="79"/>
+      <c r="HZ69" s="79"/>
+      <c r="IA69" s="79"/>
+      <c r="IB69" s="79"/>
+      <c r="IC69" s="79"/>
+      <c r="ID69" s="79"/>
+      <c r="IE69" s="79"/>
+      <c r="IF69" s="79"/>
+      <c r="IG69" s="79"/>
+      <c r="IH69" s="79"/>
+      <c r="II69" s="79"/>
+      <c r="IJ69" s="79"/>
+      <c r="IK69" s="79"/>
+      <c r="IL69" s="79"/>
+      <c r="IM69" s="79"/>
+      <c r="IN69" s="79"/>
+      <c r="IO69" s="79"/>
+      <c r="IP69" s="79"/>
+      <c r="IQ69" s="79"/>
+      <c r="IR69" s="79"/>
+      <c r="IS69" s="79"/>
+      <c r="IT69" s="79"/>
+      <c r="IU69" s="79"/>
+      <c r="IV69" s="79"/>
+      <c r="IW69" s="79"/>
+    </row>
+    <row r="70" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="D70" s="78"/>
+      <c r="E70" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F70" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G70" s="78">
+        <v>0</v>
+      </c>
+      <c r="H70" s="78">
+        <v>1</v>
+      </c>
+      <c r="I70" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J70" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K70" s="79"/>
+      <c r="L70" s="79"/>
+      <c r="M70" s="79"/>
+      <c r="N70" s="79"/>
+      <c r="O70" s="79"/>
+      <c r="P70" s="79"/>
+      <c r="Q70" s="79"/>
+      <c r="R70" s="79"/>
+      <c r="S70" s="79"/>
+      <c r="T70" s="79"/>
+      <c r="U70" s="79"/>
+      <c r="V70" s="79"/>
+      <c r="W70" s="79"/>
+      <c r="X70" s="79"/>
+      <c r="Y70" s="79"/>
+      <c r="Z70" s="79"/>
+      <c r="AA70" s="79"/>
+      <c r="AB70" s="79"/>
+      <c r="AC70" s="79"/>
+      <c r="AD70" s="79"/>
+      <c r="AE70" s="79"/>
+      <c r="AF70" s="79"/>
+      <c r="AG70" s="79"/>
+      <c r="AH70" s="79"/>
+      <c r="AI70" s="79"/>
+      <c r="AJ70" s="79"/>
+      <c r="AK70" s="79"/>
+      <c r="AL70" s="79"/>
+      <c r="AM70" s="79"/>
+      <c r="AN70" s="79"/>
+      <c r="AO70" s="79"/>
+      <c r="AP70" s="79"/>
+      <c r="AQ70" s="79"/>
+      <c r="AR70" s="79"/>
+      <c r="AS70" s="79"/>
+      <c r="AT70" s="79"/>
+      <c r="AU70" s="79"/>
+      <c r="AV70" s="79"/>
+      <c r="AW70" s="79"/>
+      <c r="AX70" s="79"/>
+      <c r="AY70" s="79"/>
+      <c r="AZ70" s="79"/>
+      <c r="BA70" s="79"/>
+      <c r="BB70" s="79"/>
+      <c r="BC70" s="79"/>
+      <c r="BD70" s="79"/>
+      <c r="BE70" s="79"/>
+      <c r="BF70" s="79"/>
+      <c r="BG70" s="79"/>
+      <c r="BH70" s="79"/>
+      <c r="BI70" s="79"/>
+      <c r="BJ70" s="79"/>
+      <c r="BK70" s="79"/>
+      <c r="BL70" s="79"/>
+      <c r="BM70" s="79"/>
+      <c r="BN70" s="79"/>
+      <c r="BO70" s="79"/>
+      <c r="BP70" s="79"/>
+      <c r="BQ70" s="79"/>
+      <c r="BR70" s="79"/>
+      <c r="BS70" s="79"/>
+      <c r="BT70" s="79"/>
+      <c r="BU70" s="79"/>
+      <c r="BV70" s="79"/>
+      <c r="BW70" s="79"/>
+      <c r="BX70" s="79"/>
+      <c r="BY70" s="79"/>
+      <c r="BZ70" s="79"/>
+      <c r="CA70" s="79"/>
+      <c r="CB70" s="79"/>
+      <c r="CC70" s="79"/>
+      <c r="CD70" s="79"/>
+      <c r="CE70" s="79"/>
+      <c r="CF70" s="79"/>
+      <c r="CG70" s="79"/>
+      <c r="CH70" s="79"/>
+      <c r="CI70" s="79"/>
+      <c r="CJ70" s="79"/>
+      <c r="CK70" s="79"/>
+      <c r="CL70" s="79"/>
+      <c r="CM70" s="79"/>
+      <c r="CN70" s="79"/>
+      <c r="CO70" s="79"/>
+      <c r="CP70" s="79"/>
+      <c r="CQ70" s="79"/>
+      <c r="CR70" s="79"/>
+      <c r="CS70" s="79"/>
+      <c r="CT70" s="79"/>
+      <c r="CU70" s="79"/>
+      <c r="CV70" s="79"/>
+      <c r="CW70" s="79"/>
+      <c r="CX70" s="79"/>
+      <c r="CY70" s="79"/>
+      <c r="CZ70" s="79"/>
+      <c r="DA70" s="79"/>
+      <c r="DB70" s="79"/>
+      <c r="DC70" s="79"/>
+      <c r="DD70" s="79"/>
+      <c r="DE70" s="79"/>
+      <c r="DF70" s="79"/>
+      <c r="DG70" s="79"/>
+      <c r="DH70" s="79"/>
+      <c r="DI70" s="79"/>
+      <c r="DJ70" s="79"/>
+      <c r="DK70" s="79"/>
+      <c r="DL70" s="79"/>
+      <c r="DM70" s="79"/>
+      <c r="DN70" s="79"/>
+      <c r="DO70" s="79"/>
+      <c r="DP70" s="79"/>
+      <c r="DQ70" s="79"/>
+      <c r="DR70" s="79"/>
+      <c r="DS70" s="79"/>
+      <c r="DT70" s="79"/>
+      <c r="DU70" s="79"/>
+      <c r="DV70" s="79"/>
+      <c r="DW70" s="79"/>
+      <c r="DX70" s="79"/>
+      <c r="DY70" s="79"/>
+      <c r="DZ70" s="79"/>
+      <c r="EA70" s="79"/>
+      <c r="EB70" s="79"/>
+      <c r="EC70" s="79"/>
+      <c r="ED70" s="79"/>
+      <c r="EE70" s="79"/>
+      <c r="EF70" s="79"/>
+      <c r="EG70" s="79"/>
+      <c r="EH70" s="79"/>
+      <c r="EI70" s="79"/>
+      <c r="EJ70" s="79"/>
+      <c r="EK70" s="79"/>
+      <c r="EL70" s="79"/>
+      <c r="EM70" s="79"/>
+      <c r="EN70" s="79"/>
+      <c r="EO70" s="79"/>
+      <c r="EP70" s="79"/>
+      <c r="EQ70" s="79"/>
+      <c r="ER70" s="79"/>
+      <c r="ES70" s="79"/>
+      <c r="ET70" s="79"/>
+      <c r="EU70" s="79"/>
+      <c r="EV70" s="79"/>
+      <c r="EW70" s="79"/>
+      <c r="EX70" s="79"/>
+      <c r="EY70" s="79"/>
+      <c r="EZ70" s="79"/>
+      <c r="FA70" s="79"/>
+      <c r="FB70" s="79"/>
+      <c r="FC70" s="79"/>
+      <c r="FD70" s="79"/>
+      <c r="FE70" s="79"/>
+      <c r="FF70" s="79"/>
+      <c r="FG70" s="79"/>
+      <c r="FH70" s="79"/>
+      <c r="FI70" s="79"/>
+      <c r="FJ70" s="79"/>
+      <c r="FK70" s="79"/>
+      <c r="FL70" s="79"/>
+      <c r="FM70" s="79"/>
+      <c r="FN70" s="79"/>
+      <c r="FO70" s="79"/>
+      <c r="FP70" s="79"/>
+      <c r="FQ70" s="79"/>
+      <c r="FR70" s="79"/>
+      <c r="FS70" s="79"/>
+      <c r="FT70" s="79"/>
+      <c r="FU70" s="79"/>
+      <c r="FV70" s="79"/>
+      <c r="FW70" s="79"/>
+      <c r="FX70" s="79"/>
+      <c r="FY70" s="79"/>
+      <c r="FZ70" s="79"/>
+      <c r="GA70" s="79"/>
+      <c r="GB70" s="79"/>
+      <c r="GC70" s="79"/>
+      <c r="GD70" s="79"/>
+      <c r="GE70" s="79"/>
+      <c r="GF70" s="79"/>
+      <c r="GG70" s="79"/>
+      <c r="GH70" s="79"/>
+      <c r="GI70" s="79"/>
+      <c r="GJ70" s="79"/>
+      <c r="GK70" s="79"/>
+      <c r="GL70" s="79"/>
+      <c r="GM70" s="79"/>
+      <c r="GN70" s="79"/>
+      <c r="GO70" s="79"/>
+      <c r="GP70" s="79"/>
+      <c r="GQ70" s="79"/>
+      <c r="GR70" s="79"/>
+      <c r="GS70" s="79"/>
+      <c r="GT70" s="79"/>
+      <c r="GU70" s="79"/>
+      <c r="GV70" s="79"/>
+      <c r="GW70" s="79"/>
+      <c r="GX70" s="79"/>
+      <c r="GY70" s="79"/>
+      <c r="GZ70" s="79"/>
+      <c r="HA70" s="79"/>
+      <c r="HB70" s="79"/>
+      <c r="HC70" s="79"/>
+      <c r="HD70" s="79"/>
+      <c r="HE70" s="79"/>
+      <c r="HF70" s="79"/>
+      <c r="HG70" s="79"/>
+      <c r="HH70" s="79"/>
+      <c r="HI70" s="79"/>
+      <c r="HJ70" s="79"/>
+      <c r="HK70" s="79"/>
+      <c r="HL70" s="79"/>
+      <c r="HM70" s="79"/>
+      <c r="HN70" s="79"/>
+      <c r="HO70" s="79"/>
+      <c r="HP70" s="79"/>
+      <c r="HQ70" s="79"/>
+      <c r="HR70" s="79"/>
+      <c r="HS70" s="79"/>
+      <c r="HT70" s="79"/>
+      <c r="HU70" s="79"/>
+      <c r="HV70" s="79"/>
+      <c r="HW70" s="79"/>
+      <c r="HX70" s="79"/>
+      <c r="HY70" s="79"/>
+      <c r="HZ70" s="79"/>
+      <c r="IA70" s="79"/>
+      <c r="IB70" s="79"/>
+      <c r="IC70" s="79"/>
+      <c r="ID70" s="79"/>
+      <c r="IE70" s="79"/>
+      <c r="IF70" s="79"/>
+      <c r="IG70" s="79"/>
+      <c r="IH70" s="79"/>
+      <c r="II70" s="79"/>
+      <c r="IJ70" s="79"/>
+      <c r="IK70" s="79"/>
+      <c r="IL70" s="79"/>
+      <c r="IM70" s="79"/>
+      <c r="IN70" s="79"/>
+      <c r="IO70" s="79"/>
+      <c r="IP70" s="79"/>
+      <c r="IQ70" s="79"/>
+      <c r="IR70" s="79"/>
+      <c r="IS70" s="79"/>
+      <c r="IT70" s="79"/>
+      <c r="IU70" s="79"/>
+      <c r="IV70" s="79"/>
+      <c r="IW70" s="79"/>
+    </row>
+    <row r="71" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="77" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C71" s="78" t="s">
+        <v>162</v>
+      </c>
+      <c r="D71" s="78"/>
+      <c r="E71" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F71" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G71" s="78">
+        <v>0</v>
+      </c>
+      <c r="H71" s="78">
+        <v>1</v>
+      </c>
+      <c r="I71" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J71" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K71" s="79"/>
+      <c r="L71" s="79"/>
+      <c r="M71" s="79"/>
+      <c r="N71" s="79"/>
+      <c r="O71" s="79"/>
+      <c r="P71" s="79"/>
+      <c r="Q71" s="79"/>
+      <c r="R71" s="79"/>
+      <c r="S71" s="79"/>
+      <c r="T71" s="79"/>
+      <c r="U71" s="79"/>
+      <c r="V71" s="79"/>
+      <c r="W71" s="79"/>
+      <c r="X71" s="79"/>
+      <c r="Y71" s="79"/>
+      <c r="Z71" s="79"/>
+      <c r="AA71" s="79"/>
+      <c r="AB71" s="79"/>
+      <c r="AC71" s="79"/>
+      <c r="AD71" s="79"/>
+      <c r="AE71" s="79"/>
+      <c r="AF71" s="79"/>
+      <c r="AG71" s="79"/>
+      <c r="AH71" s="79"/>
+      <c r="AI71" s="79"/>
+      <c r="AJ71" s="79"/>
+      <c r="AK71" s="79"/>
+      <c r="AL71" s="79"/>
+      <c r="AM71" s="79"/>
+      <c r="AN71" s="79"/>
+      <c r="AO71" s="79"/>
+      <c r="AP71" s="79"/>
+      <c r="AQ71" s="79"/>
+      <c r="AR71" s="79"/>
+      <c r="AS71" s="79"/>
+      <c r="AT71" s="79"/>
+      <c r="AU71" s="79"/>
+      <c r="AV71" s="79"/>
+      <c r="AW71" s="79"/>
+      <c r="AX71" s="79"/>
+      <c r="AY71" s="79"/>
+      <c r="AZ71" s="79"/>
+      <c r="BA71" s="79"/>
+      <c r="BB71" s="79"/>
+      <c r="BC71" s="79"/>
+      <c r="BD71" s="79"/>
+      <c r="BE71" s="79"/>
+      <c r="BF71" s="79"/>
+      <c r="BG71" s="79"/>
+      <c r="BH71" s="79"/>
+      <c r="BI71" s="79"/>
+      <c r="BJ71" s="79"/>
+      <c r="BK71" s="79"/>
+      <c r="BL71" s="79"/>
+      <c r="BM71" s="79"/>
+      <c r="BN71" s="79"/>
+      <c r="BO71" s="79"/>
+      <c r="BP71" s="79"/>
+      <c r="BQ71" s="79"/>
+      <c r="BR71" s="79"/>
+      <c r="BS71" s="79"/>
+      <c r="BT71" s="79"/>
+      <c r="BU71" s="79"/>
+      <c r="BV71" s="79"/>
+      <c r="BW71" s="79"/>
+      <c r="BX71" s="79"/>
+      <c r="BY71" s="79"/>
+      <c r="BZ71" s="79"/>
+      <c r="CA71" s="79"/>
+      <c r="CB71" s="79"/>
+      <c r="CC71" s="79"/>
+      <c r="CD71" s="79"/>
+      <c r="CE71" s="79"/>
+      <c r="CF71" s="79"/>
+      <c r="CG71" s="79"/>
+      <c r="CH71" s="79"/>
+      <c r="CI71" s="79"/>
+      <c r="CJ71" s="79"/>
+      <c r="CK71" s="79"/>
+      <c r="CL71" s="79"/>
+      <c r="CM71" s="79"/>
+      <c r="CN71" s="79"/>
+      <c r="CO71" s="79"/>
+      <c r="CP71" s="79"/>
+      <c r="CQ71" s="79"/>
+      <c r="CR71" s="79"/>
+      <c r="CS71" s="79"/>
+      <c r="CT71" s="79"/>
+      <c r="CU71" s="79"/>
+      <c r="CV71" s="79"/>
+      <c r="CW71" s="79"/>
+      <c r="CX71" s="79"/>
+      <c r="CY71" s="79"/>
+      <c r="CZ71" s="79"/>
+      <c r="DA71" s="79"/>
+      <c r="DB71" s="79"/>
+      <c r="DC71" s="79"/>
+      <c r="DD71" s="79"/>
+      <c r="DE71" s="79"/>
+      <c r="DF71" s="79"/>
+      <c r="DG71" s="79"/>
+      <c r="DH71" s="79"/>
+      <c r="DI71" s="79"/>
+      <c r="DJ71" s="79"/>
+      <c r="DK71" s="79"/>
+      <c r="DL71" s="79"/>
+      <c r="DM71" s="79"/>
+      <c r="DN71" s="79"/>
+      <c r="DO71" s="79"/>
+      <c r="DP71" s="79"/>
+      <c r="DQ71" s="79"/>
+      <c r="DR71" s="79"/>
+      <c r="DS71" s="79"/>
+      <c r="DT71" s="79"/>
+      <c r="DU71" s="79"/>
+      <c r="DV71" s="79"/>
+      <c r="DW71" s="79"/>
+      <c r="DX71" s="79"/>
+      <c r="DY71" s="79"/>
+      <c r="DZ71" s="79"/>
+      <c r="EA71" s="79"/>
+      <c r="EB71" s="79"/>
+      <c r="EC71" s="79"/>
+      <c r="ED71" s="79"/>
+      <c r="EE71" s="79"/>
+      <c r="EF71" s="79"/>
+      <c r="EG71" s="79"/>
+      <c r="EH71" s="79"/>
+      <c r="EI71" s="79"/>
+      <c r="EJ71" s="79"/>
+      <c r="EK71" s="79"/>
+      <c r="EL71" s="79"/>
+      <c r="EM71" s="79"/>
+      <c r="EN71" s="79"/>
+      <c r="EO71" s="79"/>
+      <c r="EP71" s="79"/>
+      <c r="EQ71" s="79"/>
+      <c r="ER71" s="79"/>
+      <c r="ES71" s="79"/>
+      <c r="ET71" s="79"/>
+      <c r="EU71" s="79"/>
+      <c r="EV71" s="79"/>
+      <c r="EW71" s="79"/>
+      <c r="EX71" s="79"/>
+      <c r="EY71" s="79"/>
+      <c r="EZ71" s="79"/>
+      <c r="FA71" s="79"/>
+      <c r="FB71" s="79"/>
+      <c r="FC71" s="79"/>
+      <c r="FD71" s="79"/>
+      <c r="FE71" s="79"/>
+      <c r="FF71" s="79"/>
+      <c r="FG71" s="79"/>
+      <c r="FH71" s="79"/>
+      <c r="FI71" s="79"/>
+      <c r="FJ71" s="79"/>
+      <c r="FK71" s="79"/>
+      <c r="FL71" s="79"/>
+      <c r="FM71" s="79"/>
+      <c r="FN71" s="79"/>
+      <c r="FO71" s="79"/>
+      <c r="FP71" s="79"/>
+      <c r="FQ71" s="79"/>
+      <c r="FR71" s="79"/>
+      <c r="FS71" s="79"/>
+      <c r="FT71" s="79"/>
+      <c r="FU71" s="79"/>
+      <c r="FV71" s="79"/>
+      <c r="FW71" s="79"/>
+      <c r="FX71" s="79"/>
+      <c r="FY71" s="79"/>
+      <c r="FZ71" s="79"/>
+      <c r="GA71" s="79"/>
+      <c r="GB71" s="79"/>
+      <c r="GC71" s="79"/>
+      <c r="GD71" s="79"/>
+      <c r="GE71" s="79"/>
+      <c r="GF71" s="79"/>
+      <c r="GG71" s="79"/>
+      <c r="GH71" s="79"/>
+      <c r="GI71" s="79"/>
+      <c r="GJ71" s="79"/>
+      <c r="GK71" s="79"/>
+      <c r="GL71" s="79"/>
+      <c r="GM71" s="79"/>
+      <c r="GN71" s="79"/>
+      <c r="GO71" s="79"/>
+      <c r="GP71" s="79"/>
+      <c r="GQ71" s="79"/>
+      <c r="GR71" s="79"/>
+      <c r="GS71" s="79"/>
+      <c r="GT71" s="79"/>
+      <c r="GU71" s="79"/>
+      <c r="GV71" s="79"/>
+      <c r="GW71" s="79"/>
+      <c r="GX71" s="79"/>
+      <c r="GY71" s="79"/>
+      <c r="GZ71" s="79"/>
+      <c r="HA71" s="79"/>
+      <c r="HB71" s="79"/>
+      <c r="HC71" s="79"/>
+      <c r="HD71" s="79"/>
+      <c r="HE71" s="79"/>
+      <c r="HF71" s="79"/>
+      <c r="HG71" s="79"/>
+      <c r="HH71" s="79"/>
+      <c r="HI71" s="79"/>
+      <c r="HJ71" s="79"/>
+      <c r="HK71" s="79"/>
+      <c r="HL71" s="79"/>
+      <c r="HM71" s="79"/>
+      <c r="HN71" s="79"/>
+      <c r="HO71" s="79"/>
+      <c r="HP71" s="79"/>
+      <c r="HQ71" s="79"/>
+      <c r="HR71" s="79"/>
+      <c r="HS71" s="79"/>
+      <c r="HT71" s="79"/>
+      <c r="HU71" s="79"/>
+      <c r="HV71" s="79"/>
+      <c r="HW71" s="79"/>
+      <c r="HX71" s="79"/>
+      <c r="HY71" s="79"/>
+      <c r="HZ71" s="79"/>
+      <c r="IA71" s="79"/>
+      <c r="IB71" s="79"/>
+      <c r="IC71" s="79"/>
+      <c r="ID71" s="79"/>
+      <c r="IE71" s="79"/>
+      <c r="IF71" s="79"/>
+      <c r="IG71" s="79"/>
+      <c r="IH71" s="79"/>
+      <c r="II71" s="79"/>
+      <c r="IJ71" s="79"/>
+      <c r="IK71" s="79"/>
+      <c r="IL71" s="79"/>
+      <c r="IM71" s="79"/>
+      <c r="IN71" s="79"/>
+      <c r="IO71" s="79"/>
+      <c r="IP71" s="79"/>
+      <c r="IQ71" s="79"/>
+      <c r="IR71" s="79"/>
+      <c r="IS71" s="79"/>
+      <c r="IT71" s="79"/>
+      <c r="IU71" s="79"/>
+      <c r="IV71" s="79"/>
+      <c r="IW71" s="79"/>
+    </row>
+    <row r="72" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" s="78" t="s">
+        <v>163</v>
+      </c>
+      <c r="D72" s="78"/>
+      <c r="E72" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F72" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G72" s="78">
+        <v>0</v>
+      </c>
+      <c r="H72" s="78">
+        <v>1</v>
+      </c>
+      <c r="I72" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J72" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K72" s="79"/>
+      <c r="L72" s="79"/>
+      <c r="M72" s="79"/>
+      <c r="N72" s="79"/>
+      <c r="O72" s="79"/>
+      <c r="P72" s="79"/>
+      <c r="Q72" s="79"/>
+      <c r="R72" s="79"/>
+      <c r="S72" s="79"/>
+      <c r="T72" s="79"/>
+      <c r="U72" s="79"/>
+      <c r="V72" s="79"/>
+      <c r="W72" s="79"/>
+      <c r="X72" s="79"/>
+      <c r="Y72" s="79"/>
+      <c r="Z72" s="79"/>
+      <c r="AA72" s="79"/>
+      <c r="AB72" s="79"/>
+      <c r="AC72" s="79"/>
+      <c r="AD72" s="79"/>
+      <c r="AE72" s="79"/>
+      <c r="AF72" s="79"/>
+      <c r="AG72" s="79"/>
+      <c r="AH72" s="79"/>
+      <c r="AI72" s="79"/>
+      <c r="AJ72" s="79"/>
+      <c r="AK72" s="79"/>
+      <c r="AL72" s="79"/>
+      <c r="AM72" s="79"/>
+      <c r="AN72" s="79"/>
+      <c r="AO72" s="79"/>
+      <c r="AP72" s="79"/>
+      <c r="AQ72" s="79"/>
+      <c r="AR72" s="79"/>
+      <c r="AS72" s="79"/>
+      <c r="AT72" s="79"/>
+      <c r="AU72" s="79"/>
+      <c r="AV72" s="79"/>
+      <c r="AW72" s="79"/>
+      <c r="AX72" s="79"/>
+      <c r="AY72" s="79"/>
+      <c r="AZ72" s="79"/>
+      <c r="BA72" s="79"/>
+      <c r="BB72" s="79"/>
+      <c r="BC72" s="79"/>
+      <c r="BD72" s="79"/>
+      <c r="BE72" s="79"/>
+      <c r="BF72" s="79"/>
+      <c r="BG72" s="79"/>
+      <c r="BH72" s="79"/>
+      <c r="BI72" s="79"/>
+      <c r="BJ72" s="79"/>
+      <c r="BK72" s="79"/>
+      <c r="BL72" s="79"/>
+      <c r="BM72" s="79"/>
+      <c r="BN72" s="79"/>
+      <c r="BO72" s="79"/>
+      <c r="BP72" s="79"/>
+      <c r="BQ72" s="79"/>
+      <c r="BR72" s="79"/>
+      <c r="BS72" s="79"/>
+      <c r="BT72" s="79"/>
+      <c r="BU72" s="79"/>
+      <c r="BV72" s="79"/>
+      <c r="BW72" s="79"/>
+      <c r="BX72" s="79"/>
+      <c r="BY72" s="79"/>
+      <c r="BZ72" s="79"/>
+      <c r="CA72" s="79"/>
+      <c r="CB72" s="79"/>
+      <c r="CC72" s="79"/>
+      <c r="CD72" s="79"/>
+      <c r="CE72" s="79"/>
+      <c r="CF72" s="79"/>
+      <c r="CG72" s="79"/>
+      <c r="CH72" s="79"/>
+      <c r="CI72" s="79"/>
+      <c r="CJ72" s="79"/>
+      <c r="CK72" s="79"/>
+      <c r="CL72" s="79"/>
+      <c r="CM72" s="79"/>
+      <c r="CN72" s="79"/>
+      <c r="CO72" s="79"/>
+      <c r="CP72" s="79"/>
+      <c r="CQ72" s="79"/>
+      <c r="CR72" s="79"/>
+      <c r="CS72" s="79"/>
+      <c r="CT72" s="79"/>
+      <c r="CU72" s="79"/>
+      <c r="CV72" s="79"/>
+      <c r="CW72" s="79"/>
+      <c r="CX72" s="79"/>
+      <c r="CY72" s="79"/>
+      <c r="CZ72" s="79"/>
+      <c r="DA72" s="79"/>
+      <c r="DB72" s="79"/>
+      <c r="DC72" s="79"/>
+      <c r="DD72" s="79"/>
+      <c r="DE72" s="79"/>
+      <c r="DF72" s="79"/>
+      <c r="DG72" s="79"/>
+      <c r="DH72" s="79"/>
+      <c r="DI72" s="79"/>
+      <c r="DJ72" s="79"/>
+      <c r="DK72" s="79"/>
+      <c r="DL72" s="79"/>
+      <c r="DM72" s="79"/>
+      <c r="DN72" s="79"/>
+      <c r="DO72" s="79"/>
+      <c r="DP72" s="79"/>
+      <c r="DQ72" s="79"/>
+      <c r="DR72" s="79"/>
+      <c r="DS72" s="79"/>
+      <c r="DT72" s="79"/>
+      <c r="DU72" s="79"/>
+      <c r="DV72" s="79"/>
+      <c r="DW72" s="79"/>
+      <c r="DX72" s="79"/>
+      <c r="DY72" s="79"/>
+      <c r="DZ72" s="79"/>
+      <c r="EA72" s="79"/>
+      <c r="EB72" s="79"/>
+      <c r="EC72" s="79"/>
+      <c r="ED72" s="79"/>
+      <c r="EE72" s="79"/>
+      <c r="EF72" s="79"/>
+      <c r="EG72" s="79"/>
+      <c r="EH72" s="79"/>
+      <c r="EI72" s="79"/>
+      <c r="EJ72" s="79"/>
+      <c r="EK72" s="79"/>
+      <c r="EL72" s="79"/>
+      <c r="EM72" s="79"/>
+      <c r="EN72" s="79"/>
+      <c r="EO72" s="79"/>
+      <c r="EP72" s="79"/>
+      <c r="EQ72" s="79"/>
+      <c r="ER72" s="79"/>
+      <c r="ES72" s="79"/>
+      <c r="ET72" s="79"/>
+      <c r="EU72" s="79"/>
+      <c r="EV72" s="79"/>
+      <c r="EW72" s="79"/>
+      <c r="EX72" s="79"/>
+      <c r="EY72" s="79"/>
+      <c r="EZ72" s="79"/>
+      <c r="FA72" s="79"/>
+      <c r="FB72" s="79"/>
+      <c r="FC72" s="79"/>
+      <c r="FD72" s="79"/>
+      <c r="FE72" s="79"/>
+      <c r="FF72" s="79"/>
+      <c r="FG72" s="79"/>
+      <c r="FH72" s="79"/>
+      <c r="FI72" s="79"/>
+      <c r="FJ72" s="79"/>
+      <c r="FK72" s="79"/>
+      <c r="FL72" s="79"/>
+      <c r="FM72" s="79"/>
+      <c r="FN72" s="79"/>
+      <c r="FO72" s="79"/>
+      <c r="FP72" s="79"/>
+      <c r="FQ72" s="79"/>
+      <c r="FR72" s="79"/>
+      <c r="FS72" s="79"/>
+      <c r="FT72" s="79"/>
+      <c r="FU72" s="79"/>
+      <c r="FV72" s="79"/>
+      <c r="FW72" s="79"/>
+      <c r="FX72" s="79"/>
+      <c r="FY72" s="79"/>
+      <c r="FZ72" s="79"/>
+      <c r="GA72" s="79"/>
+      <c r="GB72" s="79"/>
+      <c r="GC72" s="79"/>
+      <c r="GD72" s="79"/>
+      <c r="GE72" s="79"/>
+      <c r="GF72" s="79"/>
+      <c r="GG72" s="79"/>
+      <c r="GH72" s="79"/>
+      <c r="GI72" s="79"/>
+      <c r="GJ72" s="79"/>
+      <c r="GK72" s="79"/>
+      <c r="GL72" s="79"/>
+      <c r="GM72" s="79"/>
+      <c r="GN72" s="79"/>
+      <c r="GO72" s="79"/>
+      <c r="GP72" s="79"/>
+      <c r="GQ72" s="79"/>
+      <c r="GR72" s="79"/>
+      <c r="GS72" s="79"/>
+      <c r="GT72" s="79"/>
+      <c r="GU72" s="79"/>
+      <c r="GV72" s="79"/>
+      <c r="GW72" s="79"/>
+      <c r="GX72" s="79"/>
+      <c r="GY72" s="79"/>
+      <c r="GZ72" s="79"/>
+      <c r="HA72" s="79"/>
+      <c r="HB72" s="79"/>
+      <c r="HC72" s="79"/>
+      <c r="HD72" s="79"/>
+      <c r="HE72" s="79"/>
+      <c r="HF72" s="79"/>
+      <c r="HG72" s="79"/>
+      <c r="HH72" s="79"/>
+      <c r="HI72" s="79"/>
+      <c r="HJ72" s="79"/>
+      <c r="HK72" s="79"/>
+      <c r="HL72" s="79"/>
+      <c r="HM72" s="79"/>
+      <c r="HN72" s="79"/>
+      <c r="HO72" s="79"/>
+      <c r="HP72" s="79"/>
+      <c r="HQ72" s="79"/>
+      <c r="HR72" s="79"/>
+      <c r="HS72" s="79"/>
+      <c r="HT72" s="79"/>
+      <c r="HU72" s="79"/>
+      <c r="HV72" s="79"/>
+      <c r="HW72" s="79"/>
+      <c r="HX72" s="79"/>
+      <c r="HY72" s="79"/>
+      <c r="HZ72" s="79"/>
+      <c r="IA72" s="79"/>
+      <c r="IB72" s="79"/>
+      <c r="IC72" s="79"/>
+      <c r="ID72" s="79"/>
+      <c r="IE72" s="79"/>
+      <c r="IF72" s="79"/>
+      <c r="IG72" s="79"/>
+      <c r="IH72" s="79"/>
+      <c r="II72" s="79"/>
+      <c r="IJ72" s="79"/>
+      <c r="IK72" s="79"/>
+      <c r="IL72" s="79"/>
+      <c r="IM72" s="79"/>
+      <c r="IN72" s="79"/>
+      <c r="IO72" s="79"/>
+      <c r="IP72" s="79"/>
+      <c r="IQ72" s="79"/>
+      <c r="IR72" s="79"/>
+      <c r="IS72" s="79"/>
+      <c r="IT72" s="79"/>
+      <c r="IU72" s="79"/>
+      <c r="IV72" s="79"/>
+      <c r="IW72" s="79"/>
+    </row>
+    <row r="73" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="77" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="78" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" s="78"/>
+      <c r="E73" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F73" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G73" s="78">
+        <v>0</v>
+      </c>
+      <c r="H73" s="78">
+        <v>1</v>
+      </c>
+      <c r="I73" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J73" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K73" s="79"/>
+      <c r="L73" s="79"/>
+      <c r="M73" s="79"/>
+      <c r="N73" s="79"/>
+      <c r="O73" s="79"/>
+      <c r="P73" s="79"/>
+      <c r="Q73" s="79"/>
+      <c r="R73" s="79"/>
+      <c r="S73" s="79"/>
+      <c r="T73" s="79"/>
+      <c r="U73" s="79"/>
+      <c r="V73" s="79"/>
+      <c r="W73" s="79"/>
+      <c r="X73" s="79"/>
+      <c r="Y73" s="79"/>
+      <c r="Z73" s="79"/>
+      <c r="AA73" s="79"/>
+      <c r="AB73" s="79"/>
+      <c r="AC73" s="79"/>
+      <c r="AD73" s="79"/>
+      <c r="AE73" s="79"/>
+      <c r="AF73" s="79"/>
+      <c r="AG73" s="79"/>
+      <c r="AH73" s="79"/>
+      <c r="AI73" s="79"/>
+      <c r="AJ73" s="79"/>
+      <c r="AK73" s="79"/>
+      <c r="AL73" s="79"/>
+      <c r="AM73" s="79"/>
+      <c r="AN73" s="79"/>
+      <c r="AO73" s="79"/>
+      <c r="AP73" s="79"/>
+      <c r="AQ73" s="79"/>
+      <c r="AR73" s="79"/>
+      <c r="AS73" s="79"/>
+      <c r="AT73" s="79"/>
+      <c r="AU73" s="79"/>
+      <c r="AV73" s="79"/>
+      <c r="AW73" s="79"/>
+      <c r="AX73" s="79"/>
+      <c r="AY73" s="79"/>
+      <c r="AZ73" s="79"/>
+      <c r="BA73" s="79"/>
+      <c r="BB73" s="79"/>
+      <c r="BC73" s="79"/>
+      <c r="BD73" s="79"/>
+      <c r="BE73" s="79"/>
+      <c r="BF73" s="79"/>
+      <c r="BG73" s="79"/>
+      <c r="BH73" s="79"/>
+      <c r="BI73" s="79"/>
+      <c r="BJ73" s="79"/>
+      <c r="BK73" s="79"/>
+      <c r="BL73" s="79"/>
+      <c r="BM73" s="79"/>
+      <c r="BN73" s="79"/>
+      <c r="BO73" s="79"/>
+      <c r="BP73" s="79"/>
+      <c r="BQ73" s="79"/>
+      <c r="BR73" s="79"/>
+      <c r="BS73" s="79"/>
+      <c r="BT73" s="79"/>
+      <c r="BU73" s="79"/>
+      <c r="BV73" s="79"/>
+      <c r="BW73" s="79"/>
+      <c r="BX73" s="79"/>
+      <c r="BY73" s="79"/>
+      <c r="BZ73" s="79"/>
+      <c r="CA73" s="79"/>
+      <c r="CB73" s="79"/>
+      <c r="CC73" s="79"/>
+      <c r="CD73" s="79"/>
+      <c r="CE73" s="79"/>
+      <c r="CF73" s="79"/>
+      <c r="CG73" s="79"/>
+      <c r="CH73" s="79"/>
+      <c r="CI73" s="79"/>
+      <c r="CJ73" s="79"/>
+      <c r="CK73" s="79"/>
+      <c r="CL73" s="79"/>
+      <c r="CM73" s="79"/>
+      <c r="CN73" s="79"/>
+      <c r="CO73" s="79"/>
+      <c r="CP73" s="79"/>
+      <c r="CQ73" s="79"/>
+      <c r="CR73" s="79"/>
+      <c r="CS73" s="79"/>
+      <c r="CT73" s="79"/>
+      <c r="CU73" s="79"/>
+      <c r="CV73" s="79"/>
+      <c r="CW73" s="79"/>
+      <c r="CX73" s="79"/>
+      <c r="CY73" s="79"/>
+      <c r="CZ73" s="79"/>
+      <c r="DA73" s="79"/>
+      <c r="DB73" s="79"/>
+      <c r="DC73" s="79"/>
+      <c r="DD73" s="79"/>
+      <c r="DE73" s="79"/>
+      <c r="DF73" s="79"/>
+      <c r="DG73" s="79"/>
+      <c r="DH73" s="79"/>
+      <c r="DI73" s="79"/>
+      <c r="DJ73" s="79"/>
+      <c r="DK73" s="79"/>
+      <c r="DL73" s="79"/>
+      <c r="DM73" s="79"/>
+      <c r="DN73" s="79"/>
+      <c r="DO73" s="79"/>
+      <c r="DP73" s="79"/>
+      <c r="DQ73" s="79"/>
+      <c r="DR73" s="79"/>
+      <c r="DS73" s="79"/>
+      <c r="DT73" s="79"/>
+      <c r="DU73" s="79"/>
+      <c r="DV73" s="79"/>
+      <c r="DW73" s="79"/>
+      <c r="DX73" s="79"/>
+      <c r="DY73" s="79"/>
+      <c r="DZ73" s="79"/>
+      <c r="EA73" s="79"/>
+      <c r="EB73" s="79"/>
+      <c r="EC73" s="79"/>
+      <c r="ED73" s="79"/>
+      <c r="EE73" s="79"/>
+      <c r="EF73" s="79"/>
+      <c r="EG73" s="79"/>
+      <c r="EH73" s="79"/>
+      <c r="EI73" s="79"/>
+      <c r="EJ73" s="79"/>
+      <c r="EK73" s="79"/>
+      <c r="EL73" s="79"/>
+      <c r="EM73" s="79"/>
+      <c r="EN73" s="79"/>
+      <c r="EO73" s="79"/>
+      <c r="EP73" s="79"/>
+      <c r="EQ73" s="79"/>
+      <c r="ER73" s="79"/>
+      <c r="ES73" s="79"/>
+      <c r="ET73" s="79"/>
+      <c r="EU73" s="79"/>
+      <c r="EV73" s="79"/>
+      <c r="EW73" s="79"/>
+      <c r="EX73" s="79"/>
+      <c r="EY73" s="79"/>
+      <c r="EZ73" s="79"/>
+      <c r="FA73" s="79"/>
+      <c r="FB73" s="79"/>
+      <c r="FC73" s="79"/>
+      <c r="FD73" s="79"/>
+      <c r="FE73" s="79"/>
+      <c r="FF73" s="79"/>
+      <c r="FG73" s="79"/>
+      <c r="FH73" s="79"/>
+      <c r="FI73" s="79"/>
+      <c r="FJ73" s="79"/>
+      <c r="FK73" s="79"/>
+      <c r="FL73" s="79"/>
+      <c r="FM73" s="79"/>
+      <c r="FN73" s="79"/>
+      <c r="FO73" s="79"/>
+      <c r="FP73" s="79"/>
+      <c r="FQ73" s="79"/>
+      <c r="FR73" s="79"/>
+      <c r="FS73" s="79"/>
+      <c r="FT73" s="79"/>
+      <c r="FU73" s="79"/>
+      <c r="FV73" s="79"/>
+      <c r="FW73" s="79"/>
+      <c r="FX73" s="79"/>
+      <c r="FY73" s="79"/>
+      <c r="FZ73" s="79"/>
+      <c r="GA73" s="79"/>
+      <c r="GB73" s="79"/>
+      <c r="GC73" s="79"/>
+      <c r="GD73" s="79"/>
+      <c r="GE73" s="79"/>
+      <c r="GF73" s="79"/>
+      <c r="GG73" s="79"/>
+      <c r="GH73" s="79"/>
+      <c r="GI73" s="79"/>
+      <c r="GJ73" s="79"/>
+      <c r="GK73" s="79"/>
+      <c r="GL73" s="79"/>
+      <c r="GM73" s="79"/>
+      <c r="GN73" s="79"/>
+      <c r="GO73" s="79"/>
+      <c r="GP73" s="79"/>
+      <c r="GQ73" s="79"/>
+      <c r="GR73" s="79"/>
+      <c r="GS73" s="79"/>
+      <c r="GT73" s="79"/>
+      <c r="GU73" s="79"/>
+      <c r="GV73" s="79"/>
+      <c r="GW73" s="79"/>
+      <c r="GX73" s="79"/>
+      <c r="GY73" s="79"/>
+      <c r="GZ73" s="79"/>
+      <c r="HA73" s="79"/>
+      <c r="HB73" s="79"/>
+      <c r="HC73" s="79"/>
+      <c r="HD73" s="79"/>
+      <c r="HE73" s="79"/>
+      <c r="HF73" s="79"/>
+      <c r="HG73" s="79"/>
+      <c r="HH73" s="79"/>
+      <c r="HI73" s="79"/>
+      <c r="HJ73" s="79"/>
+      <c r="HK73" s="79"/>
+      <c r="HL73" s="79"/>
+      <c r="HM73" s="79"/>
+      <c r="HN73" s="79"/>
+      <c r="HO73" s="79"/>
+      <c r="HP73" s="79"/>
+      <c r="HQ73" s="79"/>
+      <c r="HR73" s="79"/>
+      <c r="HS73" s="79"/>
+      <c r="HT73" s="79"/>
+      <c r="HU73" s="79"/>
+      <c r="HV73" s="79"/>
+      <c r="HW73" s="79"/>
+      <c r="HX73" s="79"/>
+      <c r="HY73" s="79"/>
+      <c r="HZ73" s="79"/>
+      <c r="IA73" s="79"/>
+      <c r="IB73" s="79"/>
+      <c r="IC73" s="79"/>
+      <c r="ID73" s="79"/>
+      <c r="IE73" s="79"/>
+      <c r="IF73" s="79"/>
+      <c r="IG73" s="79"/>
+      <c r="IH73" s="79"/>
+      <c r="II73" s="79"/>
+      <c r="IJ73" s="79"/>
+      <c r="IK73" s="79"/>
+      <c r="IL73" s="79"/>
+      <c r="IM73" s="79"/>
+      <c r="IN73" s="79"/>
+      <c r="IO73" s="79"/>
+      <c r="IP73" s="79"/>
+      <c r="IQ73" s="79"/>
+      <c r="IR73" s="79"/>
+      <c r="IS73" s="79"/>
+      <c r="IT73" s="79"/>
+      <c r="IU73" s="79"/>
+      <c r="IV73" s="79"/>
+      <c r="IW73" s="79"/>
+    </row>
+    <row r="74" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C74" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F74" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G74" s="78">
+        <v>0</v>
+      </c>
+      <c r="H74" s="78">
+        <v>1</v>
+      </c>
+      <c r="I74" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J74" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="79"/>
+      <c r="O74" s="79"/>
+      <c r="P74" s="79"/>
+      <c r="Q74" s="79"/>
+      <c r="R74" s="79"/>
+      <c r="S74" s="79"/>
+      <c r="T74" s="79"/>
+      <c r="U74" s="79"/>
+      <c r="V74" s="79"/>
+      <c r="W74" s="79"/>
+      <c r="X74" s="79"/>
+      <c r="Y74" s="79"/>
+      <c r="Z74" s="79"/>
+      <c r="AA74" s="79"/>
+      <c r="AB74" s="79"/>
+      <c r="AC74" s="79"/>
+      <c r="AD74" s="79"/>
+      <c r="AE74" s="79"/>
+      <c r="AF74" s="79"/>
+      <c r="AG74" s="79"/>
+      <c r="AH74" s="79"/>
+      <c r="AI74" s="79"/>
+      <c r="AJ74" s="79"/>
+      <c r="AK74" s="79"/>
+      <c r="AL74" s="79"/>
+      <c r="AM74" s="79"/>
+      <c r="AN74" s="79"/>
+      <c r="AO74" s="79"/>
+      <c r="AP74" s="79"/>
+      <c r="AQ74" s="79"/>
+      <c r="AR74" s="79"/>
+      <c r="AS74" s="79"/>
+      <c r="AT74" s="79"/>
+      <c r="AU74" s="79"/>
+      <c r="AV74" s="79"/>
+      <c r="AW74" s="79"/>
+      <c r="AX74" s="79"/>
+      <c r="AY74" s="79"/>
+      <c r="AZ74" s="79"/>
+      <c r="BA74" s="79"/>
+      <c r="BB74" s="79"/>
+      <c r="BC74" s="79"/>
+      <c r="BD74" s="79"/>
+      <c r="BE74" s="79"/>
+      <c r="BF74" s="79"/>
+      <c r="BG74" s="79"/>
+      <c r="BH74" s="79"/>
+      <c r="BI74" s="79"/>
+      <c r="BJ74" s="79"/>
+      <c r="BK74" s="79"/>
+      <c r="BL74" s="79"/>
+      <c r="BM74" s="79"/>
+      <c r="BN74" s="79"/>
+      <c r="BO74" s="79"/>
+      <c r="BP74" s="79"/>
+      <c r="BQ74" s="79"/>
+      <c r="BR74" s="79"/>
+      <c r="BS74" s="79"/>
+      <c r="BT74" s="79"/>
+      <c r="BU74" s="79"/>
+      <c r="BV74" s="79"/>
+      <c r="BW74" s="79"/>
+      <c r="BX74" s="79"/>
+      <c r="BY74" s="79"/>
+      <c r="BZ74" s="79"/>
+      <c r="CA74" s="79"/>
+      <c r="CB74" s="79"/>
+      <c r="CC74" s="79"/>
+      <c r="CD74" s="79"/>
+      <c r="CE74" s="79"/>
+      <c r="CF74" s="79"/>
+      <c r="CG74" s="79"/>
+      <c r="CH74" s="79"/>
+      <c r="CI74" s="79"/>
+      <c r="CJ74" s="79"/>
+      <c r="CK74" s="79"/>
+      <c r="CL74" s="79"/>
+      <c r="CM74" s="79"/>
+      <c r="CN74" s="79"/>
+      <c r="CO74" s="79"/>
+      <c r="CP74" s="79"/>
+      <c r="CQ74" s="79"/>
+      <c r="CR74" s="79"/>
+      <c r="CS74" s="79"/>
+      <c r="CT74" s="79"/>
+      <c r="CU74" s="79"/>
+      <c r="CV74" s="79"/>
+      <c r="CW74" s="79"/>
+      <c r="CX74" s="79"/>
+      <c r="CY74" s="79"/>
+      <c r="CZ74" s="79"/>
+      <c r="DA74" s="79"/>
+      <c r="DB74" s="79"/>
+      <c r="DC74" s="79"/>
+      <c r="DD74" s="79"/>
+      <c r="DE74" s="79"/>
+      <c r="DF74" s="79"/>
+      <c r="DG74" s="79"/>
+      <c r="DH74" s="79"/>
+      <c r="DI74" s="79"/>
+      <c r="DJ74" s="79"/>
+      <c r="DK74" s="79"/>
+      <c r="DL74" s="79"/>
+      <c r="DM74" s="79"/>
+      <c r="DN74" s="79"/>
+      <c r="DO74" s="79"/>
+      <c r="DP74" s="79"/>
+      <c r="DQ74" s="79"/>
+      <c r="DR74" s="79"/>
+      <c r="DS74" s="79"/>
+      <c r="DT74" s="79"/>
+      <c r="DU74" s="79"/>
+      <c r="DV74" s="79"/>
+      <c r="DW74" s="79"/>
+      <c r="DX74" s="79"/>
+      <c r="DY74" s="79"/>
+      <c r="DZ74" s="79"/>
+      <c r="EA74" s="79"/>
+      <c r="EB74" s="79"/>
+      <c r="EC74" s="79"/>
+      <c r="ED74" s="79"/>
+      <c r="EE74" s="79"/>
+      <c r="EF74" s="79"/>
+      <c r="EG74" s="79"/>
+      <c r="EH74" s="79"/>
+      <c r="EI74" s="79"/>
+      <c r="EJ74" s="79"/>
+      <c r="EK74" s="79"/>
+      <c r="EL74" s="79"/>
+      <c r="EM74" s="79"/>
+      <c r="EN74" s="79"/>
+      <c r="EO74" s="79"/>
+      <c r="EP74" s="79"/>
+      <c r="EQ74" s="79"/>
+      <c r="ER74" s="79"/>
+      <c r="ES74" s="79"/>
+      <c r="ET74" s="79"/>
+      <c r="EU74" s="79"/>
+      <c r="EV74" s="79"/>
+      <c r="EW74" s="79"/>
+      <c r="EX74" s="79"/>
+      <c r="EY74" s="79"/>
+      <c r="EZ74" s="79"/>
+      <c r="FA74" s="79"/>
+      <c r="FB74" s="79"/>
+      <c r="FC74" s="79"/>
+      <c r="FD74" s="79"/>
+      <c r="FE74" s="79"/>
+      <c r="FF74" s="79"/>
+      <c r="FG74" s="79"/>
+      <c r="FH74" s="79"/>
+      <c r="FI74" s="79"/>
+      <c r="FJ74" s="79"/>
+      <c r="FK74" s="79"/>
+      <c r="FL74" s="79"/>
+      <c r="FM74" s="79"/>
+      <c r="FN74" s="79"/>
+      <c r="FO74" s="79"/>
+      <c r="FP74" s="79"/>
+      <c r="FQ74" s="79"/>
+      <c r="FR74" s="79"/>
+      <c r="FS74" s="79"/>
+      <c r="FT74" s="79"/>
+      <c r="FU74" s="79"/>
+      <c r="FV74" s="79"/>
+      <c r="FW74" s="79"/>
+      <c r="FX74" s="79"/>
+      <c r="FY74" s="79"/>
+      <c r="FZ74" s="79"/>
+      <c r="GA74" s="79"/>
+      <c r="GB74" s="79"/>
+      <c r="GC74" s="79"/>
+      <c r="GD74" s="79"/>
+      <c r="GE74" s="79"/>
+      <c r="GF74" s="79"/>
+      <c r="GG74" s="79"/>
+      <c r="GH74" s="79"/>
+      <c r="GI74" s="79"/>
+      <c r="GJ74" s="79"/>
+      <c r="GK74" s="79"/>
+      <c r="GL74" s="79"/>
+      <c r="GM74" s="79"/>
+      <c r="GN74" s="79"/>
+      <c r="GO74" s="79"/>
+      <c r="GP74" s="79"/>
+      <c r="GQ74" s="79"/>
+      <c r="GR74" s="79"/>
+      <c r="GS74" s="79"/>
+      <c r="GT74" s="79"/>
+      <c r="GU74" s="79"/>
+      <c r="GV74" s="79"/>
+      <c r="GW74" s="79"/>
+      <c r="GX74" s="79"/>
+      <c r="GY74" s="79"/>
+      <c r="GZ74" s="79"/>
+      <c r="HA74" s="79"/>
+      <c r="HB74" s="79"/>
+      <c r="HC74" s="79"/>
+      <c r="HD74" s="79"/>
+      <c r="HE74" s="79"/>
+      <c r="HF74" s="79"/>
+      <c r="HG74" s="79"/>
+      <c r="HH74" s="79"/>
+      <c r="HI74" s="79"/>
+      <c r="HJ74" s="79"/>
+      <c r="HK74" s="79"/>
+      <c r="HL74" s="79"/>
+      <c r="HM74" s="79"/>
+      <c r="HN74" s="79"/>
+      <c r="HO74" s="79"/>
+      <c r="HP74" s="79"/>
+      <c r="HQ74" s="79"/>
+      <c r="HR74" s="79"/>
+      <c r="HS74" s="79"/>
+      <c r="HT74" s="79"/>
+      <c r="HU74" s="79"/>
+      <c r="HV74" s="79"/>
+      <c r="HW74" s="79"/>
+      <c r="HX74" s="79"/>
+      <c r="HY74" s="79"/>
+      <c r="HZ74" s="79"/>
+      <c r="IA74" s="79"/>
+      <c r="IB74" s="79"/>
+      <c r="IC74" s="79"/>
+      <c r="ID74" s="79"/>
+      <c r="IE74" s="79"/>
+      <c r="IF74" s="79"/>
+      <c r="IG74" s="79"/>
+      <c r="IH74" s="79"/>
+      <c r="II74" s="79"/>
+      <c r="IJ74" s="79"/>
+      <c r="IK74" s="79"/>
+      <c r="IL74" s="79"/>
+      <c r="IM74" s="79"/>
+      <c r="IN74" s="79"/>
+      <c r="IO74" s="79"/>
+      <c r="IP74" s="79"/>
+      <c r="IQ74" s="79"/>
+      <c r="IR74" s="79"/>
+      <c r="IS74" s="79"/>
+      <c r="IT74" s="79"/>
+      <c r="IU74" s="79"/>
+      <c r="IV74" s="79"/>
+      <c r="IW74" s="79"/>
+    </row>
+    <row r="75" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="77" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C75" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="D75" s="78"/>
+      <c r="E75" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F75" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G75" s="78">
+        <v>0</v>
+      </c>
+      <c r="H75" s="78">
+        <v>1</v>
+      </c>
+      <c r="I75" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J75" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K75" s="79"/>
+      <c r="L75" s="79"/>
+      <c r="M75" s="79"/>
+      <c r="N75" s="79"/>
+      <c r="O75" s="79"/>
+      <c r="P75" s="79"/>
+      <c r="Q75" s="79"/>
+      <c r="R75" s="79"/>
+      <c r="S75" s="79"/>
+      <c r="T75" s="79"/>
+      <c r="U75" s="79"/>
+      <c r="V75" s="79"/>
+      <c r="W75" s="79"/>
+      <c r="X75" s="79"/>
+      <c r="Y75" s="79"/>
+      <c r="Z75" s="79"/>
+      <c r="AA75" s="79"/>
+      <c r="AB75" s="79"/>
+      <c r="AC75" s="79"/>
+      <c r="AD75" s="79"/>
+      <c r="AE75" s="79"/>
+      <c r="AF75" s="79"/>
+      <c r="AG75" s="79"/>
+      <c r="AH75" s="79"/>
+      <c r="AI75" s="79"/>
+      <c r="AJ75" s="79"/>
+      <c r="AK75" s="79"/>
+      <c r="AL75" s="79"/>
+      <c r="AM75" s="79"/>
+      <c r="AN75" s="79"/>
+      <c r="AO75" s="79"/>
+      <c r="AP75" s="79"/>
+      <c r="AQ75" s="79"/>
+      <c r="AR75" s="79"/>
+      <c r="AS75" s="79"/>
+      <c r="AT75" s="79"/>
+      <c r="AU75" s="79"/>
+      <c r="AV75" s="79"/>
+      <c r="AW75" s="79"/>
+      <c r="AX75" s="79"/>
+      <c r="AY75" s="79"/>
+      <c r="AZ75" s="79"/>
+      <c r="BA75" s="79"/>
+      <c r="BB75" s="79"/>
+      <c r="BC75" s="79"/>
+      <c r="BD75" s="79"/>
+      <c r="BE75" s="79"/>
+      <c r="BF75" s="79"/>
+      <c r="BG75" s="79"/>
+      <c r="BH75" s="79"/>
+      <c r="BI75" s="79"/>
+      <c r="BJ75" s="79"/>
+      <c r="BK75" s="79"/>
+      <c r="BL75" s="79"/>
+      <c r="BM75" s="79"/>
+      <c r="BN75" s="79"/>
+      <c r="BO75" s="79"/>
+      <c r="BP75" s="79"/>
+      <c r="BQ75" s="79"/>
+      <c r="BR75" s="79"/>
+      <c r="BS75" s="79"/>
+      <c r="BT75" s="79"/>
+      <c r="BU75" s="79"/>
+      <c r="BV75" s="79"/>
+      <c r="BW75" s="79"/>
+      <c r="BX75" s="79"/>
+      <c r="BY75" s="79"/>
+      <c r="BZ75" s="79"/>
+      <c r="CA75" s="79"/>
+      <c r="CB75" s="79"/>
+      <c r="CC75" s="79"/>
+      <c r="CD75" s="79"/>
+      <c r="CE75" s="79"/>
+      <c r="CF75" s="79"/>
+      <c r="CG75" s="79"/>
+      <c r="CH75" s="79"/>
+      <c r="CI75" s="79"/>
+      <c r="CJ75" s="79"/>
+      <c r="CK75" s="79"/>
+      <c r="CL75" s="79"/>
+      <c r="CM75" s="79"/>
+      <c r="CN75" s="79"/>
+      <c r="CO75" s="79"/>
+      <c r="CP75" s="79"/>
+      <c r="CQ75" s="79"/>
+      <c r="CR75" s="79"/>
+      <c r="CS75" s="79"/>
+      <c r="CT75" s="79"/>
+      <c r="CU75" s="79"/>
+      <c r="CV75" s="79"/>
+      <c r="CW75" s="79"/>
+      <c r="CX75" s="79"/>
+      <c r="CY75" s="79"/>
+      <c r="CZ75" s="79"/>
+      <c r="DA75" s="79"/>
+      <c r="DB75" s="79"/>
+      <c r="DC75" s="79"/>
+      <c r="DD75" s="79"/>
+      <c r="DE75" s="79"/>
+      <c r="DF75" s="79"/>
+      <c r="DG75" s="79"/>
+      <c r="DH75" s="79"/>
+      <c r="DI75" s="79"/>
+      <c r="DJ75" s="79"/>
+      <c r="DK75" s="79"/>
+      <c r="DL75" s="79"/>
+      <c r="DM75" s="79"/>
+      <c r="DN75" s="79"/>
+      <c r="DO75" s="79"/>
+      <c r="DP75" s="79"/>
+      <c r="DQ75" s="79"/>
+      <c r="DR75" s="79"/>
+      <c r="DS75" s="79"/>
+      <c r="DT75" s="79"/>
+      <c r="DU75" s="79"/>
+      <c r="DV75" s="79"/>
+      <c r="DW75" s="79"/>
+      <c r="DX75" s="79"/>
+      <c r="DY75" s="79"/>
+      <c r="DZ75" s="79"/>
+      <c r="EA75" s="79"/>
+      <c r="EB75" s="79"/>
+      <c r="EC75" s="79"/>
+      <c r="ED75" s="79"/>
+      <c r="EE75" s="79"/>
+      <c r="EF75" s="79"/>
+      <c r="EG75" s="79"/>
+      <c r="EH75" s="79"/>
+      <c r="EI75" s="79"/>
+      <c r="EJ75" s="79"/>
+      <c r="EK75" s="79"/>
+      <c r="EL75" s="79"/>
+      <c r="EM75" s="79"/>
+      <c r="EN75" s="79"/>
+      <c r="EO75" s="79"/>
+      <c r="EP75" s="79"/>
+      <c r="EQ75" s="79"/>
+      <c r="ER75" s="79"/>
+      <c r="ES75" s="79"/>
+      <c r="ET75" s="79"/>
+      <c r="EU75" s="79"/>
+      <c r="EV75" s="79"/>
+      <c r="EW75" s="79"/>
+      <c r="EX75" s="79"/>
+      <c r="EY75" s="79"/>
+      <c r="EZ75" s="79"/>
+      <c r="FA75" s="79"/>
+      <c r="FB75" s="79"/>
+      <c r="FC75" s="79"/>
+      <c r="FD75" s="79"/>
+      <c r="FE75" s="79"/>
+      <c r="FF75" s="79"/>
+      <c r="FG75" s="79"/>
+      <c r="FH75" s="79"/>
+      <c r="FI75" s="79"/>
+      <c r="FJ75" s="79"/>
+      <c r="FK75" s="79"/>
+      <c r="FL75" s="79"/>
+      <c r="FM75" s="79"/>
+      <c r="FN75" s="79"/>
+      <c r="FO75" s="79"/>
+      <c r="FP75" s="79"/>
+      <c r="FQ75" s="79"/>
+      <c r="FR75" s="79"/>
+      <c r="FS75" s="79"/>
+      <c r="FT75" s="79"/>
+      <c r="FU75" s="79"/>
+      <c r="FV75" s="79"/>
+      <c r="FW75" s="79"/>
+      <c r="FX75" s="79"/>
+      <c r="FY75" s="79"/>
+      <c r="FZ75" s="79"/>
+      <c r="GA75" s="79"/>
+      <c r="GB75" s="79"/>
+      <c r="GC75" s="79"/>
+      <c r="GD75" s="79"/>
+      <c r="GE75" s="79"/>
+      <c r="GF75" s="79"/>
+      <c r="GG75" s="79"/>
+      <c r="GH75" s="79"/>
+      <c r="GI75" s="79"/>
+      <c r="GJ75" s="79"/>
+      <c r="GK75" s="79"/>
+      <c r="GL75" s="79"/>
+      <c r="GM75" s="79"/>
+      <c r="GN75" s="79"/>
+      <c r="GO75" s="79"/>
+      <c r="GP75" s="79"/>
+      <c r="GQ75" s="79"/>
+      <c r="GR75" s="79"/>
+      <c r="GS75" s="79"/>
+      <c r="GT75" s="79"/>
+      <c r="GU75" s="79"/>
+      <c r="GV75" s="79"/>
+      <c r="GW75" s="79"/>
+      <c r="GX75" s="79"/>
+      <c r="GY75" s="79"/>
+      <c r="GZ75" s="79"/>
+      <c r="HA75" s="79"/>
+      <c r="HB75" s="79"/>
+      <c r="HC75" s="79"/>
+      <c r="HD75" s="79"/>
+      <c r="HE75" s="79"/>
+      <c r="HF75" s="79"/>
+      <c r="HG75" s="79"/>
+      <c r="HH75" s="79"/>
+      <c r="HI75" s="79"/>
+      <c r="HJ75" s="79"/>
+      <c r="HK75" s="79"/>
+      <c r="HL75" s="79"/>
+      <c r="HM75" s="79"/>
+      <c r="HN75" s="79"/>
+      <c r="HO75" s="79"/>
+      <c r="HP75" s="79"/>
+      <c r="HQ75" s="79"/>
+      <c r="HR75" s="79"/>
+      <c r="HS75" s="79"/>
+      <c r="HT75" s="79"/>
+      <c r="HU75" s="79"/>
+      <c r="HV75" s="79"/>
+      <c r="HW75" s="79"/>
+      <c r="HX75" s="79"/>
+      <c r="HY75" s="79"/>
+      <c r="HZ75" s="79"/>
+      <c r="IA75" s="79"/>
+      <c r="IB75" s="79"/>
+      <c r="IC75" s="79"/>
+      <c r="ID75" s="79"/>
+      <c r="IE75" s="79"/>
+      <c r="IF75" s="79"/>
+      <c r="IG75" s="79"/>
+      <c r="IH75" s="79"/>
+      <c r="II75" s="79"/>
+      <c r="IJ75" s="79"/>
+      <c r="IK75" s="79"/>
+      <c r="IL75" s="79"/>
+      <c r="IM75" s="79"/>
+      <c r="IN75" s="79"/>
+      <c r="IO75" s="79"/>
+      <c r="IP75" s="79"/>
+      <c r="IQ75" s="79"/>
+      <c r="IR75" s="79"/>
+      <c r="IS75" s="79"/>
+      <c r="IT75" s="79"/>
+      <c r="IU75" s="79"/>
+      <c r="IV75" s="79"/>
+      <c r="IW75" s="79"/>
+    </row>
+    <row r="76" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="B76" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="74" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E76" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="F76" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="74">
+        <v>0</v>
+      </c>
+      <c r="H76" s="74">
+        <v>1</v>
+      </c>
+      <c r="I76" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="J76" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="K76" s="75"/>
+      <c r="L76" s="75"/>
+      <c r="M76" s="75"/>
+      <c r="N76" s="75"/>
+      <c r="O76" s="75"/>
+      <c r="P76" s="75"/>
+      <c r="Q76" s="75"/>
+      <c r="R76" s="75"/>
+      <c r="S76" s="75"/>
+      <c r="T76" s="75"/>
+      <c r="U76" s="75"/>
+      <c r="V76" s="75"/>
+      <c r="W76" s="75"/>
+      <c r="X76" s="75"/>
+      <c r="Y76" s="75"/>
+      <c r="Z76" s="75"/>
+      <c r="AA76" s="75"/>
+      <c r="AB76" s="75"/>
+      <c r="AC76" s="75"/>
+      <c r="AD76" s="75"/>
+      <c r="AE76" s="75"/>
+      <c r="AF76" s="75"/>
+      <c r="AG76" s="75"/>
+      <c r="AH76" s="75"/>
+      <c r="AI76" s="75"/>
+      <c r="AJ76" s="75"/>
+      <c r="AK76" s="75"/>
+      <c r="AL76" s="75"/>
+      <c r="AM76" s="75"/>
+      <c r="AN76" s="75"/>
+      <c r="AO76" s="75"/>
+      <c r="AP76" s="75"/>
+      <c r="AQ76" s="75"/>
+      <c r="AR76" s="75"/>
+      <c r="AS76" s="75"/>
+      <c r="AT76" s="75"/>
+      <c r="AU76" s="75"/>
+      <c r="AV76" s="75"/>
+      <c r="AW76" s="75"/>
+      <c r="AX76" s="75"/>
+      <c r="AY76" s="75"/>
+      <c r="AZ76" s="75"/>
+      <c r="BA76" s="75"/>
+      <c r="BB76" s="75"/>
+      <c r="BC76" s="75"/>
+      <c r="BD76" s="75"/>
+      <c r="BE76" s="75"/>
+      <c r="BF76" s="75"/>
+      <c r="BG76" s="75"/>
+      <c r="BH76" s="75"/>
+      <c r="BI76" s="75"/>
+      <c r="BJ76" s="75"/>
+      <c r="BK76" s="75"/>
+      <c r="BL76" s="75"/>
+      <c r="BM76" s="75"/>
+      <c r="BN76" s="75"/>
+      <c r="BO76" s="75"/>
+      <c r="BP76" s="75"/>
+      <c r="BQ76" s="75"/>
+      <c r="BR76" s="75"/>
+      <c r="BS76" s="75"/>
+      <c r="BT76" s="75"/>
+      <c r="BU76" s="75"/>
+      <c r="BV76" s="75"/>
+      <c r="BW76" s="75"/>
+      <c r="BX76" s="75"/>
+      <c r="BY76" s="75"/>
+      <c r="BZ76" s="75"/>
+      <c r="CA76" s="75"/>
+      <c r="CB76" s="75"/>
+      <c r="CC76" s="75"/>
+      <c r="CD76" s="75"/>
+      <c r="CE76" s="75"/>
+      <c r="CF76" s="75"/>
+      <c r="CG76" s="75"/>
+      <c r="CH76" s="75"/>
+      <c r="CI76" s="75"/>
+      <c r="CJ76" s="75"/>
+      <c r="CK76" s="75"/>
+      <c r="CL76" s="75"/>
+      <c r="CM76" s="75"/>
+      <c r="CN76" s="75"/>
+      <c r="CO76" s="75"/>
+      <c r="CP76" s="75"/>
+      <c r="CQ76" s="75"/>
+      <c r="CR76" s="75"/>
+      <c r="CS76" s="75"/>
+      <c r="CT76" s="75"/>
+      <c r="CU76" s="75"/>
+      <c r="CV76" s="75"/>
+      <c r="CW76" s="75"/>
+      <c r="CX76" s="75"/>
+      <c r="CY76" s="75"/>
+      <c r="CZ76" s="75"/>
+      <c r="DA76" s="75"/>
+      <c r="DB76" s="75"/>
+      <c r="DC76" s="75"/>
+      <c r="DD76" s="75"/>
+      <c r="DE76" s="75"/>
+      <c r="DF76" s="75"/>
+      <c r="DG76" s="75"/>
+      <c r="DH76" s="75"/>
+      <c r="DI76" s="75"/>
+      <c r="DJ76" s="75"/>
+      <c r="DK76" s="75"/>
+      <c r="DL76" s="75"/>
+      <c r="DM76" s="75"/>
+      <c r="DN76" s="75"/>
+      <c r="DO76" s="75"/>
+      <c r="DP76" s="75"/>
+      <c r="DQ76" s="75"/>
+      <c r="DR76" s="75"/>
+      <c r="DS76" s="75"/>
+      <c r="DT76" s="75"/>
+      <c r="DU76" s="75"/>
+      <c r="DV76" s="75"/>
+      <c r="DW76" s="75"/>
+      <c r="DX76" s="75"/>
+      <c r="DY76" s="75"/>
+      <c r="DZ76" s="75"/>
+      <c r="EA76" s="75"/>
+      <c r="EB76" s="75"/>
+      <c r="EC76" s="75"/>
+      <c r="ED76" s="75"/>
+      <c r="EE76" s="75"/>
+      <c r="EF76" s="75"/>
+      <c r="EG76" s="75"/>
+      <c r="EH76" s="75"/>
+      <c r="EI76" s="75"/>
+      <c r="EJ76" s="75"/>
+      <c r="EK76" s="75"/>
+      <c r="EL76" s="75"/>
+      <c r="EM76" s="75"/>
+      <c r="EN76" s="75"/>
+      <c r="EO76" s="75"/>
+      <c r="EP76" s="75"/>
+      <c r="EQ76" s="75"/>
+      <c r="ER76" s="75"/>
+      <c r="ES76" s="75"/>
+      <c r="ET76" s="75"/>
+      <c r="EU76" s="75"/>
+      <c r="EV76" s="75"/>
+      <c r="EW76" s="75"/>
+      <c r="EX76" s="75"/>
+      <c r="EY76" s="75"/>
+      <c r="EZ76" s="75"/>
+      <c r="FA76" s="75"/>
+      <c r="FB76" s="75"/>
+      <c r="FC76" s="75"/>
+      <c r="FD76" s="75"/>
+      <c r="FE76" s="75"/>
+      <c r="FF76" s="75"/>
+      <c r="FG76" s="75"/>
+      <c r="FH76" s="75"/>
+      <c r="FI76" s="75"/>
+      <c r="FJ76" s="75"/>
+      <c r="FK76" s="75"/>
+      <c r="FL76" s="75"/>
+      <c r="FM76" s="75"/>
+      <c r="FN76" s="75"/>
+      <c r="FO76" s="75"/>
+      <c r="FP76" s="75"/>
+      <c r="FQ76" s="75"/>
+      <c r="FR76" s="75"/>
+      <c r="FS76" s="75"/>
+      <c r="FT76" s="75"/>
+      <c r="FU76" s="75"/>
+      <c r="FV76" s="75"/>
+      <c r="FW76" s="75"/>
+      <c r="FX76" s="75"/>
+      <c r="FY76" s="75"/>
+      <c r="FZ76" s="75"/>
+      <c r="GA76" s="75"/>
+      <c r="GB76" s="75"/>
+      <c r="GC76" s="75"/>
+      <c r="GD76" s="75"/>
+      <c r="GE76" s="75"/>
+      <c r="GF76" s="75"/>
+      <c r="GG76" s="75"/>
+      <c r="GH76" s="75"/>
+      <c r="GI76" s="75"/>
+      <c r="GJ76" s="75"/>
+      <c r="GK76" s="75"/>
+      <c r="GL76" s="75"/>
+      <c r="GM76" s="75"/>
+      <c r="GN76" s="75"/>
+      <c r="GO76" s="75"/>
+      <c r="GP76" s="75"/>
+      <c r="GQ76" s="75"/>
+      <c r="GR76" s="75"/>
+      <c r="GS76" s="75"/>
+      <c r="GT76" s="75"/>
+      <c r="GU76" s="75"/>
+      <c r="GV76" s="75"/>
+      <c r="GW76" s="75"/>
+      <c r="GX76" s="75"/>
+      <c r="GY76" s="75"/>
+      <c r="GZ76" s="75"/>
+      <c r="HA76" s="75"/>
+      <c r="HB76" s="75"/>
+      <c r="HC76" s="75"/>
+      <c r="HD76" s="75"/>
+      <c r="HE76" s="75"/>
+      <c r="HF76" s="75"/>
+      <c r="HG76" s="75"/>
+      <c r="HH76" s="75"/>
+      <c r="HI76" s="75"/>
+      <c r="HJ76" s="75"/>
+      <c r="HK76" s="75"/>
+      <c r="HL76" s="75"/>
+      <c r="HM76" s="75"/>
+      <c r="HN76" s="75"/>
+      <c r="HO76" s="75"/>
+      <c r="HP76" s="75"/>
+      <c r="HQ76" s="75"/>
+      <c r="HR76" s="75"/>
+      <c r="HS76" s="75"/>
+      <c r="HT76" s="75"/>
+      <c r="HU76" s="75"/>
+      <c r="HV76" s="75"/>
+      <c r="HW76" s="75"/>
+      <c r="HX76" s="75"/>
+      <c r="HY76" s="75"/>
+      <c r="HZ76" s="75"/>
+      <c r="IA76" s="75"/>
+      <c r="IB76" s="75"/>
+      <c r="IC76" s="75"/>
+      <c r="ID76" s="75"/>
+      <c r="IE76" s="75"/>
+      <c r="IF76" s="75"/>
+      <c r="IG76" s="75"/>
+      <c r="IH76" s="75"/>
+      <c r="II76" s="75"/>
+      <c r="IJ76" s="75"/>
+      <c r="IK76" s="75"/>
+      <c r="IL76" s="75"/>
+      <c r="IM76" s="75"/>
+      <c r="IN76" s="75"/>
+      <c r="IO76" s="75"/>
+      <c r="IP76" s="75"/>
+      <c r="IQ76" s="75"/>
+      <c r="IR76" s="75"/>
+      <c r="IS76" s="75"/>
+      <c r="IT76" s="75"/>
+      <c r="IU76" s="75"/>
+      <c r="IV76" s="75"/>
+      <c r="IW76" s="75"/>
+    </row>
+    <row r="77" spans="1:257" s="76" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="D77" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E77" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="F77" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="G77" s="74">
+        <v>0</v>
+      </c>
+      <c r="H77" s="74">
+        <v>1</v>
+      </c>
+      <c r="I77" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="J77" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="K77" s="75"/>
+      <c r="L77" s="75"/>
+      <c r="M77" s="75"/>
+      <c r="N77" s="75"/>
+      <c r="O77" s="75"/>
+      <c r="P77" s="75"/>
+      <c r="Q77" s="75"/>
+      <c r="R77" s="75"/>
+      <c r="S77" s="75"/>
+      <c r="T77" s="75"/>
+      <c r="U77" s="75"/>
+      <c r="V77" s="75"/>
+      <c r="W77" s="75"/>
+      <c r="X77" s="75"/>
+      <c r="Y77" s="75"/>
+      <c r="Z77" s="75"/>
+      <c r="AA77" s="75"/>
+      <c r="AB77" s="75"/>
+      <c r="AC77" s="75"/>
+      <c r="AD77" s="75"/>
+      <c r="AE77" s="75"/>
+      <c r="AF77" s="75"/>
+      <c r="AG77" s="75"/>
+      <c r="AH77" s="75"/>
+      <c r="AI77" s="75"/>
+      <c r="AJ77" s="75"/>
+      <c r="AK77" s="75"/>
+      <c r="AL77" s="75"/>
+      <c r="AM77" s="75"/>
+      <c r="AN77" s="75"/>
+      <c r="AO77" s="75"/>
+      <c r="AP77" s="75"/>
+      <c r="AQ77" s="75"/>
+      <c r="AR77" s="75"/>
+      <c r="AS77" s="75"/>
+      <c r="AT77" s="75"/>
+      <c r="AU77" s="75"/>
+      <c r="AV77" s="75"/>
+      <c r="AW77" s="75"/>
+      <c r="AX77" s="75"/>
+      <c r="AY77" s="75"/>
+      <c r="AZ77" s="75"/>
+      <c r="BA77" s="75"/>
+      <c r="BB77" s="75"/>
+      <c r="BC77" s="75"/>
+      <c r="BD77" s="75"/>
+      <c r="BE77" s="75"/>
+      <c r="BF77" s="75"/>
+      <c r="BG77" s="75"/>
+      <c r="BH77" s="75"/>
+      <c r="BI77" s="75"/>
+      <c r="BJ77" s="75"/>
+      <c r="BK77" s="75"/>
+      <c r="BL77" s="75"/>
+      <c r="BM77" s="75"/>
+      <c r="BN77" s="75"/>
+      <c r="BO77" s="75"/>
+      <c r="BP77" s="75"/>
+      <c r="BQ77" s="75"/>
+      <c r="BR77" s="75"/>
+      <c r="BS77" s="75"/>
+      <c r="BT77" s="75"/>
+      <c r="BU77" s="75"/>
+      <c r="BV77" s="75"/>
+      <c r="BW77" s="75"/>
+      <c r="BX77" s="75"/>
+      <c r="BY77" s="75"/>
+      <c r="BZ77" s="75"/>
+      <c r="CA77" s="75"/>
+      <c r="CB77" s="75"/>
+      <c r="CC77" s="75"/>
+      <c r="CD77" s="75"/>
+      <c r="CE77" s="75"/>
+      <c r="CF77" s="75"/>
+      <c r="CG77" s="75"/>
+      <c r="CH77" s="75"/>
+      <c r="CI77" s="75"/>
+      <c r="CJ77" s="75"/>
+      <c r="CK77" s="75"/>
+      <c r="CL77" s="75"/>
+      <c r="CM77" s="75"/>
+      <c r="CN77" s="75"/>
+      <c r="CO77" s="75"/>
+      <c r="CP77" s="75"/>
+      <c r="CQ77" s="75"/>
+      <c r="CR77" s="75"/>
+      <c r="CS77" s="75"/>
+      <c r="CT77" s="75"/>
+      <c r="CU77" s="75"/>
+      <c r="CV77" s="75"/>
+      <c r="CW77" s="75"/>
+      <c r="CX77" s="75"/>
+      <c r="CY77" s="75"/>
+      <c r="CZ77" s="75"/>
+      <c r="DA77" s="75"/>
+      <c r="DB77" s="75"/>
+      <c r="DC77" s="75"/>
+      <c r="DD77" s="75"/>
+      <c r="DE77" s="75"/>
+      <c r="DF77" s="75"/>
+      <c r="DG77" s="75"/>
+      <c r="DH77" s="75"/>
+      <c r="DI77" s="75"/>
+      <c r="DJ77" s="75"/>
+      <c r="DK77" s="75"/>
+      <c r="DL77" s="75"/>
+      <c r="DM77" s="75"/>
+      <c r="DN77" s="75"/>
+      <c r="DO77" s="75"/>
+      <c r="DP77" s="75"/>
+      <c r="DQ77" s="75"/>
+      <c r="DR77" s="75"/>
+      <c r="DS77" s="75"/>
+      <c r="DT77" s="75"/>
+      <c r="DU77" s="75"/>
+      <c r="DV77" s="75"/>
+      <c r="DW77" s="75"/>
+      <c r="DX77" s="75"/>
+      <c r="DY77" s="75"/>
+      <c r="DZ77" s="75"/>
+      <c r="EA77" s="75"/>
+      <c r="EB77" s="75"/>
+      <c r="EC77" s="75"/>
+      <c r="ED77" s="75"/>
+      <c r="EE77" s="75"/>
+      <c r="EF77" s="75"/>
+      <c r="EG77" s="75"/>
+      <c r="EH77" s="75"/>
+      <c r="EI77" s="75"/>
+      <c r="EJ77" s="75"/>
+      <c r="EK77" s="75"/>
+      <c r="EL77" s="75"/>
+      <c r="EM77" s="75"/>
+      <c r="EN77" s="75"/>
+      <c r="EO77" s="75"/>
+      <c r="EP77" s="75"/>
+      <c r="EQ77" s="75"/>
+      <c r="ER77" s="75"/>
+      <c r="ES77" s="75"/>
+      <c r="ET77" s="75"/>
+      <c r="EU77" s="75"/>
+      <c r="EV77" s="75"/>
+      <c r="EW77" s="75"/>
+      <c r="EX77" s="75"/>
+      <c r="EY77" s="75"/>
+      <c r="EZ77" s="75"/>
+      <c r="FA77" s="75"/>
+      <c r="FB77" s="75"/>
+      <c r="FC77" s="75"/>
+      <c r="FD77" s="75"/>
+      <c r="FE77" s="75"/>
+      <c r="FF77" s="75"/>
+      <c r="FG77" s="75"/>
+      <c r="FH77" s="75"/>
+      <c r="FI77" s="75"/>
+      <c r="FJ77" s="75"/>
+      <c r="FK77" s="75"/>
+      <c r="FL77" s="75"/>
+      <c r="FM77" s="75"/>
+      <c r="FN77" s="75"/>
+      <c r="FO77" s="75"/>
+      <c r="FP77" s="75"/>
+      <c r="FQ77" s="75"/>
+      <c r="FR77" s="75"/>
+      <c r="FS77" s="75"/>
+      <c r="FT77" s="75"/>
+      <c r="FU77" s="75"/>
+      <c r="FV77" s="75"/>
+      <c r="FW77" s="75"/>
+      <c r="FX77" s="75"/>
+      <c r="FY77" s="75"/>
+      <c r="FZ77" s="75"/>
+      <c r="GA77" s="75"/>
+      <c r="GB77" s="75"/>
+      <c r="GC77" s="75"/>
+      <c r="GD77" s="75"/>
+      <c r="GE77" s="75"/>
+      <c r="GF77" s="75"/>
+      <c r="GG77" s="75"/>
+      <c r="GH77" s="75"/>
+      <c r="GI77" s="75"/>
+      <c r="GJ77" s="75"/>
+      <c r="GK77" s="75"/>
+      <c r="GL77" s="75"/>
+      <c r="GM77" s="75"/>
+      <c r="GN77" s="75"/>
+      <c r="GO77" s="75"/>
+      <c r="GP77" s="75"/>
+      <c r="GQ77" s="75"/>
+      <c r="GR77" s="75"/>
+      <c r="GS77" s="75"/>
+      <c r="GT77" s="75"/>
+      <c r="GU77" s="75"/>
+      <c r="GV77" s="75"/>
+      <c r="GW77" s="75"/>
+      <c r="GX77" s="75"/>
+      <c r="GY77" s="75"/>
+      <c r="GZ77" s="75"/>
+      <c r="HA77" s="75"/>
+      <c r="HB77" s="75"/>
+      <c r="HC77" s="75"/>
+      <c r="HD77" s="75"/>
+      <c r="HE77" s="75"/>
+      <c r="HF77" s="75"/>
+      <c r="HG77" s="75"/>
+      <c r="HH77" s="75"/>
+      <c r="HI77" s="75"/>
+      <c r="HJ77" s="75"/>
+      <c r="HK77" s="75"/>
+      <c r="HL77" s="75"/>
+      <c r="HM77" s="75"/>
+      <c r="HN77" s="75"/>
+      <c r="HO77" s="75"/>
+      <c r="HP77" s="75"/>
+      <c r="HQ77" s="75"/>
+      <c r="HR77" s="75"/>
+      <c r="HS77" s="75"/>
+      <c r="HT77" s="75"/>
+      <c r="HU77" s="75"/>
+      <c r="HV77" s="75"/>
+      <c r="HW77" s="75"/>
+      <c r="HX77" s="75"/>
+      <c r="HY77" s="75"/>
+      <c r="HZ77" s="75"/>
+      <c r="IA77" s="75"/>
+      <c r="IB77" s="75"/>
+      <c r="IC77" s="75"/>
+      <c r="ID77" s="75"/>
+      <c r="IE77" s="75"/>
+      <c r="IF77" s="75"/>
+      <c r="IG77" s="75"/>
+      <c r="IH77" s="75"/>
+      <c r="II77" s="75"/>
+      <c r="IJ77" s="75"/>
+      <c r="IK77" s="75"/>
+      <c r="IL77" s="75"/>
+      <c r="IM77" s="75"/>
+      <c r="IN77" s="75"/>
+      <c r="IO77" s="75"/>
+      <c r="IP77" s="75"/>
+      <c r="IQ77" s="75"/>
+      <c r="IR77" s="75"/>
+      <c r="IS77" s="75"/>
+      <c r="IT77" s="75"/>
+      <c r="IU77" s="75"/>
+      <c r="IV77" s="75"/>
+      <c r="IW77" s="75"/>
+    </row>
+    <row r="78" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="D78" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E78" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="F78" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="G78" s="74">
+        <v>0</v>
+      </c>
+      <c r="H78" s="74">
+        <v>1</v>
+      </c>
+      <c r="I78" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="J78" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="K78" s="75"/>
+      <c r="L78" s="75"/>
+      <c r="M78" s="75"/>
+      <c r="N78" s="75"/>
+      <c r="O78" s="75"/>
+      <c r="P78" s="75"/>
+      <c r="Q78" s="75"/>
+      <c r="R78" s="75"/>
+      <c r="S78" s="75"/>
+      <c r="T78" s="75"/>
+      <c r="U78" s="75"/>
+      <c r="V78" s="75"/>
+      <c r="W78" s="75"/>
+      <c r="X78" s="75"/>
+      <c r="Y78" s="75"/>
+      <c r="Z78" s="75"/>
+      <c r="AA78" s="75"/>
+      <c r="AB78" s="75"/>
+      <c r="AC78" s="75"/>
+      <c r="AD78" s="75"/>
+      <c r="AE78" s="75"/>
+      <c r="AF78" s="75"/>
+      <c r="AG78" s="75"/>
+      <c r="AH78" s="75"/>
+      <c r="AI78" s="75"/>
+      <c r="AJ78" s="75"/>
+      <c r="AK78" s="75"/>
+      <c r="AL78" s="75"/>
+      <c r="AM78" s="75"/>
+      <c r="AN78" s="75"/>
+      <c r="AO78" s="75"/>
+      <c r="AP78" s="75"/>
+      <c r="AQ78" s="75"/>
+      <c r="AR78" s="75"/>
+      <c r="AS78" s="75"/>
+      <c r="AT78" s="75"/>
+      <c r="AU78" s="75"/>
+      <c r="AV78" s="75"/>
+      <c r="AW78" s="75"/>
+      <c r="AX78" s="75"/>
+      <c r="AY78" s="75"/>
+      <c r="AZ78" s="75"/>
+      <c r="BA78" s="75"/>
+      <c r="BB78" s="75"/>
+      <c r="BC78" s="75"/>
+      <c r="BD78" s="75"/>
+      <c r="BE78" s="75"/>
+      <c r="BF78" s="75"/>
+      <c r="BG78" s="75"/>
+      <c r="BH78" s="75"/>
+      <c r="BI78" s="75"/>
+      <c r="BJ78" s="75"/>
+      <c r="BK78" s="75"/>
+      <c r="BL78" s="75"/>
+      <c r="BM78" s="75"/>
+      <c r="BN78" s="75"/>
+      <c r="BO78" s="75"/>
+      <c r="BP78" s="75"/>
+      <c r="BQ78" s="75"/>
+      <c r="BR78" s="75"/>
+      <c r="BS78" s="75"/>
+      <c r="BT78" s="75"/>
+      <c r="BU78" s="75"/>
+      <c r="BV78" s="75"/>
+      <c r="BW78" s="75"/>
+      <c r="BX78" s="75"/>
+      <c r="BY78" s="75"/>
+      <c r="BZ78" s="75"/>
+      <c r="CA78" s="75"/>
+      <c r="CB78" s="75"/>
+      <c r="CC78" s="75"/>
+      <c r="CD78" s="75"/>
+      <c r="CE78" s="75"/>
+      <c r="CF78" s="75"/>
+      <c r="CG78" s="75"/>
+      <c r="CH78" s="75"/>
+      <c r="CI78" s="75"/>
+      <c r="CJ78" s="75"/>
+      <c r="CK78" s="75"/>
+      <c r="CL78" s="75"/>
+      <c r="CM78" s="75"/>
+      <c r="CN78" s="75"/>
+      <c r="CO78" s="75"/>
+      <c r="CP78" s="75"/>
+      <c r="CQ78" s="75"/>
+      <c r="CR78" s="75"/>
+      <c r="CS78" s="75"/>
+      <c r="CT78" s="75"/>
+      <c r="CU78" s="75"/>
+      <c r="CV78" s="75"/>
+      <c r="CW78" s="75"/>
+      <c r="CX78" s="75"/>
+      <c r="CY78" s="75"/>
+      <c r="CZ78" s="75"/>
+      <c r="DA78" s="75"/>
+      <c r="DB78" s="75"/>
+      <c r="DC78" s="75"/>
+      <c r="DD78" s="75"/>
+      <c r="DE78" s="75"/>
+      <c r="DF78" s="75"/>
+      <c r="DG78" s="75"/>
+      <c r="DH78" s="75"/>
+      <c r="DI78" s="75"/>
+      <c r="DJ78" s="75"/>
+      <c r="DK78" s="75"/>
+      <c r="DL78" s="75"/>
+      <c r="DM78" s="75"/>
+      <c r="DN78" s="75"/>
+      <c r="DO78" s="75"/>
+      <c r="DP78" s="75"/>
+      <c r="DQ78" s="75"/>
+      <c r="DR78" s="75"/>
+      <c r="DS78" s="75"/>
+      <c r="DT78" s="75"/>
+      <c r="DU78" s="75"/>
+      <c r="DV78" s="75"/>
+      <c r="DW78" s="75"/>
+      <c r="DX78" s="75"/>
+      <c r="DY78" s="75"/>
+      <c r="DZ78" s="75"/>
+      <c r="EA78" s="75"/>
+      <c r="EB78" s="75"/>
+      <c r="EC78" s="75"/>
+      <c r="ED78" s="75"/>
+      <c r="EE78" s="75"/>
+      <c r="EF78" s="75"/>
+      <c r="EG78" s="75"/>
+      <c r="EH78" s="75"/>
+      <c r="EI78" s="75"/>
+      <c r="EJ78" s="75"/>
+      <c r="EK78" s="75"/>
+      <c r="EL78" s="75"/>
+      <c r="EM78" s="75"/>
+      <c r="EN78" s="75"/>
+      <c r="EO78" s="75"/>
+      <c r="EP78" s="75"/>
+      <c r="EQ78" s="75"/>
+      <c r="ER78" s="75"/>
+      <c r="ES78" s="75"/>
+      <c r="ET78" s="75"/>
+      <c r="EU78" s="75"/>
+      <c r="EV78" s="75"/>
+      <c r="EW78" s="75"/>
+      <c r="EX78" s="75"/>
+      <c r="EY78" s="75"/>
+      <c r="EZ78" s="75"/>
+      <c r="FA78" s="75"/>
+      <c r="FB78" s="75"/>
+      <c r="FC78" s="75"/>
+      <c r="FD78" s="75"/>
+      <c r="FE78" s="75"/>
+      <c r="FF78" s="75"/>
+      <c r="FG78" s="75"/>
+      <c r="FH78" s="75"/>
+      <c r="FI78" s="75"/>
+      <c r="FJ78" s="75"/>
+      <c r="FK78" s="75"/>
+      <c r="FL78" s="75"/>
+      <c r="FM78" s="75"/>
+      <c r="FN78" s="75"/>
+      <c r="FO78" s="75"/>
+      <c r="FP78" s="75"/>
+      <c r="FQ78" s="75"/>
+      <c r="FR78" s="75"/>
+      <c r="FS78" s="75"/>
+      <c r="FT78" s="75"/>
+      <c r="FU78" s="75"/>
+      <c r="FV78" s="75"/>
+      <c r="FW78" s="75"/>
+      <c r="FX78" s="75"/>
+      <c r="FY78" s="75"/>
+      <c r="FZ78" s="75"/>
+      <c r="GA78" s="75"/>
+      <c r="GB78" s="75"/>
+      <c r="GC78" s="75"/>
+      <c r="GD78" s="75"/>
+      <c r="GE78" s="75"/>
+      <c r="GF78" s="75"/>
+      <c r="GG78" s="75"/>
+      <c r="GH78" s="75"/>
+      <c r="GI78" s="75"/>
+      <c r="GJ78" s="75"/>
+      <c r="GK78" s="75"/>
+      <c r="GL78" s="75"/>
+      <c r="GM78" s="75"/>
+      <c r="GN78" s="75"/>
+      <c r="GO78" s="75"/>
+      <c r="GP78" s="75"/>
+      <c r="GQ78" s="75"/>
+      <c r="GR78" s="75"/>
+      <c r="GS78" s="75"/>
+      <c r="GT78" s="75"/>
+      <c r="GU78" s="75"/>
+      <c r="GV78" s="75"/>
+      <c r="GW78" s="75"/>
+      <c r="GX78" s="75"/>
+      <c r="GY78" s="75"/>
+      <c r="GZ78" s="75"/>
+      <c r="HA78" s="75"/>
+      <c r="HB78" s="75"/>
+      <c r="HC78" s="75"/>
+      <c r="HD78" s="75"/>
+      <c r="HE78" s="75"/>
+      <c r="HF78" s="75"/>
+      <c r="HG78" s="75"/>
+      <c r="HH78" s="75"/>
+      <c r="HI78" s="75"/>
+      <c r="HJ78" s="75"/>
+      <c r="HK78" s="75"/>
+      <c r="HL78" s="75"/>
+      <c r="HM78" s="75"/>
+      <c r="HN78" s="75"/>
+      <c r="HO78" s="75"/>
+      <c r="HP78" s="75"/>
+      <c r="HQ78" s="75"/>
+      <c r="HR78" s="75"/>
+      <c r="HS78" s="75"/>
+      <c r="HT78" s="75"/>
+      <c r="HU78" s="75"/>
+      <c r="HV78" s="75"/>
+      <c r="HW78" s="75"/>
+      <c r="HX78" s="75"/>
+      <c r="HY78" s="75"/>
+      <c r="HZ78" s="75"/>
+      <c r="IA78" s="75"/>
+      <c r="IB78" s="75"/>
+      <c r="IC78" s="75"/>
+      <c r="ID78" s="75"/>
+      <c r="IE78" s="75"/>
+      <c r="IF78" s="75"/>
+      <c r="IG78" s="75"/>
+      <c r="IH78" s="75"/>
+      <c r="II78" s="75"/>
+      <c r="IJ78" s="75"/>
+      <c r="IK78" s="75"/>
+      <c r="IL78" s="75"/>
+      <c r="IM78" s="75"/>
+      <c r="IN78" s="75"/>
+      <c r="IO78" s="75"/>
+      <c r="IP78" s="75"/>
+      <c r="IQ78" s="75"/>
+      <c r="IR78" s="75"/>
+      <c r="IS78" s="75"/>
+      <c r="IT78" s="75"/>
+      <c r="IU78" s="75"/>
+      <c r="IV78" s="75"/>
+      <c r="IW78" s="75"/>
+    </row>
+    <row r="79" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B79" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="D79" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E79" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="F79" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="G79" s="74">
+        <v>0</v>
+      </c>
+      <c r="H79" s="74">
+        <v>1</v>
+      </c>
+      <c r="I79" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="J79" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="K79" s="75"/>
+      <c r="L79" s="75"/>
+      <c r="M79" s="75"/>
+      <c r="N79" s="75"/>
+      <c r="O79" s="75"/>
+      <c r="P79" s="75"/>
+      <c r="Q79" s="75"/>
+      <c r="R79" s="75"/>
+      <c r="S79" s="75"/>
+      <c r="T79" s="75"/>
+      <c r="U79" s="75"/>
+      <c r="V79" s="75"/>
+      <c r="W79" s="75"/>
+      <c r="X79" s="75"/>
+      <c r="Y79" s="75"/>
+      <c r="Z79" s="75"/>
+      <c r="AA79" s="75"/>
+      <c r="AB79" s="75"/>
+      <c r="AC79" s="75"/>
+      <c r="AD79" s="75"/>
+      <c r="AE79" s="75"/>
+      <c r="AF79" s="75"/>
+      <c r="AG79" s="75"/>
+      <c r="AH79" s="75"/>
+      <c r="AI79" s="75"/>
+      <c r="AJ79" s="75"/>
+      <c r="AK79" s="75"/>
+      <c r="AL79" s="75"/>
+      <c r="AM79" s="75"/>
+      <c r="AN79" s="75"/>
+      <c r="AO79" s="75"/>
+      <c r="AP79" s="75"/>
+      <c r="AQ79" s="75"/>
+      <c r="AR79" s="75"/>
+      <c r="AS79" s="75"/>
+      <c r="AT79" s="75"/>
+      <c r="AU79" s="75"/>
+      <c r="AV79" s="75"/>
+      <c r="AW79" s="75"/>
+      <c r="AX79" s="75"/>
+      <c r="AY79" s="75"/>
+      <c r="AZ79" s="75"/>
+      <c r="BA79" s="75"/>
+      <c r="BB79" s="75"/>
+      <c r="BC79" s="75"/>
+      <c r="BD79" s="75"/>
+      <c r="BE79" s="75"/>
+      <c r="BF79" s="75"/>
+      <c r="BG79" s="75"/>
+      <c r="BH79" s="75"/>
+      <c r="BI79" s="75"/>
+      <c r="BJ79" s="75"/>
+      <c r="BK79" s="75"/>
+      <c r="BL79" s="75"/>
+      <c r="BM79" s="75"/>
+      <c r="BN79" s="75"/>
+      <c r="BO79" s="75"/>
+      <c r="BP79" s="75"/>
+      <c r="BQ79" s="75"/>
+      <c r="BR79" s="75"/>
+      <c r="BS79" s="75"/>
+      <c r="BT79" s="75"/>
+      <c r="BU79" s="75"/>
+      <c r="BV79" s="75"/>
+      <c r="BW79" s="75"/>
+      <c r="BX79" s="75"/>
+      <c r="BY79" s="75"/>
+      <c r="BZ79" s="75"/>
+      <c r="CA79" s="75"/>
+      <c r="CB79" s="75"/>
+      <c r="CC79" s="75"/>
+      <c r="CD79" s="75"/>
+      <c r="CE79" s="75"/>
+      <c r="CF79" s="75"/>
+      <c r="CG79" s="75"/>
+      <c r="CH79" s="75"/>
+      <c r="CI79" s="75"/>
+      <c r="CJ79" s="75"/>
+      <c r="CK79" s="75"/>
+      <c r="CL79" s="75"/>
+      <c r="CM79" s="75"/>
+      <c r="CN79" s="75"/>
+      <c r="CO79" s="75"/>
+      <c r="CP79" s="75"/>
+      <c r="CQ79" s="75"/>
+      <c r="CR79" s="75"/>
+      <c r="CS79" s="75"/>
+      <c r="CT79" s="75"/>
+      <c r="CU79" s="75"/>
+      <c r="CV79" s="75"/>
+      <c r="CW79" s="75"/>
+      <c r="CX79" s="75"/>
+      <c r="CY79" s="75"/>
+      <c r="CZ79" s="75"/>
+      <c r="DA79" s="75"/>
+      <c r="DB79" s="75"/>
+      <c r="DC79" s="75"/>
+      <c r="DD79" s="75"/>
+      <c r="DE79" s="75"/>
+      <c r="DF79" s="75"/>
+      <c r="DG79" s="75"/>
+      <c r="DH79" s="75"/>
+      <c r="DI79" s="75"/>
+      <c r="DJ79" s="75"/>
+      <c r="DK79" s="75"/>
+      <c r="DL79" s="75"/>
+      <c r="DM79" s="75"/>
+      <c r="DN79" s="75"/>
+      <c r="DO79" s="75"/>
+      <c r="DP79" s="75"/>
+      <c r="DQ79" s="75"/>
+      <c r="DR79" s="75"/>
+      <c r="DS79" s="75"/>
+      <c r="DT79" s="75"/>
+      <c r="DU79" s="75"/>
+      <c r="DV79" s="75"/>
+      <c r="DW79" s="75"/>
+      <c r="DX79" s="75"/>
+      <c r="DY79" s="75"/>
+      <c r="DZ79" s="75"/>
+      <c r="EA79" s="75"/>
+      <c r="EB79" s="75"/>
+      <c r="EC79" s="75"/>
+      <c r="ED79" s="75"/>
+      <c r="EE79" s="75"/>
+      <c r="EF79" s="75"/>
+      <c r="EG79" s="75"/>
+      <c r="EH79" s="75"/>
+      <c r="EI79" s="75"/>
+      <c r="EJ79" s="75"/>
+      <c r="EK79" s="75"/>
+      <c r="EL79" s="75"/>
+      <c r="EM79" s="75"/>
+      <c r="EN79" s="75"/>
+      <c r="EO79" s="75"/>
+      <c r="EP79" s="75"/>
+      <c r="EQ79" s="75"/>
+      <c r="ER79" s="75"/>
+      <c r="ES79" s="75"/>
+      <c r="ET79" s="75"/>
+      <c r="EU79" s="75"/>
+      <c r="EV79" s="75"/>
+      <c r="EW79" s="75"/>
+      <c r="EX79" s="75"/>
+      <c r="EY79" s="75"/>
+      <c r="EZ79" s="75"/>
+      <c r="FA79" s="75"/>
+      <c r="FB79" s="75"/>
+      <c r="FC79" s="75"/>
+      <c r="FD79" s="75"/>
+      <c r="FE79" s="75"/>
+      <c r="FF79" s="75"/>
+      <c r="FG79" s="75"/>
+      <c r="FH79" s="75"/>
+      <c r="FI79" s="75"/>
+      <c r="FJ79" s="75"/>
+      <c r="FK79" s="75"/>
+      <c r="FL79" s="75"/>
+      <c r="FM79" s="75"/>
+      <c r="FN79" s="75"/>
+      <c r="FO79" s="75"/>
+      <c r="FP79" s="75"/>
+      <c r="FQ79" s="75"/>
+      <c r="FR79" s="75"/>
+      <c r="FS79" s="75"/>
+      <c r="FT79" s="75"/>
+      <c r="FU79" s="75"/>
+      <c r="FV79" s="75"/>
+      <c r="FW79" s="75"/>
+      <c r="FX79" s="75"/>
+      <c r="FY79" s="75"/>
+      <c r="FZ79" s="75"/>
+      <c r="GA79" s="75"/>
+      <c r="GB79" s="75"/>
+      <c r="GC79" s="75"/>
+      <c r="GD79" s="75"/>
+      <c r="GE79" s="75"/>
+      <c r="GF79" s="75"/>
+      <c r="GG79" s="75"/>
+      <c r="GH79" s="75"/>
+      <c r="GI79" s="75"/>
+      <c r="GJ79" s="75"/>
+      <c r="GK79" s="75"/>
+      <c r="GL79" s="75"/>
+      <c r="GM79" s="75"/>
+      <c r="GN79" s="75"/>
+      <c r="GO79" s="75"/>
+      <c r="GP79" s="75"/>
+      <c r="GQ79" s="75"/>
+      <c r="GR79" s="75"/>
+      <c r="GS79" s="75"/>
+      <c r="GT79" s="75"/>
+      <c r="GU79" s="75"/>
+      <c r="GV79" s="75"/>
+      <c r="GW79" s="75"/>
+      <c r="GX79" s="75"/>
+      <c r="GY79" s="75"/>
+      <c r="GZ79" s="75"/>
+      <c r="HA79" s="75"/>
+      <c r="HB79" s="75"/>
+      <c r="HC79" s="75"/>
+      <c r="HD79" s="75"/>
+      <c r="HE79" s="75"/>
+      <c r="HF79" s="75"/>
+      <c r="HG79" s="75"/>
+      <c r="HH79" s="75"/>
+      <c r="HI79" s="75"/>
+      <c r="HJ79" s="75"/>
+      <c r="HK79" s="75"/>
+      <c r="HL79" s="75"/>
+      <c r="HM79" s="75"/>
+      <c r="HN79" s="75"/>
+      <c r="HO79" s="75"/>
+      <c r="HP79" s="75"/>
+      <c r="HQ79" s="75"/>
+      <c r="HR79" s="75"/>
+      <c r="HS79" s="75"/>
+      <c r="HT79" s="75"/>
+      <c r="HU79" s="75"/>
+      <c r="HV79" s="75"/>
+      <c r="HW79" s="75"/>
+      <c r="HX79" s="75"/>
+      <c r="HY79" s="75"/>
+      <c r="HZ79" s="75"/>
+      <c r="IA79" s="75"/>
+      <c r="IB79" s="75"/>
+      <c r="IC79" s="75"/>
+      <c r="ID79" s="75"/>
+      <c r="IE79" s="75"/>
+      <c r="IF79" s="75"/>
+      <c r="IG79" s="75"/>
+      <c r="IH79" s="75"/>
+      <c r="II79" s="75"/>
+      <c r="IJ79" s="75"/>
+      <c r="IK79" s="75"/>
+      <c r="IL79" s="75"/>
+      <c r="IM79" s="75"/>
+      <c r="IN79" s="75"/>
+      <c r="IO79" s="75"/>
+      <c r="IP79" s="75"/>
+      <c r="IQ79" s="75"/>
+      <c r="IR79" s="75"/>
+      <c r="IS79" s="75"/>
+      <c r="IT79" s="75"/>
+      <c r="IU79" s="75"/>
+      <c r="IV79" s="75"/>
+      <c r="IW79" s="75"/>
+    </row>
+    <row r="80" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C80" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="D80" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E80" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="F80" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="G80" s="74">
+        <v>0</v>
+      </c>
+      <c r="H80" s="74">
+        <v>1</v>
+      </c>
+      <c r="I80" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="J80" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="K80" s="75"/>
+      <c r="L80" s="75"/>
+      <c r="M80" s="75"/>
+      <c r="N80" s="75"/>
+      <c r="O80" s="75"/>
+      <c r="P80" s="75"/>
+      <c r="Q80" s="75"/>
+      <c r="R80" s="75"/>
+      <c r="S80" s="75"/>
+      <c r="T80" s="75"/>
+      <c r="U80" s="75"/>
+      <c r="V80" s="75"/>
+      <c r="W80" s="75"/>
+      <c r="X80" s="75"/>
+      <c r="Y80" s="75"/>
+      <c r="Z80" s="75"/>
+      <c r="AA80" s="75"/>
+      <c r="AB80" s="75"/>
+      <c r="AC80" s="75"/>
+      <c r="AD80" s="75"/>
+      <c r="AE80" s="75"/>
+      <c r="AF80" s="75"/>
+      <c r="AG80" s="75"/>
+      <c r="AH80" s="75"/>
+      <c r="AI80" s="75"/>
+      <c r="AJ80" s="75"/>
+      <c r="AK80" s="75"/>
+      <c r="AL80" s="75"/>
+      <c r="AM80" s="75"/>
+      <c r="AN80" s="75"/>
+      <c r="AO80" s="75"/>
+      <c r="AP80" s="75"/>
+      <c r="AQ80" s="75"/>
+      <c r="AR80" s="75"/>
+      <c r="AS80" s="75"/>
+      <c r="AT80" s="75"/>
+      <c r="AU80" s="75"/>
+      <c r="AV80" s="75"/>
+      <c r="AW80" s="75"/>
+      <c r="AX80" s="75"/>
+      <c r="AY80" s="75"/>
+      <c r="AZ80" s="75"/>
+      <c r="BA80" s="75"/>
+      <c r="BB80" s="75"/>
+      <c r="BC80" s="75"/>
+      <c r="BD80" s="75"/>
+      <c r="BE80" s="75"/>
+      <c r="BF80" s="75"/>
+      <c r="BG80" s="75"/>
+      <c r="BH80" s="75"/>
+      <c r="BI80" s="75"/>
+      <c r="BJ80" s="75"/>
+      <c r="BK80" s="75"/>
+      <c r="BL80" s="75"/>
+      <c r="BM80" s="75"/>
+      <c r="BN80" s="75"/>
+      <c r="BO80" s="75"/>
+      <c r="BP80" s="75"/>
+      <c r="BQ80" s="75"/>
+      <c r="BR80" s="75"/>
+      <c r="BS80" s="75"/>
+      <c r="BT80" s="75"/>
+      <c r="BU80" s="75"/>
+      <c r="BV80" s="75"/>
+      <c r="BW80" s="75"/>
+      <c r="BX80" s="75"/>
+      <c r="BY80" s="75"/>
+      <c r="BZ80" s="75"/>
+      <c r="CA80" s="75"/>
+      <c r="CB80" s="75"/>
+      <c r="CC80" s="75"/>
+      <c r="CD80" s="75"/>
+      <c r="CE80" s="75"/>
+      <c r="CF80" s="75"/>
+      <c r="CG80" s="75"/>
+      <c r="CH80" s="75"/>
+      <c r="CI80" s="75"/>
+      <c r="CJ80" s="75"/>
+      <c r="CK80" s="75"/>
+      <c r="CL80" s="75"/>
+      <c r="CM80" s="75"/>
+      <c r="CN80" s="75"/>
+      <c r="CO80" s="75"/>
+      <c r="CP80" s="75"/>
+      <c r="CQ80" s="75"/>
+      <c r="CR80" s="75"/>
+      <c r="CS80" s="75"/>
+      <c r="CT80" s="75"/>
+      <c r="CU80" s="75"/>
+      <c r="CV80" s="75"/>
+      <c r="CW80" s="75"/>
+      <c r="CX80" s="75"/>
+      <c r="CY80" s="75"/>
+      <c r="CZ80" s="75"/>
+      <c r="DA80" s="75"/>
+      <c r="DB80" s="75"/>
+      <c r="DC80" s="75"/>
+      <c r="DD80" s="75"/>
+      <c r="DE80" s="75"/>
+      <c r="DF80" s="75"/>
+      <c r="DG80" s="75"/>
+      <c r="DH80" s="75"/>
+      <c r="DI80" s="75"/>
+      <c r="DJ80" s="75"/>
+      <c r="DK80" s="75"/>
+      <c r="DL80" s="75"/>
+      <c r="DM80" s="75"/>
+      <c r="DN80" s="75"/>
+      <c r="DO80" s="75"/>
+      <c r="DP80" s="75"/>
+      <c r="DQ80" s="75"/>
+      <c r="DR80" s="75"/>
+      <c r="DS80" s="75"/>
+      <c r="DT80" s="75"/>
+      <c r="DU80" s="75"/>
+      <c r="DV80" s="75"/>
+      <c r="DW80" s="75"/>
+      <c r="DX80" s="75"/>
+      <c r="DY80" s="75"/>
+      <c r="DZ80" s="75"/>
+      <c r="EA80" s="75"/>
+      <c r="EB80" s="75"/>
+      <c r="EC80" s="75"/>
+      <c r="ED80" s="75"/>
+      <c r="EE80" s="75"/>
+      <c r="EF80" s="75"/>
+      <c r="EG80" s="75"/>
+      <c r="EH80" s="75"/>
+      <c r="EI80" s="75"/>
+      <c r="EJ80" s="75"/>
+      <c r="EK80" s="75"/>
+      <c r="EL80" s="75"/>
+      <c r="EM80" s="75"/>
+      <c r="EN80" s="75"/>
+      <c r="EO80" s="75"/>
+      <c r="EP80" s="75"/>
+      <c r="EQ80" s="75"/>
+      <c r="ER80" s="75"/>
+      <c r="ES80" s="75"/>
+      <c r="ET80" s="75"/>
+      <c r="EU80" s="75"/>
+      <c r="EV80" s="75"/>
+      <c r="EW80" s="75"/>
+      <c r="EX80" s="75"/>
+      <c r="EY80" s="75"/>
+      <c r="EZ80" s="75"/>
+      <c r="FA80" s="75"/>
+      <c r="FB80" s="75"/>
+      <c r="FC80" s="75"/>
+      <c r="FD80" s="75"/>
+      <c r="FE80" s="75"/>
+      <c r="FF80" s="75"/>
+      <c r="FG80" s="75"/>
+      <c r="FH80" s="75"/>
+      <c r="FI80" s="75"/>
+      <c r="FJ80" s="75"/>
+      <c r="FK80" s="75"/>
+      <c r="FL80" s="75"/>
+      <c r="FM80" s="75"/>
+      <c r="FN80" s="75"/>
+      <c r="FO80" s="75"/>
+      <c r="FP80" s="75"/>
+      <c r="FQ80" s="75"/>
+      <c r="FR80" s="75"/>
+      <c r="FS80" s="75"/>
+      <c r="FT80" s="75"/>
+      <c r="FU80" s="75"/>
+      <c r="FV80" s="75"/>
+      <c r="FW80" s="75"/>
+      <c r="FX80" s="75"/>
+      <c r="FY80" s="75"/>
+      <c r="FZ80" s="75"/>
+      <c r="GA80" s="75"/>
+      <c r="GB80" s="75"/>
+      <c r="GC80" s="75"/>
+      <c r="GD80" s="75"/>
+      <c r="GE80" s="75"/>
+      <c r="GF80" s="75"/>
+      <c r="GG80" s="75"/>
+      <c r="GH80" s="75"/>
+      <c r="GI80" s="75"/>
+      <c r="GJ80" s="75"/>
+      <c r="GK80" s="75"/>
+      <c r="GL80" s="75"/>
+      <c r="GM80" s="75"/>
+      <c r="GN80" s="75"/>
+      <c r="GO80" s="75"/>
+      <c r="GP80" s="75"/>
+      <c r="GQ80" s="75"/>
+      <c r="GR80" s="75"/>
+      <c r="GS80" s="75"/>
+      <c r="GT80" s="75"/>
+      <c r="GU80" s="75"/>
+      <c r="GV80" s="75"/>
+      <c r="GW80" s="75"/>
+      <c r="GX80" s="75"/>
+      <c r="GY80" s="75"/>
+      <c r="GZ80" s="75"/>
+      <c r="HA80" s="75"/>
+      <c r="HB80" s="75"/>
+      <c r="HC80" s="75"/>
+      <c r="HD80" s="75"/>
+      <c r="HE80" s="75"/>
+      <c r="HF80" s="75"/>
+      <c r="HG80" s="75"/>
+      <c r="HH80" s="75"/>
+      <c r="HI80" s="75"/>
+      <c r="HJ80" s="75"/>
+      <c r="HK80" s="75"/>
+      <c r="HL80" s="75"/>
+      <c r="HM80" s="75"/>
+      <c r="HN80" s="75"/>
+      <c r="HO80" s="75"/>
+      <c r="HP80" s="75"/>
+      <c r="HQ80" s="75"/>
+      <c r="HR80" s="75"/>
+      <c r="HS80" s="75"/>
+      <c r="HT80" s="75"/>
+      <c r="HU80" s="75"/>
+      <c r="HV80" s="75"/>
+      <c r="HW80" s="75"/>
+      <c r="HX80" s="75"/>
+      <c r="HY80" s="75"/>
+      <c r="HZ80" s="75"/>
+      <c r="IA80" s="75"/>
+      <c r="IB80" s="75"/>
+      <c r="IC80" s="75"/>
+      <c r="ID80" s="75"/>
+      <c r="IE80" s="75"/>
+      <c r="IF80" s="75"/>
+      <c r="IG80" s="75"/>
+      <c r="IH80" s="75"/>
+      <c r="II80" s="75"/>
+      <c r="IJ80" s="75"/>
+      <c r="IK80" s="75"/>
+      <c r="IL80" s="75"/>
+      <c r="IM80" s="75"/>
+      <c r="IN80" s="75"/>
+      <c r="IO80" s="75"/>
+      <c r="IP80" s="75"/>
+      <c r="IQ80" s="75"/>
+      <c r="IR80" s="75"/>
+      <c r="IS80" s="75"/>
+      <c r="IT80" s="75"/>
+      <c r="IU80" s="75"/>
+      <c r="IV80" s="75"/>
+      <c r="IW80" s="75"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A81" s="73"/>
+      <c r="B81" s="73"/>
+      <c r="C81" s="73"/>
+      <c r="D81" s="73"/>
+      <c r="E81" s="73"/>
+      <c r="F81" s="73"/>
+      <c r="G81" s="73"/>
+      <c r="H81" s="73"/>
+      <c r="I81" s="73"/>
+      <c r="J81" s="73"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A82" s="73"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="73"/>
+      <c r="D82" s="73"/>
+      <c r="E82" s="73"/>
+      <c r="F82" s="73"/>
+      <c r="G82" s="73"/>
+      <c r="H82" s="73"/>
+      <c r="I82" s="73"/>
+      <c r="J82" s="73"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A83" s="73"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="73"/>
+      <c r="D83" s="73"/>
+      <c r="E83" s="73"/>
+      <c r="F83" s="73"/>
+      <c r="G83" s="73"/>
+      <c r="H83" s="73"/>
+      <c r="I83" s="73"/>
+      <c r="J83" s="73"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A84" s="73"/>
+      <c r="B84" s="73"/>
+      <c r="C84" s="73"/>
+      <c r="D84" s="73"/>
+      <c r="E84" s="73"/>
+      <c r="F84" s="73"/>
+      <c r="G84" s="73"/>
+      <c r="H84" s="73"/>
+      <c r="I84" s="73"/>
+      <c r="J84" s="73"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A85" s="73"/>
+      <c r="B85" s="73"/>
+      <c r="C85" s="73"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="73"/>
+      <c r="F85" s="73"/>
+      <c r="G85" s="73"/>
+      <c r="H85" s="73"/>
+      <c r="I85" s="73"/>
+      <c r="J85" s="73"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A86" s="73"/>
+      <c r="B86" s="73"/>
+      <c r="C86" s="73"/>
+      <c r="D86" s="73"/>
+      <c r="E86" s="73"/>
+      <c r="F86" s="73"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="73"/>
+      <c r="J86" s="73"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A87" s="73"/>
+      <c r="B87" s="73"/>
+      <c r="C87" s="73"/>
+      <c r="D87" s="73"/>
+      <c r="E87" s="73"/>
+      <c r="F87" s="73"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="73"/>
+      <c r="J87" s="73"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A88" s="73"/>
+      <c r="B88" s="73"/>
+      <c r="C88" s="73"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73"/>
+      <c r="F88" s="73"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A89" s="73"/>
+      <c r="B89" s="73"/>
+      <c r="C89" s="73"/>
+      <c r="D89" s="73"/>
+      <c r="E89" s="73"/>
+      <c r="F89" s="73"/>
+      <c r="G89" s="73"/>
+      <c r="H89" s="73"/>
+      <c r="I89" s="73"/>
+      <c r="J89" s="73"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A90" s="73"/>
+      <c r="B90" s="73"/>
+      <c r="C90" s="73"/>
+      <c r="D90" s="73"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="73"/>
+      <c r="G90" s="73"/>
+      <c r="H90" s="73"/>
+      <c r="I90" s="73"/>
+      <c r="J90" s="73"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A91" s="73"/>
+      <c r="B91" s="73"/>
+      <c r="C91" s="73"/>
+      <c r="D91" s="73"/>
+      <c r="E91" s="73"/>
+      <c r="F91" s="73"/>
+      <c r="G91" s="73"/>
+      <c r="H91" s="73"/>
+      <c r="I91" s="73"/>
+      <c r="J91" s="73"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A92" s="73"/>
+      <c r="B92" s="73"/>
+      <c r="C92" s="73"/>
+      <c r="D92" s="73"/>
+      <c r="E92" s="73"/>
+      <c r="F92" s="73"/>
+      <c r="G92" s="73"/>
+      <c r="H92" s="73"/>
+      <c r="I92" s="73"/>
+      <c r="J92" s="73"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A93" s="73"/>
+      <c r="B93" s="73"/>
+      <c r="C93" s="73"/>
+      <c r="D93" s="73"/>
+      <c r="E93" s="73"/>
+      <c r="F93" s="73"/>
+      <c r="G93" s="73"/>
+      <c r="H93" s="73"/>
+      <c r="I93" s="73"/>
+      <c r="J93" s="73"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A94" s="73"/>
+      <c r="B94" s="73"/>
+      <c r="C94" s="73"/>
+      <c r="D94" s="73"/>
+      <c r="E94" s="73"/>
+      <c r="F94" s="73"/>
+      <c r="G94" s="73"/>
+      <c r="H94" s="73"/>
+      <c r="I94" s="73"/>
+      <c r="J94" s="73"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11377,8 +15884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IW62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView showGridLines="0" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
finished working on update client legal doc for ratanak
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Home/Documents/oscar-web/db/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A566AFC7-D336-7040-9911-1E9D0DCD5B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663BEDF4-DAA3-4526-91E7-9A6209C600CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="224">
   <si>
     <t>name</t>
   </si>
@@ -653,13 +653,58 @@
   </si>
   <si>
     <t>Forms for Identification of Victim of Human Trafficking</t>
+  </si>
+  <si>
+    <t>referral_document</t>
+  </si>
+  <si>
+    <t>travel_doc</t>
+  </si>
+  <si>
+    <t>Laissez-Passer</t>
+  </si>
+  <si>
+    <t>Screening Interview Form</t>
+  </si>
+  <si>
+    <t>local_consent</t>
+  </si>
+  <si>
+    <t>Legal Representation</t>
+  </si>
+  <si>
+    <t>police_interview</t>
+  </si>
+  <si>
+    <t>Letter from Immigration Police</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labour Trafficking </t>
+  </si>
+  <si>
+    <t>Sexual Trafficking</t>
+  </si>
+  <si>
+    <t>labor_trafficking_legal_doc_option</t>
+  </si>
+  <si>
+    <t>sex_trafficking_legal_doc_option</t>
+  </si>
+  <si>
+    <t>other_legal_doc_option</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1035,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1173,6 +1218,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1558,26 +1605,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW130"/>
+  <dimension ref="A1:IW129"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.83203125" style="1"/>
+    <col min="6" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -1609,7 +1656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="66" t="s">
         <v>10</v>
       </c>
@@ -1637,7 +1684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="68" t="s">
         <v>16</v>
       </c>
@@ -1665,7 +1712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="68" t="s">
         <v>18</v>
       </c>
@@ -1693,7 +1740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="68" t="s">
         <v>20</v>
       </c>
@@ -1721,7 +1768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="68" t="s">
         <v>22</v>
       </c>
@@ -1749,7 +1796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="68" t="s">
         <v>18</v>
       </c>
@@ -1777,7 +1824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="68" t="s">
         <v>24</v>
       </c>
@@ -1805,7 +1852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -1835,7 +1882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -1865,7 +1912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -1895,7 +1942,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -1925,7 +1972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="68" t="s">
         <v>36</v>
       </c>
@@ -1953,7 +2000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="68" t="s">
         <v>38</v>
       </c>
@@ -1981,7 +2028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="68" t="s">
         <v>41</v>
       </c>
@@ -2009,7 +2056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>43</v>
       </c>
@@ -2039,7 +2086,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>45</v>
       </c>
@@ -2069,7 +2116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>47</v>
       </c>
@@ -2099,7 +2146,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>138</v>
       </c>
@@ -2153,7 +2200,7 @@
       </c>
       <c r="IW19" s="25"/>
     </row>
-    <row r="20" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="77" t="s">
         <v>136</v>
       </c>
@@ -2428,7 +2475,7 @@
       <c r="IV20"/>
       <c r="IW20"/>
     </row>
-    <row r="21" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="77" t="s">
         <v>141</v>
       </c>
@@ -2703,7 +2750,7 @@
       <c r="IV21"/>
       <c r="IW21"/>
     </row>
-    <row r="22" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="82" t="s">
         <v>51</v>
       </c>
@@ -2732,7 +2779,7 @@
       </c>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="82" t="s">
         <v>53</v>
       </c>
@@ -2760,7 +2807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>55</v>
       </c>
@@ -2790,7 +2837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>57</v>
       </c>
@@ -2820,7 +2867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="19" t="s">
         <v>60</v>
       </c>
@@ -2850,7 +2897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>62</v>
       </c>
@@ -2880,7 +2927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>64</v>
       </c>
@@ -2910,7 +2957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="19" t="s">
         <v>66</v>
       </c>
@@ -2940,7 +2987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="19" t="s">
         <v>68</v>
       </c>
@@ -2970,7 +3017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="11" t="s">
         <v>70</v>
       </c>
@@ -3000,7 +3047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="19" t="s">
         <v>72</v>
       </c>
@@ -3030,7 +3077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="19" t="s">
         <v>73</v>
       </c>
@@ -3060,7 +3107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:257" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="19" t="s">
         <v>74</v>
       </c>
@@ -3090,7 +3137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="19" t="s">
         <v>75</v>
       </c>
@@ -3367,7 +3414,7 @@
       <c r="IV35"/>
       <c r="IW35"/>
     </row>
-    <row r="36" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="19" t="s">
         <v>76</v>
       </c>
@@ -3644,7 +3691,7 @@
       <c r="IV36"/>
       <c r="IW36"/>
     </row>
-    <row r="37" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="19" t="s">
         <v>77</v>
       </c>
@@ -3921,7 +3968,7 @@
       <c r="IV37"/>
       <c r="IW37"/>
     </row>
-    <row r="38" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="19" t="s">
         <v>79</v>
       </c>
@@ -4198,7 +4245,7 @@
       <c r="IV38"/>
       <c r="IW38"/>
     </row>
-    <row r="39" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="19" t="s">
         <v>81</v>
       </c>
@@ -4475,7 +4522,7 @@
       <c r="IV39"/>
       <c r="IW39"/>
     </row>
-    <row r="40" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="19" t="s">
         <v>83</v>
       </c>
@@ -4752,7 +4799,7 @@
       <c r="IV40"/>
       <c r="IW40"/>
     </row>
-    <row r="41" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="19" t="s">
         <v>85</v>
       </c>
@@ -5029,7 +5076,7 @@
       <c r="IV41"/>
       <c r="IW41"/>
     </row>
-    <row r="42" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="19" t="s">
         <v>87</v>
       </c>
@@ -5306,7 +5353,7 @@
       <c r="IV42"/>
       <c r="IW42"/>
     </row>
-    <row r="43" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="19" t="s">
         <v>89</v>
       </c>
@@ -5583,7 +5630,7 @@
       <c r="IV43"/>
       <c r="IW43"/>
     </row>
-    <row r="44" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="19" t="s">
         <v>91</v>
       </c>
@@ -5860,7 +5907,7 @@
       <c r="IV44"/>
       <c r="IW44"/>
     </row>
-    <row r="45" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="19" t="s">
         <v>92</v>
       </c>
@@ -6137,7 +6184,7 @@
       <c r="IV45"/>
       <c r="IW45"/>
     </row>
-    <row r="46" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="53" t="s">
         <v>94</v>
       </c>
@@ -6412,7 +6459,7 @@
       <c r="IV46"/>
       <c r="IW46"/>
     </row>
-    <row r="47" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="87" t="s">
         <v>97</v>
       </c>
@@ -6689,7 +6736,7 @@
       <c r="IV47"/>
       <c r="IW47"/>
     </row>
-    <row r="48" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="87" t="s">
         <v>77</v>
       </c>
@@ -6964,7 +7011,7 @@
       <c r="IV48"/>
       <c r="IW48"/>
     </row>
-    <row r="49" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="87" t="s">
         <v>22</v>
       </c>
@@ -7239,7 +7286,7 @@
       <c r="IV49"/>
       <c r="IW49"/>
     </row>
-    <row r="50" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="87" t="s">
         <v>0</v>
       </c>
@@ -7514,7 +7561,7 @@
       <c r="IV50"/>
       <c r="IW50"/>
     </row>
-    <row r="51" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="87" t="s">
         <v>79</v>
       </c>
@@ -7789,7 +7836,7 @@
       <c r="IV51"/>
       <c r="IW51"/>
     </row>
-    <row r="52" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="87" t="s">
         <v>81</v>
       </c>
@@ -8064,7 +8111,7 @@
       <c r="IV52"/>
       <c r="IW52"/>
     </row>
-    <row r="53" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="87" t="s">
         <v>83</v>
       </c>
@@ -8339,7 +8386,7 @@
       <c r="IV53"/>
       <c r="IW53"/>
     </row>
-    <row r="54" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="87" t="s">
         <v>101</v>
       </c>
@@ -8614,7 +8661,7 @@
       <c r="IV54"/>
       <c r="IW54"/>
     </row>
-    <row r="55" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="87" t="s">
         <v>102</v>
       </c>
@@ -8889,7 +8936,7 @@
       <c r="IV55"/>
       <c r="IW55"/>
     </row>
-    <row r="56" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="87" t="s">
         <v>104</v>
       </c>
@@ -9164,7 +9211,7 @@
       <c r="IV56"/>
       <c r="IW56"/>
     </row>
-    <row r="57" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="87" t="s">
         <v>106</v>
       </c>
@@ -9439,7 +9486,7 @@
       <c r="IV57"/>
       <c r="IW57"/>
     </row>
-    <row r="58" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="87" t="s">
         <v>108</v>
       </c>
@@ -9714,7 +9761,7 @@
       <c r="IV58"/>
       <c r="IW58"/>
     </row>
-    <row r="59" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A59" s="53" t="s">
         <v>111</v>
       </c>
@@ -9989,7 +10036,7 @@
       <c r="IV59"/>
       <c r="IW59"/>
     </row>
-    <row r="60" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A60" s="53" t="s">
         <v>113</v>
       </c>
@@ -10264,7 +10311,7 @@
       <c r="IV60"/>
       <c r="IW60"/>
     </row>
-    <row r="61" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A61" s="92" t="s">
         <v>22</v>
       </c>
@@ -10539,7 +10586,7 @@
       <c r="IV61"/>
       <c r="IW61"/>
     </row>
-    <row r="62" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A62" s="53" t="s">
         <v>115</v>
       </c>
@@ -10814,7 +10861,7 @@
       <c r="IV62"/>
       <c r="IW62"/>
     </row>
-    <row r="63" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A63" s="53" t="s">
         <v>117</v>
       </c>
@@ -11089,7 +11136,7 @@
       <c r="IV63"/>
       <c r="IW63"/>
     </row>
-    <row r="64" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A64" s="40" t="s">
         <v>119</v>
       </c>
@@ -11366,7 +11413,7 @@
       <c r="IV64"/>
       <c r="IW64"/>
     </row>
-    <row r="65" spans="1:257" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A65" s="53" t="s">
         <v>120</v>
       </c>
@@ -11643,7 +11690,7 @@
       <c r="IV65"/>
       <c r="IW65"/>
     </row>
-    <row r="66" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A66" s="62" t="s">
         <v>143</v>
       </c>
@@ -11920,7 +11967,7 @@
       <c r="IV66" s="64"/>
       <c r="IW66" s="64"/>
     </row>
-    <row r="67" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A67" s="63" t="s">
         <v>144</v>
       </c>
@@ -12197,7 +12244,7 @@
       <c r="IV67" s="64"/>
       <c r="IW67" s="64"/>
     </row>
-    <row r="68" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A68" s="62" t="s">
         <v>145</v>
       </c>
@@ -12474,7 +12521,7 @@
       <c r="IV68" s="64"/>
       <c r="IW68" s="64"/>
     </row>
-    <row r="69" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A69" s="62" t="s">
         <v>146</v>
       </c>
@@ -12751,7 +12798,7 @@
       <c r="IV69" s="64"/>
       <c r="IW69" s="64"/>
     </row>
-    <row r="70" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A70" s="62" t="s">
         <v>147</v>
       </c>
@@ -13028,7 +13075,7 @@
       <c r="IV70" s="64"/>
       <c r="IW70" s="64"/>
     </row>
-    <row r="71" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A71" s="62" t="s">
         <v>148</v>
       </c>
@@ -13305,7 +13352,7 @@
       <c r="IV71" s="64"/>
       <c r="IW71" s="64"/>
     </row>
-    <row r="72" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A72" s="62" t="s">
         <v>149</v>
       </c>
@@ -13582,7 +13629,7 @@
       <c r="IV72" s="64"/>
       <c r="IW72" s="64"/>
     </row>
-    <row r="73" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A73" s="62" t="s">
         <v>150</v>
       </c>
@@ -13859,7 +13906,7 @@
       <c r="IV73" s="64"/>
       <c r="IW73" s="64"/>
     </row>
-    <row r="74" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A74" s="62" t="s">
         <v>151</v>
       </c>
@@ -14136,7 +14183,7 @@
       <c r="IV74" s="64"/>
       <c r="IW74" s="64"/>
     </row>
-    <row r="75" spans="1:257" s="65" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A75" s="62" t="s">
         <v>152</v>
       </c>
@@ -14413,7 +14460,7 @@
       <c r="IV75" s="64"/>
       <c r="IW75" s="64"/>
     </row>
-    <row r="76" spans="1:257" s="61" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A76" s="59" t="s">
         <v>153</v>
       </c>
@@ -14690,7 +14737,7 @@
       <c r="IV76" s="60"/>
       <c r="IW76" s="60"/>
     </row>
-    <row r="77" spans="1:257" s="61" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A77" s="59" t="s">
         <v>154</v>
       </c>
@@ -14967,7 +15014,7 @@
       <c r="IV77" s="60"/>
       <c r="IW77" s="60"/>
     </row>
-    <row r="78" spans="1:257" s="61" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A78" s="59" t="s">
         <v>143</v>
       </c>
@@ -15244,7 +15291,7 @@
       <c r="IV78" s="60"/>
       <c r="IW78" s="60"/>
     </row>
-    <row r="79" spans="1:257" s="61" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A79" s="59" t="s">
         <v>155</v>
       </c>
@@ -15521,7 +15568,7 @@
       <c r="IV79" s="60"/>
       <c r="IW79" s="60"/>
     </row>
-    <row r="80" spans="1:257" s="61" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A80" s="59" t="s">
         <v>156</v>
       </c>
@@ -15798,7 +15845,7 @@
       <c r="IV80" s="60"/>
       <c r="IW80" s="60"/>
     </row>
-    <row r="81" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="58" t="s">
         <v>175</v>
       </c>
@@ -15826,7 +15873,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A82" s="58" t="s">
         <v>177</v>
       </c>
@@ -15854,7 +15901,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A83" s="58" t="s">
         <v>179</v>
       </c>
@@ -15882,7 +15929,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A84" s="58" t="s">
         <v>181</v>
       </c>
@@ -15910,7 +15957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A85" s="58" t="s">
         <v>183</v>
       </c>
@@ -15938,7 +15985,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A86" s="58" t="s">
         <v>185</v>
       </c>
@@ -15966,7 +16013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A87" s="58" t="s">
         <v>187</v>
       </c>
@@ -15994,7 +16041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A88" s="58" t="s">
         <v>189</v>
       </c>
@@ -16022,7 +16069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A89" s="58" t="s">
         <v>191</v>
       </c>
@@ -16050,7 +16097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A90" s="58" t="s">
         <v>193</v>
       </c>
@@ -16078,7 +16125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A91" s="58" t="s">
         <v>195</v>
       </c>
@@ -16106,7 +16153,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A92" s="58" t="s">
         <v>197</v>
       </c>
@@ -16134,7 +16181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A93" s="58" t="s">
         <v>200</v>
       </c>
@@ -16162,7 +16209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:10" ht="18" customHeight="1">
       <c r="A94" s="58" t="s">
         <v>201</v>
       </c>
@@ -16190,9 +16237,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A95" s="58" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B95" s="58" t="s">
         <v>11</v>
@@ -16218,7 +16265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A96" s="58" t="s">
         <v>205</v>
       </c>
@@ -16246,7 +16293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A97" s="58" t="s">
         <v>207</v>
       </c>
@@ -16274,130 +16321,242 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="58"/>
-      <c r="B98" s="58"/>
-      <c r="C98" s="58"/>
+    <row r="98" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A98" s="95" t="s">
+        <v>210</v>
+      </c>
+      <c r="B98" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" s="95" t="s">
+        <v>211</v>
+      </c>
       <c r="D98" s="58"/>
-      <c r="E98" s="58"/>
-      <c r="F98" s="58"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="58"/>
-      <c r="I98" s="58"/>
-      <c r="J98" s="58"/>
+      <c r="E98" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F98" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="58">
+        <v>0</v>
+      </c>
+      <c r="H98" s="58">
+        <v>1</v>
+      </c>
+      <c r="I98" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J98" s="95" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="99" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="58"/>
-      <c r="B99" s="58"/>
-      <c r="C99" s="58"/>
+    <row r="99" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A99" s="95" t="s">
+        <v>203</v>
+      </c>
+      <c r="B99" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="95" t="s">
+        <v>212</v>
+      </c>
       <c r="D99" s="58"/>
-      <c r="E99" s="58"/>
-      <c r="F99" s="58"/>
-      <c r="G99" s="58"/>
-      <c r="H99" s="58"/>
-      <c r="I99" s="58"/>
-      <c r="J99" s="58"/>
+      <c r="E99" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="58">
+        <v>0</v>
+      </c>
+      <c r="H99" s="58">
+        <v>1</v>
+      </c>
+      <c r="I99" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J99" s="95" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="100" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="58"/>
-      <c r="B100" s="58"/>
-      <c r="C100" s="58"/>
+    <row r="100" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A100" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="B100" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="95" t="s">
+        <v>214</v>
+      </c>
       <c r="D100" s="58"/>
-      <c r="E100" s="58"/>
-      <c r="F100" s="58"/>
-      <c r="G100" s="58"/>
-      <c r="H100" s="58"/>
-      <c r="I100" s="58"/>
-      <c r="J100" s="58"/>
+      <c r="E100" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" s="58">
+        <v>0</v>
+      </c>
+      <c r="H100" s="58">
+        <v>1</v>
+      </c>
+      <c r="I100" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J100" s="95" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="101" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="58"/>
-      <c r="B101" s="58"/>
-      <c r="C101" s="58"/>
+    <row r="101" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A101" s="95" t="s">
+        <v>215</v>
+      </c>
+      <c r="B101" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="95" t="s">
+        <v>216</v>
+      </c>
       <c r="D101" s="58"/>
-      <c r="E101" s="58"/>
-      <c r="F101" s="58"/>
-      <c r="G101" s="58"/>
-      <c r="H101" s="58"/>
-      <c r="I101" s="58"/>
-      <c r="J101" s="58"/>
+      <c r="E101" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" s="58">
+        <v>0</v>
+      </c>
+      <c r="H101" s="58">
+        <v>1</v>
+      </c>
+      <c r="I101" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J101" s="95" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="102" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="58"/>
+    <row r="102" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A102" s="95" t="s">
+        <v>219</v>
+      </c>
       <c r="B102" s="58"/>
-      <c r="C102" s="58"/>
+      <c r="C102" s="95" t="s">
+        <v>217</v>
+      </c>
       <c r="D102" s="58"/>
-      <c r="E102" s="58"/>
-      <c r="F102" s="58"/>
-      <c r="G102" s="58"/>
-      <c r="H102" s="58"/>
-      <c r="I102" s="58"/>
-      <c r="J102" s="58"/>
+      <c r="E102" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102" s="58">
+        <v>0</v>
+      </c>
+      <c r="H102" s="58">
+        <v>1</v>
+      </c>
+      <c r="I102" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J102" s="95" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="103" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="58"/>
+    <row r="103" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A103" s="95" t="s">
+        <v>220</v>
+      </c>
       <c r="B103" s="58"/>
-      <c r="C103" s="58"/>
+      <c r="C103" s="95" t="s">
+        <v>218</v>
+      </c>
       <c r="D103" s="58"/>
-      <c r="E103" s="58"/>
-      <c r="F103" s="58"/>
-      <c r="G103" s="58"/>
-      <c r="H103" s="58"/>
-      <c r="I103" s="58"/>
-      <c r="J103" s="58"/>
+      <c r="E103" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" s="58">
+        <v>0</v>
+      </c>
+      <c r="H103" s="58">
+        <v>1</v>
+      </c>
+      <c r="I103" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J103" s="95" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="104" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="58"/>
+    <row r="104" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A104" s="95" t="s">
+        <v>221</v>
+      </c>
       <c r="B104" s="58"/>
-      <c r="C104" s="58"/>
+      <c r="C104" s="95" t="s">
+        <v>223</v>
+      </c>
       <c r="D104" s="58"/>
-      <c r="E104" s="58"/>
-      <c r="F104" s="58"/>
-      <c r="G104" s="58"/>
-      <c r="H104" s="58"/>
-      <c r="I104" s="58"/>
-      <c r="J104" s="58"/>
+      <c r="E104" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G104" s="58">
+        <v>0</v>
+      </c>
+      <c r="H104" s="58">
+        <v>1</v>
+      </c>
+      <c r="I104" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J104" s="95" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="105" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="58"/>
-      <c r="B105" s="58"/>
-      <c r="C105" s="58"/>
-      <c r="D105" s="58"/>
-      <c r="E105" s="58"/>
-      <c r="F105" s="58"/>
-      <c r="G105" s="58"/>
-      <c r="H105" s="58"/>
-      <c r="I105" s="58"/>
-      <c r="J105" s="58"/>
+    <row r="105" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="106" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="107" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="108" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="109" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="110" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="111" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="112" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="113" spans="3:3" ht="17.100000000000001" customHeight="1">
+      <c r="C113" s="96" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="106" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="115" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="116" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="117" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="118" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="119" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="120" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="121" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="122" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="123" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="124" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="125" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="126" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="128" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="129" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
@@ -16412,17 +16571,17 @@
       <selection activeCell="A63" sqref="A63:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16454,7 +16613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17.45" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -16484,7 +16643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="13.7" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -16514,7 +16673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13.7" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -16544,7 +16703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="13.7" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -16574,7 +16733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="13.7" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -16604,7 +16763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.7" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -16634,7 +16793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="13.7" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -16664,7 +16823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="13.7" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -16696,7 +16855,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="13.7" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -16728,7 +16887,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="13.7" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -16760,7 +16919,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="13.7" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -16789,7 +16948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="13.7" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -16819,7 +16978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="13.7" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -16846,7 +17005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="13.7" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -16873,7 +17032,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -16905,7 +17064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -16937,7 +17096,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>47</v>
       </c>
@@ -16969,7 +17128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="26" t="s">
         <v>49</v>
       </c>
@@ -16999,7 +17158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="26" t="s">
         <v>51</v>
       </c>
@@ -17029,7 +17188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>53</v>
       </c>
@@ -17056,7 +17215,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="13.7" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
@@ -17088,7 +17247,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="13.7" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>57</v>
       </c>
@@ -17120,7 +17279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" customHeight="1">
       <c r="A24" s="29" t="s">
         <v>60</v>
       </c>
@@ -17152,7 +17311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="29" t="s">
         <v>62</v>
       </c>
@@ -17184,7 +17343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" customHeight="1">
       <c r="A26" s="29" t="s">
         <v>133</v>
       </c>
@@ -17216,7 +17375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" customHeight="1">
       <c r="A27" s="29" t="s">
         <v>64</v>
       </c>
@@ -17248,7 +17407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="29" t="s">
         <v>66</v>
       </c>
@@ -17280,7 +17439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" customHeight="1">
       <c r="A29" s="29" t="s">
         <v>68</v>
       </c>
@@ -17312,7 +17471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="12.75" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>70</v>
       </c>
@@ -17344,7 +17503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" customHeight="1">
       <c r="A31" s="29" t="s">
         <v>72</v>
       </c>
@@ -17376,7 +17535,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" customHeight="1">
       <c r="A32" s="29" t="s">
         <v>73</v>
       </c>
@@ -17408,7 +17567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:257" ht="12.75" customHeight="1">
       <c r="A33" s="29" t="s">
         <v>74</v>
       </c>
@@ -17440,7 +17599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:257" ht="12.75" customHeight="1">
       <c r="A34" s="29" t="s">
         <v>75</v>
       </c>
@@ -17472,7 +17631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:257" ht="12.75" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>76</v>
       </c>
@@ -17504,7 +17663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:257" ht="12.75" customHeight="1">
       <c r="A36" s="29" t="s">
         <v>77</v>
       </c>
@@ -17534,7 +17693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:257" ht="12.75" customHeight="1">
       <c r="A37" s="29" t="s">
         <v>79</v>
       </c>
@@ -17564,7 +17723,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:257" ht="12.75" customHeight="1">
       <c r="A38" s="29" t="s">
         <v>81</v>
       </c>
@@ -17594,7 +17753,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:257" ht="12.75" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>83</v>
       </c>
@@ -17624,7 +17783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:257" ht="12.75" customHeight="1">
       <c r="A40" s="29" t="s">
         <v>85</v>
       </c>
@@ -17654,7 +17813,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:257" ht="12.75" customHeight="1">
       <c r="A41" s="29" t="s">
         <v>87</v>
       </c>
@@ -17684,7 +17843,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:257" ht="12.75" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>89</v>
       </c>
@@ -17714,7 +17873,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:257" ht="12.75" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>91</v>
       </c>
@@ -17744,7 +17903,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:257" ht="12.75" customHeight="1">
       <c r="A44" s="29" t="s">
         <v>92</v>
       </c>
@@ -17774,7 +17933,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:257" ht="12.75" customHeight="1">
       <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
@@ -17804,7 +17963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:257" ht="12.75" customHeight="1">
       <c r="A46" s="41" t="s">
         <v>97</v>
       </c>
@@ -18081,7 +18240,7 @@
       <c r="IV46" s="55"/>
       <c r="IW46" s="55"/>
     </row>
-    <row r="47" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:257" ht="12.75" customHeight="1">
       <c r="A47" s="46" t="s">
         <v>77</v>
       </c>
@@ -18356,7 +18515,7 @@
       <c r="IV47" s="55"/>
       <c r="IW47" s="55"/>
     </row>
-    <row r="48" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:257" ht="12.75" customHeight="1">
       <c r="A48" s="46" t="s">
         <v>79</v>
       </c>
@@ -18631,7 +18790,7 @@
       <c r="IV48" s="55"/>
       <c r="IW48" s="55"/>
     </row>
-    <row r="49" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:257" ht="12.75" customHeight="1">
       <c r="A49" s="46" t="s">
         <v>81</v>
       </c>
@@ -18906,7 +19065,7 @@
       <c r="IV49" s="55"/>
       <c r="IW49" s="55"/>
     </row>
-    <row r="50" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:257" ht="12.75" customHeight="1">
       <c r="A50" s="46" t="s">
         <v>83</v>
       </c>
@@ -19181,7 +19340,7 @@
       <c r="IV50" s="55"/>
       <c r="IW50" s="55"/>
     </row>
-    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:257" ht="12.75" customHeight="1">
       <c r="A51" s="46" t="s">
         <v>101</v>
       </c>
@@ -19456,7 +19615,7 @@
       <c r="IV51" s="55"/>
       <c r="IW51" s="55"/>
     </row>
-    <row r="52" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:257" ht="12.75" customHeight="1">
       <c r="A52" s="46" t="s">
         <v>102</v>
       </c>
@@ -19731,7 +19890,7 @@
       <c r="IV52" s="55"/>
       <c r="IW52" s="55"/>
     </row>
-    <row r="53" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:257" ht="12.75" customHeight="1">
       <c r="A53" s="46" t="s">
         <v>104</v>
       </c>
@@ -20006,7 +20165,7 @@
       <c r="IV53" s="55"/>
       <c r="IW53" s="55"/>
     </row>
-    <row r="54" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:257" ht="12.75" customHeight="1">
       <c r="A54" s="46" t="s">
         <v>106</v>
       </c>
@@ -20281,7 +20440,7 @@
       <c r="IV54" s="55"/>
       <c r="IW54" s="55"/>
     </row>
-    <row r="55" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:257" ht="12.75" customHeight="1">
       <c r="A55" s="46" t="s">
         <v>108</v>
       </c>
@@ -20556,7 +20715,7 @@
       <c r="IV55" s="55"/>
       <c r="IW55" s="55"/>
     </row>
-    <row r="56" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:257" ht="12.75" customHeight="1">
       <c r="A56" s="35" t="s">
         <v>22</v>
       </c>
@@ -20588,7 +20747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:257" ht="12.75" customHeight="1">
       <c r="A57" s="35" t="s">
         <v>111</v>
       </c>
@@ -20615,7 +20774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:257" ht="12.75" customHeight="1">
       <c r="A58" s="35" t="s">
         <v>117</v>
       </c>
@@ -20642,7 +20801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:257" ht="12.75" customHeight="1">
       <c r="A59" s="35" t="s">
         <v>113</v>
       </c>
@@ -20669,7 +20828,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:257" ht="12.75" customHeight="1">
       <c r="A60" s="35" t="s">
         <v>115</v>
       </c>
@@ -20699,7 +20858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:257" ht="12.75" customHeight="1">
       <c r="A61" s="37" t="s">
         <v>119</v>
       </c>
@@ -20731,7 +20890,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:257" ht="12.75" customHeight="1">
       <c r="A62" s="35" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
update user and partner header for haiti
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Home/Documents/oscar-web/db/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE9AFA-6490-304F-AC1A-17C4312ABD51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276ED3A-5BE9-4851-A7F6-5B51A532A839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31290" yWindow="1050" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="144">
   <si>
     <t>name</t>
   </si>
@@ -456,12 +456,15 @@
   <si>
     <t>View Screening Assessment</t>
   </si>
+  <si>
+    <t>user</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1324,26 +1327,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW65"/>
+  <dimension ref="A1:IW67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.83203125" style="1"/>
+    <col min="6" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17.45" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="13.7" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13.7" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="13.7" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="13.7" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.7" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="13.7" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="13.7" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="13.7" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="13.7" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="13.7" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="13.7" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="13.7" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="13.7" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:257" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:257" ht="15" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>47</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:257" ht="15" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>138</v>
       </c>
@@ -1905,7 +1908,7 @@
       </c>
       <c r="IW19" s="25"/>
     </row>
-    <row r="20" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:257" ht="15" customHeight="1">
       <c r="A20" s="62" t="s">
         <v>136</v>
       </c>
@@ -2180,7 +2183,7 @@
       <c r="IV20"/>
       <c r="IW20"/>
     </row>
-    <row r="21" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:257" ht="15" customHeight="1">
       <c r="A21" s="62" t="s">
         <v>141</v>
       </c>
@@ -2455,7 +2458,7 @@
       <c r="IV21"/>
       <c r="IW21"/>
     </row>
-    <row r="22" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:257" ht="15" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>51</v>
       </c>
@@ -2483,7 +2486,7 @@
       </c>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:257" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:257" ht="13.7" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>53</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:257" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:257" ht="13.7" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:257" ht="12.75" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>57</v>
       </c>
@@ -2568,7 +2571,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:257" ht="12.75" customHeight="1">
       <c r="A26" s="29" t="s">
         <v>60</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:257" ht="12.75" customHeight="1">
       <c r="A27" s="29" t="s">
         <v>62</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:257" ht="12.75" customHeight="1">
       <c r="A28" s="29" t="s">
         <v>64</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:257" ht="12.75" customHeight="1">
       <c r="A29" s="29" t="s">
         <v>66</v>
       </c>
@@ -2684,7 +2687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:257" ht="12.75" customHeight="1">
       <c r="A30" s="29" t="s">
         <v>68</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:257" ht="12.75" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>70</v>
       </c>
@@ -2742,7 +2745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:257" ht="12.75" customHeight="1">
       <c r="A32" s="29" t="s">
         <v>72</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:257" ht="12.75" customHeight="1">
       <c r="A33" s="29" t="s">
         <v>73</v>
       </c>
@@ -2800,7 +2803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" s="1" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:257" s="1" customFormat="1" hidden="1">
       <c r="A34" s="29" t="s">
         <v>74</v>
       </c>
@@ -2829,7 +2832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:257" ht="12.75" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>75</v>
       </c>
@@ -3105,7 +3108,7 @@
       <c r="IV35"/>
       <c r="IW35"/>
     </row>
-    <row r="36" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:257" ht="12.75" customHeight="1">
       <c r="A36" s="29" t="s">
         <v>76</v>
       </c>
@@ -3381,7 +3384,7 @@
       <c r="IV36"/>
       <c r="IW36"/>
     </row>
-    <row r="37" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:257" ht="12.75" customHeight="1">
       <c r="A37" s="29" t="s">
         <v>77</v>
       </c>
@@ -3657,7 +3660,7 @@
       <c r="IV37"/>
       <c r="IW37"/>
     </row>
-    <row r="38" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:257" ht="12.75" customHeight="1">
       <c r="A38" s="29" t="s">
         <v>79</v>
       </c>
@@ -3933,7 +3936,7 @@
       <c r="IV38"/>
       <c r="IW38"/>
     </row>
-    <row r="39" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:257" ht="12.75" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>81</v>
       </c>
@@ -4209,7 +4212,7 @@
       <c r="IV39"/>
       <c r="IW39"/>
     </row>
-    <row r="40" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:257" ht="12.75" customHeight="1">
       <c r="A40" s="29" t="s">
         <v>83</v>
       </c>
@@ -4485,7 +4488,7 @@
       <c r="IV40"/>
       <c r="IW40"/>
     </row>
-    <row r="41" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:257" ht="12.75" customHeight="1">
       <c r="A41" s="29" t="s">
         <v>85</v>
       </c>
@@ -4761,7 +4764,7 @@
       <c r="IV41"/>
       <c r="IW41"/>
     </row>
-    <row r="42" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:257" ht="12.75" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>87</v>
       </c>
@@ -5037,7 +5040,7 @@
       <c r="IV42"/>
       <c r="IW42"/>
     </row>
-    <row r="43" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:257" ht="12.75" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>89</v>
       </c>
@@ -5313,7 +5316,7 @@
       <c r="IV43"/>
       <c r="IW43"/>
     </row>
-    <row r="44" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:257" ht="12.75" customHeight="1">
       <c r="A44" s="29" t="s">
         <v>91</v>
       </c>
@@ -5589,7 +5592,7 @@
       <c r="IV44"/>
       <c r="IW44"/>
     </row>
-    <row r="45" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:257" ht="12.75" customHeight="1">
       <c r="A45" s="29" t="s">
         <v>92</v>
       </c>
@@ -5865,7 +5868,7 @@
       <c r="IV45"/>
       <c r="IW45"/>
     </row>
-    <row r="46" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:257" ht="12.75" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>94</v>
       </c>
@@ -6140,7 +6143,7 @@
       <c r="IV46"/>
       <c r="IW46"/>
     </row>
-    <row r="47" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:257" ht="12.75" customHeight="1">
       <c r="A47" s="41" t="s">
         <v>97</v>
       </c>
@@ -6417,7 +6420,7 @@
       <c r="IV47"/>
       <c r="IW47"/>
     </row>
-    <row r="48" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:257" ht="12.75" customHeight="1">
       <c r="A48" s="46" t="s">
         <v>77</v>
       </c>
@@ -6692,7 +6695,7 @@
       <c r="IV48"/>
       <c r="IW48"/>
     </row>
-    <row r="49" spans="1:257" ht="11" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:257" ht="11.1" customHeight="1">
       <c r="A49" s="46" t="s">
         <v>22</v>
       </c>
@@ -6967,7 +6970,7 @@
       <c r="IV49"/>
       <c r="IW49"/>
     </row>
-    <row r="50" spans="1:257" ht="11" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:257" ht="11.1" customHeight="1">
       <c r="A50" s="46" t="s">
         <v>0</v>
       </c>
@@ -7242,7 +7245,7 @@
       <c r="IV50"/>
       <c r="IW50"/>
     </row>
-    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:257" ht="12.75" customHeight="1">
       <c r="A51" s="46" t="s">
         <v>79</v>
       </c>
@@ -7517,7 +7520,7 @@
       <c r="IV51"/>
       <c r="IW51"/>
     </row>
-    <row r="52" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:257" ht="12.75" customHeight="1">
       <c r="A52" s="46" t="s">
         <v>81</v>
       </c>
@@ -7792,7 +7795,7 @@
       <c r="IV52"/>
       <c r="IW52"/>
     </row>
-    <row r="53" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:257" ht="12.75" customHeight="1">
       <c r="A53" s="46" t="s">
         <v>83</v>
       </c>
@@ -8067,7 +8070,7 @@
       <c r="IV53"/>
       <c r="IW53"/>
     </row>
-    <row r="54" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:257" ht="12.75" customHeight="1">
       <c r="A54" s="46" t="s">
         <v>101</v>
       </c>
@@ -8342,7 +8345,7 @@
       <c r="IV54"/>
       <c r="IW54"/>
     </row>
-    <row r="55" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:257" ht="12.75" customHeight="1">
       <c r="A55" s="46" t="s">
         <v>102</v>
       </c>
@@ -8617,7 +8620,7 @@
       <c r="IV55"/>
       <c r="IW55"/>
     </row>
-    <row r="56" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:257" ht="12.75" customHeight="1">
       <c r="A56" s="46" t="s">
         <v>104</v>
       </c>
@@ -8892,7 +8895,7 @@
       <c r="IV56"/>
       <c r="IW56"/>
     </row>
-    <row r="57" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:257" ht="12.75" customHeight="1">
       <c r="A57" s="46" t="s">
         <v>106</v>
       </c>
@@ -9167,7 +9170,7 @@
       <c r="IV57"/>
       <c r="IW57"/>
     </row>
-    <row r="58" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:257" ht="12.75" customHeight="1">
       <c r="A58" s="46" t="s">
         <v>108</v>
       </c>
@@ -9442,7 +9445,7 @@
       <c r="IV58"/>
       <c r="IW58"/>
     </row>
-    <row r="59" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:257" ht="12.75" customHeight="1">
       <c r="A59" s="35" t="s">
         <v>111</v>
       </c>
@@ -9716,7 +9719,7 @@
       <c r="IV59"/>
       <c r="IW59"/>
     </row>
-    <row r="60" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:257" ht="12.75" customHeight="1">
       <c r="A60" s="35" t="s">
         <v>113</v>
       </c>
@@ -9990,7 +9993,7 @@
       <c r="IV60"/>
       <c r="IW60"/>
     </row>
-    <row r="61" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:257" ht="12.75" customHeight="1">
       <c r="A61" s="61" t="s">
         <v>22</v>
       </c>
@@ -10264,7 +10267,7 @@
       <c r="IV61"/>
       <c r="IW61"/>
     </row>
-    <row r="62" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:257" ht="12.75" customHeight="1">
       <c r="A62" s="35" t="s">
         <v>115</v>
       </c>
@@ -10538,7 +10541,7 @@
       <c r="IV62"/>
       <c r="IW62"/>
     </row>
-    <row r="63" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:257" ht="12.75" customHeight="1">
       <c r="A63" s="35" t="s">
         <v>117</v>
       </c>
@@ -10812,7 +10815,7 @@
       <c r="IV63"/>
       <c r="IW63"/>
     </row>
-    <row r="64" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:257" ht="12.75" customHeight="1">
       <c r="A64" s="37" t="s">
         <v>119</v>
       </c>
@@ -11088,7 +11091,7 @@
       <c r="IV64"/>
       <c r="IW64"/>
     </row>
-    <row r="65" spans="1:257" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:257">
       <c r="A65" s="35" t="s">
         <v>120</v>
       </c>
@@ -11364,6 +11367,556 @@
       <c r="IV65"/>
       <c r="IW65"/>
     </row>
+    <row r="66" spans="1:257" ht="12.75" customHeight="1">
+      <c r="A66" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="F66" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="48">
+        <v>0</v>
+      </c>
+      <c r="H66" s="48">
+        <v>1</v>
+      </c>
+      <c r="I66" s="48"/>
+      <c r="J66" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66"/>
+      <c r="Y66"/>
+      <c r="Z66"/>
+      <c r="AA66"/>
+      <c r="AB66"/>
+      <c r="AC66"/>
+      <c r="AD66"/>
+      <c r="AE66"/>
+      <c r="AF66"/>
+      <c r="AG66"/>
+      <c r="AH66"/>
+      <c r="AI66"/>
+      <c r="AJ66"/>
+      <c r="AK66"/>
+      <c r="AL66"/>
+      <c r="AM66"/>
+      <c r="AN66"/>
+      <c r="AO66"/>
+      <c r="AP66"/>
+      <c r="AQ66"/>
+      <c r="AR66"/>
+      <c r="AS66"/>
+      <c r="AT66"/>
+      <c r="AU66"/>
+      <c r="AV66"/>
+      <c r="AW66"/>
+      <c r="AX66"/>
+      <c r="AY66"/>
+      <c r="AZ66"/>
+      <c r="BA66"/>
+      <c r="BB66"/>
+      <c r="BC66"/>
+      <c r="BD66"/>
+      <c r="BE66"/>
+      <c r="BF66"/>
+      <c r="BG66"/>
+      <c r="BH66"/>
+      <c r="BI66"/>
+      <c r="BJ66"/>
+      <c r="BK66"/>
+      <c r="BL66"/>
+      <c r="BM66"/>
+      <c r="BN66"/>
+      <c r="BO66"/>
+      <c r="BP66"/>
+      <c r="BQ66"/>
+      <c r="BR66"/>
+      <c r="BS66"/>
+      <c r="BT66"/>
+      <c r="BU66"/>
+      <c r="BV66"/>
+      <c r="BW66"/>
+      <c r="BX66"/>
+      <c r="BY66"/>
+      <c r="BZ66"/>
+      <c r="CA66"/>
+      <c r="CB66"/>
+      <c r="CC66"/>
+      <c r="CD66"/>
+      <c r="CE66"/>
+      <c r="CF66"/>
+      <c r="CG66"/>
+      <c r="CH66"/>
+      <c r="CI66"/>
+      <c r="CJ66"/>
+      <c r="CK66"/>
+      <c r="CL66"/>
+      <c r="CM66"/>
+      <c r="CN66"/>
+      <c r="CO66"/>
+      <c r="CP66"/>
+      <c r="CQ66"/>
+      <c r="CR66"/>
+      <c r="CS66"/>
+      <c r="CT66"/>
+      <c r="CU66"/>
+      <c r="CV66"/>
+      <c r="CW66"/>
+      <c r="CX66"/>
+      <c r="CY66"/>
+      <c r="CZ66"/>
+      <c r="DA66"/>
+      <c r="DB66"/>
+      <c r="DC66"/>
+      <c r="DD66"/>
+      <c r="DE66"/>
+      <c r="DF66"/>
+      <c r="DG66"/>
+      <c r="DH66"/>
+      <c r="DI66"/>
+      <c r="DJ66"/>
+      <c r="DK66"/>
+      <c r="DL66"/>
+      <c r="DM66"/>
+      <c r="DN66"/>
+      <c r="DO66"/>
+      <c r="DP66"/>
+      <c r="DQ66"/>
+      <c r="DR66"/>
+      <c r="DS66"/>
+      <c r="DT66"/>
+      <c r="DU66"/>
+      <c r="DV66"/>
+      <c r="DW66"/>
+      <c r="DX66"/>
+      <c r="DY66"/>
+      <c r="DZ66"/>
+      <c r="EA66"/>
+      <c r="EB66"/>
+      <c r="EC66"/>
+      <c r="ED66"/>
+      <c r="EE66"/>
+      <c r="EF66"/>
+      <c r="EG66"/>
+      <c r="EH66"/>
+      <c r="EI66"/>
+      <c r="EJ66"/>
+      <c r="EK66"/>
+      <c r="EL66"/>
+      <c r="EM66"/>
+      <c r="EN66"/>
+      <c r="EO66"/>
+      <c r="EP66"/>
+      <c r="EQ66"/>
+      <c r="ER66"/>
+      <c r="ES66"/>
+      <c r="ET66"/>
+      <c r="EU66"/>
+      <c r="EV66"/>
+      <c r="EW66"/>
+      <c r="EX66"/>
+      <c r="EY66"/>
+      <c r="EZ66"/>
+      <c r="FA66"/>
+      <c r="FB66"/>
+      <c r="FC66"/>
+      <c r="FD66"/>
+      <c r="FE66"/>
+      <c r="FF66"/>
+      <c r="FG66"/>
+      <c r="FH66"/>
+      <c r="FI66"/>
+      <c r="FJ66"/>
+      <c r="FK66"/>
+      <c r="FL66"/>
+      <c r="FM66"/>
+      <c r="FN66"/>
+      <c r="FO66"/>
+      <c r="FP66"/>
+      <c r="FQ66"/>
+      <c r="FR66"/>
+      <c r="FS66"/>
+      <c r="FT66"/>
+      <c r="FU66"/>
+      <c r="FV66"/>
+      <c r="FW66"/>
+      <c r="FX66"/>
+      <c r="FY66"/>
+      <c r="FZ66"/>
+      <c r="GA66"/>
+      <c r="GB66"/>
+      <c r="GC66"/>
+      <c r="GD66"/>
+      <c r="GE66"/>
+      <c r="GF66"/>
+      <c r="GG66"/>
+      <c r="GH66"/>
+      <c r="GI66"/>
+      <c r="GJ66"/>
+      <c r="GK66"/>
+      <c r="GL66"/>
+      <c r="GM66"/>
+      <c r="GN66"/>
+      <c r="GO66"/>
+      <c r="GP66"/>
+      <c r="GQ66"/>
+      <c r="GR66"/>
+      <c r="GS66"/>
+      <c r="GT66"/>
+      <c r="GU66"/>
+      <c r="GV66"/>
+      <c r="GW66"/>
+      <c r="GX66"/>
+      <c r="GY66"/>
+      <c r="GZ66"/>
+      <c r="HA66"/>
+      <c r="HB66"/>
+      <c r="HC66"/>
+      <c r="HD66"/>
+      <c r="HE66"/>
+      <c r="HF66"/>
+      <c r="HG66"/>
+      <c r="HH66"/>
+      <c r="HI66"/>
+      <c r="HJ66"/>
+      <c r="HK66"/>
+      <c r="HL66"/>
+      <c r="HM66"/>
+      <c r="HN66"/>
+      <c r="HO66"/>
+      <c r="HP66"/>
+      <c r="HQ66"/>
+      <c r="HR66"/>
+      <c r="HS66"/>
+      <c r="HT66"/>
+      <c r="HU66"/>
+      <c r="HV66"/>
+      <c r="HW66"/>
+      <c r="HX66"/>
+      <c r="HY66"/>
+      <c r="HZ66"/>
+      <c r="IA66"/>
+      <c r="IB66"/>
+      <c r="IC66"/>
+      <c r="ID66"/>
+      <c r="IE66"/>
+      <c r="IF66"/>
+      <c r="IG66"/>
+      <c r="IH66"/>
+      <c r="II66"/>
+      <c r="IJ66"/>
+      <c r="IK66"/>
+      <c r="IL66"/>
+      <c r="IM66"/>
+      <c r="IN66"/>
+      <c r="IO66"/>
+      <c r="IP66"/>
+      <c r="IQ66"/>
+      <c r="IR66"/>
+      <c r="IS66"/>
+      <c r="IT66"/>
+      <c r="IU66"/>
+      <c r="IV66"/>
+      <c r="IW66"/>
+    </row>
+    <row r="67" spans="1:257" ht="12.75" customHeight="1">
+      <c r="A67" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="C67" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="48">
+        <v>0</v>
+      </c>
+      <c r="H67" s="48">
+        <v>1</v>
+      </c>
+      <c r="I67" s="48"/>
+      <c r="J67" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+      <c r="X67"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+      <c r="AE67"/>
+      <c r="AF67"/>
+      <c r="AG67"/>
+      <c r="AH67"/>
+      <c r="AI67"/>
+      <c r="AJ67"/>
+      <c r="AK67"/>
+      <c r="AL67"/>
+      <c r="AM67"/>
+      <c r="AN67"/>
+      <c r="AO67"/>
+      <c r="AP67"/>
+      <c r="AQ67"/>
+      <c r="AR67"/>
+      <c r="AS67"/>
+      <c r="AT67"/>
+      <c r="AU67"/>
+      <c r="AV67"/>
+      <c r="AW67"/>
+      <c r="AX67"/>
+      <c r="AY67"/>
+      <c r="AZ67"/>
+      <c r="BA67"/>
+      <c r="BB67"/>
+      <c r="BC67"/>
+      <c r="BD67"/>
+      <c r="BE67"/>
+      <c r="BF67"/>
+      <c r="BG67"/>
+      <c r="BH67"/>
+      <c r="BI67"/>
+      <c r="BJ67"/>
+      <c r="BK67"/>
+      <c r="BL67"/>
+      <c r="BM67"/>
+      <c r="BN67"/>
+      <c r="BO67"/>
+      <c r="BP67"/>
+      <c r="BQ67"/>
+      <c r="BR67"/>
+      <c r="BS67"/>
+      <c r="BT67"/>
+      <c r="BU67"/>
+      <c r="BV67"/>
+      <c r="BW67"/>
+      <c r="BX67"/>
+      <c r="BY67"/>
+      <c r="BZ67"/>
+      <c r="CA67"/>
+      <c r="CB67"/>
+      <c r="CC67"/>
+      <c r="CD67"/>
+      <c r="CE67"/>
+      <c r="CF67"/>
+      <c r="CG67"/>
+      <c r="CH67"/>
+      <c r="CI67"/>
+      <c r="CJ67"/>
+      <c r="CK67"/>
+      <c r="CL67"/>
+      <c r="CM67"/>
+      <c r="CN67"/>
+      <c r="CO67"/>
+      <c r="CP67"/>
+      <c r="CQ67"/>
+      <c r="CR67"/>
+      <c r="CS67"/>
+      <c r="CT67"/>
+      <c r="CU67"/>
+      <c r="CV67"/>
+      <c r="CW67"/>
+      <c r="CX67"/>
+      <c r="CY67"/>
+      <c r="CZ67"/>
+      <c r="DA67"/>
+      <c r="DB67"/>
+      <c r="DC67"/>
+      <c r="DD67"/>
+      <c r="DE67"/>
+      <c r="DF67"/>
+      <c r="DG67"/>
+      <c r="DH67"/>
+      <c r="DI67"/>
+      <c r="DJ67"/>
+      <c r="DK67"/>
+      <c r="DL67"/>
+      <c r="DM67"/>
+      <c r="DN67"/>
+      <c r="DO67"/>
+      <c r="DP67"/>
+      <c r="DQ67"/>
+      <c r="DR67"/>
+      <c r="DS67"/>
+      <c r="DT67"/>
+      <c r="DU67"/>
+      <c r="DV67"/>
+      <c r="DW67"/>
+      <c r="DX67"/>
+      <c r="DY67"/>
+      <c r="DZ67"/>
+      <c r="EA67"/>
+      <c r="EB67"/>
+      <c r="EC67"/>
+      <c r="ED67"/>
+      <c r="EE67"/>
+      <c r="EF67"/>
+      <c r="EG67"/>
+      <c r="EH67"/>
+      <c r="EI67"/>
+      <c r="EJ67"/>
+      <c r="EK67"/>
+      <c r="EL67"/>
+      <c r="EM67"/>
+      <c r="EN67"/>
+      <c r="EO67"/>
+      <c r="EP67"/>
+      <c r="EQ67"/>
+      <c r="ER67"/>
+      <c r="ES67"/>
+      <c r="ET67"/>
+      <c r="EU67"/>
+      <c r="EV67"/>
+      <c r="EW67"/>
+      <c r="EX67"/>
+      <c r="EY67"/>
+      <c r="EZ67"/>
+      <c r="FA67"/>
+      <c r="FB67"/>
+      <c r="FC67"/>
+      <c r="FD67"/>
+      <c r="FE67"/>
+      <c r="FF67"/>
+      <c r="FG67"/>
+      <c r="FH67"/>
+      <c r="FI67"/>
+      <c r="FJ67"/>
+      <c r="FK67"/>
+      <c r="FL67"/>
+      <c r="FM67"/>
+      <c r="FN67"/>
+      <c r="FO67"/>
+      <c r="FP67"/>
+      <c r="FQ67"/>
+      <c r="FR67"/>
+      <c r="FS67"/>
+      <c r="FT67"/>
+      <c r="FU67"/>
+      <c r="FV67"/>
+      <c r="FW67"/>
+      <c r="FX67"/>
+      <c r="FY67"/>
+      <c r="FZ67"/>
+      <c r="GA67"/>
+      <c r="GB67"/>
+      <c r="GC67"/>
+      <c r="GD67"/>
+      <c r="GE67"/>
+      <c r="GF67"/>
+      <c r="GG67"/>
+      <c r="GH67"/>
+      <c r="GI67"/>
+      <c r="GJ67"/>
+      <c r="GK67"/>
+      <c r="GL67"/>
+      <c r="GM67"/>
+      <c r="GN67"/>
+      <c r="GO67"/>
+      <c r="GP67"/>
+      <c r="GQ67"/>
+      <c r="GR67"/>
+      <c r="GS67"/>
+      <c r="GT67"/>
+      <c r="GU67"/>
+      <c r="GV67"/>
+      <c r="GW67"/>
+      <c r="GX67"/>
+      <c r="GY67"/>
+      <c r="GZ67"/>
+      <c r="HA67"/>
+      <c r="HB67"/>
+      <c r="HC67"/>
+      <c r="HD67"/>
+      <c r="HE67"/>
+      <c r="HF67"/>
+      <c r="HG67"/>
+      <c r="HH67"/>
+      <c r="HI67"/>
+      <c r="HJ67"/>
+      <c r="HK67"/>
+      <c r="HL67"/>
+      <c r="HM67"/>
+      <c r="HN67"/>
+      <c r="HO67"/>
+      <c r="HP67"/>
+      <c r="HQ67"/>
+      <c r="HR67"/>
+      <c r="HS67"/>
+      <c r="HT67"/>
+      <c r="HU67"/>
+      <c r="HV67"/>
+      <c r="HW67"/>
+      <c r="HX67"/>
+      <c r="HY67"/>
+      <c r="HZ67"/>
+      <c r="IA67"/>
+      <c r="IB67"/>
+      <c r="IC67"/>
+      <c r="ID67"/>
+      <c r="IE67"/>
+      <c r="IF67"/>
+      <c r="IG67"/>
+      <c r="IH67"/>
+      <c r="II67"/>
+      <c r="IJ67"/>
+      <c r="IK67"/>
+      <c r="IL67"/>
+      <c r="IM67"/>
+      <c r="IN67"/>
+      <c r="IO67"/>
+      <c r="IP67"/>
+      <c r="IQ67"/>
+      <c r="IR67"/>
+      <c r="IS67"/>
+      <c r="IT67"/>
+      <c r="IU67"/>
+      <c r="IV67"/>
+      <c r="IW67"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11381,17 +11934,17 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -11423,7 +11976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17.45" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -11453,7 +12006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="13.7" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -11483,7 +12036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13.7" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -11513,7 +12066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="13.7" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -11543,7 +12096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="13.7" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -11573,7 +12126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.7" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -11603,7 +12156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="13.7" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -11633,7 +12186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="13.7" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -11665,7 +12218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="13.7" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -11697,7 +12250,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="13.7" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -11729,7 +12282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="13.7" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -11758,7 +12311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="13.7" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -11788,7 +12341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="13.7" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -11815,7 +12368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="13.7" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -11842,7 +12395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -11874,7 +12427,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -11906,7 +12459,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>47</v>
       </c>
@@ -11938,7 +12491,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="26" t="s">
         <v>49</v>
       </c>
@@ -11968,7 +12521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="26" t="s">
         <v>51</v>
       </c>
@@ -11998,7 +12551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>53</v>
       </c>
@@ -12025,7 +12578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="13.7" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
@@ -12057,7 +12610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="13.7" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>57</v>
       </c>
@@ -12089,7 +12642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" customHeight="1">
       <c r="A24" s="29" t="s">
         <v>60</v>
       </c>
@@ -12121,7 +12674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="29" t="s">
         <v>62</v>
       </c>
@@ -12153,7 +12706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" customHeight="1">
       <c r="A26" s="29" t="s">
         <v>133</v>
       </c>
@@ -12185,7 +12738,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" customHeight="1">
       <c r="A27" s="29" t="s">
         <v>64</v>
       </c>
@@ -12217,7 +12770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="29" t="s">
         <v>66</v>
       </c>
@@ -12249,7 +12802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" customHeight="1">
       <c r="A29" s="29" t="s">
         <v>68</v>
       </c>
@@ -12281,7 +12834,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="12.75" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>70</v>
       </c>
@@ -12313,7 +12866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" customHeight="1">
       <c r="A31" s="29" t="s">
         <v>72</v>
       </c>
@@ -12345,7 +12898,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" customHeight="1">
       <c r="A32" s="29" t="s">
         <v>73</v>
       </c>
@@ -12377,7 +12930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:257" ht="12.75" customHeight="1">
       <c r="A33" s="29" t="s">
         <v>74</v>
       </c>
@@ -12409,7 +12962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:257" ht="12.75" customHeight="1">
       <c r="A34" s="29" t="s">
         <v>75</v>
       </c>
@@ -12441,7 +12994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:257" ht="12.75" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>76</v>
       </c>
@@ -12473,7 +13026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:257" ht="12.75" customHeight="1">
       <c r="A36" s="29" t="s">
         <v>77</v>
       </c>
@@ -12503,7 +13056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:257" ht="12.75" customHeight="1">
       <c r="A37" s="29" t="s">
         <v>79</v>
       </c>
@@ -12533,7 +13086,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:257" ht="12.75" customHeight="1">
       <c r="A38" s="29" t="s">
         <v>81</v>
       </c>
@@ -12563,7 +13116,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:257" ht="12.75" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>83</v>
       </c>
@@ -12593,7 +13146,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:257" ht="12.75" customHeight="1">
       <c r="A40" s="29" t="s">
         <v>85</v>
       </c>
@@ -12623,7 +13176,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:257" ht="12.75" customHeight="1">
       <c r="A41" s="29" t="s">
         <v>87</v>
       </c>
@@ -12653,7 +13206,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:257" ht="12.75" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>89</v>
       </c>
@@ -12683,7 +13236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:257" ht="12.75" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>91</v>
       </c>
@@ -12713,7 +13266,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:257" ht="12.75" customHeight="1">
       <c r="A44" s="29" t="s">
         <v>92</v>
       </c>
@@ -12743,7 +13296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:257" ht="12.75" customHeight="1">
       <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
@@ -12773,7 +13326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:257" ht="12.75" customHeight="1">
       <c r="A46" s="41" t="s">
         <v>97</v>
       </c>
@@ -13050,7 +13603,7 @@
       <c r="IV46" s="56"/>
       <c r="IW46" s="56"/>
     </row>
-    <row r="47" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:257" ht="12.75" customHeight="1">
       <c r="A47" s="46" t="s">
         <v>77</v>
       </c>
@@ -13325,7 +13878,7 @@
       <c r="IV47" s="56"/>
       <c r="IW47" s="56"/>
     </row>
-    <row r="48" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:257" ht="12.75" customHeight="1">
       <c r="A48" s="46" t="s">
         <v>79</v>
       </c>
@@ -13600,7 +14153,7 @@
       <c r="IV48" s="56"/>
       <c r="IW48" s="56"/>
     </row>
-    <row r="49" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:257" ht="12.75" customHeight="1">
       <c r="A49" s="46" t="s">
         <v>81</v>
       </c>
@@ -13875,7 +14428,7 @@
       <c r="IV49" s="56"/>
       <c r="IW49" s="56"/>
     </row>
-    <row r="50" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:257" ht="12.75" customHeight="1">
       <c r="A50" s="46" t="s">
         <v>83</v>
       </c>
@@ -14150,7 +14703,7 @@
       <c r="IV50" s="56"/>
       <c r="IW50" s="56"/>
     </row>
-    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:257" ht="12.75" customHeight="1">
       <c r="A51" s="46" t="s">
         <v>101</v>
       </c>
@@ -14425,7 +14978,7 @@
       <c r="IV51" s="56"/>
       <c r="IW51" s="56"/>
     </row>
-    <row r="52" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:257" ht="12.75" customHeight="1">
       <c r="A52" s="46" t="s">
         <v>102</v>
       </c>
@@ -14700,7 +15253,7 @@
       <c r="IV52" s="56"/>
       <c r="IW52" s="56"/>
     </row>
-    <row r="53" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:257" ht="12.75" customHeight="1">
       <c r="A53" s="46" t="s">
         <v>104</v>
       </c>
@@ -14975,7 +15528,7 @@
       <c r="IV53" s="56"/>
       <c r="IW53" s="56"/>
     </row>
-    <row r="54" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:257" ht="12.75" customHeight="1">
       <c r="A54" s="46" t="s">
         <v>106</v>
       </c>
@@ -15250,7 +15803,7 @@
       <c r="IV54" s="56"/>
       <c r="IW54" s="56"/>
     </row>
-    <row r="55" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:257" ht="12.75" customHeight="1">
       <c r="A55" s="46" t="s">
         <v>108</v>
       </c>
@@ -15525,7 +16078,7 @@
       <c r="IV55" s="56"/>
       <c r="IW55" s="56"/>
     </row>
-    <row r="56" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:257" ht="12.75" customHeight="1">
       <c r="A56" s="35" t="s">
         <v>22</v>
       </c>
@@ -15557,7 +16110,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:257" ht="12.75" customHeight="1">
       <c r="A57" s="35" t="s">
         <v>111</v>
       </c>
@@ -15584,7 +16137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:257" ht="12.75" customHeight="1">
       <c r="A58" s="35" t="s">
         <v>117</v>
       </c>
@@ -15611,7 +16164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:257" ht="12.75" customHeight="1">
       <c r="A59" s="35" t="s">
         <v>113</v>
       </c>
@@ -15638,7 +16191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:257" ht="12.75" customHeight="1">
       <c r="A60" s="35" t="s">
         <v>115</v>
       </c>
@@ -15668,7 +16221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:257" ht="12.75" customHeight="1">
       <c r="A61" s="37" t="s">
         <v>119</v>
       </c>
@@ -15700,7 +16253,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:257" ht="12.75" customHeight="1">
       <c r="A62" s="35" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
finished implementing Haiti address
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276ED3A-5BE9-4851-A7F6-5B51A532A839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0351DE7B-6CB3-4A4C-B433-B0D943BD6D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31290" yWindow="1050" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="145">
   <si>
     <t>name</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>province</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1333,7 @@
   <dimension ref="A1:IW67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -11369,7 +11372,7 @@
     </row>
     <row r="66" spans="1:257" ht="12.75" customHeight="1">
       <c r="A66" s="46" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B66" s="47" t="s">
         <v>143</v>
@@ -11644,7 +11647,7 @@
     </row>
     <row r="67" spans="1:257" ht="12.75" customHeight="1">
       <c r="A67" s="46" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B67" s="47" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
fixed case conference translations
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663BEDF4-DAA3-4526-91E7-9A6209C600CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77575D9-7CA5-4FD3-A185-F371A8335D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31140" yWindow="1065" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="244">
   <si>
     <t>name</t>
   </si>
@@ -694,10 +694,70 @@
     <t>other_legal_doc_option</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>referral_date</t>
+  </si>
+  <si>
+    <t>Date of Internal Referral</t>
+  </si>
+  <si>
+    <t>internal_referral</t>
+  </si>
+  <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>Client ID</t>
+  </si>
+  <si>
+    <t>client_name</t>
+  </si>
+  <si>
+    <t>Client Name</t>
+  </si>
+  <si>
+    <t>referred_from</t>
+  </si>
+  <si>
+    <t>Referral Form</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>Referred To</t>
+  </si>
+  <si>
+    <t>client_representing_problem</t>
+  </si>
+  <si>
+    <t>CLIENT’S PRESENTING PROBLEMS</t>
+  </si>
+  <si>
+    <t>emergency_note</t>
+  </si>
+  <si>
+    <t>NOTE: EMERGENCY/CRISIS NEEDS</t>
+  </si>
+  <si>
+    <t>referral_reason</t>
+  </si>
+  <si>
+    <t>referral_decision</t>
+  </si>
+  <si>
+    <t>REFERRAL DECISION (to be approved by case management supervisor)</t>
+  </si>
+  <si>
+    <t>File Upload</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1219,7 +1279,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1607,8 +1668,8 @@
   </sheetPr>
   <dimension ref="A1:IW129"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -16293,7 +16354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="97" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A97" s="58" t="s">
         <v>207</v>
       </c>
@@ -16321,7 +16382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="98" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A98" s="95" t="s">
         <v>210</v>
       </c>
@@ -16351,7 +16412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="99" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A99" s="95" t="s">
         <v>203</v>
       </c>
@@ -16381,7 +16442,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="100" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A100" s="95" t="s">
         <v>213</v>
       </c>
@@ -16411,7 +16472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="101" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A101" s="95" t="s">
         <v>215</v>
       </c>
@@ -16441,7 +16502,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="102" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="95" t="s">
         <v>219</v>
       </c>
@@ -16469,7 +16530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="95" t="s">
         <v>220</v>
       </c>
@@ -16497,13 +16558,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="104" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="95" t="s">
         <v>221</v>
       </c>
       <c r="B104" s="58"/>
       <c r="C104" s="95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D104" s="58"/>
       <c r="E104" s="95" t="s">
@@ -16525,34 +16586,3338 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="106" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="107" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="108" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="109" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="110" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="111" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="112" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="113" spans="3:3" ht="17.100000000000001" customHeight="1">
-      <c r="C113" s="96" t="s">
-        <v>222</v>
-      </c>
+    <row r="105" spans="1:257" ht="15.75" customHeight="1">
+      <c r="A105" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="B105" s="78" t="s">
+        <v>224</v>
+      </c>
+      <c r="C105" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="D105" s="57"/>
+      <c r="E105" s="80" t="s">
+        <v>224</v>
+      </c>
+      <c r="F105" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="G105" s="81">
+        <v>0</v>
+      </c>
+      <c r="H105" s="81">
+        <v>1</v>
+      </c>
+      <c r="I105" s="96"/>
+      <c r="J105" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+      <c r="P105"/>
+      <c r="Q105"/>
+      <c r="R105"/>
+      <c r="S105"/>
+      <c r="T105"/>
+      <c r="U105"/>
+      <c r="V105"/>
+      <c r="W105"/>
+      <c r="X105"/>
+      <c r="Y105"/>
+      <c r="Z105"/>
+      <c r="AA105"/>
+      <c r="AB105"/>
+      <c r="AC105"/>
+      <c r="AD105"/>
+      <c r="AE105"/>
+      <c r="AF105"/>
+      <c r="AG105"/>
+      <c r="AH105"/>
+      <c r="AI105"/>
+      <c r="AJ105"/>
+      <c r="AK105"/>
+      <c r="AL105"/>
+      <c r="AM105"/>
+      <c r="AN105"/>
+      <c r="AO105"/>
+      <c r="AP105"/>
+      <c r="AQ105"/>
+      <c r="AR105"/>
+      <c r="AS105"/>
+      <c r="AT105"/>
+      <c r="AU105"/>
+      <c r="AV105"/>
+      <c r="AW105"/>
+      <c r="AX105"/>
+      <c r="AY105"/>
+      <c r="AZ105"/>
+      <c r="BA105"/>
+      <c r="BB105"/>
+      <c r="BC105"/>
+      <c r="BD105"/>
+      <c r="BE105"/>
+      <c r="BF105"/>
+      <c r="BG105"/>
+      <c r="BH105"/>
+      <c r="BI105"/>
+      <c r="BJ105"/>
+      <c r="BK105"/>
+      <c r="BL105"/>
+      <c r="BM105"/>
+      <c r="BN105"/>
+      <c r="BO105"/>
+      <c r="BP105"/>
+      <c r="BQ105"/>
+      <c r="BR105"/>
+      <c r="BS105"/>
+      <c r="BT105"/>
+      <c r="BU105"/>
+      <c r="BV105"/>
+      <c r="BW105"/>
+      <c r="BX105"/>
+      <c r="BY105"/>
+      <c r="BZ105"/>
+      <c r="CA105"/>
+      <c r="CB105"/>
+      <c r="CC105"/>
+      <c r="CD105"/>
+      <c r="CE105"/>
+      <c r="CF105"/>
+      <c r="CG105"/>
+      <c r="CH105"/>
+      <c r="CI105"/>
+      <c r="CJ105"/>
+      <c r="CK105"/>
+      <c r="CL105"/>
+      <c r="CM105"/>
+      <c r="CN105"/>
+      <c r="CO105"/>
+      <c r="CP105"/>
+      <c r="CQ105"/>
+      <c r="CR105"/>
+      <c r="CS105"/>
+      <c r="CT105"/>
+      <c r="CU105"/>
+      <c r="CV105"/>
+      <c r="CW105"/>
+      <c r="CX105"/>
+      <c r="CY105"/>
+      <c r="CZ105"/>
+      <c r="DA105"/>
+      <c r="DB105"/>
+      <c r="DC105"/>
+      <c r="DD105"/>
+      <c r="DE105"/>
+      <c r="DF105"/>
+      <c r="DG105"/>
+      <c r="DH105"/>
+      <c r="DI105"/>
+      <c r="DJ105"/>
+      <c r="DK105"/>
+      <c r="DL105"/>
+      <c r="DM105"/>
+      <c r="DN105"/>
+      <c r="DO105"/>
+      <c r="DP105"/>
+      <c r="DQ105"/>
+      <c r="DR105"/>
+      <c r="DS105"/>
+      <c r="DT105"/>
+      <c r="DU105"/>
+      <c r="DV105"/>
+      <c r="DW105"/>
+      <c r="DX105"/>
+      <c r="DY105"/>
+      <c r="DZ105"/>
+      <c r="EA105"/>
+      <c r="EB105"/>
+      <c r="EC105"/>
+      <c r="ED105"/>
+      <c r="EE105"/>
+      <c r="EF105"/>
+      <c r="EG105"/>
+      <c r="EH105"/>
+      <c r="EI105"/>
+      <c r="EJ105"/>
+      <c r="EK105"/>
+      <c r="EL105"/>
+      <c r="EM105"/>
+      <c r="EN105"/>
+      <c r="EO105"/>
+      <c r="EP105"/>
+      <c r="EQ105"/>
+      <c r="ER105"/>
+      <c r="ES105"/>
+      <c r="ET105"/>
+      <c r="EU105"/>
+      <c r="EV105"/>
+      <c r="EW105"/>
+      <c r="EX105"/>
+      <c r="EY105"/>
+      <c r="EZ105"/>
+      <c r="FA105"/>
+      <c r="FB105"/>
+      <c r="FC105"/>
+      <c r="FD105"/>
+      <c r="FE105"/>
+      <c r="FF105"/>
+      <c r="FG105"/>
+      <c r="FH105"/>
+      <c r="FI105"/>
+      <c r="FJ105"/>
+      <c r="FK105"/>
+      <c r="FL105"/>
+      <c r="FM105"/>
+      <c r="FN105"/>
+      <c r="FO105"/>
+      <c r="FP105"/>
+      <c r="FQ105"/>
+      <c r="FR105"/>
+      <c r="FS105"/>
+      <c r="FT105"/>
+      <c r="FU105"/>
+      <c r="FV105"/>
+      <c r="FW105"/>
+      <c r="FX105"/>
+      <c r="FY105"/>
+      <c r="FZ105"/>
+      <c r="GA105"/>
+      <c r="GB105"/>
+      <c r="GC105"/>
+      <c r="GD105"/>
+      <c r="GE105"/>
+      <c r="GF105"/>
+      <c r="GG105"/>
+      <c r="GH105"/>
+      <c r="GI105"/>
+      <c r="GJ105"/>
+      <c r="GK105"/>
+      <c r="GL105"/>
+      <c r="GM105"/>
+      <c r="GN105"/>
+      <c r="GO105"/>
+      <c r="GP105"/>
+      <c r="GQ105"/>
+      <c r="GR105"/>
+      <c r="GS105"/>
+      <c r="GT105"/>
+      <c r="GU105"/>
+      <c r="GV105"/>
+      <c r="GW105"/>
+      <c r="GX105"/>
+      <c r="GY105"/>
+      <c r="GZ105"/>
+      <c r="HA105"/>
+      <c r="HB105"/>
+      <c r="HC105"/>
+      <c r="HD105"/>
+      <c r="HE105"/>
+      <c r="HF105"/>
+      <c r="HG105"/>
+      <c r="HH105"/>
+      <c r="HI105"/>
+      <c r="HJ105"/>
+      <c r="HK105"/>
+      <c r="HL105"/>
+      <c r="HM105"/>
+      <c r="HN105"/>
+      <c r="HO105"/>
+      <c r="HP105"/>
+      <c r="HQ105"/>
+      <c r="HR105"/>
+      <c r="HS105"/>
+      <c r="HT105"/>
+      <c r="HU105"/>
+      <c r="HV105"/>
+      <c r="HW105"/>
+      <c r="HX105"/>
+      <c r="HY105"/>
+      <c r="HZ105"/>
+      <c r="IA105"/>
+      <c r="IB105"/>
+      <c r="IC105"/>
+      <c r="ID105"/>
+      <c r="IE105"/>
+      <c r="IF105"/>
+      <c r="IG105"/>
+      <c r="IH105"/>
+      <c r="II105"/>
+      <c r="IJ105"/>
+      <c r="IK105"/>
+      <c r="IL105"/>
+      <c r="IM105"/>
+      <c r="IN105"/>
+      <c r="IO105"/>
+      <c r="IP105"/>
+      <c r="IQ105"/>
+      <c r="IR105"/>
+      <c r="IS105"/>
+      <c r="IT105"/>
+      <c r="IU105"/>
+      <c r="IV105"/>
+      <c r="IW105"/>
     </row>
-    <row r="114" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="115" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="116" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="117" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="118" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="119" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="120" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="121" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="122" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="123" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="124" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="125" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="126" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="127" spans="3:3" ht="17.100000000000001" customHeight="1"/>
-    <row r="128" spans="3:3" ht="17.100000000000001" customHeight="1"/>
+    <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A106" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="B106" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C106" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="D106" s="57"/>
+      <c r="E106" s="80" t="s">
+        <v>120</v>
+      </c>
+      <c r="F106" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="G106" s="81">
+        <v>0</v>
+      </c>
+      <c r="H106" s="81">
+        <v>1</v>
+      </c>
+      <c r="I106" s="96"/>
+      <c r="J106" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K106"/>
+      <c r="L106"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+      <c r="P106"/>
+      <c r="Q106"/>
+      <c r="R106"/>
+      <c r="S106"/>
+      <c r="T106"/>
+      <c r="U106"/>
+      <c r="V106"/>
+      <c r="W106"/>
+      <c r="X106"/>
+      <c r="Y106"/>
+      <c r="Z106"/>
+      <c r="AA106"/>
+      <c r="AB106"/>
+      <c r="AC106"/>
+      <c r="AD106"/>
+      <c r="AE106"/>
+      <c r="AF106"/>
+      <c r="AG106"/>
+      <c r="AH106"/>
+      <c r="AI106"/>
+      <c r="AJ106"/>
+      <c r="AK106"/>
+      <c r="AL106"/>
+      <c r="AM106"/>
+      <c r="AN106"/>
+      <c r="AO106"/>
+      <c r="AP106"/>
+      <c r="AQ106"/>
+      <c r="AR106"/>
+      <c r="AS106"/>
+      <c r="AT106"/>
+      <c r="AU106"/>
+      <c r="AV106"/>
+      <c r="AW106"/>
+      <c r="AX106"/>
+      <c r="AY106"/>
+      <c r="AZ106"/>
+      <c r="BA106"/>
+      <c r="BB106"/>
+      <c r="BC106"/>
+      <c r="BD106"/>
+      <c r="BE106"/>
+      <c r="BF106"/>
+      <c r="BG106"/>
+      <c r="BH106"/>
+      <c r="BI106"/>
+      <c r="BJ106"/>
+      <c r="BK106"/>
+      <c r="BL106"/>
+      <c r="BM106"/>
+      <c r="BN106"/>
+      <c r="BO106"/>
+      <c r="BP106"/>
+      <c r="BQ106"/>
+      <c r="BR106"/>
+      <c r="BS106"/>
+      <c r="BT106"/>
+      <c r="BU106"/>
+      <c r="BV106"/>
+      <c r="BW106"/>
+      <c r="BX106"/>
+      <c r="BY106"/>
+      <c r="BZ106"/>
+      <c r="CA106"/>
+      <c r="CB106"/>
+      <c r="CC106"/>
+      <c r="CD106"/>
+      <c r="CE106"/>
+      <c r="CF106"/>
+      <c r="CG106"/>
+      <c r="CH106"/>
+      <c r="CI106"/>
+      <c r="CJ106"/>
+      <c r="CK106"/>
+      <c r="CL106"/>
+      <c r="CM106"/>
+      <c r="CN106"/>
+      <c r="CO106"/>
+      <c r="CP106"/>
+      <c r="CQ106"/>
+      <c r="CR106"/>
+      <c r="CS106"/>
+      <c r="CT106"/>
+      <c r="CU106"/>
+      <c r="CV106"/>
+      <c r="CW106"/>
+      <c r="CX106"/>
+      <c r="CY106"/>
+      <c r="CZ106"/>
+      <c r="DA106"/>
+      <c r="DB106"/>
+      <c r="DC106"/>
+      <c r="DD106"/>
+      <c r="DE106"/>
+      <c r="DF106"/>
+      <c r="DG106"/>
+      <c r="DH106"/>
+      <c r="DI106"/>
+      <c r="DJ106"/>
+      <c r="DK106"/>
+      <c r="DL106"/>
+      <c r="DM106"/>
+      <c r="DN106"/>
+      <c r="DO106"/>
+      <c r="DP106"/>
+      <c r="DQ106"/>
+      <c r="DR106"/>
+      <c r="DS106"/>
+      <c r="DT106"/>
+      <c r="DU106"/>
+      <c r="DV106"/>
+      <c r="DW106"/>
+      <c r="DX106"/>
+      <c r="DY106"/>
+      <c r="DZ106"/>
+      <c r="EA106"/>
+      <c r="EB106"/>
+      <c r="EC106"/>
+      <c r="ED106"/>
+      <c r="EE106"/>
+      <c r="EF106"/>
+      <c r="EG106"/>
+      <c r="EH106"/>
+      <c r="EI106"/>
+      <c r="EJ106"/>
+      <c r="EK106"/>
+      <c r="EL106"/>
+      <c r="EM106"/>
+      <c r="EN106"/>
+      <c r="EO106"/>
+      <c r="EP106"/>
+      <c r="EQ106"/>
+      <c r="ER106"/>
+      <c r="ES106"/>
+      <c r="ET106"/>
+      <c r="EU106"/>
+      <c r="EV106"/>
+      <c r="EW106"/>
+      <c r="EX106"/>
+      <c r="EY106"/>
+      <c r="EZ106"/>
+      <c r="FA106"/>
+      <c r="FB106"/>
+      <c r="FC106"/>
+      <c r="FD106"/>
+      <c r="FE106"/>
+      <c r="FF106"/>
+      <c r="FG106"/>
+      <c r="FH106"/>
+      <c r="FI106"/>
+      <c r="FJ106"/>
+      <c r="FK106"/>
+      <c r="FL106"/>
+      <c r="FM106"/>
+      <c r="FN106"/>
+      <c r="FO106"/>
+      <c r="FP106"/>
+      <c r="FQ106"/>
+      <c r="FR106"/>
+      <c r="FS106"/>
+      <c r="FT106"/>
+      <c r="FU106"/>
+      <c r="FV106"/>
+      <c r="FW106"/>
+      <c r="FX106"/>
+      <c r="FY106"/>
+      <c r="FZ106"/>
+      <c r="GA106"/>
+      <c r="GB106"/>
+      <c r="GC106"/>
+      <c r="GD106"/>
+      <c r="GE106"/>
+      <c r="GF106"/>
+      <c r="GG106"/>
+      <c r="GH106"/>
+      <c r="GI106"/>
+      <c r="GJ106"/>
+      <c r="GK106"/>
+      <c r="GL106"/>
+      <c r="GM106"/>
+      <c r="GN106"/>
+      <c r="GO106"/>
+      <c r="GP106"/>
+      <c r="GQ106"/>
+      <c r="GR106"/>
+      <c r="GS106"/>
+      <c r="GT106"/>
+      <c r="GU106"/>
+      <c r="GV106"/>
+      <c r="GW106"/>
+      <c r="GX106"/>
+      <c r="GY106"/>
+      <c r="GZ106"/>
+      <c r="HA106"/>
+      <c r="HB106"/>
+      <c r="HC106"/>
+      <c r="HD106"/>
+      <c r="HE106"/>
+      <c r="HF106"/>
+      <c r="HG106"/>
+      <c r="HH106"/>
+      <c r="HI106"/>
+      <c r="HJ106"/>
+      <c r="HK106"/>
+      <c r="HL106"/>
+      <c r="HM106"/>
+      <c r="HN106"/>
+      <c r="HO106"/>
+      <c r="HP106"/>
+      <c r="HQ106"/>
+      <c r="HR106"/>
+      <c r="HS106"/>
+      <c r="HT106"/>
+      <c r="HU106"/>
+      <c r="HV106"/>
+      <c r="HW106"/>
+      <c r="HX106"/>
+      <c r="HY106"/>
+      <c r="HZ106"/>
+      <c r="IA106"/>
+      <c r="IB106"/>
+      <c r="IC106"/>
+      <c r="ID106"/>
+      <c r="IE106"/>
+      <c r="IF106"/>
+      <c r="IG106"/>
+      <c r="IH106"/>
+      <c r="II106"/>
+      <c r="IJ106"/>
+      <c r="IK106"/>
+      <c r="IL106"/>
+      <c r="IM106"/>
+      <c r="IN106"/>
+      <c r="IO106"/>
+      <c r="IP106"/>
+      <c r="IQ106"/>
+      <c r="IR106"/>
+      <c r="IS106"/>
+      <c r="IT106"/>
+      <c r="IU106"/>
+      <c r="IV106"/>
+      <c r="IW106"/>
+    </row>
+    <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A107" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="B107" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="C107" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="D107" s="57"/>
+      <c r="E107" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F107" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G107" s="81">
+        <v>0</v>
+      </c>
+      <c r="H107" s="57">
+        <v>1</v>
+      </c>
+      <c r="I107" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J107" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K107"/>
+      <c r="L107"/>
+      <c r="M107"/>
+      <c r="N107"/>
+      <c r="O107"/>
+      <c r="P107"/>
+      <c r="Q107"/>
+      <c r="R107"/>
+      <c r="S107"/>
+      <c r="T107"/>
+      <c r="U107"/>
+      <c r="V107"/>
+      <c r="W107"/>
+      <c r="X107"/>
+      <c r="Y107"/>
+      <c r="Z107"/>
+      <c r="AA107"/>
+      <c r="AB107"/>
+      <c r="AC107"/>
+      <c r="AD107"/>
+      <c r="AE107"/>
+      <c r="AF107"/>
+      <c r="AG107"/>
+      <c r="AH107"/>
+      <c r="AI107"/>
+      <c r="AJ107"/>
+      <c r="AK107"/>
+      <c r="AL107"/>
+      <c r="AM107"/>
+      <c r="AN107"/>
+      <c r="AO107"/>
+      <c r="AP107"/>
+      <c r="AQ107"/>
+      <c r="AR107"/>
+      <c r="AS107"/>
+      <c r="AT107"/>
+      <c r="AU107"/>
+      <c r="AV107"/>
+      <c r="AW107"/>
+      <c r="AX107"/>
+      <c r="AY107"/>
+      <c r="AZ107"/>
+      <c r="BA107"/>
+      <c r="BB107"/>
+      <c r="BC107"/>
+      <c r="BD107"/>
+      <c r="BE107"/>
+      <c r="BF107"/>
+      <c r="BG107"/>
+      <c r="BH107"/>
+      <c r="BI107"/>
+      <c r="BJ107"/>
+      <c r="BK107"/>
+      <c r="BL107"/>
+      <c r="BM107"/>
+      <c r="BN107"/>
+      <c r="BO107"/>
+      <c r="BP107"/>
+      <c r="BQ107"/>
+      <c r="BR107"/>
+      <c r="BS107"/>
+      <c r="BT107"/>
+      <c r="BU107"/>
+      <c r="BV107"/>
+      <c r="BW107"/>
+      <c r="BX107"/>
+      <c r="BY107"/>
+      <c r="BZ107"/>
+      <c r="CA107"/>
+      <c r="CB107"/>
+      <c r="CC107"/>
+      <c r="CD107"/>
+      <c r="CE107"/>
+      <c r="CF107"/>
+      <c r="CG107"/>
+      <c r="CH107"/>
+      <c r="CI107"/>
+      <c r="CJ107"/>
+      <c r="CK107"/>
+      <c r="CL107"/>
+      <c r="CM107"/>
+      <c r="CN107"/>
+      <c r="CO107"/>
+      <c r="CP107"/>
+      <c r="CQ107"/>
+      <c r="CR107"/>
+      <c r="CS107"/>
+      <c r="CT107"/>
+      <c r="CU107"/>
+      <c r="CV107"/>
+      <c r="CW107"/>
+      <c r="CX107"/>
+      <c r="CY107"/>
+      <c r="CZ107"/>
+      <c r="DA107"/>
+      <c r="DB107"/>
+      <c r="DC107"/>
+      <c r="DD107"/>
+      <c r="DE107"/>
+      <c r="DF107"/>
+      <c r="DG107"/>
+      <c r="DH107"/>
+      <c r="DI107"/>
+      <c r="DJ107"/>
+      <c r="DK107"/>
+      <c r="DL107"/>
+      <c r="DM107"/>
+      <c r="DN107"/>
+      <c r="DO107"/>
+      <c r="DP107"/>
+      <c r="DQ107"/>
+      <c r="DR107"/>
+      <c r="DS107"/>
+      <c r="DT107"/>
+      <c r="DU107"/>
+      <c r="DV107"/>
+      <c r="DW107"/>
+      <c r="DX107"/>
+      <c r="DY107"/>
+      <c r="DZ107"/>
+      <c r="EA107"/>
+      <c r="EB107"/>
+      <c r="EC107"/>
+      <c r="ED107"/>
+      <c r="EE107"/>
+      <c r="EF107"/>
+      <c r="EG107"/>
+      <c r="EH107"/>
+      <c r="EI107"/>
+      <c r="EJ107"/>
+      <c r="EK107"/>
+      <c r="EL107"/>
+      <c r="EM107"/>
+      <c r="EN107"/>
+      <c r="EO107"/>
+      <c r="EP107"/>
+      <c r="EQ107"/>
+      <c r="ER107"/>
+      <c r="ES107"/>
+      <c r="ET107"/>
+      <c r="EU107"/>
+      <c r="EV107"/>
+      <c r="EW107"/>
+      <c r="EX107"/>
+      <c r="EY107"/>
+      <c r="EZ107"/>
+      <c r="FA107"/>
+      <c r="FB107"/>
+      <c r="FC107"/>
+      <c r="FD107"/>
+      <c r="FE107"/>
+      <c r="FF107"/>
+      <c r="FG107"/>
+      <c r="FH107"/>
+      <c r="FI107"/>
+      <c r="FJ107"/>
+      <c r="FK107"/>
+      <c r="FL107"/>
+      <c r="FM107"/>
+      <c r="FN107"/>
+      <c r="FO107"/>
+      <c r="FP107"/>
+      <c r="FQ107"/>
+      <c r="FR107"/>
+      <c r="FS107"/>
+      <c r="FT107"/>
+      <c r="FU107"/>
+      <c r="FV107"/>
+      <c r="FW107"/>
+      <c r="FX107"/>
+      <c r="FY107"/>
+      <c r="FZ107"/>
+      <c r="GA107"/>
+      <c r="GB107"/>
+      <c r="GC107"/>
+      <c r="GD107"/>
+      <c r="GE107"/>
+      <c r="GF107"/>
+      <c r="GG107"/>
+      <c r="GH107"/>
+      <c r="GI107"/>
+      <c r="GJ107"/>
+      <c r="GK107"/>
+      <c r="GL107"/>
+      <c r="GM107"/>
+      <c r="GN107"/>
+      <c r="GO107"/>
+      <c r="GP107"/>
+      <c r="GQ107"/>
+      <c r="GR107"/>
+      <c r="GS107"/>
+      <c r="GT107"/>
+      <c r="GU107"/>
+      <c r="GV107"/>
+      <c r="GW107"/>
+      <c r="GX107"/>
+      <c r="GY107"/>
+      <c r="GZ107"/>
+      <c r="HA107"/>
+      <c r="HB107"/>
+      <c r="HC107"/>
+      <c r="HD107"/>
+      <c r="HE107"/>
+      <c r="HF107"/>
+      <c r="HG107"/>
+      <c r="HH107"/>
+      <c r="HI107"/>
+      <c r="HJ107"/>
+      <c r="HK107"/>
+      <c r="HL107"/>
+      <c r="HM107"/>
+      <c r="HN107"/>
+      <c r="HO107"/>
+      <c r="HP107"/>
+      <c r="HQ107"/>
+      <c r="HR107"/>
+      <c r="HS107"/>
+      <c r="HT107"/>
+      <c r="HU107"/>
+      <c r="HV107"/>
+      <c r="HW107"/>
+      <c r="HX107"/>
+      <c r="HY107"/>
+      <c r="HZ107"/>
+      <c r="IA107"/>
+      <c r="IB107"/>
+      <c r="IC107"/>
+      <c r="ID107"/>
+      <c r="IE107"/>
+      <c r="IF107"/>
+      <c r="IG107"/>
+      <c r="IH107"/>
+      <c r="II107"/>
+      <c r="IJ107"/>
+      <c r="IK107"/>
+      <c r="IL107"/>
+      <c r="IM107"/>
+      <c r="IN107"/>
+      <c r="IO107"/>
+      <c r="IP107"/>
+      <c r="IQ107"/>
+      <c r="IR107"/>
+      <c r="IS107"/>
+      <c r="IT107"/>
+      <c r="IU107"/>
+      <c r="IV107"/>
+      <c r="IW107"/>
+    </row>
+    <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A108" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="B108" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C108" s="57" t="s">
+        <v>229</v>
+      </c>
+      <c r="D108" s="57"/>
+      <c r="E108" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F108" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G108" s="81">
+        <v>0</v>
+      </c>
+      <c r="H108" s="57">
+        <v>1</v>
+      </c>
+      <c r="I108" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J108" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K108"/>
+      <c r="L108"/>
+      <c r="M108"/>
+      <c r="N108"/>
+      <c r="O108"/>
+      <c r="P108"/>
+      <c r="Q108"/>
+      <c r="R108"/>
+      <c r="S108"/>
+      <c r="T108"/>
+      <c r="U108"/>
+      <c r="V108"/>
+      <c r="W108"/>
+      <c r="X108"/>
+      <c r="Y108"/>
+      <c r="Z108"/>
+      <c r="AA108"/>
+      <c r="AB108"/>
+      <c r="AC108"/>
+      <c r="AD108"/>
+      <c r="AE108"/>
+      <c r="AF108"/>
+      <c r="AG108"/>
+      <c r="AH108"/>
+      <c r="AI108"/>
+      <c r="AJ108"/>
+      <c r="AK108"/>
+      <c r="AL108"/>
+      <c r="AM108"/>
+      <c r="AN108"/>
+      <c r="AO108"/>
+      <c r="AP108"/>
+      <c r="AQ108"/>
+      <c r="AR108"/>
+      <c r="AS108"/>
+      <c r="AT108"/>
+      <c r="AU108"/>
+      <c r="AV108"/>
+      <c r="AW108"/>
+      <c r="AX108"/>
+      <c r="AY108"/>
+      <c r="AZ108"/>
+      <c r="BA108"/>
+      <c r="BB108"/>
+      <c r="BC108"/>
+      <c r="BD108"/>
+      <c r="BE108"/>
+      <c r="BF108"/>
+      <c r="BG108"/>
+      <c r="BH108"/>
+      <c r="BI108"/>
+      <c r="BJ108"/>
+      <c r="BK108"/>
+      <c r="BL108"/>
+      <c r="BM108"/>
+      <c r="BN108"/>
+      <c r="BO108"/>
+      <c r="BP108"/>
+      <c r="BQ108"/>
+      <c r="BR108"/>
+      <c r="BS108"/>
+      <c r="BT108"/>
+      <c r="BU108"/>
+      <c r="BV108"/>
+      <c r="BW108"/>
+      <c r="BX108"/>
+      <c r="BY108"/>
+      <c r="BZ108"/>
+      <c r="CA108"/>
+      <c r="CB108"/>
+      <c r="CC108"/>
+      <c r="CD108"/>
+      <c r="CE108"/>
+      <c r="CF108"/>
+      <c r="CG108"/>
+      <c r="CH108"/>
+      <c r="CI108"/>
+      <c r="CJ108"/>
+      <c r="CK108"/>
+      <c r="CL108"/>
+      <c r="CM108"/>
+      <c r="CN108"/>
+      <c r="CO108"/>
+      <c r="CP108"/>
+      <c r="CQ108"/>
+      <c r="CR108"/>
+      <c r="CS108"/>
+      <c r="CT108"/>
+      <c r="CU108"/>
+      <c r="CV108"/>
+      <c r="CW108"/>
+      <c r="CX108"/>
+      <c r="CY108"/>
+      <c r="CZ108"/>
+      <c r="DA108"/>
+      <c r="DB108"/>
+      <c r="DC108"/>
+      <c r="DD108"/>
+      <c r="DE108"/>
+      <c r="DF108"/>
+      <c r="DG108"/>
+      <c r="DH108"/>
+      <c r="DI108"/>
+      <c r="DJ108"/>
+      <c r="DK108"/>
+      <c r="DL108"/>
+      <c r="DM108"/>
+      <c r="DN108"/>
+      <c r="DO108"/>
+      <c r="DP108"/>
+      <c r="DQ108"/>
+      <c r="DR108"/>
+      <c r="DS108"/>
+      <c r="DT108"/>
+      <c r="DU108"/>
+      <c r="DV108"/>
+      <c r="DW108"/>
+      <c r="DX108"/>
+      <c r="DY108"/>
+      <c r="DZ108"/>
+      <c r="EA108"/>
+      <c r="EB108"/>
+      <c r="EC108"/>
+      <c r="ED108"/>
+      <c r="EE108"/>
+      <c r="EF108"/>
+      <c r="EG108"/>
+      <c r="EH108"/>
+      <c r="EI108"/>
+      <c r="EJ108"/>
+      <c r="EK108"/>
+      <c r="EL108"/>
+      <c r="EM108"/>
+      <c r="EN108"/>
+      <c r="EO108"/>
+      <c r="EP108"/>
+      <c r="EQ108"/>
+      <c r="ER108"/>
+      <c r="ES108"/>
+      <c r="ET108"/>
+      <c r="EU108"/>
+      <c r="EV108"/>
+      <c r="EW108"/>
+      <c r="EX108"/>
+      <c r="EY108"/>
+      <c r="EZ108"/>
+      <c r="FA108"/>
+      <c r="FB108"/>
+      <c r="FC108"/>
+      <c r="FD108"/>
+      <c r="FE108"/>
+      <c r="FF108"/>
+      <c r="FG108"/>
+      <c r="FH108"/>
+      <c r="FI108"/>
+      <c r="FJ108"/>
+      <c r="FK108"/>
+      <c r="FL108"/>
+      <c r="FM108"/>
+      <c r="FN108"/>
+      <c r="FO108"/>
+      <c r="FP108"/>
+      <c r="FQ108"/>
+      <c r="FR108"/>
+      <c r="FS108"/>
+      <c r="FT108"/>
+      <c r="FU108"/>
+      <c r="FV108"/>
+      <c r="FW108"/>
+      <c r="FX108"/>
+      <c r="FY108"/>
+      <c r="FZ108"/>
+      <c r="GA108"/>
+      <c r="GB108"/>
+      <c r="GC108"/>
+      <c r="GD108"/>
+      <c r="GE108"/>
+      <c r="GF108"/>
+      <c r="GG108"/>
+      <c r="GH108"/>
+      <c r="GI108"/>
+      <c r="GJ108"/>
+      <c r="GK108"/>
+      <c r="GL108"/>
+      <c r="GM108"/>
+      <c r="GN108"/>
+      <c r="GO108"/>
+      <c r="GP108"/>
+      <c r="GQ108"/>
+      <c r="GR108"/>
+      <c r="GS108"/>
+      <c r="GT108"/>
+      <c r="GU108"/>
+      <c r="GV108"/>
+      <c r="GW108"/>
+      <c r="GX108"/>
+      <c r="GY108"/>
+      <c r="GZ108"/>
+      <c r="HA108"/>
+      <c r="HB108"/>
+      <c r="HC108"/>
+      <c r="HD108"/>
+      <c r="HE108"/>
+      <c r="HF108"/>
+      <c r="HG108"/>
+      <c r="HH108"/>
+      <c r="HI108"/>
+      <c r="HJ108"/>
+      <c r="HK108"/>
+      <c r="HL108"/>
+      <c r="HM108"/>
+      <c r="HN108"/>
+      <c r="HO108"/>
+      <c r="HP108"/>
+      <c r="HQ108"/>
+      <c r="HR108"/>
+      <c r="HS108"/>
+      <c r="HT108"/>
+      <c r="HU108"/>
+      <c r="HV108"/>
+      <c r="HW108"/>
+      <c r="HX108"/>
+      <c r="HY108"/>
+      <c r="HZ108"/>
+      <c r="IA108"/>
+      <c r="IB108"/>
+      <c r="IC108"/>
+      <c r="ID108"/>
+      <c r="IE108"/>
+      <c r="IF108"/>
+      <c r="IG108"/>
+      <c r="IH108"/>
+      <c r="II108"/>
+      <c r="IJ108"/>
+      <c r="IK108"/>
+      <c r="IL108"/>
+      <c r="IM108"/>
+      <c r="IN108"/>
+      <c r="IO108"/>
+      <c r="IP108"/>
+      <c r="IQ108"/>
+      <c r="IR108"/>
+      <c r="IS108"/>
+      <c r="IT108"/>
+      <c r="IU108"/>
+      <c r="IV108"/>
+      <c r="IW108"/>
+    </row>
+    <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A109" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="B109" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="C109" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="D109" s="57"/>
+      <c r="E109" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F109" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" s="81">
+        <v>0</v>
+      </c>
+      <c r="H109" s="57">
+        <v>1</v>
+      </c>
+      <c r="I109" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J109" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K109"/>
+      <c r="L109"/>
+      <c r="M109"/>
+      <c r="N109"/>
+      <c r="O109"/>
+      <c r="P109"/>
+      <c r="Q109"/>
+      <c r="R109"/>
+      <c r="S109"/>
+      <c r="T109"/>
+      <c r="U109"/>
+      <c r="V109"/>
+      <c r="W109"/>
+      <c r="X109"/>
+      <c r="Y109"/>
+      <c r="Z109"/>
+      <c r="AA109"/>
+      <c r="AB109"/>
+      <c r="AC109"/>
+      <c r="AD109"/>
+      <c r="AE109"/>
+      <c r="AF109"/>
+      <c r="AG109"/>
+      <c r="AH109"/>
+      <c r="AI109"/>
+      <c r="AJ109"/>
+      <c r="AK109"/>
+      <c r="AL109"/>
+      <c r="AM109"/>
+      <c r="AN109"/>
+      <c r="AO109"/>
+      <c r="AP109"/>
+      <c r="AQ109"/>
+      <c r="AR109"/>
+      <c r="AS109"/>
+      <c r="AT109"/>
+      <c r="AU109"/>
+      <c r="AV109"/>
+      <c r="AW109"/>
+      <c r="AX109"/>
+      <c r="AY109"/>
+      <c r="AZ109"/>
+      <c r="BA109"/>
+      <c r="BB109"/>
+      <c r="BC109"/>
+      <c r="BD109"/>
+      <c r="BE109"/>
+      <c r="BF109"/>
+      <c r="BG109"/>
+      <c r="BH109"/>
+      <c r="BI109"/>
+      <c r="BJ109"/>
+      <c r="BK109"/>
+      <c r="BL109"/>
+      <c r="BM109"/>
+      <c r="BN109"/>
+      <c r="BO109"/>
+      <c r="BP109"/>
+      <c r="BQ109"/>
+      <c r="BR109"/>
+      <c r="BS109"/>
+      <c r="BT109"/>
+      <c r="BU109"/>
+      <c r="BV109"/>
+      <c r="BW109"/>
+      <c r="BX109"/>
+      <c r="BY109"/>
+      <c r="BZ109"/>
+      <c r="CA109"/>
+      <c r="CB109"/>
+      <c r="CC109"/>
+      <c r="CD109"/>
+      <c r="CE109"/>
+      <c r="CF109"/>
+      <c r="CG109"/>
+      <c r="CH109"/>
+      <c r="CI109"/>
+      <c r="CJ109"/>
+      <c r="CK109"/>
+      <c r="CL109"/>
+      <c r="CM109"/>
+      <c r="CN109"/>
+      <c r="CO109"/>
+      <c r="CP109"/>
+      <c r="CQ109"/>
+      <c r="CR109"/>
+      <c r="CS109"/>
+      <c r="CT109"/>
+      <c r="CU109"/>
+      <c r="CV109"/>
+      <c r="CW109"/>
+      <c r="CX109"/>
+      <c r="CY109"/>
+      <c r="CZ109"/>
+      <c r="DA109"/>
+      <c r="DB109"/>
+      <c r="DC109"/>
+      <c r="DD109"/>
+      <c r="DE109"/>
+      <c r="DF109"/>
+      <c r="DG109"/>
+      <c r="DH109"/>
+      <c r="DI109"/>
+      <c r="DJ109"/>
+      <c r="DK109"/>
+      <c r="DL109"/>
+      <c r="DM109"/>
+      <c r="DN109"/>
+      <c r="DO109"/>
+      <c r="DP109"/>
+      <c r="DQ109"/>
+      <c r="DR109"/>
+      <c r="DS109"/>
+      <c r="DT109"/>
+      <c r="DU109"/>
+      <c r="DV109"/>
+      <c r="DW109"/>
+      <c r="DX109"/>
+      <c r="DY109"/>
+      <c r="DZ109"/>
+      <c r="EA109"/>
+      <c r="EB109"/>
+      <c r="EC109"/>
+      <c r="ED109"/>
+      <c r="EE109"/>
+      <c r="EF109"/>
+      <c r="EG109"/>
+      <c r="EH109"/>
+      <c r="EI109"/>
+      <c r="EJ109"/>
+      <c r="EK109"/>
+      <c r="EL109"/>
+      <c r="EM109"/>
+      <c r="EN109"/>
+      <c r="EO109"/>
+      <c r="EP109"/>
+      <c r="EQ109"/>
+      <c r="ER109"/>
+      <c r="ES109"/>
+      <c r="ET109"/>
+      <c r="EU109"/>
+      <c r="EV109"/>
+      <c r="EW109"/>
+      <c r="EX109"/>
+      <c r="EY109"/>
+      <c r="EZ109"/>
+      <c r="FA109"/>
+      <c r="FB109"/>
+      <c r="FC109"/>
+      <c r="FD109"/>
+      <c r="FE109"/>
+      <c r="FF109"/>
+      <c r="FG109"/>
+      <c r="FH109"/>
+      <c r="FI109"/>
+      <c r="FJ109"/>
+      <c r="FK109"/>
+      <c r="FL109"/>
+      <c r="FM109"/>
+      <c r="FN109"/>
+      <c r="FO109"/>
+      <c r="FP109"/>
+      <c r="FQ109"/>
+      <c r="FR109"/>
+      <c r="FS109"/>
+      <c r="FT109"/>
+      <c r="FU109"/>
+      <c r="FV109"/>
+      <c r="FW109"/>
+      <c r="FX109"/>
+      <c r="FY109"/>
+      <c r="FZ109"/>
+      <c r="GA109"/>
+      <c r="GB109"/>
+      <c r="GC109"/>
+      <c r="GD109"/>
+      <c r="GE109"/>
+      <c r="GF109"/>
+      <c r="GG109"/>
+      <c r="GH109"/>
+      <c r="GI109"/>
+      <c r="GJ109"/>
+      <c r="GK109"/>
+      <c r="GL109"/>
+      <c r="GM109"/>
+      <c r="GN109"/>
+      <c r="GO109"/>
+      <c r="GP109"/>
+      <c r="GQ109"/>
+      <c r="GR109"/>
+      <c r="GS109"/>
+      <c r="GT109"/>
+      <c r="GU109"/>
+      <c r="GV109"/>
+      <c r="GW109"/>
+      <c r="GX109"/>
+      <c r="GY109"/>
+      <c r="GZ109"/>
+      <c r="HA109"/>
+      <c r="HB109"/>
+      <c r="HC109"/>
+      <c r="HD109"/>
+      <c r="HE109"/>
+      <c r="HF109"/>
+      <c r="HG109"/>
+      <c r="HH109"/>
+      <c r="HI109"/>
+      <c r="HJ109"/>
+      <c r="HK109"/>
+      <c r="HL109"/>
+      <c r="HM109"/>
+      <c r="HN109"/>
+      <c r="HO109"/>
+      <c r="HP109"/>
+      <c r="HQ109"/>
+      <c r="HR109"/>
+      <c r="HS109"/>
+      <c r="HT109"/>
+      <c r="HU109"/>
+      <c r="HV109"/>
+      <c r="HW109"/>
+      <c r="HX109"/>
+      <c r="HY109"/>
+      <c r="HZ109"/>
+      <c r="IA109"/>
+      <c r="IB109"/>
+      <c r="IC109"/>
+      <c r="ID109"/>
+      <c r="IE109"/>
+      <c r="IF109"/>
+      <c r="IG109"/>
+      <c r="IH109"/>
+      <c r="II109"/>
+      <c r="IJ109"/>
+      <c r="IK109"/>
+      <c r="IL109"/>
+      <c r="IM109"/>
+      <c r="IN109"/>
+      <c r="IO109"/>
+      <c r="IP109"/>
+      <c r="IQ109"/>
+      <c r="IR109"/>
+      <c r="IS109"/>
+      <c r="IT109"/>
+      <c r="IU109"/>
+      <c r="IV109"/>
+      <c r="IW109"/>
+    </row>
+    <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A110" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="B110" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="C110" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="D110" s="57"/>
+      <c r="E110" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F110" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G110" s="81">
+        <v>0</v>
+      </c>
+      <c r="H110" s="57">
+        <v>1</v>
+      </c>
+      <c r="I110" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J110" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K110"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110"/>
+      <c r="R110"/>
+      <c r="S110"/>
+      <c r="T110"/>
+      <c r="U110"/>
+      <c r="V110"/>
+      <c r="W110"/>
+      <c r="X110"/>
+      <c r="Y110"/>
+      <c r="Z110"/>
+      <c r="AA110"/>
+      <c r="AB110"/>
+      <c r="AC110"/>
+      <c r="AD110"/>
+      <c r="AE110"/>
+      <c r="AF110"/>
+      <c r="AG110"/>
+      <c r="AH110"/>
+      <c r="AI110"/>
+      <c r="AJ110"/>
+      <c r="AK110"/>
+      <c r="AL110"/>
+      <c r="AM110"/>
+      <c r="AN110"/>
+      <c r="AO110"/>
+      <c r="AP110"/>
+      <c r="AQ110"/>
+      <c r="AR110"/>
+      <c r="AS110"/>
+      <c r="AT110"/>
+      <c r="AU110"/>
+      <c r="AV110"/>
+      <c r="AW110"/>
+      <c r="AX110"/>
+      <c r="AY110"/>
+      <c r="AZ110"/>
+      <c r="BA110"/>
+      <c r="BB110"/>
+      <c r="BC110"/>
+      <c r="BD110"/>
+      <c r="BE110"/>
+      <c r="BF110"/>
+      <c r="BG110"/>
+      <c r="BH110"/>
+      <c r="BI110"/>
+      <c r="BJ110"/>
+      <c r="BK110"/>
+      <c r="BL110"/>
+      <c r="BM110"/>
+      <c r="BN110"/>
+      <c r="BO110"/>
+      <c r="BP110"/>
+      <c r="BQ110"/>
+      <c r="BR110"/>
+      <c r="BS110"/>
+      <c r="BT110"/>
+      <c r="BU110"/>
+      <c r="BV110"/>
+      <c r="BW110"/>
+      <c r="BX110"/>
+      <c r="BY110"/>
+      <c r="BZ110"/>
+      <c r="CA110"/>
+      <c r="CB110"/>
+      <c r="CC110"/>
+      <c r="CD110"/>
+      <c r="CE110"/>
+      <c r="CF110"/>
+      <c r="CG110"/>
+      <c r="CH110"/>
+      <c r="CI110"/>
+      <c r="CJ110"/>
+      <c r="CK110"/>
+      <c r="CL110"/>
+      <c r="CM110"/>
+      <c r="CN110"/>
+      <c r="CO110"/>
+      <c r="CP110"/>
+      <c r="CQ110"/>
+      <c r="CR110"/>
+      <c r="CS110"/>
+      <c r="CT110"/>
+      <c r="CU110"/>
+      <c r="CV110"/>
+      <c r="CW110"/>
+      <c r="CX110"/>
+      <c r="CY110"/>
+      <c r="CZ110"/>
+      <c r="DA110"/>
+      <c r="DB110"/>
+      <c r="DC110"/>
+      <c r="DD110"/>
+      <c r="DE110"/>
+      <c r="DF110"/>
+      <c r="DG110"/>
+      <c r="DH110"/>
+      <c r="DI110"/>
+      <c r="DJ110"/>
+      <c r="DK110"/>
+      <c r="DL110"/>
+      <c r="DM110"/>
+      <c r="DN110"/>
+      <c r="DO110"/>
+      <c r="DP110"/>
+      <c r="DQ110"/>
+      <c r="DR110"/>
+      <c r="DS110"/>
+      <c r="DT110"/>
+      <c r="DU110"/>
+      <c r="DV110"/>
+      <c r="DW110"/>
+      <c r="DX110"/>
+      <c r="DY110"/>
+      <c r="DZ110"/>
+      <c r="EA110"/>
+      <c r="EB110"/>
+      <c r="EC110"/>
+      <c r="ED110"/>
+      <c r="EE110"/>
+      <c r="EF110"/>
+      <c r="EG110"/>
+      <c r="EH110"/>
+      <c r="EI110"/>
+      <c r="EJ110"/>
+      <c r="EK110"/>
+      <c r="EL110"/>
+      <c r="EM110"/>
+      <c r="EN110"/>
+      <c r="EO110"/>
+      <c r="EP110"/>
+      <c r="EQ110"/>
+      <c r="ER110"/>
+      <c r="ES110"/>
+      <c r="ET110"/>
+      <c r="EU110"/>
+      <c r="EV110"/>
+      <c r="EW110"/>
+      <c r="EX110"/>
+      <c r="EY110"/>
+      <c r="EZ110"/>
+      <c r="FA110"/>
+      <c r="FB110"/>
+      <c r="FC110"/>
+      <c r="FD110"/>
+      <c r="FE110"/>
+      <c r="FF110"/>
+      <c r="FG110"/>
+      <c r="FH110"/>
+      <c r="FI110"/>
+      <c r="FJ110"/>
+      <c r="FK110"/>
+      <c r="FL110"/>
+      <c r="FM110"/>
+      <c r="FN110"/>
+      <c r="FO110"/>
+      <c r="FP110"/>
+      <c r="FQ110"/>
+      <c r="FR110"/>
+      <c r="FS110"/>
+      <c r="FT110"/>
+      <c r="FU110"/>
+      <c r="FV110"/>
+      <c r="FW110"/>
+      <c r="FX110"/>
+      <c r="FY110"/>
+      <c r="FZ110"/>
+      <c r="GA110"/>
+      <c r="GB110"/>
+      <c r="GC110"/>
+      <c r="GD110"/>
+      <c r="GE110"/>
+      <c r="GF110"/>
+      <c r="GG110"/>
+      <c r="GH110"/>
+      <c r="GI110"/>
+      <c r="GJ110"/>
+      <c r="GK110"/>
+      <c r="GL110"/>
+      <c r="GM110"/>
+      <c r="GN110"/>
+      <c r="GO110"/>
+      <c r="GP110"/>
+      <c r="GQ110"/>
+      <c r="GR110"/>
+      <c r="GS110"/>
+      <c r="GT110"/>
+      <c r="GU110"/>
+      <c r="GV110"/>
+      <c r="GW110"/>
+      <c r="GX110"/>
+      <c r="GY110"/>
+      <c r="GZ110"/>
+      <c r="HA110"/>
+      <c r="HB110"/>
+      <c r="HC110"/>
+      <c r="HD110"/>
+      <c r="HE110"/>
+      <c r="HF110"/>
+      <c r="HG110"/>
+      <c r="HH110"/>
+      <c r="HI110"/>
+      <c r="HJ110"/>
+      <c r="HK110"/>
+      <c r="HL110"/>
+      <c r="HM110"/>
+      <c r="HN110"/>
+      <c r="HO110"/>
+      <c r="HP110"/>
+      <c r="HQ110"/>
+      <c r="HR110"/>
+      <c r="HS110"/>
+      <c r="HT110"/>
+      <c r="HU110"/>
+      <c r="HV110"/>
+      <c r="HW110"/>
+      <c r="HX110"/>
+      <c r="HY110"/>
+      <c r="HZ110"/>
+      <c r="IA110"/>
+      <c r="IB110"/>
+      <c r="IC110"/>
+      <c r="ID110"/>
+      <c r="IE110"/>
+      <c r="IF110"/>
+      <c r="IG110"/>
+      <c r="IH110"/>
+      <c r="II110"/>
+      <c r="IJ110"/>
+      <c r="IK110"/>
+      <c r="IL110"/>
+      <c r="IM110"/>
+      <c r="IN110"/>
+      <c r="IO110"/>
+      <c r="IP110"/>
+      <c r="IQ110"/>
+      <c r="IR110"/>
+      <c r="IS110"/>
+      <c r="IT110"/>
+      <c r="IU110"/>
+      <c r="IV110"/>
+      <c r="IW110"/>
+    </row>
+    <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A111" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="B111" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="C111" s="57" t="s">
+        <v>235</v>
+      </c>
+      <c r="D111" s="57"/>
+      <c r="E111" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F111" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111" s="81">
+        <v>4</v>
+      </c>
+      <c r="H111" s="57">
+        <v>1</v>
+      </c>
+      <c r="I111" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J111" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K111"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+      <c r="P111"/>
+      <c r="Q111"/>
+      <c r="R111"/>
+      <c r="S111"/>
+      <c r="T111"/>
+      <c r="U111"/>
+      <c r="V111"/>
+      <c r="W111"/>
+      <c r="X111"/>
+      <c r="Y111"/>
+      <c r="Z111"/>
+      <c r="AA111"/>
+      <c r="AB111"/>
+      <c r="AC111"/>
+      <c r="AD111"/>
+      <c r="AE111"/>
+      <c r="AF111"/>
+      <c r="AG111"/>
+      <c r="AH111"/>
+      <c r="AI111"/>
+      <c r="AJ111"/>
+      <c r="AK111"/>
+      <c r="AL111"/>
+      <c r="AM111"/>
+      <c r="AN111"/>
+      <c r="AO111"/>
+      <c r="AP111"/>
+      <c r="AQ111"/>
+      <c r="AR111"/>
+      <c r="AS111"/>
+      <c r="AT111"/>
+      <c r="AU111"/>
+      <c r="AV111"/>
+      <c r="AW111"/>
+      <c r="AX111"/>
+      <c r="AY111"/>
+      <c r="AZ111"/>
+      <c r="BA111"/>
+      <c r="BB111"/>
+      <c r="BC111"/>
+      <c r="BD111"/>
+      <c r="BE111"/>
+      <c r="BF111"/>
+      <c r="BG111"/>
+      <c r="BH111"/>
+      <c r="BI111"/>
+      <c r="BJ111"/>
+      <c r="BK111"/>
+      <c r="BL111"/>
+      <c r="BM111"/>
+      <c r="BN111"/>
+      <c r="BO111"/>
+      <c r="BP111"/>
+      <c r="BQ111"/>
+      <c r="BR111"/>
+      <c r="BS111"/>
+      <c r="BT111"/>
+      <c r="BU111"/>
+      <c r="BV111"/>
+      <c r="BW111"/>
+      <c r="BX111"/>
+      <c r="BY111"/>
+      <c r="BZ111"/>
+      <c r="CA111"/>
+      <c r="CB111"/>
+      <c r="CC111"/>
+      <c r="CD111"/>
+      <c r="CE111"/>
+      <c r="CF111"/>
+      <c r="CG111"/>
+      <c r="CH111"/>
+      <c r="CI111"/>
+      <c r="CJ111"/>
+      <c r="CK111"/>
+      <c r="CL111"/>
+      <c r="CM111"/>
+      <c r="CN111"/>
+      <c r="CO111"/>
+      <c r="CP111"/>
+      <c r="CQ111"/>
+      <c r="CR111"/>
+      <c r="CS111"/>
+      <c r="CT111"/>
+      <c r="CU111"/>
+      <c r="CV111"/>
+      <c r="CW111"/>
+      <c r="CX111"/>
+      <c r="CY111"/>
+      <c r="CZ111"/>
+      <c r="DA111"/>
+      <c r="DB111"/>
+      <c r="DC111"/>
+      <c r="DD111"/>
+      <c r="DE111"/>
+      <c r="DF111"/>
+      <c r="DG111"/>
+      <c r="DH111"/>
+      <c r="DI111"/>
+      <c r="DJ111"/>
+      <c r="DK111"/>
+      <c r="DL111"/>
+      <c r="DM111"/>
+      <c r="DN111"/>
+      <c r="DO111"/>
+      <c r="DP111"/>
+      <c r="DQ111"/>
+      <c r="DR111"/>
+      <c r="DS111"/>
+      <c r="DT111"/>
+      <c r="DU111"/>
+      <c r="DV111"/>
+      <c r="DW111"/>
+      <c r="DX111"/>
+      <c r="DY111"/>
+      <c r="DZ111"/>
+      <c r="EA111"/>
+      <c r="EB111"/>
+      <c r="EC111"/>
+      <c r="ED111"/>
+      <c r="EE111"/>
+      <c r="EF111"/>
+      <c r="EG111"/>
+      <c r="EH111"/>
+      <c r="EI111"/>
+      <c r="EJ111"/>
+      <c r="EK111"/>
+      <c r="EL111"/>
+      <c r="EM111"/>
+      <c r="EN111"/>
+      <c r="EO111"/>
+      <c r="EP111"/>
+      <c r="EQ111"/>
+      <c r="ER111"/>
+      <c r="ES111"/>
+      <c r="ET111"/>
+      <c r="EU111"/>
+      <c r="EV111"/>
+      <c r="EW111"/>
+      <c r="EX111"/>
+      <c r="EY111"/>
+      <c r="EZ111"/>
+      <c r="FA111"/>
+      <c r="FB111"/>
+      <c r="FC111"/>
+      <c r="FD111"/>
+      <c r="FE111"/>
+      <c r="FF111"/>
+      <c r="FG111"/>
+      <c r="FH111"/>
+      <c r="FI111"/>
+      <c r="FJ111"/>
+      <c r="FK111"/>
+      <c r="FL111"/>
+      <c r="FM111"/>
+      <c r="FN111"/>
+      <c r="FO111"/>
+      <c r="FP111"/>
+      <c r="FQ111"/>
+      <c r="FR111"/>
+      <c r="FS111"/>
+      <c r="FT111"/>
+      <c r="FU111"/>
+      <c r="FV111"/>
+      <c r="FW111"/>
+      <c r="FX111"/>
+      <c r="FY111"/>
+      <c r="FZ111"/>
+      <c r="GA111"/>
+      <c r="GB111"/>
+      <c r="GC111"/>
+      <c r="GD111"/>
+      <c r="GE111"/>
+      <c r="GF111"/>
+      <c r="GG111"/>
+      <c r="GH111"/>
+      <c r="GI111"/>
+      <c r="GJ111"/>
+      <c r="GK111"/>
+      <c r="GL111"/>
+      <c r="GM111"/>
+      <c r="GN111"/>
+      <c r="GO111"/>
+      <c r="GP111"/>
+      <c r="GQ111"/>
+      <c r="GR111"/>
+      <c r="GS111"/>
+      <c r="GT111"/>
+      <c r="GU111"/>
+      <c r="GV111"/>
+      <c r="GW111"/>
+      <c r="GX111"/>
+      <c r="GY111"/>
+      <c r="GZ111"/>
+      <c r="HA111"/>
+      <c r="HB111"/>
+      <c r="HC111"/>
+      <c r="HD111"/>
+      <c r="HE111"/>
+      <c r="HF111"/>
+      <c r="HG111"/>
+      <c r="HH111"/>
+      <c r="HI111"/>
+      <c r="HJ111"/>
+      <c r="HK111"/>
+      <c r="HL111"/>
+      <c r="HM111"/>
+      <c r="HN111"/>
+      <c r="HO111"/>
+      <c r="HP111"/>
+      <c r="HQ111"/>
+      <c r="HR111"/>
+      <c r="HS111"/>
+      <c r="HT111"/>
+      <c r="HU111"/>
+      <c r="HV111"/>
+      <c r="HW111"/>
+      <c r="HX111"/>
+      <c r="HY111"/>
+      <c r="HZ111"/>
+      <c r="IA111"/>
+      <c r="IB111"/>
+      <c r="IC111"/>
+      <c r="ID111"/>
+      <c r="IE111"/>
+      <c r="IF111"/>
+      <c r="IG111"/>
+      <c r="IH111"/>
+      <c r="II111"/>
+      <c r="IJ111"/>
+      <c r="IK111"/>
+      <c r="IL111"/>
+      <c r="IM111"/>
+      <c r="IN111"/>
+      <c r="IO111"/>
+      <c r="IP111"/>
+      <c r="IQ111"/>
+      <c r="IR111"/>
+      <c r="IS111"/>
+      <c r="IT111"/>
+      <c r="IU111"/>
+      <c r="IV111"/>
+      <c r="IW111"/>
+    </row>
+    <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A112" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="B112" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="C112" s="57" t="s">
+        <v>237</v>
+      </c>
+      <c r="D112" s="57"/>
+      <c r="E112" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F112" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G112" s="81">
+        <v>0</v>
+      </c>
+      <c r="H112" s="57">
+        <v>1</v>
+      </c>
+      <c r="I112" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J112" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K112"/>
+      <c r="L112"/>
+      <c r="M112"/>
+      <c r="N112"/>
+      <c r="O112"/>
+      <c r="P112"/>
+      <c r="Q112"/>
+      <c r="R112"/>
+      <c r="S112"/>
+      <c r="T112"/>
+      <c r="U112"/>
+      <c r="V112"/>
+      <c r="W112"/>
+      <c r="X112"/>
+      <c r="Y112"/>
+      <c r="Z112"/>
+      <c r="AA112"/>
+      <c r="AB112"/>
+      <c r="AC112"/>
+      <c r="AD112"/>
+      <c r="AE112"/>
+      <c r="AF112"/>
+      <c r="AG112"/>
+      <c r="AH112"/>
+      <c r="AI112"/>
+      <c r="AJ112"/>
+      <c r="AK112"/>
+      <c r="AL112"/>
+      <c r="AM112"/>
+      <c r="AN112"/>
+      <c r="AO112"/>
+      <c r="AP112"/>
+      <c r="AQ112"/>
+      <c r="AR112"/>
+      <c r="AS112"/>
+      <c r="AT112"/>
+      <c r="AU112"/>
+      <c r="AV112"/>
+      <c r="AW112"/>
+      <c r="AX112"/>
+      <c r="AY112"/>
+      <c r="AZ112"/>
+      <c r="BA112"/>
+      <c r="BB112"/>
+      <c r="BC112"/>
+      <c r="BD112"/>
+      <c r="BE112"/>
+      <c r="BF112"/>
+      <c r="BG112"/>
+      <c r="BH112"/>
+      <c r="BI112"/>
+      <c r="BJ112"/>
+      <c r="BK112"/>
+      <c r="BL112"/>
+      <c r="BM112"/>
+      <c r="BN112"/>
+      <c r="BO112"/>
+      <c r="BP112"/>
+      <c r="BQ112"/>
+      <c r="BR112"/>
+      <c r="BS112"/>
+      <c r="BT112"/>
+      <c r="BU112"/>
+      <c r="BV112"/>
+      <c r="BW112"/>
+      <c r="BX112"/>
+      <c r="BY112"/>
+      <c r="BZ112"/>
+      <c r="CA112"/>
+      <c r="CB112"/>
+      <c r="CC112"/>
+      <c r="CD112"/>
+      <c r="CE112"/>
+      <c r="CF112"/>
+      <c r="CG112"/>
+      <c r="CH112"/>
+      <c r="CI112"/>
+      <c r="CJ112"/>
+      <c r="CK112"/>
+      <c r="CL112"/>
+      <c r="CM112"/>
+      <c r="CN112"/>
+      <c r="CO112"/>
+      <c r="CP112"/>
+      <c r="CQ112"/>
+      <c r="CR112"/>
+      <c r="CS112"/>
+      <c r="CT112"/>
+      <c r="CU112"/>
+      <c r="CV112"/>
+      <c r="CW112"/>
+      <c r="CX112"/>
+      <c r="CY112"/>
+      <c r="CZ112"/>
+      <c r="DA112"/>
+      <c r="DB112"/>
+      <c r="DC112"/>
+      <c r="DD112"/>
+      <c r="DE112"/>
+      <c r="DF112"/>
+      <c r="DG112"/>
+      <c r="DH112"/>
+      <c r="DI112"/>
+      <c r="DJ112"/>
+      <c r="DK112"/>
+      <c r="DL112"/>
+      <c r="DM112"/>
+      <c r="DN112"/>
+      <c r="DO112"/>
+      <c r="DP112"/>
+      <c r="DQ112"/>
+      <c r="DR112"/>
+      <c r="DS112"/>
+      <c r="DT112"/>
+      <c r="DU112"/>
+      <c r="DV112"/>
+      <c r="DW112"/>
+      <c r="DX112"/>
+      <c r="DY112"/>
+      <c r="DZ112"/>
+      <c r="EA112"/>
+      <c r="EB112"/>
+      <c r="EC112"/>
+      <c r="ED112"/>
+      <c r="EE112"/>
+      <c r="EF112"/>
+      <c r="EG112"/>
+      <c r="EH112"/>
+      <c r="EI112"/>
+      <c r="EJ112"/>
+      <c r="EK112"/>
+      <c r="EL112"/>
+      <c r="EM112"/>
+      <c r="EN112"/>
+      <c r="EO112"/>
+      <c r="EP112"/>
+      <c r="EQ112"/>
+      <c r="ER112"/>
+      <c r="ES112"/>
+      <c r="ET112"/>
+      <c r="EU112"/>
+      <c r="EV112"/>
+      <c r="EW112"/>
+      <c r="EX112"/>
+      <c r="EY112"/>
+      <c r="EZ112"/>
+      <c r="FA112"/>
+      <c r="FB112"/>
+      <c r="FC112"/>
+      <c r="FD112"/>
+      <c r="FE112"/>
+      <c r="FF112"/>
+      <c r="FG112"/>
+      <c r="FH112"/>
+      <c r="FI112"/>
+      <c r="FJ112"/>
+      <c r="FK112"/>
+      <c r="FL112"/>
+      <c r="FM112"/>
+      <c r="FN112"/>
+      <c r="FO112"/>
+      <c r="FP112"/>
+      <c r="FQ112"/>
+      <c r="FR112"/>
+      <c r="FS112"/>
+      <c r="FT112"/>
+      <c r="FU112"/>
+      <c r="FV112"/>
+      <c r="FW112"/>
+      <c r="FX112"/>
+      <c r="FY112"/>
+      <c r="FZ112"/>
+      <c r="GA112"/>
+      <c r="GB112"/>
+      <c r="GC112"/>
+      <c r="GD112"/>
+      <c r="GE112"/>
+      <c r="GF112"/>
+      <c r="GG112"/>
+      <c r="GH112"/>
+      <c r="GI112"/>
+      <c r="GJ112"/>
+      <c r="GK112"/>
+      <c r="GL112"/>
+      <c r="GM112"/>
+      <c r="GN112"/>
+      <c r="GO112"/>
+      <c r="GP112"/>
+      <c r="GQ112"/>
+      <c r="GR112"/>
+      <c r="GS112"/>
+      <c r="GT112"/>
+      <c r="GU112"/>
+      <c r="GV112"/>
+      <c r="GW112"/>
+      <c r="GX112"/>
+      <c r="GY112"/>
+      <c r="GZ112"/>
+      <c r="HA112"/>
+      <c r="HB112"/>
+      <c r="HC112"/>
+      <c r="HD112"/>
+      <c r="HE112"/>
+      <c r="HF112"/>
+      <c r="HG112"/>
+      <c r="HH112"/>
+      <c r="HI112"/>
+      <c r="HJ112"/>
+      <c r="HK112"/>
+      <c r="HL112"/>
+      <c r="HM112"/>
+      <c r="HN112"/>
+      <c r="HO112"/>
+      <c r="HP112"/>
+      <c r="HQ112"/>
+      <c r="HR112"/>
+      <c r="HS112"/>
+      <c r="HT112"/>
+      <c r="HU112"/>
+      <c r="HV112"/>
+      <c r="HW112"/>
+      <c r="HX112"/>
+      <c r="HY112"/>
+      <c r="HZ112"/>
+      <c r="IA112"/>
+      <c r="IB112"/>
+      <c r="IC112"/>
+      <c r="ID112"/>
+      <c r="IE112"/>
+      <c r="IF112"/>
+      <c r="IG112"/>
+      <c r="IH112"/>
+      <c r="II112"/>
+      <c r="IJ112"/>
+      <c r="IK112"/>
+      <c r="IL112"/>
+      <c r="IM112"/>
+      <c r="IN112"/>
+      <c r="IO112"/>
+      <c r="IP112"/>
+      <c r="IQ112"/>
+      <c r="IR112"/>
+      <c r="IS112"/>
+      <c r="IT112"/>
+      <c r="IU112"/>
+      <c r="IV112"/>
+      <c r="IW112"/>
+    </row>
+    <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A113" s="57" t="s">
+        <v>238</v>
+      </c>
+      <c r="B113" s="57" t="s">
+        <v>238</v>
+      </c>
+      <c r="C113" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="D113" s="57"/>
+      <c r="E113" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F113" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G113" s="81">
+        <v>0</v>
+      </c>
+      <c r="H113" s="57">
+        <v>1</v>
+      </c>
+      <c r="I113" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J113" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K113"/>
+      <c r="L113"/>
+      <c r="M113"/>
+      <c r="N113"/>
+      <c r="O113"/>
+      <c r="P113"/>
+      <c r="Q113"/>
+      <c r="R113"/>
+      <c r="S113"/>
+      <c r="T113"/>
+      <c r="U113"/>
+      <c r="V113"/>
+      <c r="W113"/>
+      <c r="X113"/>
+      <c r="Y113"/>
+      <c r="Z113"/>
+      <c r="AA113"/>
+      <c r="AB113"/>
+      <c r="AC113"/>
+      <c r="AD113"/>
+      <c r="AE113"/>
+      <c r="AF113"/>
+      <c r="AG113"/>
+      <c r="AH113"/>
+      <c r="AI113"/>
+      <c r="AJ113"/>
+      <c r="AK113"/>
+      <c r="AL113"/>
+      <c r="AM113"/>
+      <c r="AN113"/>
+      <c r="AO113"/>
+      <c r="AP113"/>
+      <c r="AQ113"/>
+      <c r="AR113"/>
+      <c r="AS113"/>
+      <c r="AT113"/>
+      <c r="AU113"/>
+      <c r="AV113"/>
+      <c r="AW113"/>
+      <c r="AX113"/>
+      <c r="AY113"/>
+      <c r="AZ113"/>
+      <c r="BA113"/>
+      <c r="BB113"/>
+      <c r="BC113"/>
+      <c r="BD113"/>
+      <c r="BE113"/>
+      <c r="BF113"/>
+      <c r="BG113"/>
+      <c r="BH113"/>
+      <c r="BI113"/>
+      <c r="BJ113"/>
+      <c r="BK113"/>
+      <c r="BL113"/>
+      <c r="BM113"/>
+      <c r="BN113"/>
+      <c r="BO113"/>
+      <c r="BP113"/>
+      <c r="BQ113"/>
+      <c r="BR113"/>
+      <c r="BS113"/>
+      <c r="BT113"/>
+      <c r="BU113"/>
+      <c r="BV113"/>
+      <c r="BW113"/>
+      <c r="BX113"/>
+      <c r="BY113"/>
+      <c r="BZ113"/>
+      <c r="CA113"/>
+      <c r="CB113"/>
+      <c r="CC113"/>
+      <c r="CD113"/>
+      <c r="CE113"/>
+      <c r="CF113"/>
+      <c r="CG113"/>
+      <c r="CH113"/>
+      <c r="CI113"/>
+      <c r="CJ113"/>
+      <c r="CK113"/>
+      <c r="CL113"/>
+      <c r="CM113"/>
+      <c r="CN113"/>
+      <c r="CO113"/>
+      <c r="CP113"/>
+      <c r="CQ113"/>
+      <c r="CR113"/>
+      <c r="CS113"/>
+      <c r="CT113"/>
+      <c r="CU113"/>
+      <c r="CV113"/>
+      <c r="CW113"/>
+      <c r="CX113"/>
+      <c r="CY113"/>
+      <c r="CZ113"/>
+      <c r="DA113"/>
+      <c r="DB113"/>
+      <c r="DC113"/>
+      <c r="DD113"/>
+      <c r="DE113"/>
+      <c r="DF113"/>
+      <c r="DG113"/>
+      <c r="DH113"/>
+      <c r="DI113"/>
+      <c r="DJ113"/>
+      <c r="DK113"/>
+      <c r="DL113"/>
+      <c r="DM113"/>
+      <c r="DN113"/>
+      <c r="DO113"/>
+      <c r="DP113"/>
+      <c r="DQ113"/>
+      <c r="DR113"/>
+      <c r="DS113"/>
+      <c r="DT113"/>
+      <c r="DU113"/>
+      <c r="DV113"/>
+      <c r="DW113"/>
+      <c r="DX113"/>
+      <c r="DY113"/>
+      <c r="DZ113"/>
+      <c r="EA113"/>
+      <c r="EB113"/>
+      <c r="EC113"/>
+      <c r="ED113"/>
+      <c r="EE113"/>
+      <c r="EF113"/>
+      <c r="EG113"/>
+      <c r="EH113"/>
+      <c r="EI113"/>
+      <c r="EJ113"/>
+      <c r="EK113"/>
+      <c r="EL113"/>
+      <c r="EM113"/>
+      <c r="EN113"/>
+      <c r="EO113"/>
+      <c r="EP113"/>
+      <c r="EQ113"/>
+      <c r="ER113"/>
+      <c r="ES113"/>
+      <c r="ET113"/>
+      <c r="EU113"/>
+      <c r="EV113"/>
+      <c r="EW113"/>
+      <c r="EX113"/>
+      <c r="EY113"/>
+      <c r="EZ113"/>
+      <c r="FA113"/>
+      <c r="FB113"/>
+      <c r="FC113"/>
+      <c r="FD113"/>
+      <c r="FE113"/>
+      <c r="FF113"/>
+      <c r="FG113"/>
+      <c r="FH113"/>
+      <c r="FI113"/>
+      <c r="FJ113"/>
+      <c r="FK113"/>
+      <c r="FL113"/>
+      <c r="FM113"/>
+      <c r="FN113"/>
+      <c r="FO113"/>
+      <c r="FP113"/>
+      <c r="FQ113"/>
+      <c r="FR113"/>
+      <c r="FS113"/>
+      <c r="FT113"/>
+      <c r="FU113"/>
+      <c r="FV113"/>
+      <c r="FW113"/>
+      <c r="FX113"/>
+      <c r="FY113"/>
+      <c r="FZ113"/>
+      <c r="GA113"/>
+      <c r="GB113"/>
+      <c r="GC113"/>
+      <c r="GD113"/>
+      <c r="GE113"/>
+      <c r="GF113"/>
+      <c r="GG113"/>
+      <c r="GH113"/>
+      <c r="GI113"/>
+      <c r="GJ113"/>
+      <c r="GK113"/>
+      <c r="GL113"/>
+      <c r="GM113"/>
+      <c r="GN113"/>
+      <c r="GO113"/>
+      <c r="GP113"/>
+      <c r="GQ113"/>
+      <c r="GR113"/>
+      <c r="GS113"/>
+      <c r="GT113"/>
+      <c r="GU113"/>
+      <c r="GV113"/>
+      <c r="GW113"/>
+      <c r="GX113"/>
+      <c r="GY113"/>
+      <c r="GZ113"/>
+      <c r="HA113"/>
+      <c r="HB113"/>
+      <c r="HC113"/>
+      <c r="HD113"/>
+      <c r="HE113"/>
+      <c r="HF113"/>
+      <c r="HG113"/>
+      <c r="HH113"/>
+      <c r="HI113"/>
+      <c r="HJ113"/>
+      <c r="HK113"/>
+      <c r="HL113"/>
+      <c r="HM113"/>
+      <c r="HN113"/>
+      <c r="HO113"/>
+      <c r="HP113"/>
+      <c r="HQ113"/>
+      <c r="HR113"/>
+      <c r="HS113"/>
+      <c r="HT113"/>
+      <c r="HU113"/>
+      <c r="HV113"/>
+      <c r="HW113"/>
+      <c r="HX113"/>
+      <c r="HY113"/>
+      <c r="HZ113"/>
+      <c r="IA113"/>
+      <c r="IB113"/>
+      <c r="IC113"/>
+      <c r="ID113"/>
+      <c r="IE113"/>
+      <c r="IF113"/>
+      <c r="IG113"/>
+      <c r="IH113"/>
+      <c r="II113"/>
+      <c r="IJ113"/>
+      <c r="IK113"/>
+      <c r="IL113"/>
+      <c r="IM113"/>
+      <c r="IN113"/>
+      <c r="IO113"/>
+      <c r="IP113"/>
+      <c r="IQ113"/>
+      <c r="IR113"/>
+      <c r="IS113"/>
+      <c r="IT113"/>
+      <c r="IU113"/>
+      <c r="IV113"/>
+      <c r="IW113"/>
+    </row>
+    <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A114" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="B114" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C114" s="97" t="s">
+        <v>239</v>
+      </c>
+      <c r="D114" s="57"/>
+      <c r="E114" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F114" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G114" s="81">
+        <v>0</v>
+      </c>
+      <c r="H114" s="57">
+        <v>1</v>
+      </c>
+      <c r="I114" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J114" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K114"/>
+      <c r="L114"/>
+      <c r="M114"/>
+      <c r="N114"/>
+      <c r="O114"/>
+      <c r="P114"/>
+      <c r="Q114"/>
+      <c r="R114"/>
+      <c r="S114"/>
+      <c r="T114"/>
+      <c r="U114"/>
+      <c r="V114"/>
+      <c r="W114"/>
+      <c r="X114"/>
+      <c r="Y114"/>
+      <c r="Z114"/>
+      <c r="AA114"/>
+      <c r="AB114"/>
+      <c r="AC114"/>
+      <c r="AD114"/>
+      <c r="AE114"/>
+      <c r="AF114"/>
+      <c r="AG114"/>
+      <c r="AH114"/>
+      <c r="AI114"/>
+      <c r="AJ114"/>
+      <c r="AK114"/>
+      <c r="AL114"/>
+      <c r="AM114"/>
+      <c r="AN114"/>
+      <c r="AO114"/>
+      <c r="AP114"/>
+      <c r="AQ114"/>
+      <c r="AR114"/>
+      <c r="AS114"/>
+      <c r="AT114"/>
+      <c r="AU114"/>
+      <c r="AV114"/>
+      <c r="AW114"/>
+      <c r="AX114"/>
+      <c r="AY114"/>
+      <c r="AZ114"/>
+      <c r="BA114"/>
+      <c r="BB114"/>
+      <c r="BC114"/>
+      <c r="BD114"/>
+      <c r="BE114"/>
+      <c r="BF114"/>
+      <c r="BG114"/>
+      <c r="BH114"/>
+      <c r="BI114"/>
+      <c r="BJ114"/>
+      <c r="BK114"/>
+      <c r="BL114"/>
+      <c r="BM114"/>
+      <c r="BN114"/>
+      <c r="BO114"/>
+      <c r="BP114"/>
+      <c r="BQ114"/>
+      <c r="BR114"/>
+      <c r="BS114"/>
+      <c r="BT114"/>
+      <c r="BU114"/>
+      <c r="BV114"/>
+      <c r="BW114"/>
+      <c r="BX114"/>
+      <c r="BY114"/>
+      <c r="BZ114"/>
+      <c r="CA114"/>
+      <c r="CB114"/>
+      <c r="CC114"/>
+      <c r="CD114"/>
+      <c r="CE114"/>
+      <c r="CF114"/>
+      <c r="CG114"/>
+      <c r="CH114"/>
+      <c r="CI114"/>
+      <c r="CJ114"/>
+      <c r="CK114"/>
+      <c r="CL114"/>
+      <c r="CM114"/>
+      <c r="CN114"/>
+      <c r="CO114"/>
+      <c r="CP114"/>
+      <c r="CQ114"/>
+      <c r="CR114"/>
+      <c r="CS114"/>
+      <c r="CT114"/>
+      <c r="CU114"/>
+      <c r="CV114"/>
+      <c r="CW114"/>
+      <c r="CX114"/>
+      <c r="CY114"/>
+      <c r="CZ114"/>
+      <c r="DA114"/>
+      <c r="DB114"/>
+      <c r="DC114"/>
+      <c r="DD114"/>
+      <c r="DE114"/>
+      <c r="DF114"/>
+      <c r="DG114"/>
+      <c r="DH114"/>
+      <c r="DI114"/>
+      <c r="DJ114"/>
+      <c r="DK114"/>
+      <c r="DL114"/>
+      <c r="DM114"/>
+      <c r="DN114"/>
+      <c r="DO114"/>
+      <c r="DP114"/>
+      <c r="DQ114"/>
+      <c r="DR114"/>
+      <c r="DS114"/>
+      <c r="DT114"/>
+      <c r="DU114"/>
+      <c r="DV114"/>
+      <c r="DW114"/>
+      <c r="DX114"/>
+      <c r="DY114"/>
+      <c r="DZ114"/>
+      <c r="EA114"/>
+      <c r="EB114"/>
+      <c r="EC114"/>
+      <c r="ED114"/>
+      <c r="EE114"/>
+      <c r="EF114"/>
+      <c r="EG114"/>
+      <c r="EH114"/>
+      <c r="EI114"/>
+      <c r="EJ114"/>
+      <c r="EK114"/>
+      <c r="EL114"/>
+      <c r="EM114"/>
+      <c r="EN114"/>
+      <c r="EO114"/>
+      <c r="EP114"/>
+      <c r="EQ114"/>
+      <c r="ER114"/>
+      <c r="ES114"/>
+      <c r="ET114"/>
+      <c r="EU114"/>
+      <c r="EV114"/>
+      <c r="EW114"/>
+      <c r="EX114"/>
+      <c r="EY114"/>
+      <c r="EZ114"/>
+      <c r="FA114"/>
+      <c r="FB114"/>
+      <c r="FC114"/>
+      <c r="FD114"/>
+      <c r="FE114"/>
+      <c r="FF114"/>
+      <c r="FG114"/>
+      <c r="FH114"/>
+      <c r="FI114"/>
+      <c r="FJ114"/>
+      <c r="FK114"/>
+      <c r="FL114"/>
+      <c r="FM114"/>
+      <c r="FN114"/>
+      <c r="FO114"/>
+      <c r="FP114"/>
+      <c r="FQ114"/>
+      <c r="FR114"/>
+      <c r="FS114"/>
+      <c r="FT114"/>
+      <c r="FU114"/>
+      <c r="FV114"/>
+      <c r="FW114"/>
+      <c r="FX114"/>
+      <c r="FY114"/>
+      <c r="FZ114"/>
+      <c r="GA114"/>
+      <c r="GB114"/>
+      <c r="GC114"/>
+      <c r="GD114"/>
+      <c r="GE114"/>
+      <c r="GF114"/>
+      <c r="GG114"/>
+      <c r="GH114"/>
+      <c r="GI114"/>
+      <c r="GJ114"/>
+      <c r="GK114"/>
+      <c r="GL114"/>
+      <c r="GM114"/>
+      <c r="GN114"/>
+      <c r="GO114"/>
+      <c r="GP114"/>
+      <c r="GQ114"/>
+      <c r="GR114"/>
+      <c r="GS114"/>
+      <c r="GT114"/>
+      <c r="GU114"/>
+      <c r="GV114"/>
+      <c r="GW114"/>
+      <c r="GX114"/>
+      <c r="GY114"/>
+      <c r="GZ114"/>
+      <c r="HA114"/>
+      <c r="HB114"/>
+      <c r="HC114"/>
+      <c r="HD114"/>
+      <c r="HE114"/>
+      <c r="HF114"/>
+      <c r="HG114"/>
+      <c r="HH114"/>
+      <c r="HI114"/>
+      <c r="HJ114"/>
+      <c r="HK114"/>
+      <c r="HL114"/>
+      <c r="HM114"/>
+      <c r="HN114"/>
+      <c r="HO114"/>
+      <c r="HP114"/>
+      <c r="HQ114"/>
+      <c r="HR114"/>
+      <c r="HS114"/>
+      <c r="HT114"/>
+      <c r="HU114"/>
+      <c r="HV114"/>
+      <c r="HW114"/>
+      <c r="HX114"/>
+      <c r="HY114"/>
+      <c r="HZ114"/>
+      <c r="IA114"/>
+      <c r="IB114"/>
+      <c r="IC114"/>
+      <c r="ID114"/>
+      <c r="IE114"/>
+      <c r="IF114"/>
+      <c r="IG114"/>
+      <c r="IH114"/>
+      <c r="II114"/>
+      <c r="IJ114"/>
+      <c r="IK114"/>
+      <c r="IL114"/>
+      <c r="IM114"/>
+      <c r="IN114"/>
+      <c r="IO114"/>
+      <c r="IP114"/>
+      <c r="IQ114"/>
+      <c r="IR114"/>
+      <c r="IS114"/>
+      <c r="IT114"/>
+      <c r="IU114"/>
+      <c r="IV114"/>
+      <c r="IW114"/>
+    </row>
+    <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A115" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="B115" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="C115" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="D115" s="57"/>
+      <c r="E115" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F115" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G115" s="81">
+        <v>0</v>
+      </c>
+      <c r="H115" s="57">
+        <v>1</v>
+      </c>
+      <c r="I115" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J115" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K115"/>
+      <c r="L115"/>
+      <c r="M115"/>
+      <c r="N115"/>
+      <c r="O115"/>
+      <c r="P115"/>
+      <c r="Q115"/>
+      <c r="R115"/>
+      <c r="S115"/>
+      <c r="T115"/>
+      <c r="U115"/>
+      <c r="V115"/>
+      <c r="W115"/>
+      <c r="X115"/>
+      <c r="Y115"/>
+      <c r="Z115"/>
+      <c r="AA115"/>
+      <c r="AB115"/>
+      <c r="AC115"/>
+      <c r="AD115"/>
+      <c r="AE115"/>
+      <c r="AF115"/>
+      <c r="AG115"/>
+      <c r="AH115"/>
+      <c r="AI115"/>
+      <c r="AJ115"/>
+      <c r="AK115"/>
+      <c r="AL115"/>
+      <c r="AM115"/>
+      <c r="AN115"/>
+      <c r="AO115"/>
+      <c r="AP115"/>
+      <c r="AQ115"/>
+      <c r="AR115"/>
+      <c r="AS115"/>
+      <c r="AT115"/>
+      <c r="AU115"/>
+      <c r="AV115"/>
+      <c r="AW115"/>
+      <c r="AX115"/>
+      <c r="AY115"/>
+      <c r="AZ115"/>
+      <c r="BA115"/>
+      <c r="BB115"/>
+      <c r="BC115"/>
+      <c r="BD115"/>
+      <c r="BE115"/>
+      <c r="BF115"/>
+      <c r="BG115"/>
+      <c r="BH115"/>
+      <c r="BI115"/>
+      <c r="BJ115"/>
+      <c r="BK115"/>
+      <c r="BL115"/>
+      <c r="BM115"/>
+      <c r="BN115"/>
+      <c r="BO115"/>
+      <c r="BP115"/>
+      <c r="BQ115"/>
+      <c r="BR115"/>
+      <c r="BS115"/>
+      <c r="BT115"/>
+      <c r="BU115"/>
+      <c r="BV115"/>
+      <c r="BW115"/>
+      <c r="BX115"/>
+      <c r="BY115"/>
+      <c r="BZ115"/>
+      <c r="CA115"/>
+      <c r="CB115"/>
+      <c r="CC115"/>
+      <c r="CD115"/>
+      <c r="CE115"/>
+      <c r="CF115"/>
+      <c r="CG115"/>
+      <c r="CH115"/>
+      <c r="CI115"/>
+      <c r="CJ115"/>
+      <c r="CK115"/>
+      <c r="CL115"/>
+      <c r="CM115"/>
+      <c r="CN115"/>
+      <c r="CO115"/>
+      <c r="CP115"/>
+      <c r="CQ115"/>
+      <c r="CR115"/>
+      <c r="CS115"/>
+      <c r="CT115"/>
+      <c r="CU115"/>
+      <c r="CV115"/>
+      <c r="CW115"/>
+      <c r="CX115"/>
+      <c r="CY115"/>
+      <c r="CZ115"/>
+      <c r="DA115"/>
+      <c r="DB115"/>
+      <c r="DC115"/>
+      <c r="DD115"/>
+      <c r="DE115"/>
+      <c r="DF115"/>
+      <c r="DG115"/>
+      <c r="DH115"/>
+      <c r="DI115"/>
+      <c r="DJ115"/>
+      <c r="DK115"/>
+      <c r="DL115"/>
+      <c r="DM115"/>
+      <c r="DN115"/>
+      <c r="DO115"/>
+      <c r="DP115"/>
+      <c r="DQ115"/>
+      <c r="DR115"/>
+      <c r="DS115"/>
+      <c r="DT115"/>
+      <c r="DU115"/>
+      <c r="DV115"/>
+      <c r="DW115"/>
+      <c r="DX115"/>
+      <c r="DY115"/>
+      <c r="DZ115"/>
+      <c r="EA115"/>
+      <c r="EB115"/>
+      <c r="EC115"/>
+      <c r="ED115"/>
+      <c r="EE115"/>
+      <c r="EF115"/>
+      <c r="EG115"/>
+      <c r="EH115"/>
+      <c r="EI115"/>
+      <c r="EJ115"/>
+      <c r="EK115"/>
+      <c r="EL115"/>
+      <c r="EM115"/>
+      <c r="EN115"/>
+      <c r="EO115"/>
+      <c r="EP115"/>
+      <c r="EQ115"/>
+      <c r="ER115"/>
+      <c r="ES115"/>
+      <c r="ET115"/>
+      <c r="EU115"/>
+      <c r="EV115"/>
+      <c r="EW115"/>
+      <c r="EX115"/>
+      <c r="EY115"/>
+      <c r="EZ115"/>
+      <c r="FA115"/>
+      <c r="FB115"/>
+      <c r="FC115"/>
+      <c r="FD115"/>
+      <c r="FE115"/>
+      <c r="FF115"/>
+      <c r="FG115"/>
+      <c r="FH115"/>
+      <c r="FI115"/>
+      <c r="FJ115"/>
+      <c r="FK115"/>
+      <c r="FL115"/>
+      <c r="FM115"/>
+      <c r="FN115"/>
+      <c r="FO115"/>
+      <c r="FP115"/>
+      <c r="FQ115"/>
+      <c r="FR115"/>
+      <c r="FS115"/>
+      <c r="FT115"/>
+      <c r="FU115"/>
+      <c r="FV115"/>
+      <c r="FW115"/>
+      <c r="FX115"/>
+      <c r="FY115"/>
+      <c r="FZ115"/>
+      <c r="GA115"/>
+      <c r="GB115"/>
+      <c r="GC115"/>
+      <c r="GD115"/>
+      <c r="GE115"/>
+      <c r="GF115"/>
+      <c r="GG115"/>
+      <c r="GH115"/>
+      <c r="GI115"/>
+      <c r="GJ115"/>
+      <c r="GK115"/>
+      <c r="GL115"/>
+      <c r="GM115"/>
+      <c r="GN115"/>
+      <c r="GO115"/>
+      <c r="GP115"/>
+      <c r="GQ115"/>
+      <c r="GR115"/>
+      <c r="GS115"/>
+      <c r="GT115"/>
+      <c r="GU115"/>
+      <c r="GV115"/>
+      <c r="GW115"/>
+      <c r="GX115"/>
+      <c r="GY115"/>
+      <c r="GZ115"/>
+      <c r="HA115"/>
+      <c r="HB115"/>
+      <c r="HC115"/>
+      <c r="HD115"/>
+      <c r="HE115"/>
+      <c r="HF115"/>
+      <c r="HG115"/>
+      <c r="HH115"/>
+      <c r="HI115"/>
+      <c r="HJ115"/>
+      <c r="HK115"/>
+      <c r="HL115"/>
+      <c r="HM115"/>
+      <c r="HN115"/>
+      <c r="HO115"/>
+      <c r="HP115"/>
+      <c r="HQ115"/>
+      <c r="HR115"/>
+      <c r="HS115"/>
+      <c r="HT115"/>
+      <c r="HU115"/>
+      <c r="HV115"/>
+      <c r="HW115"/>
+      <c r="HX115"/>
+      <c r="HY115"/>
+      <c r="HZ115"/>
+      <c r="IA115"/>
+      <c r="IB115"/>
+      <c r="IC115"/>
+      <c r="ID115"/>
+      <c r="IE115"/>
+      <c r="IF115"/>
+      <c r="IG115"/>
+      <c r="IH115"/>
+      <c r="II115"/>
+      <c r="IJ115"/>
+      <c r="IK115"/>
+      <c r="IL115"/>
+      <c r="IM115"/>
+      <c r="IN115"/>
+      <c r="IO115"/>
+      <c r="IP115"/>
+      <c r="IQ115"/>
+      <c r="IR115"/>
+      <c r="IS115"/>
+      <c r="IT115"/>
+      <c r="IU115"/>
+      <c r="IV115"/>
+      <c r="IW115"/>
+    </row>
+    <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A116" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="B116" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="D116" s="57"/>
+      <c r="E116" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="F116" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="81">
+        <v>0</v>
+      </c>
+      <c r="H116" s="57">
+        <v>1</v>
+      </c>
+      <c r="I116" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="J116" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K116"/>
+      <c r="L116"/>
+      <c r="M116"/>
+      <c r="N116"/>
+      <c r="O116"/>
+      <c r="P116"/>
+      <c r="Q116"/>
+      <c r="R116"/>
+      <c r="S116"/>
+      <c r="T116"/>
+      <c r="U116"/>
+      <c r="V116"/>
+      <c r="W116"/>
+      <c r="X116"/>
+      <c r="Y116"/>
+      <c r="Z116"/>
+      <c r="AA116"/>
+      <c r="AB116"/>
+      <c r="AC116"/>
+      <c r="AD116"/>
+      <c r="AE116"/>
+      <c r="AF116"/>
+      <c r="AG116"/>
+      <c r="AH116"/>
+      <c r="AI116"/>
+      <c r="AJ116"/>
+      <c r="AK116"/>
+      <c r="AL116"/>
+      <c r="AM116"/>
+      <c r="AN116"/>
+      <c r="AO116"/>
+      <c r="AP116"/>
+      <c r="AQ116"/>
+      <c r="AR116"/>
+      <c r="AS116"/>
+      <c r="AT116"/>
+      <c r="AU116"/>
+      <c r="AV116"/>
+      <c r="AW116"/>
+      <c r="AX116"/>
+      <c r="AY116"/>
+      <c r="AZ116"/>
+      <c r="BA116"/>
+      <c r="BB116"/>
+      <c r="BC116"/>
+      <c r="BD116"/>
+      <c r="BE116"/>
+      <c r="BF116"/>
+      <c r="BG116"/>
+      <c r="BH116"/>
+      <c r="BI116"/>
+      <c r="BJ116"/>
+      <c r="BK116"/>
+      <c r="BL116"/>
+      <c r="BM116"/>
+      <c r="BN116"/>
+      <c r="BO116"/>
+      <c r="BP116"/>
+      <c r="BQ116"/>
+      <c r="BR116"/>
+      <c r="BS116"/>
+      <c r="BT116"/>
+      <c r="BU116"/>
+      <c r="BV116"/>
+      <c r="BW116"/>
+      <c r="BX116"/>
+      <c r="BY116"/>
+      <c r="BZ116"/>
+      <c r="CA116"/>
+      <c r="CB116"/>
+      <c r="CC116"/>
+      <c r="CD116"/>
+      <c r="CE116"/>
+      <c r="CF116"/>
+      <c r="CG116"/>
+      <c r="CH116"/>
+      <c r="CI116"/>
+      <c r="CJ116"/>
+      <c r="CK116"/>
+      <c r="CL116"/>
+      <c r="CM116"/>
+      <c r="CN116"/>
+      <c r="CO116"/>
+      <c r="CP116"/>
+      <c r="CQ116"/>
+      <c r="CR116"/>
+      <c r="CS116"/>
+      <c r="CT116"/>
+      <c r="CU116"/>
+      <c r="CV116"/>
+      <c r="CW116"/>
+      <c r="CX116"/>
+      <c r="CY116"/>
+      <c r="CZ116"/>
+      <c r="DA116"/>
+      <c r="DB116"/>
+      <c r="DC116"/>
+      <c r="DD116"/>
+      <c r="DE116"/>
+      <c r="DF116"/>
+      <c r="DG116"/>
+      <c r="DH116"/>
+      <c r="DI116"/>
+      <c r="DJ116"/>
+      <c r="DK116"/>
+      <c r="DL116"/>
+      <c r="DM116"/>
+      <c r="DN116"/>
+      <c r="DO116"/>
+      <c r="DP116"/>
+      <c r="DQ116"/>
+      <c r="DR116"/>
+      <c r="DS116"/>
+      <c r="DT116"/>
+      <c r="DU116"/>
+      <c r="DV116"/>
+      <c r="DW116"/>
+      <c r="DX116"/>
+      <c r="DY116"/>
+      <c r="DZ116"/>
+      <c r="EA116"/>
+      <c r="EB116"/>
+      <c r="EC116"/>
+      <c r="ED116"/>
+      <c r="EE116"/>
+      <c r="EF116"/>
+      <c r="EG116"/>
+      <c r="EH116"/>
+      <c r="EI116"/>
+      <c r="EJ116"/>
+      <c r="EK116"/>
+      <c r="EL116"/>
+      <c r="EM116"/>
+      <c r="EN116"/>
+      <c r="EO116"/>
+      <c r="EP116"/>
+      <c r="EQ116"/>
+      <c r="ER116"/>
+      <c r="ES116"/>
+      <c r="ET116"/>
+      <c r="EU116"/>
+      <c r="EV116"/>
+      <c r="EW116"/>
+      <c r="EX116"/>
+      <c r="EY116"/>
+      <c r="EZ116"/>
+      <c r="FA116"/>
+      <c r="FB116"/>
+      <c r="FC116"/>
+      <c r="FD116"/>
+      <c r="FE116"/>
+      <c r="FF116"/>
+      <c r="FG116"/>
+      <c r="FH116"/>
+      <c r="FI116"/>
+      <c r="FJ116"/>
+      <c r="FK116"/>
+      <c r="FL116"/>
+      <c r="FM116"/>
+      <c r="FN116"/>
+      <c r="FO116"/>
+      <c r="FP116"/>
+      <c r="FQ116"/>
+      <c r="FR116"/>
+      <c r="FS116"/>
+      <c r="FT116"/>
+      <c r="FU116"/>
+      <c r="FV116"/>
+      <c r="FW116"/>
+      <c r="FX116"/>
+      <c r="FY116"/>
+      <c r="FZ116"/>
+      <c r="GA116"/>
+      <c r="GB116"/>
+      <c r="GC116"/>
+      <c r="GD116"/>
+      <c r="GE116"/>
+      <c r="GF116"/>
+      <c r="GG116"/>
+      <c r="GH116"/>
+      <c r="GI116"/>
+      <c r="GJ116"/>
+      <c r="GK116"/>
+      <c r="GL116"/>
+      <c r="GM116"/>
+      <c r="GN116"/>
+      <c r="GO116"/>
+      <c r="GP116"/>
+      <c r="GQ116"/>
+      <c r="GR116"/>
+      <c r="GS116"/>
+      <c r="GT116"/>
+      <c r="GU116"/>
+      <c r="GV116"/>
+      <c r="GW116"/>
+      <c r="GX116"/>
+      <c r="GY116"/>
+      <c r="GZ116"/>
+      <c r="HA116"/>
+      <c r="HB116"/>
+      <c r="HC116"/>
+      <c r="HD116"/>
+      <c r="HE116"/>
+      <c r="HF116"/>
+      <c r="HG116"/>
+      <c r="HH116"/>
+      <c r="HI116"/>
+      <c r="HJ116"/>
+      <c r="HK116"/>
+      <c r="HL116"/>
+      <c r="HM116"/>
+      <c r="HN116"/>
+      <c r="HO116"/>
+      <c r="HP116"/>
+      <c r="HQ116"/>
+      <c r="HR116"/>
+      <c r="HS116"/>
+      <c r="HT116"/>
+      <c r="HU116"/>
+      <c r="HV116"/>
+      <c r="HW116"/>
+      <c r="HX116"/>
+      <c r="HY116"/>
+      <c r="HZ116"/>
+      <c r="IA116"/>
+      <c r="IB116"/>
+      <c r="IC116"/>
+      <c r="ID116"/>
+      <c r="IE116"/>
+      <c r="IF116"/>
+      <c r="IG116"/>
+      <c r="IH116"/>
+      <c r="II116"/>
+      <c r="IJ116"/>
+      <c r="IK116"/>
+      <c r="IL116"/>
+      <c r="IM116"/>
+      <c r="IN116"/>
+      <c r="IO116"/>
+      <c r="IP116"/>
+      <c r="IQ116"/>
+      <c r="IR116"/>
+      <c r="IS116"/>
+      <c r="IT116"/>
+      <c r="IU116"/>
+      <c r="IV116"/>
+      <c r="IW116"/>
+    </row>
+    <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="125" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>

</xml_diff>

<commit_message>
added field tranlation form internal referral form
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E8A9FD-9AB0-453F-9801-D4ACBA0FEE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79F8A3C-5759-4465-ADB9-E3E3C101744A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31290" yWindow="1050" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31770" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="251">
   <si>
     <t>name</t>
   </si>
@@ -758,6 +758,27 @@
   </si>
   <si>
     <t>File Upload</t>
+  </si>
+  <si>
+    <t>REASON FOR REFERRAL AND RECOMMNEDATIONS</t>
+  </si>
+  <si>
+    <t>client_representing_problem_note</t>
+  </si>
+  <si>
+    <t>What issues/needs does the client say he or she needs help addressing:</t>
+  </si>
+  <si>
+    <t>referral_reason_note</t>
+  </si>
+  <si>
+    <t>The referral source’s reason for referral:</t>
+  </si>
+  <si>
+    <t>referral_decision_note</t>
+  </si>
+  <si>
+    <t>Action/intervention taken:</t>
   </si>
 </sst>
 </file>
@@ -1666,10 +1687,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW130"/>
+  <dimension ref="A1:IW133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -17318,13 +17339,13 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
@@ -17348,12 +17369,12 @@
     </row>
     <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B114" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="C114" s="95" t="s">
+        <v>230</v>
+      </c>
+      <c r="C114" s="58" t="s">
         <v>241</v>
       </c>
       <c r="D114" s="58"/>
@@ -17378,13 +17399,13 @@
     </row>
     <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B115" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C115" s="58" t="s">
-        <v>242</v>
+        <v>231</v>
+      </c>
+      <c r="C115" s="95" t="s">
+        <v>244</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
@@ -17408,13 +17429,13 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>152</v>
+        <v>231</v>
       </c>
       <c r="B116" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="C116" s="58" t="s">
-        <v>243</v>
+        <v>247</v>
+      </c>
+      <c r="C116" s="95" t="s">
+        <v>248</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
@@ -17436,9 +17457,96 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A117" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C117" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="D117" s="58"/>
+      <c r="E117" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F117" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G117" s="25">
+        <v>0</v>
+      </c>
+      <c r="H117" s="58">
+        <v>1</v>
+      </c>
+      <c r="I117" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J117" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A118" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B118" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="C118" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="D118" s="58"/>
+      <c r="E118" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F118" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G118" s="25">
+        <v>0</v>
+      </c>
+      <c r="H118" s="58">
+        <v>1</v>
+      </c>
+      <c r="I118" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J118" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A119" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B119" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C119" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="D119" s="58"/>
+      <c r="E119" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="F119" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G119" s="25">
+        <v>0</v>
+      </c>
+      <c r="H119" s="58">
+        <v>1</v>
+      </c>
+      <c r="I119" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J119" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1"/>
@@ -17450,6 +17558,9 @@
     <row r="128" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
     <row r="130" ht="17.100000000000001" customHeight="1"/>
+    <row r="131" ht="17.100000000000001" customHeight="1"/>
+    <row r="132" ht="17.100000000000001" customHeight="1"/>
+    <row r="133" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed case conference field setting
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77575D9-7CA5-4FD3-A185-F371A8335D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB72ACD-26EC-4578-AB7E-2656886DE83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31140" yWindow="1065" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31770" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="250">
   <si>
     <t>name</t>
   </si>
@@ -697,67 +697,85 @@
     <t>Others</t>
   </si>
   <si>
+    <t>user</t>
+  </si>
+  <si>
     <t>province</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>referral_date</t>
   </si>
   <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>referred_from</t>
+  </si>
+  <si>
+    <t>client_representing_problem</t>
+  </si>
+  <si>
+    <t>emergency_note</t>
+  </si>
+  <si>
+    <t>referral_reason</t>
+  </si>
+  <si>
+    <t>referral_decision</t>
+  </si>
+  <si>
+    <t>internal_referral</t>
+  </si>
+  <si>
     <t>Date of Internal Referral</t>
   </si>
   <si>
-    <t>internal_referral</t>
-  </si>
-  <si>
-    <t>client_id</t>
+    <t>client_name</t>
   </si>
   <si>
     <t>Client ID</t>
   </si>
   <si>
-    <t>client_name</t>
-  </si>
-  <si>
     <t>Client Name</t>
   </si>
   <si>
-    <t>referred_from</t>
-  </si>
-  <si>
     <t>Referral Form</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>Referred To</t>
   </si>
   <si>
-    <t>client_representing_problem</t>
-  </si>
-  <si>
     <t>CLIENT’S PRESENTING PROBLEMS</t>
   </si>
   <si>
-    <t>emergency_note</t>
-  </si>
-  <si>
     <t>NOTE: EMERGENCY/CRISIS NEEDS</t>
   </si>
   <si>
-    <t>referral_reason</t>
-  </si>
-  <si>
-    <t>referral_decision</t>
-  </si>
-  <si>
     <t>REFERRAL DECISION (to be approved by case management supervisor)</t>
   </si>
   <si>
-    <t>File Upload</t>
+    <t>REASON FOR REFERRAL AND RECOMMNEDATIONS</t>
+  </si>
+  <si>
+    <t>client_representing_problem_note</t>
+  </si>
+  <si>
+    <t>What issues/needs does the client say he or she needs help addressing:</t>
+  </si>
+  <si>
+    <t>referral_reason_note</t>
+  </si>
+  <si>
+    <t>The referral source’s reason for referral:</t>
+  </si>
+  <si>
+    <t>referral_decision_note</t>
+  </si>
+  <si>
+    <t>Action/intervention taken:</t>
+  </si>
+  <si>
+    <t>program_stream_ids</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1297,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1666,10 +1684,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW129"/>
+  <dimension ref="A1:IW133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -16506,7 +16524,9 @@
       <c r="A102" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="B102" s="58"/>
+      <c r="B102" s="58" t="s">
+        <v>11</v>
+      </c>
       <c r="C102" s="95" t="s">
         <v>217</v>
       </c>
@@ -16534,7 +16554,9 @@
       <c r="A103" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="B103" s="58"/>
+      <c r="B103" s="58" t="s">
+        <v>11</v>
+      </c>
       <c r="C103" s="95" t="s">
         <v>218</v>
       </c>
@@ -16562,7 +16584,9 @@
       <c r="A104" s="95" t="s">
         <v>221</v>
       </c>
-      <c r="B104" s="58"/>
+      <c r="B104" s="58" t="s">
+        <v>11</v>
+      </c>
       <c r="C104" s="95" t="s">
         <v>222</v>
       </c>
@@ -16586,31 +16610,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:257" ht="15.75" customHeight="1">
-      <c r="A105" s="78" t="s">
+    <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A105" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B105" s="19" t="s">
         <v>223</v>
-      </c>
-      <c r="B105" s="78" t="s">
-        <v>224</v>
       </c>
       <c r="C105" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="D105" s="57"/>
-      <c r="E105" s="80" t="s">
-        <v>224</v>
-      </c>
-      <c r="F105" s="80" t="s">
+      <c r="D105" s="58"/>
+      <c r="E105" s="76" t="s">
+        <v>223</v>
+      </c>
+      <c r="F105" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="G105" s="81">
-        <v>0</v>
-      </c>
-      <c r="H105" s="81">
+      <c r="G105" s="25">
+        <v>0</v>
+      </c>
+      <c r="H105" s="25">
         <v>1</v>
       </c>
-      <c r="I105" s="96"/>
-      <c r="J105" s="81" t="s">
+      <c r="I105" s="10"/>
+      <c r="J105" s="25" t="s">
         <v>15</v>
       </c>
       <c r="K105"/>
@@ -16862,30 +16886,30 @@
       <c r="IW105"/>
     </row>
     <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A106" s="78" t="s">
-        <v>223</v>
-      </c>
-      <c r="B106" s="78" t="s">
+      <c r="A106" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>120</v>
       </c>
       <c r="C106" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="D106" s="57"/>
-      <c r="E106" s="80" t="s">
+      <c r="D106" s="58"/>
+      <c r="E106" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="F106" s="80" t="s">
+      <c r="F106" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="G106" s="81">
-        <v>0</v>
-      </c>
-      <c r="H106" s="81">
+      <c r="G106" s="25">
+        <v>0</v>
+      </c>
+      <c r="H106" s="25">
         <v>1</v>
       </c>
-      <c r="I106" s="96"/>
-      <c r="J106" s="81" t="s">
+      <c r="I106" s="10"/>
+      <c r="J106" s="25" t="s">
         <v>15</v>
       </c>
       <c r="K106"/>
@@ -17137,2788 +17161,409 @@
       <c r="IW106"/>
     </row>
     <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A107" s="57" t="s">
+      <c r="A107" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B107" s="57" t="s">
-        <v>225</v>
-      </c>
-      <c r="C107" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="D107" s="57"/>
-      <c r="E107" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F107" s="97" t="s">
+      <c r="B107" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C107" s="58" t="s">
+        <v>233</v>
+      </c>
+      <c r="D107" s="58"/>
+      <c r="E107" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F107" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G107" s="81">
-        <v>0</v>
-      </c>
-      <c r="H107" s="57">
+      <c r="G107" s="25">
+        <v>0</v>
+      </c>
+      <c r="H107" s="97">
         <v>1</v>
       </c>
-      <c r="I107" s="97" t="s">
+      <c r="I107" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J107" s="97" t="s">
+      <c r="J107" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K107"/>
-      <c r="L107"/>
-      <c r="M107"/>
-      <c r="N107"/>
-      <c r="O107"/>
-      <c r="P107"/>
-      <c r="Q107"/>
-      <c r="R107"/>
-      <c r="S107"/>
-      <c r="T107"/>
-      <c r="U107"/>
-      <c r="V107"/>
-      <c r="W107"/>
-      <c r="X107"/>
-      <c r="Y107"/>
-      <c r="Z107"/>
-      <c r="AA107"/>
-      <c r="AB107"/>
-      <c r="AC107"/>
-      <c r="AD107"/>
-      <c r="AE107"/>
-      <c r="AF107"/>
-      <c r="AG107"/>
-      <c r="AH107"/>
-      <c r="AI107"/>
-      <c r="AJ107"/>
-      <c r="AK107"/>
-      <c r="AL107"/>
-      <c r="AM107"/>
-      <c r="AN107"/>
-      <c r="AO107"/>
-      <c r="AP107"/>
-      <c r="AQ107"/>
-      <c r="AR107"/>
-      <c r="AS107"/>
-      <c r="AT107"/>
-      <c r="AU107"/>
-      <c r="AV107"/>
-      <c r="AW107"/>
-      <c r="AX107"/>
-      <c r="AY107"/>
-      <c r="AZ107"/>
-      <c r="BA107"/>
-      <c r="BB107"/>
-      <c r="BC107"/>
-      <c r="BD107"/>
-      <c r="BE107"/>
-      <c r="BF107"/>
-      <c r="BG107"/>
-      <c r="BH107"/>
-      <c r="BI107"/>
-      <c r="BJ107"/>
-      <c r="BK107"/>
-      <c r="BL107"/>
-      <c r="BM107"/>
-      <c r="BN107"/>
-      <c r="BO107"/>
-      <c r="BP107"/>
-      <c r="BQ107"/>
-      <c r="BR107"/>
-      <c r="BS107"/>
-      <c r="BT107"/>
-      <c r="BU107"/>
-      <c r="BV107"/>
-      <c r="BW107"/>
-      <c r="BX107"/>
-      <c r="BY107"/>
-      <c r="BZ107"/>
-      <c r="CA107"/>
-      <c r="CB107"/>
-      <c r="CC107"/>
-      <c r="CD107"/>
-      <c r="CE107"/>
-      <c r="CF107"/>
-      <c r="CG107"/>
-      <c r="CH107"/>
-      <c r="CI107"/>
-      <c r="CJ107"/>
-      <c r="CK107"/>
-      <c r="CL107"/>
-      <c r="CM107"/>
-      <c r="CN107"/>
-      <c r="CO107"/>
-      <c r="CP107"/>
-      <c r="CQ107"/>
-      <c r="CR107"/>
-      <c r="CS107"/>
-      <c r="CT107"/>
-      <c r="CU107"/>
-      <c r="CV107"/>
-      <c r="CW107"/>
-      <c r="CX107"/>
-      <c r="CY107"/>
-      <c r="CZ107"/>
-      <c r="DA107"/>
-      <c r="DB107"/>
-      <c r="DC107"/>
-      <c r="DD107"/>
-      <c r="DE107"/>
-      <c r="DF107"/>
-      <c r="DG107"/>
-      <c r="DH107"/>
-      <c r="DI107"/>
-      <c r="DJ107"/>
-      <c r="DK107"/>
-      <c r="DL107"/>
-      <c r="DM107"/>
-      <c r="DN107"/>
-      <c r="DO107"/>
-      <c r="DP107"/>
-      <c r="DQ107"/>
-      <c r="DR107"/>
-      <c r="DS107"/>
-      <c r="DT107"/>
-      <c r="DU107"/>
-      <c r="DV107"/>
-      <c r="DW107"/>
-      <c r="DX107"/>
-      <c r="DY107"/>
-      <c r="DZ107"/>
-      <c r="EA107"/>
-      <c r="EB107"/>
-      <c r="EC107"/>
-      <c r="ED107"/>
-      <c r="EE107"/>
-      <c r="EF107"/>
-      <c r="EG107"/>
-      <c r="EH107"/>
-      <c r="EI107"/>
-      <c r="EJ107"/>
-      <c r="EK107"/>
-      <c r="EL107"/>
-      <c r="EM107"/>
-      <c r="EN107"/>
-      <c r="EO107"/>
-      <c r="EP107"/>
-      <c r="EQ107"/>
-      <c r="ER107"/>
-      <c r="ES107"/>
-      <c r="ET107"/>
-      <c r="EU107"/>
-      <c r="EV107"/>
-      <c r="EW107"/>
-      <c r="EX107"/>
-      <c r="EY107"/>
-      <c r="EZ107"/>
-      <c r="FA107"/>
-      <c r="FB107"/>
-      <c r="FC107"/>
-      <c r="FD107"/>
-      <c r="FE107"/>
-      <c r="FF107"/>
-      <c r="FG107"/>
-      <c r="FH107"/>
-      <c r="FI107"/>
-      <c r="FJ107"/>
-      <c r="FK107"/>
-      <c r="FL107"/>
-      <c r="FM107"/>
-      <c r="FN107"/>
-      <c r="FO107"/>
-      <c r="FP107"/>
-      <c r="FQ107"/>
-      <c r="FR107"/>
-      <c r="FS107"/>
-      <c r="FT107"/>
-      <c r="FU107"/>
-      <c r="FV107"/>
-      <c r="FW107"/>
-      <c r="FX107"/>
-      <c r="FY107"/>
-      <c r="FZ107"/>
-      <c r="GA107"/>
-      <c r="GB107"/>
-      <c r="GC107"/>
-      <c r="GD107"/>
-      <c r="GE107"/>
-      <c r="GF107"/>
-      <c r="GG107"/>
-      <c r="GH107"/>
-      <c r="GI107"/>
-      <c r="GJ107"/>
-      <c r="GK107"/>
-      <c r="GL107"/>
-      <c r="GM107"/>
-      <c r="GN107"/>
-      <c r="GO107"/>
-      <c r="GP107"/>
-      <c r="GQ107"/>
-      <c r="GR107"/>
-      <c r="GS107"/>
-      <c r="GT107"/>
-      <c r="GU107"/>
-      <c r="GV107"/>
-      <c r="GW107"/>
-      <c r="GX107"/>
-      <c r="GY107"/>
-      <c r="GZ107"/>
-      <c r="HA107"/>
-      <c r="HB107"/>
-      <c r="HC107"/>
-      <c r="HD107"/>
-      <c r="HE107"/>
-      <c r="HF107"/>
-      <c r="HG107"/>
-      <c r="HH107"/>
-      <c r="HI107"/>
-      <c r="HJ107"/>
-      <c r="HK107"/>
-      <c r="HL107"/>
-      <c r="HM107"/>
-      <c r="HN107"/>
-      <c r="HO107"/>
-      <c r="HP107"/>
-      <c r="HQ107"/>
-      <c r="HR107"/>
-      <c r="HS107"/>
-      <c r="HT107"/>
-      <c r="HU107"/>
-      <c r="HV107"/>
-      <c r="HW107"/>
-      <c r="HX107"/>
-      <c r="HY107"/>
-      <c r="HZ107"/>
-      <c r="IA107"/>
-      <c r="IB107"/>
-      <c r="IC107"/>
-      <c r="ID107"/>
-      <c r="IE107"/>
-      <c r="IF107"/>
-      <c r="IG107"/>
-      <c r="IH107"/>
-      <c r="II107"/>
-      <c r="IJ107"/>
-      <c r="IK107"/>
-      <c r="IL107"/>
-      <c r="IM107"/>
-      <c r="IN107"/>
-      <c r="IO107"/>
-      <c r="IP107"/>
-      <c r="IQ107"/>
-      <c r="IR107"/>
-      <c r="IS107"/>
-      <c r="IT107"/>
-      <c r="IU107"/>
-      <c r="IV107"/>
-      <c r="IW107"/>
     </row>
     <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A108" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="B108" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="C108" s="57" t="s">
-        <v>229</v>
-      </c>
-      <c r="D108" s="57"/>
-      <c r="E108" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F108" s="97" t="s">
+      <c r="A108" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C108" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="D108" s="58"/>
+      <c r="E108" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F108" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G108" s="81">
-        <v>0</v>
-      </c>
-      <c r="H108" s="57">
+      <c r="G108" s="25">
+        <v>0</v>
+      </c>
+      <c r="H108" s="58">
         <v>1</v>
       </c>
-      <c r="I108" s="97" t="s">
+      <c r="I108" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J108" s="97" t="s">
+      <c r="J108" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K108"/>
-      <c r="L108"/>
-      <c r="M108"/>
-      <c r="N108"/>
-      <c r="O108"/>
-      <c r="P108"/>
-      <c r="Q108"/>
-      <c r="R108"/>
-      <c r="S108"/>
-      <c r="T108"/>
-      <c r="U108"/>
-      <c r="V108"/>
-      <c r="W108"/>
-      <c r="X108"/>
-      <c r="Y108"/>
-      <c r="Z108"/>
-      <c r="AA108"/>
-      <c r="AB108"/>
-      <c r="AC108"/>
-      <c r="AD108"/>
-      <c r="AE108"/>
-      <c r="AF108"/>
-      <c r="AG108"/>
-      <c r="AH108"/>
-      <c r="AI108"/>
-      <c r="AJ108"/>
-      <c r="AK108"/>
-      <c r="AL108"/>
-      <c r="AM108"/>
-      <c r="AN108"/>
-      <c r="AO108"/>
-      <c r="AP108"/>
-      <c r="AQ108"/>
-      <c r="AR108"/>
-      <c r="AS108"/>
-      <c r="AT108"/>
-      <c r="AU108"/>
-      <c r="AV108"/>
-      <c r="AW108"/>
-      <c r="AX108"/>
-      <c r="AY108"/>
-      <c r="AZ108"/>
-      <c r="BA108"/>
-      <c r="BB108"/>
-      <c r="BC108"/>
-      <c r="BD108"/>
-      <c r="BE108"/>
-      <c r="BF108"/>
-      <c r="BG108"/>
-      <c r="BH108"/>
-      <c r="BI108"/>
-      <c r="BJ108"/>
-      <c r="BK108"/>
-      <c r="BL108"/>
-      <c r="BM108"/>
-      <c r="BN108"/>
-      <c r="BO108"/>
-      <c r="BP108"/>
-      <c r="BQ108"/>
-      <c r="BR108"/>
-      <c r="BS108"/>
-      <c r="BT108"/>
-      <c r="BU108"/>
-      <c r="BV108"/>
-      <c r="BW108"/>
-      <c r="BX108"/>
-      <c r="BY108"/>
-      <c r="BZ108"/>
-      <c r="CA108"/>
-      <c r="CB108"/>
-      <c r="CC108"/>
-      <c r="CD108"/>
-      <c r="CE108"/>
-      <c r="CF108"/>
-      <c r="CG108"/>
-      <c r="CH108"/>
-      <c r="CI108"/>
-      <c r="CJ108"/>
-      <c r="CK108"/>
-      <c r="CL108"/>
-      <c r="CM108"/>
-      <c r="CN108"/>
-      <c r="CO108"/>
-      <c r="CP108"/>
-      <c r="CQ108"/>
-      <c r="CR108"/>
-      <c r="CS108"/>
-      <c r="CT108"/>
-      <c r="CU108"/>
-      <c r="CV108"/>
-      <c r="CW108"/>
-      <c r="CX108"/>
-      <c r="CY108"/>
-      <c r="CZ108"/>
-      <c r="DA108"/>
-      <c r="DB108"/>
-      <c r="DC108"/>
-      <c r="DD108"/>
-      <c r="DE108"/>
-      <c r="DF108"/>
-      <c r="DG108"/>
-      <c r="DH108"/>
-      <c r="DI108"/>
-      <c r="DJ108"/>
-      <c r="DK108"/>
-      <c r="DL108"/>
-      <c r="DM108"/>
-      <c r="DN108"/>
-      <c r="DO108"/>
-      <c r="DP108"/>
-      <c r="DQ108"/>
-      <c r="DR108"/>
-      <c r="DS108"/>
-      <c r="DT108"/>
-      <c r="DU108"/>
-      <c r="DV108"/>
-      <c r="DW108"/>
-      <c r="DX108"/>
-      <c r="DY108"/>
-      <c r="DZ108"/>
-      <c r="EA108"/>
-      <c r="EB108"/>
-      <c r="EC108"/>
-      <c r="ED108"/>
-      <c r="EE108"/>
-      <c r="EF108"/>
-      <c r="EG108"/>
-      <c r="EH108"/>
-      <c r="EI108"/>
-      <c r="EJ108"/>
-      <c r="EK108"/>
-      <c r="EL108"/>
-      <c r="EM108"/>
-      <c r="EN108"/>
-      <c r="EO108"/>
-      <c r="EP108"/>
-      <c r="EQ108"/>
-      <c r="ER108"/>
-      <c r="ES108"/>
-      <c r="ET108"/>
-      <c r="EU108"/>
-      <c r="EV108"/>
-      <c r="EW108"/>
-      <c r="EX108"/>
-      <c r="EY108"/>
-      <c r="EZ108"/>
-      <c r="FA108"/>
-      <c r="FB108"/>
-      <c r="FC108"/>
-      <c r="FD108"/>
-      <c r="FE108"/>
-      <c r="FF108"/>
-      <c r="FG108"/>
-      <c r="FH108"/>
-      <c r="FI108"/>
-      <c r="FJ108"/>
-      <c r="FK108"/>
-      <c r="FL108"/>
-      <c r="FM108"/>
-      <c r="FN108"/>
-      <c r="FO108"/>
-      <c r="FP108"/>
-      <c r="FQ108"/>
-      <c r="FR108"/>
-      <c r="FS108"/>
-      <c r="FT108"/>
-      <c r="FU108"/>
-      <c r="FV108"/>
-      <c r="FW108"/>
-      <c r="FX108"/>
-      <c r="FY108"/>
-      <c r="FZ108"/>
-      <c r="GA108"/>
-      <c r="GB108"/>
-      <c r="GC108"/>
-      <c r="GD108"/>
-      <c r="GE108"/>
-      <c r="GF108"/>
-      <c r="GG108"/>
-      <c r="GH108"/>
-      <c r="GI108"/>
-      <c r="GJ108"/>
-      <c r="GK108"/>
-      <c r="GL108"/>
-      <c r="GM108"/>
-      <c r="GN108"/>
-      <c r="GO108"/>
-      <c r="GP108"/>
-      <c r="GQ108"/>
-      <c r="GR108"/>
-      <c r="GS108"/>
-      <c r="GT108"/>
-      <c r="GU108"/>
-      <c r="GV108"/>
-      <c r="GW108"/>
-      <c r="GX108"/>
-      <c r="GY108"/>
-      <c r="GZ108"/>
-      <c r="HA108"/>
-      <c r="HB108"/>
-      <c r="HC108"/>
-      <c r="HD108"/>
-      <c r="HE108"/>
-      <c r="HF108"/>
-      <c r="HG108"/>
-      <c r="HH108"/>
-      <c r="HI108"/>
-      <c r="HJ108"/>
-      <c r="HK108"/>
-      <c r="HL108"/>
-      <c r="HM108"/>
-      <c r="HN108"/>
-      <c r="HO108"/>
-      <c r="HP108"/>
-      <c r="HQ108"/>
-      <c r="HR108"/>
-      <c r="HS108"/>
-      <c r="HT108"/>
-      <c r="HU108"/>
-      <c r="HV108"/>
-      <c r="HW108"/>
-      <c r="HX108"/>
-      <c r="HY108"/>
-      <c r="HZ108"/>
-      <c r="IA108"/>
-      <c r="IB108"/>
-      <c r="IC108"/>
-      <c r="ID108"/>
-      <c r="IE108"/>
-      <c r="IF108"/>
-      <c r="IG108"/>
-      <c r="IH108"/>
-      <c r="II108"/>
-      <c r="IJ108"/>
-      <c r="IK108"/>
-      <c r="IL108"/>
-      <c r="IM108"/>
-      <c r="IN108"/>
-      <c r="IO108"/>
-      <c r="IP108"/>
-      <c r="IQ108"/>
-      <c r="IR108"/>
-      <c r="IS108"/>
-      <c r="IT108"/>
-      <c r="IU108"/>
-      <c r="IV108"/>
-      <c r="IW108"/>
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A109" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="B109" s="57" t="s">
-        <v>230</v>
-      </c>
-      <c r="C109" s="57" t="s">
-        <v>231</v>
-      </c>
-      <c r="D109" s="57"/>
-      <c r="E109" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F109" s="97" t="s">
+      <c r="A109" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B109" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C109" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="D109" s="58"/>
+      <c r="E109" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F109" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G109" s="81">
-        <v>0</v>
-      </c>
-      <c r="H109" s="57">
+      <c r="G109" s="25">
+        <v>0</v>
+      </c>
+      <c r="H109" s="58">
         <v>1</v>
       </c>
-      <c r="I109" s="97" t="s">
+      <c r="I109" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J109" s="97" t="s">
+      <c r="J109" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-      <c r="N109"/>
-      <c r="O109"/>
-      <c r="P109"/>
-      <c r="Q109"/>
-      <c r="R109"/>
-      <c r="S109"/>
-      <c r="T109"/>
-      <c r="U109"/>
-      <c r="V109"/>
-      <c r="W109"/>
-      <c r="X109"/>
-      <c r="Y109"/>
-      <c r="Z109"/>
-      <c r="AA109"/>
-      <c r="AB109"/>
-      <c r="AC109"/>
-      <c r="AD109"/>
-      <c r="AE109"/>
-      <c r="AF109"/>
-      <c r="AG109"/>
-      <c r="AH109"/>
-      <c r="AI109"/>
-      <c r="AJ109"/>
-      <c r="AK109"/>
-      <c r="AL109"/>
-      <c r="AM109"/>
-      <c r="AN109"/>
-      <c r="AO109"/>
-      <c r="AP109"/>
-      <c r="AQ109"/>
-      <c r="AR109"/>
-      <c r="AS109"/>
-      <c r="AT109"/>
-      <c r="AU109"/>
-      <c r="AV109"/>
-      <c r="AW109"/>
-      <c r="AX109"/>
-      <c r="AY109"/>
-      <c r="AZ109"/>
-      <c r="BA109"/>
-      <c r="BB109"/>
-      <c r="BC109"/>
-      <c r="BD109"/>
-      <c r="BE109"/>
-      <c r="BF109"/>
-      <c r="BG109"/>
-      <c r="BH109"/>
-      <c r="BI109"/>
-      <c r="BJ109"/>
-      <c r="BK109"/>
-      <c r="BL109"/>
-      <c r="BM109"/>
-      <c r="BN109"/>
-      <c r="BO109"/>
-      <c r="BP109"/>
-      <c r="BQ109"/>
-      <c r="BR109"/>
-      <c r="BS109"/>
-      <c r="BT109"/>
-      <c r="BU109"/>
-      <c r="BV109"/>
-      <c r="BW109"/>
-      <c r="BX109"/>
-      <c r="BY109"/>
-      <c r="BZ109"/>
-      <c r="CA109"/>
-      <c r="CB109"/>
-      <c r="CC109"/>
-      <c r="CD109"/>
-      <c r="CE109"/>
-      <c r="CF109"/>
-      <c r="CG109"/>
-      <c r="CH109"/>
-      <c r="CI109"/>
-      <c r="CJ109"/>
-      <c r="CK109"/>
-      <c r="CL109"/>
-      <c r="CM109"/>
-      <c r="CN109"/>
-      <c r="CO109"/>
-      <c r="CP109"/>
-      <c r="CQ109"/>
-      <c r="CR109"/>
-      <c r="CS109"/>
-      <c r="CT109"/>
-      <c r="CU109"/>
-      <c r="CV109"/>
-      <c r="CW109"/>
-      <c r="CX109"/>
-      <c r="CY109"/>
-      <c r="CZ109"/>
-      <c r="DA109"/>
-      <c r="DB109"/>
-      <c r="DC109"/>
-      <c r="DD109"/>
-      <c r="DE109"/>
-      <c r="DF109"/>
-      <c r="DG109"/>
-      <c r="DH109"/>
-      <c r="DI109"/>
-      <c r="DJ109"/>
-      <c r="DK109"/>
-      <c r="DL109"/>
-      <c r="DM109"/>
-      <c r="DN109"/>
-      <c r="DO109"/>
-      <c r="DP109"/>
-      <c r="DQ109"/>
-      <c r="DR109"/>
-      <c r="DS109"/>
-      <c r="DT109"/>
-      <c r="DU109"/>
-      <c r="DV109"/>
-      <c r="DW109"/>
-      <c r="DX109"/>
-      <c r="DY109"/>
-      <c r="DZ109"/>
-      <c r="EA109"/>
-      <c r="EB109"/>
-      <c r="EC109"/>
-      <c r="ED109"/>
-      <c r="EE109"/>
-      <c r="EF109"/>
-      <c r="EG109"/>
-      <c r="EH109"/>
-      <c r="EI109"/>
-      <c r="EJ109"/>
-      <c r="EK109"/>
-      <c r="EL109"/>
-      <c r="EM109"/>
-      <c r="EN109"/>
-      <c r="EO109"/>
-      <c r="EP109"/>
-      <c r="EQ109"/>
-      <c r="ER109"/>
-      <c r="ES109"/>
-      <c r="ET109"/>
-      <c r="EU109"/>
-      <c r="EV109"/>
-      <c r="EW109"/>
-      <c r="EX109"/>
-      <c r="EY109"/>
-      <c r="EZ109"/>
-      <c r="FA109"/>
-      <c r="FB109"/>
-      <c r="FC109"/>
-      <c r="FD109"/>
-      <c r="FE109"/>
-      <c r="FF109"/>
-      <c r="FG109"/>
-      <c r="FH109"/>
-      <c r="FI109"/>
-      <c r="FJ109"/>
-      <c r="FK109"/>
-      <c r="FL109"/>
-      <c r="FM109"/>
-      <c r="FN109"/>
-      <c r="FO109"/>
-      <c r="FP109"/>
-      <c r="FQ109"/>
-      <c r="FR109"/>
-      <c r="FS109"/>
-      <c r="FT109"/>
-      <c r="FU109"/>
-      <c r="FV109"/>
-      <c r="FW109"/>
-      <c r="FX109"/>
-      <c r="FY109"/>
-      <c r="FZ109"/>
-      <c r="GA109"/>
-      <c r="GB109"/>
-      <c r="GC109"/>
-      <c r="GD109"/>
-      <c r="GE109"/>
-      <c r="GF109"/>
-      <c r="GG109"/>
-      <c r="GH109"/>
-      <c r="GI109"/>
-      <c r="GJ109"/>
-      <c r="GK109"/>
-      <c r="GL109"/>
-      <c r="GM109"/>
-      <c r="GN109"/>
-      <c r="GO109"/>
-      <c r="GP109"/>
-      <c r="GQ109"/>
-      <c r="GR109"/>
-      <c r="GS109"/>
-      <c r="GT109"/>
-      <c r="GU109"/>
-      <c r="GV109"/>
-      <c r="GW109"/>
-      <c r="GX109"/>
-      <c r="GY109"/>
-      <c r="GZ109"/>
-      <c r="HA109"/>
-      <c r="HB109"/>
-      <c r="HC109"/>
-      <c r="HD109"/>
-      <c r="HE109"/>
-      <c r="HF109"/>
-      <c r="HG109"/>
-      <c r="HH109"/>
-      <c r="HI109"/>
-      <c r="HJ109"/>
-      <c r="HK109"/>
-      <c r="HL109"/>
-      <c r="HM109"/>
-      <c r="HN109"/>
-      <c r="HO109"/>
-      <c r="HP109"/>
-      <c r="HQ109"/>
-      <c r="HR109"/>
-      <c r="HS109"/>
-      <c r="HT109"/>
-      <c r="HU109"/>
-      <c r="HV109"/>
-      <c r="HW109"/>
-      <c r="HX109"/>
-      <c r="HY109"/>
-      <c r="HZ109"/>
-      <c r="IA109"/>
-      <c r="IB109"/>
-      <c r="IC109"/>
-      <c r="ID109"/>
-      <c r="IE109"/>
-      <c r="IF109"/>
-      <c r="IG109"/>
-      <c r="IH109"/>
-      <c r="II109"/>
-      <c r="IJ109"/>
-      <c r="IK109"/>
-      <c r="IL109"/>
-      <c r="IM109"/>
-      <c r="IN109"/>
-      <c r="IO109"/>
-      <c r="IP109"/>
-      <c r="IQ109"/>
-      <c r="IR109"/>
-      <c r="IS109"/>
-      <c r="IT109"/>
-      <c r="IU109"/>
-      <c r="IV109"/>
-      <c r="IW109"/>
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A110" s="57" t="s">
+      <c r="A110" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B110" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="B110" s="57" t="s">
+      <c r="C110" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="D110" s="58"/>
+      <c r="E110" s="96" t="s">
         <v>232</v>
       </c>
-      <c r="C110" s="57" t="s">
-        <v>233</v>
-      </c>
-      <c r="D110" s="57"/>
-      <c r="E110" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F110" s="97" t="s">
+      <c r="F110" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G110" s="81">
-        <v>0</v>
-      </c>
-      <c r="H110" s="57">
+      <c r="G110" s="25">
+        <v>0</v>
+      </c>
+      <c r="H110" s="58">
         <v>1</v>
       </c>
-      <c r="I110" s="97" t="s">
+      <c r="I110" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J110" s="97" t="s">
+      <c r="J110" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K110"/>
-      <c r="L110"/>
-      <c r="M110"/>
-      <c r="N110"/>
-      <c r="O110"/>
-      <c r="P110"/>
-      <c r="Q110"/>
-      <c r="R110"/>
-      <c r="S110"/>
-      <c r="T110"/>
-      <c r="U110"/>
-      <c r="V110"/>
-      <c r="W110"/>
-      <c r="X110"/>
-      <c r="Y110"/>
-      <c r="Z110"/>
-      <c r="AA110"/>
-      <c r="AB110"/>
-      <c r="AC110"/>
-      <c r="AD110"/>
-      <c r="AE110"/>
-      <c r="AF110"/>
-      <c r="AG110"/>
-      <c r="AH110"/>
-      <c r="AI110"/>
-      <c r="AJ110"/>
-      <c r="AK110"/>
-      <c r="AL110"/>
-      <c r="AM110"/>
-      <c r="AN110"/>
-      <c r="AO110"/>
-      <c r="AP110"/>
-      <c r="AQ110"/>
-      <c r="AR110"/>
-      <c r="AS110"/>
-      <c r="AT110"/>
-      <c r="AU110"/>
-      <c r="AV110"/>
-      <c r="AW110"/>
-      <c r="AX110"/>
-      <c r="AY110"/>
-      <c r="AZ110"/>
-      <c r="BA110"/>
-      <c r="BB110"/>
-      <c r="BC110"/>
-      <c r="BD110"/>
-      <c r="BE110"/>
-      <c r="BF110"/>
-      <c r="BG110"/>
-      <c r="BH110"/>
-      <c r="BI110"/>
-      <c r="BJ110"/>
-      <c r="BK110"/>
-      <c r="BL110"/>
-      <c r="BM110"/>
-      <c r="BN110"/>
-      <c r="BO110"/>
-      <c r="BP110"/>
-      <c r="BQ110"/>
-      <c r="BR110"/>
-      <c r="BS110"/>
-      <c r="BT110"/>
-      <c r="BU110"/>
-      <c r="BV110"/>
-      <c r="BW110"/>
-      <c r="BX110"/>
-      <c r="BY110"/>
-      <c r="BZ110"/>
-      <c r="CA110"/>
-      <c r="CB110"/>
-      <c r="CC110"/>
-      <c r="CD110"/>
-      <c r="CE110"/>
-      <c r="CF110"/>
-      <c r="CG110"/>
-      <c r="CH110"/>
-      <c r="CI110"/>
-      <c r="CJ110"/>
-      <c r="CK110"/>
-      <c r="CL110"/>
-      <c r="CM110"/>
-      <c r="CN110"/>
-      <c r="CO110"/>
-      <c r="CP110"/>
-      <c r="CQ110"/>
-      <c r="CR110"/>
-      <c r="CS110"/>
-      <c r="CT110"/>
-      <c r="CU110"/>
-      <c r="CV110"/>
-      <c r="CW110"/>
-      <c r="CX110"/>
-      <c r="CY110"/>
-      <c r="CZ110"/>
-      <c r="DA110"/>
-      <c r="DB110"/>
-      <c r="DC110"/>
-      <c r="DD110"/>
-      <c r="DE110"/>
-      <c r="DF110"/>
-      <c r="DG110"/>
-      <c r="DH110"/>
-      <c r="DI110"/>
-      <c r="DJ110"/>
-      <c r="DK110"/>
-      <c r="DL110"/>
-      <c r="DM110"/>
-      <c r="DN110"/>
-      <c r="DO110"/>
-      <c r="DP110"/>
-      <c r="DQ110"/>
-      <c r="DR110"/>
-      <c r="DS110"/>
-      <c r="DT110"/>
-      <c r="DU110"/>
-      <c r="DV110"/>
-      <c r="DW110"/>
-      <c r="DX110"/>
-      <c r="DY110"/>
-      <c r="DZ110"/>
-      <c r="EA110"/>
-      <c r="EB110"/>
-      <c r="EC110"/>
-      <c r="ED110"/>
-      <c r="EE110"/>
-      <c r="EF110"/>
-      <c r="EG110"/>
-      <c r="EH110"/>
-      <c r="EI110"/>
-      <c r="EJ110"/>
-      <c r="EK110"/>
-      <c r="EL110"/>
-      <c r="EM110"/>
-      <c r="EN110"/>
-      <c r="EO110"/>
-      <c r="EP110"/>
-      <c r="EQ110"/>
-      <c r="ER110"/>
-      <c r="ES110"/>
-      <c r="ET110"/>
-      <c r="EU110"/>
-      <c r="EV110"/>
-      <c r="EW110"/>
-      <c r="EX110"/>
-      <c r="EY110"/>
-      <c r="EZ110"/>
-      <c r="FA110"/>
-      <c r="FB110"/>
-      <c r="FC110"/>
-      <c r="FD110"/>
-      <c r="FE110"/>
-      <c r="FF110"/>
-      <c r="FG110"/>
-      <c r="FH110"/>
-      <c r="FI110"/>
-      <c r="FJ110"/>
-      <c r="FK110"/>
-      <c r="FL110"/>
-      <c r="FM110"/>
-      <c r="FN110"/>
-      <c r="FO110"/>
-      <c r="FP110"/>
-      <c r="FQ110"/>
-      <c r="FR110"/>
-      <c r="FS110"/>
-      <c r="FT110"/>
-      <c r="FU110"/>
-      <c r="FV110"/>
-      <c r="FW110"/>
-      <c r="FX110"/>
-      <c r="FY110"/>
-      <c r="FZ110"/>
-      <c r="GA110"/>
-      <c r="GB110"/>
-      <c r="GC110"/>
-      <c r="GD110"/>
-      <c r="GE110"/>
-      <c r="GF110"/>
-      <c r="GG110"/>
-      <c r="GH110"/>
-      <c r="GI110"/>
-      <c r="GJ110"/>
-      <c r="GK110"/>
-      <c r="GL110"/>
-      <c r="GM110"/>
-      <c r="GN110"/>
-      <c r="GO110"/>
-      <c r="GP110"/>
-      <c r="GQ110"/>
-      <c r="GR110"/>
-      <c r="GS110"/>
-      <c r="GT110"/>
-      <c r="GU110"/>
-      <c r="GV110"/>
-      <c r="GW110"/>
-      <c r="GX110"/>
-      <c r="GY110"/>
-      <c r="GZ110"/>
-      <c r="HA110"/>
-      <c r="HB110"/>
-      <c r="HC110"/>
-      <c r="HD110"/>
-      <c r="HE110"/>
-      <c r="HF110"/>
-      <c r="HG110"/>
-      <c r="HH110"/>
-      <c r="HI110"/>
-      <c r="HJ110"/>
-      <c r="HK110"/>
-      <c r="HL110"/>
-      <c r="HM110"/>
-      <c r="HN110"/>
-      <c r="HO110"/>
-      <c r="HP110"/>
-      <c r="HQ110"/>
-      <c r="HR110"/>
-      <c r="HS110"/>
-      <c r="HT110"/>
-      <c r="HU110"/>
-      <c r="HV110"/>
-      <c r="HW110"/>
-      <c r="HX110"/>
-      <c r="HY110"/>
-      <c r="HZ110"/>
-      <c r="IA110"/>
-      <c r="IB110"/>
-      <c r="IC110"/>
-      <c r="ID110"/>
-      <c r="IE110"/>
-      <c r="IF110"/>
-      <c r="IG110"/>
-      <c r="IH110"/>
-      <c r="II110"/>
-      <c r="IJ110"/>
-      <c r="IK110"/>
-      <c r="IL110"/>
-      <c r="IM110"/>
-      <c r="IN110"/>
-      <c r="IO110"/>
-      <c r="IP110"/>
-      <c r="IQ110"/>
-      <c r="IR110"/>
-      <c r="IS110"/>
-      <c r="IT110"/>
-      <c r="IU110"/>
-      <c r="IV110"/>
-      <c r="IW110"/>
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A111" s="57" t="s">
-        <v>234</v>
-      </c>
-      <c r="B111" s="57" t="s">
-        <v>234</v>
-      </c>
-      <c r="C111" s="57" t="s">
-        <v>235</v>
-      </c>
-      <c r="D111" s="57"/>
-      <c r="E111" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F111" s="97" t="s">
+      <c r="A111" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B111" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C111" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="D111" s="58"/>
+      <c r="E111" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F111" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G111" s="81">
+      <c r="G111" s="25">
         <v>4</v>
       </c>
-      <c r="H111" s="57">
+      <c r="H111" s="58">
         <v>1</v>
       </c>
-      <c r="I111" s="97" t="s">
+      <c r="I111" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J111" s="97" t="s">
+      <c r="J111" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K111"/>
-      <c r="L111"/>
-      <c r="M111"/>
-      <c r="N111"/>
-      <c r="O111"/>
-      <c r="P111"/>
-      <c r="Q111"/>
-      <c r="R111"/>
-      <c r="S111"/>
-      <c r="T111"/>
-      <c r="U111"/>
-      <c r="V111"/>
-      <c r="W111"/>
-      <c r="X111"/>
-      <c r="Y111"/>
-      <c r="Z111"/>
-      <c r="AA111"/>
-      <c r="AB111"/>
-      <c r="AC111"/>
-      <c r="AD111"/>
-      <c r="AE111"/>
-      <c r="AF111"/>
-      <c r="AG111"/>
-      <c r="AH111"/>
-      <c r="AI111"/>
-      <c r="AJ111"/>
-      <c r="AK111"/>
-      <c r="AL111"/>
-      <c r="AM111"/>
-      <c r="AN111"/>
-      <c r="AO111"/>
-      <c r="AP111"/>
-      <c r="AQ111"/>
-      <c r="AR111"/>
-      <c r="AS111"/>
-      <c r="AT111"/>
-      <c r="AU111"/>
-      <c r="AV111"/>
-      <c r="AW111"/>
-      <c r="AX111"/>
-      <c r="AY111"/>
-      <c r="AZ111"/>
-      <c r="BA111"/>
-      <c r="BB111"/>
-      <c r="BC111"/>
-      <c r="BD111"/>
-      <c r="BE111"/>
-      <c r="BF111"/>
-      <c r="BG111"/>
-      <c r="BH111"/>
-      <c r="BI111"/>
-      <c r="BJ111"/>
-      <c r="BK111"/>
-      <c r="BL111"/>
-      <c r="BM111"/>
-      <c r="BN111"/>
-      <c r="BO111"/>
-      <c r="BP111"/>
-      <c r="BQ111"/>
-      <c r="BR111"/>
-      <c r="BS111"/>
-      <c r="BT111"/>
-      <c r="BU111"/>
-      <c r="BV111"/>
-      <c r="BW111"/>
-      <c r="BX111"/>
-      <c r="BY111"/>
-      <c r="BZ111"/>
-      <c r="CA111"/>
-      <c r="CB111"/>
-      <c r="CC111"/>
-      <c r="CD111"/>
-      <c r="CE111"/>
-      <c r="CF111"/>
-      <c r="CG111"/>
-      <c r="CH111"/>
-      <c r="CI111"/>
-      <c r="CJ111"/>
-      <c r="CK111"/>
-      <c r="CL111"/>
-      <c r="CM111"/>
-      <c r="CN111"/>
-      <c r="CO111"/>
-      <c r="CP111"/>
-      <c r="CQ111"/>
-      <c r="CR111"/>
-      <c r="CS111"/>
-      <c r="CT111"/>
-      <c r="CU111"/>
-      <c r="CV111"/>
-      <c r="CW111"/>
-      <c r="CX111"/>
-      <c r="CY111"/>
-      <c r="CZ111"/>
-      <c r="DA111"/>
-      <c r="DB111"/>
-      <c r="DC111"/>
-      <c r="DD111"/>
-      <c r="DE111"/>
-      <c r="DF111"/>
-      <c r="DG111"/>
-      <c r="DH111"/>
-      <c r="DI111"/>
-      <c r="DJ111"/>
-      <c r="DK111"/>
-      <c r="DL111"/>
-      <c r="DM111"/>
-      <c r="DN111"/>
-      <c r="DO111"/>
-      <c r="DP111"/>
-      <c r="DQ111"/>
-      <c r="DR111"/>
-      <c r="DS111"/>
-      <c r="DT111"/>
-      <c r="DU111"/>
-      <c r="DV111"/>
-      <c r="DW111"/>
-      <c r="DX111"/>
-      <c r="DY111"/>
-      <c r="DZ111"/>
-      <c r="EA111"/>
-      <c r="EB111"/>
-      <c r="EC111"/>
-      <c r="ED111"/>
-      <c r="EE111"/>
-      <c r="EF111"/>
-      <c r="EG111"/>
-      <c r="EH111"/>
-      <c r="EI111"/>
-      <c r="EJ111"/>
-      <c r="EK111"/>
-      <c r="EL111"/>
-      <c r="EM111"/>
-      <c r="EN111"/>
-      <c r="EO111"/>
-      <c r="EP111"/>
-      <c r="EQ111"/>
-      <c r="ER111"/>
-      <c r="ES111"/>
-      <c r="ET111"/>
-      <c r="EU111"/>
-      <c r="EV111"/>
-      <c r="EW111"/>
-      <c r="EX111"/>
-      <c r="EY111"/>
-      <c r="EZ111"/>
-      <c r="FA111"/>
-      <c r="FB111"/>
-      <c r="FC111"/>
-      <c r="FD111"/>
-      <c r="FE111"/>
-      <c r="FF111"/>
-      <c r="FG111"/>
-      <c r="FH111"/>
-      <c r="FI111"/>
-      <c r="FJ111"/>
-      <c r="FK111"/>
-      <c r="FL111"/>
-      <c r="FM111"/>
-      <c r="FN111"/>
-      <c r="FO111"/>
-      <c r="FP111"/>
-      <c r="FQ111"/>
-      <c r="FR111"/>
-      <c r="FS111"/>
-      <c r="FT111"/>
-      <c r="FU111"/>
-      <c r="FV111"/>
-      <c r="FW111"/>
-      <c r="FX111"/>
-      <c r="FY111"/>
-      <c r="FZ111"/>
-      <c r="GA111"/>
-      <c r="GB111"/>
-      <c r="GC111"/>
-      <c r="GD111"/>
-      <c r="GE111"/>
-      <c r="GF111"/>
-      <c r="GG111"/>
-      <c r="GH111"/>
-      <c r="GI111"/>
-      <c r="GJ111"/>
-      <c r="GK111"/>
-      <c r="GL111"/>
-      <c r="GM111"/>
-      <c r="GN111"/>
-      <c r="GO111"/>
-      <c r="GP111"/>
-      <c r="GQ111"/>
-      <c r="GR111"/>
-      <c r="GS111"/>
-      <c r="GT111"/>
-      <c r="GU111"/>
-      <c r="GV111"/>
-      <c r="GW111"/>
-      <c r="GX111"/>
-      <c r="GY111"/>
-      <c r="GZ111"/>
-      <c r="HA111"/>
-      <c r="HB111"/>
-      <c r="HC111"/>
-      <c r="HD111"/>
-      <c r="HE111"/>
-      <c r="HF111"/>
-      <c r="HG111"/>
-      <c r="HH111"/>
-      <c r="HI111"/>
-      <c r="HJ111"/>
-      <c r="HK111"/>
-      <c r="HL111"/>
-      <c r="HM111"/>
-      <c r="HN111"/>
-      <c r="HO111"/>
-      <c r="HP111"/>
-      <c r="HQ111"/>
-      <c r="HR111"/>
-      <c r="HS111"/>
-      <c r="HT111"/>
-      <c r="HU111"/>
-      <c r="HV111"/>
-      <c r="HW111"/>
-      <c r="HX111"/>
-      <c r="HY111"/>
-      <c r="HZ111"/>
-      <c r="IA111"/>
-      <c r="IB111"/>
-      <c r="IC111"/>
-      <c r="ID111"/>
-      <c r="IE111"/>
-      <c r="IF111"/>
-      <c r="IG111"/>
-      <c r="IH111"/>
-      <c r="II111"/>
-      <c r="IJ111"/>
-      <c r="IK111"/>
-      <c r="IL111"/>
-      <c r="IM111"/>
-      <c r="IN111"/>
-      <c r="IO111"/>
-      <c r="IP111"/>
-      <c r="IQ111"/>
-      <c r="IR111"/>
-      <c r="IS111"/>
-      <c r="IT111"/>
-      <c r="IU111"/>
-      <c r="IV111"/>
-      <c r="IW111"/>
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A112" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="B112" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="C112" s="57" t="s">
-        <v>237</v>
-      </c>
-      <c r="D112" s="57"/>
-      <c r="E112" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F112" s="97" t="s">
+      <c r="A112" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B112" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C112" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="D112" s="58"/>
+      <c r="E112" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F112" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G112" s="81">
-        <v>0</v>
-      </c>
-      <c r="H112" s="57">
+      <c r="G112" s="25">
+        <v>0</v>
+      </c>
+      <c r="H112" s="58">
         <v>1</v>
       </c>
-      <c r="I112" s="97" t="s">
+      <c r="I112" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J112" s="97" t="s">
+      <c r="J112" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K112"/>
-      <c r="L112"/>
-      <c r="M112"/>
-      <c r="N112"/>
-      <c r="O112"/>
-      <c r="P112"/>
-      <c r="Q112"/>
-      <c r="R112"/>
-      <c r="S112"/>
-      <c r="T112"/>
-      <c r="U112"/>
-      <c r="V112"/>
-      <c r="W112"/>
-      <c r="X112"/>
-      <c r="Y112"/>
-      <c r="Z112"/>
-      <c r="AA112"/>
-      <c r="AB112"/>
-      <c r="AC112"/>
-      <c r="AD112"/>
-      <c r="AE112"/>
-      <c r="AF112"/>
-      <c r="AG112"/>
-      <c r="AH112"/>
-      <c r="AI112"/>
-      <c r="AJ112"/>
-      <c r="AK112"/>
-      <c r="AL112"/>
-      <c r="AM112"/>
-      <c r="AN112"/>
-      <c r="AO112"/>
-      <c r="AP112"/>
-      <c r="AQ112"/>
-      <c r="AR112"/>
-      <c r="AS112"/>
-      <c r="AT112"/>
-      <c r="AU112"/>
-      <c r="AV112"/>
-      <c r="AW112"/>
-      <c r="AX112"/>
-      <c r="AY112"/>
-      <c r="AZ112"/>
-      <c r="BA112"/>
-      <c r="BB112"/>
-      <c r="BC112"/>
-      <c r="BD112"/>
-      <c r="BE112"/>
-      <c r="BF112"/>
-      <c r="BG112"/>
-      <c r="BH112"/>
-      <c r="BI112"/>
-      <c r="BJ112"/>
-      <c r="BK112"/>
-      <c r="BL112"/>
-      <c r="BM112"/>
-      <c r="BN112"/>
-      <c r="BO112"/>
-      <c r="BP112"/>
-      <c r="BQ112"/>
-      <c r="BR112"/>
-      <c r="BS112"/>
-      <c r="BT112"/>
-      <c r="BU112"/>
-      <c r="BV112"/>
-      <c r="BW112"/>
-      <c r="BX112"/>
-      <c r="BY112"/>
-      <c r="BZ112"/>
-      <c r="CA112"/>
-      <c r="CB112"/>
-      <c r="CC112"/>
-      <c r="CD112"/>
-      <c r="CE112"/>
-      <c r="CF112"/>
-      <c r="CG112"/>
-      <c r="CH112"/>
-      <c r="CI112"/>
-      <c r="CJ112"/>
-      <c r="CK112"/>
-      <c r="CL112"/>
-      <c r="CM112"/>
-      <c r="CN112"/>
-      <c r="CO112"/>
-      <c r="CP112"/>
-      <c r="CQ112"/>
-      <c r="CR112"/>
-      <c r="CS112"/>
-      <c r="CT112"/>
-      <c r="CU112"/>
-      <c r="CV112"/>
-      <c r="CW112"/>
-      <c r="CX112"/>
-      <c r="CY112"/>
-      <c r="CZ112"/>
-      <c r="DA112"/>
-      <c r="DB112"/>
-      <c r="DC112"/>
-      <c r="DD112"/>
-      <c r="DE112"/>
-      <c r="DF112"/>
-      <c r="DG112"/>
-      <c r="DH112"/>
-      <c r="DI112"/>
-      <c r="DJ112"/>
-      <c r="DK112"/>
-      <c r="DL112"/>
-      <c r="DM112"/>
-      <c r="DN112"/>
-      <c r="DO112"/>
-      <c r="DP112"/>
-      <c r="DQ112"/>
-      <c r="DR112"/>
-      <c r="DS112"/>
-      <c r="DT112"/>
-      <c r="DU112"/>
-      <c r="DV112"/>
-      <c r="DW112"/>
-      <c r="DX112"/>
-      <c r="DY112"/>
-      <c r="DZ112"/>
-      <c r="EA112"/>
-      <c r="EB112"/>
-      <c r="EC112"/>
-      <c r="ED112"/>
-      <c r="EE112"/>
-      <c r="EF112"/>
-      <c r="EG112"/>
-      <c r="EH112"/>
-      <c r="EI112"/>
-      <c r="EJ112"/>
-      <c r="EK112"/>
-      <c r="EL112"/>
-      <c r="EM112"/>
-      <c r="EN112"/>
-      <c r="EO112"/>
-      <c r="EP112"/>
-      <c r="EQ112"/>
-      <c r="ER112"/>
-      <c r="ES112"/>
-      <c r="ET112"/>
-      <c r="EU112"/>
-      <c r="EV112"/>
-      <c r="EW112"/>
-      <c r="EX112"/>
-      <c r="EY112"/>
-      <c r="EZ112"/>
-      <c r="FA112"/>
-      <c r="FB112"/>
-      <c r="FC112"/>
-      <c r="FD112"/>
-      <c r="FE112"/>
-      <c r="FF112"/>
-      <c r="FG112"/>
-      <c r="FH112"/>
-      <c r="FI112"/>
-      <c r="FJ112"/>
-      <c r="FK112"/>
-      <c r="FL112"/>
-      <c r="FM112"/>
-      <c r="FN112"/>
-      <c r="FO112"/>
-      <c r="FP112"/>
-      <c r="FQ112"/>
-      <c r="FR112"/>
-      <c r="FS112"/>
-      <c r="FT112"/>
-      <c r="FU112"/>
-      <c r="FV112"/>
-      <c r="FW112"/>
-      <c r="FX112"/>
-      <c r="FY112"/>
-      <c r="FZ112"/>
-      <c r="GA112"/>
-      <c r="GB112"/>
-      <c r="GC112"/>
-      <c r="GD112"/>
-      <c r="GE112"/>
-      <c r="GF112"/>
-      <c r="GG112"/>
-      <c r="GH112"/>
-      <c r="GI112"/>
-      <c r="GJ112"/>
-      <c r="GK112"/>
-      <c r="GL112"/>
-      <c r="GM112"/>
-      <c r="GN112"/>
-      <c r="GO112"/>
-      <c r="GP112"/>
-      <c r="GQ112"/>
-      <c r="GR112"/>
-      <c r="GS112"/>
-      <c r="GT112"/>
-      <c r="GU112"/>
-      <c r="GV112"/>
-      <c r="GW112"/>
-      <c r="GX112"/>
-      <c r="GY112"/>
-      <c r="GZ112"/>
-      <c r="HA112"/>
-      <c r="HB112"/>
-      <c r="HC112"/>
-      <c r="HD112"/>
-      <c r="HE112"/>
-      <c r="HF112"/>
-      <c r="HG112"/>
-      <c r="HH112"/>
-      <c r="HI112"/>
-      <c r="HJ112"/>
-      <c r="HK112"/>
-      <c r="HL112"/>
-      <c r="HM112"/>
-      <c r="HN112"/>
-      <c r="HO112"/>
-      <c r="HP112"/>
-      <c r="HQ112"/>
-      <c r="HR112"/>
-      <c r="HS112"/>
-      <c r="HT112"/>
-      <c r="HU112"/>
-      <c r="HV112"/>
-      <c r="HW112"/>
-      <c r="HX112"/>
-      <c r="HY112"/>
-      <c r="HZ112"/>
-      <c r="IA112"/>
-      <c r="IB112"/>
-      <c r="IC112"/>
-      <c r="ID112"/>
-      <c r="IE112"/>
-      <c r="IF112"/>
-      <c r="IG112"/>
-      <c r="IH112"/>
-      <c r="II112"/>
-      <c r="IJ112"/>
-      <c r="IK112"/>
-      <c r="IL112"/>
-      <c r="IM112"/>
-      <c r="IN112"/>
-      <c r="IO112"/>
-      <c r="IP112"/>
-      <c r="IQ112"/>
-      <c r="IR112"/>
-      <c r="IS112"/>
-      <c r="IT112"/>
-      <c r="IU112"/>
-      <c r="IV112"/>
-      <c r="IW112"/>
     </row>
-    <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A113" s="57" t="s">
-        <v>238</v>
-      </c>
-      <c r="B113" s="57" t="s">
-        <v>238</v>
-      </c>
-      <c r="C113" s="57" t="s">
-        <v>239</v>
-      </c>
-      <c r="D113" s="57"/>
-      <c r="E113" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F113" s="97" t="s">
+    <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A113" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B113" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C113" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="D113" s="58"/>
+      <c r="E113" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F113" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G113" s="81">
-        <v>0</v>
-      </c>
-      <c r="H113" s="57">
+      <c r="G113" s="25">
+        <v>0</v>
+      </c>
+      <c r="H113" s="58">
         <v>1</v>
       </c>
-      <c r="I113" s="97" t="s">
+      <c r="I113" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J113" s="97" t="s">
+      <c r="J113" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K113"/>
-      <c r="L113"/>
-      <c r="M113"/>
-      <c r="N113"/>
-      <c r="O113"/>
-      <c r="P113"/>
-      <c r="Q113"/>
-      <c r="R113"/>
-      <c r="S113"/>
-      <c r="T113"/>
-      <c r="U113"/>
-      <c r="V113"/>
-      <c r="W113"/>
-      <c r="X113"/>
-      <c r="Y113"/>
-      <c r="Z113"/>
-      <c r="AA113"/>
-      <c r="AB113"/>
-      <c r="AC113"/>
-      <c r="AD113"/>
-      <c r="AE113"/>
-      <c r="AF113"/>
-      <c r="AG113"/>
-      <c r="AH113"/>
-      <c r="AI113"/>
-      <c r="AJ113"/>
-      <c r="AK113"/>
-      <c r="AL113"/>
-      <c r="AM113"/>
-      <c r="AN113"/>
-      <c r="AO113"/>
-      <c r="AP113"/>
-      <c r="AQ113"/>
-      <c r="AR113"/>
-      <c r="AS113"/>
-      <c r="AT113"/>
-      <c r="AU113"/>
-      <c r="AV113"/>
-      <c r="AW113"/>
-      <c r="AX113"/>
-      <c r="AY113"/>
-      <c r="AZ113"/>
-      <c r="BA113"/>
-      <c r="BB113"/>
-      <c r="BC113"/>
-      <c r="BD113"/>
-      <c r="BE113"/>
-      <c r="BF113"/>
-      <c r="BG113"/>
-      <c r="BH113"/>
-      <c r="BI113"/>
-      <c r="BJ113"/>
-      <c r="BK113"/>
-      <c r="BL113"/>
-      <c r="BM113"/>
-      <c r="BN113"/>
-      <c r="BO113"/>
-      <c r="BP113"/>
-      <c r="BQ113"/>
-      <c r="BR113"/>
-      <c r="BS113"/>
-      <c r="BT113"/>
-      <c r="BU113"/>
-      <c r="BV113"/>
-      <c r="BW113"/>
-      <c r="BX113"/>
-      <c r="BY113"/>
-      <c r="BZ113"/>
-      <c r="CA113"/>
-      <c r="CB113"/>
-      <c r="CC113"/>
-      <c r="CD113"/>
-      <c r="CE113"/>
-      <c r="CF113"/>
-      <c r="CG113"/>
-      <c r="CH113"/>
-      <c r="CI113"/>
-      <c r="CJ113"/>
-      <c r="CK113"/>
-      <c r="CL113"/>
-      <c r="CM113"/>
-      <c r="CN113"/>
-      <c r="CO113"/>
-      <c r="CP113"/>
-      <c r="CQ113"/>
-      <c r="CR113"/>
-      <c r="CS113"/>
-      <c r="CT113"/>
-      <c r="CU113"/>
-      <c r="CV113"/>
-      <c r="CW113"/>
-      <c r="CX113"/>
-      <c r="CY113"/>
-      <c r="CZ113"/>
-      <c r="DA113"/>
-      <c r="DB113"/>
-      <c r="DC113"/>
-      <c r="DD113"/>
-      <c r="DE113"/>
-      <c r="DF113"/>
-      <c r="DG113"/>
-      <c r="DH113"/>
-      <c r="DI113"/>
-      <c r="DJ113"/>
-      <c r="DK113"/>
-      <c r="DL113"/>
-      <c r="DM113"/>
-      <c r="DN113"/>
-      <c r="DO113"/>
-      <c r="DP113"/>
-      <c r="DQ113"/>
-      <c r="DR113"/>
-      <c r="DS113"/>
-      <c r="DT113"/>
-      <c r="DU113"/>
-      <c r="DV113"/>
-      <c r="DW113"/>
-      <c r="DX113"/>
-      <c r="DY113"/>
-      <c r="DZ113"/>
-      <c r="EA113"/>
-      <c r="EB113"/>
-      <c r="EC113"/>
-      <c r="ED113"/>
-      <c r="EE113"/>
-      <c r="EF113"/>
-      <c r="EG113"/>
-      <c r="EH113"/>
-      <c r="EI113"/>
-      <c r="EJ113"/>
-      <c r="EK113"/>
-      <c r="EL113"/>
-      <c r="EM113"/>
-      <c r="EN113"/>
-      <c r="EO113"/>
-      <c r="EP113"/>
-      <c r="EQ113"/>
-      <c r="ER113"/>
-      <c r="ES113"/>
-      <c r="ET113"/>
-      <c r="EU113"/>
-      <c r="EV113"/>
-      <c r="EW113"/>
-      <c r="EX113"/>
-      <c r="EY113"/>
-      <c r="EZ113"/>
-      <c r="FA113"/>
-      <c r="FB113"/>
-      <c r="FC113"/>
-      <c r="FD113"/>
-      <c r="FE113"/>
-      <c r="FF113"/>
-      <c r="FG113"/>
-      <c r="FH113"/>
-      <c r="FI113"/>
-      <c r="FJ113"/>
-      <c r="FK113"/>
-      <c r="FL113"/>
-      <c r="FM113"/>
-      <c r="FN113"/>
-      <c r="FO113"/>
-      <c r="FP113"/>
-      <c r="FQ113"/>
-      <c r="FR113"/>
-      <c r="FS113"/>
-      <c r="FT113"/>
-      <c r="FU113"/>
-      <c r="FV113"/>
-      <c r="FW113"/>
-      <c r="FX113"/>
-      <c r="FY113"/>
-      <c r="FZ113"/>
-      <c r="GA113"/>
-      <c r="GB113"/>
-      <c r="GC113"/>
-      <c r="GD113"/>
-      <c r="GE113"/>
-      <c r="GF113"/>
-      <c r="GG113"/>
-      <c r="GH113"/>
-      <c r="GI113"/>
-      <c r="GJ113"/>
-      <c r="GK113"/>
-      <c r="GL113"/>
-      <c r="GM113"/>
-      <c r="GN113"/>
-      <c r="GO113"/>
-      <c r="GP113"/>
-      <c r="GQ113"/>
-      <c r="GR113"/>
-      <c r="GS113"/>
-      <c r="GT113"/>
-      <c r="GU113"/>
-      <c r="GV113"/>
-      <c r="GW113"/>
-      <c r="GX113"/>
-      <c r="GY113"/>
-      <c r="GZ113"/>
-      <c r="HA113"/>
-      <c r="HB113"/>
-      <c r="HC113"/>
-      <c r="HD113"/>
-      <c r="HE113"/>
-      <c r="HF113"/>
-      <c r="HG113"/>
-      <c r="HH113"/>
-      <c r="HI113"/>
-      <c r="HJ113"/>
-      <c r="HK113"/>
-      <c r="HL113"/>
-      <c r="HM113"/>
-      <c r="HN113"/>
-      <c r="HO113"/>
-      <c r="HP113"/>
-      <c r="HQ113"/>
-      <c r="HR113"/>
-      <c r="HS113"/>
-      <c r="HT113"/>
-      <c r="HU113"/>
-      <c r="HV113"/>
-      <c r="HW113"/>
-      <c r="HX113"/>
-      <c r="HY113"/>
-      <c r="HZ113"/>
-      <c r="IA113"/>
-      <c r="IB113"/>
-      <c r="IC113"/>
-      <c r="ID113"/>
-      <c r="IE113"/>
-      <c r="IF113"/>
-      <c r="IG113"/>
-      <c r="IH113"/>
-      <c r="II113"/>
-      <c r="IJ113"/>
-      <c r="IK113"/>
-      <c r="IL113"/>
-      <c r="IM113"/>
-      <c r="IN113"/>
-      <c r="IO113"/>
-      <c r="IP113"/>
-      <c r="IQ113"/>
-      <c r="IR113"/>
-      <c r="IS113"/>
-      <c r="IT113"/>
-      <c r="IU113"/>
-      <c r="IV113"/>
-      <c r="IW113"/>
     </row>
-    <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A114" s="57" t="s">
+    <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A114" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B114" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C114" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="B114" s="57" t="s">
-        <v>240</v>
-      </c>
-      <c r="C114" s="97" t="s">
-        <v>239</v>
-      </c>
-      <c r="D114" s="57"/>
-      <c r="E114" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F114" s="97" t="s">
+      <c r="D114" s="58"/>
+      <c r="E114" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F114" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G114" s="81">
-        <v>0</v>
-      </c>
-      <c r="H114" s="57">
+      <c r="G114" s="25">
+        <v>0</v>
+      </c>
+      <c r="H114" s="58">
         <v>1</v>
       </c>
-      <c r="I114" s="97" t="s">
+      <c r="I114" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J114" s="97" t="s">
+      <c r="J114" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K114"/>
-      <c r="L114"/>
-      <c r="M114"/>
-      <c r="N114"/>
-      <c r="O114"/>
-      <c r="P114"/>
-      <c r="Q114"/>
-      <c r="R114"/>
-      <c r="S114"/>
-      <c r="T114"/>
-      <c r="U114"/>
-      <c r="V114"/>
-      <c r="W114"/>
-      <c r="X114"/>
-      <c r="Y114"/>
-      <c r="Z114"/>
-      <c r="AA114"/>
-      <c r="AB114"/>
-      <c r="AC114"/>
-      <c r="AD114"/>
-      <c r="AE114"/>
-      <c r="AF114"/>
-      <c r="AG114"/>
-      <c r="AH114"/>
-      <c r="AI114"/>
-      <c r="AJ114"/>
-      <c r="AK114"/>
-      <c r="AL114"/>
-      <c r="AM114"/>
-      <c r="AN114"/>
-      <c r="AO114"/>
-      <c r="AP114"/>
-      <c r="AQ114"/>
-      <c r="AR114"/>
-      <c r="AS114"/>
-      <c r="AT114"/>
-      <c r="AU114"/>
-      <c r="AV114"/>
-      <c r="AW114"/>
-      <c r="AX114"/>
-      <c r="AY114"/>
-      <c r="AZ114"/>
-      <c r="BA114"/>
-      <c r="BB114"/>
-      <c r="BC114"/>
-      <c r="BD114"/>
-      <c r="BE114"/>
-      <c r="BF114"/>
-      <c r="BG114"/>
-      <c r="BH114"/>
-      <c r="BI114"/>
-      <c r="BJ114"/>
-      <c r="BK114"/>
-      <c r="BL114"/>
-      <c r="BM114"/>
-      <c r="BN114"/>
-      <c r="BO114"/>
-      <c r="BP114"/>
-      <c r="BQ114"/>
-      <c r="BR114"/>
-      <c r="BS114"/>
-      <c r="BT114"/>
-      <c r="BU114"/>
-      <c r="BV114"/>
-      <c r="BW114"/>
-      <c r="BX114"/>
-      <c r="BY114"/>
-      <c r="BZ114"/>
-      <c r="CA114"/>
-      <c r="CB114"/>
-      <c r="CC114"/>
-      <c r="CD114"/>
-      <c r="CE114"/>
-      <c r="CF114"/>
-      <c r="CG114"/>
-      <c r="CH114"/>
-      <c r="CI114"/>
-      <c r="CJ114"/>
-      <c r="CK114"/>
-      <c r="CL114"/>
-      <c r="CM114"/>
-      <c r="CN114"/>
-      <c r="CO114"/>
-      <c r="CP114"/>
-      <c r="CQ114"/>
-      <c r="CR114"/>
-      <c r="CS114"/>
-      <c r="CT114"/>
-      <c r="CU114"/>
-      <c r="CV114"/>
-      <c r="CW114"/>
-      <c r="CX114"/>
-      <c r="CY114"/>
-      <c r="CZ114"/>
-      <c r="DA114"/>
-      <c r="DB114"/>
-      <c r="DC114"/>
-      <c r="DD114"/>
-      <c r="DE114"/>
-      <c r="DF114"/>
-      <c r="DG114"/>
-      <c r="DH114"/>
-      <c r="DI114"/>
-      <c r="DJ114"/>
-      <c r="DK114"/>
-      <c r="DL114"/>
-      <c r="DM114"/>
-      <c r="DN114"/>
-      <c r="DO114"/>
-      <c r="DP114"/>
-      <c r="DQ114"/>
-      <c r="DR114"/>
-      <c r="DS114"/>
-      <c r="DT114"/>
-      <c r="DU114"/>
-      <c r="DV114"/>
-      <c r="DW114"/>
-      <c r="DX114"/>
-      <c r="DY114"/>
-      <c r="DZ114"/>
-      <c r="EA114"/>
-      <c r="EB114"/>
-      <c r="EC114"/>
-      <c r="ED114"/>
-      <c r="EE114"/>
-      <c r="EF114"/>
-      <c r="EG114"/>
-      <c r="EH114"/>
-      <c r="EI114"/>
-      <c r="EJ114"/>
-      <c r="EK114"/>
-      <c r="EL114"/>
-      <c r="EM114"/>
-      <c r="EN114"/>
-      <c r="EO114"/>
-      <c r="EP114"/>
-      <c r="EQ114"/>
-      <c r="ER114"/>
-      <c r="ES114"/>
-      <c r="ET114"/>
-      <c r="EU114"/>
-      <c r="EV114"/>
-      <c r="EW114"/>
-      <c r="EX114"/>
-      <c r="EY114"/>
-      <c r="EZ114"/>
-      <c r="FA114"/>
-      <c r="FB114"/>
-      <c r="FC114"/>
-      <c r="FD114"/>
-      <c r="FE114"/>
-      <c r="FF114"/>
-      <c r="FG114"/>
-      <c r="FH114"/>
-      <c r="FI114"/>
-      <c r="FJ114"/>
-      <c r="FK114"/>
-      <c r="FL114"/>
-      <c r="FM114"/>
-      <c r="FN114"/>
-      <c r="FO114"/>
-      <c r="FP114"/>
-      <c r="FQ114"/>
-      <c r="FR114"/>
-      <c r="FS114"/>
-      <c r="FT114"/>
-      <c r="FU114"/>
-      <c r="FV114"/>
-      <c r="FW114"/>
-      <c r="FX114"/>
-      <c r="FY114"/>
-      <c r="FZ114"/>
-      <c r="GA114"/>
-      <c r="GB114"/>
-      <c r="GC114"/>
-      <c r="GD114"/>
-      <c r="GE114"/>
-      <c r="GF114"/>
-      <c r="GG114"/>
-      <c r="GH114"/>
-      <c r="GI114"/>
-      <c r="GJ114"/>
-      <c r="GK114"/>
-      <c r="GL114"/>
-      <c r="GM114"/>
-      <c r="GN114"/>
-      <c r="GO114"/>
-      <c r="GP114"/>
-      <c r="GQ114"/>
-      <c r="GR114"/>
-      <c r="GS114"/>
-      <c r="GT114"/>
-      <c r="GU114"/>
-      <c r="GV114"/>
-      <c r="GW114"/>
-      <c r="GX114"/>
-      <c r="GY114"/>
-      <c r="GZ114"/>
-      <c r="HA114"/>
-      <c r="HB114"/>
-      <c r="HC114"/>
-      <c r="HD114"/>
-      <c r="HE114"/>
-      <c r="HF114"/>
-      <c r="HG114"/>
-      <c r="HH114"/>
-      <c r="HI114"/>
-      <c r="HJ114"/>
-      <c r="HK114"/>
-      <c r="HL114"/>
-      <c r="HM114"/>
-      <c r="HN114"/>
-      <c r="HO114"/>
-      <c r="HP114"/>
-      <c r="HQ114"/>
-      <c r="HR114"/>
-      <c r="HS114"/>
-      <c r="HT114"/>
-      <c r="HU114"/>
-      <c r="HV114"/>
-      <c r="HW114"/>
-      <c r="HX114"/>
-      <c r="HY114"/>
-      <c r="HZ114"/>
-      <c r="IA114"/>
-      <c r="IB114"/>
-      <c r="IC114"/>
-      <c r="ID114"/>
-      <c r="IE114"/>
-      <c r="IF114"/>
-      <c r="IG114"/>
-      <c r="IH114"/>
-      <c r="II114"/>
-      <c r="IJ114"/>
-      <c r="IK114"/>
-      <c r="IL114"/>
-      <c r="IM114"/>
-      <c r="IN114"/>
-      <c r="IO114"/>
-      <c r="IP114"/>
-      <c r="IQ114"/>
-      <c r="IR114"/>
-      <c r="IS114"/>
-      <c r="IT114"/>
-      <c r="IU114"/>
-      <c r="IV114"/>
-      <c r="IW114"/>
     </row>
-    <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A115" s="57" t="s">
+    <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A115" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B115" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C115" s="95" t="s">
+        <v>242</v>
+      </c>
+      <c r="D115" s="58"/>
+      <c r="E115" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F115" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G115" s="25">
+        <v>0</v>
+      </c>
+      <c r="H115" s="58">
+        <v>1</v>
+      </c>
+      <c r="I115" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J115" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A116" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B116" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C116" s="95" t="s">
+        <v>246</v>
+      </c>
+      <c r="D116" s="58"/>
+      <c r="E116" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F116" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="25">
+        <v>0</v>
+      </c>
+      <c r="H116" s="58">
+        <v>1</v>
+      </c>
+      <c r="I116" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J116" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A117" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B117" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C117" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="B115" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="C115" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="D115" s="57"/>
-      <c r="E115" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F115" s="97" t="s">
+      <c r="D117" s="58"/>
+      <c r="E117" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F117" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G115" s="81">
-        <v>0</v>
-      </c>
-      <c r="H115" s="57">
+      <c r="G117" s="25">
+        <v>0</v>
+      </c>
+      <c r="H117" s="58">
         <v>1</v>
       </c>
-      <c r="I115" s="97" t="s">
+      <c r="I117" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J115" s="97" t="s">
+      <c r="J117" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K115"/>
-      <c r="L115"/>
-      <c r="M115"/>
-      <c r="N115"/>
-      <c r="O115"/>
-      <c r="P115"/>
-      <c r="Q115"/>
-      <c r="R115"/>
-      <c r="S115"/>
-      <c r="T115"/>
-      <c r="U115"/>
-      <c r="V115"/>
-      <c r="W115"/>
-      <c r="X115"/>
-      <c r="Y115"/>
-      <c r="Z115"/>
-      <c r="AA115"/>
-      <c r="AB115"/>
-      <c r="AC115"/>
-      <c r="AD115"/>
-      <c r="AE115"/>
-      <c r="AF115"/>
-      <c r="AG115"/>
-      <c r="AH115"/>
-      <c r="AI115"/>
-      <c r="AJ115"/>
-      <c r="AK115"/>
-      <c r="AL115"/>
-      <c r="AM115"/>
-      <c r="AN115"/>
-      <c r="AO115"/>
-      <c r="AP115"/>
-      <c r="AQ115"/>
-      <c r="AR115"/>
-      <c r="AS115"/>
-      <c r="AT115"/>
-      <c r="AU115"/>
-      <c r="AV115"/>
-      <c r="AW115"/>
-      <c r="AX115"/>
-      <c r="AY115"/>
-      <c r="AZ115"/>
-      <c r="BA115"/>
-      <c r="BB115"/>
-      <c r="BC115"/>
-      <c r="BD115"/>
-      <c r="BE115"/>
-      <c r="BF115"/>
-      <c r="BG115"/>
-      <c r="BH115"/>
-      <c r="BI115"/>
-      <c r="BJ115"/>
-      <c r="BK115"/>
-      <c r="BL115"/>
-      <c r="BM115"/>
-      <c r="BN115"/>
-      <c r="BO115"/>
-      <c r="BP115"/>
-      <c r="BQ115"/>
-      <c r="BR115"/>
-      <c r="BS115"/>
-      <c r="BT115"/>
-      <c r="BU115"/>
-      <c r="BV115"/>
-      <c r="BW115"/>
-      <c r="BX115"/>
-      <c r="BY115"/>
-      <c r="BZ115"/>
-      <c r="CA115"/>
-      <c r="CB115"/>
-      <c r="CC115"/>
-      <c r="CD115"/>
-      <c r="CE115"/>
-      <c r="CF115"/>
-      <c r="CG115"/>
-      <c r="CH115"/>
-      <c r="CI115"/>
-      <c r="CJ115"/>
-      <c r="CK115"/>
-      <c r="CL115"/>
-      <c r="CM115"/>
-      <c r="CN115"/>
-      <c r="CO115"/>
-      <c r="CP115"/>
-      <c r="CQ115"/>
-      <c r="CR115"/>
-      <c r="CS115"/>
-      <c r="CT115"/>
-      <c r="CU115"/>
-      <c r="CV115"/>
-      <c r="CW115"/>
-      <c r="CX115"/>
-      <c r="CY115"/>
-      <c r="CZ115"/>
-      <c r="DA115"/>
-      <c r="DB115"/>
-      <c r="DC115"/>
-      <c r="DD115"/>
-      <c r="DE115"/>
-      <c r="DF115"/>
-      <c r="DG115"/>
-      <c r="DH115"/>
-      <c r="DI115"/>
-      <c r="DJ115"/>
-      <c r="DK115"/>
-      <c r="DL115"/>
-      <c r="DM115"/>
-      <c r="DN115"/>
-      <c r="DO115"/>
-      <c r="DP115"/>
-      <c r="DQ115"/>
-      <c r="DR115"/>
-      <c r="DS115"/>
-      <c r="DT115"/>
-      <c r="DU115"/>
-      <c r="DV115"/>
-      <c r="DW115"/>
-      <c r="DX115"/>
-      <c r="DY115"/>
-      <c r="DZ115"/>
-      <c r="EA115"/>
-      <c r="EB115"/>
-      <c r="EC115"/>
-      <c r="ED115"/>
-      <c r="EE115"/>
-      <c r="EF115"/>
-      <c r="EG115"/>
-      <c r="EH115"/>
-      <c r="EI115"/>
-      <c r="EJ115"/>
-      <c r="EK115"/>
-      <c r="EL115"/>
-      <c r="EM115"/>
-      <c r="EN115"/>
-      <c r="EO115"/>
-      <c r="EP115"/>
-      <c r="EQ115"/>
-      <c r="ER115"/>
-      <c r="ES115"/>
-      <c r="ET115"/>
-      <c r="EU115"/>
-      <c r="EV115"/>
-      <c r="EW115"/>
-      <c r="EX115"/>
-      <c r="EY115"/>
-      <c r="EZ115"/>
-      <c r="FA115"/>
-      <c r="FB115"/>
-      <c r="FC115"/>
-      <c r="FD115"/>
-      <c r="FE115"/>
-      <c r="FF115"/>
-      <c r="FG115"/>
-      <c r="FH115"/>
-      <c r="FI115"/>
-      <c r="FJ115"/>
-      <c r="FK115"/>
-      <c r="FL115"/>
-      <c r="FM115"/>
-      <c r="FN115"/>
-      <c r="FO115"/>
-      <c r="FP115"/>
-      <c r="FQ115"/>
-      <c r="FR115"/>
-      <c r="FS115"/>
-      <c r="FT115"/>
-      <c r="FU115"/>
-      <c r="FV115"/>
-      <c r="FW115"/>
-      <c r="FX115"/>
-      <c r="FY115"/>
-      <c r="FZ115"/>
-      <c r="GA115"/>
-      <c r="GB115"/>
-      <c r="GC115"/>
-      <c r="GD115"/>
-      <c r="GE115"/>
-      <c r="GF115"/>
-      <c r="GG115"/>
-      <c r="GH115"/>
-      <c r="GI115"/>
-      <c r="GJ115"/>
-      <c r="GK115"/>
-      <c r="GL115"/>
-      <c r="GM115"/>
-      <c r="GN115"/>
-      <c r="GO115"/>
-      <c r="GP115"/>
-      <c r="GQ115"/>
-      <c r="GR115"/>
-      <c r="GS115"/>
-      <c r="GT115"/>
-      <c r="GU115"/>
-      <c r="GV115"/>
-      <c r="GW115"/>
-      <c r="GX115"/>
-      <c r="GY115"/>
-      <c r="GZ115"/>
-      <c r="HA115"/>
-      <c r="HB115"/>
-      <c r="HC115"/>
-      <c r="HD115"/>
-      <c r="HE115"/>
-      <c r="HF115"/>
-      <c r="HG115"/>
-      <c r="HH115"/>
-      <c r="HI115"/>
-      <c r="HJ115"/>
-      <c r="HK115"/>
-      <c r="HL115"/>
-      <c r="HM115"/>
-      <c r="HN115"/>
-      <c r="HO115"/>
-      <c r="HP115"/>
-      <c r="HQ115"/>
-      <c r="HR115"/>
-      <c r="HS115"/>
-      <c r="HT115"/>
-      <c r="HU115"/>
-      <c r="HV115"/>
-      <c r="HW115"/>
-      <c r="HX115"/>
-      <c r="HY115"/>
-      <c r="HZ115"/>
-      <c r="IA115"/>
-      <c r="IB115"/>
-      <c r="IC115"/>
-      <c r="ID115"/>
-      <c r="IE115"/>
-      <c r="IF115"/>
-      <c r="IG115"/>
-      <c r="IH115"/>
-      <c r="II115"/>
-      <c r="IJ115"/>
-      <c r="IK115"/>
-      <c r="IL115"/>
-      <c r="IM115"/>
-      <c r="IN115"/>
-      <c r="IO115"/>
-      <c r="IP115"/>
-      <c r="IQ115"/>
-      <c r="IR115"/>
-      <c r="IS115"/>
-      <c r="IT115"/>
-      <c r="IU115"/>
-      <c r="IV115"/>
-      <c r="IW115"/>
     </row>
-    <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A116" s="57" t="s">
+    <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A118" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B118" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C118" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="D118" s="58"/>
+      <c r="E118" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F118" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G118" s="25">
+        <v>0</v>
+      </c>
+      <c r="H118" s="58">
+        <v>1</v>
+      </c>
+      <c r="I118" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J118" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A119" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B116" s="57" t="s">
-        <v>152</v>
-      </c>
-      <c r="C116" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="D116" s="57"/>
-      <c r="E116" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="F116" s="97" t="s">
+      <c r="B119" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C119" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D119" s="58"/>
+      <c r="E119" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F119" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G116" s="81">
-        <v>0</v>
-      </c>
-      <c r="H116" s="57">
+      <c r="G119" s="25">
+        <v>0</v>
+      </c>
+      <c r="H119" s="58">
         <v>1</v>
       </c>
-      <c r="I116" s="97" t="s">
+      <c r="I119" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J116" s="97" t="s">
+      <c r="J119" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K116"/>
-      <c r="L116"/>
-      <c r="M116"/>
-      <c r="N116"/>
-      <c r="O116"/>
-      <c r="P116"/>
-      <c r="Q116"/>
-      <c r="R116"/>
-      <c r="S116"/>
-      <c r="T116"/>
-      <c r="U116"/>
-      <c r="V116"/>
-      <c r="W116"/>
-      <c r="X116"/>
-      <c r="Y116"/>
-      <c r="Z116"/>
-      <c r="AA116"/>
-      <c r="AB116"/>
-      <c r="AC116"/>
-      <c r="AD116"/>
-      <c r="AE116"/>
-      <c r="AF116"/>
-      <c r="AG116"/>
-      <c r="AH116"/>
-      <c r="AI116"/>
-      <c r="AJ116"/>
-      <c r="AK116"/>
-      <c r="AL116"/>
-      <c r="AM116"/>
-      <c r="AN116"/>
-      <c r="AO116"/>
-      <c r="AP116"/>
-      <c r="AQ116"/>
-      <c r="AR116"/>
-      <c r="AS116"/>
-      <c r="AT116"/>
-      <c r="AU116"/>
-      <c r="AV116"/>
-      <c r="AW116"/>
-      <c r="AX116"/>
-      <c r="AY116"/>
-      <c r="AZ116"/>
-      <c r="BA116"/>
-      <c r="BB116"/>
-      <c r="BC116"/>
-      <c r="BD116"/>
-      <c r="BE116"/>
-      <c r="BF116"/>
-      <c r="BG116"/>
-      <c r="BH116"/>
-      <c r="BI116"/>
-      <c r="BJ116"/>
-      <c r="BK116"/>
-      <c r="BL116"/>
-      <c r="BM116"/>
-      <c r="BN116"/>
-      <c r="BO116"/>
-      <c r="BP116"/>
-      <c r="BQ116"/>
-      <c r="BR116"/>
-      <c r="BS116"/>
-      <c r="BT116"/>
-      <c r="BU116"/>
-      <c r="BV116"/>
-      <c r="BW116"/>
-      <c r="BX116"/>
-      <c r="BY116"/>
-      <c r="BZ116"/>
-      <c r="CA116"/>
-      <c r="CB116"/>
-      <c r="CC116"/>
-      <c r="CD116"/>
-      <c r="CE116"/>
-      <c r="CF116"/>
-      <c r="CG116"/>
-      <c r="CH116"/>
-      <c r="CI116"/>
-      <c r="CJ116"/>
-      <c r="CK116"/>
-      <c r="CL116"/>
-      <c r="CM116"/>
-      <c r="CN116"/>
-      <c r="CO116"/>
-      <c r="CP116"/>
-      <c r="CQ116"/>
-      <c r="CR116"/>
-      <c r="CS116"/>
-      <c r="CT116"/>
-      <c r="CU116"/>
-      <c r="CV116"/>
-      <c r="CW116"/>
-      <c r="CX116"/>
-      <c r="CY116"/>
-      <c r="CZ116"/>
-      <c r="DA116"/>
-      <c r="DB116"/>
-      <c r="DC116"/>
-      <c r="DD116"/>
-      <c r="DE116"/>
-      <c r="DF116"/>
-      <c r="DG116"/>
-      <c r="DH116"/>
-      <c r="DI116"/>
-      <c r="DJ116"/>
-      <c r="DK116"/>
-      <c r="DL116"/>
-      <c r="DM116"/>
-      <c r="DN116"/>
-      <c r="DO116"/>
-      <c r="DP116"/>
-      <c r="DQ116"/>
-      <c r="DR116"/>
-      <c r="DS116"/>
-      <c r="DT116"/>
-      <c r="DU116"/>
-      <c r="DV116"/>
-      <c r="DW116"/>
-      <c r="DX116"/>
-      <c r="DY116"/>
-      <c r="DZ116"/>
-      <c r="EA116"/>
-      <c r="EB116"/>
-      <c r="EC116"/>
-      <c r="ED116"/>
-      <c r="EE116"/>
-      <c r="EF116"/>
-      <c r="EG116"/>
-      <c r="EH116"/>
-      <c r="EI116"/>
-      <c r="EJ116"/>
-      <c r="EK116"/>
-      <c r="EL116"/>
-      <c r="EM116"/>
-      <c r="EN116"/>
-      <c r="EO116"/>
-      <c r="EP116"/>
-      <c r="EQ116"/>
-      <c r="ER116"/>
-      <c r="ES116"/>
-      <c r="ET116"/>
-      <c r="EU116"/>
-      <c r="EV116"/>
-      <c r="EW116"/>
-      <c r="EX116"/>
-      <c r="EY116"/>
-      <c r="EZ116"/>
-      <c r="FA116"/>
-      <c r="FB116"/>
-      <c r="FC116"/>
-      <c r="FD116"/>
-      <c r="FE116"/>
-      <c r="FF116"/>
-      <c r="FG116"/>
-      <c r="FH116"/>
-      <c r="FI116"/>
-      <c r="FJ116"/>
-      <c r="FK116"/>
-      <c r="FL116"/>
-      <c r="FM116"/>
-      <c r="FN116"/>
-      <c r="FO116"/>
-      <c r="FP116"/>
-      <c r="FQ116"/>
-      <c r="FR116"/>
-      <c r="FS116"/>
-      <c r="FT116"/>
-      <c r="FU116"/>
-      <c r="FV116"/>
-      <c r="FW116"/>
-      <c r="FX116"/>
-      <c r="FY116"/>
-      <c r="FZ116"/>
-      <c r="GA116"/>
-      <c r="GB116"/>
-      <c r="GC116"/>
-      <c r="GD116"/>
-      <c r="GE116"/>
-      <c r="GF116"/>
-      <c r="GG116"/>
-      <c r="GH116"/>
-      <c r="GI116"/>
-      <c r="GJ116"/>
-      <c r="GK116"/>
-      <c r="GL116"/>
-      <c r="GM116"/>
-      <c r="GN116"/>
-      <c r="GO116"/>
-      <c r="GP116"/>
-      <c r="GQ116"/>
-      <c r="GR116"/>
-      <c r="GS116"/>
-      <c r="GT116"/>
-      <c r="GU116"/>
-      <c r="GV116"/>
-      <c r="GW116"/>
-      <c r="GX116"/>
-      <c r="GY116"/>
-      <c r="GZ116"/>
-      <c r="HA116"/>
-      <c r="HB116"/>
-      <c r="HC116"/>
-      <c r="HD116"/>
-      <c r="HE116"/>
-      <c r="HF116"/>
-      <c r="HG116"/>
-      <c r="HH116"/>
-      <c r="HI116"/>
-      <c r="HJ116"/>
-      <c r="HK116"/>
-      <c r="HL116"/>
-      <c r="HM116"/>
-      <c r="HN116"/>
-      <c r="HO116"/>
-      <c r="HP116"/>
-      <c r="HQ116"/>
-      <c r="HR116"/>
-      <c r="HS116"/>
-      <c r="HT116"/>
-      <c r="HU116"/>
-      <c r="HV116"/>
-      <c r="HW116"/>
-      <c r="HX116"/>
-      <c r="HY116"/>
-      <c r="HZ116"/>
-      <c r="IA116"/>
-      <c r="IB116"/>
-      <c r="IC116"/>
-      <c r="ID116"/>
-      <c r="IE116"/>
-      <c r="IF116"/>
-      <c r="IG116"/>
-      <c r="IH116"/>
-      <c r="II116"/>
-      <c r="IJ116"/>
-      <c r="IK116"/>
-      <c r="IL116"/>
-      <c r="IM116"/>
-      <c r="IN116"/>
-      <c r="IO116"/>
-      <c r="IP116"/>
-      <c r="IQ116"/>
-      <c r="IR116"/>
-      <c r="IS116"/>
-      <c r="IT116"/>
-      <c r="IU116"/>
-      <c r="IV116"/>
-      <c r="IW116"/>
     </row>
-    <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="125" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="123" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="124" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="125" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="126" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="128" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
+    <row r="130" ht="17.100000000000001" customHeight="1"/>
+    <row r="131" ht="17.100000000000001" customHeight="1"/>
+    <row r="132" ht="17.100000000000001" customHeight="1"/>
+    <row r="133" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated referred from field setting
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61191AA-56C2-48CF-9B29-5E7181DA3DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD7F9D4-FB76-4380-80DE-D2A32AFC2267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31770" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="250">
   <si>
     <t>name</t>
   </si>
@@ -739,9 +739,6 @@
     <t>Client Name</t>
   </si>
   <si>
-    <t>Referral Form</t>
-  </si>
-  <si>
     <t>Referred To</t>
   </si>
   <si>
@@ -776,6 +773,9 @@
   </si>
   <si>
     <t>program_stream_ids</t>
+  </si>
+  <si>
+    <t>Referred From</t>
   </si>
 </sst>
 </file>
@@ -1686,8 +1686,8 @@
   </sheetPr>
   <dimension ref="A1:IW133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -16524,7 +16524,9 @@
       <c r="A102" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="B102" s="58"/>
+      <c r="B102" s="58" t="s">
+        <v>11</v>
+      </c>
       <c r="C102" s="95" t="s">
         <v>217</v>
       </c>
@@ -16552,7 +16554,9 @@
       <c r="A103" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="B103" s="58"/>
+      <c r="B103" s="58" t="s">
+        <v>11</v>
+      </c>
       <c r="C103" s="95" t="s">
         <v>218</v>
       </c>
@@ -16580,7 +16584,9 @@
       <c r="A104" s="95" t="s">
         <v>221</v>
       </c>
-      <c r="B104" s="58"/>
+      <c r="B104" s="58" t="s">
+        <v>11</v>
+      </c>
       <c r="C104" s="95" t="s">
         <v>222</v>
       </c>
@@ -17252,7 +17258,7 @@
         <v>232</v>
       </c>
       <c r="C110" s="58" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="D110" s="58"/>
       <c r="E110" s="96" t="s">
@@ -17276,13 +17282,13 @@
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B111" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C111" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
@@ -17312,7 +17318,7 @@
         <v>232</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
@@ -17336,13 +17342,13 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B113" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
@@ -17372,7 +17378,7 @@
         <v>232</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
@@ -17402,7 +17408,7 @@
         <v>232</v>
       </c>
       <c r="C115" s="95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
@@ -17426,13 +17432,13 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B116" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C116" s="95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
@@ -17462,7 +17468,7 @@
         <v>232</v>
       </c>
       <c r="C117" s="58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
@@ -17486,13 +17492,13 @@
     </row>
     <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B118" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C118" s="58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">

</xml_diff>

<commit_message>
updated service delivery field settings
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB72ACD-26EC-4578-AB7E-2656886DE83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44792CE5-0415-4FD1-9DDC-EBD00E61EB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31770" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="252">
   <si>
     <t>name</t>
   </si>
@@ -739,9 +739,6 @@
     <t>Client Name</t>
   </si>
   <si>
-    <t>Referral Form</t>
-  </si>
-  <si>
     <t>Referred To</t>
   </si>
   <si>
@@ -776,6 +773,15 @@
   </si>
   <si>
     <t>program_stream_ids</t>
+  </si>
+  <si>
+    <t>Referred From</t>
+  </si>
+  <si>
+    <t>task_completed_date</t>
+  </si>
+  <si>
+    <t>Task Completed Date</t>
   </si>
 </sst>
 </file>
@@ -1684,10 +1690,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW133"/>
+  <dimension ref="A1:IW134"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15924,43 +15930,292 @@
       <c r="IV80" s="60"/>
       <c r="IW80" s="60"/>
     </row>
-    <row r="81" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A81" s="58" t="s">
+    <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A81" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" s="59" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" s="59"/>
+      <c r="E81" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="F81" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G81" s="59">
+        <v>0</v>
+      </c>
+      <c r="H81" s="59">
+        <v>1</v>
+      </c>
+      <c r="I81" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="J81" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K81" s="60"/>
+      <c r="L81" s="60"/>
+      <c r="M81" s="60"/>
+      <c r="N81" s="60"/>
+      <c r="O81" s="60"/>
+      <c r="P81" s="60"/>
+      <c r="Q81" s="60"/>
+      <c r="R81" s="60"/>
+      <c r="S81" s="60"/>
+      <c r="T81" s="60"/>
+      <c r="U81" s="60"/>
+      <c r="V81" s="60"/>
+      <c r="W81" s="60"/>
+      <c r="X81" s="60"/>
+      <c r="Y81" s="60"/>
+      <c r="Z81" s="60"/>
+      <c r="AA81" s="60"/>
+      <c r="AB81" s="60"/>
+      <c r="AC81" s="60"/>
+      <c r="AD81" s="60"/>
+      <c r="AE81" s="60"/>
+      <c r="AF81" s="60"/>
+      <c r="AG81" s="60"/>
+      <c r="AH81" s="60"/>
+      <c r="AI81" s="60"/>
+      <c r="AJ81" s="60"/>
+      <c r="AK81" s="60"/>
+      <c r="AL81" s="60"/>
+      <c r="AM81" s="60"/>
+      <c r="AN81" s="60"/>
+      <c r="AO81" s="60"/>
+      <c r="AP81" s="60"/>
+      <c r="AQ81" s="60"/>
+      <c r="AR81" s="60"/>
+      <c r="AS81" s="60"/>
+      <c r="AT81" s="60"/>
+      <c r="AU81" s="60"/>
+      <c r="AV81" s="60"/>
+      <c r="AW81" s="60"/>
+      <c r="AX81" s="60"/>
+      <c r="AY81" s="60"/>
+      <c r="AZ81" s="60"/>
+      <c r="BA81" s="60"/>
+      <c r="BB81" s="60"/>
+      <c r="BC81" s="60"/>
+      <c r="BD81" s="60"/>
+      <c r="BE81" s="60"/>
+      <c r="BF81" s="60"/>
+      <c r="BG81" s="60"/>
+      <c r="BH81" s="60"/>
+      <c r="BI81" s="60"/>
+      <c r="BJ81" s="60"/>
+      <c r="BK81" s="60"/>
+      <c r="BL81" s="60"/>
+      <c r="BM81" s="60"/>
+      <c r="BN81" s="60"/>
+      <c r="BO81" s="60"/>
+      <c r="BP81" s="60"/>
+      <c r="BQ81" s="60"/>
+      <c r="BR81" s="60"/>
+      <c r="BS81" s="60"/>
+      <c r="BT81" s="60"/>
+      <c r="BU81" s="60"/>
+      <c r="BV81" s="60"/>
+      <c r="BW81" s="60"/>
+      <c r="BX81" s="60"/>
+      <c r="BY81" s="60"/>
+      <c r="BZ81" s="60"/>
+      <c r="CA81" s="60"/>
+      <c r="CB81" s="60"/>
+      <c r="CC81" s="60"/>
+      <c r="CD81" s="60"/>
+      <c r="CE81" s="60"/>
+      <c r="CF81" s="60"/>
+      <c r="CG81" s="60"/>
+      <c r="CH81" s="60"/>
+      <c r="CI81" s="60"/>
+      <c r="CJ81" s="60"/>
+      <c r="CK81" s="60"/>
+      <c r="CL81" s="60"/>
+      <c r="CM81" s="60"/>
+      <c r="CN81" s="60"/>
+      <c r="CO81" s="60"/>
+      <c r="CP81" s="60"/>
+      <c r="CQ81" s="60"/>
+      <c r="CR81" s="60"/>
+      <c r="CS81" s="60"/>
+      <c r="CT81" s="60"/>
+      <c r="CU81" s="60"/>
+      <c r="CV81" s="60"/>
+      <c r="CW81" s="60"/>
+      <c r="CX81" s="60"/>
+      <c r="CY81" s="60"/>
+      <c r="CZ81" s="60"/>
+      <c r="DA81" s="60"/>
+      <c r="DB81" s="60"/>
+      <c r="DC81" s="60"/>
+      <c r="DD81" s="60"/>
+      <c r="DE81" s="60"/>
+      <c r="DF81" s="60"/>
+      <c r="DG81" s="60"/>
+      <c r="DH81" s="60"/>
+      <c r="DI81" s="60"/>
+      <c r="DJ81" s="60"/>
+      <c r="DK81" s="60"/>
+      <c r="DL81" s="60"/>
+      <c r="DM81" s="60"/>
+      <c r="DN81" s="60"/>
+      <c r="DO81" s="60"/>
+      <c r="DP81" s="60"/>
+      <c r="DQ81" s="60"/>
+      <c r="DR81" s="60"/>
+      <c r="DS81" s="60"/>
+      <c r="DT81" s="60"/>
+      <c r="DU81" s="60"/>
+      <c r="DV81" s="60"/>
+      <c r="DW81" s="60"/>
+      <c r="DX81" s="60"/>
+      <c r="DY81" s="60"/>
+      <c r="DZ81" s="60"/>
+      <c r="EA81" s="60"/>
+      <c r="EB81" s="60"/>
+      <c r="EC81" s="60"/>
+      <c r="ED81" s="60"/>
+      <c r="EE81" s="60"/>
+      <c r="EF81" s="60"/>
+      <c r="EG81" s="60"/>
+      <c r="EH81" s="60"/>
+      <c r="EI81" s="60"/>
+      <c r="EJ81" s="60"/>
+      <c r="EK81" s="60"/>
+      <c r="EL81" s="60"/>
+      <c r="EM81" s="60"/>
+      <c r="EN81" s="60"/>
+      <c r="EO81" s="60"/>
+      <c r="EP81" s="60"/>
+      <c r="EQ81" s="60"/>
+      <c r="ER81" s="60"/>
+      <c r="ES81" s="60"/>
+      <c r="ET81" s="60"/>
+      <c r="EU81" s="60"/>
+      <c r="EV81" s="60"/>
+      <c r="EW81" s="60"/>
+      <c r="EX81" s="60"/>
+      <c r="EY81" s="60"/>
+      <c r="EZ81" s="60"/>
+      <c r="FA81" s="60"/>
+      <c r="FB81" s="60"/>
+      <c r="FC81" s="60"/>
+      <c r="FD81" s="60"/>
+      <c r="FE81" s="60"/>
+      <c r="FF81" s="60"/>
+      <c r="FG81" s="60"/>
+      <c r="FH81" s="60"/>
+      <c r="FI81" s="60"/>
+      <c r="FJ81" s="60"/>
+      <c r="FK81" s="60"/>
+      <c r="FL81" s="60"/>
+      <c r="FM81" s="60"/>
+      <c r="FN81" s="60"/>
+      <c r="FO81" s="60"/>
+      <c r="FP81" s="60"/>
+      <c r="FQ81" s="60"/>
+      <c r="FR81" s="60"/>
+      <c r="FS81" s="60"/>
+      <c r="FT81" s="60"/>
+      <c r="FU81" s="60"/>
+      <c r="FV81" s="60"/>
+      <c r="FW81" s="60"/>
+      <c r="FX81" s="60"/>
+      <c r="FY81" s="60"/>
+      <c r="FZ81" s="60"/>
+      <c r="GA81" s="60"/>
+      <c r="GB81" s="60"/>
+      <c r="GC81" s="60"/>
+      <c r="GD81" s="60"/>
+      <c r="GE81" s="60"/>
+      <c r="GF81" s="60"/>
+      <c r="GG81" s="60"/>
+      <c r="GH81" s="60"/>
+      <c r="GI81" s="60"/>
+      <c r="GJ81" s="60"/>
+      <c r="GK81" s="60"/>
+      <c r="GL81" s="60"/>
+      <c r="GM81" s="60"/>
+      <c r="GN81" s="60"/>
+      <c r="GO81" s="60"/>
+      <c r="GP81" s="60"/>
+      <c r="GQ81" s="60"/>
+      <c r="GR81" s="60"/>
+      <c r="GS81" s="60"/>
+      <c r="GT81" s="60"/>
+      <c r="GU81" s="60"/>
+      <c r="GV81" s="60"/>
+      <c r="GW81" s="60"/>
+      <c r="GX81" s="60"/>
+      <c r="GY81" s="60"/>
+      <c r="GZ81" s="60"/>
+      <c r="HA81" s="60"/>
+      <c r="HB81" s="60"/>
+      <c r="HC81" s="60"/>
+      <c r="HD81" s="60"/>
+      <c r="HE81" s="60"/>
+      <c r="HF81" s="60"/>
+      <c r="HG81" s="60"/>
+      <c r="HH81" s="60"/>
+      <c r="HI81" s="60"/>
+      <c r="HJ81" s="60"/>
+      <c r="HK81" s="60"/>
+      <c r="HL81" s="60"/>
+      <c r="HM81" s="60"/>
+      <c r="HN81" s="60"/>
+      <c r="HO81" s="60"/>
+      <c r="HP81" s="60"/>
+      <c r="HQ81" s="60"/>
+      <c r="HR81" s="60"/>
+      <c r="HS81" s="60"/>
+      <c r="HT81" s="60"/>
+      <c r="HU81" s="60"/>
+      <c r="HV81" s="60"/>
+      <c r="HW81" s="60"/>
+      <c r="HX81" s="60"/>
+      <c r="HY81" s="60"/>
+      <c r="HZ81" s="60"/>
+      <c r="IA81" s="60"/>
+      <c r="IB81" s="60"/>
+      <c r="IC81" s="60"/>
+      <c r="ID81" s="60"/>
+      <c r="IE81" s="60"/>
+      <c r="IF81" s="60"/>
+      <c r="IG81" s="60"/>
+      <c r="IH81" s="60"/>
+      <c r="II81" s="60"/>
+      <c r="IJ81" s="60"/>
+      <c r="IK81" s="60"/>
+      <c r="IL81" s="60"/>
+      <c r="IM81" s="60"/>
+      <c r="IN81" s="60"/>
+      <c r="IO81" s="60"/>
+      <c r="IP81" s="60"/>
+      <c r="IQ81" s="60"/>
+      <c r="IR81" s="60"/>
+      <c r="IS81" s="60"/>
+      <c r="IT81" s="60"/>
+      <c r="IU81" s="60"/>
+      <c r="IV81" s="60"/>
+      <c r="IW81" s="60"/>
+    </row>
+    <row r="82" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A82" s="58" t="s">
         <v>175</v>
-      </c>
-      <c r="B81" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C81" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="G81" s="58">
-        <v>0</v>
-      </c>
-      <c r="H81" s="58">
-        <v>1</v>
-      </c>
-      <c r="I81" s="58"/>
-      <c r="J81" s="58" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A82" s="58" t="s">
-        <v>177</v>
       </c>
       <c r="B82" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C82" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D82" s="58"/>
       <c r="E82" s="58" t="s">
@@ -15980,15 +16235,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="83" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A83" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B83" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D83" s="58"/>
       <c r="E83" s="58" t="s">
@@ -16008,15 +16263,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="84" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A84" s="58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B84" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D84" s="58"/>
       <c r="E84" s="58" t="s">
@@ -16036,15 +16291,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="85" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A85" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B85" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C85" s="58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D85" s="58"/>
       <c r="E85" s="58" t="s">
@@ -16064,15 +16319,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="86" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A86" s="58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B86" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C86" s="58" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D86" s="58"/>
       <c r="E86" s="58" t="s">
@@ -16092,15 +16347,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="87" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A87" s="58" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B87" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="58" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D87" s="58"/>
       <c r="E87" s="58" t="s">
@@ -16120,15 +16375,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="88" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A88" s="58" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B88" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C88" s="58" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D88" s="58"/>
       <c r="E88" s="58" t="s">
@@ -16148,15 +16403,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="89" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A89" s="58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B89" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C89" s="58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D89" s="58"/>
       <c r="E89" s="58" t="s">
@@ -16176,15 +16431,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="90" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A90" s="58" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B90" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C90" s="58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D90" s="58"/>
       <c r="E90" s="58" t="s">
@@ -16204,15 +16459,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="91" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A91" s="58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B91" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="58" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D91" s="58"/>
       <c r="E91" s="58" t="s">
@@ -16232,15 +16487,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="92" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A92" s="58" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B92" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="58" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D92" s="58"/>
       <c r="E92" s="58" t="s">
@@ -16260,15 +16515,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="93" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A93" s="58" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B93" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C93" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D93" s="58"/>
       <c r="E93" s="58" t="s">
@@ -16285,18 +16540,18 @@
       </c>
       <c r="I93" s="58"/>
       <c r="J93" s="58" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="18" customHeight="1">
+    <row r="94" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A94" s="58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B94" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="58" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D94" s="58"/>
       <c r="E94" s="58" t="s">
@@ -16316,15 +16571,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="95" spans="1:257" ht="18" customHeight="1">
       <c r="A95" s="58" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B95" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C95" s="58" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D95" s="58"/>
       <c r="E95" s="58" t="s">
@@ -16344,15 +16599,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="96" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A96" s="58" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B96" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C96" s="58" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D96" s="58"/>
       <c r="E96" s="58" t="s">
@@ -16374,13 +16629,13 @@
     </row>
     <row r="97" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A97" s="58" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B97" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C97" s="58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D97" s="58"/>
       <c r="E97" s="58" t="s">
@@ -16401,20 +16656,20 @@
       </c>
     </row>
     <row r="98" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A98" s="95" t="s">
-        <v>210</v>
-      </c>
-      <c r="B98" s="95" t="s">
+      <c r="A98" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="B98" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="95" t="s">
-        <v>211</v>
+      <c r="C98" s="58" t="s">
+        <v>208</v>
       </c>
       <c r="D98" s="58"/>
-      <c r="E98" s="95" t="s">
+      <c r="E98" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F98" s="95" t="s">
+      <c r="F98" s="58" t="s">
         <v>13</v>
       </c>
       <c r="G98" s="58">
@@ -16423,22 +16678,20 @@
       <c r="H98" s="58">
         <v>1</v>
       </c>
-      <c r="I98" s="95" t="s">
-        <v>174</v>
-      </c>
-      <c r="J98" s="95" t="s">
-        <v>15</v>
+      <c r="I98" s="58"/>
+      <c r="J98" s="58" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A99" s="95" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B99" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C99" s="95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D99" s="58"/>
       <c r="E99" s="95" t="s">
@@ -16457,18 +16710,18 @@
         <v>174</v>
       </c>
       <c r="J99" s="95" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A100" s="95" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B100" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C100" s="95" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D100" s="58"/>
       <c r="E100" s="95" t="s">
@@ -16487,18 +16740,18 @@
         <v>174</v>
       </c>
       <c r="J100" s="95" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A101" s="95" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B101" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C101" s="95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D101" s="58"/>
       <c r="E101" s="95" t="s">
@@ -16517,18 +16770,18 @@
         <v>174</v>
       </c>
       <c r="J101" s="95" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="95" t="s">
-        <v>219</v>
-      </c>
-      <c r="B102" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B102" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C102" s="95" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D102" s="58"/>
       <c r="E102" s="95" t="s">
@@ -16547,18 +16800,18 @@
         <v>174</v>
       </c>
       <c r="J102" s="95" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="95" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B103" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C103" s="95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D103" s="58"/>
       <c r="E103" s="95" t="s">
@@ -16582,13 +16835,13 @@
     </row>
     <row r="104" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="95" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B104" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="95" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D104" s="58"/>
       <c r="E104" s="95" t="s">
@@ -16611,293 +16864,48 @@
       </c>
     </row>
     <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A105" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="B105" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="C105" s="85" t="s">
-        <v>78</v>
+      <c r="A105" s="95" t="s">
+        <v>221</v>
+      </c>
+      <c r="B105" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105" s="95" t="s">
+        <v>222</v>
       </c>
       <c r="D105" s="58"/>
-      <c r="E105" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="F105" s="76" t="s">
+      <c r="E105" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="G105" s="25">
-        <v>0</v>
-      </c>
-      <c r="H105" s="25">
+      <c r="G105" s="58">
+        <v>0</v>
+      </c>
+      <c r="H105" s="58">
         <v>1</v>
       </c>
-      <c r="I105" s="10"/>
-      <c r="J105" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K105"/>
-      <c r="L105"/>
-      <c r="M105"/>
-      <c r="N105"/>
-      <c r="O105"/>
-      <c r="P105"/>
-      <c r="Q105"/>
-      <c r="R105"/>
-      <c r="S105"/>
-      <c r="T105"/>
-      <c r="U105"/>
-      <c r="V105"/>
-      <c r="W105"/>
-      <c r="X105"/>
-      <c r="Y105"/>
-      <c r="Z105"/>
-      <c r="AA105"/>
-      <c r="AB105"/>
-      <c r="AC105"/>
-      <c r="AD105"/>
-      <c r="AE105"/>
-      <c r="AF105"/>
-      <c r="AG105"/>
-      <c r="AH105"/>
-      <c r="AI105"/>
-      <c r="AJ105"/>
-      <c r="AK105"/>
-      <c r="AL105"/>
-      <c r="AM105"/>
-      <c r="AN105"/>
-      <c r="AO105"/>
-      <c r="AP105"/>
-      <c r="AQ105"/>
-      <c r="AR105"/>
-      <c r="AS105"/>
-      <c r="AT105"/>
-      <c r="AU105"/>
-      <c r="AV105"/>
-      <c r="AW105"/>
-      <c r="AX105"/>
-      <c r="AY105"/>
-      <c r="AZ105"/>
-      <c r="BA105"/>
-      <c r="BB105"/>
-      <c r="BC105"/>
-      <c r="BD105"/>
-      <c r="BE105"/>
-      <c r="BF105"/>
-      <c r="BG105"/>
-      <c r="BH105"/>
-      <c r="BI105"/>
-      <c r="BJ105"/>
-      <c r="BK105"/>
-      <c r="BL105"/>
-      <c r="BM105"/>
-      <c r="BN105"/>
-      <c r="BO105"/>
-      <c r="BP105"/>
-      <c r="BQ105"/>
-      <c r="BR105"/>
-      <c r="BS105"/>
-      <c r="BT105"/>
-      <c r="BU105"/>
-      <c r="BV105"/>
-      <c r="BW105"/>
-      <c r="BX105"/>
-      <c r="BY105"/>
-      <c r="BZ105"/>
-      <c r="CA105"/>
-      <c r="CB105"/>
-      <c r="CC105"/>
-      <c r="CD105"/>
-      <c r="CE105"/>
-      <c r="CF105"/>
-      <c r="CG105"/>
-      <c r="CH105"/>
-      <c r="CI105"/>
-      <c r="CJ105"/>
-      <c r="CK105"/>
-      <c r="CL105"/>
-      <c r="CM105"/>
-      <c r="CN105"/>
-      <c r="CO105"/>
-      <c r="CP105"/>
-      <c r="CQ105"/>
-      <c r="CR105"/>
-      <c r="CS105"/>
-      <c r="CT105"/>
-      <c r="CU105"/>
-      <c r="CV105"/>
-      <c r="CW105"/>
-      <c r="CX105"/>
-      <c r="CY105"/>
-      <c r="CZ105"/>
-      <c r="DA105"/>
-      <c r="DB105"/>
-      <c r="DC105"/>
-      <c r="DD105"/>
-      <c r="DE105"/>
-      <c r="DF105"/>
-      <c r="DG105"/>
-      <c r="DH105"/>
-      <c r="DI105"/>
-      <c r="DJ105"/>
-      <c r="DK105"/>
-      <c r="DL105"/>
-      <c r="DM105"/>
-      <c r="DN105"/>
-      <c r="DO105"/>
-      <c r="DP105"/>
-      <c r="DQ105"/>
-      <c r="DR105"/>
-      <c r="DS105"/>
-      <c r="DT105"/>
-      <c r="DU105"/>
-      <c r="DV105"/>
-      <c r="DW105"/>
-      <c r="DX105"/>
-      <c r="DY105"/>
-      <c r="DZ105"/>
-      <c r="EA105"/>
-      <c r="EB105"/>
-      <c r="EC105"/>
-      <c r="ED105"/>
-      <c r="EE105"/>
-      <c r="EF105"/>
-      <c r="EG105"/>
-      <c r="EH105"/>
-      <c r="EI105"/>
-      <c r="EJ105"/>
-      <c r="EK105"/>
-      <c r="EL105"/>
-      <c r="EM105"/>
-      <c r="EN105"/>
-      <c r="EO105"/>
-      <c r="EP105"/>
-      <c r="EQ105"/>
-      <c r="ER105"/>
-      <c r="ES105"/>
-      <c r="ET105"/>
-      <c r="EU105"/>
-      <c r="EV105"/>
-      <c r="EW105"/>
-      <c r="EX105"/>
-      <c r="EY105"/>
-      <c r="EZ105"/>
-      <c r="FA105"/>
-      <c r="FB105"/>
-      <c r="FC105"/>
-      <c r="FD105"/>
-      <c r="FE105"/>
-      <c r="FF105"/>
-      <c r="FG105"/>
-      <c r="FH105"/>
-      <c r="FI105"/>
-      <c r="FJ105"/>
-      <c r="FK105"/>
-      <c r="FL105"/>
-      <c r="FM105"/>
-      <c r="FN105"/>
-      <c r="FO105"/>
-      <c r="FP105"/>
-      <c r="FQ105"/>
-      <c r="FR105"/>
-      <c r="FS105"/>
-      <c r="FT105"/>
-      <c r="FU105"/>
-      <c r="FV105"/>
-      <c r="FW105"/>
-      <c r="FX105"/>
-      <c r="FY105"/>
-      <c r="FZ105"/>
-      <c r="GA105"/>
-      <c r="GB105"/>
-      <c r="GC105"/>
-      <c r="GD105"/>
-      <c r="GE105"/>
-      <c r="GF105"/>
-      <c r="GG105"/>
-      <c r="GH105"/>
-      <c r="GI105"/>
-      <c r="GJ105"/>
-      <c r="GK105"/>
-      <c r="GL105"/>
-      <c r="GM105"/>
-      <c r="GN105"/>
-      <c r="GO105"/>
-      <c r="GP105"/>
-      <c r="GQ105"/>
-      <c r="GR105"/>
-      <c r="GS105"/>
-      <c r="GT105"/>
-      <c r="GU105"/>
-      <c r="GV105"/>
-      <c r="GW105"/>
-      <c r="GX105"/>
-      <c r="GY105"/>
-      <c r="GZ105"/>
-      <c r="HA105"/>
-      <c r="HB105"/>
-      <c r="HC105"/>
-      <c r="HD105"/>
-      <c r="HE105"/>
-      <c r="HF105"/>
-      <c r="HG105"/>
-      <c r="HH105"/>
-      <c r="HI105"/>
-      <c r="HJ105"/>
-      <c r="HK105"/>
-      <c r="HL105"/>
-      <c r="HM105"/>
-      <c r="HN105"/>
-      <c r="HO105"/>
-      <c r="HP105"/>
-      <c r="HQ105"/>
-      <c r="HR105"/>
-      <c r="HS105"/>
-      <c r="HT105"/>
-      <c r="HU105"/>
-      <c r="HV105"/>
-      <c r="HW105"/>
-      <c r="HX105"/>
-      <c r="HY105"/>
-      <c r="HZ105"/>
-      <c r="IA105"/>
-      <c r="IB105"/>
-      <c r="IC105"/>
-      <c r="ID105"/>
-      <c r="IE105"/>
-      <c r="IF105"/>
-      <c r="IG105"/>
-      <c r="IH105"/>
-      <c r="II105"/>
-      <c r="IJ105"/>
-      <c r="IK105"/>
-      <c r="IL105"/>
-      <c r="IM105"/>
-      <c r="IN105"/>
-      <c r="IO105"/>
-      <c r="IP105"/>
-      <c r="IQ105"/>
-      <c r="IR105"/>
-      <c r="IS105"/>
-      <c r="IT105"/>
-      <c r="IU105"/>
-      <c r="IV105"/>
-      <c r="IW105"/>
+      <c r="I105" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="J105" s="95" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A106" s="19" t="s">
         <v>224</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>120</v>
+        <v>223</v>
       </c>
       <c r="C106" s="85" t="s">
         <v>78</v>
       </c>
       <c r="D106" s="58"/>
       <c r="E106" s="76" t="s">
-        <v>120</v>
+        <v>223</v>
       </c>
       <c r="F106" s="76" t="s">
         <v>13</v>
@@ -17161,44 +17169,289 @@
       <c r="IW106"/>
     </row>
     <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A107" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B107" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C107" s="58" t="s">
-        <v>233</v>
+      <c r="A107" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C107" s="85" t="s">
+        <v>78</v>
       </c>
       <c r="D107" s="58"/>
-      <c r="E107" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="F107" s="96" t="s">
+      <c r="E107" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F107" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G107" s="25">
         <v>0</v>
       </c>
-      <c r="H107" s="97">
+      <c r="H107" s="25">
         <v>1</v>
       </c>
-      <c r="I107" s="96" t="s">
-        <v>174</v>
-      </c>
-      <c r="J107" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I107" s="10"/>
+      <c r="J107" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K107"/>
+      <c r="L107"/>
+      <c r="M107"/>
+      <c r="N107"/>
+      <c r="O107"/>
+      <c r="P107"/>
+      <c r="Q107"/>
+      <c r="R107"/>
+      <c r="S107"/>
+      <c r="T107"/>
+      <c r="U107"/>
+      <c r="V107"/>
+      <c r="W107"/>
+      <c r="X107"/>
+      <c r="Y107"/>
+      <c r="Z107"/>
+      <c r="AA107"/>
+      <c r="AB107"/>
+      <c r="AC107"/>
+      <c r="AD107"/>
+      <c r="AE107"/>
+      <c r="AF107"/>
+      <c r="AG107"/>
+      <c r="AH107"/>
+      <c r="AI107"/>
+      <c r="AJ107"/>
+      <c r="AK107"/>
+      <c r="AL107"/>
+      <c r="AM107"/>
+      <c r="AN107"/>
+      <c r="AO107"/>
+      <c r="AP107"/>
+      <c r="AQ107"/>
+      <c r="AR107"/>
+      <c r="AS107"/>
+      <c r="AT107"/>
+      <c r="AU107"/>
+      <c r="AV107"/>
+      <c r="AW107"/>
+      <c r="AX107"/>
+      <c r="AY107"/>
+      <c r="AZ107"/>
+      <c r="BA107"/>
+      <c r="BB107"/>
+      <c r="BC107"/>
+      <c r="BD107"/>
+      <c r="BE107"/>
+      <c r="BF107"/>
+      <c r="BG107"/>
+      <c r="BH107"/>
+      <c r="BI107"/>
+      <c r="BJ107"/>
+      <c r="BK107"/>
+      <c r="BL107"/>
+      <c r="BM107"/>
+      <c r="BN107"/>
+      <c r="BO107"/>
+      <c r="BP107"/>
+      <c r="BQ107"/>
+      <c r="BR107"/>
+      <c r="BS107"/>
+      <c r="BT107"/>
+      <c r="BU107"/>
+      <c r="BV107"/>
+      <c r="BW107"/>
+      <c r="BX107"/>
+      <c r="BY107"/>
+      <c r="BZ107"/>
+      <c r="CA107"/>
+      <c r="CB107"/>
+      <c r="CC107"/>
+      <c r="CD107"/>
+      <c r="CE107"/>
+      <c r="CF107"/>
+      <c r="CG107"/>
+      <c r="CH107"/>
+      <c r="CI107"/>
+      <c r="CJ107"/>
+      <c r="CK107"/>
+      <c r="CL107"/>
+      <c r="CM107"/>
+      <c r="CN107"/>
+      <c r="CO107"/>
+      <c r="CP107"/>
+      <c r="CQ107"/>
+      <c r="CR107"/>
+      <c r="CS107"/>
+      <c r="CT107"/>
+      <c r="CU107"/>
+      <c r="CV107"/>
+      <c r="CW107"/>
+      <c r="CX107"/>
+      <c r="CY107"/>
+      <c r="CZ107"/>
+      <c r="DA107"/>
+      <c r="DB107"/>
+      <c r="DC107"/>
+      <c r="DD107"/>
+      <c r="DE107"/>
+      <c r="DF107"/>
+      <c r="DG107"/>
+      <c r="DH107"/>
+      <c r="DI107"/>
+      <c r="DJ107"/>
+      <c r="DK107"/>
+      <c r="DL107"/>
+      <c r="DM107"/>
+      <c r="DN107"/>
+      <c r="DO107"/>
+      <c r="DP107"/>
+      <c r="DQ107"/>
+      <c r="DR107"/>
+      <c r="DS107"/>
+      <c r="DT107"/>
+      <c r="DU107"/>
+      <c r="DV107"/>
+      <c r="DW107"/>
+      <c r="DX107"/>
+      <c r="DY107"/>
+      <c r="DZ107"/>
+      <c r="EA107"/>
+      <c r="EB107"/>
+      <c r="EC107"/>
+      <c r="ED107"/>
+      <c r="EE107"/>
+      <c r="EF107"/>
+      <c r="EG107"/>
+      <c r="EH107"/>
+      <c r="EI107"/>
+      <c r="EJ107"/>
+      <c r="EK107"/>
+      <c r="EL107"/>
+      <c r="EM107"/>
+      <c r="EN107"/>
+      <c r="EO107"/>
+      <c r="EP107"/>
+      <c r="EQ107"/>
+      <c r="ER107"/>
+      <c r="ES107"/>
+      <c r="ET107"/>
+      <c r="EU107"/>
+      <c r="EV107"/>
+      <c r="EW107"/>
+      <c r="EX107"/>
+      <c r="EY107"/>
+      <c r="EZ107"/>
+      <c r="FA107"/>
+      <c r="FB107"/>
+      <c r="FC107"/>
+      <c r="FD107"/>
+      <c r="FE107"/>
+      <c r="FF107"/>
+      <c r="FG107"/>
+      <c r="FH107"/>
+      <c r="FI107"/>
+      <c r="FJ107"/>
+      <c r="FK107"/>
+      <c r="FL107"/>
+      <c r="FM107"/>
+      <c r="FN107"/>
+      <c r="FO107"/>
+      <c r="FP107"/>
+      <c r="FQ107"/>
+      <c r="FR107"/>
+      <c r="FS107"/>
+      <c r="FT107"/>
+      <c r="FU107"/>
+      <c r="FV107"/>
+      <c r="FW107"/>
+      <c r="FX107"/>
+      <c r="FY107"/>
+      <c r="FZ107"/>
+      <c r="GA107"/>
+      <c r="GB107"/>
+      <c r="GC107"/>
+      <c r="GD107"/>
+      <c r="GE107"/>
+      <c r="GF107"/>
+      <c r="GG107"/>
+      <c r="GH107"/>
+      <c r="GI107"/>
+      <c r="GJ107"/>
+      <c r="GK107"/>
+      <c r="GL107"/>
+      <c r="GM107"/>
+      <c r="GN107"/>
+      <c r="GO107"/>
+      <c r="GP107"/>
+      <c r="GQ107"/>
+      <c r="GR107"/>
+      <c r="GS107"/>
+      <c r="GT107"/>
+      <c r="GU107"/>
+      <c r="GV107"/>
+      <c r="GW107"/>
+      <c r="GX107"/>
+      <c r="GY107"/>
+      <c r="GZ107"/>
+      <c r="HA107"/>
+      <c r="HB107"/>
+      <c r="HC107"/>
+      <c r="HD107"/>
+      <c r="HE107"/>
+      <c r="HF107"/>
+      <c r="HG107"/>
+      <c r="HH107"/>
+      <c r="HI107"/>
+      <c r="HJ107"/>
+      <c r="HK107"/>
+      <c r="HL107"/>
+      <c r="HM107"/>
+      <c r="HN107"/>
+      <c r="HO107"/>
+      <c r="HP107"/>
+      <c r="HQ107"/>
+      <c r="HR107"/>
+      <c r="HS107"/>
+      <c r="HT107"/>
+      <c r="HU107"/>
+      <c r="HV107"/>
+      <c r="HW107"/>
+      <c r="HX107"/>
+      <c r="HY107"/>
+      <c r="HZ107"/>
+      <c r="IA107"/>
+      <c r="IB107"/>
+      <c r="IC107"/>
+      <c r="ID107"/>
+      <c r="IE107"/>
+      <c r="IF107"/>
+      <c r="IG107"/>
+      <c r="IH107"/>
+      <c r="II107"/>
+      <c r="IJ107"/>
+      <c r="IK107"/>
+      <c r="IL107"/>
+      <c r="IM107"/>
+      <c r="IN107"/>
+      <c r="IO107"/>
+      <c r="IP107"/>
+      <c r="IQ107"/>
+      <c r="IR107"/>
+      <c r="IS107"/>
+      <c r="IT107"/>
+      <c r="IU107"/>
+      <c r="IV107"/>
+      <c r="IW107"/>
     </row>
     <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B108" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C108" s="58" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D108" s="58"/>
       <c r="E108" s="96" t="s">
@@ -17210,7 +17463,7 @@
       <c r="G108" s="25">
         <v>0</v>
       </c>
-      <c r="H108" s="58">
+      <c r="H108" s="97">
         <v>1</v>
       </c>
       <c r="I108" s="96" t="s">
@@ -17222,13 +17475,13 @@
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B109" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C109" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="96" t="s">
@@ -17252,13 +17505,13 @@
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B110" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C110" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D110" s="58"/>
       <c r="E110" s="96" t="s">
@@ -17282,13 +17535,13 @@
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="B111" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C111" s="58" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
@@ -17298,7 +17551,7 @@
         <v>13</v>
       </c>
       <c r="G111" s="25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H111" s="58">
         <v>1</v>
@@ -17312,13 +17565,13 @@
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="B112" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
@@ -17328,7 +17581,7 @@
         <v>13</v>
       </c>
       <c r="G112" s="25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H112" s="58">
         <v>1</v>
@@ -17342,13 +17595,13 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B113" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
@@ -17372,13 +17625,13 @@
     </row>
     <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="B114" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
@@ -17402,13 +17655,13 @@
     </row>
     <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B115" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="C115" s="95" t="s">
-        <v>242</v>
+      <c r="C115" s="58" t="s">
+        <v>239</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
@@ -17432,13 +17685,13 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="B116" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C116" s="95" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
@@ -17462,13 +17715,13 @@
     </row>
     <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="B117" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="C117" s="58" t="s">
-        <v>241</v>
+      <c r="C117" s="95" t="s">
+        <v>245</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
@@ -17492,13 +17745,13 @@
     </row>
     <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B118" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C118" s="58" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
@@ -17522,13 +17775,13 @@
     </row>
     <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="B119" s="58" t="s">
         <v>232</v>
       </c>
       <c r="C119" s="58" t="s">
-        <v>168</v>
+        <v>247</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
@@ -17550,7 +17803,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A120" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B120" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C120" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D120" s="58"/>
+      <c r="E120" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F120" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G120" s="25">
+        <v>0</v>
+      </c>
+      <c r="H120" s="58">
+        <v>1</v>
+      </c>
+      <c r="I120" s="96" t="s">
+        <v>174</v>
+      </c>
+      <c r="J120" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="123" spans="1:10" ht="17.100000000000001" customHeight="1"/>
@@ -17564,6 +17846,7 @@
     <row r="131" ht="17.100000000000001" customHeight="1"/>
     <row r="132" ht="17.100000000000001" customHeight="1"/>
     <row r="133" ht="17.100000000000001" customHeight="1"/>
+    <row r="134" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated field settings for service deliveries
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44792CE5-0415-4FD1-9DDC-EBD00E61EB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C0492E-3113-4C4A-8765-7BE79A7138FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31770" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="257">
   <si>
     <t>name</t>
   </si>
@@ -493,9 +493,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>service_deliveries</t>
-  </si>
-  <si>
     <t>service_provided</t>
   </si>
   <si>
@@ -782,6 +779,24 @@
   </si>
   <si>
     <t>Task Completed Date</t>
+  </si>
+  <si>
+    <t>service_received</t>
+  </si>
+  <si>
+    <t>Service Received</t>
+  </si>
+  <si>
+    <t>done_by</t>
+  </si>
+  <si>
+    <t>Done by</t>
+  </si>
+  <si>
+    <t>manage</t>
+  </si>
+  <si>
+    <t>Manage</t>
   </si>
 </sst>
 </file>
@@ -1690,10 +1705,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW134"/>
+  <dimension ref="A1:IW137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2035,7 +2050,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D12" s="58"/>
       <c r="E12" s="11" t="s">
@@ -11780,14 +11795,14 @@
         <v>143</v>
       </c>
       <c r="B66" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C66" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D66" s="63"/>
       <c r="E66" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F66" s="63" t="s">
         <v>13</v>
@@ -11799,7 +11814,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J66" s="63" t="s">
         <v>15</v>
@@ -12057,14 +12072,14 @@
         <v>144</v>
       </c>
       <c r="B67" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C67" s="63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D67" s="63"/>
       <c r="E67" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F67" s="63" t="s">
         <v>13</v>
@@ -12076,7 +12091,7 @@
         <v>1</v>
       </c>
       <c r="I67" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J67" s="63" t="s">
         <v>15</v>
@@ -12334,14 +12349,14 @@
         <v>145</v>
       </c>
       <c r="B68" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C68" s="63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" s="63"/>
       <c r="E68" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F68" s="63" t="s">
         <v>13</v>
@@ -12353,7 +12368,7 @@
         <v>1</v>
       </c>
       <c r="I68" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J68" s="63" t="s">
         <v>15</v>
@@ -12611,14 +12626,14 @@
         <v>146</v>
       </c>
       <c r="B69" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C69" s="63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D69" s="63"/>
       <c r="E69" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F69" s="63" t="s">
         <v>13</v>
@@ -12630,7 +12645,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J69" s="63" t="s">
         <v>15</v>
@@ -12888,14 +12903,14 @@
         <v>147</v>
       </c>
       <c r="B70" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C70" s="63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D70" s="63"/>
       <c r="E70" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F70" s="63" t="s">
         <v>13</v>
@@ -12907,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="I70" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J70" s="63" t="s">
         <v>15</v>
@@ -13165,14 +13180,14 @@
         <v>148</v>
       </c>
       <c r="B71" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C71" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D71" s="63"/>
       <c r="E71" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F71" s="63" t="s">
         <v>13</v>
@@ -13184,7 +13199,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J71" s="63" t="s">
         <v>15</v>
@@ -13442,14 +13457,14 @@
         <v>149</v>
       </c>
       <c r="B72" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C72" s="63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D72" s="63"/>
       <c r="E72" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F72" s="63" t="s">
         <v>13</v>
@@ -13461,7 +13476,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J72" s="94" t="s">
         <v>3</v>
@@ -13719,14 +13734,14 @@
         <v>150</v>
       </c>
       <c r="B73" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C73" s="63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D73" s="63"/>
       <c r="E73" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F73" s="63" t="s">
         <v>13</v>
@@ -13738,7 +13753,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J73" s="63" t="s">
         <v>15</v>
@@ -13996,14 +14011,14 @@
         <v>151</v>
       </c>
       <c r="B74" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C74" s="63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D74" s="63"/>
       <c r="E74" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F74" s="63" t="s">
         <v>13</v>
@@ -14015,7 +14030,7 @@
         <v>1</v>
       </c>
       <c r="I74" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J74" s="94" t="s">
         <v>3</v>
@@ -14273,14 +14288,14 @@
         <v>152</v>
       </c>
       <c r="B75" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C75" s="63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D75" s="63"/>
       <c r="E75" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F75" s="63" t="s">
         <v>13</v>
@@ -14292,7 +14307,7 @@
         <v>1</v>
       </c>
       <c r="I75" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J75" s="63" t="s">
         <v>15</v>
@@ -14550,14 +14565,14 @@
         <v>153</v>
       </c>
       <c r="B76" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C76" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D76" s="59"/>
       <c r="E76" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F76" s="59" t="s">
         <v>13</v>
@@ -14569,7 +14584,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J76" s="59" t="s">
         <v>15</v>
@@ -14827,14 +14842,14 @@
         <v>154</v>
       </c>
       <c r="B77" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C77" s="59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D77" s="59"/>
       <c r="E77" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F77" s="59" t="s">
         <v>13</v>
@@ -14846,7 +14861,7 @@
         <v>1</v>
       </c>
       <c r="I77" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J77" s="59" t="s">
         <v>15</v>
@@ -15104,14 +15119,14 @@
         <v>143</v>
       </c>
       <c r="B78" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="59" t="s">
         <v>158</v>
-      </c>
-      <c r="C78" s="59" t="s">
-        <v>159</v>
       </c>
       <c r="D78" s="59"/>
       <c r="E78" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F78" s="59" t="s">
         <v>13</v>
@@ -15123,7 +15138,7 @@
         <v>1</v>
       </c>
       <c r="I78" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J78" s="59" t="s">
         <v>15</v>
@@ -15378,17 +15393,17 @@
     </row>
     <row r="79" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A79" s="59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B79" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C79" s="59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D79" s="59"/>
       <c r="E79" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F79" s="59" t="s">
         <v>13</v>
@@ -15400,7 +15415,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J79" s="59" t="s">
         <v>15</v>
@@ -15655,17 +15670,17 @@
     </row>
     <row r="80" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A80" s="59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B80" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C80" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D80" s="59"/>
       <c r="E80" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F80" s="59" t="s">
         <v>13</v>
@@ -15677,7 +15692,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J80" s="59" t="s">
         <v>15</v>
@@ -15932,17 +15947,17 @@
     </row>
     <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="59" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B81" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C81" s="59" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D81" s="59"/>
       <c r="E81" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F81" s="59" t="s">
         <v>13</v>
@@ -15954,7 +15969,7 @@
         <v>1</v>
       </c>
       <c r="I81" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J81" s="59" t="s">
         <v>15</v>
@@ -16207,99 +16222,846 @@
       <c r="IV81" s="60"/>
       <c r="IW81" s="60"/>
     </row>
-    <row r="82" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A82" s="58" t="s">
-        <v>175</v>
-      </c>
-      <c r="B82" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C82" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="58" t="s">
+    <row r="82" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A82" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="B82" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="D82" s="59"/>
+      <c r="E82" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="F82" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G82" s="58">
+      <c r="G82" s="59">
         <v>0</v>
       </c>
-      <c r="H82" s="58">
+      <c r="H82" s="59">
         <v>1</v>
       </c>
-      <c r="I82" s="58"/>
-      <c r="J82" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="I82" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="J82" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K82" s="60"/>
+      <c r="L82" s="60"/>
+      <c r="M82" s="60"/>
+      <c r="N82" s="60"/>
+      <c r="O82" s="60"/>
+      <c r="P82" s="60"/>
+      <c r="Q82" s="60"/>
+      <c r="R82" s="60"/>
+      <c r="S82" s="60"/>
+      <c r="T82" s="60"/>
+      <c r="U82" s="60"/>
+      <c r="V82" s="60"/>
+      <c r="W82" s="60"/>
+      <c r="X82" s="60"/>
+      <c r="Y82" s="60"/>
+      <c r="Z82" s="60"/>
+      <c r="AA82" s="60"/>
+      <c r="AB82" s="60"/>
+      <c r="AC82" s="60"/>
+      <c r="AD82" s="60"/>
+      <c r="AE82" s="60"/>
+      <c r="AF82" s="60"/>
+      <c r="AG82" s="60"/>
+      <c r="AH82" s="60"/>
+      <c r="AI82" s="60"/>
+      <c r="AJ82" s="60"/>
+      <c r="AK82" s="60"/>
+      <c r="AL82" s="60"/>
+      <c r="AM82" s="60"/>
+      <c r="AN82" s="60"/>
+      <c r="AO82" s="60"/>
+      <c r="AP82" s="60"/>
+      <c r="AQ82" s="60"/>
+      <c r="AR82" s="60"/>
+      <c r="AS82" s="60"/>
+      <c r="AT82" s="60"/>
+      <c r="AU82" s="60"/>
+      <c r="AV82" s="60"/>
+      <c r="AW82" s="60"/>
+      <c r="AX82" s="60"/>
+      <c r="AY82" s="60"/>
+      <c r="AZ82" s="60"/>
+      <c r="BA82" s="60"/>
+      <c r="BB82" s="60"/>
+      <c r="BC82" s="60"/>
+      <c r="BD82" s="60"/>
+      <c r="BE82" s="60"/>
+      <c r="BF82" s="60"/>
+      <c r="BG82" s="60"/>
+      <c r="BH82" s="60"/>
+      <c r="BI82" s="60"/>
+      <c r="BJ82" s="60"/>
+      <c r="BK82" s="60"/>
+      <c r="BL82" s="60"/>
+      <c r="BM82" s="60"/>
+      <c r="BN82" s="60"/>
+      <c r="BO82" s="60"/>
+      <c r="BP82" s="60"/>
+      <c r="BQ82" s="60"/>
+      <c r="BR82" s="60"/>
+      <c r="BS82" s="60"/>
+      <c r="BT82" s="60"/>
+      <c r="BU82" s="60"/>
+      <c r="BV82" s="60"/>
+      <c r="BW82" s="60"/>
+      <c r="BX82" s="60"/>
+      <c r="BY82" s="60"/>
+      <c r="BZ82" s="60"/>
+      <c r="CA82" s="60"/>
+      <c r="CB82" s="60"/>
+      <c r="CC82" s="60"/>
+      <c r="CD82" s="60"/>
+      <c r="CE82" s="60"/>
+      <c r="CF82" s="60"/>
+      <c r="CG82" s="60"/>
+      <c r="CH82" s="60"/>
+      <c r="CI82" s="60"/>
+      <c r="CJ82" s="60"/>
+      <c r="CK82" s="60"/>
+      <c r="CL82" s="60"/>
+      <c r="CM82" s="60"/>
+      <c r="CN82" s="60"/>
+      <c r="CO82" s="60"/>
+      <c r="CP82" s="60"/>
+      <c r="CQ82" s="60"/>
+      <c r="CR82" s="60"/>
+      <c r="CS82" s="60"/>
+      <c r="CT82" s="60"/>
+      <c r="CU82" s="60"/>
+      <c r="CV82" s="60"/>
+      <c r="CW82" s="60"/>
+      <c r="CX82" s="60"/>
+      <c r="CY82" s="60"/>
+      <c r="CZ82" s="60"/>
+      <c r="DA82" s="60"/>
+      <c r="DB82" s="60"/>
+      <c r="DC82" s="60"/>
+      <c r="DD82" s="60"/>
+      <c r="DE82" s="60"/>
+      <c r="DF82" s="60"/>
+      <c r="DG82" s="60"/>
+      <c r="DH82" s="60"/>
+      <c r="DI82" s="60"/>
+      <c r="DJ82" s="60"/>
+      <c r="DK82" s="60"/>
+      <c r="DL82" s="60"/>
+      <c r="DM82" s="60"/>
+      <c r="DN82" s="60"/>
+      <c r="DO82" s="60"/>
+      <c r="DP82" s="60"/>
+      <c r="DQ82" s="60"/>
+      <c r="DR82" s="60"/>
+      <c r="DS82" s="60"/>
+      <c r="DT82" s="60"/>
+      <c r="DU82" s="60"/>
+      <c r="DV82" s="60"/>
+      <c r="DW82" s="60"/>
+      <c r="DX82" s="60"/>
+      <c r="DY82" s="60"/>
+      <c r="DZ82" s="60"/>
+      <c r="EA82" s="60"/>
+      <c r="EB82" s="60"/>
+      <c r="EC82" s="60"/>
+      <c r="ED82" s="60"/>
+      <c r="EE82" s="60"/>
+      <c r="EF82" s="60"/>
+      <c r="EG82" s="60"/>
+      <c r="EH82" s="60"/>
+      <c r="EI82" s="60"/>
+      <c r="EJ82" s="60"/>
+      <c r="EK82" s="60"/>
+      <c r="EL82" s="60"/>
+      <c r="EM82" s="60"/>
+      <c r="EN82" s="60"/>
+      <c r="EO82" s="60"/>
+      <c r="EP82" s="60"/>
+      <c r="EQ82" s="60"/>
+      <c r="ER82" s="60"/>
+      <c r="ES82" s="60"/>
+      <c r="ET82" s="60"/>
+      <c r="EU82" s="60"/>
+      <c r="EV82" s="60"/>
+      <c r="EW82" s="60"/>
+      <c r="EX82" s="60"/>
+      <c r="EY82" s="60"/>
+      <c r="EZ82" s="60"/>
+      <c r="FA82" s="60"/>
+      <c r="FB82" s="60"/>
+      <c r="FC82" s="60"/>
+      <c r="FD82" s="60"/>
+      <c r="FE82" s="60"/>
+      <c r="FF82" s="60"/>
+      <c r="FG82" s="60"/>
+      <c r="FH82" s="60"/>
+      <c r="FI82" s="60"/>
+      <c r="FJ82" s="60"/>
+      <c r="FK82" s="60"/>
+      <c r="FL82" s="60"/>
+      <c r="FM82" s="60"/>
+      <c r="FN82" s="60"/>
+      <c r="FO82" s="60"/>
+      <c r="FP82" s="60"/>
+      <c r="FQ82" s="60"/>
+      <c r="FR82" s="60"/>
+      <c r="FS82" s="60"/>
+      <c r="FT82" s="60"/>
+      <c r="FU82" s="60"/>
+      <c r="FV82" s="60"/>
+      <c r="FW82" s="60"/>
+      <c r="FX82" s="60"/>
+      <c r="FY82" s="60"/>
+      <c r="FZ82" s="60"/>
+      <c r="GA82" s="60"/>
+      <c r="GB82" s="60"/>
+      <c r="GC82" s="60"/>
+      <c r="GD82" s="60"/>
+      <c r="GE82" s="60"/>
+      <c r="GF82" s="60"/>
+      <c r="GG82" s="60"/>
+      <c r="GH82" s="60"/>
+      <c r="GI82" s="60"/>
+      <c r="GJ82" s="60"/>
+      <c r="GK82" s="60"/>
+      <c r="GL82" s="60"/>
+      <c r="GM82" s="60"/>
+      <c r="GN82" s="60"/>
+      <c r="GO82" s="60"/>
+      <c r="GP82" s="60"/>
+      <c r="GQ82" s="60"/>
+      <c r="GR82" s="60"/>
+      <c r="GS82" s="60"/>
+      <c r="GT82" s="60"/>
+      <c r="GU82" s="60"/>
+      <c r="GV82" s="60"/>
+      <c r="GW82" s="60"/>
+      <c r="GX82" s="60"/>
+      <c r="GY82" s="60"/>
+      <c r="GZ82" s="60"/>
+      <c r="HA82" s="60"/>
+      <c r="HB82" s="60"/>
+      <c r="HC82" s="60"/>
+      <c r="HD82" s="60"/>
+      <c r="HE82" s="60"/>
+      <c r="HF82" s="60"/>
+      <c r="HG82" s="60"/>
+      <c r="HH82" s="60"/>
+      <c r="HI82" s="60"/>
+      <c r="HJ82" s="60"/>
+      <c r="HK82" s="60"/>
+      <c r="HL82" s="60"/>
+      <c r="HM82" s="60"/>
+      <c r="HN82" s="60"/>
+      <c r="HO82" s="60"/>
+      <c r="HP82" s="60"/>
+      <c r="HQ82" s="60"/>
+      <c r="HR82" s="60"/>
+      <c r="HS82" s="60"/>
+      <c r="HT82" s="60"/>
+      <c r="HU82" s="60"/>
+      <c r="HV82" s="60"/>
+      <c r="HW82" s="60"/>
+      <c r="HX82" s="60"/>
+      <c r="HY82" s="60"/>
+      <c r="HZ82" s="60"/>
+      <c r="IA82" s="60"/>
+      <c r="IB82" s="60"/>
+      <c r="IC82" s="60"/>
+      <c r="ID82" s="60"/>
+      <c r="IE82" s="60"/>
+      <c r="IF82" s="60"/>
+      <c r="IG82" s="60"/>
+      <c r="IH82" s="60"/>
+      <c r="II82" s="60"/>
+      <c r="IJ82" s="60"/>
+      <c r="IK82" s="60"/>
+      <c r="IL82" s="60"/>
+      <c r="IM82" s="60"/>
+      <c r="IN82" s="60"/>
+      <c r="IO82" s="60"/>
+      <c r="IP82" s="60"/>
+      <c r="IQ82" s="60"/>
+      <c r="IR82" s="60"/>
+      <c r="IS82" s="60"/>
+      <c r="IT82" s="60"/>
+      <c r="IU82" s="60"/>
+      <c r="IV82" s="60"/>
+      <c r="IW82" s="60"/>
     </row>
-    <row r="83" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A83" s="58" t="s">
-        <v>177</v>
-      </c>
-      <c r="B83" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" s="58" t="s">
+    <row r="83" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A83" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="59" t="s">
+        <v>254</v>
+      </c>
+      <c r="D83" s="59"/>
+      <c r="E83" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="F83" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G83" s="58">
+      <c r="G83" s="59">
         <v>0</v>
       </c>
-      <c r="H83" s="58">
+      <c r="H83" s="59">
         <v>1</v>
       </c>
-      <c r="I83" s="58"/>
-      <c r="J83" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="I83" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="J83" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K83" s="60"/>
+      <c r="L83" s="60"/>
+      <c r="M83" s="60"/>
+      <c r="N83" s="60"/>
+      <c r="O83" s="60"/>
+      <c r="P83" s="60"/>
+      <c r="Q83" s="60"/>
+      <c r="R83" s="60"/>
+      <c r="S83" s="60"/>
+      <c r="T83" s="60"/>
+      <c r="U83" s="60"/>
+      <c r="V83" s="60"/>
+      <c r="W83" s="60"/>
+      <c r="X83" s="60"/>
+      <c r="Y83" s="60"/>
+      <c r="Z83" s="60"/>
+      <c r="AA83" s="60"/>
+      <c r="AB83" s="60"/>
+      <c r="AC83" s="60"/>
+      <c r="AD83" s="60"/>
+      <c r="AE83" s="60"/>
+      <c r="AF83" s="60"/>
+      <c r="AG83" s="60"/>
+      <c r="AH83" s="60"/>
+      <c r="AI83" s="60"/>
+      <c r="AJ83" s="60"/>
+      <c r="AK83" s="60"/>
+      <c r="AL83" s="60"/>
+      <c r="AM83" s="60"/>
+      <c r="AN83" s="60"/>
+      <c r="AO83" s="60"/>
+      <c r="AP83" s="60"/>
+      <c r="AQ83" s="60"/>
+      <c r="AR83" s="60"/>
+      <c r="AS83" s="60"/>
+      <c r="AT83" s="60"/>
+      <c r="AU83" s="60"/>
+      <c r="AV83" s="60"/>
+      <c r="AW83" s="60"/>
+      <c r="AX83" s="60"/>
+      <c r="AY83" s="60"/>
+      <c r="AZ83" s="60"/>
+      <c r="BA83" s="60"/>
+      <c r="BB83" s="60"/>
+      <c r="BC83" s="60"/>
+      <c r="BD83" s="60"/>
+      <c r="BE83" s="60"/>
+      <c r="BF83" s="60"/>
+      <c r="BG83" s="60"/>
+      <c r="BH83" s="60"/>
+      <c r="BI83" s="60"/>
+      <c r="BJ83" s="60"/>
+      <c r="BK83" s="60"/>
+      <c r="BL83" s="60"/>
+      <c r="BM83" s="60"/>
+      <c r="BN83" s="60"/>
+      <c r="BO83" s="60"/>
+      <c r="BP83" s="60"/>
+      <c r="BQ83" s="60"/>
+      <c r="BR83" s="60"/>
+      <c r="BS83" s="60"/>
+      <c r="BT83" s="60"/>
+      <c r="BU83" s="60"/>
+      <c r="BV83" s="60"/>
+      <c r="BW83" s="60"/>
+      <c r="BX83" s="60"/>
+      <c r="BY83" s="60"/>
+      <c r="BZ83" s="60"/>
+      <c r="CA83" s="60"/>
+      <c r="CB83" s="60"/>
+      <c r="CC83" s="60"/>
+      <c r="CD83" s="60"/>
+      <c r="CE83" s="60"/>
+      <c r="CF83" s="60"/>
+      <c r="CG83" s="60"/>
+      <c r="CH83" s="60"/>
+      <c r="CI83" s="60"/>
+      <c r="CJ83" s="60"/>
+      <c r="CK83" s="60"/>
+      <c r="CL83" s="60"/>
+      <c r="CM83" s="60"/>
+      <c r="CN83" s="60"/>
+      <c r="CO83" s="60"/>
+      <c r="CP83" s="60"/>
+      <c r="CQ83" s="60"/>
+      <c r="CR83" s="60"/>
+      <c r="CS83" s="60"/>
+      <c r="CT83" s="60"/>
+      <c r="CU83" s="60"/>
+      <c r="CV83" s="60"/>
+      <c r="CW83" s="60"/>
+      <c r="CX83" s="60"/>
+      <c r="CY83" s="60"/>
+      <c r="CZ83" s="60"/>
+      <c r="DA83" s="60"/>
+      <c r="DB83" s="60"/>
+      <c r="DC83" s="60"/>
+      <c r="DD83" s="60"/>
+      <c r="DE83" s="60"/>
+      <c r="DF83" s="60"/>
+      <c r="DG83" s="60"/>
+      <c r="DH83" s="60"/>
+      <c r="DI83" s="60"/>
+      <c r="DJ83" s="60"/>
+      <c r="DK83" s="60"/>
+      <c r="DL83" s="60"/>
+      <c r="DM83" s="60"/>
+      <c r="DN83" s="60"/>
+      <c r="DO83" s="60"/>
+      <c r="DP83" s="60"/>
+      <c r="DQ83" s="60"/>
+      <c r="DR83" s="60"/>
+      <c r="DS83" s="60"/>
+      <c r="DT83" s="60"/>
+      <c r="DU83" s="60"/>
+      <c r="DV83" s="60"/>
+      <c r="DW83" s="60"/>
+      <c r="DX83" s="60"/>
+      <c r="DY83" s="60"/>
+      <c r="DZ83" s="60"/>
+      <c r="EA83" s="60"/>
+      <c r="EB83" s="60"/>
+      <c r="EC83" s="60"/>
+      <c r="ED83" s="60"/>
+      <c r="EE83" s="60"/>
+      <c r="EF83" s="60"/>
+      <c r="EG83" s="60"/>
+      <c r="EH83" s="60"/>
+      <c r="EI83" s="60"/>
+      <c r="EJ83" s="60"/>
+      <c r="EK83" s="60"/>
+      <c r="EL83" s="60"/>
+      <c r="EM83" s="60"/>
+      <c r="EN83" s="60"/>
+      <c r="EO83" s="60"/>
+      <c r="EP83" s="60"/>
+      <c r="EQ83" s="60"/>
+      <c r="ER83" s="60"/>
+      <c r="ES83" s="60"/>
+      <c r="ET83" s="60"/>
+      <c r="EU83" s="60"/>
+      <c r="EV83" s="60"/>
+      <c r="EW83" s="60"/>
+      <c r="EX83" s="60"/>
+      <c r="EY83" s="60"/>
+      <c r="EZ83" s="60"/>
+      <c r="FA83" s="60"/>
+      <c r="FB83" s="60"/>
+      <c r="FC83" s="60"/>
+      <c r="FD83" s="60"/>
+      <c r="FE83" s="60"/>
+      <c r="FF83" s="60"/>
+      <c r="FG83" s="60"/>
+      <c r="FH83" s="60"/>
+      <c r="FI83" s="60"/>
+      <c r="FJ83" s="60"/>
+      <c r="FK83" s="60"/>
+      <c r="FL83" s="60"/>
+      <c r="FM83" s="60"/>
+      <c r="FN83" s="60"/>
+      <c r="FO83" s="60"/>
+      <c r="FP83" s="60"/>
+      <c r="FQ83" s="60"/>
+      <c r="FR83" s="60"/>
+      <c r="FS83" s="60"/>
+      <c r="FT83" s="60"/>
+      <c r="FU83" s="60"/>
+      <c r="FV83" s="60"/>
+      <c r="FW83" s="60"/>
+      <c r="FX83" s="60"/>
+      <c r="FY83" s="60"/>
+      <c r="FZ83" s="60"/>
+      <c r="GA83" s="60"/>
+      <c r="GB83" s="60"/>
+      <c r="GC83" s="60"/>
+      <c r="GD83" s="60"/>
+      <c r="GE83" s="60"/>
+      <c r="GF83" s="60"/>
+      <c r="GG83" s="60"/>
+      <c r="GH83" s="60"/>
+      <c r="GI83" s="60"/>
+      <c r="GJ83" s="60"/>
+      <c r="GK83" s="60"/>
+      <c r="GL83" s="60"/>
+      <c r="GM83" s="60"/>
+      <c r="GN83" s="60"/>
+      <c r="GO83" s="60"/>
+      <c r="GP83" s="60"/>
+      <c r="GQ83" s="60"/>
+      <c r="GR83" s="60"/>
+      <c r="GS83" s="60"/>
+      <c r="GT83" s="60"/>
+      <c r="GU83" s="60"/>
+      <c r="GV83" s="60"/>
+      <c r="GW83" s="60"/>
+      <c r="GX83" s="60"/>
+      <c r="GY83" s="60"/>
+      <c r="GZ83" s="60"/>
+      <c r="HA83" s="60"/>
+      <c r="HB83" s="60"/>
+      <c r="HC83" s="60"/>
+      <c r="HD83" s="60"/>
+      <c r="HE83" s="60"/>
+      <c r="HF83" s="60"/>
+      <c r="HG83" s="60"/>
+      <c r="HH83" s="60"/>
+      <c r="HI83" s="60"/>
+      <c r="HJ83" s="60"/>
+      <c r="HK83" s="60"/>
+      <c r="HL83" s="60"/>
+      <c r="HM83" s="60"/>
+      <c r="HN83" s="60"/>
+      <c r="HO83" s="60"/>
+      <c r="HP83" s="60"/>
+      <c r="HQ83" s="60"/>
+      <c r="HR83" s="60"/>
+      <c r="HS83" s="60"/>
+      <c r="HT83" s="60"/>
+      <c r="HU83" s="60"/>
+      <c r="HV83" s="60"/>
+      <c r="HW83" s="60"/>
+      <c r="HX83" s="60"/>
+      <c r="HY83" s="60"/>
+      <c r="HZ83" s="60"/>
+      <c r="IA83" s="60"/>
+      <c r="IB83" s="60"/>
+      <c r="IC83" s="60"/>
+      <c r="ID83" s="60"/>
+      <c r="IE83" s="60"/>
+      <c r="IF83" s="60"/>
+      <c r="IG83" s="60"/>
+      <c r="IH83" s="60"/>
+      <c r="II83" s="60"/>
+      <c r="IJ83" s="60"/>
+      <c r="IK83" s="60"/>
+      <c r="IL83" s="60"/>
+      <c r="IM83" s="60"/>
+      <c r="IN83" s="60"/>
+      <c r="IO83" s="60"/>
+      <c r="IP83" s="60"/>
+      <c r="IQ83" s="60"/>
+      <c r="IR83" s="60"/>
+      <c r="IS83" s="60"/>
+      <c r="IT83" s="60"/>
+      <c r="IU83" s="60"/>
+      <c r="IV83" s="60"/>
+      <c r="IW83" s="60"/>
     </row>
-    <row r="84" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A84" s="58" t="s">
-        <v>179</v>
-      </c>
-      <c r="B84" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C84" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" s="58" t="s">
+    <row r="84" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A84" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="B84" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="D84" s="59"/>
+      <c r="E84" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="F84" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G84" s="58">
+      <c r="G84" s="59">
         <v>0</v>
       </c>
-      <c r="H84" s="58">
+      <c r="H84" s="59">
         <v>1</v>
       </c>
-      <c r="I84" s="58"/>
-      <c r="J84" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="I84" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="J84" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K84" s="60"/>
+      <c r="L84" s="60"/>
+      <c r="M84" s="60"/>
+      <c r="N84" s="60"/>
+      <c r="O84" s="60"/>
+      <c r="P84" s="60"/>
+      <c r="Q84" s="60"/>
+      <c r="R84" s="60"/>
+      <c r="S84" s="60"/>
+      <c r="T84" s="60"/>
+      <c r="U84" s="60"/>
+      <c r="V84" s="60"/>
+      <c r="W84" s="60"/>
+      <c r="X84" s="60"/>
+      <c r="Y84" s="60"/>
+      <c r="Z84" s="60"/>
+      <c r="AA84" s="60"/>
+      <c r="AB84" s="60"/>
+      <c r="AC84" s="60"/>
+      <c r="AD84" s="60"/>
+      <c r="AE84" s="60"/>
+      <c r="AF84" s="60"/>
+      <c r="AG84" s="60"/>
+      <c r="AH84" s="60"/>
+      <c r="AI84" s="60"/>
+      <c r="AJ84" s="60"/>
+      <c r="AK84" s="60"/>
+      <c r="AL84" s="60"/>
+      <c r="AM84" s="60"/>
+      <c r="AN84" s="60"/>
+      <c r="AO84" s="60"/>
+      <c r="AP84" s="60"/>
+      <c r="AQ84" s="60"/>
+      <c r="AR84" s="60"/>
+      <c r="AS84" s="60"/>
+      <c r="AT84" s="60"/>
+      <c r="AU84" s="60"/>
+      <c r="AV84" s="60"/>
+      <c r="AW84" s="60"/>
+      <c r="AX84" s="60"/>
+      <c r="AY84" s="60"/>
+      <c r="AZ84" s="60"/>
+      <c r="BA84" s="60"/>
+      <c r="BB84" s="60"/>
+      <c r="BC84" s="60"/>
+      <c r="BD84" s="60"/>
+      <c r="BE84" s="60"/>
+      <c r="BF84" s="60"/>
+      <c r="BG84" s="60"/>
+      <c r="BH84" s="60"/>
+      <c r="BI84" s="60"/>
+      <c r="BJ84" s="60"/>
+      <c r="BK84" s="60"/>
+      <c r="BL84" s="60"/>
+      <c r="BM84" s="60"/>
+      <c r="BN84" s="60"/>
+      <c r="BO84" s="60"/>
+      <c r="BP84" s="60"/>
+      <c r="BQ84" s="60"/>
+      <c r="BR84" s="60"/>
+      <c r="BS84" s="60"/>
+      <c r="BT84" s="60"/>
+      <c r="BU84" s="60"/>
+      <c r="BV84" s="60"/>
+      <c r="BW84" s="60"/>
+      <c r="BX84" s="60"/>
+      <c r="BY84" s="60"/>
+      <c r="BZ84" s="60"/>
+      <c r="CA84" s="60"/>
+      <c r="CB84" s="60"/>
+      <c r="CC84" s="60"/>
+      <c r="CD84" s="60"/>
+      <c r="CE84" s="60"/>
+      <c r="CF84" s="60"/>
+      <c r="CG84" s="60"/>
+      <c r="CH84" s="60"/>
+      <c r="CI84" s="60"/>
+      <c r="CJ84" s="60"/>
+      <c r="CK84" s="60"/>
+      <c r="CL84" s="60"/>
+      <c r="CM84" s="60"/>
+      <c r="CN84" s="60"/>
+      <c r="CO84" s="60"/>
+      <c r="CP84" s="60"/>
+      <c r="CQ84" s="60"/>
+      <c r="CR84" s="60"/>
+      <c r="CS84" s="60"/>
+      <c r="CT84" s="60"/>
+      <c r="CU84" s="60"/>
+      <c r="CV84" s="60"/>
+      <c r="CW84" s="60"/>
+      <c r="CX84" s="60"/>
+      <c r="CY84" s="60"/>
+      <c r="CZ84" s="60"/>
+      <c r="DA84" s="60"/>
+      <c r="DB84" s="60"/>
+      <c r="DC84" s="60"/>
+      <c r="DD84" s="60"/>
+      <c r="DE84" s="60"/>
+      <c r="DF84" s="60"/>
+      <c r="DG84" s="60"/>
+      <c r="DH84" s="60"/>
+      <c r="DI84" s="60"/>
+      <c r="DJ84" s="60"/>
+      <c r="DK84" s="60"/>
+      <c r="DL84" s="60"/>
+      <c r="DM84" s="60"/>
+      <c r="DN84" s="60"/>
+      <c r="DO84" s="60"/>
+      <c r="DP84" s="60"/>
+      <c r="DQ84" s="60"/>
+      <c r="DR84" s="60"/>
+      <c r="DS84" s="60"/>
+      <c r="DT84" s="60"/>
+      <c r="DU84" s="60"/>
+      <c r="DV84" s="60"/>
+      <c r="DW84" s="60"/>
+      <c r="DX84" s="60"/>
+      <c r="DY84" s="60"/>
+      <c r="DZ84" s="60"/>
+      <c r="EA84" s="60"/>
+      <c r="EB84" s="60"/>
+      <c r="EC84" s="60"/>
+      <c r="ED84" s="60"/>
+      <c r="EE84" s="60"/>
+      <c r="EF84" s="60"/>
+      <c r="EG84" s="60"/>
+      <c r="EH84" s="60"/>
+      <c r="EI84" s="60"/>
+      <c r="EJ84" s="60"/>
+      <c r="EK84" s="60"/>
+      <c r="EL84" s="60"/>
+      <c r="EM84" s="60"/>
+      <c r="EN84" s="60"/>
+      <c r="EO84" s="60"/>
+      <c r="EP84" s="60"/>
+      <c r="EQ84" s="60"/>
+      <c r="ER84" s="60"/>
+      <c r="ES84" s="60"/>
+      <c r="ET84" s="60"/>
+      <c r="EU84" s="60"/>
+      <c r="EV84" s="60"/>
+      <c r="EW84" s="60"/>
+      <c r="EX84" s="60"/>
+      <c r="EY84" s="60"/>
+      <c r="EZ84" s="60"/>
+      <c r="FA84" s="60"/>
+      <c r="FB84" s="60"/>
+      <c r="FC84" s="60"/>
+      <c r="FD84" s="60"/>
+      <c r="FE84" s="60"/>
+      <c r="FF84" s="60"/>
+      <c r="FG84" s="60"/>
+      <c r="FH84" s="60"/>
+      <c r="FI84" s="60"/>
+      <c r="FJ84" s="60"/>
+      <c r="FK84" s="60"/>
+      <c r="FL84" s="60"/>
+      <c r="FM84" s="60"/>
+      <c r="FN84" s="60"/>
+      <c r="FO84" s="60"/>
+      <c r="FP84" s="60"/>
+      <c r="FQ84" s="60"/>
+      <c r="FR84" s="60"/>
+      <c r="FS84" s="60"/>
+      <c r="FT84" s="60"/>
+      <c r="FU84" s="60"/>
+      <c r="FV84" s="60"/>
+      <c r="FW84" s="60"/>
+      <c r="FX84" s="60"/>
+      <c r="FY84" s="60"/>
+      <c r="FZ84" s="60"/>
+      <c r="GA84" s="60"/>
+      <c r="GB84" s="60"/>
+      <c r="GC84" s="60"/>
+      <c r="GD84" s="60"/>
+      <c r="GE84" s="60"/>
+      <c r="GF84" s="60"/>
+      <c r="GG84" s="60"/>
+      <c r="GH84" s="60"/>
+      <c r="GI84" s="60"/>
+      <c r="GJ84" s="60"/>
+      <c r="GK84" s="60"/>
+      <c r="GL84" s="60"/>
+      <c r="GM84" s="60"/>
+      <c r="GN84" s="60"/>
+      <c r="GO84" s="60"/>
+      <c r="GP84" s="60"/>
+      <c r="GQ84" s="60"/>
+      <c r="GR84" s="60"/>
+      <c r="GS84" s="60"/>
+      <c r="GT84" s="60"/>
+      <c r="GU84" s="60"/>
+      <c r="GV84" s="60"/>
+      <c r="GW84" s="60"/>
+      <c r="GX84" s="60"/>
+      <c r="GY84" s="60"/>
+      <c r="GZ84" s="60"/>
+      <c r="HA84" s="60"/>
+      <c r="HB84" s="60"/>
+      <c r="HC84" s="60"/>
+      <c r="HD84" s="60"/>
+      <c r="HE84" s="60"/>
+      <c r="HF84" s="60"/>
+      <c r="HG84" s="60"/>
+      <c r="HH84" s="60"/>
+      <c r="HI84" s="60"/>
+      <c r="HJ84" s="60"/>
+      <c r="HK84" s="60"/>
+      <c r="HL84" s="60"/>
+      <c r="HM84" s="60"/>
+      <c r="HN84" s="60"/>
+      <c r="HO84" s="60"/>
+      <c r="HP84" s="60"/>
+      <c r="HQ84" s="60"/>
+      <c r="HR84" s="60"/>
+      <c r="HS84" s="60"/>
+      <c r="HT84" s="60"/>
+      <c r="HU84" s="60"/>
+      <c r="HV84" s="60"/>
+      <c r="HW84" s="60"/>
+      <c r="HX84" s="60"/>
+      <c r="HY84" s="60"/>
+      <c r="HZ84" s="60"/>
+      <c r="IA84" s="60"/>
+      <c r="IB84" s="60"/>
+      <c r="IC84" s="60"/>
+      <c r="ID84" s="60"/>
+      <c r="IE84" s="60"/>
+      <c r="IF84" s="60"/>
+      <c r="IG84" s="60"/>
+      <c r="IH84" s="60"/>
+      <c r="II84" s="60"/>
+      <c r="IJ84" s="60"/>
+      <c r="IK84" s="60"/>
+      <c r="IL84" s="60"/>
+      <c r="IM84" s="60"/>
+      <c r="IN84" s="60"/>
+      <c r="IO84" s="60"/>
+      <c r="IP84" s="60"/>
+      <c r="IQ84" s="60"/>
+      <c r="IR84" s="60"/>
+      <c r="IS84" s="60"/>
+      <c r="IT84" s="60"/>
+      <c r="IU84" s="60"/>
+      <c r="IV84" s="60"/>
+      <c r="IW84" s="60"/>
     </row>
     <row r="85" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A85" s="58" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B85" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C85" s="58" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D85" s="58"/>
       <c r="E85" s="58" t="s">
@@ -16321,13 +17083,13 @@
     </row>
     <row r="86" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A86" s="58" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B86" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C86" s="58" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D86" s="58"/>
       <c r="E86" s="58" t="s">
@@ -16349,13 +17111,13 @@
     </row>
     <row r="87" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A87" s="58" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B87" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="58" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D87" s="58"/>
       <c r="E87" s="58" t="s">
@@ -16377,13 +17139,13 @@
     </row>
     <row r="88" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A88" s="58" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B88" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C88" s="58" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D88" s="58"/>
       <c r="E88" s="58" t="s">
@@ -16405,13 +17167,13 @@
     </row>
     <row r="89" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A89" s="58" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B89" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C89" s="58" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D89" s="58"/>
       <c r="E89" s="58" t="s">
@@ -16433,13 +17195,13 @@
     </row>
     <row r="90" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A90" s="58" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B90" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C90" s="58" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D90" s="58"/>
       <c r="E90" s="58" t="s">
@@ -16461,13 +17223,13 @@
     </row>
     <row r="91" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A91" s="58" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B91" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="58" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D91" s="58"/>
       <c r="E91" s="58" t="s">
@@ -16489,13 +17251,13 @@
     </row>
     <row r="92" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A92" s="58" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B92" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="58" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D92" s="58"/>
       <c r="E92" s="58" t="s">
@@ -16517,13 +17279,13 @@
     </row>
     <row r="93" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A93" s="58" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B93" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C93" s="58" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D93" s="58"/>
       <c r="E93" s="58" t="s">
@@ -16545,13 +17307,13 @@
     </row>
     <row r="94" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A94" s="58" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B94" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="58" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D94" s="58"/>
       <c r="E94" s="58" t="s">
@@ -16568,18 +17330,18 @@
       </c>
       <c r="I94" s="58"/>
       <c r="J94" s="58" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:257" ht="18" customHeight="1">
+    <row r="95" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A95" s="58" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B95" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C95" s="58" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D95" s="58"/>
       <c r="E95" s="58" t="s">
@@ -16596,18 +17358,18 @@
       </c>
       <c r="I95" s="58"/>
       <c r="J95" s="58" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A96" s="58" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B96" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C96" s="58" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D96" s="58"/>
       <c r="E96" s="58" t="s">
@@ -16624,18 +17386,18 @@
       </c>
       <c r="I96" s="58"/>
       <c r="J96" s="58" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A97" s="58" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B97" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C97" s="58" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D97" s="58"/>
       <c r="E97" s="58" t="s">
@@ -16655,15 +17417,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="98" spans="1:257" ht="18" customHeight="1">
       <c r="A98" s="58" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B98" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C98" s="58" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D98" s="58"/>
       <c r="E98" s="58" t="s">
@@ -16684,20 +17446,20 @@
       </c>
     </row>
     <row r="99" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A99" s="95" t="s">
-        <v>210</v>
-      </c>
-      <c r="B99" s="95" t="s">
+      <c r="A99" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="B99" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C99" s="95" t="s">
-        <v>211</v>
+      <c r="C99" s="58" t="s">
+        <v>203</v>
       </c>
       <c r="D99" s="58"/>
-      <c r="E99" s="95" t="s">
+      <c r="E99" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F99" s="95" t="s">
+      <c r="F99" s="58" t="s">
         <v>13</v>
       </c>
       <c r="G99" s="58">
@@ -16706,28 +17468,26 @@
       <c r="H99" s="58">
         <v>1</v>
       </c>
-      <c r="I99" s="95" t="s">
-        <v>174</v>
-      </c>
-      <c r="J99" s="95" t="s">
-        <v>15</v>
+      <c r="I99" s="58"/>
+      <c r="J99" s="58" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A100" s="95" t="s">
-        <v>203</v>
-      </c>
-      <c r="B100" s="95" t="s">
+      <c r="A100" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C100" s="95" t="s">
-        <v>212</v>
+      <c r="C100" s="58" t="s">
+        <v>205</v>
       </c>
       <c r="D100" s="58"/>
-      <c r="E100" s="95" t="s">
+      <c r="E100" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F100" s="95" t="s">
+      <c r="F100" s="58" t="s">
         <v>13</v>
       </c>
       <c r="G100" s="58">
@@ -16736,28 +17496,26 @@
       <c r="H100" s="58">
         <v>1</v>
       </c>
-      <c r="I100" s="95" t="s">
-        <v>174</v>
-      </c>
-      <c r="J100" s="95" t="s">
-        <v>140</v>
+      <c r="I100" s="58"/>
+      <c r="J100" s="58" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A101" s="95" t="s">
-        <v>213</v>
-      </c>
-      <c r="B101" s="95" t="s">
+      <c r="A101" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="B101" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="95" t="s">
-        <v>214</v>
+      <c r="C101" s="58" t="s">
+        <v>207</v>
       </c>
       <c r="D101" s="58"/>
-      <c r="E101" s="95" t="s">
+      <c r="E101" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F101" s="95" t="s">
+      <c r="F101" s="58" t="s">
         <v>13</v>
       </c>
       <c r="G101" s="58">
@@ -16766,22 +17524,20 @@
       <c r="H101" s="58">
         <v>1</v>
       </c>
-      <c r="I101" s="95" t="s">
-        <v>174</v>
-      </c>
-      <c r="J101" s="95" t="s">
-        <v>15</v>
+      <c r="I101" s="58"/>
+      <c r="J101" s="58" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="95" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B102" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C102" s="95" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D102" s="58"/>
       <c r="E102" s="95" t="s">
@@ -16797,21 +17553,21 @@
         <v>1</v>
       </c>
       <c r="I102" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J102" s="95" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="95" t="s">
-        <v>219</v>
-      </c>
-      <c r="B103" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C103" s="95" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D103" s="58"/>
       <c r="E103" s="95" t="s">
@@ -16827,21 +17583,21 @@
         <v>1</v>
       </c>
       <c r="I103" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J103" s="95" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="95" t="s">
-        <v>220</v>
-      </c>
-      <c r="B104" s="58" t="s">
+        <v>212</v>
+      </c>
+      <c r="B104" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="95" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D104" s="58"/>
       <c r="E104" s="95" t="s">
@@ -16857,21 +17613,21 @@
         <v>1</v>
       </c>
       <c r="I104" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J104" s="95" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A105" s="95" t="s">
-        <v>221</v>
-      </c>
-      <c r="B105" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="B105" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C105" s="95" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D105" s="58"/>
       <c r="E105" s="95" t="s">
@@ -16887,665 +17643,665 @@
         <v>1</v>
       </c>
       <c r="I105" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J105" s="95" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A106" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="C106" s="85" t="s">
-        <v>78</v>
+      <c r="A106" s="95" t="s">
+        <v>218</v>
+      </c>
+      <c r="B106" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106" s="95" t="s">
+        <v>216</v>
       </c>
       <c r="D106" s="58"/>
-      <c r="E106" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="F106" s="76" t="s">
+      <c r="E106" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="G106" s="25">
+      <c r="G106" s="58">
         <v>0</v>
       </c>
-      <c r="H106" s="25">
+      <c r="H106" s="58">
         <v>1</v>
       </c>
-      <c r="I106" s="10"/>
-      <c r="J106" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K106"/>
-      <c r="L106"/>
-      <c r="M106"/>
-      <c r="N106"/>
-      <c r="O106"/>
-      <c r="P106"/>
-      <c r="Q106"/>
-      <c r="R106"/>
-      <c r="S106"/>
-      <c r="T106"/>
-      <c r="U106"/>
-      <c r="V106"/>
-      <c r="W106"/>
-      <c r="X106"/>
-      <c r="Y106"/>
-      <c r="Z106"/>
-      <c r="AA106"/>
-      <c r="AB106"/>
-      <c r="AC106"/>
-      <c r="AD106"/>
-      <c r="AE106"/>
-      <c r="AF106"/>
-      <c r="AG106"/>
-      <c r="AH106"/>
-      <c r="AI106"/>
-      <c r="AJ106"/>
-      <c r="AK106"/>
-      <c r="AL106"/>
-      <c r="AM106"/>
-      <c r="AN106"/>
-      <c r="AO106"/>
-      <c r="AP106"/>
-      <c r="AQ106"/>
-      <c r="AR106"/>
-      <c r="AS106"/>
-      <c r="AT106"/>
-      <c r="AU106"/>
-      <c r="AV106"/>
-      <c r="AW106"/>
-      <c r="AX106"/>
-      <c r="AY106"/>
-      <c r="AZ106"/>
-      <c r="BA106"/>
-      <c r="BB106"/>
-      <c r="BC106"/>
-      <c r="BD106"/>
-      <c r="BE106"/>
-      <c r="BF106"/>
-      <c r="BG106"/>
-      <c r="BH106"/>
-      <c r="BI106"/>
-      <c r="BJ106"/>
-      <c r="BK106"/>
-      <c r="BL106"/>
-      <c r="BM106"/>
-      <c r="BN106"/>
-      <c r="BO106"/>
-      <c r="BP106"/>
-      <c r="BQ106"/>
-      <c r="BR106"/>
-      <c r="BS106"/>
-      <c r="BT106"/>
-      <c r="BU106"/>
-      <c r="BV106"/>
-      <c r="BW106"/>
-      <c r="BX106"/>
-      <c r="BY106"/>
-      <c r="BZ106"/>
-      <c r="CA106"/>
-      <c r="CB106"/>
-      <c r="CC106"/>
-      <c r="CD106"/>
-      <c r="CE106"/>
-      <c r="CF106"/>
-      <c r="CG106"/>
-      <c r="CH106"/>
-      <c r="CI106"/>
-      <c r="CJ106"/>
-      <c r="CK106"/>
-      <c r="CL106"/>
-      <c r="CM106"/>
-      <c r="CN106"/>
-      <c r="CO106"/>
-      <c r="CP106"/>
-      <c r="CQ106"/>
-      <c r="CR106"/>
-      <c r="CS106"/>
-      <c r="CT106"/>
-      <c r="CU106"/>
-      <c r="CV106"/>
-      <c r="CW106"/>
-      <c r="CX106"/>
-      <c r="CY106"/>
-      <c r="CZ106"/>
-      <c r="DA106"/>
-      <c r="DB106"/>
-      <c r="DC106"/>
-      <c r="DD106"/>
-      <c r="DE106"/>
-      <c r="DF106"/>
-      <c r="DG106"/>
-      <c r="DH106"/>
-      <c r="DI106"/>
-      <c r="DJ106"/>
-      <c r="DK106"/>
-      <c r="DL106"/>
-      <c r="DM106"/>
-      <c r="DN106"/>
-      <c r="DO106"/>
-      <c r="DP106"/>
-      <c r="DQ106"/>
-      <c r="DR106"/>
-      <c r="DS106"/>
-      <c r="DT106"/>
-      <c r="DU106"/>
-      <c r="DV106"/>
-      <c r="DW106"/>
-      <c r="DX106"/>
-      <c r="DY106"/>
-      <c r="DZ106"/>
-      <c r="EA106"/>
-      <c r="EB106"/>
-      <c r="EC106"/>
-      <c r="ED106"/>
-      <c r="EE106"/>
-      <c r="EF106"/>
-      <c r="EG106"/>
-      <c r="EH106"/>
-      <c r="EI106"/>
-      <c r="EJ106"/>
-      <c r="EK106"/>
-      <c r="EL106"/>
-      <c r="EM106"/>
-      <c r="EN106"/>
-      <c r="EO106"/>
-      <c r="EP106"/>
-      <c r="EQ106"/>
-      <c r="ER106"/>
-      <c r="ES106"/>
-      <c r="ET106"/>
-      <c r="EU106"/>
-      <c r="EV106"/>
-      <c r="EW106"/>
-      <c r="EX106"/>
-      <c r="EY106"/>
-      <c r="EZ106"/>
-      <c r="FA106"/>
-      <c r="FB106"/>
-      <c r="FC106"/>
-      <c r="FD106"/>
-      <c r="FE106"/>
-      <c r="FF106"/>
-      <c r="FG106"/>
-      <c r="FH106"/>
-      <c r="FI106"/>
-      <c r="FJ106"/>
-      <c r="FK106"/>
-      <c r="FL106"/>
-      <c r="FM106"/>
-      <c r="FN106"/>
-      <c r="FO106"/>
-      <c r="FP106"/>
-      <c r="FQ106"/>
-      <c r="FR106"/>
-      <c r="FS106"/>
-      <c r="FT106"/>
-      <c r="FU106"/>
-      <c r="FV106"/>
-      <c r="FW106"/>
-      <c r="FX106"/>
-      <c r="FY106"/>
-      <c r="FZ106"/>
-      <c r="GA106"/>
-      <c r="GB106"/>
-      <c r="GC106"/>
-      <c r="GD106"/>
-      <c r="GE106"/>
-      <c r="GF106"/>
-      <c r="GG106"/>
-      <c r="GH106"/>
-      <c r="GI106"/>
-      <c r="GJ106"/>
-      <c r="GK106"/>
-      <c r="GL106"/>
-      <c r="GM106"/>
-      <c r="GN106"/>
-      <c r="GO106"/>
-      <c r="GP106"/>
-      <c r="GQ106"/>
-      <c r="GR106"/>
-      <c r="GS106"/>
-      <c r="GT106"/>
-      <c r="GU106"/>
-      <c r="GV106"/>
-      <c r="GW106"/>
-      <c r="GX106"/>
-      <c r="GY106"/>
-      <c r="GZ106"/>
-      <c r="HA106"/>
-      <c r="HB106"/>
-      <c r="HC106"/>
-      <c r="HD106"/>
-      <c r="HE106"/>
-      <c r="HF106"/>
-      <c r="HG106"/>
-      <c r="HH106"/>
-      <c r="HI106"/>
-      <c r="HJ106"/>
-      <c r="HK106"/>
-      <c r="HL106"/>
-      <c r="HM106"/>
-      <c r="HN106"/>
-      <c r="HO106"/>
-      <c r="HP106"/>
-      <c r="HQ106"/>
-      <c r="HR106"/>
-      <c r="HS106"/>
-      <c r="HT106"/>
-      <c r="HU106"/>
-      <c r="HV106"/>
-      <c r="HW106"/>
-      <c r="HX106"/>
-      <c r="HY106"/>
-      <c r="HZ106"/>
-      <c r="IA106"/>
-      <c r="IB106"/>
-      <c r="IC106"/>
-      <c r="ID106"/>
-      <c r="IE106"/>
-      <c r="IF106"/>
-      <c r="IG106"/>
-      <c r="IH106"/>
-      <c r="II106"/>
-      <c r="IJ106"/>
-      <c r="IK106"/>
-      <c r="IL106"/>
-      <c r="IM106"/>
-      <c r="IN106"/>
-      <c r="IO106"/>
-      <c r="IP106"/>
-      <c r="IQ106"/>
-      <c r="IR106"/>
-      <c r="IS106"/>
-      <c r="IT106"/>
-      <c r="IU106"/>
-      <c r="IV106"/>
-      <c r="IW106"/>
+      <c r="I106" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="J106" s="95" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A107" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="B107" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C107" s="85" t="s">
-        <v>78</v>
+      <c r="A107" s="95" t="s">
+        <v>219</v>
+      </c>
+      <c r="B107" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="95" t="s">
+        <v>217</v>
       </c>
       <c r="D107" s="58"/>
-      <c r="E107" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="F107" s="76" t="s">
+      <c r="E107" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="G107" s="25">
+      <c r="G107" s="58">
         <v>0</v>
       </c>
-      <c r="H107" s="25">
+      <c r="H107" s="58">
         <v>1</v>
       </c>
-      <c r="I107" s="10"/>
-      <c r="J107" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K107"/>
-      <c r="L107"/>
-      <c r="M107"/>
-      <c r="N107"/>
-      <c r="O107"/>
-      <c r="P107"/>
-      <c r="Q107"/>
-      <c r="R107"/>
-      <c r="S107"/>
-      <c r="T107"/>
-      <c r="U107"/>
-      <c r="V107"/>
-      <c r="W107"/>
-      <c r="X107"/>
-      <c r="Y107"/>
-      <c r="Z107"/>
-      <c r="AA107"/>
-      <c r="AB107"/>
-      <c r="AC107"/>
-      <c r="AD107"/>
-      <c r="AE107"/>
-      <c r="AF107"/>
-      <c r="AG107"/>
-      <c r="AH107"/>
-      <c r="AI107"/>
-      <c r="AJ107"/>
-      <c r="AK107"/>
-      <c r="AL107"/>
-      <c r="AM107"/>
-      <c r="AN107"/>
-      <c r="AO107"/>
-      <c r="AP107"/>
-      <c r="AQ107"/>
-      <c r="AR107"/>
-      <c r="AS107"/>
-      <c r="AT107"/>
-      <c r="AU107"/>
-      <c r="AV107"/>
-      <c r="AW107"/>
-      <c r="AX107"/>
-      <c r="AY107"/>
-      <c r="AZ107"/>
-      <c r="BA107"/>
-      <c r="BB107"/>
-      <c r="BC107"/>
-      <c r="BD107"/>
-      <c r="BE107"/>
-      <c r="BF107"/>
-      <c r="BG107"/>
-      <c r="BH107"/>
-      <c r="BI107"/>
-      <c r="BJ107"/>
-      <c r="BK107"/>
-      <c r="BL107"/>
-      <c r="BM107"/>
-      <c r="BN107"/>
-      <c r="BO107"/>
-      <c r="BP107"/>
-      <c r="BQ107"/>
-      <c r="BR107"/>
-      <c r="BS107"/>
-      <c r="BT107"/>
-      <c r="BU107"/>
-      <c r="BV107"/>
-      <c r="BW107"/>
-      <c r="BX107"/>
-      <c r="BY107"/>
-      <c r="BZ107"/>
-      <c r="CA107"/>
-      <c r="CB107"/>
-      <c r="CC107"/>
-      <c r="CD107"/>
-      <c r="CE107"/>
-      <c r="CF107"/>
-      <c r="CG107"/>
-      <c r="CH107"/>
-      <c r="CI107"/>
-      <c r="CJ107"/>
-      <c r="CK107"/>
-      <c r="CL107"/>
-      <c r="CM107"/>
-      <c r="CN107"/>
-      <c r="CO107"/>
-      <c r="CP107"/>
-      <c r="CQ107"/>
-      <c r="CR107"/>
-      <c r="CS107"/>
-      <c r="CT107"/>
-      <c r="CU107"/>
-      <c r="CV107"/>
-      <c r="CW107"/>
-      <c r="CX107"/>
-      <c r="CY107"/>
-      <c r="CZ107"/>
-      <c r="DA107"/>
-      <c r="DB107"/>
-      <c r="DC107"/>
-      <c r="DD107"/>
-      <c r="DE107"/>
-      <c r="DF107"/>
-      <c r="DG107"/>
-      <c r="DH107"/>
-      <c r="DI107"/>
-      <c r="DJ107"/>
-      <c r="DK107"/>
-      <c r="DL107"/>
-      <c r="DM107"/>
-      <c r="DN107"/>
-      <c r="DO107"/>
-      <c r="DP107"/>
-      <c r="DQ107"/>
-      <c r="DR107"/>
-      <c r="DS107"/>
-      <c r="DT107"/>
-      <c r="DU107"/>
-      <c r="DV107"/>
-      <c r="DW107"/>
-      <c r="DX107"/>
-      <c r="DY107"/>
-      <c r="DZ107"/>
-      <c r="EA107"/>
-      <c r="EB107"/>
-      <c r="EC107"/>
-      <c r="ED107"/>
-      <c r="EE107"/>
-      <c r="EF107"/>
-      <c r="EG107"/>
-      <c r="EH107"/>
-      <c r="EI107"/>
-      <c r="EJ107"/>
-      <c r="EK107"/>
-      <c r="EL107"/>
-      <c r="EM107"/>
-      <c r="EN107"/>
-      <c r="EO107"/>
-      <c r="EP107"/>
-      <c r="EQ107"/>
-      <c r="ER107"/>
-      <c r="ES107"/>
-      <c r="ET107"/>
-      <c r="EU107"/>
-      <c r="EV107"/>
-      <c r="EW107"/>
-      <c r="EX107"/>
-      <c r="EY107"/>
-      <c r="EZ107"/>
-      <c r="FA107"/>
-      <c r="FB107"/>
-      <c r="FC107"/>
-      <c r="FD107"/>
-      <c r="FE107"/>
-      <c r="FF107"/>
-      <c r="FG107"/>
-      <c r="FH107"/>
-      <c r="FI107"/>
-      <c r="FJ107"/>
-      <c r="FK107"/>
-      <c r="FL107"/>
-      <c r="FM107"/>
-      <c r="FN107"/>
-      <c r="FO107"/>
-      <c r="FP107"/>
-      <c r="FQ107"/>
-      <c r="FR107"/>
-      <c r="FS107"/>
-      <c r="FT107"/>
-      <c r="FU107"/>
-      <c r="FV107"/>
-      <c r="FW107"/>
-      <c r="FX107"/>
-      <c r="FY107"/>
-      <c r="FZ107"/>
-      <c r="GA107"/>
-      <c r="GB107"/>
-      <c r="GC107"/>
-      <c r="GD107"/>
-      <c r="GE107"/>
-      <c r="GF107"/>
-      <c r="GG107"/>
-      <c r="GH107"/>
-      <c r="GI107"/>
-      <c r="GJ107"/>
-      <c r="GK107"/>
-      <c r="GL107"/>
-      <c r="GM107"/>
-      <c r="GN107"/>
-      <c r="GO107"/>
-      <c r="GP107"/>
-      <c r="GQ107"/>
-      <c r="GR107"/>
-      <c r="GS107"/>
-      <c r="GT107"/>
-      <c r="GU107"/>
-      <c r="GV107"/>
-      <c r="GW107"/>
-      <c r="GX107"/>
-      <c r="GY107"/>
-      <c r="GZ107"/>
-      <c r="HA107"/>
-      <c r="HB107"/>
-      <c r="HC107"/>
-      <c r="HD107"/>
-      <c r="HE107"/>
-      <c r="HF107"/>
-      <c r="HG107"/>
-      <c r="HH107"/>
-      <c r="HI107"/>
-      <c r="HJ107"/>
-      <c r="HK107"/>
-      <c r="HL107"/>
-      <c r="HM107"/>
-      <c r="HN107"/>
-      <c r="HO107"/>
-      <c r="HP107"/>
-      <c r="HQ107"/>
-      <c r="HR107"/>
-      <c r="HS107"/>
-      <c r="HT107"/>
-      <c r="HU107"/>
-      <c r="HV107"/>
-      <c r="HW107"/>
-      <c r="HX107"/>
-      <c r="HY107"/>
-      <c r="HZ107"/>
-      <c r="IA107"/>
-      <c r="IB107"/>
-      <c r="IC107"/>
-      <c r="ID107"/>
-      <c r="IE107"/>
-      <c r="IF107"/>
-      <c r="IG107"/>
-      <c r="IH107"/>
-      <c r="II107"/>
-      <c r="IJ107"/>
-      <c r="IK107"/>
-      <c r="IL107"/>
-      <c r="IM107"/>
-      <c r="IN107"/>
-      <c r="IO107"/>
-      <c r="IP107"/>
-      <c r="IQ107"/>
-      <c r="IR107"/>
-      <c r="IS107"/>
-      <c r="IT107"/>
-      <c r="IU107"/>
-      <c r="IV107"/>
-      <c r="IW107"/>
+      <c r="I107" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="J107" s="95" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A108" s="1" t="s">
-        <v>225</v>
+      <c r="A108" s="95" t="s">
+        <v>220</v>
       </c>
       <c r="B108" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C108" s="58" t="s">
-        <v>233</v>
+        <v>11</v>
+      </c>
+      <c r="C108" s="95" t="s">
+        <v>221</v>
       </c>
       <c r="D108" s="58"/>
-      <c r="E108" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="F108" s="96" t="s">
+      <c r="E108" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="G108" s="25">
+      <c r="G108" s="58">
         <v>0</v>
       </c>
-      <c r="H108" s="97">
+      <c r="H108" s="58">
         <v>1</v>
       </c>
-      <c r="I108" s="96" t="s">
-        <v>174</v>
-      </c>
-      <c r="J108" s="96" t="s">
-        <v>29</v>
+      <c r="I108" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="J108" s="95" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A109" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B109" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C109" s="58" t="s">
-        <v>235</v>
+      <c r="A109" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B109" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C109" s="85" t="s">
+        <v>78</v>
       </c>
       <c r="D109" s="58"/>
-      <c r="E109" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="F109" s="96" t="s">
+      <c r="E109" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="F109" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G109" s="25">
         <v>0</v>
       </c>
-      <c r="H109" s="58">
+      <c r="H109" s="25">
         <v>1</v>
       </c>
-      <c r="I109" s="96" t="s">
-        <v>174</v>
-      </c>
-      <c r="J109" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I109" s="10"/>
+      <c r="J109" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K109"/>
+      <c r="L109"/>
+      <c r="M109"/>
+      <c r="N109"/>
+      <c r="O109"/>
+      <c r="P109"/>
+      <c r="Q109"/>
+      <c r="R109"/>
+      <c r="S109"/>
+      <c r="T109"/>
+      <c r="U109"/>
+      <c r="V109"/>
+      <c r="W109"/>
+      <c r="X109"/>
+      <c r="Y109"/>
+      <c r="Z109"/>
+      <c r="AA109"/>
+      <c r="AB109"/>
+      <c r="AC109"/>
+      <c r="AD109"/>
+      <c r="AE109"/>
+      <c r="AF109"/>
+      <c r="AG109"/>
+      <c r="AH109"/>
+      <c r="AI109"/>
+      <c r="AJ109"/>
+      <c r="AK109"/>
+      <c r="AL109"/>
+      <c r="AM109"/>
+      <c r="AN109"/>
+      <c r="AO109"/>
+      <c r="AP109"/>
+      <c r="AQ109"/>
+      <c r="AR109"/>
+      <c r="AS109"/>
+      <c r="AT109"/>
+      <c r="AU109"/>
+      <c r="AV109"/>
+      <c r="AW109"/>
+      <c r="AX109"/>
+      <c r="AY109"/>
+      <c r="AZ109"/>
+      <c r="BA109"/>
+      <c r="BB109"/>
+      <c r="BC109"/>
+      <c r="BD109"/>
+      <c r="BE109"/>
+      <c r="BF109"/>
+      <c r="BG109"/>
+      <c r="BH109"/>
+      <c r="BI109"/>
+      <c r="BJ109"/>
+      <c r="BK109"/>
+      <c r="BL109"/>
+      <c r="BM109"/>
+      <c r="BN109"/>
+      <c r="BO109"/>
+      <c r="BP109"/>
+      <c r="BQ109"/>
+      <c r="BR109"/>
+      <c r="BS109"/>
+      <c r="BT109"/>
+      <c r="BU109"/>
+      <c r="BV109"/>
+      <c r="BW109"/>
+      <c r="BX109"/>
+      <c r="BY109"/>
+      <c r="BZ109"/>
+      <c r="CA109"/>
+      <c r="CB109"/>
+      <c r="CC109"/>
+      <c r="CD109"/>
+      <c r="CE109"/>
+      <c r="CF109"/>
+      <c r="CG109"/>
+      <c r="CH109"/>
+      <c r="CI109"/>
+      <c r="CJ109"/>
+      <c r="CK109"/>
+      <c r="CL109"/>
+      <c r="CM109"/>
+      <c r="CN109"/>
+      <c r="CO109"/>
+      <c r="CP109"/>
+      <c r="CQ109"/>
+      <c r="CR109"/>
+      <c r="CS109"/>
+      <c r="CT109"/>
+      <c r="CU109"/>
+      <c r="CV109"/>
+      <c r="CW109"/>
+      <c r="CX109"/>
+      <c r="CY109"/>
+      <c r="CZ109"/>
+      <c r="DA109"/>
+      <c r="DB109"/>
+      <c r="DC109"/>
+      <c r="DD109"/>
+      <c r="DE109"/>
+      <c r="DF109"/>
+      <c r="DG109"/>
+      <c r="DH109"/>
+      <c r="DI109"/>
+      <c r="DJ109"/>
+      <c r="DK109"/>
+      <c r="DL109"/>
+      <c r="DM109"/>
+      <c r="DN109"/>
+      <c r="DO109"/>
+      <c r="DP109"/>
+      <c r="DQ109"/>
+      <c r="DR109"/>
+      <c r="DS109"/>
+      <c r="DT109"/>
+      <c r="DU109"/>
+      <c r="DV109"/>
+      <c r="DW109"/>
+      <c r="DX109"/>
+      <c r="DY109"/>
+      <c r="DZ109"/>
+      <c r="EA109"/>
+      <c r="EB109"/>
+      <c r="EC109"/>
+      <c r="ED109"/>
+      <c r="EE109"/>
+      <c r="EF109"/>
+      <c r="EG109"/>
+      <c r="EH109"/>
+      <c r="EI109"/>
+      <c r="EJ109"/>
+      <c r="EK109"/>
+      <c r="EL109"/>
+      <c r="EM109"/>
+      <c r="EN109"/>
+      <c r="EO109"/>
+      <c r="EP109"/>
+      <c r="EQ109"/>
+      <c r="ER109"/>
+      <c r="ES109"/>
+      <c r="ET109"/>
+      <c r="EU109"/>
+      <c r="EV109"/>
+      <c r="EW109"/>
+      <c r="EX109"/>
+      <c r="EY109"/>
+      <c r="EZ109"/>
+      <c r="FA109"/>
+      <c r="FB109"/>
+      <c r="FC109"/>
+      <c r="FD109"/>
+      <c r="FE109"/>
+      <c r="FF109"/>
+      <c r="FG109"/>
+      <c r="FH109"/>
+      <c r="FI109"/>
+      <c r="FJ109"/>
+      <c r="FK109"/>
+      <c r="FL109"/>
+      <c r="FM109"/>
+      <c r="FN109"/>
+      <c r="FO109"/>
+      <c r="FP109"/>
+      <c r="FQ109"/>
+      <c r="FR109"/>
+      <c r="FS109"/>
+      <c r="FT109"/>
+      <c r="FU109"/>
+      <c r="FV109"/>
+      <c r="FW109"/>
+      <c r="FX109"/>
+      <c r="FY109"/>
+      <c r="FZ109"/>
+      <c r="GA109"/>
+      <c r="GB109"/>
+      <c r="GC109"/>
+      <c r="GD109"/>
+      <c r="GE109"/>
+      <c r="GF109"/>
+      <c r="GG109"/>
+      <c r="GH109"/>
+      <c r="GI109"/>
+      <c r="GJ109"/>
+      <c r="GK109"/>
+      <c r="GL109"/>
+      <c r="GM109"/>
+      <c r="GN109"/>
+      <c r="GO109"/>
+      <c r="GP109"/>
+      <c r="GQ109"/>
+      <c r="GR109"/>
+      <c r="GS109"/>
+      <c r="GT109"/>
+      <c r="GU109"/>
+      <c r="GV109"/>
+      <c r="GW109"/>
+      <c r="GX109"/>
+      <c r="GY109"/>
+      <c r="GZ109"/>
+      <c r="HA109"/>
+      <c r="HB109"/>
+      <c r="HC109"/>
+      <c r="HD109"/>
+      <c r="HE109"/>
+      <c r="HF109"/>
+      <c r="HG109"/>
+      <c r="HH109"/>
+      <c r="HI109"/>
+      <c r="HJ109"/>
+      <c r="HK109"/>
+      <c r="HL109"/>
+      <c r="HM109"/>
+      <c r="HN109"/>
+      <c r="HO109"/>
+      <c r="HP109"/>
+      <c r="HQ109"/>
+      <c r="HR109"/>
+      <c r="HS109"/>
+      <c r="HT109"/>
+      <c r="HU109"/>
+      <c r="HV109"/>
+      <c r="HW109"/>
+      <c r="HX109"/>
+      <c r="HY109"/>
+      <c r="HZ109"/>
+      <c r="IA109"/>
+      <c r="IB109"/>
+      <c r="IC109"/>
+      <c r="ID109"/>
+      <c r="IE109"/>
+      <c r="IF109"/>
+      <c r="IG109"/>
+      <c r="IH109"/>
+      <c r="II109"/>
+      <c r="IJ109"/>
+      <c r="IK109"/>
+      <c r="IL109"/>
+      <c r="IM109"/>
+      <c r="IN109"/>
+      <c r="IO109"/>
+      <c r="IP109"/>
+      <c r="IQ109"/>
+      <c r="IR109"/>
+      <c r="IS109"/>
+      <c r="IT109"/>
+      <c r="IU109"/>
+      <c r="IV109"/>
+      <c r="IW109"/>
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B110" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C110" s="58" t="s">
-        <v>236</v>
+      <c r="A110" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>78</v>
       </c>
       <c r="D110" s="58"/>
-      <c r="E110" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="F110" s="96" t="s">
+      <c r="E110" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F110" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="25">
         <v>0</v>
       </c>
-      <c r="H110" s="58">
+      <c r="H110" s="25">
         <v>1</v>
       </c>
-      <c r="I110" s="96" t="s">
-        <v>174</v>
-      </c>
-      <c r="J110" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I110" s="10"/>
+      <c r="J110" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K110"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110"/>
+      <c r="R110"/>
+      <c r="S110"/>
+      <c r="T110"/>
+      <c r="U110"/>
+      <c r="V110"/>
+      <c r="W110"/>
+      <c r="X110"/>
+      <c r="Y110"/>
+      <c r="Z110"/>
+      <c r="AA110"/>
+      <c r="AB110"/>
+      <c r="AC110"/>
+      <c r="AD110"/>
+      <c r="AE110"/>
+      <c r="AF110"/>
+      <c r="AG110"/>
+      <c r="AH110"/>
+      <c r="AI110"/>
+      <c r="AJ110"/>
+      <c r="AK110"/>
+      <c r="AL110"/>
+      <c r="AM110"/>
+      <c r="AN110"/>
+      <c r="AO110"/>
+      <c r="AP110"/>
+      <c r="AQ110"/>
+      <c r="AR110"/>
+      <c r="AS110"/>
+      <c r="AT110"/>
+      <c r="AU110"/>
+      <c r="AV110"/>
+      <c r="AW110"/>
+      <c r="AX110"/>
+      <c r="AY110"/>
+      <c r="AZ110"/>
+      <c r="BA110"/>
+      <c r="BB110"/>
+      <c r="BC110"/>
+      <c r="BD110"/>
+      <c r="BE110"/>
+      <c r="BF110"/>
+      <c r="BG110"/>
+      <c r="BH110"/>
+      <c r="BI110"/>
+      <c r="BJ110"/>
+      <c r="BK110"/>
+      <c r="BL110"/>
+      <c r="BM110"/>
+      <c r="BN110"/>
+      <c r="BO110"/>
+      <c r="BP110"/>
+      <c r="BQ110"/>
+      <c r="BR110"/>
+      <c r="BS110"/>
+      <c r="BT110"/>
+      <c r="BU110"/>
+      <c r="BV110"/>
+      <c r="BW110"/>
+      <c r="BX110"/>
+      <c r="BY110"/>
+      <c r="BZ110"/>
+      <c r="CA110"/>
+      <c r="CB110"/>
+      <c r="CC110"/>
+      <c r="CD110"/>
+      <c r="CE110"/>
+      <c r="CF110"/>
+      <c r="CG110"/>
+      <c r="CH110"/>
+      <c r="CI110"/>
+      <c r="CJ110"/>
+      <c r="CK110"/>
+      <c r="CL110"/>
+      <c r="CM110"/>
+      <c r="CN110"/>
+      <c r="CO110"/>
+      <c r="CP110"/>
+      <c r="CQ110"/>
+      <c r="CR110"/>
+      <c r="CS110"/>
+      <c r="CT110"/>
+      <c r="CU110"/>
+      <c r="CV110"/>
+      <c r="CW110"/>
+      <c r="CX110"/>
+      <c r="CY110"/>
+      <c r="CZ110"/>
+      <c r="DA110"/>
+      <c r="DB110"/>
+      <c r="DC110"/>
+      <c r="DD110"/>
+      <c r="DE110"/>
+      <c r="DF110"/>
+      <c r="DG110"/>
+      <c r="DH110"/>
+      <c r="DI110"/>
+      <c r="DJ110"/>
+      <c r="DK110"/>
+      <c r="DL110"/>
+      <c r="DM110"/>
+      <c r="DN110"/>
+      <c r="DO110"/>
+      <c r="DP110"/>
+      <c r="DQ110"/>
+      <c r="DR110"/>
+      <c r="DS110"/>
+      <c r="DT110"/>
+      <c r="DU110"/>
+      <c r="DV110"/>
+      <c r="DW110"/>
+      <c r="DX110"/>
+      <c r="DY110"/>
+      <c r="DZ110"/>
+      <c r="EA110"/>
+      <c r="EB110"/>
+      <c r="EC110"/>
+      <c r="ED110"/>
+      <c r="EE110"/>
+      <c r="EF110"/>
+      <c r="EG110"/>
+      <c r="EH110"/>
+      <c r="EI110"/>
+      <c r="EJ110"/>
+      <c r="EK110"/>
+      <c r="EL110"/>
+      <c r="EM110"/>
+      <c r="EN110"/>
+      <c r="EO110"/>
+      <c r="EP110"/>
+      <c r="EQ110"/>
+      <c r="ER110"/>
+      <c r="ES110"/>
+      <c r="ET110"/>
+      <c r="EU110"/>
+      <c r="EV110"/>
+      <c r="EW110"/>
+      <c r="EX110"/>
+      <c r="EY110"/>
+      <c r="EZ110"/>
+      <c r="FA110"/>
+      <c r="FB110"/>
+      <c r="FC110"/>
+      <c r="FD110"/>
+      <c r="FE110"/>
+      <c r="FF110"/>
+      <c r="FG110"/>
+      <c r="FH110"/>
+      <c r="FI110"/>
+      <c r="FJ110"/>
+      <c r="FK110"/>
+      <c r="FL110"/>
+      <c r="FM110"/>
+      <c r="FN110"/>
+      <c r="FO110"/>
+      <c r="FP110"/>
+      <c r="FQ110"/>
+      <c r="FR110"/>
+      <c r="FS110"/>
+      <c r="FT110"/>
+      <c r="FU110"/>
+      <c r="FV110"/>
+      <c r="FW110"/>
+      <c r="FX110"/>
+      <c r="FY110"/>
+      <c r="FZ110"/>
+      <c r="GA110"/>
+      <c r="GB110"/>
+      <c r="GC110"/>
+      <c r="GD110"/>
+      <c r="GE110"/>
+      <c r="GF110"/>
+      <c r="GG110"/>
+      <c r="GH110"/>
+      <c r="GI110"/>
+      <c r="GJ110"/>
+      <c r="GK110"/>
+      <c r="GL110"/>
+      <c r="GM110"/>
+      <c r="GN110"/>
+      <c r="GO110"/>
+      <c r="GP110"/>
+      <c r="GQ110"/>
+      <c r="GR110"/>
+      <c r="GS110"/>
+      <c r="GT110"/>
+      <c r="GU110"/>
+      <c r="GV110"/>
+      <c r="GW110"/>
+      <c r="GX110"/>
+      <c r="GY110"/>
+      <c r="GZ110"/>
+      <c r="HA110"/>
+      <c r="HB110"/>
+      <c r="HC110"/>
+      <c r="HD110"/>
+      <c r="HE110"/>
+      <c r="HF110"/>
+      <c r="HG110"/>
+      <c r="HH110"/>
+      <c r="HI110"/>
+      <c r="HJ110"/>
+      <c r="HK110"/>
+      <c r="HL110"/>
+      <c r="HM110"/>
+      <c r="HN110"/>
+      <c r="HO110"/>
+      <c r="HP110"/>
+      <c r="HQ110"/>
+      <c r="HR110"/>
+      <c r="HS110"/>
+      <c r="HT110"/>
+      <c r="HU110"/>
+      <c r="HV110"/>
+      <c r="HW110"/>
+      <c r="HX110"/>
+      <c r="HY110"/>
+      <c r="HZ110"/>
+      <c r="IA110"/>
+      <c r="IB110"/>
+      <c r="IC110"/>
+      <c r="ID110"/>
+      <c r="IE110"/>
+      <c r="IF110"/>
+      <c r="IG110"/>
+      <c r="IH110"/>
+      <c r="II110"/>
+      <c r="IJ110"/>
+      <c r="IK110"/>
+      <c r="IL110"/>
+      <c r="IM110"/>
+      <c r="IN110"/>
+      <c r="IO110"/>
+      <c r="IP110"/>
+      <c r="IQ110"/>
+      <c r="IR110"/>
+      <c r="IS110"/>
+      <c r="IT110"/>
+      <c r="IU110"/>
+      <c r="IV110"/>
+      <c r="IW110"/>
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B111" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C111" s="58" t="s">
         <v>232</v>
-      </c>
-      <c r="C111" s="58" t="s">
-        <v>249</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F111" s="96" t="s">
         <v>13</v>
@@ -17553,11 +18309,11 @@
       <c r="G111" s="25">
         <v>0</v>
       </c>
-      <c r="H111" s="58">
+      <c r="H111" s="97">
         <v>1</v>
       </c>
       <c r="I111" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J111" s="96" t="s">
         <v>29</v>
@@ -17565,29 +18321,29 @@
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B112" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F112" s="96" t="s">
         <v>13</v>
       </c>
       <c r="G112" s="25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H112" s="58">
         <v>1</v>
       </c>
       <c r="I112" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J112" s="96" t="s">
         <v>29</v>
@@ -17595,17 +18351,17 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F113" s="96" t="s">
         <v>13</v>
@@ -17617,7 +18373,7 @@
         <v>1</v>
       </c>
       <c r="I113" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J113" s="96" t="s">
         <v>29</v>
@@ -17625,17 +18381,17 @@
     </row>
     <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B114" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F114" s="96" t="s">
         <v>13</v>
@@ -17647,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="I114" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J114" s="96" t="s">
         <v>29</v>
@@ -17655,29 +18411,29 @@
     </row>
     <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B115" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C115" s="58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F115" s="96" t="s">
         <v>13</v>
       </c>
       <c r="G115" s="25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H115" s="58">
         <v>1</v>
       </c>
       <c r="I115" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J115" s="96" t="s">
         <v>29</v>
@@ -17685,17 +18441,17 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B116" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C116" s="95" t="s">
-        <v>241</v>
+        <v>231</v>
+      </c>
+      <c r="C116" s="58" t="s">
+        <v>237</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F116" s="96" t="s">
         <v>13</v>
@@ -17707,7 +18463,7 @@
         <v>1</v>
       </c>
       <c r="I116" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J116" s="96" t="s">
         <v>29</v>
@@ -17715,17 +18471,17 @@
     </row>
     <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B117" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C117" s="95" t="s">
-        <v>245</v>
+        <v>231</v>
+      </c>
+      <c r="C117" s="58" t="s">
+        <v>242</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F117" s="96" t="s">
         <v>13</v>
@@ -17737,7 +18493,7 @@
         <v>1</v>
       </c>
       <c r="I117" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J117" s="96" t="s">
         <v>29</v>
@@ -17745,17 +18501,17 @@
     </row>
     <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B118" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="B118" s="58" t="s">
-        <v>232</v>
-      </c>
       <c r="C118" s="58" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F118" s="96" t="s">
         <v>13</v>
@@ -17767,7 +18523,7 @@
         <v>1</v>
       </c>
       <c r="I118" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J118" s="96" t="s">
         <v>29</v>
@@ -17775,17 +18531,17 @@
     </row>
     <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="B119" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C119" s="58" t="s">
-        <v>247</v>
+        <v>231</v>
+      </c>
+      <c r="C119" s="95" t="s">
+        <v>240</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F119" s="96" t="s">
         <v>13</v>
@@ -17797,7 +18553,7 @@
         <v>1</v>
       </c>
       <c r="I119" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J119" s="96" t="s">
         <v>29</v>
@@ -17805,17 +18561,17 @@
     </row>
     <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>152</v>
+        <v>243</v>
       </c>
       <c r="B120" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C120" s="58" t="s">
-        <v>168</v>
+        <v>231</v>
+      </c>
+      <c r="C120" s="95" t="s">
+        <v>244</v>
       </c>
       <c r="D120" s="58"/>
       <c r="E120" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F120" s="96" t="s">
         <v>13</v>
@@ -17827,15 +18583,102 @@
         <v>1</v>
       </c>
       <c r="I120" s="96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J120" s="96" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="123" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A121" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B121" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C121" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="D121" s="58"/>
+      <c r="E121" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="F121" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G121" s="25">
+        <v>0</v>
+      </c>
+      <c r="H121" s="58">
+        <v>1</v>
+      </c>
+      <c r="I121" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="J121" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A122" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B122" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C122" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="D122" s="58"/>
+      <c r="E122" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="F122" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" s="25">
+        <v>0</v>
+      </c>
+      <c r="H122" s="58">
+        <v>1</v>
+      </c>
+      <c r="I122" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="J122" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A123" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B123" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C123" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D123" s="58"/>
+      <c r="E123" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="F123" s="96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G123" s="25">
+        <v>0</v>
+      </c>
+      <c r="H123" s="58">
+        <v>1</v>
+      </c>
+      <c r="I123" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="J123" s="96" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="124" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="125" spans="1:10" ht="17.100000000000001" customHeight="1"/>
     <row r="126" spans="1:10" ht="17.100000000000001" customHeight="1"/>
@@ -17847,6 +18690,9 @@
     <row r="132" ht="17.100000000000001" customHeight="1"/>
     <row r="133" ht="17.100000000000001" customHeight="1"/>
     <row r="134" ht="17.100000000000001" customHeight="1"/>
+    <row r="135" ht="17.100000000000001" customHeight="1"/>
+    <row r="136" ht="17.100000000000001" customHeight="1"/>
+    <row r="137" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated field setting file
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD7F9D4-FB76-4380-80DE-D2A32AFC2267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A1AF92-740E-46F4-8FC1-3361E1E0EB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31770" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,9 +709,6 @@
     <t>client_id</t>
   </si>
   <si>
-    <t>referred_from</t>
-  </si>
-  <si>
     <t>client_representing_problem</t>
   </si>
   <si>
@@ -776,6 +773,9 @@
   </si>
   <si>
     <t>Referred From</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -1686,8 +1686,8 @@
   </sheetPr>
   <dimension ref="A1:IW133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -17165,14 +17165,14 @@
         <v>225</v>
       </c>
       <c r="B107" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C107" s="58" t="s">
         <v>232</v>
-      </c>
-      <c r="C107" s="58" t="s">
-        <v>233</v>
       </c>
       <c r="D107" s="58"/>
       <c r="E107" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F107" s="96" t="s">
         <v>13</v>
@@ -17195,14 +17195,14 @@
         <v>226</v>
       </c>
       <c r="B108" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C108" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D108" s="58"/>
       <c r="E108" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F108" s="96" t="s">
         <v>13</v>
@@ -17222,17 +17222,17 @@
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B109" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C109" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F109" s="96" t="s">
         <v>13</v>
@@ -17252,17 +17252,17 @@
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="B110" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C110" s="58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D110" s="58"/>
       <c r="E110" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F110" s="96" t="s">
         <v>13</v>
@@ -17282,17 +17282,17 @@
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B111" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C111" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F111" s="96" t="s">
         <v>13</v>
@@ -17312,17 +17312,17 @@
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B112" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F112" s="96" t="s">
         <v>13</v>
@@ -17342,17 +17342,17 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B113" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C113" s="58" t="s">
         <v>242</v>
-      </c>
-      <c r="B113" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C113" s="58" t="s">
-        <v>243</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F113" s="96" t="s">
         <v>13</v>
@@ -17372,17 +17372,17 @@
     </row>
     <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B114" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F114" s="96" t="s">
         <v>13</v>
@@ -17402,17 +17402,17 @@
     </row>
     <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B115" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C115" s="95" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F115" s="96" t="s">
         <v>13</v>
@@ -17432,17 +17432,17 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B116" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C116" s="95" t="s">
         <v>244</v>
-      </c>
-      <c r="B116" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C116" s="95" t="s">
-        <v>245</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F116" s="96" t="s">
         <v>13</v>
@@ -17462,17 +17462,17 @@
     </row>
     <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="B117" s="58" t="s">
-        <v>232</v>
-      </c>
       <c r="C117" s="58" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F117" s="96" t="s">
         <v>13</v>
@@ -17492,17 +17492,17 @@
     </row>
     <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B118" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C118" s="58" t="s">
         <v>246</v>
-      </c>
-      <c r="B118" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C118" s="58" t="s">
-        <v>247</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F118" s="96" t="s">
         <v>13</v>
@@ -17525,14 +17525,14 @@
         <v>152</v>
       </c>
       <c r="B119" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C119" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F119" s="96" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
fixed legal document field translation and datatype
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE91FA9-391C-4B19-98B1-D29AEF85E564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5F4F66-827E-4B7F-8C0C-448D6627B9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30915" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -634,9 +634,6 @@
     <t>Temporary Travel Documents</t>
   </si>
   <si>
-    <t>referral_doc</t>
-  </si>
-  <si>
     <t>Referral Documents</t>
   </si>
   <si>
@@ -797,6 +794,9 @@
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>screening_interview_form</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1707,8 @@
   </sheetPr>
   <dimension ref="A1:IW137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15947,13 +15947,13 @@
     </row>
     <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B81" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C81" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D81" s="59"/>
       <c r="E81" s="59" t="s">
@@ -16224,13 +16224,13 @@
     </row>
     <row r="82" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A82" s="59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B82" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C82" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D82" s="59"/>
       <c r="E82" s="59" t="s">
@@ -16501,13 +16501,13 @@
     </row>
     <row r="83" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A83" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B83" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C83" s="59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D83" s="59"/>
       <c r="E83" s="59" t="s">
@@ -16778,13 +16778,13 @@
     </row>
     <row r="84" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A84" s="59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B84" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C84" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D84" s="59"/>
       <c r="E84" s="59" t="s">
@@ -17447,13 +17447,13 @@
     </row>
     <row r="99" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A99" s="58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B99" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C99" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D99" s="58"/>
       <c r="E99" s="58" t="s">
@@ -17475,13 +17475,13 @@
     </row>
     <row r="100" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A100" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B100" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C100" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D100" s="58"/>
       <c r="E100" s="58" t="s">
@@ -17503,13 +17503,13 @@
     </row>
     <row r="101" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A101" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B101" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C101" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D101" s="58"/>
       <c r="E101" s="58" t="s">
@@ -17531,13 +17531,13 @@
     </row>
     <row r="102" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="95" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B102" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C102" s="95" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D102" s="58"/>
       <c r="E102" s="95" t="s">
@@ -17561,13 +17561,13 @@
     </row>
     <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="95" t="s">
-        <v>202</v>
+        <v>256</v>
       </c>
       <c r="B103" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C103" s="95" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D103" s="58"/>
       <c r="E103" s="95" t="s">
@@ -17591,13 +17591,13 @@
     </row>
     <row r="104" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B104" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="95" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D104" s="58"/>
       <c r="E104" s="95" t="s">
@@ -17621,13 +17621,13 @@
     </row>
     <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A105" s="95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B105" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C105" s="95" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D105" s="58"/>
       <c r="E105" s="95" t="s">
@@ -17651,13 +17651,13 @@
     </row>
     <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A106" s="95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B106" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C106" s="95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D106" s="58"/>
       <c r="E106" s="95" t="s">
@@ -17681,13 +17681,13 @@
     </row>
     <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A107" s="95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B107" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="95" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D107" s="58"/>
       <c r="E107" s="95" t="s">
@@ -17711,13 +17711,13 @@
     </row>
     <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A108" s="95" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B108" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C108" s="95" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D108" s="58"/>
       <c r="E108" s="95" t="s">
@@ -17741,17 +17741,17 @@
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C109" s="85" t="s">
         <v>78</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="76" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F109" s="76" t="s">
         <v>13</v>
@@ -18016,7 +18016,7 @@
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A110" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B110" s="19" t="s">
         <v>120</v>
@@ -18291,17 +18291,17 @@
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B111" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C111" s="58" t="s">
         <v>230</v>
-      </c>
-      <c r="C111" s="58" t="s">
-        <v>231</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F111" s="96" t="s">
         <v>13</v>
@@ -18321,17 +18321,17 @@
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B112" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F112" s="96" t="s">
         <v>13</v>
@@ -18351,17 +18351,17 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F113" s="96" t="s">
         <v>13</v>
@@ -18381,17 +18381,17 @@
     </row>
     <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B114" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F114" s="96" t="s">
         <v>13</v>
@@ -18411,17 +18411,17 @@
     </row>
     <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B115" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C115" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F115" s="96" t="s">
         <v>13</v>
@@ -18441,17 +18441,17 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B116" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C116" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F116" s="96" t="s">
         <v>13</v>
@@ -18471,17 +18471,17 @@
     </row>
     <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B117" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" s="58" t="s">
         <v>240</v>
-      </c>
-      <c r="B117" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="C117" s="58" t="s">
-        <v>241</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F117" s="96" t="s">
         <v>13</v>
@@ -18501,17 +18501,17 @@
     </row>
     <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B118" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C118" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F118" s="96" t="s">
         <v>13</v>
@@ -18531,17 +18531,17 @@
     </row>
     <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B119" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C119" s="95" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F119" s="96" t="s">
         <v>13</v>
@@ -18561,17 +18561,17 @@
     </row>
     <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B120" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C120" s="95" t="s">
         <v>242</v>
-      </c>
-      <c r="B120" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="C120" s="95" t="s">
-        <v>243</v>
       </c>
       <c r="D120" s="58"/>
       <c r="E120" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F120" s="96" t="s">
         <v>13</v>
@@ -18591,17 +18591,17 @@
     </row>
     <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A121" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B121" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="B121" s="58" t="s">
-        <v>230</v>
-      </c>
       <c r="C121" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D121" s="58"/>
       <c r="E121" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F121" s="96" t="s">
         <v>13</v>
@@ -18621,17 +18621,17 @@
     </row>
     <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A122" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B122" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C122" s="58" t="s">
         <v>244</v>
-      </c>
-      <c r="B122" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="C122" s="58" t="s">
-        <v>245</v>
       </c>
       <c r="D122" s="58"/>
       <c r="E122" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F122" s="96" t="s">
         <v>13</v>
@@ -18654,14 +18654,14 @@
         <v>152</v>
       </c>
       <c r="B123" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C123" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D123" s="58"/>
       <c r="E123" s="96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F123" s="96" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
added field Letter from Immigration Police Legal doc
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5F4F66-827E-4B7F-8C0C-448D6627B9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B39F8D8-6E7D-4762-A1C9-9DB2DE86FA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,9 +667,6 @@
     <t>Legal Representation</t>
   </si>
   <si>
-    <t>police_interview</t>
-  </si>
-  <si>
     <t>Letter from Immigration Police</t>
   </si>
   <si>
@@ -797,6 +794,9 @@
   </si>
   <si>
     <t>screening_interview_form</t>
+  </si>
+  <si>
+    <t>letter_from_immigration_police</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1707,8 @@
   </sheetPr>
   <dimension ref="A1:IW137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15947,13 +15947,13 @@
     </row>
     <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B81" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C81" s="59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D81" s="59"/>
       <c r="E81" s="59" t="s">
@@ -16224,13 +16224,13 @@
     </row>
     <row r="82" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A82" s="59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B82" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C82" s="59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D82" s="59"/>
       <c r="E82" s="59" t="s">
@@ -16501,13 +16501,13 @@
     </row>
     <row r="83" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A83" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B83" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C83" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D83" s="59"/>
       <c r="E83" s="59" t="s">
@@ -16778,13 +16778,13 @@
     </row>
     <row r="84" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A84" s="59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B84" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C84" s="59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D84" s="59"/>
       <c r="E84" s="59" t="s">
@@ -17561,7 +17561,7 @@
     </row>
     <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B103" s="95" t="s">
         <v>11</v>
@@ -17621,13 +17621,13 @@
     </row>
     <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A105" s="95" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="B105" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C105" s="95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D105" s="58"/>
       <c r="E105" s="95" t="s">
@@ -17651,13 +17651,13 @@
     </row>
     <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A106" s="95" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B106" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C106" s="95" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D106" s="58"/>
       <c r="E106" s="95" t="s">
@@ -17681,13 +17681,13 @@
     </row>
     <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A107" s="95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B107" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D107" s="58"/>
       <c r="E107" s="95" t="s">
@@ -17711,13 +17711,13 @@
     </row>
     <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A108" s="95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B108" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C108" s="95" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D108" s="58"/>
       <c r="E108" s="95" t="s">
@@ -17741,17 +17741,17 @@
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C109" s="85" t="s">
         <v>78</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="76" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F109" s="76" t="s">
         <v>13</v>
@@ -18016,7 +18016,7 @@
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A110" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B110" s="19" t="s">
         <v>120</v>
@@ -18291,17 +18291,17 @@
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B111" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C111" s="58" t="s">
         <v>229</v>
-      </c>
-      <c r="C111" s="58" t="s">
-        <v>230</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F111" s="96" t="s">
         <v>13</v>
@@ -18321,17 +18321,17 @@
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B112" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F112" s="96" t="s">
         <v>13</v>
@@ -18351,17 +18351,17 @@
     </row>
     <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F113" s="96" t="s">
         <v>13</v>
@@ -18381,17 +18381,17 @@
     </row>
     <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B114" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F114" s="96" t="s">
         <v>13</v>
@@ -18411,17 +18411,17 @@
     </row>
     <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B115" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C115" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F115" s="96" t="s">
         <v>13</v>
@@ -18441,17 +18441,17 @@
     </row>
     <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B116" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C116" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F116" s="96" t="s">
         <v>13</v>
@@ -18471,17 +18471,17 @@
     </row>
     <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B117" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C117" s="58" t="s">
         <v>239</v>
-      </c>
-      <c r="B117" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="C117" s="58" t="s">
-        <v>240</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F117" s="96" t="s">
         <v>13</v>
@@ -18501,17 +18501,17 @@
     </row>
     <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B118" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C118" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F118" s="96" t="s">
         <v>13</v>
@@ -18531,17 +18531,17 @@
     </row>
     <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B119" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C119" s="95" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F119" s="96" t="s">
         <v>13</v>
@@ -18561,17 +18561,17 @@
     </row>
     <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B120" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C120" s="95" t="s">
         <v>241</v>
-      </c>
-      <c r="B120" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="C120" s="95" t="s">
-        <v>242</v>
       </c>
       <c r="D120" s="58"/>
       <c r="E120" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F120" s="96" t="s">
         <v>13</v>
@@ -18591,17 +18591,17 @@
     </row>
     <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A121" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B121" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="B121" s="58" t="s">
-        <v>229</v>
-      </c>
       <c r="C121" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D121" s="58"/>
       <c r="E121" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F121" s="96" t="s">
         <v>13</v>
@@ -18621,17 +18621,17 @@
     </row>
     <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A122" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C122" s="58" t="s">
         <v>243</v>
-      </c>
-      <c r="B122" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="C122" s="58" t="s">
-        <v>244</v>
       </c>
       <c r="D122" s="58"/>
       <c r="E122" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F122" s="96" t="s">
         <v>13</v>
@@ -18654,14 +18654,14 @@
         <v>152</v>
       </c>
       <c r="B123" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C123" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D123" s="58"/>
       <c r="E123" s="96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F123" s="96" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
added setting for internal referral
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B39F8D8-6E7D-4762-A1C9-9DB2DE86FA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CED9619-A600-429F-AB7C-FE50856C3E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="795" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7155" yWindow="1230" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="260">
   <si>
     <t>name</t>
   </si>
@@ -797,6 +797,15 @@
   </si>
   <si>
     <t>letter_from_immigration_police</t>
+  </si>
+  <si>
+    <t>Internal Referral</t>
+  </si>
+  <si>
+    <t>internal_referral_edit_duration</t>
+  </si>
+  <si>
+    <t>Internal Referral Editable Duration</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1320,6 +1329,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1705,10 +1716,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW137"/>
+  <dimension ref="A1:IW139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -18349,7 +18360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>230</v>
       </c>
@@ -18379,7 +18390,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
         <v>254</v>
       </c>
@@ -18409,7 +18420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
         <v>244</v>
       </c>
@@ -18439,7 +18450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
         <v>224</v>
       </c>
@@ -18469,7 +18480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
         <v>238</v>
       </c>
@@ -18499,7 +18510,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
         <v>225</v>
       </c>
@@ -18529,7 +18540,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
         <v>226</v>
       </c>
@@ -18559,7 +18570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
         <v>240</v>
       </c>
@@ -18589,7 +18600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A121" s="1" t="s">
         <v>227</v>
       </c>
@@ -18619,7 +18630,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A122" s="1" t="s">
         <v>242</v>
       </c>
@@ -18649,7 +18660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A123" s="1" t="s">
         <v>152</v>
       </c>
@@ -18679,11 +18690,563 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="125" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="126" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="127" spans="1:10" ht="17.100000000000001" customHeight="1"/>
-    <row r="128" spans="1:10" ht="17.100000000000001" customHeight="1"/>
+    <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A124" t="s">
+        <v>228</v>
+      </c>
+      <c r="B124" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C124" s="57" t="s">
+        <v>257</v>
+      </c>
+      <c r="D124" s="57"/>
+      <c r="E124" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="F124" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G124" s="81">
+        <v>0</v>
+      </c>
+      <c r="H124" s="57">
+        <v>1</v>
+      </c>
+      <c r="I124" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J124" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K124"/>
+      <c r="L124"/>
+      <c r="M124"/>
+      <c r="N124"/>
+      <c r="O124"/>
+      <c r="P124"/>
+      <c r="Q124"/>
+      <c r="R124"/>
+      <c r="S124"/>
+      <c r="T124"/>
+      <c r="U124"/>
+      <c r="V124"/>
+      <c r="W124"/>
+      <c r="X124"/>
+      <c r="Y124"/>
+      <c r="Z124"/>
+      <c r="AA124"/>
+      <c r="AB124"/>
+      <c r="AC124"/>
+      <c r="AD124"/>
+      <c r="AE124"/>
+      <c r="AF124"/>
+      <c r="AG124"/>
+      <c r="AH124"/>
+      <c r="AI124"/>
+      <c r="AJ124"/>
+      <c r="AK124"/>
+      <c r="AL124"/>
+      <c r="AM124"/>
+      <c r="AN124"/>
+      <c r="AO124"/>
+      <c r="AP124"/>
+      <c r="AQ124"/>
+      <c r="AR124"/>
+      <c r="AS124"/>
+      <c r="AT124"/>
+      <c r="AU124"/>
+      <c r="AV124"/>
+      <c r="AW124"/>
+      <c r="AX124"/>
+      <c r="AY124"/>
+      <c r="AZ124"/>
+      <c r="BA124"/>
+      <c r="BB124"/>
+      <c r="BC124"/>
+      <c r="BD124"/>
+      <c r="BE124"/>
+      <c r="BF124"/>
+      <c r="BG124"/>
+      <c r="BH124"/>
+      <c r="BI124"/>
+      <c r="BJ124"/>
+      <c r="BK124"/>
+      <c r="BL124"/>
+      <c r="BM124"/>
+      <c r="BN124"/>
+      <c r="BO124"/>
+      <c r="BP124"/>
+      <c r="BQ124"/>
+      <c r="BR124"/>
+      <c r="BS124"/>
+      <c r="BT124"/>
+      <c r="BU124"/>
+      <c r="BV124"/>
+      <c r="BW124"/>
+      <c r="BX124"/>
+      <c r="BY124"/>
+      <c r="BZ124"/>
+      <c r="CA124"/>
+      <c r="CB124"/>
+      <c r="CC124"/>
+      <c r="CD124"/>
+      <c r="CE124"/>
+      <c r="CF124"/>
+      <c r="CG124"/>
+      <c r="CH124"/>
+      <c r="CI124"/>
+      <c r="CJ124"/>
+      <c r="CK124"/>
+      <c r="CL124"/>
+      <c r="CM124"/>
+      <c r="CN124"/>
+      <c r="CO124"/>
+      <c r="CP124"/>
+      <c r="CQ124"/>
+      <c r="CR124"/>
+      <c r="CS124"/>
+      <c r="CT124"/>
+      <c r="CU124"/>
+      <c r="CV124"/>
+      <c r="CW124"/>
+      <c r="CX124"/>
+      <c r="CY124"/>
+      <c r="CZ124"/>
+      <c r="DA124"/>
+      <c r="DB124"/>
+      <c r="DC124"/>
+      <c r="DD124"/>
+      <c r="DE124"/>
+      <c r="DF124"/>
+      <c r="DG124"/>
+      <c r="DH124"/>
+      <c r="DI124"/>
+      <c r="DJ124"/>
+      <c r="DK124"/>
+      <c r="DL124"/>
+      <c r="DM124"/>
+      <c r="DN124"/>
+      <c r="DO124"/>
+      <c r="DP124"/>
+      <c r="DQ124"/>
+      <c r="DR124"/>
+      <c r="DS124"/>
+      <c r="DT124"/>
+      <c r="DU124"/>
+      <c r="DV124"/>
+      <c r="DW124"/>
+      <c r="DX124"/>
+      <c r="DY124"/>
+      <c r="DZ124"/>
+      <c r="EA124"/>
+      <c r="EB124"/>
+      <c r="EC124"/>
+      <c r="ED124"/>
+      <c r="EE124"/>
+      <c r="EF124"/>
+      <c r="EG124"/>
+      <c r="EH124"/>
+      <c r="EI124"/>
+      <c r="EJ124"/>
+      <c r="EK124"/>
+      <c r="EL124"/>
+      <c r="EM124"/>
+      <c r="EN124"/>
+      <c r="EO124"/>
+      <c r="EP124"/>
+      <c r="EQ124"/>
+      <c r="ER124"/>
+      <c r="ES124"/>
+      <c r="ET124"/>
+      <c r="EU124"/>
+      <c r="EV124"/>
+      <c r="EW124"/>
+      <c r="EX124"/>
+      <c r="EY124"/>
+      <c r="EZ124"/>
+      <c r="FA124"/>
+      <c r="FB124"/>
+      <c r="FC124"/>
+      <c r="FD124"/>
+      <c r="FE124"/>
+      <c r="FF124"/>
+      <c r="FG124"/>
+      <c r="FH124"/>
+      <c r="FI124"/>
+      <c r="FJ124"/>
+      <c r="FK124"/>
+      <c r="FL124"/>
+      <c r="FM124"/>
+      <c r="FN124"/>
+      <c r="FO124"/>
+      <c r="FP124"/>
+      <c r="FQ124"/>
+      <c r="FR124"/>
+      <c r="FS124"/>
+      <c r="FT124"/>
+      <c r="FU124"/>
+      <c r="FV124"/>
+      <c r="FW124"/>
+      <c r="FX124"/>
+      <c r="FY124"/>
+      <c r="FZ124"/>
+      <c r="GA124"/>
+      <c r="GB124"/>
+      <c r="GC124"/>
+      <c r="GD124"/>
+      <c r="GE124"/>
+      <c r="GF124"/>
+      <c r="GG124"/>
+      <c r="GH124"/>
+      <c r="GI124"/>
+      <c r="GJ124"/>
+      <c r="GK124"/>
+      <c r="GL124"/>
+      <c r="GM124"/>
+      <c r="GN124"/>
+      <c r="GO124"/>
+      <c r="GP124"/>
+      <c r="GQ124"/>
+      <c r="GR124"/>
+      <c r="GS124"/>
+      <c r="GT124"/>
+      <c r="GU124"/>
+      <c r="GV124"/>
+      <c r="GW124"/>
+      <c r="GX124"/>
+      <c r="GY124"/>
+      <c r="GZ124"/>
+      <c r="HA124"/>
+      <c r="HB124"/>
+      <c r="HC124"/>
+      <c r="HD124"/>
+      <c r="HE124"/>
+      <c r="HF124"/>
+      <c r="HG124"/>
+      <c r="HH124"/>
+      <c r="HI124"/>
+      <c r="HJ124"/>
+      <c r="HK124"/>
+      <c r="HL124"/>
+      <c r="HM124"/>
+      <c r="HN124"/>
+      <c r="HO124"/>
+      <c r="HP124"/>
+      <c r="HQ124"/>
+      <c r="HR124"/>
+      <c r="HS124"/>
+      <c r="HT124"/>
+      <c r="HU124"/>
+      <c r="HV124"/>
+      <c r="HW124"/>
+      <c r="HX124"/>
+      <c r="HY124"/>
+      <c r="HZ124"/>
+      <c r="IA124"/>
+      <c r="IB124"/>
+      <c r="IC124"/>
+      <c r="ID124"/>
+      <c r="IE124"/>
+      <c r="IF124"/>
+      <c r="IG124"/>
+      <c r="IH124"/>
+      <c r="II124"/>
+      <c r="IJ124"/>
+      <c r="IK124"/>
+      <c r="IL124"/>
+      <c r="IM124"/>
+      <c r="IN124"/>
+      <c r="IO124"/>
+      <c r="IP124"/>
+      <c r="IQ124"/>
+      <c r="IR124"/>
+      <c r="IS124"/>
+      <c r="IT124"/>
+      <c r="IU124"/>
+      <c r="IV124"/>
+      <c r="IW124"/>
+    </row>
+    <row r="125" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A125" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="B125" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C125" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="D125" s="57"/>
+      <c r="E125" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="F125" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125" s="81">
+        <v>0</v>
+      </c>
+      <c r="H125" s="57">
+        <v>1</v>
+      </c>
+      <c r="I125" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J125" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K125"/>
+      <c r="L125"/>
+      <c r="M125"/>
+      <c r="N125"/>
+      <c r="O125"/>
+      <c r="P125"/>
+      <c r="Q125"/>
+      <c r="R125"/>
+      <c r="S125"/>
+      <c r="T125"/>
+      <c r="U125"/>
+      <c r="V125"/>
+      <c r="W125"/>
+      <c r="X125"/>
+      <c r="Y125"/>
+      <c r="Z125"/>
+      <c r="AA125"/>
+      <c r="AB125"/>
+      <c r="AC125"/>
+      <c r="AD125"/>
+      <c r="AE125"/>
+      <c r="AF125"/>
+      <c r="AG125"/>
+      <c r="AH125"/>
+      <c r="AI125"/>
+      <c r="AJ125"/>
+      <c r="AK125"/>
+      <c r="AL125"/>
+      <c r="AM125"/>
+      <c r="AN125"/>
+      <c r="AO125"/>
+      <c r="AP125"/>
+      <c r="AQ125"/>
+      <c r="AR125"/>
+      <c r="AS125"/>
+      <c r="AT125"/>
+      <c r="AU125"/>
+      <c r="AV125"/>
+      <c r="AW125"/>
+      <c r="AX125"/>
+      <c r="AY125"/>
+      <c r="AZ125"/>
+      <c r="BA125"/>
+      <c r="BB125"/>
+      <c r="BC125"/>
+      <c r="BD125"/>
+      <c r="BE125"/>
+      <c r="BF125"/>
+      <c r="BG125"/>
+      <c r="BH125"/>
+      <c r="BI125"/>
+      <c r="BJ125"/>
+      <c r="BK125"/>
+      <c r="BL125"/>
+      <c r="BM125"/>
+      <c r="BN125"/>
+      <c r="BO125"/>
+      <c r="BP125"/>
+      <c r="BQ125"/>
+      <c r="BR125"/>
+      <c r="BS125"/>
+      <c r="BT125"/>
+      <c r="BU125"/>
+      <c r="BV125"/>
+      <c r="BW125"/>
+      <c r="BX125"/>
+      <c r="BY125"/>
+      <c r="BZ125"/>
+      <c r="CA125"/>
+      <c r="CB125"/>
+      <c r="CC125"/>
+      <c r="CD125"/>
+      <c r="CE125"/>
+      <c r="CF125"/>
+      <c r="CG125"/>
+      <c r="CH125"/>
+      <c r="CI125"/>
+      <c r="CJ125"/>
+      <c r="CK125"/>
+      <c r="CL125"/>
+      <c r="CM125"/>
+      <c r="CN125"/>
+      <c r="CO125"/>
+      <c r="CP125"/>
+      <c r="CQ125"/>
+      <c r="CR125"/>
+      <c r="CS125"/>
+      <c r="CT125"/>
+      <c r="CU125"/>
+      <c r="CV125"/>
+      <c r="CW125"/>
+      <c r="CX125"/>
+      <c r="CY125"/>
+      <c r="CZ125"/>
+      <c r="DA125"/>
+      <c r="DB125"/>
+      <c r="DC125"/>
+      <c r="DD125"/>
+      <c r="DE125"/>
+      <c r="DF125"/>
+      <c r="DG125"/>
+      <c r="DH125"/>
+      <c r="DI125"/>
+      <c r="DJ125"/>
+      <c r="DK125"/>
+      <c r="DL125"/>
+      <c r="DM125"/>
+      <c r="DN125"/>
+      <c r="DO125"/>
+      <c r="DP125"/>
+      <c r="DQ125"/>
+      <c r="DR125"/>
+      <c r="DS125"/>
+      <c r="DT125"/>
+      <c r="DU125"/>
+      <c r="DV125"/>
+      <c r="DW125"/>
+      <c r="DX125"/>
+      <c r="DY125"/>
+      <c r="DZ125"/>
+      <c r="EA125"/>
+      <c r="EB125"/>
+      <c r="EC125"/>
+      <c r="ED125"/>
+      <c r="EE125"/>
+      <c r="EF125"/>
+      <c r="EG125"/>
+      <c r="EH125"/>
+      <c r="EI125"/>
+      <c r="EJ125"/>
+      <c r="EK125"/>
+      <c r="EL125"/>
+      <c r="EM125"/>
+      <c r="EN125"/>
+      <c r="EO125"/>
+      <c r="EP125"/>
+      <c r="EQ125"/>
+      <c r="ER125"/>
+      <c r="ES125"/>
+      <c r="ET125"/>
+      <c r="EU125"/>
+      <c r="EV125"/>
+      <c r="EW125"/>
+      <c r="EX125"/>
+      <c r="EY125"/>
+      <c r="EZ125"/>
+      <c r="FA125"/>
+      <c r="FB125"/>
+      <c r="FC125"/>
+      <c r="FD125"/>
+      <c r="FE125"/>
+      <c r="FF125"/>
+      <c r="FG125"/>
+      <c r="FH125"/>
+      <c r="FI125"/>
+      <c r="FJ125"/>
+      <c r="FK125"/>
+      <c r="FL125"/>
+      <c r="FM125"/>
+      <c r="FN125"/>
+      <c r="FO125"/>
+      <c r="FP125"/>
+      <c r="FQ125"/>
+      <c r="FR125"/>
+      <c r="FS125"/>
+      <c r="FT125"/>
+      <c r="FU125"/>
+      <c r="FV125"/>
+      <c r="FW125"/>
+      <c r="FX125"/>
+      <c r="FY125"/>
+      <c r="FZ125"/>
+      <c r="GA125"/>
+      <c r="GB125"/>
+      <c r="GC125"/>
+      <c r="GD125"/>
+      <c r="GE125"/>
+      <c r="GF125"/>
+      <c r="GG125"/>
+      <c r="GH125"/>
+      <c r="GI125"/>
+      <c r="GJ125"/>
+      <c r="GK125"/>
+      <c r="GL125"/>
+      <c r="GM125"/>
+      <c r="GN125"/>
+      <c r="GO125"/>
+      <c r="GP125"/>
+      <c r="GQ125"/>
+      <c r="GR125"/>
+      <c r="GS125"/>
+      <c r="GT125"/>
+      <c r="GU125"/>
+      <c r="GV125"/>
+      <c r="GW125"/>
+      <c r="GX125"/>
+      <c r="GY125"/>
+      <c r="GZ125"/>
+      <c r="HA125"/>
+      <c r="HB125"/>
+      <c r="HC125"/>
+      <c r="HD125"/>
+      <c r="HE125"/>
+      <c r="HF125"/>
+      <c r="HG125"/>
+      <c r="HH125"/>
+      <c r="HI125"/>
+      <c r="HJ125"/>
+      <c r="HK125"/>
+      <c r="HL125"/>
+      <c r="HM125"/>
+      <c r="HN125"/>
+      <c r="HO125"/>
+      <c r="HP125"/>
+      <c r="HQ125"/>
+      <c r="HR125"/>
+      <c r="HS125"/>
+      <c r="HT125"/>
+      <c r="HU125"/>
+      <c r="HV125"/>
+      <c r="HW125"/>
+      <c r="HX125"/>
+      <c r="HY125"/>
+      <c r="HZ125"/>
+      <c r="IA125"/>
+      <c r="IB125"/>
+      <c r="IC125"/>
+      <c r="ID125"/>
+      <c r="IE125"/>
+      <c r="IF125"/>
+      <c r="IG125"/>
+      <c r="IH125"/>
+      <c r="II125"/>
+      <c r="IJ125"/>
+      <c r="IK125"/>
+      <c r="IL125"/>
+      <c r="IM125"/>
+      <c r="IN125"/>
+      <c r="IO125"/>
+      <c r="IP125"/>
+      <c r="IQ125"/>
+      <c r="IR125"/>
+      <c r="IS125"/>
+      <c r="IT125"/>
+      <c r="IU125"/>
+      <c r="IV125"/>
+      <c r="IW125"/>
+    </row>
+    <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
     <row r="130" ht="17.100000000000001" customHeight="1"/>
     <row r="131" ht="17.100000000000001" customHeight="1"/>
@@ -18693,6 +19256,8 @@
     <row r="135" ht="17.100000000000001" customHeight="1"/>
     <row r="136" ht="17.100000000000001" customHeight="1"/>
     <row r="137" ht="17.100000000000001" customHeight="1"/>
+    <row r="138" ht="17.100000000000001" customHeight="1"/>
+    <row r="139" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added option to disable future date picker to case note task
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CED9619-A600-429F-AB7C-FE50856C3E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F44B3C-970A-4334-ADD6-B30571ECD02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7155" yWindow="1230" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="263">
   <si>
     <t>name</t>
   </si>
@@ -806,6 +806,15 @@
   </si>
   <si>
     <t>Internal Referral Editable Duration</t>
+  </si>
+  <si>
+    <t>disable_future_completion_date</t>
+  </si>
+  <si>
+    <t>case_note</t>
+  </si>
+  <si>
+    <t>Disable Future Completion Date for Task</t>
   </si>
 </sst>
 </file>
@@ -1716,10 +1725,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW139"/>
+  <dimension ref="A1:IW140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J126" sqref="J126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -19244,7 +19253,283 @@
       <c r="IV125"/>
       <c r="IW125"/>
     </row>
-    <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A126" s="99" t="s">
+        <v>260</v>
+      </c>
+      <c r="B126" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="C126" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="D126" s="57"/>
+      <c r="E126" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="F126" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G126" s="81">
+        <v>0</v>
+      </c>
+      <c r="H126" s="57">
+        <v>1</v>
+      </c>
+      <c r="I126" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J126" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K126"/>
+      <c r="L126"/>
+      <c r="M126"/>
+      <c r="N126"/>
+      <c r="O126"/>
+      <c r="P126"/>
+      <c r="Q126"/>
+      <c r="R126"/>
+      <c r="S126"/>
+      <c r="T126"/>
+      <c r="U126"/>
+      <c r="V126"/>
+      <c r="W126"/>
+      <c r="X126"/>
+      <c r="Y126"/>
+      <c r="Z126"/>
+      <c r="AA126"/>
+      <c r="AB126"/>
+      <c r="AC126"/>
+      <c r="AD126"/>
+      <c r="AE126"/>
+      <c r="AF126"/>
+      <c r="AG126"/>
+      <c r="AH126"/>
+      <c r="AI126"/>
+      <c r="AJ126"/>
+      <c r="AK126"/>
+      <c r="AL126"/>
+      <c r="AM126"/>
+      <c r="AN126"/>
+      <c r="AO126"/>
+      <c r="AP126"/>
+      <c r="AQ126"/>
+      <c r="AR126"/>
+      <c r="AS126"/>
+      <c r="AT126"/>
+      <c r="AU126"/>
+      <c r="AV126"/>
+      <c r="AW126"/>
+      <c r="AX126"/>
+      <c r="AY126"/>
+      <c r="AZ126"/>
+      <c r="BA126"/>
+      <c r="BB126"/>
+      <c r="BC126"/>
+      <c r="BD126"/>
+      <c r="BE126"/>
+      <c r="BF126"/>
+      <c r="BG126"/>
+      <c r="BH126"/>
+      <c r="BI126"/>
+      <c r="BJ126"/>
+      <c r="BK126"/>
+      <c r="BL126"/>
+      <c r="BM126"/>
+      <c r="BN126"/>
+      <c r="BO126"/>
+      <c r="BP126"/>
+      <c r="BQ126"/>
+      <c r="BR126"/>
+      <c r="BS126"/>
+      <c r="BT126"/>
+      <c r="BU126"/>
+      <c r="BV126"/>
+      <c r="BW126"/>
+      <c r="BX126"/>
+      <c r="BY126"/>
+      <c r="BZ126"/>
+      <c r="CA126"/>
+      <c r="CB126"/>
+      <c r="CC126"/>
+      <c r="CD126"/>
+      <c r="CE126"/>
+      <c r="CF126"/>
+      <c r="CG126"/>
+      <c r="CH126"/>
+      <c r="CI126"/>
+      <c r="CJ126"/>
+      <c r="CK126"/>
+      <c r="CL126"/>
+      <c r="CM126"/>
+      <c r="CN126"/>
+      <c r="CO126"/>
+      <c r="CP126"/>
+      <c r="CQ126"/>
+      <c r="CR126"/>
+      <c r="CS126"/>
+      <c r="CT126"/>
+      <c r="CU126"/>
+      <c r="CV126"/>
+      <c r="CW126"/>
+      <c r="CX126"/>
+      <c r="CY126"/>
+      <c r="CZ126"/>
+      <c r="DA126"/>
+      <c r="DB126"/>
+      <c r="DC126"/>
+      <c r="DD126"/>
+      <c r="DE126"/>
+      <c r="DF126"/>
+      <c r="DG126"/>
+      <c r="DH126"/>
+      <c r="DI126"/>
+      <c r="DJ126"/>
+      <c r="DK126"/>
+      <c r="DL126"/>
+      <c r="DM126"/>
+      <c r="DN126"/>
+      <c r="DO126"/>
+      <c r="DP126"/>
+      <c r="DQ126"/>
+      <c r="DR126"/>
+      <c r="DS126"/>
+      <c r="DT126"/>
+      <c r="DU126"/>
+      <c r="DV126"/>
+      <c r="DW126"/>
+      <c r="DX126"/>
+      <c r="DY126"/>
+      <c r="DZ126"/>
+      <c r="EA126"/>
+      <c r="EB126"/>
+      <c r="EC126"/>
+      <c r="ED126"/>
+      <c r="EE126"/>
+      <c r="EF126"/>
+      <c r="EG126"/>
+      <c r="EH126"/>
+      <c r="EI126"/>
+      <c r="EJ126"/>
+      <c r="EK126"/>
+      <c r="EL126"/>
+      <c r="EM126"/>
+      <c r="EN126"/>
+      <c r="EO126"/>
+      <c r="EP126"/>
+      <c r="EQ126"/>
+      <c r="ER126"/>
+      <c r="ES126"/>
+      <c r="ET126"/>
+      <c r="EU126"/>
+      <c r="EV126"/>
+      <c r="EW126"/>
+      <c r="EX126"/>
+      <c r="EY126"/>
+      <c r="EZ126"/>
+      <c r="FA126"/>
+      <c r="FB126"/>
+      <c r="FC126"/>
+      <c r="FD126"/>
+      <c r="FE126"/>
+      <c r="FF126"/>
+      <c r="FG126"/>
+      <c r="FH126"/>
+      <c r="FI126"/>
+      <c r="FJ126"/>
+      <c r="FK126"/>
+      <c r="FL126"/>
+      <c r="FM126"/>
+      <c r="FN126"/>
+      <c r="FO126"/>
+      <c r="FP126"/>
+      <c r="FQ126"/>
+      <c r="FR126"/>
+      <c r="FS126"/>
+      <c r="FT126"/>
+      <c r="FU126"/>
+      <c r="FV126"/>
+      <c r="FW126"/>
+      <c r="FX126"/>
+      <c r="FY126"/>
+      <c r="FZ126"/>
+      <c r="GA126"/>
+      <c r="GB126"/>
+      <c r="GC126"/>
+      <c r="GD126"/>
+      <c r="GE126"/>
+      <c r="GF126"/>
+      <c r="GG126"/>
+      <c r="GH126"/>
+      <c r="GI126"/>
+      <c r="GJ126"/>
+      <c r="GK126"/>
+      <c r="GL126"/>
+      <c r="GM126"/>
+      <c r="GN126"/>
+      <c r="GO126"/>
+      <c r="GP126"/>
+      <c r="GQ126"/>
+      <c r="GR126"/>
+      <c r="GS126"/>
+      <c r="GT126"/>
+      <c r="GU126"/>
+      <c r="GV126"/>
+      <c r="GW126"/>
+      <c r="GX126"/>
+      <c r="GY126"/>
+      <c r="GZ126"/>
+      <c r="HA126"/>
+      <c r="HB126"/>
+      <c r="HC126"/>
+      <c r="HD126"/>
+      <c r="HE126"/>
+      <c r="HF126"/>
+      <c r="HG126"/>
+      <c r="HH126"/>
+      <c r="HI126"/>
+      <c r="HJ126"/>
+      <c r="HK126"/>
+      <c r="HL126"/>
+      <c r="HM126"/>
+      <c r="HN126"/>
+      <c r="HO126"/>
+      <c r="HP126"/>
+      <c r="HQ126"/>
+      <c r="HR126"/>
+      <c r="HS126"/>
+      <c r="HT126"/>
+      <c r="HU126"/>
+      <c r="HV126"/>
+      <c r="HW126"/>
+      <c r="HX126"/>
+      <c r="HY126"/>
+      <c r="HZ126"/>
+      <c r="IA126"/>
+      <c r="IB126"/>
+      <c r="IC126"/>
+      <c r="ID126"/>
+      <c r="IE126"/>
+      <c r="IF126"/>
+      <c r="IG126"/>
+      <c r="IH126"/>
+      <c r="II126"/>
+      <c r="IJ126"/>
+      <c r="IK126"/>
+      <c r="IL126"/>
+      <c r="IM126"/>
+      <c r="IN126"/>
+      <c r="IO126"/>
+      <c r="IP126"/>
+      <c r="IQ126"/>
+      <c r="IR126"/>
+      <c r="IS126"/>
+      <c r="IT126"/>
+      <c r="IU126"/>
+      <c r="IV126"/>
+      <c r="IW126"/>
+    </row>
     <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
@@ -19258,6 +19543,7 @@
     <row r="137" ht="17.100000000000001" customHeight="1"/>
     <row r="138" ht="17.100000000000001" customHeight="1"/>
     <row r="139" ht="17.100000000000001" customHeight="1"/>
+    <row r="140" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated case note limit setting
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F44B3C-970A-4334-ADD6-B30571ECD02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC624A6-B3AC-4C75-A50E-D57F535F6BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="265">
   <si>
     <t>name</t>
   </si>
@@ -815,6 +815,12 @@
   </si>
   <si>
     <t>Disable Future Completion Date for Task</t>
+  </si>
+  <si>
+    <t>case_note_edit_limit</t>
+  </si>
+  <si>
+    <t>Implementation Log Edit Limitation</t>
   </si>
 </sst>
 </file>
@@ -1725,10 +1731,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW140"/>
+  <dimension ref="A1:IW141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J126" sqref="J126"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -19530,7 +19536,283 @@
       <c r="IV126"/>
       <c r="IW126"/>
     </row>
-    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A127" s="99" t="s">
+        <v>263</v>
+      </c>
+      <c r="B127" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="C127" s="98" t="s">
+        <v>264</v>
+      </c>
+      <c r="D127" s="57"/>
+      <c r="E127" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="F127" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="81">
+        <v>0</v>
+      </c>
+      <c r="H127" s="57">
+        <v>1</v>
+      </c>
+      <c r="I127" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J127" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127"/>
+      <c r="N127"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
+      <c r="R127"/>
+      <c r="S127"/>
+      <c r="T127"/>
+      <c r="U127"/>
+      <c r="V127"/>
+      <c r="W127"/>
+      <c r="X127"/>
+      <c r="Y127"/>
+      <c r="Z127"/>
+      <c r="AA127"/>
+      <c r="AB127"/>
+      <c r="AC127"/>
+      <c r="AD127"/>
+      <c r="AE127"/>
+      <c r="AF127"/>
+      <c r="AG127"/>
+      <c r="AH127"/>
+      <c r="AI127"/>
+      <c r="AJ127"/>
+      <c r="AK127"/>
+      <c r="AL127"/>
+      <c r="AM127"/>
+      <c r="AN127"/>
+      <c r="AO127"/>
+      <c r="AP127"/>
+      <c r="AQ127"/>
+      <c r="AR127"/>
+      <c r="AS127"/>
+      <c r="AT127"/>
+      <c r="AU127"/>
+      <c r="AV127"/>
+      <c r="AW127"/>
+      <c r="AX127"/>
+      <c r="AY127"/>
+      <c r="AZ127"/>
+      <c r="BA127"/>
+      <c r="BB127"/>
+      <c r="BC127"/>
+      <c r="BD127"/>
+      <c r="BE127"/>
+      <c r="BF127"/>
+      <c r="BG127"/>
+      <c r="BH127"/>
+      <c r="BI127"/>
+      <c r="BJ127"/>
+      <c r="BK127"/>
+      <c r="BL127"/>
+      <c r="BM127"/>
+      <c r="BN127"/>
+      <c r="BO127"/>
+      <c r="BP127"/>
+      <c r="BQ127"/>
+      <c r="BR127"/>
+      <c r="BS127"/>
+      <c r="BT127"/>
+      <c r="BU127"/>
+      <c r="BV127"/>
+      <c r="BW127"/>
+      <c r="BX127"/>
+      <c r="BY127"/>
+      <c r="BZ127"/>
+      <c r="CA127"/>
+      <c r="CB127"/>
+      <c r="CC127"/>
+      <c r="CD127"/>
+      <c r="CE127"/>
+      <c r="CF127"/>
+      <c r="CG127"/>
+      <c r="CH127"/>
+      <c r="CI127"/>
+      <c r="CJ127"/>
+      <c r="CK127"/>
+      <c r="CL127"/>
+      <c r="CM127"/>
+      <c r="CN127"/>
+      <c r="CO127"/>
+      <c r="CP127"/>
+      <c r="CQ127"/>
+      <c r="CR127"/>
+      <c r="CS127"/>
+      <c r="CT127"/>
+      <c r="CU127"/>
+      <c r="CV127"/>
+      <c r="CW127"/>
+      <c r="CX127"/>
+      <c r="CY127"/>
+      <c r="CZ127"/>
+      <c r="DA127"/>
+      <c r="DB127"/>
+      <c r="DC127"/>
+      <c r="DD127"/>
+      <c r="DE127"/>
+      <c r="DF127"/>
+      <c r="DG127"/>
+      <c r="DH127"/>
+      <c r="DI127"/>
+      <c r="DJ127"/>
+      <c r="DK127"/>
+      <c r="DL127"/>
+      <c r="DM127"/>
+      <c r="DN127"/>
+      <c r="DO127"/>
+      <c r="DP127"/>
+      <c r="DQ127"/>
+      <c r="DR127"/>
+      <c r="DS127"/>
+      <c r="DT127"/>
+      <c r="DU127"/>
+      <c r="DV127"/>
+      <c r="DW127"/>
+      <c r="DX127"/>
+      <c r="DY127"/>
+      <c r="DZ127"/>
+      <c r="EA127"/>
+      <c r="EB127"/>
+      <c r="EC127"/>
+      <c r="ED127"/>
+      <c r="EE127"/>
+      <c r="EF127"/>
+      <c r="EG127"/>
+      <c r="EH127"/>
+      <c r="EI127"/>
+      <c r="EJ127"/>
+      <c r="EK127"/>
+      <c r="EL127"/>
+      <c r="EM127"/>
+      <c r="EN127"/>
+      <c r="EO127"/>
+      <c r="EP127"/>
+      <c r="EQ127"/>
+      <c r="ER127"/>
+      <c r="ES127"/>
+      <c r="ET127"/>
+      <c r="EU127"/>
+      <c r="EV127"/>
+      <c r="EW127"/>
+      <c r="EX127"/>
+      <c r="EY127"/>
+      <c r="EZ127"/>
+      <c r="FA127"/>
+      <c r="FB127"/>
+      <c r="FC127"/>
+      <c r="FD127"/>
+      <c r="FE127"/>
+      <c r="FF127"/>
+      <c r="FG127"/>
+      <c r="FH127"/>
+      <c r="FI127"/>
+      <c r="FJ127"/>
+      <c r="FK127"/>
+      <c r="FL127"/>
+      <c r="FM127"/>
+      <c r="FN127"/>
+      <c r="FO127"/>
+      <c r="FP127"/>
+      <c r="FQ127"/>
+      <c r="FR127"/>
+      <c r="FS127"/>
+      <c r="FT127"/>
+      <c r="FU127"/>
+      <c r="FV127"/>
+      <c r="FW127"/>
+      <c r="FX127"/>
+      <c r="FY127"/>
+      <c r="FZ127"/>
+      <c r="GA127"/>
+      <c r="GB127"/>
+      <c r="GC127"/>
+      <c r="GD127"/>
+      <c r="GE127"/>
+      <c r="GF127"/>
+      <c r="GG127"/>
+      <c r="GH127"/>
+      <c r="GI127"/>
+      <c r="GJ127"/>
+      <c r="GK127"/>
+      <c r="GL127"/>
+      <c r="GM127"/>
+      <c r="GN127"/>
+      <c r="GO127"/>
+      <c r="GP127"/>
+      <c r="GQ127"/>
+      <c r="GR127"/>
+      <c r="GS127"/>
+      <c r="GT127"/>
+      <c r="GU127"/>
+      <c r="GV127"/>
+      <c r="GW127"/>
+      <c r="GX127"/>
+      <c r="GY127"/>
+      <c r="GZ127"/>
+      <c r="HA127"/>
+      <c r="HB127"/>
+      <c r="HC127"/>
+      <c r="HD127"/>
+      <c r="HE127"/>
+      <c r="HF127"/>
+      <c r="HG127"/>
+      <c r="HH127"/>
+      <c r="HI127"/>
+      <c r="HJ127"/>
+      <c r="HK127"/>
+      <c r="HL127"/>
+      <c r="HM127"/>
+      <c r="HN127"/>
+      <c r="HO127"/>
+      <c r="HP127"/>
+      <c r="HQ127"/>
+      <c r="HR127"/>
+      <c r="HS127"/>
+      <c r="HT127"/>
+      <c r="HU127"/>
+      <c r="HV127"/>
+      <c r="HW127"/>
+      <c r="HX127"/>
+      <c r="HY127"/>
+      <c r="HZ127"/>
+      <c r="IA127"/>
+      <c r="IB127"/>
+      <c r="IC127"/>
+      <c r="ID127"/>
+      <c r="IE127"/>
+      <c r="IF127"/>
+      <c r="IG127"/>
+      <c r="IH127"/>
+      <c r="II127"/>
+      <c r="IJ127"/>
+      <c r="IK127"/>
+      <c r="IL127"/>
+      <c r="IM127"/>
+      <c r="IN127"/>
+      <c r="IO127"/>
+      <c r="IP127"/>
+      <c r="IQ127"/>
+      <c r="IR127"/>
+      <c r="IS127"/>
+      <c r="IT127"/>
+      <c r="IU127"/>
+      <c r="IV127"/>
+      <c r="IW127"/>
+    </row>
     <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
     <row r="130" ht="17.100000000000001" customHeight="1"/>
@@ -19544,6 +19826,7 @@
     <row r="138" ht="17.100000000000001" customHeight="1"/>
     <row r="139" ht="17.100000000000001" customHeight="1"/>
     <row r="140" ht="17.100000000000001" customHeight="1"/>
+    <row r="141" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
removed service received from setting spreadsheet
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC624A6-B3AC-4C75-A50E-D57F535F6BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4139C4-6C0F-4A48-8F2D-88FADC8987A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="263">
   <si>
     <t>name</t>
   </si>
@@ -770,12 +770,6 @@
   </si>
   <si>
     <t>Task Completed Date</t>
-  </si>
-  <si>
-    <t>service_received</t>
-  </si>
-  <si>
-    <t>Service Received</t>
   </si>
   <si>
     <t>done_by</t>
@@ -1731,10 +1725,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW141"/>
+  <dimension ref="A1:IW140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:XFD81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15973,13 +15967,13 @@
     </row>
     <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="59" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B81" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C81" s="59" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D81" s="59"/>
       <c r="E81" s="59" t="s">
@@ -16250,13 +16244,13 @@
     </row>
     <row r="82" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A82" s="59" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B82" s="59" t="s">
         <v>157</v>
       </c>
       <c r="C82" s="59" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D82" s="59"/>
       <c r="E82" s="59" t="s">
@@ -16802,292 +16796,43 @@
       <c r="IV83" s="60"/>
       <c r="IW83" s="60"/>
     </row>
-    <row r="84" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A84" s="59" t="s">
-        <v>252</v>
-      </c>
-      <c r="B84" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="C84" s="59" t="s">
-        <v>253</v>
-      </c>
-      <c r="D84" s="59"/>
-      <c r="E84" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="F84" s="59" t="s">
+    <row r="84" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A84" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="D84" s="58"/>
+      <c r="E84" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G84" s="59">
+      <c r="G84" s="58">
         <v>0</v>
       </c>
-      <c r="H84" s="59">
+      <c r="H84" s="58">
         <v>1</v>
       </c>
-      <c r="I84" s="63" t="s">
-        <v>173</v>
-      </c>
-      <c r="J84" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="K84" s="60"/>
-      <c r="L84" s="60"/>
-      <c r="M84" s="60"/>
-      <c r="N84" s="60"/>
-      <c r="O84" s="60"/>
-      <c r="P84" s="60"/>
-      <c r="Q84" s="60"/>
-      <c r="R84" s="60"/>
-      <c r="S84" s="60"/>
-      <c r="T84" s="60"/>
-      <c r="U84" s="60"/>
-      <c r="V84" s="60"/>
-      <c r="W84" s="60"/>
-      <c r="X84" s="60"/>
-      <c r="Y84" s="60"/>
-      <c r="Z84" s="60"/>
-      <c r="AA84" s="60"/>
-      <c r="AB84" s="60"/>
-      <c r="AC84" s="60"/>
-      <c r="AD84" s="60"/>
-      <c r="AE84" s="60"/>
-      <c r="AF84" s="60"/>
-      <c r="AG84" s="60"/>
-      <c r="AH84" s="60"/>
-      <c r="AI84" s="60"/>
-      <c r="AJ84" s="60"/>
-      <c r="AK84" s="60"/>
-      <c r="AL84" s="60"/>
-      <c r="AM84" s="60"/>
-      <c r="AN84" s="60"/>
-      <c r="AO84" s="60"/>
-      <c r="AP84" s="60"/>
-      <c r="AQ84" s="60"/>
-      <c r="AR84" s="60"/>
-      <c r="AS84" s="60"/>
-      <c r="AT84" s="60"/>
-      <c r="AU84" s="60"/>
-      <c r="AV84" s="60"/>
-      <c r="AW84" s="60"/>
-      <c r="AX84" s="60"/>
-      <c r="AY84" s="60"/>
-      <c r="AZ84" s="60"/>
-      <c r="BA84" s="60"/>
-      <c r="BB84" s="60"/>
-      <c r="BC84" s="60"/>
-      <c r="BD84" s="60"/>
-      <c r="BE84" s="60"/>
-      <c r="BF84" s="60"/>
-      <c r="BG84" s="60"/>
-      <c r="BH84" s="60"/>
-      <c r="BI84" s="60"/>
-      <c r="BJ84" s="60"/>
-      <c r="BK84" s="60"/>
-      <c r="BL84" s="60"/>
-      <c r="BM84" s="60"/>
-      <c r="BN84" s="60"/>
-      <c r="BO84" s="60"/>
-      <c r="BP84" s="60"/>
-      <c r="BQ84" s="60"/>
-      <c r="BR84" s="60"/>
-      <c r="BS84" s="60"/>
-      <c r="BT84" s="60"/>
-      <c r="BU84" s="60"/>
-      <c r="BV84" s="60"/>
-      <c r="BW84" s="60"/>
-      <c r="BX84" s="60"/>
-      <c r="BY84" s="60"/>
-      <c r="BZ84" s="60"/>
-      <c r="CA84" s="60"/>
-      <c r="CB84" s="60"/>
-      <c r="CC84" s="60"/>
-      <c r="CD84" s="60"/>
-      <c r="CE84" s="60"/>
-      <c r="CF84" s="60"/>
-      <c r="CG84" s="60"/>
-      <c r="CH84" s="60"/>
-      <c r="CI84" s="60"/>
-      <c r="CJ84" s="60"/>
-      <c r="CK84" s="60"/>
-      <c r="CL84" s="60"/>
-      <c r="CM84" s="60"/>
-      <c r="CN84" s="60"/>
-      <c r="CO84" s="60"/>
-      <c r="CP84" s="60"/>
-      <c r="CQ84" s="60"/>
-      <c r="CR84" s="60"/>
-      <c r="CS84" s="60"/>
-      <c r="CT84" s="60"/>
-      <c r="CU84" s="60"/>
-      <c r="CV84" s="60"/>
-      <c r="CW84" s="60"/>
-      <c r="CX84" s="60"/>
-      <c r="CY84" s="60"/>
-      <c r="CZ84" s="60"/>
-      <c r="DA84" s="60"/>
-      <c r="DB84" s="60"/>
-      <c r="DC84" s="60"/>
-      <c r="DD84" s="60"/>
-      <c r="DE84" s="60"/>
-      <c r="DF84" s="60"/>
-      <c r="DG84" s="60"/>
-      <c r="DH84" s="60"/>
-      <c r="DI84" s="60"/>
-      <c r="DJ84" s="60"/>
-      <c r="DK84" s="60"/>
-      <c r="DL84" s="60"/>
-      <c r="DM84" s="60"/>
-      <c r="DN84" s="60"/>
-      <c r="DO84" s="60"/>
-      <c r="DP84" s="60"/>
-      <c r="DQ84" s="60"/>
-      <c r="DR84" s="60"/>
-      <c r="DS84" s="60"/>
-      <c r="DT84" s="60"/>
-      <c r="DU84" s="60"/>
-      <c r="DV84" s="60"/>
-      <c r="DW84" s="60"/>
-      <c r="DX84" s="60"/>
-      <c r="DY84" s="60"/>
-      <c r="DZ84" s="60"/>
-      <c r="EA84" s="60"/>
-      <c r="EB84" s="60"/>
-      <c r="EC84" s="60"/>
-      <c r="ED84" s="60"/>
-      <c r="EE84" s="60"/>
-      <c r="EF84" s="60"/>
-      <c r="EG84" s="60"/>
-      <c r="EH84" s="60"/>
-      <c r="EI84" s="60"/>
-      <c r="EJ84" s="60"/>
-      <c r="EK84" s="60"/>
-      <c r="EL84" s="60"/>
-      <c r="EM84" s="60"/>
-      <c r="EN84" s="60"/>
-      <c r="EO84" s="60"/>
-      <c r="EP84" s="60"/>
-      <c r="EQ84" s="60"/>
-      <c r="ER84" s="60"/>
-      <c r="ES84" s="60"/>
-      <c r="ET84" s="60"/>
-      <c r="EU84" s="60"/>
-      <c r="EV84" s="60"/>
-      <c r="EW84" s="60"/>
-      <c r="EX84" s="60"/>
-      <c r="EY84" s="60"/>
-      <c r="EZ84" s="60"/>
-      <c r="FA84" s="60"/>
-      <c r="FB84" s="60"/>
-      <c r="FC84" s="60"/>
-      <c r="FD84" s="60"/>
-      <c r="FE84" s="60"/>
-      <c r="FF84" s="60"/>
-      <c r="FG84" s="60"/>
-      <c r="FH84" s="60"/>
-      <c r="FI84" s="60"/>
-      <c r="FJ84" s="60"/>
-      <c r="FK84" s="60"/>
-      <c r="FL84" s="60"/>
-      <c r="FM84" s="60"/>
-      <c r="FN84" s="60"/>
-      <c r="FO84" s="60"/>
-      <c r="FP84" s="60"/>
-      <c r="FQ84" s="60"/>
-      <c r="FR84" s="60"/>
-      <c r="FS84" s="60"/>
-      <c r="FT84" s="60"/>
-      <c r="FU84" s="60"/>
-      <c r="FV84" s="60"/>
-      <c r="FW84" s="60"/>
-      <c r="FX84" s="60"/>
-      <c r="FY84" s="60"/>
-      <c r="FZ84" s="60"/>
-      <c r="GA84" s="60"/>
-      <c r="GB84" s="60"/>
-      <c r="GC84" s="60"/>
-      <c r="GD84" s="60"/>
-      <c r="GE84" s="60"/>
-      <c r="GF84" s="60"/>
-      <c r="GG84" s="60"/>
-      <c r="GH84" s="60"/>
-      <c r="GI84" s="60"/>
-      <c r="GJ84" s="60"/>
-      <c r="GK84" s="60"/>
-      <c r="GL84" s="60"/>
-      <c r="GM84" s="60"/>
-      <c r="GN84" s="60"/>
-      <c r="GO84" s="60"/>
-      <c r="GP84" s="60"/>
-      <c r="GQ84" s="60"/>
-      <c r="GR84" s="60"/>
-      <c r="GS84" s="60"/>
-      <c r="GT84" s="60"/>
-      <c r="GU84" s="60"/>
-      <c r="GV84" s="60"/>
-      <c r="GW84" s="60"/>
-      <c r="GX84" s="60"/>
-      <c r="GY84" s="60"/>
-      <c r="GZ84" s="60"/>
-      <c r="HA84" s="60"/>
-      <c r="HB84" s="60"/>
-      <c r="HC84" s="60"/>
-      <c r="HD84" s="60"/>
-      <c r="HE84" s="60"/>
-      <c r="HF84" s="60"/>
-      <c r="HG84" s="60"/>
-      <c r="HH84" s="60"/>
-      <c r="HI84" s="60"/>
-      <c r="HJ84" s="60"/>
-      <c r="HK84" s="60"/>
-      <c r="HL84" s="60"/>
-      <c r="HM84" s="60"/>
-      <c r="HN84" s="60"/>
-      <c r="HO84" s="60"/>
-      <c r="HP84" s="60"/>
-      <c r="HQ84" s="60"/>
-      <c r="HR84" s="60"/>
-      <c r="HS84" s="60"/>
-      <c r="HT84" s="60"/>
-      <c r="HU84" s="60"/>
-      <c r="HV84" s="60"/>
-      <c r="HW84" s="60"/>
-      <c r="HX84" s="60"/>
-      <c r="HY84" s="60"/>
-      <c r="HZ84" s="60"/>
-      <c r="IA84" s="60"/>
-      <c r="IB84" s="60"/>
-      <c r="IC84" s="60"/>
-      <c r="ID84" s="60"/>
-      <c r="IE84" s="60"/>
-      <c r="IF84" s="60"/>
-      <c r="IG84" s="60"/>
-      <c r="IH84" s="60"/>
-      <c r="II84" s="60"/>
-      <c r="IJ84" s="60"/>
-      <c r="IK84" s="60"/>
-      <c r="IL84" s="60"/>
-      <c r="IM84" s="60"/>
-      <c r="IN84" s="60"/>
-      <c r="IO84" s="60"/>
-      <c r="IP84" s="60"/>
-      <c r="IQ84" s="60"/>
-      <c r="IR84" s="60"/>
-      <c r="IS84" s="60"/>
-      <c r="IT84" s="60"/>
-      <c r="IU84" s="60"/>
-      <c r="IV84" s="60"/>
-      <c r="IW84" s="60"/>
+      <c r="I84" s="58"/>
+      <c r="J84" s="58" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="85" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A85" s="58" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B85" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C85" s="58" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D85" s="58"/>
       <c r="E85" s="58" t="s">
@@ -17109,13 +16854,13 @@
     </row>
     <row r="86" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A86" s="58" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B86" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C86" s="58" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D86" s="58"/>
       <c r="E86" s="58" t="s">
@@ -17137,13 +16882,13 @@
     </row>
     <row r="87" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A87" s="58" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B87" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="58" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D87" s="58"/>
       <c r="E87" s="58" t="s">
@@ -17165,13 +16910,13 @@
     </row>
     <row r="88" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A88" s="58" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B88" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C88" s="58" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D88" s="58"/>
       <c r="E88" s="58" t="s">
@@ -17193,13 +16938,13 @@
     </row>
     <row r="89" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A89" s="58" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B89" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C89" s="58" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D89" s="58"/>
       <c r="E89" s="58" t="s">
@@ -17221,13 +16966,13 @@
     </row>
     <row r="90" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A90" s="58" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B90" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C90" s="58" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D90" s="58"/>
       <c r="E90" s="58" t="s">
@@ -17249,13 +16994,13 @@
     </row>
     <row r="91" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A91" s="58" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B91" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="58" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D91" s="58"/>
       <c r="E91" s="58" t="s">
@@ -17277,13 +17022,13 @@
     </row>
     <row r="92" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A92" s="58" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B92" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="58" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D92" s="58"/>
       <c r="E92" s="58" t="s">
@@ -17305,13 +17050,13 @@
     </row>
     <row r="93" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A93" s="58" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B93" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C93" s="58" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D93" s="58"/>
       <c r="E93" s="58" t="s">
@@ -17333,13 +17078,13 @@
     </row>
     <row r="94" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A94" s="58" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B94" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="58" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D94" s="58"/>
       <c r="E94" s="58" t="s">
@@ -17361,13 +17106,13 @@
     </row>
     <row r="95" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A95" s="58" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B95" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C95" s="58" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D95" s="58"/>
       <c r="E95" s="58" t="s">
@@ -17389,13 +17134,13 @@
     </row>
     <row r="96" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A96" s="58" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B96" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C96" s="58" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D96" s="58"/>
       <c r="E96" s="58" t="s">
@@ -17412,18 +17157,18 @@
       </c>
       <c r="I96" s="58"/>
       <c r="J96" s="58" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="97" spans="1:257" ht="18" customHeight="1">
       <c r="A97" s="58" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B97" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C97" s="58" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D97" s="58"/>
       <c r="E97" s="58" t="s">
@@ -17443,15 +17188,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:257" ht="18" customHeight="1">
+    <row r="98" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A98" s="58" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B98" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C98" s="58" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D98" s="58"/>
       <c r="E98" s="58" t="s">
@@ -17473,13 +17218,13 @@
     </row>
     <row r="99" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A99" s="58" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B99" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C99" s="58" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D99" s="58"/>
       <c r="E99" s="58" t="s">
@@ -17501,13 +17246,13 @@
     </row>
     <row r="100" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A100" s="58" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B100" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C100" s="58" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D100" s="58"/>
       <c r="E100" s="58" t="s">
@@ -17528,20 +17273,20 @@
       </c>
     </row>
     <row r="101" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A101" s="58" t="s">
-        <v>205</v>
-      </c>
-      <c r="B101" s="58" t="s">
+      <c r="A101" s="95" t="s">
+        <v>208</v>
+      </c>
+      <c r="B101" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="58" t="s">
-        <v>206</v>
+      <c r="C101" s="95" t="s">
+        <v>209</v>
       </c>
       <c r="D101" s="58"/>
-      <c r="E101" s="58" t="s">
+      <c r="E101" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="F101" s="58" t="s">
+      <c r="F101" s="95" t="s">
         <v>13</v>
       </c>
       <c r="G101" s="58">
@@ -17550,20 +17295,22 @@
       <c r="H101" s="58">
         <v>1</v>
       </c>
-      <c r="I101" s="58"/>
-      <c r="J101" s="58" t="s">
-        <v>3</v>
+      <c r="I101" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="J101" s="95" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="95" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="B102" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C102" s="95" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D102" s="58"/>
       <c r="E102" s="95" t="s">
@@ -17582,18 +17329,18 @@
         <v>173</v>
       </c>
       <c r="J102" s="95" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="95" t="s">
-        <v>255</v>
+        <v>211</v>
       </c>
       <c r="B103" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C103" s="95" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D103" s="58"/>
       <c r="E103" s="95" t="s">
@@ -17612,18 +17359,18 @@
         <v>173</v>
       </c>
       <c r="J103" s="95" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="95" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="B104" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="95" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D104" s="58"/>
       <c r="E104" s="95" t="s">
@@ -17642,18 +17389,18 @@
         <v>173</v>
       </c>
       <c r="J104" s="95" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A105" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="B105" s="95" t="s">
+        <v>216</v>
+      </c>
+      <c r="B105" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C105" s="95" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D105" s="58"/>
       <c r="E105" s="95" t="s">
@@ -17672,18 +17419,18 @@
         <v>173</v>
       </c>
       <c r="J105" s="95" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A106" s="95" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B106" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C106" s="95" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D106" s="58"/>
       <c r="E106" s="95" t="s">
@@ -17707,13 +17454,13 @@
     </row>
     <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A107" s="95" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B107" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="95" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D107" s="58"/>
       <c r="E107" s="95" t="s">
@@ -17736,48 +17483,293 @@
       </c>
     </row>
     <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A108" s="95" t="s">
-        <v>218</v>
-      </c>
-      <c r="B108" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" s="95" t="s">
-        <v>219</v>
+      <c r="A108" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C108" s="85" t="s">
+        <v>78</v>
       </c>
       <c r="D108" s="58"/>
-      <c r="E108" s="95" t="s">
-        <v>11</v>
-      </c>
-      <c r="F108" s="95" t="s">
+      <c r="E108" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F108" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="G108" s="58">
+      <c r="G108" s="25">
         <v>0</v>
       </c>
-      <c r="H108" s="58">
+      <c r="H108" s="25">
         <v>1</v>
       </c>
-      <c r="I108" s="95" t="s">
-        <v>173</v>
-      </c>
-      <c r="J108" s="95" t="s">
-        <v>3</v>
-      </c>
+      <c r="I108" s="10"/>
+      <c r="J108" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K108"/>
+      <c r="L108"/>
+      <c r="M108"/>
+      <c r="N108"/>
+      <c r="O108"/>
+      <c r="P108"/>
+      <c r="Q108"/>
+      <c r="R108"/>
+      <c r="S108"/>
+      <c r="T108"/>
+      <c r="U108"/>
+      <c r="V108"/>
+      <c r="W108"/>
+      <c r="X108"/>
+      <c r="Y108"/>
+      <c r="Z108"/>
+      <c r="AA108"/>
+      <c r="AB108"/>
+      <c r="AC108"/>
+      <c r="AD108"/>
+      <c r="AE108"/>
+      <c r="AF108"/>
+      <c r="AG108"/>
+      <c r="AH108"/>
+      <c r="AI108"/>
+      <c r="AJ108"/>
+      <c r="AK108"/>
+      <c r="AL108"/>
+      <c r="AM108"/>
+      <c r="AN108"/>
+      <c r="AO108"/>
+      <c r="AP108"/>
+      <c r="AQ108"/>
+      <c r="AR108"/>
+      <c r="AS108"/>
+      <c r="AT108"/>
+      <c r="AU108"/>
+      <c r="AV108"/>
+      <c r="AW108"/>
+      <c r="AX108"/>
+      <c r="AY108"/>
+      <c r="AZ108"/>
+      <c r="BA108"/>
+      <c r="BB108"/>
+      <c r="BC108"/>
+      <c r="BD108"/>
+      <c r="BE108"/>
+      <c r="BF108"/>
+      <c r="BG108"/>
+      <c r="BH108"/>
+      <c r="BI108"/>
+      <c r="BJ108"/>
+      <c r="BK108"/>
+      <c r="BL108"/>
+      <c r="BM108"/>
+      <c r="BN108"/>
+      <c r="BO108"/>
+      <c r="BP108"/>
+      <c r="BQ108"/>
+      <c r="BR108"/>
+      <c r="BS108"/>
+      <c r="BT108"/>
+      <c r="BU108"/>
+      <c r="BV108"/>
+      <c r="BW108"/>
+      <c r="BX108"/>
+      <c r="BY108"/>
+      <c r="BZ108"/>
+      <c r="CA108"/>
+      <c r="CB108"/>
+      <c r="CC108"/>
+      <c r="CD108"/>
+      <c r="CE108"/>
+      <c r="CF108"/>
+      <c r="CG108"/>
+      <c r="CH108"/>
+      <c r="CI108"/>
+      <c r="CJ108"/>
+      <c r="CK108"/>
+      <c r="CL108"/>
+      <c r="CM108"/>
+      <c r="CN108"/>
+      <c r="CO108"/>
+      <c r="CP108"/>
+      <c r="CQ108"/>
+      <c r="CR108"/>
+      <c r="CS108"/>
+      <c r="CT108"/>
+      <c r="CU108"/>
+      <c r="CV108"/>
+      <c r="CW108"/>
+      <c r="CX108"/>
+      <c r="CY108"/>
+      <c r="CZ108"/>
+      <c r="DA108"/>
+      <c r="DB108"/>
+      <c r="DC108"/>
+      <c r="DD108"/>
+      <c r="DE108"/>
+      <c r="DF108"/>
+      <c r="DG108"/>
+      <c r="DH108"/>
+      <c r="DI108"/>
+      <c r="DJ108"/>
+      <c r="DK108"/>
+      <c r="DL108"/>
+      <c r="DM108"/>
+      <c r="DN108"/>
+      <c r="DO108"/>
+      <c r="DP108"/>
+      <c r="DQ108"/>
+      <c r="DR108"/>
+      <c r="DS108"/>
+      <c r="DT108"/>
+      <c r="DU108"/>
+      <c r="DV108"/>
+      <c r="DW108"/>
+      <c r="DX108"/>
+      <c r="DY108"/>
+      <c r="DZ108"/>
+      <c r="EA108"/>
+      <c r="EB108"/>
+      <c r="EC108"/>
+      <c r="ED108"/>
+      <c r="EE108"/>
+      <c r="EF108"/>
+      <c r="EG108"/>
+      <c r="EH108"/>
+      <c r="EI108"/>
+      <c r="EJ108"/>
+      <c r="EK108"/>
+      <c r="EL108"/>
+      <c r="EM108"/>
+      <c r="EN108"/>
+      <c r="EO108"/>
+      <c r="EP108"/>
+      <c r="EQ108"/>
+      <c r="ER108"/>
+      <c r="ES108"/>
+      <c r="ET108"/>
+      <c r="EU108"/>
+      <c r="EV108"/>
+      <c r="EW108"/>
+      <c r="EX108"/>
+      <c r="EY108"/>
+      <c r="EZ108"/>
+      <c r="FA108"/>
+      <c r="FB108"/>
+      <c r="FC108"/>
+      <c r="FD108"/>
+      <c r="FE108"/>
+      <c r="FF108"/>
+      <c r="FG108"/>
+      <c r="FH108"/>
+      <c r="FI108"/>
+      <c r="FJ108"/>
+      <c r="FK108"/>
+      <c r="FL108"/>
+      <c r="FM108"/>
+      <c r="FN108"/>
+      <c r="FO108"/>
+      <c r="FP108"/>
+      <c r="FQ108"/>
+      <c r="FR108"/>
+      <c r="FS108"/>
+      <c r="FT108"/>
+      <c r="FU108"/>
+      <c r="FV108"/>
+      <c r="FW108"/>
+      <c r="FX108"/>
+      <c r="FY108"/>
+      <c r="FZ108"/>
+      <c r="GA108"/>
+      <c r="GB108"/>
+      <c r="GC108"/>
+      <c r="GD108"/>
+      <c r="GE108"/>
+      <c r="GF108"/>
+      <c r="GG108"/>
+      <c r="GH108"/>
+      <c r="GI108"/>
+      <c r="GJ108"/>
+      <c r="GK108"/>
+      <c r="GL108"/>
+      <c r="GM108"/>
+      <c r="GN108"/>
+      <c r="GO108"/>
+      <c r="GP108"/>
+      <c r="GQ108"/>
+      <c r="GR108"/>
+      <c r="GS108"/>
+      <c r="GT108"/>
+      <c r="GU108"/>
+      <c r="GV108"/>
+      <c r="GW108"/>
+      <c r="GX108"/>
+      <c r="GY108"/>
+      <c r="GZ108"/>
+      <c r="HA108"/>
+      <c r="HB108"/>
+      <c r="HC108"/>
+      <c r="HD108"/>
+      <c r="HE108"/>
+      <c r="HF108"/>
+      <c r="HG108"/>
+      <c r="HH108"/>
+      <c r="HI108"/>
+      <c r="HJ108"/>
+      <c r="HK108"/>
+      <c r="HL108"/>
+      <c r="HM108"/>
+      <c r="HN108"/>
+      <c r="HO108"/>
+      <c r="HP108"/>
+      <c r="HQ108"/>
+      <c r="HR108"/>
+      <c r="HS108"/>
+      <c r="HT108"/>
+      <c r="HU108"/>
+      <c r="HV108"/>
+      <c r="HW108"/>
+      <c r="HX108"/>
+      <c r="HY108"/>
+      <c r="HZ108"/>
+      <c r="IA108"/>
+      <c r="IB108"/>
+      <c r="IC108"/>
+      <c r="ID108"/>
+      <c r="IE108"/>
+      <c r="IF108"/>
+      <c r="IG108"/>
+      <c r="IH108"/>
+      <c r="II108"/>
+      <c r="IJ108"/>
+      <c r="IK108"/>
+      <c r="IL108"/>
+      <c r="IM108"/>
+      <c r="IN108"/>
+      <c r="IO108"/>
+      <c r="IP108"/>
+      <c r="IQ108"/>
+      <c r="IR108"/>
+      <c r="IS108"/>
+      <c r="IT108"/>
+      <c r="IU108"/>
+      <c r="IV108"/>
+      <c r="IW108"/>
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="19" t="s">
         <v>221</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="C109" s="85" t="s">
         <v>78</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="76" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="F109" s="76" t="s">
         <v>13</v>
@@ -18041,289 +18033,44 @@
       <c r="IW109"/>
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A110" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="B110" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C110" s="85" t="s">
-        <v>78</v>
+      <c r="A110" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B110" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C110" s="58" t="s">
+        <v>229</v>
       </c>
       <c r="D110" s="58"/>
-      <c r="E110" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="F110" s="76" t="s">
+      <c r="E110" s="96" t="s">
+        <v>228</v>
+      </c>
+      <c r="F110" s="96" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="25">
         <v>0</v>
       </c>
-      <c r="H110" s="25">
+      <c r="H110" s="97">
         <v>1</v>
       </c>
-      <c r="I110" s="10"/>
-      <c r="J110" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K110"/>
-      <c r="L110"/>
-      <c r="M110"/>
-      <c r="N110"/>
-      <c r="O110"/>
-      <c r="P110"/>
-      <c r="Q110"/>
-      <c r="R110"/>
-      <c r="S110"/>
-      <c r="T110"/>
-      <c r="U110"/>
-      <c r="V110"/>
-      <c r="W110"/>
-      <c r="X110"/>
-      <c r="Y110"/>
-      <c r="Z110"/>
-      <c r="AA110"/>
-      <c r="AB110"/>
-      <c r="AC110"/>
-      <c r="AD110"/>
-      <c r="AE110"/>
-      <c r="AF110"/>
-      <c r="AG110"/>
-      <c r="AH110"/>
-      <c r="AI110"/>
-      <c r="AJ110"/>
-      <c r="AK110"/>
-      <c r="AL110"/>
-      <c r="AM110"/>
-      <c r="AN110"/>
-      <c r="AO110"/>
-      <c r="AP110"/>
-      <c r="AQ110"/>
-      <c r="AR110"/>
-      <c r="AS110"/>
-      <c r="AT110"/>
-      <c r="AU110"/>
-      <c r="AV110"/>
-      <c r="AW110"/>
-      <c r="AX110"/>
-      <c r="AY110"/>
-      <c r="AZ110"/>
-      <c r="BA110"/>
-      <c r="BB110"/>
-      <c r="BC110"/>
-      <c r="BD110"/>
-      <c r="BE110"/>
-      <c r="BF110"/>
-      <c r="BG110"/>
-      <c r="BH110"/>
-      <c r="BI110"/>
-      <c r="BJ110"/>
-      <c r="BK110"/>
-      <c r="BL110"/>
-      <c r="BM110"/>
-      <c r="BN110"/>
-      <c r="BO110"/>
-      <c r="BP110"/>
-      <c r="BQ110"/>
-      <c r="BR110"/>
-      <c r="BS110"/>
-      <c r="BT110"/>
-      <c r="BU110"/>
-      <c r="BV110"/>
-      <c r="BW110"/>
-      <c r="BX110"/>
-      <c r="BY110"/>
-      <c r="BZ110"/>
-      <c r="CA110"/>
-      <c r="CB110"/>
-      <c r="CC110"/>
-      <c r="CD110"/>
-      <c r="CE110"/>
-      <c r="CF110"/>
-      <c r="CG110"/>
-      <c r="CH110"/>
-      <c r="CI110"/>
-      <c r="CJ110"/>
-      <c r="CK110"/>
-      <c r="CL110"/>
-      <c r="CM110"/>
-      <c r="CN110"/>
-      <c r="CO110"/>
-      <c r="CP110"/>
-      <c r="CQ110"/>
-      <c r="CR110"/>
-      <c r="CS110"/>
-      <c r="CT110"/>
-      <c r="CU110"/>
-      <c r="CV110"/>
-      <c r="CW110"/>
-      <c r="CX110"/>
-      <c r="CY110"/>
-      <c r="CZ110"/>
-      <c r="DA110"/>
-      <c r="DB110"/>
-      <c r="DC110"/>
-      <c r="DD110"/>
-      <c r="DE110"/>
-      <c r="DF110"/>
-      <c r="DG110"/>
-      <c r="DH110"/>
-      <c r="DI110"/>
-      <c r="DJ110"/>
-      <c r="DK110"/>
-      <c r="DL110"/>
-      <c r="DM110"/>
-      <c r="DN110"/>
-      <c r="DO110"/>
-      <c r="DP110"/>
-      <c r="DQ110"/>
-      <c r="DR110"/>
-      <c r="DS110"/>
-      <c r="DT110"/>
-      <c r="DU110"/>
-      <c r="DV110"/>
-      <c r="DW110"/>
-      <c r="DX110"/>
-      <c r="DY110"/>
-      <c r="DZ110"/>
-      <c r="EA110"/>
-      <c r="EB110"/>
-      <c r="EC110"/>
-      <c r="ED110"/>
-      <c r="EE110"/>
-      <c r="EF110"/>
-      <c r="EG110"/>
-      <c r="EH110"/>
-      <c r="EI110"/>
-      <c r="EJ110"/>
-      <c r="EK110"/>
-      <c r="EL110"/>
-      <c r="EM110"/>
-      <c r="EN110"/>
-      <c r="EO110"/>
-      <c r="EP110"/>
-      <c r="EQ110"/>
-      <c r="ER110"/>
-      <c r="ES110"/>
-      <c r="ET110"/>
-      <c r="EU110"/>
-      <c r="EV110"/>
-      <c r="EW110"/>
-      <c r="EX110"/>
-      <c r="EY110"/>
-      <c r="EZ110"/>
-      <c r="FA110"/>
-      <c r="FB110"/>
-      <c r="FC110"/>
-      <c r="FD110"/>
-      <c r="FE110"/>
-      <c r="FF110"/>
-      <c r="FG110"/>
-      <c r="FH110"/>
-      <c r="FI110"/>
-      <c r="FJ110"/>
-      <c r="FK110"/>
-      <c r="FL110"/>
-      <c r="FM110"/>
-      <c r="FN110"/>
-      <c r="FO110"/>
-      <c r="FP110"/>
-      <c r="FQ110"/>
-      <c r="FR110"/>
-      <c r="FS110"/>
-      <c r="FT110"/>
-      <c r="FU110"/>
-      <c r="FV110"/>
-      <c r="FW110"/>
-      <c r="FX110"/>
-      <c r="FY110"/>
-      <c r="FZ110"/>
-      <c r="GA110"/>
-      <c r="GB110"/>
-      <c r="GC110"/>
-      <c r="GD110"/>
-      <c r="GE110"/>
-      <c r="GF110"/>
-      <c r="GG110"/>
-      <c r="GH110"/>
-      <c r="GI110"/>
-      <c r="GJ110"/>
-      <c r="GK110"/>
-      <c r="GL110"/>
-      <c r="GM110"/>
-      <c r="GN110"/>
-      <c r="GO110"/>
-      <c r="GP110"/>
-      <c r="GQ110"/>
-      <c r="GR110"/>
-      <c r="GS110"/>
-      <c r="GT110"/>
-      <c r="GU110"/>
-      <c r="GV110"/>
-      <c r="GW110"/>
-      <c r="GX110"/>
-      <c r="GY110"/>
-      <c r="GZ110"/>
-      <c r="HA110"/>
-      <c r="HB110"/>
-      <c r="HC110"/>
-      <c r="HD110"/>
-      <c r="HE110"/>
-      <c r="HF110"/>
-      <c r="HG110"/>
-      <c r="HH110"/>
-      <c r="HI110"/>
-      <c r="HJ110"/>
-      <c r="HK110"/>
-      <c r="HL110"/>
-      <c r="HM110"/>
-      <c r="HN110"/>
-      <c r="HO110"/>
-      <c r="HP110"/>
-      <c r="HQ110"/>
-      <c r="HR110"/>
-      <c r="HS110"/>
-      <c r="HT110"/>
-      <c r="HU110"/>
-      <c r="HV110"/>
-      <c r="HW110"/>
-      <c r="HX110"/>
-      <c r="HY110"/>
-      <c r="HZ110"/>
-      <c r="IA110"/>
-      <c r="IB110"/>
-      <c r="IC110"/>
-      <c r="ID110"/>
-      <c r="IE110"/>
-      <c r="IF110"/>
-      <c r="IG110"/>
-      <c r="IH110"/>
-      <c r="II110"/>
-      <c r="IJ110"/>
-      <c r="IK110"/>
-      <c r="IL110"/>
-      <c r="IM110"/>
-      <c r="IN110"/>
-      <c r="IO110"/>
-      <c r="IP110"/>
-      <c r="IQ110"/>
-      <c r="IR110"/>
-      <c r="IS110"/>
-      <c r="IT110"/>
-      <c r="IU110"/>
-      <c r="IV110"/>
-      <c r="IW110"/>
+      <c r="I110" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="J110" s="96" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B111" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C111" s="58" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D111" s="58"/>
       <c r="E111" s="96" t="s">
@@ -18335,7 +18082,7 @@
       <c r="G111" s="25">
         <v>0</v>
       </c>
-      <c r="H111" s="97">
+      <c r="H111" s="58">
         <v>1</v>
       </c>
       <c r="I111" s="96" t="s">
@@ -18347,13 +18094,13 @@
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B112" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
@@ -18377,13 +18124,13 @@
     </row>
     <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="B113" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
@@ -18407,13 +18154,13 @@
     </row>
     <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B114" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
@@ -18423,7 +18170,7 @@
         <v>13</v>
       </c>
       <c r="G114" s="25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H114" s="58">
         <v>1</v>
@@ -18437,13 +18184,13 @@
     </row>
     <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B115" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C115" s="58" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
@@ -18453,7 +18200,7 @@
         <v>13</v>
       </c>
       <c r="G115" s="25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H115" s="58">
         <v>1</v>
@@ -18467,13 +18214,13 @@
     </row>
     <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="B116" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C116" s="58" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
@@ -18497,13 +18244,13 @@
     </row>
     <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B117" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C117" s="58" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
@@ -18527,13 +18274,13 @@
     </row>
     <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B118" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C118" s="58" t="s">
-        <v>235</v>
+      <c r="C118" s="95" t="s">
+        <v>237</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
@@ -18557,13 +18304,13 @@
     </row>
     <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B119" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C119" s="95" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
@@ -18587,13 +18334,13 @@
     </row>
     <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B120" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C120" s="95" t="s">
-        <v>241</v>
+      <c r="C120" s="58" t="s">
+        <v>236</v>
       </c>
       <c r="D120" s="58"/>
       <c r="E120" s="96" t="s">
@@ -18617,13 +18364,13 @@
     </row>
     <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="B121" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C121" s="58" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D121" s="58"/>
       <c r="E121" s="96" t="s">
@@ -18647,13 +18394,13 @@
     </row>
     <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>242</v>
+        <v>152</v>
       </c>
       <c r="B122" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C122" s="58" t="s">
-        <v>243</v>
+        <v>167</v>
       </c>
       <c r="D122" s="58"/>
       <c r="E122" s="96" t="s">
@@ -18676,43 +18423,290 @@
       </c>
     </row>
     <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A123" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B123" s="58" t="s">
+      <c r="A123" t="s">
         <v>228</v>
       </c>
-      <c r="C123" s="58" t="s">
-        <v>167</v>
-      </c>
-      <c r="D123" s="58"/>
-      <c r="E123" s="96" t="s">
+      <c r="B123" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="F123" s="96" t="s">
+      <c r="C123" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="D123" s="57"/>
+      <c r="E123" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="F123" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="G123" s="25">
+      <c r="G123" s="81">
         <v>0</v>
       </c>
-      <c r="H123" s="58">
+      <c r="H123" s="57">
         <v>1</v>
       </c>
-      <c r="I123" s="96" t="s">
+      <c r="I123" s="98" t="s">
         <v>173</v>
       </c>
-      <c r="J123" s="96" t="s">
+      <c r="J123" s="98" t="s">
         <v>29</v>
       </c>
+      <c r="K123"/>
+      <c r="L123"/>
+      <c r="M123"/>
+      <c r="N123"/>
+      <c r="O123"/>
+      <c r="P123"/>
+      <c r="Q123"/>
+      <c r="R123"/>
+      <c r="S123"/>
+      <c r="T123"/>
+      <c r="U123"/>
+      <c r="V123"/>
+      <c r="W123"/>
+      <c r="X123"/>
+      <c r="Y123"/>
+      <c r="Z123"/>
+      <c r="AA123"/>
+      <c r="AB123"/>
+      <c r="AC123"/>
+      <c r="AD123"/>
+      <c r="AE123"/>
+      <c r="AF123"/>
+      <c r="AG123"/>
+      <c r="AH123"/>
+      <c r="AI123"/>
+      <c r="AJ123"/>
+      <c r="AK123"/>
+      <c r="AL123"/>
+      <c r="AM123"/>
+      <c r="AN123"/>
+      <c r="AO123"/>
+      <c r="AP123"/>
+      <c r="AQ123"/>
+      <c r="AR123"/>
+      <c r="AS123"/>
+      <c r="AT123"/>
+      <c r="AU123"/>
+      <c r="AV123"/>
+      <c r="AW123"/>
+      <c r="AX123"/>
+      <c r="AY123"/>
+      <c r="AZ123"/>
+      <c r="BA123"/>
+      <c r="BB123"/>
+      <c r="BC123"/>
+      <c r="BD123"/>
+      <c r="BE123"/>
+      <c r="BF123"/>
+      <c r="BG123"/>
+      <c r="BH123"/>
+      <c r="BI123"/>
+      <c r="BJ123"/>
+      <c r="BK123"/>
+      <c r="BL123"/>
+      <c r="BM123"/>
+      <c r="BN123"/>
+      <c r="BO123"/>
+      <c r="BP123"/>
+      <c r="BQ123"/>
+      <c r="BR123"/>
+      <c r="BS123"/>
+      <c r="BT123"/>
+      <c r="BU123"/>
+      <c r="BV123"/>
+      <c r="BW123"/>
+      <c r="BX123"/>
+      <c r="BY123"/>
+      <c r="BZ123"/>
+      <c r="CA123"/>
+      <c r="CB123"/>
+      <c r="CC123"/>
+      <c r="CD123"/>
+      <c r="CE123"/>
+      <c r="CF123"/>
+      <c r="CG123"/>
+      <c r="CH123"/>
+      <c r="CI123"/>
+      <c r="CJ123"/>
+      <c r="CK123"/>
+      <c r="CL123"/>
+      <c r="CM123"/>
+      <c r="CN123"/>
+      <c r="CO123"/>
+      <c r="CP123"/>
+      <c r="CQ123"/>
+      <c r="CR123"/>
+      <c r="CS123"/>
+      <c r="CT123"/>
+      <c r="CU123"/>
+      <c r="CV123"/>
+      <c r="CW123"/>
+      <c r="CX123"/>
+      <c r="CY123"/>
+      <c r="CZ123"/>
+      <c r="DA123"/>
+      <c r="DB123"/>
+      <c r="DC123"/>
+      <c r="DD123"/>
+      <c r="DE123"/>
+      <c r="DF123"/>
+      <c r="DG123"/>
+      <c r="DH123"/>
+      <c r="DI123"/>
+      <c r="DJ123"/>
+      <c r="DK123"/>
+      <c r="DL123"/>
+      <c r="DM123"/>
+      <c r="DN123"/>
+      <c r="DO123"/>
+      <c r="DP123"/>
+      <c r="DQ123"/>
+      <c r="DR123"/>
+      <c r="DS123"/>
+      <c r="DT123"/>
+      <c r="DU123"/>
+      <c r="DV123"/>
+      <c r="DW123"/>
+      <c r="DX123"/>
+      <c r="DY123"/>
+      <c r="DZ123"/>
+      <c r="EA123"/>
+      <c r="EB123"/>
+      <c r="EC123"/>
+      <c r="ED123"/>
+      <c r="EE123"/>
+      <c r="EF123"/>
+      <c r="EG123"/>
+      <c r="EH123"/>
+      <c r="EI123"/>
+      <c r="EJ123"/>
+      <c r="EK123"/>
+      <c r="EL123"/>
+      <c r="EM123"/>
+      <c r="EN123"/>
+      <c r="EO123"/>
+      <c r="EP123"/>
+      <c r="EQ123"/>
+      <c r="ER123"/>
+      <c r="ES123"/>
+      <c r="ET123"/>
+      <c r="EU123"/>
+      <c r="EV123"/>
+      <c r="EW123"/>
+      <c r="EX123"/>
+      <c r="EY123"/>
+      <c r="EZ123"/>
+      <c r="FA123"/>
+      <c r="FB123"/>
+      <c r="FC123"/>
+      <c r="FD123"/>
+      <c r="FE123"/>
+      <c r="FF123"/>
+      <c r="FG123"/>
+      <c r="FH123"/>
+      <c r="FI123"/>
+      <c r="FJ123"/>
+      <c r="FK123"/>
+      <c r="FL123"/>
+      <c r="FM123"/>
+      <c r="FN123"/>
+      <c r="FO123"/>
+      <c r="FP123"/>
+      <c r="FQ123"/>
+      <c r="FR123"/>
+      <c r="FS123"/>
+      <c r="FT123"/>
+      <c r="FU123"/>
+      <c r="FV123"/>
+      <c r="FW123"/>
+      <c r="FX123"/>
+      <c r="FY123"/>
+      <c r="FZ123"/>
+      <c r="GA123"/>
+      <c r="GB123"/>
+      <c r="GC123"/>
+      <c r="GD123"/>
+      <c r="GE123"/>
+      <c r="GF123"/>
+      <c r="GG123"/>
+      <c r="GH123"/>
+      <c r="GI123"/>
+      <c r="GJ123"/>
+      <c r="GK123"/>
+      <c r="GL123"/>
+      <c r="GM123"/>
+      <c r="GN123"/>
+      <c r="GO123"/>
+      <c r="GP123"/>
+      <c r="GQ123"/>
+      <c r="GR123"/>
+      <c r="GS123"/>
+      <c r="GT123"/>
+      <c r="GU123"/>
+      <c r="GV123"/>
+      <c r="GW123"/>
+      <c r="GX123"/>
+      <c r="GY123"/>
+      <c r="GZ123"/>
+      <c r="HA123"/>
+      <c r="HB123"/>
+      <c r="HC123"/>
+      <c r="HD123"/>
+      <c r="HE123"/>
+      <c r="HF123"/>
+      <c r="HG123"/>
+      <c r="HH123"/>
+      <c r="HI123"/>
+      <c r="HJ123"/>
+      <c r="HK123"/>
+      <c r="HL123"/>
+      <c r="HM123"/>
+      <c r="HN123"/>
+      <c r="HO123"/>
+      <c r="HP123"/>
+      <c r="HQ123"/>
+      <c r="HR123"/>
+      <c r="HS123"/>
+      <c r="HT123"/>
+      <c r="HU123"/>
+      <c r="HV123"/>
+      <c r="HW123"/>
+      <c r="HX123"/>
+      <c r="HY123"/>
+      <c r="HZ123"/>
+      <c r="IA123"/>
+      <c r="IB123"/>
+      <c r="IC123"/>
+      <c r="ID123"/>
+      <c r="IE123"/>
+      <c r="IF123"/>
+      <c r="IG123"/>
+      <c r="IH123"/>
+      <c r="II123"/>
+      <c r="IJ123"/>
+      <c r="IK123"/>
+      <c r="IL123"/>
+      <c r="IM123"/>
+      <c r="IN123"/>
+      <c r="IO123"/>
+      <c r="IP123"/>
+      <c r="IQ123"/>
+      <c r="IR123"/>
+      <c r="IS123"/>
+      <c r="IT123"/>
+      <c r="IU123"/>
+      <c r="IV123"/>
+      <c r="IW123"/>
     </row>
     <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A124" t="s">
-        <v>228</v>
+      <c r="A124" s="99" t="s">
+        <v>256</v>
       </c>
       <c r="B124" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="C124" s="57" t="s">
+      <c r="C124" s="98" t="s">
         <v>257</v>
       </c>
       <c r="D124" s="57"/>
@@ -18986,15 +18980,15 @@
       <c r="A125" s="99" t="s">
         <v>258</v>
       </c>
-      <c r="B125" s="57" t="s">
-        <v>228</v>
+      <c r="B125" s="98" t="s">
+        <v>259</v>
       </c>
       <c r="C125" s="98" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D125" s="57"/>
       <c r="E125" s="98" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="F125" s="98" t="s">
         <v>13</v>
@@ -19261,17 +19255,17 @@
     </row>
     <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A126" s="99" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B126" s="98" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C126" s="98" t="s">
         <v>262</v>
       </c>
       <c r="D126" s="57"/>
       <c r="E126" s="98" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F126" s="98" t="s">
         <v>13</v>
@@ -19536,283 +19530,7 @@
       <c r="IV126"/>
       <c r="IW126"/>
     </row>
-    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A127" s="99" t="s">
-        <v>263</v>
-      </c>
-      <c r="B127" s="98" t="s">
-        <v>261</v>
-      </c>
-      <c r="C127" s="98" t="s">
-        <v>264</v>
-      </c>
-      <c r="D127" s="57"/>
-      <c r="E127" s="98" t="s">
-        <v>261</v>
-      </c>
-      <c r="F127" s="98" t="s">
-        <v>13</v>
-      </c>
-      <c r="G127" s="81">
-        <v>0</v>
-      </c>
-      <c r="H127" s="57">
-        <v>1</v>
-      </c>
-      <c r="I127" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="J127" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="K127"/>
-      <c r="L127"/>
-      <c r="M127"/>
-      <c r="N127"/>
-      <c r="O127"/>
-      <c r="P127"/>
-      <c r="Q127"/>
-      <c r="R127"/>
-      <c r="S127"/>
-      <c r="T127"/>
-      <c r="U127"/>
-      <c r="V127"/>
-      <c r="W127"/>
-      <c r="X127"/>
-      <c r="Y127"/>
-      <c r="Z127"/>
-      <c r="AA127"/>
-      <c r="AB127"/>
-      <c r="AC127"/>
-      <c r="AD127"/>
-      <c r="AE127"/>
-      <c r="AF127"/>
-      <c r="AG127"/>
-      <c r="AH127"/>
-      <c r="AI127"/>
-      <c r="AJ127"/>
-      <c r="AK127"/>
-      <c r="AL127"/>
-      <c r="AM127"/>
-      <c r="AN127"/>
-      <c r="AO127"/>
-      <c r="AP127"/>
-      <c r="AQ127"/>
-      <c r="AR127"/>
-      <c r="AS127"/>
-      <c r="AT127"/>
-      <c r="AU127"/>
-      <c r="AV127"/>
-      <c r="AW127"/>
-      <c r="AX127"/>
-      <c r="AY127"/>
-      <c r="AZ127"/>
-      <c r="BA127"/>
-      <c r="BB127"/>
-      <c r="BC127"/>
-      <c r="BD127"/>
-      <c r="BE127"/>
-      <c r="BF127"/>
-      <c r="BG127"/>
-      <c r="BH127"/>
-      <c r="BI127"/>
-      <c r="BJ127"/>
-      <c r="BK127"/>
-      <c r="BL127"/>
-      <c r="BM127"/>
-      <c r="BN127"/>
-      <c r="BO127"/>
-      <c r="BP127"/>
-      <c r="BQ127"/>
-      <c r="BR127"/>
-      <c r="BS127"/>
-      <c r="BT127"/>
-      <c r="BU127"/>
-      <c r="BV127"/>
-      <c r="BW127"/>
-      <c r="BX127"/>
-      <c r="BY127"/>
-      <c r="BZ127"/>
-      <c r="CA127"/>
-      <c r="CB127"/>
-      <c r="CC127"/>
-      <c r="CD127"/>
-      <c r="CE127"/>
-      <c r="CF127"/>
-      <c r="CG127"/>
-      <c r="CH127"/>
-      <c r="CI127"/>
-      <c r="CJ127"/>
-      <c r="CK127"/>
-      <c r="CL127"/>
-      <c r="CM127"/>
-      <c r="CN127"/>
-      <c r="CO127"/>
-      <c r="CP127"/>
-      <c r="CQ127"/>
-      <c r="CR127"/>
-      <c r="CS127"/>
-      <c r="CT127"/>
-      <c r="CU127"/>
-      <c r="CV127"/>
-      <c r="CW127"/>
-      <c r="CX127"/>
-      <c r="CY127"/>
-      <c r="CZ127"/>
-      <c r="DA127"/>
-      <c r="DB127"/>
-      <c r="DC127"/>
-      <c r="DD127"/>
-      <c r="DE127"/>
-      <c r="DF127"/>
-      <c r="DG127"/>
-      <c r="DH127"/>
-      <c r="DI127"/>
-      <c r="DJ127"/>
-      <c r="DK127"/>
-      <c r="DL127"/>
-      <c r="DM127"/>
-      <c r="DN127"/>
-      <c r="DO127"/>
-      <c r="DP127"/>
-      <c r="DQ127"/>
-      <c r="DR127"/>
-      <c r="DS127"/>
-      <c r="DT127"/>
-      <c r="DU127"/>
-      <c r="DV127"/>
-      <c r="DW127"/>
-      <c r="DX127"/>
-      <c r="DY127"/>
-      <c r="DZ127"/>
-      <c r="EA127"/>
-      <c r="EB127"/>
-      <c r="EC127"/>
-      <c r="ED127"/>
-      <c r="EE127"/>
-      <c r="EF127"/>
-      <c r="EG127"/>
-      <c r="EH127"/>
-      <c r="EI127"/>
-      <c r="EJ127"/>
-      <c r="EK127"/>
-      <c r="EL127"/>
-      <c r="EM127"/>
-      <c r="EN127"/>
-      <c r="EO127"/>
-      <c r="EP127"/>
-      <c r="EQ127"/>
-      <c r="ER127"/>
-      <c r="ES127"/>
-      <c r="ET127"/>
-      <c r="EU127"/>
-      <c r="EV127"/>
-      <c r="EW127"/>
-      <c r="EX127"/>
-      <c r="EY127"/>
-      <c r="EZ127"/>
-      <c r="FA127"/>
-      <c r="FB127"/>
-      <c r="FC127"/>
-      <c r="FD127"/>
-      <c r="FE127"/>
-      <c r="FF127"/>
-      <c r="FG127"/>
-      <c r="FH127"/>
-      <c r="FI127"/>
-      <c r="FJ127"/>
-      <c r="FK127"/>
-      <c r="FL127"/>
-      <c r="FM127"/>
-      <c r="FN127"/>
-      <c r="FO127"/>
-      <c r="FP127"/>
-      <c r="FQ127"/>
-      <c r="FR127"/>
-      <c r="FS127"/>
-      <c r="FT127"/>
-      <c r="FU127"/>
-      <c r="FV127"/>
-      <c r="FW127"/>
-      <c r="FX127"/>
-      <c r="FY127"/>
-      <c r="FZ127"/>
-      <c r="GA127"/>
-      <c r="GB127"/>
-      <c r="GC127"/>
-      <c r="GD127"/>
-      <c r="GE127"/>
-      <c r="GF127"/>
-      <c r="GG127"/>
-      <c r="GH127"/>
-      <c r="GI127"/>
-      <c r="GJ127"/>
-      <c r="GK127"/>
-      <c r="GL127"/>
-      <c r="GM127"/>
-      <c r="GN127"/>
-      <c r="GO127"/>
-      <c r="GP127"/>
-      <c r="GQ127"/>
-      <c r="GR127"/>
-      <c r="GS127"/>
-      <c r="GT127"/>
-      <c r="GU127"/>
-      <c r="GV127"/>
-      <c r="GW127"/>
-      <c r="GX127"/>
-      <c r="GY127"/>
-      <c r="GZ127"/>
-      <c r="HA127"/>
-      <c r="HB127"/>
-      <c r="HC127"/>
-      <c r="HD127"/>
-      <c r="HE127"/>
-      <c r="HF127"/>
-      <c r="HG127"/>
-      <c r="HH127"/>
-      <c r="HI127"/>
-      <c r="HJ127"/>
-      <c r="HK127"/>
-      <c r="HL127"/>
-      <c r="HM127"/>
-      <c r="HN127"/>
-      <c r="HO127"/>
-      <c r="HP127"/>
-      <c r="HQ127"/>
-      <c r="HR127"/>
-      <c r="HS127"/>
-      <c r="HT127"/>
-      <c r="HU127"/>
-      <c r="HV127"/>
-      <c r="HW127"/>
-      <c r="HX127"/>
-      <c r="HY127"/>
-      <c r="HZ127"/>
-      <c r="IA127"/>
-      <c r="IB127"/>
-      <c r="IC127"/>
-      <c r="ID127"/>
-      <c r="IE127"/>
-      <c r="IF127"/>
-      <c r="IG127"/>
-      <c r="IH127"/>
-      <c r="II127"/>
-      <c r="IJ127"/>
-      <c r="IK127"/>
-      <c r="IL127"/>
-      <c r="IM127"/>
-      <c r="IN127"/>
-      <c r="IO127"/>
-      <c r="IP127"/>
-      <c r="IQ127"/>
-      <c r="IR127"/>
-      <c r="IS127"/>
-      <c r="IT127"/>
-      <c r="IU127"/>
-      <c r="IV127"/>
-      <c r="IW127"/>
-    </row>
+    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
     <row r="130" ht="17.100000000000001" customHeight="1"/>
@@ -19826,7 +19544,6 @@
     <row r="138" ht="17.100000000000001" customHeight="1"/>
     <row r="139" ht="17.100000000000001" customHeight="1"/>
     <row r="140" ht="17.100000000000001" customHeight="1"/>
-    <row r="141" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
2021091711 added field setting to partner
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4139C4-6C0F-4A48-8F2D-88FADC8987A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC223F2-5974-492E-B392-E56DE6E59B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="267">
   <si>
     <t>name</t>
   </si>
@@ -815,6 +815,18 @@
   </si>
   <si>
     <t>Implementation Log Edit Limitation</t>
+  </si>
+  <si>
+    <t>engagement</t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>Background</t>
   </si>
 </sst>
 </file>
@@ -1725,23 +1737,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW140"/>
+  <dimension ref="A1:IW142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:XFD81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.85546875" style="1"/>
+    <col min="6" max="8" width="11.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -17759,13 +17771,13 @@
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="19" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B109" s="19" t="s">
         <v>120</v>
       </c>
       <c r="C109" s="85" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="76" t="s">
@@ -18033,74 +18045,564 @@
       <c r="IW109"/>
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B110" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="C110" s="58" t="s">
-        <v>229</v>
+      <c r="A110" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>266</v>
       </c>
       <c r="D110" s="58"/>
-      <c r="E110" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="F110" s="96" t="s">
+      <c r="E110" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F110" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="25">
         <v>0</v>
       </c>
-      <c r="H110" s="97">
+      <c r="H110" s="25">
         <v>1</v>
       </c>
-      <c r="I110" s="96" t="s">
-        <v>173</v>
-      </c>
-      <c r="J110" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I110" s="10"/>
+      <c r="J110" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K110"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110"/>
+      <c r="R110"/>
+      <c r="S110"/>
+      <c r="T110"/>
+      <c r="U110"/>
+      <c r="V110"/>
+      <c r="W110"/>
+      <c r="X110"/>
+      <c r="Y110"/>
+      <c r="Z110"/>
+      <c r="AA110"/>
+      <c r="AB110"/>
+      <c r="AC110"/>
+      <c r="AD110"/>
+      <c r="AE110"/>
+      <c r="AF110"/>
+      <c r="AG110"/>
+      <c r="AH110"/>
+      <c r="AI110"/>
+      <c r="AJ110"/>
+      <c r="AK110"/>
+      <c r="AL110"/>
+      <c r="AM110"/>
+      <c r="AN110"/>
+      <c r="AO110"/>
+      <c r="AP110"/>
+      <c r="AQ110"/>
+      <c r="AR110"/>
+      <c r="AS110"/>
+      <c r="AT110"/>
+      <c r="AU110"/>
+      <c r="AV110"/>
+      <c r="AW110"/>
+      <c r="AX110"/>
+      <c r="AY110"/>
+      <c r="AZ110"/>
+      <c r="BA110"/>
+      <c r="BB110"/>
+      <c r="BC110"/>
+      <c r="BD110"/>
+      <c r="BE110"/>
+      <c r="BF110"/>
+      <c r="BG110"/>
+      <c r="BH110"/>
+      <c r="BI110"/>
+      <c r="BJ110"/>
+      <c r="BK110"/>
+      <c r="BL110"/>
+      <c r="BM110"/>
+      <c r="BN110"/>
+      <c r="BO110"/>
+      <c r="BP110"/>
+      <c r="BQ110"/>
+      <c r="BR110"/>
+      <c r="BS110"/>
+      <c r="BT110"/>
+      <c r="BU110"/>
+      <c r="BV110"/>
+      <c r="BW110"/>
+      <c r="BX110"/>
+      <c r="BY110"/>
+      <c r="BZ110"/>
+      <c r="CA110"/>
+      <c r="CB110"/>
+      <c r="CC110"/>
+      <c r="CD110"/>
+      <c r="CE110"/>
+      <c r="CF110"/>
+      <c r="CG110"/>
+      <c r="CH110"/>
+      <c r="CI110"/>
+      <c r="CJ110"/>
+      <c r="CK110"/>
+      <c r="CL110"/>
+      <c r="CM110"/>
+      <c r="CN110"/>
+      <c r="CO110"/>
+      <c r="CP110"/>
+      <c r="CQ110"/>
+      <c r="CR110"/>
+      <c r="CS110"/>
+      <c r="CT110"/>
+      <c r="CU110"/>
+      <c r="CV110"/>
+      <c r="CW110"/>
+      <c r="CX110"/>
+      <c r="CY110"/>
+      <c r="CZ110"/>
+      <c r="DA110"/>
+      <c r="DB110"/>
+      <c r="DC110"/>
+      <c r="DD110"/>
+      <c r="DE110"/>
+      <c r="DF110"/>
+      <c r="DG110"/>
+      <c r="DH110"/>
+      <c r="DI110"/>
+      <c r="DJ110"/>
+      <c r="DK110"/>
+      <c r="DL110"/>
+      <c r="DM110"/>
+      <c r="DN110"/>
+      <c r="DO110"/>
+      <c r="DP110"/>
+      <c r="DQ110"/>
+      <c r="DR110"/>
+      <c r="DS110"/>
+      <c r="DT110"/>
+      <c r="DU110"/>
+      <c r="DV110"/>
+      <c r="DW110"/>
+      <c r="DX110"/>
+      <c r="DY110"/>
+      <c r="DZ110"/>
+      <c r="EA110"/>
+      <c r="EB110"/>
+      <c r="EC110"/>
+      <c r="ED110"/>
+      <c r="EE110"/>
+      <c r="EF110"/>
+      <c r="EG110"/>
+      <c r="EH110"/>
+      <c r="EI110"/>
+      <c r="EJ110"/>
+      <c r="EK110"/>
+      <c r="EL110"/>
+      <c r="EM110"/>
+      <c r="EN110"/>
+      <c r="EO110"/>
+      <c r="EP110"/>
+      <c r="EQ110"/>
+      <c r="ER110"/>
+      <c r="ES110"/>
+      <c r="ET110"/>
+      <c r="EU110"/>
+      <c r="EV110"/>
+      <c r="EW110"/>
+      <c r="EX110"/>
+      <c r="EY110"/>
+      <c r="EZ110"/>
+      <c r="FA110"/>
+      <c r="FB110"/>
+      <c r="FC110"/>
+      <c r="FD110"/>
+      <c r="FE110"/>
+      <c r="FF110"/>
+      <c r="FG110"/>
+      <c r="FH110"/>
+      <c r="FI110"/>
+      <c r="FJ110"/>
+      <c r="FK110"/>
+      <c r="FL110"/>
+      <c r="FM110"/>
+      <c r="FN110"/>
+      <c r="FO110"/>
+      <c r="FP110"/>
+      <c r="FQ110"/>
+      <c r="FR110"/>
+      <c r="FS110"/>
+      <c r="FT110"/>
+      <c r="FU110"/>
+      <c r="FV110"/>
+      <c r="FW110"/>
+      <c r="FX110"/>
+      <c r="FY110"/>
+      <c r="FZ110"/>
+      <c r="GA110"/>
+      <c r="GB110"/>
+      <c r="GC110"/>
+      <c r="GD110"/>
+      <c r="GE110"/>
+      <c r="GF110"/>
+      <c r="GG110"/>
+      <c r="GH110"/>
+      <c r="GI110"/>
+      <c r="GJ110"/>
+      <c r="GK110"/>
+      <c r="GL110"/>
+      <c r="GM110"/>
+      <c r="GN110"/>
+      <c r="GO110"/>
+      <c r="GP110"/>
+      <c r="GQ110"/>
+      <c r="GR110"/>
+      <c r="GS110"/>
+      <c r="GT110"/>
+      <c r="GU110"/>
+      <c r="GV110"/>
+      <c r="GW110"/>
+      <c r="GX110"/>
+      <c r="GY110"/>
+      <c r="GZ110"/>
+      <c r="HA110"/>
+      <c r="HB110"/>
+      <c r="HC110"/>
+      <c r="HD110"/>
+      <c r="HE110"/>
+      <c r="HF110"/>
+      <c r="HG110"/>
+      <c r="HH110"/>
+      <c r="HI110"/>
+      <c r="HJ110"/>
+      <c r="HK110"/>
+      <c r="HL110"/>
+      <c r="HM110"/>
+      <c r="HN110"/>
+      <c r="HO110"/>
+      <c r="HP110"/>
+      <c r="HQ110"/>
+      <c r="HR110"/>
+      <c r="HS110"/>
+      <c r="HT110"/>
+      <c r="HU110"/>
+      <c r="HV110"/>
+      <c r="HW110"/>
+      <c r="HX110"/>
+      <c r="HY110"/>
+      <c r="HZ110"/>
+      <c r="IA110"/>
+      <c r="IB110"/>
+      <c r="IC110"/>
+      <c r="ID110"/>
+      <c r="IE110"/>
+      <c r="IF110"/>
+      <c r="IG110"/>
+      <c r="IH110"/>
+      <c r="II110"/>
+      <c r="IJ110"/>
+      <c r="IK110"/>
+      <c r="IL110"/>
+      <c r="IM110"/>
+      <c r="IN110"/>
+      <c r="IO110"/>
+      <c r="IP110"/>
+      <c r="IQ110"/>
+      <c r="IR110"/>
+      <c r="IS110"/>
+      <c r="IT110"/>
+      <c r="IU110"/>
+      <c r="IV110"/>
+      <c r="IW110"/>
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B111" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="C111" s="58" t="s">
-        <v>231</v>
+      <c r="A111" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" s="85" t="s">
+        <v>78</v>
       </c>
       <c r="D111" s="58"/>
-      <c r="E111" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="F111" s="96" t="s">
+      <c r="E111" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F111" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G111" s="25">
         <v>0</v>
       </c>
-      <c r="H111" s="58">
+      <c r="H111" s="25">
         <v>1</v>
       </c>
-      <c r="I111" s="96" t="s">
-        <v>173</v>
-      </c>
-      <c r="J111" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I111" s="10"/>
+      <c r="J111" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K111"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+      <c r="P111"/>
+      <c r="Q111"/>
+      <c r="R111"/>
+      <c r="S111"/>
+      <c r="T111"/>
+      <c r="U111"/>
+      <c r="V111"/>
+      <c r="W111"/>
+      <c r="X111"/>
+      <c r="Y111"/>
+      <c r="Z111"/>
+      <c r="AA111"/>
+      <c r="AB111"/>
+      <c r="AC111"/>
+      <c r="AD111"/>
+      <c r="AE111"/>
+      <c r="AF111"/>
+      <c r="AG111"/>
+      <c r="AH111"/>
+      <c r="AI111"/>
+      <c r="AJ111"/>
+      <c r="AK111"/>
+      <c r="AL111"/>
+      <c r="AM111"/>
+      <c r="AN111"/>
+      <c r="AO111"/>
+      <c r="AP111"/>
+      <c r="AQ111"/>
+      <c r="AR111"/>
+      <c r="AS111"/>
+      <c r="AT111"/>
+      <c r="AU111"/>
+      <c r="AV111"/>
+      <c r="AW111"/>
+      <c r="AX111"/>
+      <c r="AY111"/>
+      <c r="AZ111"/>
+      <c r="BA111"/>
+      <c r="BB111"/>
+      <c r="BC111"/>
+      <c r="BD111"/>
+      <c r="BE111"/>
+      <c r="BF111"/>
+      <c r="BG111"/>
+      <c r="BH111"/>
+      <c r="BI111"/>
+      <c r="BJ111"/>
+      <c r="BK111"/>
+      <c r="BL111"/>
+      <c r="BM111"/>
+      <c r="BN111"/>
+      <c r="BO111"/>
+      <c r="BP111"/>
+      <c r="BQ111"/>
+      <c r="BR111"/>
+      <c r="BS111"/>
+      <c r="BT111"/>
+      <c r="BU111"/>
+      <c r="BV111"/>
+      <c r="BW111"/>
+      <c r="BX111"/>
+      <c r="BY111"/>
+      <c r="BZ111"/>
+      <c r="CA111"/>
+      <c r="CB111"/>
+      <c r="CC111"/>
+      <c r="CD111"/>
+      <c r="CE111"/>
+      <c r="CF111"/>
+      <c r="CG111"/>
+      <c r="CH111"/>
+      <c r="CI111"/>
+      <c r="CJ111"/>
+      <c r="CK111"/>
+      <c r="CL111"/>
+      <c r="CM111"/>
+      <c r="CN111"/>
+      <c r="CO111"/>
+      <c r="CP111"/>
+      <c r="CQ111"/>
+      <c r="CR111"/>
+      <c r="CS111"/>
+      <c r="CT111"/>
+      <c r="CU111"/>
+      <c r="CV111"/>
+      <c r="CW111"/>
+      <c r="CX111"/>
+      <c r="CY111"/>
+      <c r="CZ111"/>
+      <c r="DA111"/>
+      <c r="DB111"/>
+      <c r="DC111"/>
+      <c r="DD111"/>
+      <c r="DE111"/>
+      <c r="DF111"/>
+      <c r="DG111"/>
+      <c r="DH111"/>
+      <c r="DI111"/>
+      <c r="DJ111"/>
+      <c r="DK111"/>
+      <c r="DL111"/>
+      <c r="DM111"/>
+      <c r="DN111"/>
+      <c r="DO111"/>
+      <c r="DP111"/>
+      <c r="DQ111"/>
+      <c r="DR111"/>
+      <c r="DS111"/>
+      <c r="DT111"/>
+      <c r="DU111"/>
+      <c r="DV111"/>
+      <c r="DW111"/>
+      <c r="DX111"/>
+      <c r="DY111"/>
+      <c r="DZ111"/>
+      <c r="EA111"/>
+      <c r="EB111"/>
+      <c r="EC111"/>
+      <c r="ED111"/>
+      <c r="EE111"/>
+      <c r="EF111"/>
+      <c r="EG111"/>
+      <c r="EH111"/>
+      <c r="EI111"/>
+      <c r="EJ111"/>
+      <c r="EK111"/>
+      <c r="EL111"/>
+      <c r="EM111"/>
+      <c r="EN111"/>
+      <c r="EO111"/>
+      <c r="EP111"/>
+      <c r="EQ111"/>
+      <c r="ER111"/>
+      <c r="ES111"/>
+      <c r="ET111"/>
+      <c r="EU111"/>
+      <c r="EV111"/>
+      <c r="EW111"/>
+      <c r="EX111"/>
+      <c r="EY111"/>
+      <c r="EZ111"/>
+      <c r="FA111"/>
+      <c r="FB111"/>
+      <c r="FC111"/>
+      <c r="FD111"/>
+      <c r="FE111"/>
+      <c r="FF111"/>
+      <c r="FG111"/>
+      <c r="FH111"/>
+      <c r="FI111"/>
+      <c r="FJ111"/>
+      <c r="FK111"/>
+      <c r="FL111"/>
+      <c r="FM111"/>
+      <c r="FN111"/>
+      <c r="FO111"/>
+      <c r="FP111"/>
+      <c r="FQ111"/>
+      <c r="FR111"/>
+      <c r="FS111"/>
+      <c r="FT111"/>
+      <c r="FU111"/>
+      <c r="FV111"/>
+      <c r="FW111"/>
+      <c r="FX111"/>
+      <c r="FY111"/>
+      <c r="FZ111"/>
+      <c r="GA111"/>
+      <c r="GB111"/>
+      <c r="GC111"/>
+      <c r="GD111"/>
+      <c r="GE111"/>
+      <c r="GF111"/>
+      <c r="GG111"/>
+      <c r="GH111"/>
+      <c r="GI111"/>
+      <c r="GJ111"/>
+      <c r="GK111"/>
+      <c r="GL111"/>
+      <c r="GM111"/>
+      <c r="GN111"/>
+      <c r="GO111"/>
+      <c r="GP111"/>
+      <c r="GQ111"/>
+      <c r="GR111"/>
+      <c r="GS111"/>
+      <c r="GT111"/>
+      <c r="GU111"/>
+      <c r="GV111"/>
+      <c r="GW111"/>
+      <c r="GX111"/>
+      <c r="GY111"/>
+      <c r="GZ111"/>
+      <c r="HA111"/>
+      <c r="HB111"/>
+      <c r="HC111"/>
+      <c r="HD111"/>
+      <c r="HE111"/>
+      <c r="HF111"/>
+      <c r="HG111"/>
+      <c r="HH111"/>
+      <c r="HI111"/>
+      <c r="HJ111"/>
+      <c r="HK111"/>
+      <c r="HL111"/>
+      <c r="HM111"/>
+      <c r="HN111"/>
+      <c r="HO111"/>
+      <c r="HP111"/>
+      <c r="HQ111"/>
+      <c r="HR111"/>
+      <c r="HS111"/>
+      <c r="HT111"/>
+      <c r="HU111"/>
+      <c r="HV111"/>
+      <c r="HW111"/>
+      <c r="HX111"/>
+      <c r="HY111"/>
+      <c r="HZ111"/>
+      <c r="IA111"/>
+      <c r="IB111"/>
+      <c r="IC111"/>
+      <c r="ID111"/>
+      <c r="IE111"/>
+      <c r="IF111"/>
+      <c r="IG111"/>
+      <c r="IH111"/>
+      <c r="II111"/>
+      <c r="IJ111"/>
+      <c r="IK111"/>
+      <c r="IL111"/>
+      <c r="IM111"/>
+      <c r="IN111"/>
+      <c r="IO111"/>
+      <c r="IP111"/>
+      <c r="IQ111"/>
+      <c r="IR111"/>
+      <c r="IS111"/>
+      <c r="IT111"/>
+      <c r="IU111"/>
+      <c r="IV111"/>
+      <c r="IW111"/>
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B112" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
@@ -18112,7 +18614,7 @@
       <c r="G112" s="25">
         <v>0</v>
       </c>
-      <c r="H112" s="58">
+      <c r="H112" s="97">
         <v>1</v>
       </c>
       <c r="I112" s="96" t="s">
@@ -18124,13 +18626,13 @@
     </row>
     <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="B113" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
@@ -18154,13 +18656,13 @@
     </row>
     <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B114" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
@@ -18170,7 +18672,7 @@
         <v>13</v>
       </c>
       <c r="G114" s="25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H114" s="58">
         <v>1</v>
@@ -18184,13 +18686,13 @@
     </row>
     <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="B115" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C115" s="58" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
@@ -18214,13 +18716,13 @@
     </row>
     <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B116" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C116" s="58" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
@@ -18230,7 +18732,7 @@
         <v>13</v>
       </c>
       <c r="G116" s="25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H116" s="58">
         <v>1</v>
@@ -18244,13 +18746,13 @@
     </row>
     <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B117" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C117" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
@@ -18274,13 +18776,13 @@
     </row>
     <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B118" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C118" s="95" t="s">
-        <v>237</v>
+      <c r="C118" s="58" t="s">
+        <v>239</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
@@ -18304,13 +18806,13 @@
     </row>
     <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B119" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C119" s="95" t="s">
-        <v>241</v>
+      <c r="C119" s="58" t="s">
+        <v>235</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
@@ -18334,13 +18836,13 @@
     </row>
     <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B120" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C120" s="58" t="s">
-        <v>236</v>
+      <c r="C120" s="95" t="s">
+        <v>237</v>
       </c>
       <c r="D120" s="58"/>
       <c r="E120" s="96" t="s">
@@ -18364,13 +18866,13 @@
     </row>
     <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B121" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C121" s="58" t="s">
-        <v>243</v>
+      <c r="C121" s="95" t="s">
+        <v>241</v>
       </c>
       <c r="D121" s="58"/>
       <c r="E121" s="96" t="s">
@@ -18394,13 +18896,13 @@
     </row>
     <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>152</v>
+        <v>227</v>
       </c>
       <c r="B122" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C122" s="58" t="s">
-        <v>167</v>
+        <v>236</v>
       </c>
       <c r="D122" s="58"/>
       <c r="E122" s="96" t="s">
@@ -18423,572 +18925,78 @@
       </c>
     </row>
     <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="B123" s="57" t="s">
+      <c r="C123" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="D123" s="58"/>
+      <c r="E123" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="C123" s="57" t="s">
-        <v>255</v>
-      </c>
-      <c r="D123" s="57"/>
-      <c r="E123" s="98" t="s">
-        <v>228</v>
-      </c>
-      <c r="F123" s="98" t="s">
+      <c r="F123" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G123" s="81">
+      <c r="G123" s="25">
         <v>0</v>
       </c>
-      <c r="H123" s="57">
+      <c r="H123" s="58">
         <v>1</v>
       </c>
-      <c r="I123" s="98" t="s">
+      <c r="I123" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="J123" s="98" t="s">
+      <c r="J123" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K123"/>
-      <c r="L123"/>
-      <c r="M123"/>
-      <c r="N123"/>
-      <c r="O123"/>
-      <c r="P123"/>
-      <c r="Q123"/>
-      <c r="R123"/>
-      <c r="S123"/>
-      <c r="T123"/>
-      <c r="U123"/>
-      <c r="V123"/>
-      <c r="W123"/>
-      <c r="X123"/>
-      <c r="Y123"/>
-      <c r="Z123"/>
-      <c r="AA123"/>
-      <c r="AB123"/>
-      <c r="AC123"/>
-      <c r="AD123"/>
-      <c r="AE123"/>
-      <c r="AF123"/>
-      <c r="AG123"/>
-      <c r="AH123"/>
-      <c r="AI123"/>
-      <c r="AJ123"/>
-      <c r="AK123"/>
-      <c r="AL123"/>
-      <c r="AM123"/>
-      <c r="AN123"/>
-      <c r="AO123"/>
-      <c r="AP123"/>
-      <c r="AQ123"/>
-      <c r="AR123"/>
-      <c r="AS123"/>
-      <c r="AT123"/>
-      <c r="AU123"/>
-      <c r="AV123"/>
-      <c r="AW123"/>
-      <c r="AX123"/>
-      <c r="AY123"/>
-      <c r="AZ123"/>
-      <c r="BA123"/>
-      <c r="BB123"/>
-      <c r="BC123"/>
-      <c r="BD123"/>
-      <c r="BE123"/>
-      <c r="BF123"/>
-      <c r="BG123"/>
-      <c r="BH123"/>
-      <c r="BI123"/>
-      <c r="BJ123"/>
-      <c r="BK123"/>
-      <c r="BL123"/>
-      <c r="BM123"/>
-      <c r="BN123"/>
-      <c r="BO123"/>
-      <c r="BP123"/>
-      <c r="BQ123"/>
-      <c r="BR123"/>
-      <c r="BS123"/>
-      <c r="BT123"/>
-      <c r="BU123"/>
-      <c r="BV123"/>
-      <c r="BW123"/>
-      <c r="BX123"/>
-      <c r="BY123"/>
-      <c r="BZ123"/>
-      <c r="CA123"/>
-      <c r="CB123"/>
-      <c r="CC123"/>
-      <c r="CD123"/>
-      <c r="CE123"/>
-      <c r="CF123"/>
-      <c r="CG123"/>
-      <c r="CH123"/>
-      <c r="CI123"/>
-      <c r="CJ123"/>
-      <c r="CK123"/>
-      <c r="CL123"/>
-      <c r="CM123"/>
-      <c r="CN123"/>
-      <c r="CO123"/>
-      <c r="CP123"/>
-      <c r="CQ123"/>
-      <c r="CR123"/>
-      <c r="CS123"/>
-      <c r="CT123"/>
-      <c r="CU123"/>
-      <c r="CV123"/>
-      <c r="CW123"/>
-      <c r="CX123"/>
-      <c r="CY123"/>
-      <c r="CZ123"/>
-      <c r="DA123"/>
-      <c r="DB123"/>
-      <c r="DC123"/>
-      <c r="DD123"/>
-      <c r="DE123"/>
-      <c r="DF123"/>
-      <c r="DG123"/>
-      <c r="DH123"/>
-      <c r="DI123"/>
-      <c r="DJ123"/>
-      <c r="DK123"/>
-      <c r="DL123"/>
-      <c r="DM123"/>
-      <c r="DN123"/>
-      <c r="DO123"/>
-      <c r="DP123"/>
-      <c r="DQ123"/>
-      <c r="DR123"/>
-      <c r="DS123"/>
-      <c r="DT123"/>
-      <c r="DU123"/>
-      <c r="DV123"/>
-      <c r="DW123"/>
-      <c r="DX123"/>
-      <c r="DY123"/>
-      <c r="DZ123"/>
-      <c r="EA123"/>
-      <c r="EB123"/>
-      <c r="EC123"/>
-      <c r="ED123"/>
-      <c r="EE123"/>
-      <c r="EF123"/>
-      <c r="EG123"/>
-      <c r="EH123"/>
-      <c r="EI123"/>
-      <c r="EJ123"/>
-      <c r="EK123"/>
-      <c r="EL123"/>
-      <c r="EM123"/>
-      <c r="EN123"/>
-      <c r="EO123"/>
-      <c r="EP123"/>
-      <c r="EQ123"/>
-      <c r="ER123"/>
-      <c r="ES123"/>
-      <c r="ET123"/>
-      <c r="EU123"/>
-      <c r="EV123"/>
-      <c r="EW123"/>
-      <c r="EX123"/>
-      <c r="EY123"/>
-      <c r="EZ123"/>
-      <c r="FA123"/>
-      <c r="FB123"/>
-      <c r="FC123"/>
-      <c r="FD123"/>
-      <c r="FE123"/>
-      <c r="FF123"/>
-      <c r="FG123"/>
-      <c r="FH123"/>
-      <c r="FI123"/>
-      <c r="FJ123"/>
-      <c r="FK123"/>
-      <c r="FL123"/>
-      <c r="FM123"/>
-      <c r="FN123"/>
-      <c r="FO123"/>
-      <c r="FP123"/>
-      <c r="FQ123"/>
-      <c r="FR123"/>
-      <c r="FS123"/>
-      <c r="FT123"/>
-      <c r="FU123"/>
-      <c r="FV123"/>
-      <c r="FW123"/>
-      <c r="FX123"/>
-      <c r="FY123"/>
-      <c r="FZ123"/>
-      <c r="GA123"/>
-      <c r="GB123"/>
-      <c r="GC123"/>
-      <c r="GD123"/>
-      <c r="GE123"/>
-      <c r="GF123"/>
-      <c r="GG123"/>
-      <c r="GH123"/>
-      <c r="GI123"/>
-      <c r="GJ123"/>
-      <c r="GK123"/>
-      <c r="GL123"/>
-      <c r="GM123"/>
-      <c r="GN123"/>
-      <c r="GO123"/>
-      <c r="GP123"/>
-      <c r="GQ123"/>
-      <c r="GR123"/>
-      <c r="GS123"/>
-      <c r="GT123"/>
-      <c r="GU123"/>
-      <c r="GV123"/>
-      <c r="GW123"/>
-      <c r="GX123"/>
-      <c r="GY123"/>
-      <c r="GZ123"/>
-      <c r="HA123"/>
-      <c r="HB123"/>
-      <c r="HC123"/>
-      <c r="HD123"/>
-      <c r="HE123"/>
-      <c r="HF123"/>
-      <c r="HG123"/>
-      <c r="HH123"/>
-      <c r="HI123"/>
-      <c r="HJ123"/>
-      <c r="HK123"/>
-      <c r="HL123"/>
-      <c r="HM123"/>
-      <c r="HN123"/>
-      <c r="HO123"/>
-      <c r="HP123"/>
-      <c r="HQ123"/>
-      <c r="HR123"/>
-      <c r="HS123"/>
-      <c r="HT123"/>
-      <c r="HU123"/>
-      <c r="HV123"/>
-      <c r="HW123"/>
-      <c r="HX123"/>
-      <c r="HY123"/>
-      <c r="HZ123"/>
-      <c r="IA123"/>
-      <c r="IB123"/>
-      <c r="IC123"/>
-      <c r="ID123"/>
-      <c r="IE123"/>
-      <c r="IF123"/>
-      <c r="IG123"/>
-      <c r="IH123"/>
-      <c r="II123"/>
-      <c r="IJ123"/>
-      <c r="IK123"/>
-      <c r="IL123"/>
-      <c r="IM123"/>
-      <c r="IN123"/>
-      <c r="IO123"/>
-      <c r="IP123"/>
-      <c r="IQ123"/>
-      <c r="IR123"/>
-      <c r="IS123"/>
-      <c r="IT123"/>
-      <c r="IU123"/>
-      <c r="IV123"/>
-      <c r="IW123"/>
     </row>
     <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A124" s="99" t="s">
-        <v>256</v>
-      </c>
-      <c r="B124" s="57" t="s">
+      <c r="A124" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B124" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C124" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="D124" s="57"/>
-      <c r="E124" s="98" t="s">
+      <c r="C124" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D124" s="58"/>
+      <c r="E124" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="F124" s="98" t="s">
+      <c r="F124" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G124" s="81">
+      <c r="G124" s="25">
         <v>0</v>
       </c>
-      <c r="H124" s="57">
+      <c r="H124" s="58">
         <v>1</v>
       </c>
-      <c r="I124" s="98" t="s">
+      <c r="I124" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="J124" s="98" t="s">
+      <c r="J124" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K124"/>
-      <c r="L124"/>
-      <c r="M124"/>
-      <c r="N124"/>
-      <c r="O124"/>
-      <c r="P124"/>
-      <c r="Q124"/>
-      <c r="R124"/>
-      <c r="S124"/>
-      <c r="T124"/>
-      <c r="U124"/>
-      <c r="V124"/>
-      <c r="W124"/>
-      <c r="X124"/>
-      <c r="Y124"/>
-      <c r="Z124"/>
-      <c r="AA124"/>
-      <c r="AB124"/>
-      <c r="AC124"/>
-      <c r="AD124"/>
-      <c r="AE124"/>
-      <c r="AF124"/>
-      <c r="AG124"/>
-      <c r="AH124"/>
-      <c r="AI124"/>
-      <c r="AJ124"/>
-      <c r="AK124"/>
-      <c r="AL124"/>
-      <c r="AM124"/>
-      <c r="AN124"/>
-      <c r="AO124"/>
-      <c r="AP124"/>
-      <c r="AQ124"/>
-      <c r="AR124"/>
-      <c r="AS124"/>
-      <c r="AT124"/>
-      <c r="AU124"/>
-      <c r="AV124"/>
-      <c r="AW124"/>
-      <c r="AX124"/>
-      <c r="AY124"/>
-      <c r="AZ124"/>
-      <c r="BA124"/>
-      <c r="BB124"/>
-      <c r="BC124"/>
-      <c r="BD124"/>
-      <c r="BE124"/>
-      <c r="BF124"/>
-      <c r="BG124"/>
-      <c r="BH124"/>
-      <c r="BI124"/>
-      <c r="BJ124"/>
-      <c r="BK124"/>
-      <c r="BL124"/>
-      <c r="BM124"/>
-      <c r="BN124"/>
-      <c r="BO124"/>
-      <c r="BP124"/>
-      <c r="BQ124"/>
-      <c r="BR124"/>
-      <c r="BS124"/>
-      <c r="BT124"/>
-      <c r="BU124"/>
-      <c r="BV124"/>
-      <c r="BW124"/>
-      <c r="BX124"/>
-      <c r="BY124"/>
-      <c r="BZ124"/>
-      <c r="CA124"/>
-      <c r="CB124"/>
-      <c r="CC124"/>
-      <c r="CD124"/>
-      <c r="CE124"/>
-      <c r="CF124"/>
-      <c r="CG124"/>
-      <c r="CH124"/>
-      <c r="CI124"/>
-      <c r="CJ124"/>
-      <c r="CK124"/>
-      <c r="CL124"/>
-      <c r="CM124"/>
-      <c r="CN124"/>
-      <c r="CO124"/>
-      <c r="CP124"/>
-      <c r="CQ124"/>
-      <c r="CR124"/>
-      <c r="CS124"/>
-      <c r="CT124"/>
-      <c r="CU124"/>
-      <c r="CV124"/>
-      <c r="CW124"/>
-      <c r="CX124"/>
-      <c r="CY124"/>
-      <c r="CZ124"/>
-      <c r="DA124"/>
-      <c r="DB124"/>
-      <c r="DC124"/>
-      <c r="DD124"/>
-      <c r="DE124"/>
-      <c r="DF124"/>
-      <c r="DG124"/>
-      <c r="DH124"/>
-      <c r="DI124"/>
-      <c r="DJ124"/>
-      <c r="DK124"/>
-      <c r="DL124"/>
-      <c r="DM124"/>
-      <c r="DN124"/>
-      <c r="DO124"/>
-      <c r="DP124"/>
-      <c r="DQ124"/>
-      <c r="DR124"/>
-      <c r="DS124"/>
-      <c r="DT124"/>
-      <c r="DU124"/>
-      <c r="DV124"/>
-      <c r="DW124"/>
-      <c r="DX124"/>
-      <c r="DY124"/>
-      <c r="DZ124"/>
-      <c r="EA124"/>
-      <c r="EB124"/>
-      <c r="EC124"/>
-      <c r="ED124"/>
-      <c r="EE124"/>
-      <c r="EF124"/>
-      <c r="EG124"/>
-      <c r="EH124"/>
-      <c r="EI124"/>
-      <c r="EJ124"/>
-      <c r="EK124"/>
-      <c r="EL124"/>
-      <c r="EM124"/>
-      <c r="EN124"/>
-      <c r="EO124"/>
-      <c r="EP124"/>
-      <c r="EQ124"/>
-      <c r="ER124"/>
-      <c r="ES124"/>
-      <c r="ET124"/>
-      <c r="EU124"/>
-      <c r="EV124"/>
-      <c r="EW124"/>
-      <c r="EX124"/>
-      <c r="EY124"/>
-      <c r="EZ124"/>
-      <c r="FA124"/>
-      <c r="FB124"/>
-      <c r="FC124"/>
-      <c r="FD124"/>
-      <c r="FE124"/>
-      <c r="FF124"/>
-      <c r="FG124"/>
-      <c r="FH124"/>
-      <c r="FI124"/>
-      <c r="FJ124"/>
-      <c r="FK124"/>
-      <c r="FL124"/>
-      <c r="FM124"/>
-      <c r="FN124"/>
-      <c r="FO124"/>
-      <c r="FP124"/>
-      <c r="FQ124"/>
-      <c r="FR124"/>
-      <c r="FS124"/>
-      <c r="FT124"/>
-      <c r="FU124"/>
-      <c r="FV124"/>
-      <c r="FW124"/>
-      <c r="FX124"/>
-      <c r="FY124"/>
-      <c r="FZ124"/>
-      <c r="GA124"/>
-      <c r="GB124"/>
-      <c r="GC124"/>
-      <c r="GD124"/>
-      <c r="GE124"/>
-      <c r="GF124"/>
-      <c r="GG124"/>
-      <c r="GH124"/>
-      <c r="GI124"/>
-      <c r="GJ124"/>
-      <c r="GK124"/>
-      <c r="GL124"/>
-      <c r="GM124"/>
-      <c r="GN124"/>
-      <c r="GO124"/>
-      <c r="GP124"/>
-      <c r="GQ124"/>
-      <c r="GR124"/>
-      <c r="GS124"/>
-      <c r="GT124"/>
-      <c r="GU124"/>
-      <c r="GV124"/>
-      <c r="GW124"/>
-      <c r="GX124"/>
-      <c r="GY124"/>
-      <c r="GZ124"/>
-      <c r="HA124"/>
-      <c r="HB124"/>
-      <c r="HC124"/>
-      <c r="HD124"/>
-      <c r="HE124"/>
-      <c r="HF124"/>
-      <c r="HG124"/>
-      <c r="HH124"/>
-      <c r="HI124"/>
-      <c r="HJ124"/>
-      <c r="HK124"/>
-      <c r="HL124"/>
-      <c r="HM124"/>
-      <c r="HN124"/>
-      <c r="HO124"/>
-      <c r="HP124"/>
-      <c r="HQ124"/>
-      <c r="HR124"/>
-      <c r="HS124"/>
-      <c r="HT124"/>
-      <c r="HU124"/>
-      <c r="HV124"/>
-      <c r="HW124"/>
-      <c r="HX124"/>
-      <c r="HY124"/>
-      <c r="HZ124"/>
-      <c r="IA124"/>
-      <c r="IB124"/>
-      <c r="IC124"/>
-      <c r="ID124"/>
-      <c r="IE124"/>
-      <c r="IF124"/>
-      <c r="IG124"/>
-      <c r="IH124"/>
-      <c r="II124"/>
-      <c r="IJ124"/>
-      <c r="IK124"/>
-      <c r="IL124"/>
-      <c r="IM124"/>
-      <c r="IN124"/>
-      <c r="IO124"/>
-      <c r="IP124"/>
-      <c r="IQ124"/>
-      <c r="IR124"/>
-      <c r="IS124"/>
-      <c r="IT124"/>
-      <c r="IU124"/>
-      <c r="IV124"/>
-      <c r="IW124"/>
     </row>
     <row r="125" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A125" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="B125" s="98" t="s">
-        <v>259</v>
-      </c>
-      <c r="C125" s="98" t="s">
-        <v>260</v>
+      <c r="A125" t="s">
+        <v>228</v>
+      </c>
+      <c r="B125" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C125" s="57" t="s">
+        <v>255</v>
       </c>
       <c r="D125" s="57"/>
       <c r="E125" s="98" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="F125" s="98" t="s">
         <v>13</v>
@@ -19255,17 +19263,17 @@
     </row>
     <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A126" s="99" t="s">
-        <v>261</v>
-      </c>
-      <c r="B126" s="98" t="s">
-        <v>259</v>
+        <v>256</v>
+      </c>
+      <c r="B126" s="57" t="s">
+        <v>228</v>
       </c>
       <c r="C126" s="98" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D126" s="57"/>
       <c r="E126" s="98" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="F126" s="98" t="s">
         <v>13</v>
@@ -19530,8 +19538,560 @@
       <c r="IV126"/>
       <c r="IW126"/>
     </row>
-    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A127" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="B127" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C127" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="D127" s="57"/>
+      <c r="E127" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="F127" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="81">
+        <v>0</v>
+      </c>
+      <c r="H127" s="57">
+        <v>1</v>
+      </c>
+      <c r="I127" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J127" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127"/>
+      <c r="N127"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
+      <c r="R127"/>
+      <c r="S127"/>
+      <c r="T127"/>
+      <c r="U127"/>
+      <c r="V127"/>
+      <c r="W127"/>
+      <c r="X127"/>
+      <c r="Y127"/>
+      <c r="Z127"/>
+      <c r="AA127"/>
+      <c r="AB127"/>
+      <c r="AC127"/>
+      <c r="AD127"/>
+      <c r="AE127"/>
+      <c r="AF127"/>
+      <c r="AG127"/>
+      <c r="AH127"/>
+      <c r="AI127"/>
+      <c r="AJ127"/>
+      <c r="AK127"/>
+      <c r="AL127"/>
+      <c r="AM127"/>
+      <c r="AN127"/>
+      <c r="AO127"/>
+      <c r="AP127"/>
+      <c r="AQ127"/>
+      <c r="AR127"/>
+      <c r="AS127"/>
+      <c r="AT127"/>
+      <c r="AU127"/>
+      <c r="AV127"/>
+      <c r="AW127"/>
+      <c r="AX127"/>
+      <c r="AY127"/>
+      <c r="AZ127"/>
+      <c r="BA127"/>
+      <c r="BB127"/>
+      <c r="BC127"/>
+      <c r="BD127"/>
+      <c r="BE127"/>
+      <c r="BF127"/>
+      <c r="BG127"/>
+      <c r="BH127"/>
+      <c r="BI127"/>
+      <c r="BJ127"/>
+      <c r="BK127"/>
+      <c r="BL127"/>
+      <c r="BM127"/>
+      <c r="BN127"/>
+      <c r="BO127"/>
+      <c r="BP127"/>
+      <c r="BQ127"/>
+      <c r="BR127"/>
+      <c r="BS127"/>
+      <c r="BT127"/>
+      <c r="BU127"/>
+      <c r="BV127"/>
+      <c r="BW127"/>
+      <c r="BX127"/>
+      <c r="BY127"/>
+      <c r="BZ127"/>
+      <c r="CA127"/>
+      <c r="CB127"/>
+      <c r="CC127"/>
+      <c r="CD127"/>
+      <c r="CE127"/>
+      <c r="CF127"/>
+      <c r="CG127"/>
+      <c r="CH127"/>
+      <c r="CI127"/>
+      <c r="CJ127"/>
+      <c r="CK127"/>
+      <c r="CL127"/>
+      <c r="CM127"/>
+      <c r="CN127"/>
+      <c r="CO127"/>
+      <c r="CP127"/>
+      <c r="CQ127"/>
+      <c r="CR127"/>
+      <c r="CS127"/>
+      <c r="CT127"/>
+      <c r="CU127"/>
+      <c r="CV127"/>
+      <c r="CW127"/>
+      <c r="CX127"/>
+      <c r="CY127"/>
+      <c r="CZ127"/>
+      <c r="DA127"/>
+      <c r="DB127"/>
+      <c r="DC127"/>
+      <c r="DD127"/>
+      <c r="DE127"/>
+      <c r="DF127"/>
+      <c r="DG127"/>
+      <c r="DH127"/>
+      <c r="DI127"/>
+      <c r="DJ127"/>
+      <c r="DK127"/>
+      <c r="DL127"/>
+      <c r="DM127"/>
+      <c r="DN127"/>
+      <c r="DO127"/>
+      <c r="DP127"/>
+      <c r="DQ127"/>
+      <c r="DR127"/>
+      <c r="DS127"/>
+      <c r="DT127"/>
+      <c r="DU127"/>
+      <c r="DV127"/>
+      <c r="DW127"/>
+      <c r="DX127"/>
+      <c r="DY127"/>
+      <c r="DZ127"/>
+      <c r="EA127"/>
+      <c r="EB127"/>
+      <c r="EC127"/>
+      <c r="ED127"/>
+      <c r="EE127"/>
+      <c r="EF127"/>
+      <c r="EG127"/>
+      <c r="EH127"/>
+      <c r="EI127"/>
+      <c r="EJ127"/>
+      <c r="EK127"/>
+      <c r="EL127"/>
+      <c r="EM127"/>
+      <c r="EN127"/>
+      <c r="EO127"/>
+      <c r="EP127"/>
+      <c r="EQ127"/>
+      <c r="ER127"/>
+      <c r="ES127"/>
+      <c r="ET127"/>
+      <c r="EU127"/>
+      <c r="EV127"/>
+      <c r="EW127"/>
+      <c r="EX127"/>
+      <c r="EY127"/>
+      <c r="EZ127"/>
+      <c r="FA127"/>
+      <c r="FB127"/>
+      <c r="FC127"/>
+      <c r="FD127"/>
+      <c r="FE127"/>
+      <c r="FF127"/>
+      <c r="FG127"/>
+      <c r="FH127"/>
+      <c r="FI127"/>
+      <c r="FJ127"/>
+      <c r="FK127"/>
+      <c r="FL127"/>
+      <c r="FM127"/>
+      <c r="FN127"/>
+      <c r="FO127"/>
+      <c r="FP127"/>
+      <c r="FQ127"/>
+      <c r="FR127"/>
+      <c r="FS127"/>
+      <c r="FT127"/>
+      <c r="FU127"/>
+      <c r="FV127"/>
+      <c r="FW127"/>
+      <c r="FX127"/>
+      <c r="FY127"/>
+      <c r="FZ127"/>
+      <c r="GA127"/>
+      <c r="GB127"/>
+      <c r="GC127"/>
+      <c r="GD127"/>
+      <c r="GE127"/>
+      <c r="GF127"/>
+      <c r="GG127"/>
+      <c r="GH127"/>
+      <c r="GI127"/>
+      <c r="GJ127"/>
+      <c r="GK127"/>
+      <c r="GL127"/>
+      <c r="GM127"/>
+      <c r="GN127"/>
+      <c r="GO127"/>
+      <c r="GP127"/>
+      <c r="GQ127"/>
+      <c r="GR127"/>
+      <c r="GS127"/>
+      <c r="GT127"/>
+      <c r="GU127"/>
+      <c r="GV127"/>
+      <c r="GW127"/>
+      <c r="GX127"/>
+      <c r="GY127"/>
+      <c r="GZ127"/>
+      <c r="HA127"/>
+      <c r="HB127"/>
+      <c r="HC127"/>
+      <c r="HD127"/>
+      <c r="HE127"/>
+      <c r="HF127"/>
+      <c r="HG127"/>
+      <c r="HH127"/>
+      <c r="HI127"/>
+      <c r="HJ127"/>
+      <c r="HK127"/>
+      <c r="HL127"/>
+      <c r="HM127"/>
+      <c r="HN127"/>
+      <c r="HO127"/>
+      <c r="HP127"/>
+      <c r="HQ127"/>
+      <c r="HR127"/>
+      <c r="HS127"/>
+      <c r="HT127"/>
+      <c r="HU127"/>
+      <c r="HV127"/>
+      <c r="HW127"/>
+      <c r="HX127"/>
+      <c r="HY127"/>
+      <c r="HZ127"/>
+      <c r="IA127"/>
+      <c r="IB127"/>
+      <c r="IC127"/>
+      <c r="ID127"/>
+      <c r="IE127"/>
+      <c r="IF127"/>
+      <c r="IG127"/>
+      <c r="IH127"/>
+      <c r="II127"/>
+      <c r="IJ127"/>
+      <c r="IK127"/>
+      <c r="IL127"/>
+      <c r="IM127"/>
+      <c r="IN127"/>
+      <c r="IO127"/>
+      <c r="IP127"/>
+      <c r="IQ127"/>
+      <c r="IR127"/>
+      <c r="IS127"/>
+      <c r="IT127"/>
+      <c r="IU127"/>
+      <c r="IV127"/>
+      <c r="IW127"/>
+    </row>
+    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A128" s="99" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C128" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="D128" s="57"/>
+      <c r="E128" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="F128" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G128" s="81">
+        <v>0</v>
+      </c>
+      <c r="H128" s="57">
+        <v>1</v>
+      </c>
+      <c r="I128" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J128" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K128"/>
+      <c r="L128"/>
+      <c r="M128"/>
+      <c r="N128"/>
+      <c r="O128"/>
+      <c r="P128"/>
+      <c r="Q128"/>
+      <c r="R128"/>
+      <c r="S128"/>
+      <c r="T128"/>
+      <c r="U128"/>
+      <c r="V128"/>
+      <c r="W128"/>
+      <c r="X128"/>
+      <c r="Y128"/>
+      <c r="Z128"/>
+      <c r="AA128"/>
+      <c r="AB128"/>
+      <c r="AC128"/>
+      <c r="AD128"/>
+      <c r="AE128"/>
+      <c r="AF128"/>
+      <c r="AG128"/>
+      <c r="AH128"/>
+      <c r="AI128"/>
+      <c r="AJ128"/>
+      <c r="AK128"/>
+      <c r="AL128"/>
+      <c r="AM128"/>
+      <c r="AN128"/>
+      <c r="AO128"/>
+      <c r="AP128"/>
+      <c r="AQ128"/>
+      <c r="AR128"/>
+      <c r="AS128"/>
+      <c r="AT128"/>
+      <c r="AU128"/>
+      <c r="AV128"/>
+      <c r="AW128"/>
+      <c r="AX128"/>
+      <c r="AY128"/>
+      <c r="AZ128"/>
+      <c r="BA128"/>
+      <c r="BB128"/>
+      <c r="BC128"/>
+      <c r="BD128"/>
+      <c r="BE128"/>
+      <c r="BF128"/>
+      <c r="BG128"/>
+      <c r="BH128"/>
+      <c r="BI128"/>
+      <c r="BJ128"/>
+      <c r="BK128"/>
+      <c r="BL128"/>
+      <c r="BM128"/>
+      <c r="BN128"/>
+      <c r="BO128"/>
+      <c r="BP128"/>
+      <c r="BQ128"/>
+      <c r="BR128"/>
+      <c r="BS128"/>
+      <c r="BT128"/>
+      <c r="BU128"/>
+      <c r="BV128"/>
+      <c r="BW128"/>
+      <c r="BX128"/>
+      <c r="BY128"/>
+      <c r="BZ128"/>
+      <c r="CA128"/>
+      <c r="CB128"/>
+      <c r="CC128"/>
+      <c r="CD128"/>
+      <c r="CE128"/>
+      <c r="CF128"/>
+      <c r="CG128"/>
+      <c r="CH128"/>
+      <c r="CI128"/>
+      <c r="CJ128"/>
+      <c r="CK128"/>
+      <c r="CL128"/>
+      <c r="CM128"/>
+      <c r="CN128"/>
+      <c r="CO128"/>
+      <c r="CP128"/>
+      <c r="CQ128"/>
+      <c r="CR128"/>
+      <c r="CS128"/>
+      <c r="CT128"/>
+      <c r="CU128"/>
+      <c r="CV128"/>
+      <c r="CW128"/>
+      <c r="CX128"/>
+      <c r="CY128"/>
+      <c r="CZ128"/>
+      <c r="DA128"/>
+      <c r="DB128"/>
+      <c r="DC128"/>
+      <c r="DD128"/>
+      <c r="DE128"/>
+      <c r="DF128"/>
+      <c r="DG128"/>
+      <c r="DH128"/>
+      <c r="DI128"/>
+      <c r="DJ128"/>
+      <c r="DK128"/>
+      <c r="DL128"/>
+      <c r="DM128"/>
+      <c r="DN128"/>
+      <c r="DO128"/>
+      <c r="DP128"/>
+      <c r="DQ128"/>
+      <c r="DR128"/>
+      <c r="DS128"/>
+      <c r="DT128"/>
+      <c r="DU128"/>
+      <c r="DV128"/>
+      <c r="DW128"/>
+      <c r="DX128"/>
+      <c r="DY128"/>
+      <c r="DZ128"/>
+      <c r="EA128"/>
+      <c r="EB128"/>
+      <c r="EC128"/>
+      <c r="ED128"/>
+      <c r="EE128"/>
+      <c r="EF128"/>
+      <c r="EG128"/>
+      <c r="EH128"/>
+      <c r="EI128"/>
+      <c r="EJ128"/>
+      <c r="EK128"/>
+      <c r="EL128"/>
+      <c r="EM128"/>
+      <c r="EN128"/>
+      <c r="EO128"/>
+      <c r="EP128"/>
+      <c r="EQ128"/>
+      <c r="ER128"/>
+      <c r="ES128"/>
+      <c r="ET128"/>
+      <c r="EU128"/>
+      <c r="EV128"/>
+      <c r="EW128"/>
+      <c r="EX128"/>
+      <c r="EY128"/>
+      <c r="EZ128"/>
+      <c r="FA128"/>
+      <c r="FB128"/>
+      <c r="FC128"/>
+      <c r="FD128"/>
+      <c r="FE128"/>
+      <c r="FF128"/>
+      <c r="FG128"/>
+      <c r="FH128"/>
+      <c r="FI128"/>
+      <c r="FJ128"/>
+      <c r="FK128"/>
+      <c r="FL128"/>
+      <c r="FM128"/>
+      <c r="FN128"/>
+      <c r="FO128"/>
+      <c r="FP128"/>
+      <c r="FQ128"/>
+      <c r="FR128"/>
+      <c r="FS128"/>
+      <c r="FT128"/>
+      <c r="FU128"/>
+      <c r="FV128"/>
+      <c r="FW128"/>
+      <c r="FX128"/>
+      <c r="FY128"/>
+      <c r="FZ128"/>
+      <c r="GA128"/>
+      <c r="GB128"/>
+      <c r="GC128"/>
+      <c r="GD128"/>
+      <c r="GE128"/>
+      <c r="GF128"/>
+      <c r="GG128"/>
+      <c r="GH128"/>
+      <c r="GI128"/>
+      <c r="GJ128"/>
+      <c r="GK128"/>
+      <c r="GL128"/>
+      <c r="GM128"/>
+      <c r="GN128"/>
+      <c r="GO128"/>
+      <c r="GP128"/>
+      <c r="GQ128"/>
+      <c r="GR128"/>
+      <c r="GS128"/>
+      <c r="GT128"/>
+      <c r="GU128"/>
+      <c r="GV128"/>
+      <c r="GW128"/>
+      <c r="GX128"/>
+      <c r="GY128"/>
+      <c r="GZ128"/>
+      <c r="HA128"/>
+      <c r="HB128"/>
+      <c r="HC128"/>
+      <c r="HD128"/>
+      <c r="HE128"/>
+      <c r="HF128"/>
+      <c r="HG128"/>
+      <c r="HH128"/>
+      <c r="HI128"/>
+      <c r="HJ128"/>
+      <c r="HK128"/>
+      <c r="HL128"/>
+      <c r="HM128"/>
+      <c r="HN128"/>
+      <c r="HO128"/>
+      <c r="HP128"/>
+      <c r="HQ128"/>
+      <c r="HR128"/>
+      <c r="HS128"/>
+      <c r="HT128"/>
+      <c r="HU128"/>
+      <c r="HV128"/>
+      <c r="HW128"/>
+      <c r="HX128"/>
+      <c r="HY128"/>
+      <c r="HZ128"/>
+      <c r="IA128"/>
+      <c r="IB128"/>
+      <c r="IC128"/>
+      <c r="ID128"/>
+      <c r="IE128"/>
+      <c r="IF128"/>
+      <c r="IG128"/>
+      <c r="IH128"/>
+      <c r="II128"/>
+      <c r="IJ128"/>
+      <c r="IK128"/>
+      <c r="IL128"/>
+      <c r="IM128"/>
+      <c r="IN128"/>
+      <c r="IO128"/>
+      <c r="IP128"/>
+      <c r="IQ128"/>
+      <c r="IR128"/>
+      <c r="IS128"/>
+      <c r="IT128"/>
+      <c r="IU128"/>
+      <c r="IV128"/>
+      <c r="IW128"/>
+    </row>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
     <row r="130" ht="17.100000000000001" customHeight="1"/>
     <row r="131" ht="17.100000000000001" customHeight="1"/>
@@ -19544,6 +20104,8 @@
     <row r="138" ht="17.100000000000001" customHeight="1"/>
     <row r="139" ht="17.100000000000001" customHeight="1"/>
     <row r="140" ht="17.100000000000001" customHeight="1"/>
+    <row r="141" ht="17.100000000000001" customHeight="1"/>
+    <row r="142" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -19561,17 +20123,17 @@
       <selection activeCell="A63" sqref="A63:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="8" width="11.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="28.44140625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="11.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.45" customHeight="1">
+    <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19603,7 +20165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.45" customHeight="1">
+    <row r="2" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -19633,7 +20195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.7" customHeight="1">
+    <row r="3" spans="1:10" ht="13.65" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -19663,7 +20225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.7" customHeight="1">
+    <row r="4" spans="1:10" ht="13.65" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -19693,7 +20255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.7" customHeight="1">
+    <row r="5" spans="1:10" ht="13.65" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -19723,7 +20285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.7" customHeight="1">
+    <row r="6" spans="1:10" ht="13.65" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -19753,7 +20315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.7" customHeight="1">
+    <row r="7" spans="1:10" ht="13.65" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -19783,7 +20345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.7" customHeight="1">
+    <row r="8" spans="1:10" ht="13.65" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -19813,7 +20375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.7" customHeight="1">
+    <row r="9" spans="1:10" ht="13.65" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -19845,7 +20407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.7" customHeight="1">
+    <row r="10" spans="1:10" ht="13.65" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -19877,7 +20439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.7" customHeight="1">
+    <row r="11" spans="1:10" ht="13.65" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -19909,7 +20471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.7" customHeight="1">
+    <row r="12" spans="1:10" ht="13.65" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -19938,7 +20500,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.7" customHeight="1">
+    <row r="13" spans="1:10" ht="13.65" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -19968,7 +20530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.7" customHeight="1">
+    <row r="14" spans="1:10" ht="13.65" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -19995,7 +20557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.7" customHeight="1">
+    <row r="15" spans="1:10" ht="13.65" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -20205,7 +20767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.7" customHeight="1">
+    <row r="22" spans="1:10" ht="13.65" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
@@ -20237,7 +20799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.7" customHeight="1">
+    <row r="23" spans="1:10" ht="13.65" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
merged with with pull request
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kiry\Documents\oscar-web\db\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4139C4-6C0F-4A48-8F2D-88FADC8987A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC223F2-5974-492E-B392-E56DE6E59B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="267">
   <si>
     <t>name</t>
   </si>
@@ -815,6 +815,18 @@
   </si>
   <si>
     <t>Implementation Log Edit Limitation</t>
+  </si>
+  <si>
+    <t>engagement</t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>Background</t>
   </si>
 </sst>
 </file>
@@ -1725,23 +1737,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW140"/>
+  <dimension ref="A1:IW142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:XFD81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.85546875" style="1"/>
+    <col min="6" max="8" width="11.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -17759,13 +17771,13 @@
     </row>
     <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="19" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B109" s="19" t="s">
         <v>120</v>
       </c>
       <c r="C109" s="85" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D109" s="58"/>
       <c r="E109" s="76" t="s">
@@ -18033,74 +18045,564 @@
       <c r="IW109"/>
     </row>
     <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B110" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="C110" s="58" t="s">
-        <v>229</v>
+      <c r="A110" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>266</v>
       </c>
       <c r="D110" s="58"/>
-      <c r="E110" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="F110" s="96" t="s">
+      <c r="E110" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F110" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="25">
         <v>0</v>
       </c>
-      <c r="H110" s="97">
+      <c r="H110" s="25">
         <v>1</v>
       </c>
-      <c r="I110" s="96" t="s">
-        <v>173</v>
-      </c>
-      <c r="J110" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I110" s="10"/>
+      <c r="J110" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K110"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110"/>
+      <c r="R110"/>
+      <c r="S110"/>
+      <c r="T110"/>
+      <c r="U110"/>
+      <c r="V110"/>
+      <c r="W110"/>
+      <c r="X110"/>
+      <c r="Y110"/>
+      <c r="Z110"/>
+      <c r="AA110"/>
+      <c r="AB110"/>
+      <c r="AC110"/>
+      <c r="AD110"/>
+      <c r="AE110"/>
+      <c r="AF110"/>
+      <c r="AG110"/>
+      <c r="AH110"/>
+      <c r="AI110"/>
+      <c r="AJ110"/>
+      <c r="AK110"/>
+      <c r="AL110"/>
+      <c r="AM110"/>
+      <c r="AN110"/>
+      <c r="AO110"/>
+      <c r="AP110"/>
+      <c r="AQ110"/>
+      <c r="AR110"/>
+      <c r="AS110"/>
+      <c r="AT110"/>
+      <c r="AU110"/>
+      <c r="AV110"/>
+      <c r="AW110"/>
+      <c r="AX110"/>
+      <c r="AY110"/>
+      <c r="AZ110"/>
+      <c r="BA110"/>
+      <c r="BB110"/>
+      <c r="BC110"/>
+      <c r="BD110"/>
+      <c r="BE110"/>
+      <c r="BF110"/>
+      <c r="BG110"/>
+      <c r="BH110"/>
+      <c r="BI110"/>
+      <c r="BJ110"/>
+      <c r="BK110"/>
+      <c r="BL110"/>
+      <c r="BM110"/>
+      <c r="BN110"/>
+      <c r="BO110"/>
+      <c r="BP110"/>
+      <c r="BQ110"/>
+      <c r="BR110"/>
+      <c r="BS110"/>
+      <c r="BT110"/>
+      <c r="BU110"/>
+      <c r="BV110"/>
+      <c r="BW110"/>
+      <c r="BX110"/>
+      <c r="BY110"/>
+      <c r="BZ110"/>
+      <c r="CA110"/>
+      <c r="CB110"/>
+      <c r="CC110"/>
+      <c r="CD110"/>
+      <c r="CE110"/>
+      <c r="CF110"/>
+      <c r="CG110"/>
+      <c r="CH110"/>
+      <c r="CI110"/>
+      <c r="CJ110"/>
+      <c r="CK110"/>
+      <c r="CL110"/>
+      <c r="CM110"/>
+      <c r="CN110"/>
+      <c r="CO110"/>
+      <c r="CP110"/>
+      <c r="CQ110"/>
+      <c r="CR110"/>
+      <c r="CS110"/>
+      <c r="CT110"/>
+      <c r="CU110"/>
+      <c r="CV110"/>
+      <c r="CW110"/>
+      <c r="CX110"/>
+      <c r="CY110"/>
+      <c r="CZ110"/>
+      <c r="DA110"/>
+      <c r="DB110"/>
+      <c r="DC110"/>
+      <c r="DD110"/>
+      <c r="DE110"/>
+      <c r="DF110"/>
+      <c r="DG110"/>
+      <c r="DH110"/>
+      <c r="DI110"/>
+      <c r="DJ110"/>
+      <c r="DK110"/>
+      <c r="DL110"/>
+      <c r="DM110"/>
+      <c r="DN110"/>
+      <c r="DO110"/>
+      <c r="DP110"/>
+      <c r="DQ110"/>
+      <c r="DR110"/>
+      <c r="DS110"/>
+      <c r="DT110"/>
+      <c r="DU110"/>
+      <c r="DV110"/>
+      <c r="DW110"/>
+      <c r="DX110"/>
+      <c r="DY110"/>
+      <c r="DZ110"/>
+      <c r="EA110"/>
+      <c r="EB110"/>
+      <c r="EC110"/>
+      <c r="ED110"/>
+      <c r="EE110"/>
+      <c r="EF110"/>
+      <c r="EG110"/>
+      <c r="EH110"/>
+      <c r="EI110"/>
+      <c r="EJ110"/>
+      <c r="EK110"/>
+      <c r="EL110"/>
+      <c r="EM110"/>
+      <c r="EN110"/>
+      <c r="EO110"/>
+      <c r="EP110"/>
+      <c r="EQ110"/>
+      <c r="ER110"/>
+      <c r="ES110"/>
+      <c r="ET110"/>
+      <c r="EU110"/>
+      <c r="EV110"/>
+      <c r="EW110"/>
+      <c r="EX110"/>
+      <c r="EY110"/>
+      <c r="EZ110"/>
+      <c r="FA110"/>
+      <c r="FB110"/>
+      <c r="FC110"/>
+      <c r="FD110"/>
+      <c r="FE110"/>
+      <c r="FF110"/>
+      <c r="FG110"/>
+      <c r="FH110"/>
+      <c r="FI110"/>
+      <c r="FJ110"/>
+      <c r="FK110"/>
+      <c r="FL110"/>
+      <c r="FM110"/>
+      <c r="FN110"/>
+      <c r="FO110"/>
+      <c r="FP110"/>
+      <c r="FQ110"/>
+      <c r="FR110"/>
+      <c r="FS110"/>
+      <c r="FT110"/>
+      <c r="FU110"/>
+      <c r="FV110"/>
+      <c r="FW110"/>
+      <c r="FX110"/>
+      <c r="FY110"/>
+      <c r="FZ110"/>
+      <c r="GA110"/>
+      <c r="GB110"/>
+      <c r="GC110"/>
+      <c r="GD110"/>
+      <c r="GE110"/>
+      <c r="GF110"/>
+      <c r="GG110"/>
+      <c r="GH110"/>
+      <c r="GI110"/>
+      <c r="GJ110"/>
+      <c r="GK110"/>
+      <c r="GL110"/>
+      <c r="GM110"/>
+      <c r="GN110"/>
+      <c r="GO110"/>
+      <c r="GP110"/>
+      <c r="GQ110"/>
+      <c r="GR110"/>
+      <c r="GS110"/>
+      <c r="GT110"/>
+      <c r="GU110"/>
+      <c r="GV110"/>
+      <c r="GW110"/>
+      <c r="GX110"/>
+      <c r="GY110"/>
+      <c r="GZ110"/>
+      <c r="HA110"/>
+      <c r="HB110"/>
+      <c r="HC110"/>
+      <c r="HD110"/>
+      <c r="HE110"/>
+      <c r="HF110"/>
+      <c r="HG110"/>
+      <c r="HH110"/>
+      <c r="HI110"/>
+      <c r="HJ110"/>
+      <c r="HK110"/>
+      <c r="HL110"/>
+      <c r="HM110"/>
+      <c r="HN110"/>
+      <c r="HO110"/>
+      <c r="HP110"/>
+      <c r="HQ110"/>
+      <c r="HR110"/>
+      <c r="HS110"/>
+      <c r="HT110"/>
+      <c r="HU110"/>
+      <c r="HV110"/>
+      <c r="HW110"/>
+      <c r="HX110"/>
+      <c r="HY110"/>
+      <c r="HZ110"/>
+      <c r="IA110"/>
+      <c r="IB110"/>
+      <c r="IC110"/>
+      <c r="ID110"/>
+      <c r="IE110"/>
+      <c r="IF110"/>
+      <c r="IG110"/>
+      <c r="IH110"/>
+      <c r="II110"/>
+      <c r="IJ110"/>
+      <c r="IK110"/>
+      <c r="IL110"/>
+      <c r="IM110"/>
+      <c r="IN110"/>
+      <c r="IO110"/>
+      <c r="IP110"/>
+      <c r="IQ110"/>
+      <c r="IR110"/>
+      <c r="IS110"/>
+      <c r="IT110"/>
+      <c r="IU110"/>
+      <c r="IV110"/>
+      <c r="IW110"/>
     </row>
     <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B111" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="C111" s="58" t="s">
-        <v>231</v>
+      <c r="A111" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" s="85" t="s">
+        <v>78</v>
       </c>
       <c r="D111" s="58"/>
-      <c r="E111" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="F111" s="96" t="s">
+      <c r="E111" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F111" s="76" t="s">
         <v>13</v>
       </c>
       <c r="G111" s="25">
         <v>0</v>
       </c>
-      <c r="H111" s="58">
+      <c r="H111" s="25">
         <v>1</v>
       </c>
-      <c r="I111" s="96" t="s">
-        <v>173</v>
-      </c>
-      <c r="J111" s="96" t="s">
-        <v>29</v>
-      </c>
+      <c r="I111" s="10"/>
+      <c r="J111" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K111"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+      <c r="P111"/>
+      <c r="Q111"/>
+      <c r="R111"/>
+      <c r="S111"/>
+      <c r="T111"/>
+      <c r="U111"/>
+      <c r="V111"/>
+      <c r="W111"/>
+      <c r="X111"/>
+      <c r="Y111"/>
+      <c r="Z111"/>
+      <c r="AA111"/>
+      <c r="AB111"/>
+      <c r="AC111"/>
+      <c r="AD111"/>
+      <c r="AE111"/>
+      <c r="AF111"/>
+      <c r="AG111"/>
+      <c r="AH111"/>
+      <c r="AI111"/>
+      <c r="AJ111"/>
+      <c r="AK111"/>
+      <c r="AL111"/>
+      <c r="AM111"/>
+      <c r="AN111"/>
+      <c r="AO111"/>
+      <c r="AP111"/>
+      <c r="AQ111"/>
+      <c r="AR111"/>
+      <c r="AS111"/>
+      <c r="AT111"/>
+      <c r="AU111"/>
+      <c r="AV111"/>
+      <c r="AW111"/>
+      <c r="AX111"/>
+      <c r="AY111"/>
+      <c r="AZ111"/>
+      <c r="BA111"/>
+      <c r="BB111"/>
+      <c r="BC111"/>
+      <c r="BD111"/>
+      <c r="BE111"/>
+      <c r="BF111"/>
+      <c r="BG111"/>
+      <c r="BH111"/>
+      <c r="BI111"/>
+      <c r="BJ111"/>
+      <c r="BK111"/>
+      <c r="BL111"/>
+      <c r="BM111"/>
+      <c r="BN111"/>
+      <c r="BO111"/>
+      <c r="BP111"/>
+      <c r="BQ111"/>
+      <c r="BR111"/>
+      <c r="BS111"/>
+      <c r="BT111"/>
+      <c r="BU111"/>
+      <c r="BV111"/>
+      <c r="BW111"/>
+      <c r="BX111"/>
+      <c r="BY111"/>
+      <c r="BZ111"/>
+      <c r="CA111"/>
+      <c r="CB111"/>
+      <c r="CC111"/>
+      <c r="CD111"/>
+      <c r="CE111"/>
+      <c r="CF111"/>
+      <c r="CG111"/>
+      <c r="CH111"/>
+      <c r="CI111"/>
+      <c r="CJ111"/>
+      <c r="CK111"/>
+      <c r="CL111"/>
+      <c r="CM111"/>
+      <c r="CN111"/>
+      <c r="CO111"/>
+      <c r="CP111"/>
+      <c r="CQ111"/>
+      <c r="CR111"/>
+      <c r="CS111"/>
+      <c r="CT111"/>
+      <c r="CU111"/>
+      <c r="CV111"/>
+      <c r="CW111"/>
+      <c r="CX111"/>
+      <c r="CY111"/>
+      <c r="CZ111"/>
+      <c r="DA111"/>
+      <c r="DB111"/>
+      <c r="DC111"/>
+      <c r="DD111"/>
+      <c r="DE111"/>
+      <c r="DF111"/>
+      <c r="DG111"/>
+      <c r="DH111"/>
+      <c r="DI111"/>
+      <c r="DJ111"/>
+      <c r="DK111"/>
+      <c r="DL111"/>
+      <c r="DM111"/>
+      <c r="DN111"/>
+      <c r="DO111"/>
+      <c r="DP111"/>
+      <c r="DQ111"/>
+      <c r="DR111"/>
+      <c r="DS111"/>
+      <c r="DT111"/>
+      <c r="DU111"/>
+      <c r="DV111"/>
+      <c r="DW111"/>
+      <c r="DX111"/>
+      <c r="DY111"/>
+      <c r="DZ111"/>
+      <c r="EA111"/>
+      <c r="EB111"/>
+      <c r="EC111"/>
+      <c r="ED111"/>
+      <c r="EE111"/>
+      <c r="EF111"/>
+      <c r="EG111"/>
+      <c r="EH111"/>
+      <c r="EI111"/>
+      <c r="EJ111"/>
+      <c r="EK111"/>
+      <c r="EL111"/>
+      <c r="EM111"/>
+      <c r="EN111"/>
+      <c r="EO111"/>
+      <c r="EP111"/>
+      <c r="EQ111"/>
+      <c r="ER111"/>
+      <c r="ES111"/>
+      <c r="ET111"/>
+      <c r="EU111"/>
+      <c r="EV111"/>
+      <c r="EW111"/>
+      <c r="EX111"/>
+      <c r="EY111"/>
+      <c r="EZ111"/>
+      <c r="FA111"/>
+      <c r="FB111"/>
+      <c r="FC111"/>
+      <c r="FD111"/>
+      <c r="FE111"/>
+      <c r="FF111"/>
+      <c r="FG111"/>
+      <c r="FH111"/>
+      <c r="FI111"/>
+      <c r="FJ111"/>
+      <c r="FK111"/>
+      <c r="FL111"/>
+      <c r="FM111"/>
+      <c r="FN111"/>
+      <c r="FO111"/>
+      <c r="FP111"/>
+      <c r="FQ111"/>
+      <c r="FR111"/>
+      <c r="FS111"/>
+      <c r="FT111"/>
+      <c r="FU111"/>
+      <c r="FV111"/>
+      <c r="FW111"/>
+      <c r="FX111"/>
+      <c r="FY111"/>
+      <c r="FZ111"/>
+      <c r="GA111"/>
+      <c r="GB111"/>
+      <c r="GC111"/>
+      <c r="GD111"/>
+      <c r="GE111"/>
+      <c r="GF111"/>
+      <c r="GG111"/>
+      <c r="GH111"/>
+      <c r="GI111"/>
+      <c r="GJ111"/>
+      <c r="GK111"/>
+      <c r="GL111"/>
+      <c r="GM111"/>
+      <c r="GN111"/>
+      <c r="GO111"/>
+      <c r="GP111"/>
+      <c r="GQ111"/>
+      <c r="GR111"/>
+      <c r="GS111"/>
+      <c r="GT111"/>
+      <c r="GU111"/>
+      <c r="GV111"/>
+      <c r="GW111"/>
+      <c r="GX111"/>
+      <c r="GY111"/>
+      <c r="GZ111"/>
+      <c r="HA111"/>
+      <c r="HB111"/>
+      <c r="HC111"/>
+      <c r="HD111"/>
+      <c r="HE111"/>
+      <c r="HF111"/>
+      <c r="HG111"/>
+      <c r="HH111"/>
+      <c r="HI111"/>
+      <c r="HJ111"/>
+      <c r="HK111"/>
+      <c r="HL111"/>
+      <c r="HM111"/>
+      <c r="HN111"/>
+      <c r="HO111"/>
+      <c r="HP111"/>
+      <c r="HQ111"/>
+      <c r="HR111"/>
+      <c r="HS111"/>
+      <c r="HT111"/>
+      <c r="HU111"/>
+      <c r="HV111"/>
+      <c r="HW111"/>
+      <c r="HX111"/>
+      <c r="HY111"/>
+      <c r="HZ111"/>
+      <c r="IA111"/>
+      <c r="IB111"/>
+      <c r="IC111"/>
+      <c r="ID111"/>
+      <c r="IE111"/>
+      <c r="IF111"/>
+      <c r="IG111"/>
+      <c r="IH111"/>
+      <c r="II111"/>
+      <c r="IJ111"/>
+      <c r="IK111"/>
+      <c r="IL111"/>
+      <c r="IM111"/>
+      <c r="IN111"/>
+      <c r="IO111"/>
+      <c r="IP111"/>
+      <c r="IQ111"/>
+      <c r="IR111"/>
+      <c r="IS111"/>
+      <c r="IT111"/>
+      <c r="IU111"/>
+      <c r="IV111"/>
+      <c r="IW111"/>
     </row>
     <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B112" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C112" s="58" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D112" s="58"/>
       <c r="E112" s="96" t="s">
@@ -18112,7 +18614,7 @@
       <c r="G112" s="25">
         <v>0</v>
       </c>
-      <c r="H112" s="58">
+      <c r="H112" s="97">
         <v>1</v>
       </c>
       <c r="I112" s="96" t="s">
@@ -18124,13 +18626,13 @@
     </row>
     <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="B113" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C113" s="58" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="D113" s="58"/>
       <c r="E113" s="96" t="s">
@@ -18154,13 +18656,13 @@
     </row>
     <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B114" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C114" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D114" s="58"/>
       <c r="E114" s="96" t="s">
@@ -18170,7 +18672,7 @@
         <v>13</v>
       </c>
       <c r="G114" s="25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H114" s="58">
         <v>1</v>
@@ -18184,13 +18686,13 @@
     </row>
     <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="B115" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C115" s="58" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="D115" s="58"/>
       <c r="E115" s="96" t="s">
@@ -18214,13 +18716,13 @@
     </row>
     <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B116" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C116" s="58" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D116" s="58"/>
       <c r="E116" s="96" t="s">
@@ -18230,7 +18732,7 @@
         <v>13</v>
       </c>
       <c r="G116" s="25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H116" s="58">
         <v>1</v>
@@ -18244,13 +18746,13 @@
     </row>
     <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B117" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C117" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D117" s="58"/>
       <c r="E117" s="96" t="s">
@@ -18274,13 +18776,13 @@
     </row>
     <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B118" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C118" s="95" t="s">
-        <v>237</v>
+      <c r="C118" s="58" t="s">
+        <v>239</v>
       </c>
       <c r="D118" s="58"/>
       <c r="E118" s="96" t="s">
@@ -18304,13 +18806,13 @@
     </row>
     <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B119" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C119" s="95" t="s">
-        <v>241</v>
+      <c r="C119" s="58" t="s">
+        <v>235</v>
       </c>
       <c r="D119" s="58"/>
       <c r="E119" s="96" t="s">
@@ -18334,13 +18836,13 @@
     </row>
     <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B120" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C120" s="58" t="s">
-        <v>236</v>
+      <c r="C120" s="95" t="s">
+        <v>237</v>
       </c>
       <c r="D120" s="58"/>
       <c r="E120" s="96" t="s">
@@ -18364,13 +18866,13 @@
     </row>
     <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B121" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C121" s="58" t="s">
-        <v>243</v>
+      <c r="C121" s="95" t="s">
+        <v>241</v>
       </c>
       <c r="D121" s="58"/>
       <c r="E121" s="96" t="s">
@@ -18394,13 +18896,13 @@
     </row>
     <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>152</v>
+        <v>227</v>
       </c>
       <c r="B122" s="58" t="s">
         <v>228</v>
       </c>
       <c r="C122" s="58" t="s">
-        <v>167</v>
+        <v>236</v>
       </c>
       <c r="D122" s="58"/>
       <c r="E122" s="96" t="s">
@@ -18423,572 +18925,78 @@
       </c>
     </row>
     <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="B123" s="57" t="s">
+      <c r="C123" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="D123" s="58"/>
+      <c r="E123" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="C123" s="57" t="s">
-        <v>255</v>
-      </c>
-      <c r="D123" s="57"/>
-      <c r="E123" s="98" t="s">
-        <v>228</v>
-      </c>
-      <c r="F123" s="98" t="s">
+      <c r="F123" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G123" s="81">
+      <c r="G123" s="25">
         <v>0</v>
       </c>
-      <c r="H123" s="57">
+      <c r="H123" s="58">
         <v>1</v>
       </c>
-      <c r="I123" s="98" t="s">
+      <c r="I123" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="J123" s="98" t="s">
+      <c r="J123" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K123"/>
-      <c r="L123"/>
-      <c r="M123"/>
-      <c r="N123"/>
-      <c r="O123"/>
-      <c r="P123"/>
-      <c r="Q123"/>
-      <c r="R123"/>
-      <c r="S123"/>
-      <c r="T123"/>
-      <c r="U123"/>
-      <c r="V123"/>
-      <c r="W123"/>
-      <c r="X123"/>
-      <c r="Y123"/>
-      <c r="Z123"/>
-      <c r="AA123"/>
-      <c r="AB123"/>
-      <c r="AC123"/>
-      <c r="AD123"/>
-      <c r="AE123"/>
-      <c r="AF123"/>
-      <c r="AG123"/>
-      <c r="AH123"/>
-      <c r="AI123"/>
-      <c r="AJ123"/>
-      <c r="AK123"/>
-      <c r="AL123"/>
-      <c r="AM123"/>
-      <c r="AN123"/>
-      <c r="AO123"/>
-      <c r="AP123"/>
-      <c r="AQ123"/>
-      <c r="AR123"/>
-      <c r="AS123"/>
-      <c r="AT123"/>
-      <c r="AU123"/>
-      <c r="AV123"/>
-      <c r="AW123"/>
-      <c r="AX123"/>
-      <c r="AY123"/>
-      <c r="AZ123"/>
-      <c r="BA123"/>
-      <c r="BB123"/>
-      <c r="BC123"/>
-      <c r="BD123"/>
-      <c r="BE123"/>
-      <c r="BF123"/>
-      <c r="BG123"/>
-      <c r="BH123"/>
-      <c r="BI123"/>
-      <c r="BJ123"/>
-      <c r="BK123"/>
-      <c r="BL123"/>
-      <c r="BM123"/>
-      <c r="BN123"/>
-      <c r="BO123"/>
-      <c r="BP123"/>
-      <c r="BQ123"/>
-      <c r="BR123"/>
-      <c r="BS123"/>
-      <c r="BT123"/>
-      <c r="BU123"/>
-      <c r="BV123"/>
-      <c r="BW123"/>
-      <c r="BX123"/>
-      <c r="BY123"/>
-      <c r="BZ123"/>
-      <c r="CA123"/>
-      <c r="CB123"/>
-      <c r="CC123"/>
-      <c r="CD123"/>
-      <c r="CE123"/>
-      <c r="CF123"/>
-      <c r="CG123"/>
-      <c r="CH123"/>
-      <c r="CI123"/>
-      <c r="CJ123"/>
-      <c r="CK123"/>
-      <c r="CL123"/>
-      <c r="CM123"/>
-      <c r="CN123"/>
-      <c r="CO123"/>
-      <c r="CP123"/>
-      <c r="CQ123"/>
-      <c r="CR123"/>
-      <c r="CS123"/>
-      <c r="CT123"/>
-      <c r="CU123"/>
-      <c r="CV123"/>
-      <c r="CW123"/>
-      <c r="CX123"/>
-      <c r="CY123"/>
-      <c r="CZ123"/>
-      <c r="DA123"/>
-      <c r="DB123"/>
-      <c r="DC123"/>
-      <c r="DD123"/>
-      <c r="DE123"/>
-      <c r="DF123"/>
-      <c r="DG123"/>
-      <c r="DH123"/>
-      <c r="DI123"/>
-      <c r="DJ123"/>
-      <c r="DK123"/>
-      <c r="DL123"/>
-      <c r="DM123"/>
-      <c r="DN123"/>
-      <c r="DO123"/>
-      <c r="DP123"/>
-      <c r="DQ123"/>
-      <c r="DR123"/>
-      <c r="DS123"/>
-      <c r="DT123"/>
-      <c r="DU123"/>
-      <c r="DV123"/>
-      <c r="DW123"/>
-      <c r="DX123"/>
-      <c r="DY123"/>
-      <c r="DZ123"/>
-      <c r="EA123"/>
-      <c r="EB123"/>
-      <c r="EC123"/>
-      <c r="ED123"/>
-      <c r="EE123"/>
-      <c r="EF123"/>
-      <c r="EG123"/>
-      <c r="EH123"/>
-      <c r="EI123"/>
-      <c r="EJ123"/>
-      <c r="EK123"/>
-      <c r="EL123"/>
-      <c r="EM123"/>
-      <c r="EN123"/>
-      <c r="EO123"/>
-      <c r="EP123"/>
-      <c r="EQ123"/>
-      <c r="ER123"/>
-      <c r="ES123"/>
-      <c r="ET123"/>
-      <c r="EU123"/>
-      <c r="EV123"/>
-      <c r="EW123"/>
-      <c r="EX123"/>
-      <c r="EY123"/>
-      <c r="EZ123"/>
-      <c r="FA123"/>
-      <c r="FB123"/>
-      <c r="FC123"/>
-      <c r="FD123"/>
-      <c r="FE123"/>
-      <c r="FF123"/>
-      <c r="FG123"/>
-      <c r="FH123"/>
-      <c r="FI123"/>
-      <c r="FJ123"/>
-      <c r="FK123"/>
-      <c r="FL123"/>
-      <c r="FM123"/>
-      <c r="FN123"/>
-      <c r="FO123"/>
-      <c r="FP123"/>
-      <c r="FQ123"/>
-      <c r="FR123"/>
-      <c r="FS123"/>
-      <c r="FT123"/>
-      <c r="FU123"/>
-      <c r="FV123"/>
-      <c r="FW123"/>
-      <c r="FX123"/>
-      <c r="FY123"/>
-      <c r="FZ123"/>
-      <c r="GA123"/>
-      <c r="GB123"/>
-      <c r="GC123"/>
-      <c r="GD123"/>
-      <c r="GE123"/>
-      <c r="GF123"/>
-      <c r="GG123"/>
-      <c r="GH123"/>
-      <c r="GI123"/>
-      <c r="GJ123"/>
-      <c r="GK123"/>
-      <c r="GL123"/>
-      <c r="GM123"/>
-      <c r="GN123"/>
-      <c r="GO123"/>
-      <c r="GP123"/>
-      <c r="GQ123"/>
-      <c r="GR123"/>
-      <c r="GS123"/>
-      <c r="GT123"/>
-      <c r="GU123"/>
-      <c r="GV123"/>
-      <c r="GW123"/>
-      <c r="GX123"/>
-      <c r="GY123"/>
-      <c r="GZ123"/>
-      <c r="HA123"/>
-      <c r="HB123"/>
-      <c r="HC123"/>
-      <c r="HD123"/>
-      <c r="HE123"/>
-      <c r="HF123"/>
-      <c r="HG123"/>
-      <c r="HH123"/>
-      <c r="HI123"/>
-      <c r="HJ123"/>
-      <c r="HK123"/>
-      <c r="HL123"/>
-      <c r="HM123"/>
-      <c r="HN123"/>
-      <c r="HO123"/>
-      <c r="HP123"/>
-      <c r="HQ123"/>
-      <c r="HR123"/>
-      <c r="HS123"/>
-      <c r="HT123"/>
-      <c r="HU123"/>
-      <c r="HV123"/>
-      <c r="HW123"/>
-      <c r="HX123"/>
-      <c r="HY123"/>
-      <c r="HZ123"/>
-      <c r="IA123"/>
-      <c r="IB123"/>
-      <c r="IC123"/>
-      <c r="ID123"/>
-      <c r="IE123"/>
-      <c r="IF123"/>
-      <c r="IG123"/>
-      <c r="IH123"/>
-      <c r="II123"/>
-      <c r="IJ123"/>
-      <c r="IK123"/>
-      <c r="IL123"/>
-      <c r="IM123"/>
-      <c r="IN123"/>
-      <c r="IO123"/>
-      <c r="IP123"/>
-      <c r="IQ123"/>
-      <c r="IR123"/>
-      <c r="IS123"/>
-      <c r="IT123"/>
-      <c r="IU123"/>
-      <c r="IV123"/>
-      <c r="IW123"/>
     </row>
     <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A124" s="99" t="s">
-        <v>256</v>
-      </c>
-      <c r="B124" s="57" t="s">
+      <c r="A124" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B124" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C124" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="D124" s="57"/>
-      <c r="E124" s="98" t="s">
+      <c r="C124" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D124" s="58"/>
+      <c r="E124" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="F124" s="98" t="s">
+      <c r="F124" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G124" s="81">
+      <c r="G124" s="25">
         <v>0</v>
       </c>
-      <c r="H124" s="57">
+      <c r="H124" s="58">
         <v>1</v>
       </c>
-      <c r="I124" s="98" t="s">
+      <c r="I124" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="J124" s="98" t="s">
+      <c r="J124" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K124"/>
-      <c r="L124"/>
-      <c r="M124"/>
-      <c r="N124"/>
-      <c r="O124"/>
-      <c r="P124"/>
-      <c r="Q124"/>
-      <c r="R124"/>
-      <c r="S124"/>
-      <c r="T124"/>
-      <c r="U124"/>
-      <c r="V124"/>
-      <c r="W124"/>
-      <c r="X124"/>
-      <c r="Y124"/>
-      <c r="Z124"/>
-      <c r="AA124"/>
-      <c r="AB124"/>
-      <c r="AC124"/>
-      <c r="AD124"/>
-      <c r="AE124"/>
-      <c r="AF124"/>
-      <c r="AG124"/>
-      <c r="AH124"/>
-      <c r="AI124"/>
-      <c r="AJ124"/>
-      <c r="AK124"/>
-      <c r="AL124"/>
-      <c r="AM124"/>
-      <c r="AN124"/>
-      <c r="AO124"/>
-      <c r="AP124"/>
-      <c r="AQ124"/>
-      <c r="AR124"/>
-      <c r="AS124"/>
-      <c r="AT124"/>
-      <c r="AU124"/>
-      <c r="AV124"/>
-      <c r="AW124"/>
-      <c r="AX124"/>
-      <c r="AY124"/>
-      <c r="AZ124"/>
-      <c r="BA124"/>
-      <c r="BB124"/>
-      <c r="BC124"/>
-      <c r="BD124"/>
-      <c r="BE124"/>
-      <c r="BF124"/>
-      <c r="BG124"/>
-      <c r="BH124"/>
-      <c r="BI124"/>
-      <c r="BJ124"/>
-      <c r="BK124"/>
-      <c r="BL124"/>
-      <c r="BM124"/>
-      <c r="BN124"/>
-      <c r="BO124"/>
-      <c r="BP124"/>
-      <c r="BQ124"/>
-      <c r="BR124"/>
-      <c r="BS124"/>
-      <c r="BT124"/>
-      <c r="BU124"/>
-      <c r="BV124"/>
-      <c r="BW124"/>
-      <c r="BX124"/>
-      <c r="BY124"/>
-      <c r="BZ124"/>
-      <c r="CA124"/>
-      <c r="CB124"/>
-      <c r="CC124"/>
-      <c r="CD124"/>
-      <c r="CE124"/>
-      <c r="CF124"/>
-      <c r="CG124"/>
-      <c r="CH124"/>
-      <c r="CI124"/>
-      <c r="CJ124"/>
-      <c r="CK124"/>
-      <c r="CL124"/>
-      <c r="CM124"/>
-      <c r="CN124"/>
-      <c r="CO124"/>
-      <c r="CP124"/>
-      <c r="CQ124"/>
-      <c r="CR124"/>
-      <c r="CS124"/>
-      <c r="CT124"/>
-      <c r="CU124"/>
-      <c r="CV124"/>
-      <c r="CW124"/>
-      <c r="CX124"/>
-      <c r="CY124"/>
-      <c r="CZ124"/>
-      <c r="DA124"/>
-      <c r="DB124"/>
-      <c r="DC124"/>
-      <c r="DD124"/>
-      <c r="DE124"/>
-      <c r="DF124"/>
-      <c r="DG124"/>
-      <c r="DH124"/>
-      <c r="DI124"/>
-      <c r="DJ124"/>
-      <c r="DK124"/>
-      <c r="DL124"/>
-      <c r="DM124"/>
-      <c r="DN124"/>
-      <c r="DO124"/>
-      <c r="DP124"/>
-      <c r="DQ124"/>
-      <c r="DR124"/>
-      <c r="DS124"/>
-      <c r="DT124"/>
-      <c r="DU124"/>
-      <c r="DV124"/>
-      <c r="DW124"/>
-      <c r="DX124"/>
-      <c r="DY124"/>
-      <c r="DZ124"/>
-      <c r="EA124"/>
-      <c r="EB124"/>
-      <c r="EC124"/>
-      <c r="ED124"/>
-      <c r="EE124"/>
-      <c r="EF124"/>
-      <c r="EG124"/>
-      <c r="EH124"/>
-      <c r="EI124"/>
-      <c r="EJ124"/>
-      <c r="EK124"/>
-      <c r="EL124"/>
-      <c r="EM124"/>
-      <c r="EN124"/>
-      <c r="EO124"/>
-      <c r="EP124"/>
-      <c r="EQ124"/>
-      <c r="ER124"/>
-      <c r="ES124"/>
-      <c r="ET124"/>
-      <c r="EU124"/>
-      <c r="EV124"/>
-      <c r="EW124"/>
-      <c r="EX124"/>
-      <c r="EY124"/>
-      <c r="EZ124"/>
-      <c r="FA124"/>
-      <c r="FB124"/>
-      <c r="FC124"/>
-      <c r="FD124"/>
-      <c r="FE124"/>
-      <c r="FF124"/>
-      <c r="FG124"/>
-      <c r="FH124"/>
-      <c r="FI124"/>
-      <c r="FJ124"/>
-      <c r="FK124"/>
-      <c r="FL124"/>
-      <c r="FM124"/>
-      <c r="FN124"/>
-      <c r="FO124"/>
-      <c r="FP124"/>
-      <c r="FQ124"/>
-      <c r="FR124"/>
-      <c r="FS124"/>
-      <c r="FT124"/>
-      <c r="FU124"/>
-      <c r="FV124"/>
-      <c r="FW124"/>
-      <c r="FX124"/>
-      <c r="FY124"/>
-      <c r="FZ124"/>
-      <c r="GA124"/>
-      <c r="GB124"/>
-      <c r="GC124"/>
-      <c r="GD124"/>
-      <c r="GE124"/>
-      <c r="GF124"/>
-      <c r="GG124"/>
-      <c r="GH124"/>
-      <c r="GI124"/>
-      <c r="GJ124"/>
-      <c r="GK124"/>
-      <c r="GL124"/>
-      <c r="GM124"/>
-      <c r="GN124"/>
-      <c r="GO124"/>
-      <c r="GP124"/>
-      <c r="GQ124"/>
-      <c r="GR124"/>
-      <c r="GS124"/>
-      <c r="GT124"/>
-      <c r="GU124"/>
-      <c r="GV124"/>
-      <c r="GW124"/>
-      <c r="GX124"/>
-      <c r="GY124"/>
-      <c r="GZ124"/>
-      <c r="HA124"/>
-      <c r="HB124"/>
-      <c r="HC124"/>
-      <c r="HD124"/>
-      <c r="HE124"/>
-      <c r="HF124"/>
-      <c r="HG124"/>
-      <c r="HH124"/>
-      <c r="HI124"/>
-      <c r="HJ124"/>
-      <c r="HK124"/>
-      <c r="HL124"/>
-      <c r="HM124"/>
-      <c r="HN124"/>
-      <c r="HO124"/>
-      <c r="HP124"/>
-      <c r="HQ124"/>
-      <c r="HR124"/>
-      <c r="HS124"/>
-      <c r="HT124"/>
-      <c r="HU124"/>
-      <c r="HV124"/>
-      <c r="HW124"/>
-      <c r="HX124"/>
-      <c r="HY124"/>
-      <c r="HZ124"/>
-      <c r="IA124"/>
-      <c r="IB124"/>
-      <c r="IC124"/>
-      <c r="ID124"/>
-      <c r="IE124"/>
-      <c r="IF124"/>
-      <c r="IG124"/>
-      <c r="IH124"/>
-      <c r="II124"/>
-      <c r="IJ124"/>
-      <c r="IK124"/>
-      <c r="IL124"/>
-      <c r="IM124"/>
-      <c r="IN124"/>
-      <c r="IO124"/>
-      <c r="IP124"/>
-      <c r="IQ124"/>
-      <c r="IR124"/>
-      <c r="IS124"/>
-      <c r="IT124"/>
-      <c r="IU124"/>
-      <c r="IV124"/>
-      <c r="IW124"/>
     </row>
     <row r="125" spans="1:257" ht="17.100000000000001" customHeight="1">
-      <c r="A125" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="B125" s="98" t="s">
-        <v>259</v>
-      </c>
-      <c r="C125" s="98" t="s">
-        <v>260</v>
+      <c r="A125" t="s">
+        <v>228</v>
+      </c>
+      <c r="B125" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C125" s="57" t="s">
+        <v>255</v>
       </c>
       <c r="D125" s="57"/>
       <c r="E125" s="98" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="F125" s="98" t="s">
         <v>13</v>
@@ -19255,17 +19263,17 @@
     </row>
     <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1">
       <c r="A126" s="99" t="s">
-        <v>261</v>
-      </c>
-      <c r="B126" s="98" t="s">
-        <v>259</v>
+        <v>256</v>
+      </c>
+      <c r="B126" s="57" t="s">
+        <v>228</v>
       </c>
       <c r="C126" s="98" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D126" s="57"/>
       <c r="E126" s="98" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="F126" s="98" t="s">
         <v>13</v>
@@ -19530,8 +19538,560 @@
       <c r="IV126"/>
       <c r="IW126"/>
     </row>
-    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1"/>
-    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1"/>
+    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A127" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="B127" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C127" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="D127" s="57"/>
+      <c r="E127" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="F127" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="81">
+        <v>0</v>
+      </c>
+      <c r="H127" s="57">
+        <v>1</v>
+      </c>
+      <c r="I127" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J127" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127"/>
+      <c r="N127"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
+      <c r="R127"/>
+      <c r="S127"/>
+      <c r="T127"/>
+      <c r="U127"/>
+      <c r="V127"/>
+      <c r="W127"/>
+      <c r="X127"/>
+      <c r="Y127"/>
+      <c r="Z127"/>
+      <c r="AA127"/>
+      <c r="AB127"/>
+      <c r="AC127"/>
+      <c r="AD127"/>
+      <c r="AE127"/>
+      <c r="AF127"/>
+      <c r="AG127"/>
+      <c r="AH127"/>
+      <c r="AI127"/>
+      <c r="AJ127"/>
+      <c r="AK127"/>
+      <c r="AL127"/>
+      <c r="AM127"/>
+      <c r="AN127"/>
+      <c r="AO127"/>
+      <c r="AP127"/>
+      <c r="AQ127"/>
+      <c r="AR127"/>
+      <c r="AS127"/>
+      <c r="AT127"/>
+      <c r="AU127"/>
+      <c r="AV127"/>
+      <c r="AW127"/>
+      <c r="AX127"/>
+      <c r="AY127"/>
+      <c r="AZ127"/>
+      <c r="BA127"/>
+      <c r="BB127"/>
+      <c r="BC127"/>
+      <c r="BD127"/>
+      <c r="BE127"/>
+      <c r="BF127"/>
+      <c r="BG127"/>
+      <c r="BH127"/>
+      <c r="BI127"/>
+      <c r="BJ127"/>
+      <c r="BK127"/>
+      <c r="BL127"/>
+      <c r="BM127"/>
+      <c r="BN127"/>
+      <c r="BO127"/>
+      <c r="BP127"/>
+      <c r="BQ127"/>
+      <c r="BR127"/>
+      <c r="BS127"/>
+      <c r="BT127"/>
+      <c r="BU127"/>
+      <c r="BV127"/>
+      <c r="BW127"/>
+      <c r="BX127"/>
+      <c r="BY127"/>
+      <c r="BZ127"/>
+      <c r="CA127"/>
+      <c r="CB127"/>
+      <c r="CC127"/>
+      <c r="CD127"/>
+      <c r="CE127"/>
+      <c r="CF127"/>
+      <c r="CG127"/>
+      <c r="CH127"/>
+      <c r="CI127"/>
+      <c r="CJ127"/>
+      <c r="CK127"/>
+      <c r="CL127"/>
+      <c r="CM127"/>
+      <c r="CN127"/>
+      <c r="CO127"/>
+      <c r="CP127"/>
+      <c r="CQ127"/>
+      <c r="CR127"/>
+      <c r="CS127"/>
+      <c r="CT127"/>
+      <c r="CU127"/>
+      <c r="CV127"/>
+      <c r="CW127"/>
+      <c r="CX127"/>
+      <c r="CY127"/>
+      <c r="CZ127"/>
+      <c r="DA127"/>
+      <c r="DB127"/>
+      <c r="DC127"/>
+      <c r="DD127"/>
+      <c r="DE127"/>
+      <c r="DF127"/>
+      <c r="DG127"/>
+      <c r="DH127"/>
+      <c r="DI127"/>
+      <c r="DJ127"/>
+      <c r="DK127"/>
+      <c r="DL127"/>
+      <c r="DM127"/>
+      <c r="DN127"/>
+      <c r="DO127"/>
+      <c r="DP127"/>
+      <c r="DQ127"/>
+      <c r="DR127"/>
+      <c r="DS127"/>
+      <c r="DT127"/>
+      <c r="DU127"/>
+      <c r="DV127"/>
+      <c r="DW127"/>
+      <c r="DX127"/>
+      <c r="DY127"/>
+      <c r="DZ127"/>
+      <c r="EA127"/>
+      <c r="EB127"/>
+      <c r="EC127"/>
+      <c r="ED127"/>
+      <c r="EE127"/>
+      <c r="EF127"/>
+      <c r="EG127"/>
+      <c r="EH127"/>
+      <c r="EI127"/>
+      <c r="EJ127"/>
+      <c r="EK127"/>
+      <c r="EL127"/>
+      <c r="EM127"/>
+      <c r="EN127"/>
+      <c r="EO127"/>
+      <c r="EP127"/>
+      <c r="EQ127"/>
+      <c r="ER127"/>
+      <c r="ES127"/>
+      <c r="ET127"/>
+      <c r="EU127"/>
+      <c r="EV127"/>
+      <c r="EW127"/>
+      <c r="EX127"/>
+      <c r="EY127"/>
+      <c r="EZ127"/>
+      <c r="FA127"/>
+      <c r="FB127"/>
+      <c r="FC127"/>
+      <c r="FD127"/>
+      <c r="FE127"/>
+      <c r="FF127"/>
+      <c r="FG127"/>
+      <c r="FH127"/>
+      <c r="FI127"/>
+      <c r="FJ127"/>
+      <c r="FK127"/>
+      <c r="FL127"/>
+      <c r="FM127"/>
+      <c r="FN127"/>
+      <c r="FO127"/>
+      <c r="FP127"/>
+      <c r="FQ127"/>
+      <c r="FR127"/>
+      <c r="FS127"/>
+      <c r="FT127"/>
+      <c r="FU127"/>
+      <c r="FV127"/>
+      <c r="FW127"/>
+      <c r="FX127"/>
+      <c r="FY127"/>
+      <c r="FZ127"/>
+      <c r="GA127"/>
+      <c r="GB127"/>
+      <c r="GC127"/>
+      <c r="GD127"/>
+      <c r="GE127"/>
+      <c r="GF127"/>
+      <c r="GG127"/>
+      <c r="GH127"/>
+      <c r="GI127"/>
+      <c r="GJ127"/>
+      <c r="GK127"/>
+      <c r="GL127"/>
+      <c r="GM127"/>
+      <c r="GN127"/>
+      <c r="GO127"/>
+      <c r="GP127"/>
+      <c r="GQ127"/>
+      <c r="GR127"/>
+      <c r="GS127"/>
+      <c r="GT127"/>
+      <c r="GU127"/>
+      <c r="GV127"/>
+      <c r="GW127"/>
+      <c r="GX127"/>
+      <c r="GY127"/>
+      <c r="GZ127"/>
+      <c r="HA127"/>
+      <c r="HB127"/>
+      <c r="HC127"/>
+      <c r="HD127"/>
+      <c r="HE127"/>
+      <c r="HF127"/>
+      <c r="HG127"/>
+      <c r="HH127"/>
+      <c r="HI127"/>
+      <c r="HJ127"/>
+      <c r="HK127"/>
+      <c r="HL127"/>
+      <c r="HM127"/>
+      <c r="HN127"/>
+      <c r="HO127"/>
+      <c r="HP127"/>
+      <c r="HQ127"/>
+      <c r="HR127"/>
+      <c r="HS127"/>
+      <c r="HT127"/>
+      <c r="HU127"/>
+      <c r="HV127"/>
+      <c r="HW127"/>
+      <c r="HX127"/>
+      <c r="HY127"/>
+      <c r="HZ127"/>
+      <c r="IA127"/>
+      <c r="IB127"/>
+      <c r="IC127"/>
+      <c r="ID127"/>
+      <c r="IE127"/>
+      <c r="IF127"/>
+      <c r="IG127"/>
+      <c r="IH127"/>
+      <c r="II127"/>
+      <c r="IJ127"/>
+      <c r="IK127"/>
+      <c r="IL127"/>
+      <c r="IM127"/>
+      <c r="IN127"/>
+      <c r="IO127"/>
+      <c r="IP127"/>
+      <c r="IQ127"/>
+      <c r="IR127"/>
+      <c r="IS127"/>
+      <c r="IT127"/>
+      <c r="IU127"/>
+      <c r="IV127"/>
+      <c r="IW127"/>
+    </row>
+    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1">
+      <c r="A128" s="99" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C128" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="D128" s="57"/>
+      <c r="E128" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="F128" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G128" s="81">
+        <v>0</v>
+      </c>
+      <c r="H128" s="57">
+        <v>1</v>
+      </c>
+      <c r="I128" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="J128" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="K128"/>
+      <c r="L128"/>
+      <c r="M128"/>
+      <c r="N128"/>
+      <c r="O128"/>
+      <c r="P128"/>
+      <c r="Q128"/>
+      <c r="R128"/>
+      <c r="S128"/>
+      <c r="T128"/>
+      <c r="U128"/>
+      <c r="V128"/>
+      <c r="W128"/>
+      <c r="X128"/>
+      <c r="Y128"/>
+      <c r="Z128"/>
+      <c r="AA128"/>
+      <c r="AB128"/>
+      <c r="AC128"/>
+      <c r="AD128"/>
+      <c r="AE128"/>
+      <c r="AF128"/>
+      <c r="AG128"/>
+      <c r="AH128"/>
+      <c r="AI128"/>
+      <c r="AJ128"/>
+      <c r="AK128"/>
+      <c r="AL128"/>
+      <c r="AM128"/>
+      <c r="AN128"/>
+      <c r="AO128"/>
+      <c r="AP128"/>
+      <c r="AQ128"/>
+      <c r="AR128"/>
+      <c r="AS128"/>
+      <c r="AT128"/>
+      <c r="AU128"/>
+      <c r="AV128"/>
+      <c r="AW128"/>
+      <c r="AX128"/>
+      <c r="AY128"/>
+      <c r="AZ128"/>
+      <c r="BA128"/>
+      <c r="BB128"/>
+      <c r="BC128"/>
+      <c r="BD128"/>
+      <c r="BE128"/>
+      <c r="BF128"/>
+      <c r="BG128"/>
+      <c r="BH128"/>
+      <c r="BI128"/>
+      <c r="BJ128"/>
+      <c r="BK128"/>
+      <c r="BL128"/>
+      <c r="BM128"/>
+      <c r="BN128"/>
+      <c r="BO128"/>
+      <c r="BP128"/>
+      <c r="BQ128"/>
+      <c r="BR128"/>
+      <c r="BS128"/>
+      <c r="BT128"/>
+      <c r="BU128"/>
+      <c r="BV128"/>
+      <c r="BW128"/>
+      <c r="BX128"/>
+      <c r="BY128"/>
+      <c r="BZ128"/>
+      <c r="CA128"/>
+      <c r="CB128"/>
+      <c r="CC128"/>
+      <c r="CD128"/>
+      <c r="CE128"/>
+      <c r="CF128"/>
+      <c r="CG128"/>
+      <c r="CH128"/>
+      <c r="CI128"/>
+      <c r="CJ128"/>
+      <c r="CK128"/>
+      <c r="CL128"/>
+      <c r="CM128"/>
+      <c r="CN128"/>
+      <c r="CO128"/>
+      <c r="CP128"/>
+      <c r="CQ128"/>
+      <c r="CR128"/>
+      <c r="CS128"/>
+      <c r="CT128"/>
+      <c r="CU128"/>
+      <c r="CV128"/>
+      <c r="CW128"/>
+      <c r="CX128"/>
+      <c r="CY128"/>
+      <c r="CZ128"/>
+      <c r="DA128"/>
+      <c r="DB128"/>
+      <c r="DC128"/>
+      <c r="DD128"/>
+      <c r="DE128"/>
+      <c r="DF128"/>
+      <c r="DG128"/>
+      <c r="DH128"/>
+      <c r="DI128"/>
+      <c r="DJ128"/>
+      <c r="DK128"/>
+      <c r="DL128"/>
+      <c r="DM128"/>
+      <c r="DN128"/>
+      <c r="DO128"/>
+      <c r="DP128"/>
+      <c r="DQ128"/>
+      <c r="DR128"/>
+      <c r="DS128"/>
+      <c r="DT128"/>
+      <c r="DU128"/>
+      <c r="DV128"/>
+      <c r="DW128"/>
+      <c r="DX128"/>
+      <c r="DY128"/>
+      <c r="DZ128"/>
+      <c r="EA128"/>
+      <c r="EB128"/>
+      <c r="EC128"/>
+      <c r="ED128"/>
+      <c r="EE128"/>
+      <c r="EF128"/>
+      <c r="EG128"/>
+      <c r="EH128"/>
+      <c r="EI128"/>
+      <c r="EJ128"/>
+      <c r="EK128"/>
+      <c r="EL128"/>
+      <c r="EM128"/>
+      <c r="EN128"/>
+      <c r="EO128"/>
+      <c r="EP128"/>
+      <c r="EQ128"/>
+      <c r="ER128"/>
+      <c r="ES128"/>
+      <c r="ET128"/>
+      <c r="EU128"/>
+      <c r="EV128"/>
+      <c r="EW128"/>
+      <c r="EX128"/>
+      <c r="EY128"/>
+      <c r="EZ128"/>
+      <c r="FA128"/>
+      <c r="FB128"/>
+      <c r="FC128"/>
+      <c r="FD128"/>
+      <c r="FE128"/>
+      <c r="FF128"/>
+      <c r="FG128"/>
+      <c r="FH128"/>
+      <c r="FI128"/>
+      <c r="FJ128"/>
+      <c r="FK128"/>
+      <c r="FL128"/>
+      <c r="FM128"/>
+      <c r="FN128"/>
+      <c r="FO128"/>
+      <c r="FP128"/>
+      <c r="FQ128"/>
+      <c r="FR128"/>
+      <c r="FS128"/>
+      <c r="FT128"/>
+      <c r="FU128"/>
+      <c r="FV128"/>
+      <c r="FW128"/>
+      <c r="FX128"/>
+      <c r="FY128"/>
+      <c r="FZ128"/>
+      <c r="GA128"/>
+      <c r="GB128"/>
+      <c r="GC128"/>
+      <c r="GD128"/>
+      <c r="GE128"/>
+      <c r="GF128"/>
+      <c r="GG128"/>
+      <c r="GH128"/>
+      <c r="GI128"/>
+      <c r="GJ128"/>
+      <c r="GK128"/>
+      <c r="GL128"/>
+      <c r="GM128"/>
+      <c r="GN128"/>
+      <c r="GO128"/>
+      <c r="GP128"/>
+      <c r="GQ128"/>
+      <c r="GR128"/>
+      <c r="GS128"/>
+      <c r="GT128"/>
+      <c r="GU128"/>
+      <c r="GV128"/>
+      <c r="GW128"/>
+      <c r="GX128"/>
+      <c r="GY128"/>
+      <c r="GZ128"/>
+      <c r="HA128"/>
+      <c r="HB128"/>
+      <c r="HC128"/>
+      <c r="HD128"/>
+      <c r="HE128"/>
+      <c r="HF128"/>
+      <c r="HG128"/>
+      <c r="HH128"/>
+      <c r="HI128"/>
+      <c r="HJ128"/>
+      <c r="HK128"/>
+      <c r="HL128"/>
+      <c r="HM128"/>
+      <c r="HN128"/>
+      <c r="HO128"/>
+      <c r="HP128"/>
+      <c r="HQ128"/>
+      <c r="HR128"/>
+      <c r="HS128"/>
+      <c r="HT128"/>
+      <c r="HU128"/>
+      <c r="HV128"/>
+      <c r="HW128"/>
+      <c r="HX128"/>
+      <c r="HY128"/>
+      <c r="HZ128"/>
+      <c r="IA128"/>
+      <c r="IB128"/>
+      <c r="IC128"/>
+      <c r="ID128"/>
+      <c r="IE128"/>
+      <c r="IF128"/>
+      <c r="IG128"/>
+      <c r="IH128"/>
+      <c r="II128"/>
+      <c r="IJ128"/>
+      <c r="IK128"/>
+      <c r="IL128"/>
+      <c r="IM128"/>
+      <c r="IN128"/>
+      <c r="IO128"/>
+      <c r="IP128"/>
+      <c r="IQ128"/>
+      <c r="IR128"/>
+      <c r="IS128"/>
+      <c r="IT128"/>
+      <c r="IU128"/>
+      <c r="IV128"/>
+      <c r="IW128"/>
+    </row>
     <row r="129" ht="17.100000000000001" customHeight="1"/>
     <row r="130" ht="17.100000000000001" customHeight="1"/>
     <row r="131" ht="17.100000000000001" customHeight="1"/>
@@ -19544,6 +20104,8 @@
     <row r="138" ht="17.100000000000001" customHeight="1"/>
     <row r="139" ht="17.100000000000001" customHeight="1"/>
     <row r="140" ht="17.100000000000001" customHeight="1"/>
+    <row r="141" ht="17.100000000000001" customHeight="1"/>
+    <row r="142" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -19561,17 +20123,17 @@
       <selection activeCell="A63" sqref="A63:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="8" width="11.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="28.44140625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="11.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.45" customHeight="1">
+    <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19603,7 +20165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.45" customHeight="1">
+    <row r="2" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -19633,7 +20195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.7" customHeight="1">
+    <row r="3" spans="1:10" ht="13.65" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -19663,7 +20225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.7" customHeight="1">
+    <row r="4" spans="1:10" ht="13.65" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -19693,7 +20255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.7" customHeight="1">
+    <row r="5" spans="1:10" ht="13.65" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -19723,7 +20285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.7" customHeight="1">
+    <row r="6" spans="1:10" ht="13.65" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -19753,7 +20315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.7" customHeight="1">
+    <row r="7" spans="1:10" ht="13.65" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -19783,7 +20345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.7" customHeight="1">
+    <row r="8" spans="1:10" ht="13.65" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -19813,7 +20375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.7" customHeight="1">
+    <row r="9" spans="1:10" ht="13.65" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -19845,7 +20407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.7" customHeight="1">
+    <row r="10" spans="1:10" ht="13.65" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -19877,7 +20439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.7" customHeight="1">
+    <row r="11" spans="1:10" ht="13.65" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -19909,7 +20471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.7" customHeight="1">
+    <row r="12" spans="1:10" ht="13.65" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -19938,7 +20500,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.7" customHeight="1">
+    <row r="13" spans="1:10" ht="13.65" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -19968,7 +20530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.7" customHeight="1">
+    <row r="14" spans="1:10" ht="13.65" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -19995,7 +20557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.7" customHeight="1">
+    <row r="15" spans="1:10" ht="13.65" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -20205,7 +20767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.7" customHeight="1">
+    <row r="22" spans="1:10" ht="13.65" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
@@ -20237,7 +20799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.7" customHeight="1">
+    <row r="23" spans="1:10" ht="13.65" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
worked on hide/show fields setting
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC223F2-5974-492E-B392-E56DE6E59B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F214B31F-A304-4952-85FC-6292827BBD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3108" yWindow="1920" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
     <sheet name="brc" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">default!$B$1:$B$143</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="278">
   <si>
     <t>name</t>
   </si>
@@ -827,13 +830,46 @@
   </si>
   <si>
     <t>Background</t>
+  </si>
+  <si>
+    <t>Complete screening assessment</t>
+  </si>
+  <si>
+    <t>View Screening assessment</t>
+  </si>
+  <si>
+    <t>assessment</t>
+  </si>
+  <si>
+    <t>gov_government_form</t>
+  </si>
+  <si>
+    <t>Government Form</t>
+  </si>
+  <si>
+    <t>National ID Number</t>
+  </si>
+  <si>
+    <t>national_id_number</t>
+  </si>
+  <si>
+    <t>Passport Number</t>
+  </si>
+  <si>
+    <t>passport_number</t>
+  </si>
+  <si>
+    <t>stakeholder_contacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stakeholder contact </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -959,6 +995,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -974,7 +1016,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1205,11 +1247,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1352,6 +1407,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1734,18 +1797,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW142"/>
+  <dimension ref="A1:IW143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K110" sqref="K110"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
@@ -1788,7 +1851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A2" s="66" t="s">
         <v>10</v>
       </c>
@@ -1816,7 +1879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A3" s="68" t="s">
         <v>16</v>
       </c>
@@ -1844,7 +1907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A4" s="68" t="s">
         <v>18</v>
       </c>
@@ -1872,7 +1935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A5" s="68" t="s">
         <v>20</v>
       </c>
@@ -1900,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A6" s="68" t="s">
         <v>22</v>
       </c>
@@ -1928,7 +1991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A7" s="68" t="s">
         <v>18</v>
       </c>
@@ -1956,7 +2019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A8" s="68" t="s">
         <v>24</v>
       </c>
@@ -1984,7 +2047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -2014,7 +2077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -2044,7 +2107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -2074,7 +2137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -2104,7 +2167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A13" s="68" t="s">
         <v>36</v>
       </c>
@@ -2132,7 +2195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A14" s="68" t="s">
         <v>38</v>
       </c>
@@ -2160,7 +2223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A15" s="68" t="s">
         <v>41</v>
       </c>
@@ -2188,7 +2251,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:10" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>43</v>
       </c>
@@ -2218,7 +2281,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>45</v>
       </c>
@@ -2248,7 +2311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>47</v>
       </c>
@@ -2278,7 +2341,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>138</v>
       </c>
@@ -2332,7 +2395,7 @@
       </c>
       <c r="IW19" s="25"/>
     </row>
-    <row r="20" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A20" s="77" t="s">
         <v>136</v>
       </c>
@@ -2607,7 +2670,7 @@
       <c r="IV20"/>
       <c r="IW20"/>
     </row>
-    <row r="21" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A21" s="77" t="s">
         <v>141</v>
       </c>
@@ -2882,7 +2945,7 @@
       <c r="IV21"/>
       <c r="IW21"/>
     </row>
-    <row r="22" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A22" s="82" t="s">
         <v>51</v>
       </c>
@@ -2911,7 +2974,7 @@
       </c>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A23" s="82" t="s">
         <v>53</v>
       </c>
@@ -2939,7 +3002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>55</v>
       </c>
@@ -2969,7 +3032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>57</v>
       </c>
@@ -2999,7 +3062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A26" s="19" t="s">
         <v>60</v>
       </c>
@@ -3029,7 +3092,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>62</v>
       </c>
@@ -3059,7 +3122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>64</v>
       </c>
@@ -3089,7 +3152,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A29" s="19" t="s">
         <v>66</v>
       </c>
@@ -3119,7 +3182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A30" s="19" t="s">
         <v>68</v>
       </c>
@@ -3149,7 +3212,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A31" s="11" t="s">
         <v>70</v>
       </c>
@@ -3179,7 +3242,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A32" s="19" t="s">
         <v>72</v>
       </c>
@@ -3209,7 +3272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A33" s="19" t="s">
         <v>73</v>
       </c>
@@ -3239,7 +3302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:257" s="1" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A34" s="19" t="s">
         <v>74</v>
       </c>
@@ -3269,7 +3332,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A35" s="19" t="s">
         <v>75</v>
       </c>
@@ -3546,7 +3609,7 @@
       <c r="IV35"/>
       <c r="IW35"/>
     </row>
-    <row r="36" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A36" s="19" t="s">
         <v>76</v>
       </c>
@@ -3823,7 +3886,7 @@
       <c r="IV36"/>
       <c r="IW36"/>
     </row>
-    <row r="37" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A37" s="19" t="s">
         <v>77</v>
       </c>
@@ -4100,7 +4163,7 @@
       <c r="IV37"/>
       <c r="IW37"/>
     </row>
-    <row r="38" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A38" s="19" t="s">
         <v>79</v>
       </c>
@@ -4377,7 +4440,7 @@
       <c r="IV38"/>
       <c r="IW38"/>
     </row>
-    <row r="39" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A39" s="19" t="s">
         <v>81</v>
       </c>
@@ -4654,7 +4717,7 @@
       <c r="IV39"/>
       <c r="IW39"/>
     </row>
-    <row r="40" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="40" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A40" s="19" t="s">
         <v>83</v>
       </c>
@@ -4931,7 +4994,7 @@
       <c r="IV40"/>
       <c r="IW40"/>
     </row>
-    <row r="41" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A41" s="19" t="s">
         <v>85</v>
       </c>
@@ -5208,7 +5271,7 @@
       <c r="IV41"/>
       <c r="IW41"/>
     </row>
-    <row r="42" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A42" s="19" t="s">
         <v>87</v>
       </c>
@@ -5485,7 +5548,7 @@
       <c r="IV42"/>
       <c r="IW42"/>
     </row>
-    <row r="43" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="43" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A43" s="19" t="s">
         <v>89</v>
       </c>
@@ -5762,7 +5825,7 @@
       <c r="IV43"/>
       <c r="IW43"/>
     </row>
-    <row r="44" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="44" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A44" s="19" t="s">
         <v>91</v>
       </c>
@@ -6039,7 +6102,7 @@
       <c r="IV44"/>
       <c r="IW44"/>
     </row>
-    <row r="45" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A45" s="19" t="s">
         <v>92</v>
       </c>
@@ -7151,7 +7214,7 @@
         <v>95</v>
       </c>
       <c r="C49" s="86" t="s">
-        <v>135</v>
+        <v>23</v>
       </c>
       <c r="D49" s="75"/>
       <c r="E49" s="87" t="s">
@@ -7426,7 +7489,7 @@
         <v>95</v>
       </c>
       <c r="C50" s="86" t="s">
-        <v>23</v>
+        <v>135</v>
       </c>
       <c r="D50" s="75"/>
       <c r="E50" s="87" t="s">
@@ -9893,7 +9956,7 @@
       <c r="IV58"/>
       <c r="IW58"/>
     </row>
-    <row r="59" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="59" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A59" s="53" t="s">
         <v>111</v>
       </c>
@@ -10168,7 +10231,7 @@
       <c r="IV59"/>
       <c r="IW59"/>
     </row>
-    <row r="60" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="60" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A60" s="53" t="s">
         <v>113</v>
       </c>
@@ -10443,7 +10506,7 @@
       <c r="IV60"/>
       <c r="IW60"/>
     </row>
-    <row r="61" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="61" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A61" s="92" t="s">
         <v>22</v>
       </c>
@@ -10718,7 +10781,7 @@
       <c r="IV61"/>
       <c r="IW61"/>
     </row>
-    <row r="62" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="62" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A62" s="53" t="s">
         <v>115</v>
       </c>
@@ -10993,7 +11056,7 @@
       <c r="IV62"/>
       <c r="IW62"/>
     </row>
-    <row r="63" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="63" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A63" s="53" t="s">
         <v>117</v>
       </c>
@@ -11268,7 +11331,7 @@
       <c r="IV63"/>
       <c r="IW63"/>
     </row>
-    <row r="64" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="64" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A64" s="40" t="s">
         <v>119</v>
       </c>
@@ -11822,7 +11885,7 @@
       <c r="IV65"/>
       <c r="IW65"/>
     </row>
-    <row r="66" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="66" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A66" s="62" t="s">
         <v>143</v>
       </c>
@@ -12099,7 +12162,7 @@
       <c r="IV66" s="64"/>
       <c r="IW66" s="64"/>
     </row>
-    <row r="67" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="67" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A67" s="63" t="s">
         <v>144</v>
       </c>
@@ -12376,7 +12439,7 @@
       <c r="IV67" s="64"/>
       <c r="IW67" s="64"/>
     </row>
-    <row r="68" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="68" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A68" s="62" t="s">
         <v>145</v>
       </c>
@@ -12653,7 +12716,7 @@
       <c r="IV68" s="64"/>
       <c r="IW68" s="64"/>
     </row>
-    <row r="69" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="69" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A69" s="62" t="s">
         <v>146</v>
       </c>
@@ -12930,7 +12993,7 @@
       <c r="IV69" s="64"/>
       <c r="IW69" s="64"/>
     </row>
-    <row r="70" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="70" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A70" s="62" t="s">
         <v>147</v>
       </c>
@@ -13207,7 +13270,7 @@
       <c r="IV70" s="64"/>
       <c r="IW70" s="64"/>
     </row>
-    <row r="71" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="71" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A71" s="62" t="s">
         <v>148</v>
       </c>
@@ -13484,7 +13547,7 @@
       <c r="IV71" s="64"/>
       <c r="IW71" s="64"/>
     </row>
-    <row r="72" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="72" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A72" s="62" t="s">
         <v>149</v>
       </c>
@@ -13761,7 +13824,7 @@
       <c r="IV72" s="64"/>
       <c r="IW72" s="64"/>
     </row>
-    <row r="73" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="73" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A73" s="62" t="s">
         <v>150</v>
       </c>
@@ -14038,7 +14101,7 @@
       <c r="IV73" s="64"/>
       <c r="IW73" s="64"/>
     </row>
-    <row r="74" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="74" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A74" s="62" t="s">
         <v>151</v>
       </c>
@@ -14315,7 +14378,7 @@
       <c r="IV74" s="64"/>
       <c r="IW74" s="64"/>
     </row>
-    <row r="75" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="75" spans="1:257" s="65" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A75" s="62" t="s">
         <v>152</v>
       </c>
@@ -14592,7 +14655,7 @@
       <c r="IV75" s="64"/>
       <c r="IW75" s="64"/>
     </row>
-    <row r="76" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="76" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A76" s="59" t="s">
         <v>153</v>
       </c>
@@ -14869,7 +14932,7 @@
       <c r="IV76" s="60"/>
       <c r="IW76" s="60"/>
     </row>
-    <row r="77" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="77" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A77" s="59" t="s">
         <v>154</v>
       </c>
@@ -15146,7 +15209,7 @@
       <c r="IV77" s="60"/>
       <c r="IW77" s="60"/>
     </row>
-    <row r="78" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="78" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A78" s="59" t="s">
         <v>143</v>
       </c>
@@ -15423,7 +15486,7 @@
       <c r="IV78" s="60"/>
       <c r="IW78" s="60"/>
     </row>
-    <row r="79" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="79" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A79" s="59" t="s">
         <v>157</v>
       </c>
@@ -15700,7 +15763,7 @@
       <c r="IV79" s="60"/>
       <c r="IW79" s="60"/>
     </row>
-    <row r="80" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="80" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A80" s="59" t="s">
         <v>155</v>
       </c>
@@ -15977,7 +16040,7 @@
       <c r="IV80" s="60"/>
       <c r="IW80" s="60"/>
     </row>
-    <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="81" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A81" s="59" t="s">
         <v>246</v>
       </c>
@@ -16254,7 +16317,7 @@
       <c r="IV81" s="60"/>
       <c r="IW81" s="60"/>
     </row>
-    <row r="82" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="82" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A82" s="59" t="s">
         <v>248</v>
       </c>
@@ -16531,7 +16594,7 @@
       <c r="IV82" s="60"/>
       <c r="IW82" s="60"/>
     </row>
-    <row r="83" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="83" spans="1:257" s="61" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A83" s="59" t="s">
         <v>250</v>
       </c>
@@ -16808,7 +16871,7 @@
       <c r="IV83" s="60"/>
       <c r="IW83" s="60"/>
     </row>
-    <row r="84" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="84" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A84" s="58" t="s">
         <v>174</v>
       </c>
@@ -16836,7 +16899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="85" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A85" s="58" t="s">
         <v>176</v>
       </c>
@@ -16864,7 +16927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="86" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A86" s="58" t="s">
         <v>178</v>
       </c>
@@ -16892,7 +16955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="87" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A87" s="58" t="s">
         <v>180</v>
       </c>
@@ -16920,7 +16983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="88" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A88" s="58" t="s">
         <v>182</v>
       </c>
@@ -16948,7 +17011,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="89" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A89" s="58" t="s">
         <v>184</v>
       </c>
@@ -16976,7 +17039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="90" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A90" s="58" t="s">
         <v>186</v>
       </c>
@@ -17004,7 +17067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="91" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A91" s="58" t="s">
         <v>188</v>
       </c>
@@ -17032,7 +17095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="92" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A92" s="58" t="s">
         <v>190</v>
       </c>
@@ -17060,7 +17123,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="93" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A93" s="58" t="s">
         <v>192</v>
       </c>
@@ -17088,7 +17151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="94" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A94" s="58" t="s">
         <v>194</v>
       </c>
@@ -17116,7 +17179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="95" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A95" s="58" t="s">
         <v>196</v>
       </c>
@@ -17144,7 +17207,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="96" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A96" s="58" t="s">
         <v>199</v>
       </c>
@@ -17172,7 +17235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:257" ht="18" customHeight="1">
+    <row r="97" spans="1:257" ht="18" hidden="1" customHeight="1">
       <c r="A97" s="58" t="s">
         <v>200</v>
       </c>
@@ -17200,7 +17263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="98" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A98" s="58" t="s">
         <v>207</v>
       </c>
@@ -17228,7 +17291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="99" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A99" s="58" t="s">
         <v>203</v>
       </c>
@@ -17256,7 +17319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="100" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A100" s="58" t="s">
         <v>205</v>
       </c>
@@ -17284,7 +17347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="101" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A101" s="95" t="s">
         <v>208</v>
       </c>
@@ -17314,7 +17377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="102" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A102" s="95" t="s">
         <v>253</v>
       </c>
@@ -17344,7 +17407,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="103" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A103" s="95" t="s">
         <v>211</v>
       </c>
@@ -17374,7 +17437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="104" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A104" s="95" t="s">
         <v>254</v>
       </c>
@@ -17404,7 +17467,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="105" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A105" s="95" t="s">
         <v>216</v>
       </c>
@@ -17434,7 +17497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="106" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A106" s="95" t="s">
         <v>217</v>
       </c>
@@ -17464,7 +17527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="107" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A107" s="95" t="s">
         <v>218</v>
       </c>
@@ -17494,7 +17557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="108" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A108" s="19" t="s">
         <v>221</v>
       </c>
@@ -17769,7 +17832,7 @@
       <c r="IV108"/>
       <c r="IW108"/>
     </row>
-    <row r="109" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="109" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A109" s="19" t="s">
         <v>263</v>
       </c>
@@ -18044,7 +18107,7 @@
       <c r="IV109"/>
       <c r="IW109"/>
     </row>
-    <row r="110" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="110" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A110" s="19" t="s">
         <v>265</v>
       </c>
@@ -18319,7 +18382,7 @@
       <c r="IV110"/>
       <c r="IW110"/>
     </row>
-    <row r="111" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="111" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A111" s="19" t="s">
         <v>221</v>
       </c>
@@ -18594,7 +18657,7 @@
       <c r="IV111"/>
       <c r="IW111"/>
     </row>
-    <row r="112" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="112" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A112" s="1" t="s">
         <v>222</v>
       </c>
@@ -18624,7 +18687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="113" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>223</v>
       </c>
@@ -18654,7 +18717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="114" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A114" s="1" t="s">
         <v>230</v>
       </c>
@@ -18684,7 +18747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="115" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A115" s="1" t="s">
         <v>252</v>
       </c>
@@ -18714,7 +18777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="116" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A116" s="1" t="s">
         <v>244</v>
       </c>
@@ -18744,7 +18807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="117" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A117" s="1" t="s">
         <v>224</v>
       </c>
@@ -18774,7 +18837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="118" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A118" s="1" t="s">
         <v>238</v>
       </c>
@@ -18804,7 +18867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="119" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A119" s="1" t="s">
         <v>225</v>
       </c>
@@ -18834,7 +18897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="120" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A120" s="1" t="s">
         <v>226</v>
       </c>
@@ -18864,7 +18927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="121" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A121" s="1" t="s">
         <v>240</v>
       </c>
@@ -18894,7 +18957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="122" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A122" s="1" t="s">
         <v>227</v>
       </c>
@@ -18924,7 +18987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="123" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A123" s="1" t="s">
         <v>242</v>
       </c>
@@ -18954,7 +19017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="124" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A124" s="1" t="s">
         <v>152</v>
       </c>
@@ -18984,7 +19047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="125" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A125" t="s">
         <v>228</v>
       </c>
@@ -19261,7 +19324,7 @@
       <c r="IV125"/>
       <c r="IW125"/>
     </row>
-    <row r="126" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="126" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A126" s="99" t="s">
         <v>256</v>
       </c>
@@ -19538,7 +19601,7 @@
       <c r="IV126"/>
       <c r="IW126"/>
     </row>
-    <row r="127" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="127" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A127" s="99" t="s">
         <v>258</v>
       </c>
@@ -19815,7 +19878,7 @@
       <c r="IV127"/>
       <c r="IW127"/>
     </row>
-    <row r="128" spans="1:257" ht="17.100000000000001" customHeight="1">
+    <row r="128" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
       <c r="A128" s="99" t="s">
         <v>261</v>
       </c>
@@ -20092,21 +20155,677 @@
       <c r="IV128"/>
       <c r="IW128"/>
     </row>
-    <row r="129" ht="17.100000000000001" customHeight="1"/>
-    <row r="130" ht="17.100000000000001" customHeight="1"/>
-    <row r="131" ht="17.100000000000001" customHeight="1"/>
-    <row r="132" ht="17.100000000000001" customHeight="1"/>
-    <row r="133" ht="17.100000000000001" customHeight="1"/>
-    <row r="134" ht="17.100000000000001" customHeight="1"/>
-    <row r="135" ht="17.100000000000001" customHeight="1"/>
-    <row r="136" ht="17.100000000000001" customHeight="1"/>
-    <row r="137" ht="17.100000000000001" customHeight="1"/>
-    <row r="138" ht="17.100000000000001" customHeight="1"/>
-    <row r="139" ht="17.100000000000001" customHeight="1"/>
-    <row r="140" ht="17.100000000000001" customHeight="1"/>
-    <row r="141" ht="17.100000000000001" customHeight="1"/>
-    <row r="142" ht="17.100000000000001" customHeight="1"/>
+    <row r="129" spans="1:257" s="99" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" thickBot="1">
+      <c r="A129" s="103" t="s">
+        <v>136</v>
+      </c>
+      <c r="B129" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="C129" s="103" t="s">
+        <v>267</v>
+      </c>
+      <c r="D129" s="100"/>
+      <c r="E129" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="F129" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G129" s="104">
+        <v>0</v>
+      </c>
+      <c r="H129" s="102">
+        <v>1</v>
+      </c>
+      <c r="I129" s="100"/>
+      <c r="J129" s="100" t="s">
+        <v>29</v>
+      </c>
+      <c r="K129" s="100"/>
+      <c r="L129" s="100"/>
+      <c r="M129" s="100"/>
+      <c r="N129" s="100"/>
+      <c r="O129" s="100"/>
+      <c r="P129" s="100"/>
+      <c r="Q129" s="100"/>
+      <c r="R129" s="100"/>
+      <c r="S129" s="100"/>
+      <c r="T129" s="100"/>
+      <c r="U129" s="100"/>
+      <c r="V129" s="100"/>
+      <c r="W129" s="100"/>
+      <c r="X129" s="100"/>
+      <c r="Y129" s="100"/>
+      <c r="Z129" s="100"/>
+      <c r="AA129" s="100"/>
+      <c r="AB129" s="100"/>
+      <c r="AC129" s="100"/>
+      <c r="AD129" s="100"/>
+      <c r="AE129" s="100"/>
+      <c r="AF129" s="100"/>
+      <c r="AG129" s="100"/>
+      <c r="AH129" s="100"/>
+      <c r="AI129" s="100"/>
+      <c r="AJ129" s="100"/>
+      <c r="AK129" s="100"/>
+      <c r="AL129" s="100"/>
+      <c r="AM129" s="100"/>
+      <c r="AN129" s="100"/>
+      <c r="AO129" s="100"/>
+      <c r="AP129" s="100"/>
+      <c r="AQ129" s="100"/>
+      <c r="AR129" s="100"/>
+      <c r="AS129" s="100"/>
+      <c r="AT129" s="100"/>
+      <c r="AU129" s="100"/>
+      <c r="AV129" s="100"/>
+      <c r="AW129" s="100"/>
+      <c r="AX129" s="100"/>
+      <c r="AY129" s="100"/>
+      <c r="AZ129" s="100"/>
+      <c r="BA129" s="100"/>
+      <c r="BB129" s="100"/>
+      <c r="BC129" s="100"/>
+      <c r="BD129" s="100"/>
+      <c r="BE129" s="100"/>
+      <c r="BF129" s="100"/>
+      <c r="BG129" s="100"/>
+      <c r="BH129" s="100"/>
+      <c r="BI129" s="100"/>
+      <c r="BJ129" s="100"/>
+      <c r="BK129" s="100"/>
+      <c r="BL129" s="100"/>
+      <c r="BM129" s="100"/>
+      <c r="BN129" s="100"/>
+      <c r="BO129" s="100"/>
+      <c r="BP129" s="100"/>
+      <c r="BQ129" s="100"/>
+      <c r="BR129" s="100"/>
+      <c r="BS129" s="100"/>
+      <c r="BT129" s="100"/>
+      <c r="BU129" s="100"/>
+      <c r="BV129" s="100"/>
+      <c r="BW129" s="100"/>
+      <c r="BX129" s="100"/>
+      <c r="BY129" s="100"/>
+      <c r="BZ129" s="100"/>
+      <c r="CA129" s="100"/>
+      <c r="CB129" s="100"/>
+      <c r="CC129" s="100"/>
+      <c r="CD129" s="100"/>
+      <c r="CE129" s="100"/>
+      <c r="CF129" s="100"/>
+      <c r="CG129" s="100"/>
+      <c r="CH129" s="100"/>
+      <c r="CI129" s="100"/>
+      <c r="CJ129" s="100"/>
+      <c r="CK129" s="100"/>
+      <c r="CL129" s="100"/>
+      <c r="CM129" s="100"/>
+      <c r="CN129" s="100"/>
+      <c r="CO129" s="100"/>
+      <c r="CP129" s="100"/>
+      <c r="CQ129" s="100"/>
+      <c r="CR129" s="100"/>
+      <c r="CS129" s="100"/>
+      <c r="CT129" s="100"/>
+      <c r="CU129" s="100"/>
+      <c r="CV129" s="100"/>
+      <c r="CW129" s="100"/>
+      <c r="CX129" s="100"/>
+      <c r="CY129" s="100"/>
+      <c r="CZ129" s="100"/>
+      <c r="DA129" s="100"/>
+      <c r="DB129" s="100"/>
+      <c r="DC129" s="100"/>
+      <c r="DD129" s="100"/>
+      <c r="DE129" s="100"/>
+      <c r="DF129" s="100"/>
+      <c r="DG129" s="100"/>
+      <c r="DH129" s="100"/>
+      <c r="DI129" s="100"/>
+      <c r="DJ129" s="100"/>
+      <c r="DK129" s="100"/>
+      <c r="DL129" s="100"/>
+      <c r="DM129" s="100"/>
+      <c r="DN129" s="100"/>
+      <c r="DO129" s="100"/>
+      <c r="DP129" s="100"/>
+      <c r="DQ129" s="100"/>
+      <c r="DR129" s="100"/>
+      <c r="DS129" s="100"/>
+      <c r="DT129" s="100"/>
+      <c r="DU129" s="100"/>
+      <c r="DV129" s="100"/>
+      <c r="DW129" s="100"/>
+      <c r="DX129" s="100"/>
+      <c r="DY129" s="100"/>
+      <c r="DZ129" s="100"/>
+      <c r="EA129" s="100"/>
+      <c r="EB129" s="100"/>
+      <c r="EC129" s="100"/>
+      <c r="ED129" s="100"/>
+      <c r="EE129" s="100"/>
+      <c r="EF129" s="100"/>
+      <c r="EG129" s="100"/>
+      <c r="EH129" s="100"/>
+      <c r="EI129" s="100"/>
+      <c r="EJ129" s="100"/>
+      <c r="EK129" s="100"/>
+      <c r="EL129" s="100"/>
+      <c r="EM129" s="100"/>
+      <c r="EN129" s="100"/>
+      <c r="EO129" s="100"/>
+      <c r="EP129" s="100"/>
+      <c r="EQ129" s="100"/>
+      <c r="ER129" s="100"/>
+      <c r="ES129" s="100"/>
+      <c r="ET129" s="100"/>
+      <c r="EU129" s="100"/>
+      <c r="EV129" s="100"/>
+      <c r="EW129" s="100"/>
+      <c r="EX129" s="100"/>
+      <c r="EY129" s="100"/>
+      <c r="EZ129" s="100"/>
+      <c r="FA129" s="100"/>
+      <c r="FB129" s="100"/>
+      <c r="FC129" s="100"/>
+      <c r="FD129" s="100"/>
+      <c r="FE129" s="100"/>
+      <c r="FF129" s="100"/>
+      <c r="FG129" s="100"/>
+      <c r="FH129" s="100"/>
+      <c r="FI129" s="100"/>
+      <c r="FJ129" s="100"/>
+      <c r="FK129" s="100"/>
+      <c r="FL129" s="100"/>
+      <c r="FM129" s="100"/>
+      <c r="FN129" s="100"/>
+      <c r="FO129" s="100"/>
+      <c r="FP129" s="100"/>
+      <c r="FQ129" s="100"/>
+      <c r="FR129" s="100"/>
+      <c r="FS129" s="100"/>
+      <c r="FT129" s="100"/>
+      <c r="FU129" s="100"/>
+      <c r="FV129" s="100"/>
+      <c r="FW129" s="100"/>
+      <c r="FX129" s="100"/>
+      <c r="FY129" s="100"/>
+      <c r="FZ129" s="100"/>
+      <c r="GA129" s="100"/>
+      <c r="GB129" s="100"/>
+      <c r="GC129" s="100"/>
+      <c r="GD129" s="100"/>
+      <c r="GE129" s="100"/>
+      <c r="GF129" s="100"/>
+      <c r="GG129" s="100"/>
+      <c r="GH129" s="100"/>
+      <c r="GI129" s="100"/>
+      <c r="GJ129" s="100"/>
+      <c r="GK129" s="100"/>
+      <c r="GL129" s="100"/>
+      <c r="GM129" s="100"/>
+      <c r="GN129" s="100"/>
+      <c r="GO129" s="100"/>
+      <c r="GP129" s="100"/>
+      <c r="GQ129" s="100"/>
+      <c r="GR129" s="100"/>
+      <c r="GS129" s="100"/>
+      <c r="GT129" s="100"/>
+      <c r="GU129" s="100"/>
+      <c r="GV129" s="100"/>
+      <c r="GW129" s="100"/>
+      <c r="GX129" s="100"/>
+      <c r="GY129" s="100"/>
+      <c r="GZ129" s="100"/>
+      <c r="HA129" s="100"/>
+      <c r="HB129" s="100"/>
+      <c r="HC129" s="100"/>
+      <c r="HD129" s="100"/>
+      <c r="HE129" s="100"/>
+      <c r="HF129" s="100"/>
+      <c r="HG129" s="100"/>
+      <c r="HH129" s="100"/>
+      <c r="HI129" s="100"/>
+      <c r="HJ129" s="100"/>
+      <c r="HK129" s="100"/>
+      <c r="HL129" s="100"/>
+      <c r="HM129" s="100"/>
+      <c r="HN129" s="100"/>
+      <c r="HO129" s="100"/>
+      <c r="HP129" s="100"/>
+      <c r="HQ129" s="100"/>
+      <c r="HR129" s="100"/>
+      <c r="HS129" s="100"/>
+      <c r="HT129" s="100"/>
+      <c r="HU129" s="100"/>
+      <c r="HV129" s="100"/>
+      <c r="HW129" s="100"/>
+      <c r="HX129" s="100"/>
+      <c r="HY129" s="100"/>
+      <c r="HZ129" s="100"/>
+      <c r="IA129" s="100"/>
+      <c r="IB129" s="100"/>
+      <c r="IC129" s="100"/>
+      <c r="ID129" s="100"/>
+      <c r="IE129" s="100"/>
+      <c r="IF129" s="100"/>
+      <c r="IG129" s="100"/>
+      <c r="IH129" s="100"/>
+      <c r="II129" s="100"/>
+      <c r="IJ129" s="100"/>
+      <c r="IK129" s="100"/>
+      <c r="IL129" s="100"/>
+      <c r="IM129" s="100"/>
+      <c r="IN129" s="100"/>
+      <c r="IO129" s="100"/>
+      <c r="IP129" s="100"/>
+      <c r="IQ129" s="100"/>
+      <c r="IR129" s="100"/>
+      <c r="IS129" s="100"/>
+      <c r="IT129" s="100"/>
+      <c r="IU129" s="100"/>
+      <c r="IV129" s="100"/>
+      <c r="IW129" s="100"/>
+    </row>
+    <row r="130" spans="1:257" s="99" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" thickBot="1">
+      <c r="A130" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="C130" s="103" t="s">
+        <v>268</v>
+      </c>
+      <c r="D130" s="100"/>
+      <c r="E130" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="F130" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G130" s="104">
+        <v>0</v>
+      </c>
+      <c r="H130" s="102">
+        <v>1</v>
+      </c>
+      <c r="I130" s="100"/>
+      <c r="J130" s="100" t="s">
+        <v>29</v>
+      </c>
+      <c r="K130" s="100"/>
+      <c r="L130" s="100"/>
+      <c r="M130" s="100"/>
+      <c r="N130" s="100"/>
+      <c r="O130" s="100"/>
+      <c r="P130" s="100"/>
+      <c r="Q130" s="100"/>
+      <c r="R130" s="100"/>
+      <c r="S130" s="100"/>
+      <c r="T130" s="100"/>
+      <c r="U130" s="100"/>
+      <c r="V130" s="100"/>
+      <c r="W130" s="100"/>
+      <c r="X130" s="100"/>
+      <c r="Y130" s="100"/>
+      <c r="Z130" s="100"/>
+      <c r="AA130" s="100"/>
+      <c r="AB130" s="100"/>
+      <c r="AC130" s="100"/>
+      <c r="AD130" s="100"/>
+      <c r="AE130" s="100"/>
+      <c r="AF130" s="100"/>
+      <c r="AG130" s="100"/>
+      <c r="AH130" s="100"/>
+      <c r="AI130" s="100"/>
+      <c r="AJ130" s="100"/>
+      <c r="AK130" s="100"/>
+      <c r="AL130" s="100"/>
+      <c r="AM130" s="100"/>
+      <c r="AN130" s="100"/>
+      <c r="AO130" s="100"/>
+      <c r="AP130" s="100"/>
+      <c r="AQ130" s="100"/>
+      <c r="AR130" s="100"/>
+      <c r="AS130" s="100"/>
+      <c r="AT130" s="100"/>
+      <c r="AU130" s="100"/>
+      <c r="AV130" s="100"/>
+      <c r="AW130" s="100"/>
+      <c r="AX130" s="100"/>
+      <c r="AY130" s="100"/>
+      <c r="AZ130" s="100"/>
+      <c r="BA130" s="100"/>
+      <c r="BB130" s="100"/>
+      <c r="BC130" s="100"/>
+      <c r="BD130" s="100"/>
+      <c r="BE130" s="100"/>
+      <c r="BF130" s="100"/>
+      <c r="BG130" s="100"/>
+      <c r="BH130" s="100"/>
+      <c r="BI130" s="100"/>
+      <c r="BJ130" s="100"/>
+      <c r="BK130" s="100"/>
+      <c r="BL130" s="100"/>
+      <c r="BM130" s="100"/>
+      <c r="BN130" s="100"/>
+      <c r="BO130" s="100"/>
+      <c r="BP130" s="100"/>
+      <c r="BQ130" s="100"/>
+      <c r="BR130" s="100"/>
+      <c r="BS130" s="100"/>
+      <c r="BT130" s="100"/>
+      <c r="BU130" s="100"/>
+      <c r="BV130" s="100"/>
+      <c r="BW130" s="100"/>
+      <c r="BX130" s="100"/>
+      <c r="BY130" s="100"/>
+      <c r="BZ130" s="100"/>
+      <c r="CA130" s="100"/>
+      <c r="CB130" s="100"/>
+      <c r="CC130" s="100"/>
+      <c r="CD130" s="100"/>
+      <c r="CE130" s="100"/>
+      <c r="CF130" s="100"/>
+      <c r="CG130" s="100"/>
+      <c r="CH130" s="100"/>
+      <c r="CI130" s="100"/>
+      <c r="CJ130" s="100"/>
+      <c r="CK130" s="100"/>
+      <c r="CL130" s="100"/>
+      <c r="CM130" s="100"/>
+      <c r="CN130" s="100"/>
+      <c r="CO130" s="100"/>
+      <c r="CP130" s="100"/>
+      <c r="CQ130" s="100"/>
+      <c r="CR130" s="100"/>
+      <c r="CS130" s="100"/>
+      <c r="CT130" s="100"/>
+      <c r="CU130" s="100"/>
+      <c r="CV130" s="100"/>
+      <c r="CW130" s="100"/>
+      <c r="CX130" s="100"/>
+      <c r="CY130" s="100"/>
+      <c r="CZ130" s="100"/>
+      <c r="DA130" s="100"/>
+      <c r="DB130" s="100"/>
+      <c r="DC130" s="100"/>
+      <c r="DD130" s="100"/>
+      <c r="DE130" s="100"/>
+      <c r="DF130" s="100"/>
+      <c r="DG130" s="100"/>
+      <c r="DH130" s="100"/>
+      <c r="DI130" s="100"/>
+      <c r="DJ130" s="100"/>
+      <c r="DK130" s="100"/>
+      <c r="DL130" s="100"/>
+      <c r="DM130" s="100"/>
+      <c r="DN130" s="100"/>
+      <c r="DO130" s="100"/>
+      <c r="DP130" s="100"/>
+      <c r="DQ130" s="100"/>
+      <c r="DR130" s="100"/>
+      <c r="DS130" s="100"/>
+      <c r="DT130" s="100"/>
+      <c r="DU130" s="100"/>
+      <c r="DV130" s="100"/>
+      <c r="DW130" s="100"/>
+      <c r="DX130" s="100"/>
+      <c r="DY130" s="100"/>
+      <c r="DZ130" s="100"/>
+      <c r="EA130" s="100"/>
+      <c r="EB130" s="100"/>
+      <c r="EC130" s="100"/>
+      <c r="ED130" s="100"/>
+      <c r="EE130" s="100"/>
+      <c r="EF130" s="100"/>
+      <c r="EG130" s="100"/>
+      <c r="EH130" s="100"/>
+      <c r="EI130" s="100"/>
+      <c r="EJ130" s="100"/>
+      <c r="EK130" s="100"/>
+      <c r="EL130" s="100"/>
+      <c r="EM130" s="100"/>
+      <c r="EN130" s="100"/>
+      <c r="EO130" s="100"/>
+      <c r="EP130" s="100"/>
+      <c r="EQ130" s="100"/>
+      <c r="ER130" s="100"/>
+      <c r="ES130" s="100"/>
+      <c r="ET130" s="100"/>
+      <c r="EU130" s="100"/>
+      <c r="EV130" s="100"/>
+      <c r="EW130" s="100"/>
+      <c r="EX130" s="100"/>
+      <c r="EY130" s="100"/>
+      <c r="EZ130" s="100"/>
+      <c r="FA130" s="100"/>
+      <c r="FB130" s="100"/>
+      <c r="FC130" s="100"/>
+      <c r="FD130" s="100"/>
+      <c r="FE130" s="100"/>
+      <c r="FF130" s="100"/>
+      <c r="FG130" s="100"/>
+      <c r="FH130" s="100"/>
+      <c r="FI130" s="100"/>
+      <c r="FJ130" s="100"/>
+      <c r="FK130" s="100"/>
+      <c r="FL130" s="100"/>
+      <c r="FM130" s="100"/>
+      <c r="FN130" s="100"/>
+      <c r="FO130" s="100"/>
+      <c r="FP130" s="100"/>
+      <c r="FQ130" s="100"/>
+      <c r="FR130" s="100"/>
+      <c r="FS130" s="100"/>
+      <c r="FT130" s="100"/>
+      <c r="FU130" s="100"/>
+      <c r="FV130" s="100"/>
+      <c r="FW130" s="100"/>
+      <c r="FX130" s="100"/>
+      <c r="FY130" s="100"/>
+      <c r="FZ130" s="100"/>
+      <c r="GA130" s="100"/>
+      <c r="GB130" s="100"/>
+      <c r="GC130" s="100"/>
+      <c r="GD130" s="100"/>
+      <c r="GE130" s="100"/>
+      <c r="GF130" s="100"/>
+      <c r="GG130" s="100"/>
+      <c r="GH130" s="100"/>
+      <c r="GI130" s="100"/>
+      <c r="GJ130" s="100"/>
+      <c r="GK130" s="100"/>
+      <c r="GL130" s="100"/>
+      <c r="GM130" s="100"/>
+      <c r="GN130" s="100"/>
+      <c r="GO130" s="100"/>
+      <c r="GP130" s="100"/>
+      <c r="GQ130" s="100"/>
+      <c r="GR130" s="100"/>
+      <c r="GS130" s="100"/>
+      <c r="GT130" s="100"/>
+      <c r="GU130" s="100"/>
+      <c r="GV130" s="100"/>
+      <c r="GW130" s="100"/>
+      <c r="GX130" s="100"/>
+      <c r="GY130" s="100"/>
+      <c r="GZ130" s="100"/>
+      <c r="HA130" s="100"/>
+      <c r="HB130" s="100"/>
+      <c r="HC130" s="100"/>
+      <c r="HD130" s="100"/>
+      <c r="HE130" s="100"/>
+      <c r="HF130" s="100"/>
+      <c r="HG130" s="100"/>
+      <c r="HH130" s="100"/>
+      <c r="HI130" s="100"/>
+      <c r="HJ130" s="100"/>
+      <c r="HK130" s="100"/>
+      <c r="HL130" s="100"/>
+      <c r="HM130" s="100"/>
+      <c r="HN130" s="100"/>
+      <c r="HO130" s="100"/>
+      <c r="HP130" s="100"/>
+      <c r="HQ130" s="100"/>
+      <c r="HR130" s="100"/>
+      <c r="HS130" s="100"/>
+      <c r="HT130" s="100"/>
+      <c r="HU130" s="100"/>
+      <c r="HV130" s="100"/>
+      <c r="HW130" s="100"/>
+      <c r="HX130" s="100"/>
+      <c r="HY130" s="100"/>
+      <c r="HZ130" s="100"/>
+      <c r="IA130" s="100"/>
+      <c r="IB130" s="100"/>
+      <c r="IC130" s="100"/>
+      <c r="ID130" s="100"/>
+      <c r="IE130" s="100"/>
+      <c r="IF130" s="100"/>
+      <c r="IG130" s="100"/>
+      <c r="IH130" s="100"/>
+      <c r="II130" s="100"/>
+      <c r="IJ130" s="100"/>
+      <c r="IK130" s="100"/>
+      <c r="IL130" s="100"/>
+      <c r="IM130" s="100"/>
+      <c r="IN130" s="100"/>
+      <c r="IO130" s="100"/>
+      <c r="IP130" s="100"/>
+      <c r="IQ130" s="100"/>
+      <c r="IR130" s="100"/>
+      <c r="IS130" s="100"/>
+      <c r="IT130" s="100"/>
+      <c r="IU130" s="100"/>
+      <c r="IV130" s="100"/>
+      <c r="IW130" s="100"/>
+    </row>
+    <row r="131" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
+      <c r="A131" s="100" t="s">
+        <v>270</v>
+      </c>
+      <c r="B131" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="E131" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G131" s="32">
+        <v>0</v>
+      </c>
+      <c r="H131" s="101">
+        <v>1</v>
+      </c>
+      <c r="J131" s="100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="132" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
+      <c r="A132" s="100" t="s">
+        <v>273</v>
+      </c>
+      <c r="B132" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="E132" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G132" s="104">
+        <v>0</v>
+      </c>
+      <c r="H132" s="102">
+        <v>1</v>
+      </c>
+      <c r="J132" s="100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="133" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
+      <c r="A133" s="100" t="s">
+        <v>275</v>
+      </c>
+      <c r="B133" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133" s="100" t="s">
+        <v>274</v>
+      </c>
+      <c r="E133" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G133" s="104">
+        <v>0</v>
+      </c>
+      <c r="H133" s="102">
+        <v>1</v>
+      </c>
+      <c r="J133" s="100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="134" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1">
+      <c r="A134" s="100" t="s">
+        <v>276</v>
+      </c>
+      <c r="B134" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C134" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="E134" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G134" s="104">
+        <v>0</v>
+      </c>
+      <c r="H134" s="102">
+        <v>1</v>
+      </c>
+      <c r="J134" s="100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="136" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="137" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="138" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="139" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="140" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="141" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="142" spans="1:257" ht="17.100000000000001" hidden="1" customHeight="1"/>
+    <row r="143" spans="1:257" hidden="1"/>
   </sheetData>
+  <autoFilter ref="B1:B143" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="family"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added Issue to be Addressed to Case conference
- Add new table called case_conference_addressed_issues
- Write spec for case_conference_addressed_issues and update case
  conference domain
- Fixed N+1 in Case Conference form and show page
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Home/Documents/oscar-web/db/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A04C3-7F51-0148-AE6A-5BFA1D650B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B093566-E024-4AD7-B7FA-A852223C03CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="440" windowWidth="29380" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="1365" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -564,12 +564,21 @@
   <si>
     <t>service_delivery</t>
   </si>
+  <si>
+    <t>issue_to_be_addressed</t>
+  </si>
+  <si>
+    <t>Issue to be address</t>
+  </si>
+  <si>
+    <t>ratanak</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -997,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1112,6 +1121,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1498,26 +1510,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW94"/>
+  <dimension ref="A1:IW95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.83203125" style="1"/>
+    <col min="6" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1549,7 +1561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17.45" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1576,7 +1588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="13.7" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1603,7 +1615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13.7" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1630,7 +1642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="13.7" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1657,7 +1669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="13.7" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1685,7 +1697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.7" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -1712,7 +1724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="13.7" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1740,7 +1752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="13.7" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -1770,7 +1782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="13.7" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -1799,7 +1811,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="13.7" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="13.7" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -1857,7 +1869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="13.7" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1884,7 +1896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="13.7" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -1911,7 +1923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="13.7" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1938,7 +1950,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -1967,7 +1979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:257" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:257" ht="15" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>47</v>
       </c>
@@ -2026,7 +2038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:257" ht="15" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>138</v>
       </c>
@@ -2079,7 +2091,7 @@
       </c>
       <c r="IW19" s="25"/>
     </row>
-    <row r="20" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:257" ht="15" customHeight="1">
       <c r="A20" s="62" t="s">
         <v>136</v>
       </c>
@@ -2354,7 +2366,7 @@
       <c r="IV20"/>
       <c r="IW20"/>
     </row>
-    <row r="21" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:257" ht="15" customHeight="1">
       <c r="A21" s="62" t="s">
         <v>141</v>
       </c>
@@ -2629,7 +2641,7 @@
       <c r="IV21"/>
       <c r="IW21"/>
     </row>
-    <row r="22" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:257" ht="15" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>51</v>
       </c>
@@ -2657,7 +2669,7 @@
       </c>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:257" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:257" ht="13.7" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>53</v>
       </c>
@@ -2684,7 +2696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:257" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:257" ht="13.7" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
@@ -2713,7 +2725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:257" ht="12.75" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>57</v>
       </c>
@@ -2742,7 +2754,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:257" ht="12.75" customHeight="1">
       <c r="A26" s="29" t="s">
         <v>60</v>
       </c>
@@ -2771,7 +2783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:257" ht="12.75" customHeight="1">
       <c r="A27" s="29" t="s">
         <v>62</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:257" ht="12.75" customHeight="1">
       <c r="A28" s="29" t="s">
         <v>64</v>
       </c>
@@ -2829,7 +2841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:257" ht="12.75" customHeight="1">
       <c r="A29" s="29" t="s">
         <v>66</v>
       </c>
@@ -2858,7 +2870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:257" ht="12.75" customHeight="1">
       <c r="A30" s="29" t="s">
         <v>68</v>
       </c>
@@ -2887,7 +2899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:257" ht="12.75" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>70</v>
       </c>
@@ -2916,7 +2928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:257" ht="12.75" customHeight="1">
       <c r="A32" s="29" t="s">
         <v>72</v>
       </c>
@@ -2945,7 +2957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:257" ht="12.75" customHeight="1">
       <c r="A33" s="29" t="s">
         <v>73</v>
       </c>
@@ -2974,7 +2986,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" s="1" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:257" s="1" customFormat="1" hidden="1">
       <c r="A34" s="29" t="s">
         <v>74</v>
       </c>
@@ -3003,7 +3015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:257" ht="12.75" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>75</v>
       </c>
@@ -3279,7 +3291,7 @@
       <c r="IV35"/>
       <c r="IW35"/>
     </row>
-    <row r="36" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:257" ht="12.75" customHeight="1">
       <c r="A36" s="29" t="s">
         <v>76</v>
       </c>
@@ -3555,7 +3567,7 @@
       <c r="IV36"/>
       <c r="IW36"/>
     </row>
-    <row r="37" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:257" ht="12.75" customHeight="1">
       <c r="A37" s="29" t="s">
         <v>77</v>
       </c>
@@ -3831,7 +3843,7 @@
       <c r="IV37"/>
       <c r="IW37"/>
     </row>
-    <row r="38" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:257" ht="12.75" customHeight="1">
       <c r="A38" s="29" t="s">
         <v>79</v>
       </c>
@@ -4107,7 +4119,7 @@
       <c r="IV38"/>
       <c r="IW38"/>
     </row>
-    <row r="39" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:257" ht="12.75" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>81</v>
       </c>
@@ -4383,7 +4395,7 @@
       <c r="IV39"/>
       <c r="IW39"/>
     </row>
-    <row r="40" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:257" ht="12.75" customHeight="1">
       <c r="A40" s="29" t="s">
         <v>83</v>
       </c>
@@ -4659,7 +4671,7 @@
       <c r="IV40"/>
       <c r="IW40"/>
     </row>
-    <row r="41" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:257" ht="12.75" customHeight="1">
       <c r="A41" s="29" t="s">
         <v>85</v>
       </c>
@@ -4935,7 +4947,7 @@
       <c r="IV41"/>
       <c r="IW41"/>
     </row>
-    <row r="42" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:257" ht="12.75" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>87</v>
       </c>
@@ -5211,7 +5223,7 @@
       <c r="IV42"/>
       <c r="IW42"/>
     </row>
-    <row r="43" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:257" ht="12.75" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>89</v>
       </c>
@@ -5487,7 +5499,7 @@
       <c r="IV43"/>
       <c r="IW43"/>
     </row>
-    <row r="44" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:257" ht="12.75" customHeight="1">
       <c r="A44" s="29" t="s">
         <v>91</v>
       </c>
@@ -5763,7 +5775,7 @@
       <c r="IV44"/>
       <c r="IW44"/>
     </row>
-    <row r="45" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:257" ht="12.75" customHeight="1">
       <c r="A45" s="29" t="s">
         <v>92</v>
       </c>
@@ -6039,7 +6051,7 @@
       <c r="IV45"/>
       <c r="IW45"/>
     </row>
-    <row r="46" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:257" ht="12.75" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>94</v>
       </c>
@@ -6314,7 +6326,7 @@
       <c r="IV46"/>
       <c r="IW46"/>
     </row>
-    <row r="47" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:257" ht="12.75" customHeight="1">
       <c r="A47" s="41" t="s">
         <v>97</v>
       </c>
@@ -6591,7 +6603,7 @@
       <c r="IV47"/>
       <c r="IW47"/>
     </row>
-    <row r="48" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:257" ht="12.75" customHeight="1">
       <c r="A48" s="46" t="s">
         <v>77</v>
       </c>
@@ -6866,7 +6878,7 @@
       <c r="IV48"/>
       <c r="IW48"/>
     </row>
-    <row r="49" spans="1:257" ht="11" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:257" ht="11.1" customHeight="1">
       <c r="A49" s="46" t="s">
         <v>22</v>
       </c>
@@ -7141,7 +7153,7 @@
       <c r="IV49"/>
       <c r="IW49"/>
     </row>
-    <row r="50" spans="1:257" ht="11" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:257" ht="11.1" customHeight="1">
       <c r="A50" s="46" t="s">
         <v>0</v>
       </c>
@@ -7416,7 +7428,7 @@
       <c r="IV50"/>
       <c r="IW50"/>
     </row>
-    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:257" ht="12.75" customHeight="1">
       <c r="A51" s="46" t="s">
         <v>79</v>
       </c>
@@ -7691,7 +7703,7 @@
       <c r="IV51"/>
       <c r="IW51"/>
     </row>
-    <row r="52" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:257" ht="12.75" customHeight="1">
       <c r="A52" s="46" t="s">
         <v>81</v>
       </c>
@@ -7966,7 +7978,7 @@
       <c r="IV52"/>
       <c r="IW52"/>
     </row>
-    <row r="53" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:257" ht="12.75" customHeight="1">
       <c r="A53" s="46" t="s">
         <v>83</v>
       </c>
@@ -8241,7 +8253,7 @@
       <c r="IV53"/>
       <c r="IW53"/>
     </row>
-    <row r="54" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:257" ht="12.75" customHeight="1">
       <c r="A54" s="46" t="s">
         <v>101</v>
       </c>
@@ -8516,7 +8528,7 @@
       <c r="IV54"/>
       <c r="IW54"/>
     </row>
-    <row r="55" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:257" ht="12.75" customHeight="1">
       <c r="A55" s="46" t="s">
         <v>102</v>
       </c>
@@ -8791,7 +8803,7 @@
       <c r="IV55"/>
       <c r="IW55"/>
     </row>
-    <row r="56" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:257" ht="12.75" customHeight="1">
       <c r="A56" s="46" t="s">
         <v>104</v>
       </c>
@@ -9066,7 +9078,7 @@
       <c r="IV56"/>
       <c r="IW56"/>
     </row>
-    <row r="57" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:257" ht="12.75" customHeight="1">
       <c r="A57" s="46" t="s">
         <v>106</v>
       </c>
@@ -9341,7 +9353,7 @@
       <c r="IV57"/>
       <c r="IW57"/>
     </row>
-    <row r="58" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:257" ht="12.75" customHeight="1">
       <c r="A58" s="46" t="s">
         <v>108</v>
       </c>
@@ -9616,7 +9628,7 @@
       <c r="IV58"/>
       <c r="IW58"/>
     </row>
-    <row r="59" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:257" ht="12.75" customHeight="1">
       <c r="A59" s="35" t="s">
         <v>111</v>
       </c>
@@ -9890,7 +9902,7 @@
       <c r="IV59"/>
       <c r="IW59"/>
     </row>
-    <row r="60" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:257" ht="12.75" customHeight="1">
       <c r="A60" s="35" t="s">
         <v>113</v>
       </c>
@@ -10164,7 +10176,7 @@
       <c r="IV60"/>
       <c r="IW60"/>
     </row>
-    <row r="61" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:257" ht="12.75" customHeight="1">
       <c r="A61" s="61" t="s">
         <v>22</v>
       </c>
@@ -10438,7 +10450,7 @@
       <c r="IV61"/>
       <c r="IW61"/>
     </row>
-    <row r="62" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:257" ht="12.75" customHeight="1">
       <c r="A62" s="35" t="s">
         <v>115</v>
       </c>
@@ -10712,7 +10724,7 @@
       <c r="IV62"/>
       <c r="IW62"/>
     </row>
-    <row r="63" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:257" ht="12.75" customHeight="1">
       <c r="A63" s="35" t="s">
         <v>117</v>
       </c>
@@ -10986,7 +10998,7 @@
       <c r="IV63"/>
       <c r="IW63"/>
     </row>
-    <row r="64" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:257" ht="12.75" customHeight="1">
       <c r="A64" s="37" t="s">
         <v>119</v>
       </c>
@@ -11262,7 +11274,7 @@
       <c r="IV64"/>
       <c r="IW64"/>
     </row>
-    <row r="65" spans="1:257" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:257">
       <c r="A65" s="68" t="s">
         <v>120</v>
       </c>
@@ -11538,7 +11550,7 @@
       <c r="IV65"/>
       <c r="IW65"/>
     </row>
-    <row r="66" spans="1:257" s="80" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:257" s="80" customFormat="1" ht="9" customHeight="1">
       <c r="A66" s="77" t="s">
         <v>143</v>
       </c>
@@ -11815,7 +11827,7 @@
       <c r="IV66" s="79"/>
       <c r="IW66" s="79"/>
     </row>
-    <row r="67" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:257" s="80" customFormat="1">
       <c r="A67" s="79" t="s">
         <v>145</v>
       </c>
@@ -12092,7 +12104,7 @@
       <c r="IV67" s="79"/>
       <c r="IW67" s="79"/>
     </row>
-    <row r="68" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:257" s="80" customFormat="1">
       <c r="A68" s="77" t="s">
         <v>146</v>
       </c>
@@ -12369,7 +12381,7 @@
       <c r="IV68" s="79"/>
       <c r="IW68" s="79"/>
     </row>
-    <row r="69" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:257" s="80" customFormat="1">
       <c r="A69" s="77" t="s">
         <v>147</v>
       </c>
@@ -12646,7 +12658,7 @@
       <c r="IV69" s="79"/>
       <c r="IW69" s="79"/>
     </row>
-    <row r="70" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:257" s="80" customFormat="1">
       <c r="A70" s="77" t="s">
         <v>148</v>
       </c>
@@ -12923,7 +12935,7 @@
       <c r="IV70" s="79"/>
       <c r="IW70" s="79"/>
     </row>
-    <row r="71" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:257" s="80" customFormat="1">
       <c r="A71" s="77" t="s">
         <v>149</v>
       </c>
@@ -13200,7 +13212,7 @@
       <c r="IV71" s="79"/>
       <c r="IW71" s="79"/>
     </row>
-    <row r="72" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:257" s="80" customFormat="1">
       <c r="A72" s="77" t="s">
         <v>150</v>
       </c>
@@ -13477,7 +13489,7 @@
       <c r="IV72" s="79"/>
       <c r="IW72" s="79"/>
     </row>
-    <row r="73" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:257" s="80" customFormat="1">
       <c r="A73" s="77" t="s">
         <v>151</v>
       </c>
@@ -13754,7 +13766,7 @@
       <c r="IV73" s="79"/>
       <c r="IW73" s="79"/>
     </row>
-    <row r="74" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:257" s="80" customFormat="1">
       <c r="A74" s="77" t="s">
         <v>152</v>
       </c>
@@ -14031,34 +14043,34 @@
       <c r="IV74" s="79"/>
       <c r="IW74" s="79"/>
     </row>
-    <row r="75" spans="1:257" s="80" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:257" s="80" customFormat="1">
       <c r="A75" s="77" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="B75" s="78" t="s">
         <v>177</v>
       </c>
       <c r="C75" s="78" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="D75" s="78"/>
       <c r="E75" s="78" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="F75" s="78" t="s">
-        <v>156</v>
-      </c>
-      <c r="G75" s="78">
+        <v>13</v>
+      </c>
+      <c r="G75" s="81">
         <v>0</v>
       </c>
-      <c r="H75" s="78">
+      <c r="H75" s="81">
         <v>1</v>
       </c>
       <c r="I75" s="78" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="J75" s="78" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="K75" s="79"/>
       <c r="L75" s="79"/>
@@ -14308,294 +14320,292 @@
       <c r="IV75" s="79"/>
       <c r="IW75" s="79"/>
     </row>
-    <row r="76" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="74" t="s">
+    <row r="76" spans="1:257" s="80" customFormat="1">
+      <c r="A76" s="77" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C76" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="D76" s="78"/>
+      <c r="E76" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="F76" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="78">
+        <v>0</v>
+      </c>
+      <c r="H76" s="78">
+        <v>1</v>
+      </c>
+      <c r="I76" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="J76" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="K76" s="79"/>
+      <c r="L76" s="79"/>
+      <c r="M76" s="79"/>
+      <c r="N76" s="79"/>
+      <c r="O76" s="79"/>
+      <c r="P76" s="79"/>
+      <c r="Q76" s="79"/>
+      <c r="R76" s="79"/>
+      <c r="S76" s="79"/>
+      <c r="T76" s="79"/>
+      <c r="U76" s="79"/>
+      <c r="V76" s="79"/>
+      <c r="W76" s="79"/>
+      <c r="X76" s="79"/>
+      <c r="Y76" s="79"/>
+      <c r="Z76" s="79"/>
+      <c r="AA76" s="79"/>
+      <c r="AB76" s="79"/>
+      <c r="AC76" s="79"/>
+      <c r="AD76" s="79"/>
+      <c r="AE76" s="79"/>
+      <c r="AF76" s="79"/>
+      <c r="AG76" s="79"/>
+      <c r="AH76" s="79"/>
+      <c r="AI76" s="79"/>
+      <c r="AJ76" s="79"/>
+      <c r="AK76" s="79"/>
+      <c r="AL76" s="79"/>
+      <c r="AM76" s="79"/>
+      <c r="AN76" s="79"/>
+      <c r="AO76" s="79"/>
+      <c r="AP76" s="79"/>
+      <c r="AQ76" s="79"/>
+      <c r="AR76" s="79"/>
+      <c r="AS76" s="79"/>
+      <c r="AT76" s="79"/>
+      <c r="AU76" s="79"/>
+      <c r="AV76" s="79"/>
+      <c r="AW76" s="79"/>
+      <c r="AX76" s="79"/>
+      <c r="AY76" s="79"/>
+      <c r="AZ76" s="79"/>
+      <c r="BA76" s="79"/>
+      <c r="BB76" s="79"/>
+      <c r="BC76" s="79"/>
+      <c r="BD76" s="79"/>
+      <c r="BE76" s="79"/>
+      <c r="BF76" s="79"/>
+      <c r="BG76" s="79"/>
+      <c r="BH76" s="79"/>
+      <c r="BI76" s="79"/>
+      <c r="BJ76" s="79"/>
+      <c r="BK76" s="79"/>
+      <c r="BL76" s="79"/>
+      <c r="BM76" s="79"/>
+      <c r="BN76" s="79"/>
+      <c r="BO76" s="79"/>
+      <c r="BP76" s="79"/>
+      <c r="BQ76" s="79"/>
+      <c r="BR76" s="79"/>
+      <c r="BS76" s="79"/>
+      <c r="BT76" s="79"/>
+      <c r="BU76" s="79"/>
+      <c r="BV76" s="79"/>
+      <c r="BW76" s="79"/>
+      <c r="BX76" s="79"/>
+      <c r="BY76" s="79"/>
+      <c r="BZ76" s="79"/>
+      <c r="CA76" s="79"/>
+      <c r="CB76" s="79"/>
+      <c r="CC76" s="79"/>
+      <c r="CD76" s="79"/>
+      <c r="CE76" s="79"/>
+      <c r="CF76" s="79"/>
+      <c r="CG76" s="79"/>
+      <c r="CH76" s="79"/>
+      <c r="CI76" s="79"/>
+      <c r="CJ76" s="79"/>
+      <c r="CK76" s="79"/>
+      <c r="CL76" s="79"/>
+      <c r="CM76" s="79"/>
+      <c r="CN76" s="79"/>
+      <c r="CO76" s="79"/>
+      <c r="CP76" s="79"/>
+      <c r="CQ76" s="79"/>
+      <c r="CR76" s="79"/>
+      <c r="CS76" s="79"/>
+      <c r="CT76" s="79"/>
+      <c r="CU76" s="79"/>
+      <c r="CV76" s="79"/>
+      <c r="CW76" s="79"/>
+      <c r="CX76" s="79"/>
+      <c r="CY76" s="79"/>
+      <c r="CZ76" s="79"/>
+      <c r="DA76" s="79"/>
+      <c r="DB76" s="79"/>
+      <c r="DC76" s="79"/>
+      <c r="DD76" s="79"/>
+      <c r="DE76" s="79"/>
+      <c r="DF76" s="79"/>
+      <c r="DG76" s="79"/>
+      <c r="DH76" s="79"/>
+      <c r="DI76" s="79"/>
+      <c r="DJ76" s="79"/>
+      <c r="DK76" s="79"/>
+      <c r="DL76" s="79"/>
+      <c r="DM76" s="79"/>
+      <c r="DN76" s="79"/>
+      <c r="DO76" s="79"/>
+      <c r="DP76" s="79"/>
+      <c r="DQ76" s="79"/>
+      <c r="DR76" s="79"/>
+      <c r="DS76" s="79"/>
+      <c r="DT76" s="79"/>
+      <c r="DU76" s="79"/>
+      <c r="DV76" s="79"/>
+      <c r="DW76" s="79"/>
+      <c r="DX76" s="79"/>
+      <c r="DY76" s="79"/>
+      <c r="DZ76" s="79"/>
+      <c r="EA76" s="79"/>
+      <c r="EB76" s="79"/>
+      <c r="EC76" s="79"/>
+      <c r="ED76" s="79"/>
+      <c r="EE76" s="79"/>
+      <c r="EF76" s="79"/>
+      <c r="EG76" s="79"/>
+      <c r="EH76" s="79"/>
+      <c r="EI76" s="79"/>
+      <c r="EJ76" s="79"/>
+      <c r="EK76" s="79"/>
+      <c r="EL76" s="79"/>
+      <c r="EM76" s="79"/>
+      <c r="EN76" s="79"/>
+      <c r="EO76" s="79"/>
+      <c r="EP76" s="79"/>
+      <c r="EQ76" s="79"/>
+      <c r="ER76" s="79"/>
+      <c r="ES76" s="79"/>
+      <c r="ET76" s="79"/>
+      <c r="EU76" s="79"/>
+      <c r="EV76" s="79"/>
+      <c r="EW76" s="79"/>
+      <c r="EX76" s="79"/>
+      <c r="EY76" s="79"/>
+      <c r="EZ76" s="79"/>
+      <c r="FA76" s="79"/>
+      <c r="FB76" s="79"/>
+      <c r="FC76" s="79"/>
+      <c r="FD76" s="79"/>
+      <c r="FE76" s="79"/>
+      <c r="FF76" s="79"/>
+      <c r="FG76" s="79"/>
+      <c r="FH76" s="79"/>
+      <c r="FI76" s="79"/>
+      <c r="FJ76" s="79"/>
+      <c r="FK76" s="79"/>
+      <c r="FL76" s="79"/>
+      <c r="FM76" s="79"/>
+      <c r="FN76" s="79"/>
+      <c r="FO76" s="79"/>
+      <c r="FP76" s="79"/>
+      <c r="FQ76" s="79"/>
+      <c r="FR76" s="79"/>
+      <c r="FS76" s="79"/>
+      <c r="FT76" s="79"/>
+      <c r="FU76" s="79"/>
+      <c r="FV76" s="79"/>
+      <c r="FW76" s="79"/>
+      <c r="FX76" s="79"/>
+      <c r="FY76" s="79"/>
+      <c r="FZ76" s="79"/>
+      <c r="GA76" s="79"/>
+      <c r="GB76" s="79"/>
+      <c r="GC76" s="79"/>
+      <c r="GD76" s="79"/>
+      <c r="GE76" s="79"/>
+      <c r="GF76" s="79"/>
+      <c r="GG76" s="79"/>
+      <c r="GH76" s="79"/>
+      <c r="GI76" s="79"/>
+      <c r="GJ76" s="79"/>
+      <c r="GK76" s="79"/>
+      <c r="GL76" s="79"/>
+      <c r="GM76" s="79"/>
+      <c r="GN76" s="79"/>
+      <c r="GO76" s="79"/>
+      <c r="GP76" s="79"/>
+      <c r="GQ76" s="79"/>
+      <c r="GR76" s="79"/>
+      <c r="GS76" s="79"/>
+      <c r="GT76" s="79"/>
+      <c r="GU76" s="79"/>
+      <c r="GV76" s="79"/>
+      <c r="GW76" s="79"/>
+      <c r="GX76" s="79"/>
+      <c r="GY76" s="79"/>
+      <c r="GZ76" s="79"/>
+      <c r="HA76" s="79"/>
+      <c r="HB76" s="79"/>
+      <c r="HC76" s="79"/>
+      <c r="HD76" s="79"/>
+      <c r="HE76" s="79"/>
+      <c r="HF76" s="79"/>
+      <c r="HG76" s="79"/>
+      <c r="HH76" s="79"/>
+      <c r="HI76" s="79"/>
+      <c r="HJ76" s="79"/>
+      <c r="HK76" s="79"/>
+      <c r="HL76" s="79"/>
+      <c r="HM76" s="79"/>
+      <c r="HN76" s="79"/>
+      <c r="HO76" s="79"/>
+      <c r="HP76" s="79"/>
+      <c r="HQ76" s="79"/>
+      <c r="HR76" s="79"/>
+      <c r="HS76" s="79"/>
+      <c r="HT76" s="79"/>
+      <c r="HU76" s="79"/>
+      <c r="HV76" s="79"/>
+      <c r="HW76" s="79"/>
+      <c r="HX76" s="79"/>
+      <c r="HY76" s="79"/>
+      <c r="HZ76" s="79"/>
+      <c r="IA76" s="79"/>
+      <c r="IB76" s="79"/>
+      <c r="IC76" s="79"/>
+      <c r="ID76" s="79"/>
+      <c r="IE76" s="79"/>
+      <c r="IF76" s="79"/>
+      <c r="IG76" s="79"/>
+      <c r="IH76" s="79"/>
+      <c r="II76" s="79"/>
+      <c r="IJ76" s="79"/>
+      <c r="IK76" s="79"/>
+      <c r="IL76" s="79"/>
+      <c r="IM76" s="79"/>
+      <c r="IN76" s="79"/>
+      <c r="IO76" s="79"/>
+      <c r="IP76" s="79"/>
+      <c r="IQ76" s="79"/>
+      <c r="IR76" s="79"/>
+      <c r="IS76" s="79"/>
+      <c r="IT76" s="79"/>
+      <c r="IU76" s="79"/>
+      <c r="IV76" s="79"/>
+      <c r="IW76" s="79"/>
+    </row>
+    <row r="77" spans="1:257" s="76" customFormat="1">
+      <c r="A77" s="74" t="s">
         <v>167</v>
-      </c>
-      <c r="B76" s="74" t="s">
-        <v>178</v>
-      </c>
-      <c r="C76" s="74" t="s">
-        <v>168</v>
-      </c>
-      <c r="D76" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="E76" s="74" t="s">
-        <v>170</v>
-      </c>
-      <c r="F76" s="74" t="s">
-        <v>156</v>
-      </c>
-      <c r="G76" s="74">
-        <v>0</v>
-      </c>
-      <c r="H76" s="74">
-        <v>1</v>
-      </c>
-      <c r="I76" s="74" t="s">
-        <v>144</v>
-      </c>
-      <c r="J76" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="K76" s="75"/>
-      <c r="L76" s="75"/>
-      <c r="M76" s="75"/>
-      <c r="N76" s="75"/>
-      <c r="O76" s="75"/>
-      <c r="P76" s="75"/>
-      <c r="Q76" s="75"/>
-      <c r="R76" s="75"/>
-      <c r="S76" s="75"/>
-      <c r="T76" s="75"/>
-      <c r="U76" s="75"/>
-      <c r="V76" s="75"/>
-      <c r="W76" s="75"/>
-      <c r="X76" s="75"/>
-      <c r="Y76" s="75"/>
-      <c r="Z76" s="75"/>
-      <c r="AA76" s="75"/>
-      <c r="AB76" s="75"/>
-      <c r="AC76" s="75"/>
-      <c r="AD76" s="75"/>
-      <c r="AE76" s="75"/>
-      <c r="AF76" s="75"/>
-      <c r="AG76" s="75"/>
-      <c r="AH76" s="75"/>
-      <c r="AI76" s="75"/>
-      <c r="AJ76" s="75"/>
-      <c r="AK76" s="75"/>
-      <c r="AL76" s="75"/>
-      <c r="AM76" s="75"/>
-      <c r="AN76" s="75"/>
-      <c r="AO76" s="75"/>
-      <c r="AP76" s="75"/>
-      <c r="AQ76" s="75"/>
-      <c r="AR76" s="75"/>
-      <c r="AS76" s="75"/>
-      <c r="AT76" s="75"/>
-      <c r="AU76" s="75"/>
-      <c r="AV76" s="75"/>
-      <c r="AW76" s="75"/>
-      <c r="AX76" s="75"/>
-      <c r="AY76" s="75"/>
-      <c r="AZ76" s="75"/>
-      <c r="BA76" s="75"/>
-      <c r="BB76" s="75"/>
-      <c r="BC76" s="75"/>
-      <c r="BD76" s="75"/>
-      <c r="BE76" s="75"/>
-      <c r="BF76" s="75"/>
-      <c r="BG76" s="75"/>
-      <c r="BH76" s="75"/>
-      <c r="BI76" s="75"/>
-      <c r="BJ76" s="75"/>
-      <c r="BK76" s="75"/>
-      <c r="BL76" s="75"/>
-      <c r="BM76" s="75"/>
-      <c r="BN76" s="75"/>
-      <c r="BO76" s="75"/>
-      <c r="BP76" s="75"/>
-      <c r="BQ76" s="75"/>
-      <c r="BR76" s="75"/>
-      <c r="BS76" s="75"/>
-      <c r="BT76" s="75"/>
-      <c r="BU76" s="75"/>
-      <c r="BV76" s="75"/>
-      <c r="BW76" s="75"/>
-      <c r="BX76" s="75"/>
-      <c r="BY76" s="75"/>
-      <c r="BZ76" s="75"/>
-      <c r="CA76" s="75"/>
-      <c r="CB76" s="75"/>
-      <c r="CC76" s="75"/>
-      <c r="CD76" s="75"/>
-      <c r="CE76" s="75"/>
-      <c r="CF76" s="75"/>
-      <c r="CG76" s="75"/>
-      <c r="CH76" s="75"/>
-      <c r="CI76" s="75"/>
-      <c r="CJ76" s="75"/>
-      <c r="CK76" s="75"/>
-      <c r="CL76" s="75"/>
-      <c r="CM76" s="75"/>
-      <c r="CN76" s="75"/>
-      <c r="CO76" s="75"/>
-      <c r="CP76" s="75"/>
-      <c r="CQ76" s="75"/>
-      <c r="CR76" s="75"/>
-      <c r="CS76" s="75"/>
-      <c r="CT76" s="75"/>
-      <c r="CU76" s="75"/>
-      <c r="CV76" s="75"/>
-      <c r="CW76" s="75"/>
-      <c r="CX76" s="75"/>
-      <c r="CY76" s="75"/>
-      <c r="CZ76" s="75"/>
-      <c r="DA76" s="75"/>
-      <c r="DB76" s="75"/>
-      <c r="DC76" s="75"/>
-      <c r="DD76" s="75"/>
-      <c r="DE76" s="75"/>
-      <c r="DF76" s="75"/>
-      <c r="DG76" s="75"/>
-      <c r="DH76" s="75"/>
-      <c r="DI76" s="75"/>
-      <c r="DJ76" s="75"/>
-      <c r="DK76" s="75"/>
-      <c r="DL76" s="75"/>
-      <c r="DM76" s="75"/>
-      <c r="DN76" s="75"/>
-      <c r="DO76" s="75"/>
-      <c r="DP76" s="75"/>
-      <c r="DQ76" s="75"/>
-      <c r="DR76" s="75"/>
-      <c r="DS76" s="75"/>
-      <c r="DT76" s="75"/>
-      <c r="DU76" s="75"/>
-      <c r="DV76" s="75"/>
-      <c r="DW76" s="75"/>
-      <c r="DX76" s="75"/>
-      <c r="DY76" s="75"/>
-      <c r="DZ76" s="75"/>
-      <c r="EA76" s="75"/>
-      <c r="EB76" s="75"/>
-      <c r="EC76" s="75"/>
-      <c r="ED76" s="75"/>
-      <c r="EE76" s="75"/>
-      <c r="EF76" s="75"/>
-      <c r="EG76" s="75"/>
-      <c r="EH76" s="75"/>
-      <c r="EI76" s="75"/>
-      <c r="EJ76" s="75"/>
-      <c r="EK76" s="75"/>
-      <c r="EL76" s="75"/>
-      <c r="EM76" s="75"/>
-      <c r="EN76" s="75"/>
-      <c r="EO76" s="75"/>
-      <c r="EP76" s="75"/>
-      <c r="EQ76" s="75"/>
-      <c r="ER76" s="75"/>
-      <c r="ES76" s="75"/>
-      <c r="ET76" s="75"/>
-      <c r="EU76" s="75"/>
-      <c r="EV76" s="75"/>
-      <c r="EW76" s="75"/>
-      <c r="EX76" s="75"/>
-      <c r="EY76" s="75"/>
-      <c r="EZ76" s="75"/>
-      <c r="FA76" s="75"/>
-      <c r="FB76" s="75"/>
-      <c r="FC76" s="75"/>
-      <c r="FD76" s="75"/>
-      <c r="FE76" s="75"/>
-      <c r="FF76" s="75"/>
-      <c r="FG76" s="75"/>
-      <c r="FH76" s="75"/>
-      <c r="FI76" s="75"/>
-      <c r="FJ76" s="75"/>
-      <c r="FK76" s="75"/>
-      <c r="FL76" s="75"/>
-      <c r="FM76" s="75"/>
-      <c r="FN76" s="75"/>
-      <c r="FO76" s="75"/>
-      <c r="FP76" s="75"/>
-      <c r="FQ76" s="75"/>
-      <c r="FR76" s="75"/>
-      <c r="FS76" s="75"/>
-      <c r="FT76" s="75"/>
-      <c r="FU76" s="75"/>
-      <c r="FV76" s="75"/>
-      <c r="FW76" s="75"/>
-      <c r="FX76" s="75"/>
-      <c r="FY76" s="75"/>
-      <c r="FZ76" s="75"/>
-      <c r="GA76" s="75"/>
-      <c r="GB76" s="75"/>
-      <c r="GC76" s="75"/>
-      <c r="GD76" s="75"/>
-      <c r="GE76" s="75"/>
-      <c r="GF76" s="75"/>
-      <c r="GG76" s="75"/>
-      <c r="GH76" s="75"/>
-      <c r="GI76" s="75"/>
-      <c r="GJ76" s="75"/>
-      <c r="GK76" s="75"/>
-      <c r="GL76" s="75"/>
-      <c r="GM76" s="75"/>
-      <c r="GN76" s="75"/>
-      <c r="GO76" s="75"/>
-      <c r="GP76" s="75"/>
-      <c r="GQ76" s="75"/>
-      <c r="GR76" s="75"/>
-      <c r="GS76" s="75"/>
-      <c r="GT76" s="75"/>
-      <c r="GU76" s="75"/>
-      <c r="GV76" s="75"/>
-      <c r="GW76" s="75"/>
-      <c r="GX76" s="75"/>
-      <c r="GY76" s="75"/>
-      <c r="GZ76" s="75"/>
-      <c r="HA76" s="75"/>
-      <c r="HB76" s="75"/>
-      <c r="HC76" s="75"/>
-      <c r="HD76" s="75"/>
-      <c r="HE76" s="75"/>
-      <c r="HF76" s="75"/>
-      <c r="HG76" s="75"/>
-      <c r="HH76" s="75"/>
-      <c r="HI76" s="75"/>
-      <c r="HJ76" s="75"/>
-      <c r="HK76" s="75"/>
-      <c r="HL76" s="75"/>
-      <c r="HM76" s="75"/>
-      <c r="HN76" s="75"/>
-      <c r="HO76" s="75"/>
-      <c r="HP76" s="75"/>
-      <c r="HQ76" s="75"/>
-      <c r="HR76" s="75"/>
-      <c r="HS76" s="75"/>
-      <c r="HT76" s="75"/>
-      <c r="HU76" s="75"/>
-      <c r="HV76" s="75"/>
-      <c r="HW76" s="75"/>
-      <c r="HX76" s="75"/>
-      <c r="HY76" s="75"/>
-      <c r="HZ76" s="75"/>
-      <c r="IA76" s="75"/>
-      <c r="IB76" s="75"/>
-      <c r="IC76" s="75"/>
-      <c r="ID76" s="75"/>
-      <c r="IE76" s="75"/>
-      <c r="IF76" s="75"/>
-      <c r="IG76" s="75"/>
-      <c r="IH76" s="75"/>
-      <c r="II76" s="75"/>
-      <c r="IJ76" s="75"/>
-      <c r="IK76" s="75"/>
-      <c r="IL76" s="75"/>
-      <c r="IM76" s="75"/>
-      <c r="IN76" s="75"/>
-      <c r="IO76" s="75"/>
-      <c r="IP76" s="75"/>
-      <c r="IQ76" s="75"/>
-      <c r="IR76" s="75"/>
-      <c r="IS76" s="75"/>
-      <c r="IT76" s="75"/>
-      <c r="IU76" s="75"/>
-      <c r="IV76" s="75"/>
-      <c r="IW76" s="75"/>
-    </row>
-    <row r="77" spans="1:257" s="76" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="74" t="s">
-        <v>171</v>
       </c>
       <c r="B77" s="74" t="s">
         <v>178</v>
       </c>
       <c r="C77" s="74" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D77" s="74" t="s">
         <v>169</v>
@@ -14866,15 +14876,15 @@
       <c r="IV77" s="75"/>
       <c r="IW77" s="75"/>
     </row>
-    <row r="78" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:257" s="76" customFormat="1" ht="14.1" customHeight="1">
       <c r="A78" s="74" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="B78" s="74" t="s">
         <v>178</v>
       </c>
       <c r="C78" s="74" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="D78" s="74" t="s">
         <v>169</v>
@@ -15145,15 +15155,15 @@
       <c r="IV78" s="75"/>
       <c r="IW78" s="75"/>
     </row>
-    <row r="79" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:257" s="76" customFormat="1">
       <c r="A79" s="74" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="B79" s="74" t="s">
         <v>178</v>
       </c>
       <c r="C79" s="74" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D79" s="74" t="s">
         <v>169</v>
@@ -15424,15 +15434,15 @@
       <c r="IV79" s="75"/>
       <c r="IW79" s="75"/>
     </row>
-    <row r="80" spans="1:257" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:257" s="76" customFormat="1">
       <c r="A80" s="74" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B80" s="74" t="s">
         <v>178</v>
       </c>
       <c r="C80" s="74" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D80" s="74" t="s">
         <v>169</v>
@@ -15703,19 +15713,286 @@
       <c r="IV80" s="75"/>
       <c r="IW80" s="75"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A81" s="73"/>
-      <c r="B81" s="73"/>
-      <c r="C81" s="73"/>
-      <c r="D81" s="73"/>
-      <c r="E81" s="73"/>
-      <c r="F81" s="73"/>
-      <c r="G81" s="73"/>
-      <c r="H81" s="73"/>
-      <c r="I81" s="73"/>
-      <c r="J81" s="73"/>
+    <row r="81" spans="1:257" s="76" customFormat="1">
+      <c r="A81" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="B81" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C81" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="D81" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="G81" s="74">
+        <v>0</v>
+      </c>
+      <c r="H81" s="74">
+        <v>1</v>
+      </c>
+      <c r="I81" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="J81" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="K81" s="75"/>
+      <c r="L81" s="75"/>
+      <c r="M81" s="75"/>
+      <c r="N81" s="75"/>
+      <c r="O81" s="75"/>
+      <c r="P81" s="75"/>
+      <c r="Q81" s="75"/>
+      <c r="R81" s="75"/>
+      <c r="S81" s="75"/>
+      <c r="T81" s="75"/>
+      <c r="U81" s="75"/>
+      <c r="V81" s="75"/>
+      <c r="W81" s="75"/>
+      <c r="X81" s="75"/>
+      <c r="Y81" s="75"/>
+      <c r="Z81" s="75"/>
+      <c r="AA81" s="75"/>
+      <c r="AB81" s="75"/>
+      <c r="AC81" s="75"/>
+      <c r="AD81" s="75"/>
+      <c r="AE81" s="75"/>
+      <c r="AF81" s="75"/>
+      <c r="AG81" s="75"/>
+      <c r="AH81" s="75"/>
+      <c r="AI81" s="75"/>
+      <c r="AJ81" s="75"/>
+      <c r="AK81" s="75"/>
+      <c r="AL81" s="75"/>
+      <c r="AM81" s="75"/>
+      <c r="AN81" s="75"/>
+      <c r="AO81" s="75"/>
+      <c r="AP81" s="75"/>
+      <c r="AQ81" s="75"/>
+      <c r="AR81" s="75"/>
+      <c r="AS81" s="75"/>
+      <c r="AT81" s="75"/>
+      <c r="AU81" s="75"/>
+      <c r="AV81" s="75"/>
+      <c r="AW81" s="75"/>
+      <c r="AX81" s="75"/>
+      <c r="AY81" s="75"/>
+      <c r="AZ81" s="75"/>
+      <c r="BA81" s="75"/>
+      <c r="BB81" s="75"/>
+      <c r="BC81" s="75"/>
+      <c r="BD81" s="75"/>
+      <c r="BE81" s="75"/>
+      <c r="BF81" s="75"/>
+      <c r="BG81" s="75"/>
+      <c r="BH81" s="75"/>
+      <c r="BI81" s="75"/>
+      <c r="BJ81" s="75"/>
+      <c r="BK81" s="75"/>
+      <c r="BL81" s="75"/>
+      <c r="BM81" s="75"/>
+      <c r="BN81" s="75"/>
+      <c r="BO81" s="75"/>
+      <c r="BP81" s="75"/>
+      <c r="BQ81" s="75"/>
+      <c r="BR81" s="75"/>
+      <c r="BS81" s="75"/>
+      <c r="BT81" s="75"/>
+      <c r="BU81" s="75"/>
+      <c r="BV81" s="75"/>
+      <c r="BW81" s="75"/>
+      <c r="BX81" s="75"/>
+      <c r="BY81" s="75"/>
+      <c r="BZ81" s="75"/>
+      <c r="CA81" s="75"/>
+      <c r="CB81" s="75"/>
+      <c r="CC81" s="75"/>
+      <c r="CD81" s="75"/>
+      <c r="CE81" s="75"/>
+      <c r="CF81" s="75"/>
+      <c r="CG81" s="75"/>
+      <c r="CH81" s="75"/>
+      <c r="CI81" s="75"/>
+      <c r="CJ81" s="75"/>
+      <c r="CK81" s="75"/>
+      <c r="CL81" s="75"/>
+      <c r="CM81" s="75"/>
+      <c r="CN81" s="75"/>
+      <c r="CO81" s="75"/>
+      <c r="CP81" s="75"/>
+      <c r="CQ81" s="75"/>
+      <c r="CR81" s="75"/>
+      <c r="CS81" s="75"/>
+      <c r="CT81" s="75"/>
+      <c r="CU81" s="75"/>
+      <c r="CV81" s="75"/>
+      <c r="CW81" s="75"/>
+      <c r="CX81" s="75"/>
+      <c r="CY81" s="75"/>
+      <c r="CZ81" s="75"/>
+      <c r="DA81" s="75"/>
+      <c r="DB81" s="75"/>
+      <c r="DC81" s="75"/>
+      <c r="DD81" s="75"/>
+      <c r="DE81" s="75"/>
+      <c r="DF81" s="75"/>
+      <c r="DG81" s="75"/>
+      <c r="DH81" s="75"/>
+      <c r="DI81" s="75"/>
+      <c r="DJ81" s="75"/>
+      <c r="DK81" s="75"/>
+      <c r="DL81" s="75"/>
+      <c r="DM81" s="75"/>
+      <c r="DN81" s="75"/>
+      <c r="DO81" s="75"/>
+      <c r="DP81" s="75"/>
+      <c r="DQ81" s="75"/>
+      <c r="DR81" s="75"/>
+      <c r="DS81" s="75"/>
+      <c r="DT81" s="75"/>
+      <c r="DU81" s="75"/>
+      <c r="DV81" s="75"/>
+      <c r="DW81" s="75"/>
+      <c r="DX81" s="75"/>
+      <c r="DY81" s="75"/>
+      <c r="DZ81" s="75"/>
+      <c r="EA81" s="75"/>
+      <c r="EB81" s="75"/>
+      <c r="EC81" s="75"/>
+      <c r="ED81" s="75"/>
+      <c r="EE81" s="75"/>
+      <c r="EF81" s="75"/>
+      <c r="EG81" s="75"/>
+      <c r="EH81" s="75"/>
+      <c r="EI81" s="75"/>
+      <c r="EJ81" s="75"/>
+      <c r="EK81" s="75"/>
+      <c r="EL81" s="75"/>
+      <c r="EM81" s="75"/>
+      <c r="EN81" s="75"/>
+      <c r="EO81" s="75"/>
+      <c r="EP81" s="75"/>
+      <c r="EQ81" s="75"/>
+      <c r="ER81" s="75"/>
+      <c r="ES81" s="75"/>
+      <c r="ET81" s="75"/>
+      <c r="EU81" s="75"/>
+      <c r="EV81" s="75"/>
+      <c r="EW81" s="75"/>
+      <c r="EX81" s="75"/>
+      <c r="EY81" s="75"/>
+      <c r="EZ81" s="75"/>
+      <c r="FA81" s="75"/>
+      <c r="FB81" s="75"/>
+      <c r="FC81" s="75"/>
+      <c r="FD81" s="75"/>
+      <c r="FE81" s="75"/>
+      <c r="FF81" s="75"/>
+      <c r="FG81" s="75"/>
+      <c r="FH81" s="75"/>
+      <c r="FI81" s="75"/>
+      <c r="FJ81" s="75"/>
+      <c r="FK81" s="75"/>
+      <c r="FL81" s="75"/>
+      <c r="FM81" s="75"/>
+      <c r="FN81" s="75"/>
+      <c r="FO81" s="75"/>
+      <c r="FP81" s="75"/>
+      <c r="FQ81" s="75"/>
+      <c r="FR81" s="75"/>
+      <c r="FS81" s="75"/>
+      <c r="FT81" s="75"/>
+      <c r="FU81" s="75"/>
+      <c r="FV81" s="75"/>
+      <c r="FW81" s="75"/>
+      <c r="FX81" s="75"/>
+      <c r="FY81" s="75"/>
+      <c r="FZ81" s="75"/>
+      <c r="GA81" s="75"/>
+      <c r="GB81" s="75"/>
+      <c r="GC81" s="75"/>
+      <c r="GD81" s="75"/>
+      <c r="GE81" s="75"/>
+      <c r="GF81" s="75"/>
+      <c r="GG81" s="75"/>
+      <c r="GH81" s="75"/>
+      <c r="GI81" s="75"/>
+      <c r="GJ81" s="75"/>
+      <c r="GK81" s="75"/>
+      <c r="GL81" s="75"/>
+      <c r="GM81" s="75"/>
+      <c r="GN81" s="75"/>
+      <c r="GO81" s="75"/>
+      <c r="GP81" s="75"/>
+      <c r="GQ81" s="75"/>
+      <c r="GR81" s="75"/>
+      <c r="GS81" s="75"/>
+      <c r="GT81" s="75"/>
+      <c r="GU81" s="75"/>
+      <c r="GV81" s="75"/>
+      <c r="GW81" s="75"/>
+      <c r="GX81" s="75"/>
+      <c r="GY81" s="75"/>
+      <c r="GZ81" s="75"/>
+      <c r="HA81" s="75"/>
+      <c r="HB81" s="75"/>
+      <c r="HC81" s="75"/>
+      <c r="HD81" s="75"/>
+      <c r="HE81" s="75"/>
+      <c r="HF81" s="75"/>
+      <c r="HG81" s="75"/>
+      <c r="HH81" s="75"/>
+      <c r="HI81" s="75"/>
+      <c r="HJ81" s="75"/>
+      <c r="HK81" s="75"/>
+      <c r="HL81" s="75"/>
+      <c r="HM81" s="75"/>
+      <c r="HN81" s="75"/>
+      <c r="HO81" s="75"/>
+      <c r="HP81" s="75"/>
+      <c r="HQ81" s="75"/>
+      <c r="HR81" s="75"/>
+      <c r="HS81" s="75"/>
+      <c r="HT81" s="75"/>
+      <c r="HU81" s="75"/>
+      <c r="HV81" s="75"/>
+      <c r="HW81" s="75"/>
+      <c r="HX81" s="75"/>
+      <c r="HY81" s="75"/>
+      <c r="HZ81" s="75"/>
+      <c r="IA81" s="75"/>
+      <c r="IB81" s="75"/>
+      <c r="IC81" s="75"/>
+      <c r="ID81" s="75"/>
+      <c r="IE81" s="75"/>
+      <c r="IF81" s="75"/>
+      <c r="IG81" s="75"/>
+      <c r="IH81" s="75"/>
+      <c r="II81" s="75"/>
+      <c r="IJ81" s="75"/>
+      <c r="IK81" s="75"/>
+      <c r="IL81" s="75"/>
+      <c r="IM81" s="75"/>
+      <c r="IN81" s="75"/>
+      <c r="IO81" s="75"/>
+      <c r="IP81" s="75"/>
+      <c r="IQ81" s="75"/>
+      <c r="IR81" s="75"/>
+      <c r="IS81" s="75"/>
+      <c r="IT81" s="75"/>
+      <c r="IU81" s="75"/>
+      <c r="IV81" s="75"/>
+      <c r="IW81" s="75"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:257">
       <c r="A82" s="73"/>
       <c r="B82" s="73"/>
       <c r="C82" s="73"/>
@@ -15727,7 +16004,7 @@
       <c r="I82" s="73"/>
       <c r="J82" s="73"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:257">
       <c r="A83" s="73"/>
       <c r="B83" s="73"/>
       <c r="C83" s="73"/>
@@ -15739,7 +16016,7 @@
       <c r="I83" s="73"/>
       <c r="J83" s="73"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:257">
       <c r="A84" s="73"/>
       <c r="B84" s="73"/>
       <c r="C84" s="73"/>
@@ -15751,7 +16028,7 @@
       <c r="I84" s="73"/>
       <c r="J84" s="73"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:257">
       <c r="A85" s="73"/>
       <c r="B85" s="73"/>
       <c r="C85" s="73"/>
@@ -15763,7 +16040,7 @@
       <c r="I85" s="73"/>
       <c r="J85" s="73"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:257">
       <c r="A86" s="73"/>
       <c r="B86" s="73"/>
       <c r="C86" s="73"/>
@@ -15775,7 +16052,7 @@
       <c r="I86" s="73"/>
       <c r="J86" s="73"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:257">
       <c r="A87" s="73"/>
       <c r="B87" s="73"/>
       <c r="C87" s="73"/>
@@ -15787,7 +16064,7 @@
       <c r="I87" s="73"/>
       <c r="J87" s="73"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:257">
       <c r="A88" s="73"/>
       <c r="B88" s="73"/>
       <c r="C88" s="73"/>
@@ -15799,7 +16076,7 @@
       <c r="I88" s="73"/>
       <c r="J88" s="73"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:257">
       <c r="A89" s="73"/>
       <c r="B89" s="73"/>
       <c r="C89" s="73"/>
@@ -15811,7 +16088,7 @@
       <c r="I89" s="73"/>
       <c r="J89" s="73"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:257">
       <c r="A90" s="73"/>
       <c r="B90" s="73"/>
       <c r="C90" s="73"/>
@@ -15823,7 +16100,7 @@
       <c r="I90" s="73"/>
       <c r="J90" s="73"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:257">
       <c r="A91" s="73"/>
       <c r="B91" s="73"/>
       <c r="C91" s="73"/>
@@ -15835,7 +16112,7 @@
       <c r="I91" s="73"/>
       <c r="J91" s="73"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:257">
       <c r="A92" s="73"/>
       <c r="B92" s="73"/>
       <c r="C92" s="73"/>
@@ -15847,7 +16124,7 @@
       <c r="I92" s="73"/>
       <c r="J92" s="73"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:257">
       <c r="A93" s="73"/>
       <c r="B93" s="73"/>
       <c r="C93" s="73"/>
@@ -15859,7 +16136,7 @@
       <c r="I93" s="73"/>
       <c r="J93" s="73"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:257">
       <c r="A94" s="73"/>
       <c r="B94" s="73"/>
       <c r="C94" s="73"/>
@@ -15870,6 +16147,18 @@
       <c r="H94" s="73"/>
       <c r="I94" s="73"/>
       <c r="J94" s="73"/>
+    </row>
+    <row r="95" spans="1:257">
+      <c r="A95" s="73"/>
+      <c r="B95" s="73"/>
+      <c r="C95" s="73"/>
+      <c r="D95" s="73"/>
+      <c r="E95" s="73"/>
+      <c r="F95" s="73"/>
+      <c r="G95" s="73"/>
+      <c r="H95" s="73"/>
+      <c r="I95" s="73"/>
+      <c r="J95" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
@@ -15882,23 +16171,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IW62"/>
+  <dimension ref="A1:IW63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD77"/>
+    <sheetView showGridLines="0" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="257" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="257" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.45" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -15930,7 +16219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17.45" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -15960,7 +16249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="13.7" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -15990,7 +16279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13.7" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -16020,7 +16309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="13.7" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -16050,7 +16339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="13.7" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -16080,7 +16369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.7" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -16110,7 +16399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="13.7" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -16140,7 +16429,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="13.7" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>26</v>
       </c>
@@ -16172,7 +16461,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="13.7" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -16204,7 +16493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="13.7" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
@@ -16236,7 +16525,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="13.7" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -16265,7 +16554,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="13.7" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -16295,7 +16584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="13.7" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -16322,7 +16611,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="13.7" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -16349,7 +16638,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -16381,7 +16670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -16413,7 +16702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>47</v>
       </c>
@@ -16445,7 +16734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="26" t="s">
         <v>49</v>
       </c>
@@ -16475,7 +16764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="26" t="s">
         <v>51</v>
       </c>
@@ -16505,7 +16794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>53</v>
       </c>
@@ -16532,7 +16821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="13.7" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
@@ -16564,7 +16853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="13.7" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>57</v>
       </c>
@@ -16596,7 +16885,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" customHeight="1">
       <c r="A24" s="29" t="s">
         <v>60</v>
       </c>
@@ -16628,7 +16917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="29" t="s">
         <v>62</v>
       </c>
@@ -16660,7 +16949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" customHeight="1">
       <c r="A26" s="29" t="s">
         <v>133</v>
       </c>
@@ -16692,7 +16981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" customHeight="1">
       <c r="A27" s="29" t="s">
         <v>64</v>
       </c>
@@ -16724,7 +17013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="29" t="s">
         <v>66</v>
       </c>
@@ -16756,7 +17045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" customHeight="1">
       <c r="A29" s="29" t="s">
         <v>68</v>
       </c>
@@ -16788,7 +17077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="12.75" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>70</v>
       </c>
@@ -16820,7 +17109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" customHeight="1">
       <c r="A31" s="29" t="s">
         <v>72</v>
       </c>
@@ -16852,7 +17141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" customHeight="1">
       <c r="A32" s="29" t="s">
         <v>73</v>
       </c>
@@ -16884,7 +17173,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:257" ht="12.75" customHeight="1">
       <c r="A33" s="29" t="s">
         <v>74</v>
       </c>
@@ -16916,7 +17205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:257" ht="12.75" customHeight="1">
       <c r="A34" s="29" t="s">
         <v>75</v>
       </c>
@@ -16948,7 +17237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:257" ht="12.75" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>76</v>
       </c>
@@ -16980,7 +17269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:257" ht="12.75" customHeight="1">
       <c r="A36" s="29" t="s">
         <v>77</v>
       </c>
@@ -17010,7 +17299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:257" ht="12.75" customHeight="1">
       <c r="A37" s="29" t="s">
         <v>79</v>
       </c>
@@ -17040,7 +17329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:257" ht="12.75" customHeight="1">
       <c r="A38" s="29" t="s">
         <v>81</v>
       </c>
@@ -17070,7 +17359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:257" ht="12.75" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>83</v>
       </c>
@@ -17100,7 +17389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:257" ht="12.75" customHeight="1">
       <c r="A40" s="29" t="s">
         <v>85</v>
       </c>
@@ -17130,7 +17419,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:257" ht="12.75" customHeight="1">
       <c r="A41" s="29" t="s">
         <v>87</v>
       </c>
@@ -17160,7 +17449,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:257" ht="12.75" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>89</v>
       </c>
@@ -17190,7 +17479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:257" ht="12.75" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>91</v>
       </c>
@@ -17220,7 +17509,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:257" ht="12.75" customHeight="1">
       <c r="A44" s="29" t="s">
         <v>92</v>
       </c>
@@ -17250,7 +17539,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:257" ht="12.75" customHeight="1">
       <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
@@ -17280,7 +17569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:257" ht="12.75" customHeight="1">
       <c r="A46" s="41" t="s">
         <v>97</v>
       </c>
@@ -17557,7 +17846,7 @@
       <c r="IV46" s="56"/>
       <c r="IW46" s="56"/>
     </row>
-    <row r="47" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:257" ht="12.75" customHeight="1">
       <c r="A47" s="46" t="s">
         <v>77</v>
       </c>
@@ -17832,7 +18121,7 @@
       <c r="IV47" s="56"/>
       <c r="IW47" s="56"/>
     </row>
-    <row r="48" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:257" ht="12.75" customHeight="1">
       <c r="A48" s="46" t="s">
         <v>79</v>
       </c>
@@ -18107,7 +18396,7 @@
       <c r="IV48" s="56"/>
       <c r="IW48" s="56"/>
     </row>
-    <row r="49" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:257" ht="12.75" customHeight="1">
       <c r="A49" s="46" t="s">
         <v>81</v>
       </c>
@@ -18382,7 +18671,7 @@
       <c r="IV49" s="56"/>
       <c r="IW49" s="56"/>
     </row>
-    <row r="50" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:257" ht="12.75" customHeight="1">
       <c r="A50" s="46" t="s">
         <v>83</v>
       </c>
@@ -18657,7 +18946,7 @@
       <c r="IV50" s="56"/>
       <c r="IW50" s="56"/>
     </row>
-    <row r="51" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:257" ht="12.75" customHeight="1">
       <c r="A51" s="46" t="s">
         <v>101</v>
       </c>
@@ -18932,7 +19221,7 @@
       <c r="IV51" s="56"/>
       <c r="IW51" s="56"/>
     </row>
-    <row r="52" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:257" ht="12.75" customHeight="1">
       <c r="A52" s="46" t="s">
         <v>102</v>
       </c>
@@ -19207,7 +19496,7 @@
       <c r="IV52" s="56"/>
       <c r="IW52" s="56"/>
     </row>
-    <row r="53" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:257" ht="12.75" customHeight="1">
       <c r="A53" s="46" t="s">
         <v>104</v>
       </c>
@@ -19482,7 +19771,7 @@
       <c r="IV53" s="56"/>
       <c r="IW53" s="56"/>
     </row>
-    <row r="54" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:257" ht="12.75" customHeight="1">
       <c r="A54" s="46" t="s">
         <v>106</v>
       </c>
@@ -19757,7 +20046,7 @@
       <c r="IV54" s="56"/>
       <c r="IW54" s="56"/>
     </row>
-    <row r="55" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:257" ht="12.75" customHeight="1">
       <c r="A55" s="46" t="s">
         <v>108</v>
       </c>
@@ -20032,7 +20321,7 @@
       <c r="IV55" s="56"/>
       <c r="IW55" s="56"/>
     </row>
-    <row r="56" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:257" ht="12.75" customHeight="1">
       <c r="A56" s="35" t="s">
         <v>22</v>
       </c>
@@ -20064,7 +20353,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:257" ht="12.75" customHeight="1">
       <c r="A57" s="35" t="s">
         <v>111</v>
       </c>
@@ -20091,7 +20380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:257" ht="12.75" customHeight="1">
       <c r="A58" s="35" t="s">
         <v>117</v>
       </c>
@@ -20118,7 +20407,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:257" ht="12.75" customHeight="1">
       <c r="A59" s="35" t="s">
         <v>113</v>
       </c>
@@ -20145,7 +20434,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:257" ht="12.75" customHeight="1">
       <c r="A60" s="35" t="s">
         <v>115</v>
       </c>
@@ -20175,7 +20464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:257" ht="12.75" customHeight="1">
       <c r="A61" s="37" t="s">
         <v>119</v>
       </c>
@@ -20207,7 +20496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:257" ht="12.75" customHeight="1">
       <c r="A62" s="35" t="s">
         <v>120</v>
       </c>
@@ -20238,6 +20527,265 @@
       <c r="J62" s="54" t="s">
         <v>122</v>
       </c>
+    </row>
+    <row r="63" spans="1:257" s="80" customFormat="1">
+      <c r="A63" s="77"/>
+      <c r="B63" s="78"/>
+      <c r="C63" s="78"/>
+      <c r="D63" s="78"/>
+      <c r="E63" s="78"/>
+      <c r="F63" s="78"/>
+      <c r="G63" s="81"/>
+      <c r="H63" s="81"/>
+      <c r="I63" s="78"/>
+      <c r="J63" s="78"/>
+      <c r="K63" s="79"/>
+      <c r="L63" s="79"/>
+      <c r="M63" s="79"/>
+      <c r="N63" s="79"/>
+      <c r="O63" s="79"/>
+      <c r="P63" s="79"/>
+      <c r="Q63" s="79"/>
+      <c r="R63" s="79"/>
+      <c r="S63" s="79"/>
+      <c r="T63" s="79"/>
+      <c r="U63" s="79"/>
+      <c r="V63" s="79"/>
+      <c r="W63" s="79"/>
+      <c r="X63" s="79"/>
+      <c r="Y63" s="79"/>
+      <c r="Z63" s="79"/>
+      <c r="AA63" s="79"/>
+      <c r="AB63" s="79"/>
+      <c r="AC63" s="79"/>
+      <c r="AD63" s="79"/>
+      <c r="AE63" s="79"/>
+      <c r="AF63" s="79"/>
+      <c r="AG63" s="79"/>
+      <c r="AH63" s="79"/>
+      <c r="AI63" s="79"/>
+      <c r="AJ63" s="79"/>
+      <c r="AK63" s="79"/>
+      <c r="AL63" s="79"/>
+      <c r="AM63" s="79"/>
+      <c r="AN63" s="79"/>
+      <c r="AO63" s="79"/>
+      <c r="AP63" s="79"/>
+      <c r="AQ63" s="79"/>
+      <c r="AR63" s="79"/>
+      <c r="AS63" s="79"/>
+      <c r="AT63" s="79"/>
+      <c r="AU63" s="79"/>
+      <c r="AV63" s="79"/>
+      <c r="AW63" s="79"/>
+      <c r="AX63" s="79"/>
+      <c r="AY63" s="79"/>
+      <c r="AZ63" s="79"/>
+      <c r="BA63" s="79"/>
+      <c r="BB63" s="79"/>
+      <c r="BC63" s="79"/>
+      <c r="BD63" s="79"/>
+      <c r="BE63" s="79"/>
+      <c r="BF63" s="79"/>
+      <c r="BG63" s="79"/>
+      <c r="BH63" s="79"/>
+      <c r="BI63" s="79"/>
+      <c r="BJ63" s="79"/>
+      <c r="BK63" s="79"/>
+      <c r="BL63" s="79"/>
+      <c r="BM63" s="79"/>
+      <c r="BN63" s="79"/>
+      <c r="BO63" s="79"/>
+      <c r="BP63" s="79"/>
+      <c r="BQ63" s="79"/>
+      <c r="BR63" s="79"/>
+      <c r="BS63" s="79"/>
+      <c r="BT63" s="79"/>
+      <c r="BU63" s="79"/>
+      <c r="BV63" s="79"/>
+      <c r="BW63" s="79"/>
+      <c r="BX63" s="79"/>
+      <c r="BY63" s="79"/>
+      <c r="BZ63" s="79"/>
+      <c r="CA63" s="79"/>
+      <c r="CB63" s="79"/>
+      <c r="CC63" s="79"/>
+      <c r="CD63" s="79"/>
+      <c r="CE63" s="79"/>
+      <c r="CF63" s="79"/>
+      <c r="CG63" s="79"/>
+      <c r="CH63" s="79"/>
+      <c r="CI63" s="79"/>
+      <c r="CJ63" s="79"/>
+      <c r="CK63" s="79"/>
+      <c r="CL63" s="79"/>
+      <c r="CM63" s="79"/>
+      <c r="CN63" s="79"/>
+      <c r="CO63" s="79"/>
+      <c r="CP63" s="79"/>
+      <c r="CQ63" s="79"/>
+      <c r="CR63" s="79"/>
+      <c r="CS63" s="79"/>
+      <c r="CT63" s="79"/>
+      <c r="CU63" s="79"/>
+      <c r="CV63" s="79"/>
+      <c r="CW63" s="79"/>
+      <c r="CX63" s="79"/>
+      <c r="CY63" s="79"/>
+      <c r="CZ63" s="79"/>
+      <c r="DA63" s="79"/>
+      <c r="DB63" s="79"/>
+      <c r="DC63" s="79"/>
+      <c r="DD63" s="79"/>
+      <c r="DE63" s="79"/>
+      <c r="DF63" s="79"/>
+      <c r="DG63" s="79"/>
+      <c r="DH63" s="79"/>
+      <c r="DI63" s="79"/>
+      <c r="DJ63" s="79"/>
+      <c r="DK63" s="79"/>
+      <c r="DL63" s="79"/>
+      <c r="DM63" s="79"/>
+      <c r="DN63" s="79"/>
+      <c r="DO63" s="79"/>
+      <c r="DP63" s="79"/>
+      <c r="DQ63" s="79"/>
+      <c r="DR63" s="79"/>
+      <c r="DS63" s="79"/>
+      <c r="DT63" s="79"/>
+      <c r="DU63" s="79"/>
+      <c r="DV63" s="79"/>
+      <c r="DW63" s="79"/>
+      <c r="DX63" s="79"/>
+      <c r="DY63" s="79"/>
+      <c r="DZ63" s="79"/>
+      <c r="EA63" s="79"/>
+      <c r="EB63" s="79"/>
+      <c r="EC63" s="79"/>
+      <c r="ED63" s="79"/>
+      <c r="EE63" s="79"/>
+      <c r="EF63" s="79"/>
+      <c r="EG63" s="79"/>
+      <c r="EH63" s="79"/>
+      <c r="EI63" s="79"/>
+      <c r="EJ63" s="79"/>
+      <c r="EK63" s="79"/>
+      <c r="EL63" s="79"/>
+      <c r="EM63" s="79"/>
+      <c r="EN63" s="79"/>
+      <c r="EO63" s="79"/>
+      <c r="EP63" s="79"/>
+      <c r="EQ63" s="79"/>
+      <c r="ER63" s="79"/>
+      <c r="ES63" s="79"/>
+      <c r="ET63" s="79"/>
+      <c r="EU63" s="79"/>
+      <c r="EV63" s="79"/>
+      <c r="EW63" s="79"/>
+      <c r="EX63" s="79"/>
+      <c r="EY63" s="79"/>
+      <c r="EZ63" s="79"/>
+      <c r="FA63" s="79"/>
+      <c r="FB63" s="79"/>
+      <c r="FC63" s="79"/>
+      <c r="FD63" s="79"/>
+      <c r="FE63" s="79"/>
+      <c r="FF63" s="79"/>
+      <c r="FG63" s="79"/>
+      <c r="FH63" s="79"/>
+      <c r="FI63" s="79"/>
+      <c r="FJ63" s="79"/>
+      <c r="FK63" s="79"/>
+      <c r="FL63" s="79"/>
+      <c r="FM63" s="79"/>
+      <c r="FN63" s="79"/>
+      <c r="FO63" s="79"/>
+      <c r="FP63" s="79"/>
+      <c r="FQ63" s="79"/>
+      <c r="FR63" s="79"/>
+      <c r="FS63" s="79"/>
+      <c r="FT63" s="79"/>
+      <c r="FU63" s="79"/>
+      <c r="FV63" s="79"/>
+      <c r="FW63" s="79"/>
+      <c r="FX63" s="79"/>
+      <c r="FY63" s="79"/>
+      <c r="FZ63" s="79"/>
+      <c r="GA63" s="79"/>
+      <c r="GB63" s="79"/>
+      <c r="GC63" s="79"/>
+      <c r="GD63" s="79"/>
+      <c r="GE63" s="79"/>
+      <c r="GF63" s="79"/>
+      <c r="GG63" s="79"/>
+      <c r="GH63" s="79"/>
+      <c r="GI63" s="79"/>
+      <c r="GJ63" s="79"/>
+      <c r="GK63" s="79"/>
+      <c r="GL63" s="79"/>
+      <c r="GM63" s="79"/>
+      <c r="GN63" s="79"/>
+      <c r="GO63" s="79"/>
+      <c r="GP63" s="79"/>
+      <c r="GQ63" s="79"/>
+      <c r="GR63" s="79"/>
+      <c r="GS63" s="79"/>
+      <c r="GT63" s="79"/>
+      <c r="GU63" s="79"/>
+      <c r="GV63" s="79"/>
+      <c r="GW63" s="79"/>
+      <c r="GX63" s="79"/>
+      <c r="GY63" s="79"/>
+      <c r="GZ63" s="79"/>
+      <c r="HA63" s="79"/>
+      <c r="HB63" s="79"/>
+      <c r="HC63" s="79"/>
+      <c r="HD63" s="79"/>
+      <c r="HE63" s="79"/>
+      <c r="HF63" s="79"/>
+      <c r="HG63" s="79"/>
+      <c r="HH63" s="79"/>
+      <c r="HI63" s="79"/>
+      <c r="HJ63" s="79"/>
+      <c r="HK63" s="79"/>
+      <c r="HL63" s="79"/>
+      <c r="HM63" s="79"/>
+      <c r="HN63" s="79"/>
+      <c r="HO63" s="79"/>
+      <c r="HP63" s="79"/>
+      <c r="HQ63" s="79"/>
+      <c r="HR63" s="79"/>
+      <c r="HS63" s="79"/>
+      <c r="HT63" s="79"/>
+      <c r="HU63" s="79"/>
+      <c r="HV63" s="79"/>
+      <c r="HW63" s="79"/>
+      <c r="HX63" s="79"/>
+      <c r="HY63" s="79"/>
+      <c r="HZ63" s="79"/>
+      <c r="IA63" s="79"/>
+      <c r="IB63" s="79"/>
+      <c r="IC63" s="79"/>
+      <c r="ID63" s="79"/>
+      <c r="IE63" s="79"/>
+      <c r="IF63" s="79"/>
+      <c r="IG63" s="79"/>
+      <c r="IH63" s="79"/>
+      <c r="II63" s="79"/>
+      <c r="IJ63" s="79"/>
+      <c r="IK63" s="79"/>
+      <c r="IL63" s="79"/>
+      <c r="IM63" s="79"/>
+      <c r="IN63" s="79"/>
+      <c r="IO63" s="79"/>
+      <c r="IP63" s="79"/>
+      <c r="IQ63" s="79"/>
+      <c r="IR63" s="79"/>
+      <c r="IS63" s="79"/>
+      <c r="IT63" s="79"/>
+      <c r="IU63" s="79"/>
+      <c r="IV63" s="79"/>
+      <c r="IW63" s="79"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
translated task to intervention for ratanak
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC88DA5-EC2A-4B13-A1A6-479AAA4DBD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0659D45-370F-4B79-8369-28EF6619EA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="1575" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="239">
   <si>
     <t>name</t>
   </si>
@@ -748,6 +748,9 @@
   </si>
   <si>
     <t>datagrid</t>
+  </si>
+  <si>
+    <t>care_plan</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1696,7 @@
   <dimension ref="A1:IW126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -27530,16 +27533,34 @@
       <c r="IW122"/>
     </row>
     <row r="123" spans="1:257">
-      <c r="A123" s="81"/>
-      <c r="B123" s="82"/>
-      <c r="C123" s="81"/>
+      <c r="A123" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="B123" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="C123" s="82" t="s">
+        <v>185</v>
+      </c>
       <c r="D123" s="82"/>
-      <c r="E123" s="82"/>
-      <c r="F123" s="82"/>
-      <c r="G123" s="83"/>
-      <c r="H123" s="83"/>
-      <c r="I123" s="82"/>
-      <c r="J123" s="82"/>
+      <c r="E123" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="F123" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="G123" s="83">
+        <v>0</v>
+      </c>
+      <c r="H123" s="83">
+        <v>1</v>
+      </c>
+      <c r="I123" s="82" t="s">
+        <v>181</v>
+      </c>
+      <c r="J123" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="K123"/>
       <c r="L123"/>
       <c r="M123"/>

</xml_diff>

<commit_message>
Fixed Translation in case_notes/form
</commit_message>
<xml_diff>
--- a/db/support/field_settings.xlsx
+++ b/db/support/field_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0659D45-370F-4B79-8369-28EF6619EA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9142068C-11CE-4EAE-A174-09F58ED11E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1575" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4350" yWindow="1920" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="241">
   <si>
     <t>name</t>
   </si>
@@ -751,6 +751,12 @@
   </si>
   <si>
     <t>care_plan</t>
+  </si>
+  <si>
+    <t>on_going_tasks</t>
+  </si>
+  <si>
+    <t>On Going Intervention</t>
   </si>
 </sst>
 </file>
@@ -1693,10 +1699,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW126"/>
+  <dimension ref="A1:IW127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -23379,17 +23385,17 @@
     </row>
     <row r="108" spans="1:257">
       <c r="A108" s="81" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="B108" s="81" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C108" s="81" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="D108" s="82"/>
       <c r="E108" s="81" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F108" s="82" t="s">
         <v>13</v>
@@ -23656,13 +23662,13 @@
     </row>
     <row r="109" spans="1:257">
       <c r="A109" s="81" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B109" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C109" s="81" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D109" s="82"/>
       <c r="E109" s="81" t="s">
@@ -23933,13 +23939,13 @@
     </row>
     <row r="110" spans="1:257">
       <c r="A110" s="81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B110" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C110" s="81" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D110" s="82"/>
       <c r="E110" s="81" t="s">
@@ -24210,13 +24216,13 @@
     </row>
     <row r="111" spans="1:257">
       <c r="A111" s="81" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B111" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C111" s="81" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D111" s="82"/>
       <c r="E111" s="81" t="s">
@@ -24487,13 +24493,13 @@
     </row>
     <row r="112" spans="1:257">
       <c r="A112" s="81" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B112" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C112" s="81" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D112" s="82"/>
       <c r="E112" s="81" t="s">
@@ -24764,13 +24770,13 @@
     </row>
     <row r="113" spans="1:257">
       <c r="A113" s="81" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B113" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C113" s="81" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D113" s="82"/>
       <c r="E113" s="81" t="s">
@@ -25041,17 +25047,17 @@
     </row>
     <row r="114" spans="1:257">
       <c r="A114" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="B114" s="82" t="s">
-        <v>234</v>
+        <v>231</v>
+      </c>
+      <c r="B114" s="81" t="s">
+        <v>221</v>
       </c>
       <c r="C114" s="81" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="D114" s="82"/>
-      <c r="E114" s="82" t="s">
-        <v>234</v>
+      <c r="E114" s="81" t="s">
+        <v>221</v>
       </c>
       <c r="F114" s="82" t="s">
         <v>13</v>
@@ -25318,13 +25324,13 @@
     </row>
     <row r="115" spans="1:257">
       <c r="A115" s="81" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B115" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C115" s="81" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D115" s="82"/>
       <c r="E115" s="82" t="s">
@@ -25595,13 +25601,13 @@
     </row>
     <row r="116" spans="1:257">
       <c r="A116" s="81" t="s">
-        <v>235</v>
+        <v>186</v>
       </c>
       <c r="B116" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C116" s="81" t="s">
-        <v>236</v>
+        <v>187</v>
       </c>
       <c r="D116" s="82"/>
       <c r="E116" s="82" t="s">
@@ -25872,13 +25878,13 @@
     </row>
     <row r="117" spans="1:257">
       <c r="A117" s="81" t="s">
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="B117" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C117" s="81" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="D117" s="82"/>
       <c r="E117" s="82" t="s">
@@ -26149,13 +26155,13 @@
     </row>
     <row r="118" spans="1:257">
       <c r="A118" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B118" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C118" s="81" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D118" s="82"/>
       <c r="E118" s="82" t="s">
@@ -26426,13 +26432,13 @@
     </row>
     <row r="119" spans="1:257">
       <c r="A119" s="81" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B119" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C119" s="81" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D119" s="82"/>
       <c r="E119" s="82" t="s">
@@ -26703,13 +26709,13 @@
     </row>
     <row r="120" spans="1:257">
       <c r="A120" s="81" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B120" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C120" s="81" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D120" s="82"/>
       <c r="E120" s="82" t="s">
@@ -26980,13 +26986,13 @@
     </row>
     <row r="121" spans="1:257">
       <c r="A121" s="81" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="B121" s="82" t="s">
         <v>234</v>
       </c>
       <c r="C121" s="81" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D121" s="82"/>
       <c r="E121" s="82" t="s">
@@ -27257,17 +27263,17 @@
     </row>
     <row r="122" spans="1:257">
       <c r="A122" s="81" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="B122" s="82" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C122" s="81" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D122" s="82"/>
       <c r="E122" s="82" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F122" s="82" t="s">
         <v>13</v>
@@ -27533,18 +27539,18 @@
       <c r="IW122"/>
     </row>
     <row r="123" spans="1:257">
-      <c r="A123" s="82" t="s">
-        <v>184</v>
+      <c r="A123" s="81" t="s">
+        <v>207</v>
       </c>
       <c r="B123" s="82" t="s">
-        <v>238</v>
-      </c>
-      <c r="C123" s="82" t="s">
-        <v>185</v>
+        <v>237</v>
+      </c>
+      <c r="C123" s="81" t="s">
+        <v>208</v>
       </c>
       <c r="D123" s="82"/>
       <c r="E123" s="82" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F123" s="82" t="s">
         <v>13</v>
@@ -27810,16 +27816,34 @@
       <c r="IW123"/>
     </row>
     <row r="124" spans="1:257">
-      <c r="A124" s="81"/>
-      <c r="B124" s="82"/>
-      <c r="C124" s="81"/>
+      <c r="A124" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="B124" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="C124" s="82" t="s">
+        <v>185</v>
+      </c>
       <c r="D124" s="82"/>
-      <c r="E124" s="82"/>
-      <c r="F124" s="82"/>
-      <c r="G124" s="83"/>
-      <c r="H124" s="83"/>
-      <c r="I124" s="82"/>
-      <c r="J124" s="82"/>
+      <c r="E124" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="F124" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="G124" s="83">
+        <v>0</v>
+      </c>
+      <c r="H124" s="83">
+        <v>1</v>
+      </c>
+      <c r="I124" s="82" t="s">
+        <v>181</v>
+      </c>
+      <c r="J124" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="K124"/>
       <c r="L124"/>
       <c r="M124"/>
@@ -28586,6 +28610,265 @@
       <c r="IV126"/>
       <c r="IW126"/>
     </row>
+    <row r="127" spans="1:257">
+      <c r="A127" s="81"/>
+      <c r="B127" s="82"/>
+      <c r="C127" s="81"/>
+      <c r="D127" s="82"/>
+      <c r="E127" s="82"/>
+      <c r="F127" s="82"/>
+      <c r="G127" s="83"/>
+      <c r="H127" s="83"/>
+      <c r="I127" s="82"/>
+      <c r="J127" s="82"/>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127"/>
+      <c r="N127"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
+      <c r="R127"/>
+      <c r="S127"/>
+      <c r="T127"/>
+      <c r="U127"/>
+      <c r="V127"/>
+      <c r="W127"/>
+      <c r="X127"/>
+      <c r="Y127"/>
+      <c r="Z127"/>
+      <c r="AA127"/>
+      <c r="AB127"/>
+      <c r="AC127"/>
+      <c r="AD127"/>
+      <c r="AE127"/>
+      <c r="AF127"/>
+      <c r="AG127"/>
+      <c r="AH127"/>
+      <c r="AI127"/>
+      <c r="AJ127"/>
+      <c r="AK127"/>
+      <c r="AL127"/>
+      <c r="AM127"/>
+      <c r="AN127"/>
+      <c r="AO127"/>
+      <c r="AP127"/>
+      <c r="AQ127"/>
+      <c r="AR127"/>
+      <c r="AS127"/>
+      <c r="AT127"/>
+      <c r="AU127"/>
+      <c r="AV127"/>
+      <c r="AW127"/>
+      <c r="AX127"/>
+      <c r="AY127"/>
+      <c r="AZ127"/>
+      <c r="BA127"/>
+      <c r="BB127"/>
+      <c r="BC127"/>
+      <c r="BD127"/>
+      <c r="BE127"/>
+      <c r="BF127"/>
+      <c r="BG127"/>
+      <c r="BH127"/>
+      <c r="BI127"/>
+      <c r="BJ127"/>
+      <c r="BK127"/>
+      <c r="BL127"/>
+      <c r="BM127"/>
+      <c r="BN127"/>
+      <c r="BO127"/>
+      <c r="BP127"/>
+      <c r="BQ127"/>
+      <c r="BR127"/>
+      <c r="BS127"/>
+      <c r="BT127"/>
+      <c r="BU127"/>
+      <c r="BV127"/>
+      <c r="BW127"/>
+      <c r="BX127"/>
+      <c r="BY127"/>
+      <c r="BZ127"/>
+      <c r="CA127"/>
+      <c r="CB127"/>
+      <c r="CC127"/>
+      <c r="CD127"/>
+      <c r="CE127"/>
+      <c r="CF127"/>
+      <c r="CG127"/>
+      <c r="CH127"/>
+      <c r="CI127"/>
+      <c r="CJ127"/>
+      <c r="CK127"/>
+      <c r="CL127"/>
+      <c r="CM127"/>
+      <c r="CN127"/>
+      <c r="CO127"/>
+      <c r="CP127"/>
+      <c r="CQ127"/>
+      <c r="CR127"/>
+      <c r="CS127"/>
+      <c r="CT127"/>
+      <c r="CU127"/>
+      <c r="CV127"/>
+      <c r="CW127"/>
+      <c r="CX127"/>
+      <c r="CY127"/>
+      <c r="CZ127"/>
+      <c r="DA127"/>
+      <c r="DB127"/>
+      <c r="DC127"/>
+      <c r="DD127"/>
+      <c r="DE127"/>
+      <c r="DF127"/>
+      <c r="DG127"/>
+      <c r="DH127"/>
+      <c r="DI127"/>
+      <c r="DJ127"/>
+      <c r="DK127"/>
+      <c r="DL127"/>
+      <c r="DM127"/>
+      <c r="DN127"/>
+      <c r="DO127"/>
+      <c r="DP127"/>
+      <c r="DQ127"/>
+      <c r="DR127"/>
+      <c r="DS127"/>
+      <c r="DT127"/>
+      <c r="DU127"/>
+      <c r="DV127"/>
+      <c r="DW127"/>
+      <c r="DX127"/>
+      <c r="DY127"/>
+      <c r="DZ127"/>
+      <c r="EA127"/>
+      <c r="EB127"/>
+      <c r="EC127"/>
+      <c r="ED127"/>
+      <c r="EE127"/>
+      <c r="EF127"/>
+      <c r="EG127"/>
+      <c r="EH127"/>
+      <c r="EI127"/>
+      <c r="EJ127"/>
+      <c r="EK127"/>
+      <c r="EL127"/>
+      <c r="EM127"/>
+      <c r="EN127"/>
+      <c r="EO127"/>
+      <c r="EP127"/>
+      <c r="EQ127"/>
+      <c r="ER127"/>
+      <c r="ES127"/>
+      <c r="ET127"/>
+      <c r="EU127"/>
+      <c r="EV127"/>
+      <c r="EW127"/>
+      <c r="EX127"/>
+      <c r="EY127"/>
+      <c r="EZ127"/>
+      <c r="FA127"/>
+      <c r="FB127"/>
+      <c r="FC127"/>
+      <c r="FD127"/>
+      <c r="FE127"/>
+      <c r="FF127"/>
+      <c r="FG127"/>
+      <c r="FH127"/>
+      <c r="FI127"/>
+      <c r="FJ127"/>
+      <c r="FK127"/>
+      <c r="FL127"/>
+      <c r="FM127"/>
+      <c r="FN127"/>
+      <c r="FO127"/>
+      <c r="FP127"/>
+      <c r="FQ127"/>
+      <c r="FR127"/>
+      <c r="FS127"/>
+      <c r="FT127"/>
+      <c r="FU127"/>
+      <c r="FV127"/>
+      <c r="FW127"/>
+      <c r="FX127"/>
+      <c r="FY127"/>
+      <c r="FZ127"/>
+      <c r="GA127"/>
+      <c r="GB127"/>
+      <c r="GC127"/>
+      <c r="GD127"/>
+      <c r="GE127"/>
+      <c r="GF127"/>
+      <c r="GG127"/>
+      <c r="GH127"/>
+      <c r="GI127"/>
+      <c r="GJ127"/>
+      <c r="GK127"/>
+      <c r="GL127"/>
+      <c r="GM127"/>
+      <c r="GN127"/>
+      <c r="GO127"/>
+      <c r="GP127"/>
+      <c r="GQ127"/>
+      <c r="GR127"/>
+      <c r="GS127"/>
+      <c r="GT127"/>
+      <c r="GU127"/>
+      <c r="GV127"/>
+      <c r="GW127"/>
+      <c r="GX127"/>
+      <c r="GY127"/>
+      <c r="GZ127"/>
+      <c r="HA127"/>
+      <c r="HB127"/>
+      <c r="HC127"/>
+      <c r="HD127"/>
+      <c r="HE127"/>
+      <c r="HF127"/>
+      <c r="HG127"/>
+      <c r="HH127"/>
+      <c r="HI127"/>
+      <c r="HJ127"/>
+      <c r="HK127"/>
+      <c r="HL127"/>
+      <c r="HM127"/>
+      <c r="HN127"/>
+      <c r="HO127"/>
+      <c r="HP127"/>
+      <c r="HQ127"/>
+      <c r="HR127"/>
+      <c r="HS127"/>
+      <c r="HT127"/>
+      <c r="HU127"/>
+      <c r="HV127"/>
+      <c r="HW127"/>
+      <c r="HX127"/>
+      <c r="HY127"/>
+      <c r="HZ127"/>
+      <c r="IA127"/>
+      <c r="IB127"/>
+      <c r="IC127"/>
+      <c r="ID127"/>
+      <c r="IE127"/>
+      <c r="IF127"/>
+      <c r="IG127"/>
+      <c r="IH127"/>
+      <c r="II127"/>
+      <c r="IJ127"/>
+      <c r="IK127"/>
+      <c r="IL127"/>
+      <c r="IM127"/>
+      <c r="IN127"/>
+      <c r="IO127"/>
+      <c r="IP127"/>
+      <c r="IQ127"/>
+      <c r="IR127"/>
+      <c r="IS127"/>
+      <c r="IT127"/>
+      <c r="IU127"/>
+      <c r="IV127"/>
+      <c r="IW127"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>